<commit_message>
Code updated 23-02-14 11:30:34
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G159"/>
+  <dimension ref="A1:I160"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,6 +426,16 @@
           <t>02-12_0</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>02-13_A</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>02-13_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -452,9 +462,15 @@
       <c r="F2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2470</t>
         </is>
       </c>
     </row>
@@ -483,9 +499,15 @@
       <c r="F3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>2835</t>
+      <c r="G3" t="n">
+        <v>2835</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>3098</t>
         </is>
       </c>
     </row>
@@ -514,9 +536,15 @@
       <c r="F4" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>2994</t>
+      <c r="G4" t="n">
+        <v>2994</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>3428</t>
         </is>
       </c>
     </row>
@@ -545,9 +573,15 @@
       <c r="F5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>2817</t>
+      <c r="G5" t="n">
+        <v>2817</v>
+      </c>
+      <c r="H5" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2903</t>
         </is>
       </c>
     </row>
@@ -576,9 +610,15 @@
       <c r="F6" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>2807</t>
+      <c r="G6" t="n">
+        <v>2807</v>
+      </c>
+      <c r="H6" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>3143</t>
         </is>
       </c>
     </row>
@@ -607,9 +647,15 @@
       <c r="F7" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>3051</t>
+      <c r="G7" t="n">
+        <v>3051</v>
+      </c>
+      <c r="H7" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>3564</t>
         </is>
       </c>
     </row>
@@ -638,9 +684,15 @@
       <c r="F8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>2814</t>
+      <c r="G8" t="n">
+        <v>2814</v>
+      </c>
+      <c r="H8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>3089</t>
         </is>
       </c>
     </row>
@@ -669,9 +721,15 @@
       <c r="F9" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>2949</t>
+      <c r="G9" t="n">
+        <v>2949</v>
+      </c>
+      <c r="H9" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>3118</t>
         </is>
       </c>
     </row>
@@ -700,9 +758,15 @@
       <c r="F10" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>2894</t>
+      <c r="G10" t="n">
+        <v>2894</v>
+      </c>
+      <c r="H10" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>3194</t>
         </is>
       </c>
     </row>
@@ -731,9 +795,15 @@
       <c r="F11" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>2754</t>
+      <c r="G11" t="n">
+        <v>2754</v>
+      </c>
+      <c r="H11" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>3052</t>
         </is>
       </c>
     </row>
@@ -762,9 +832,15 @@
       <c r="F12" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>2634</t>
+      <c r="G12" t="n">
+        <v>2634</v>
+      </c>
+      <c r="H12" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>2677</t>
         </is>
       </c>
     </row>
@@ -793,9 +869,15 @@
       <c r="F13" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>3053</t>
+      <c r="G13" t="n">
+        <v>3053</v>
+      </c>
+      <c r="H13" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>3497</t>
         </is>
       </c>
     </row>
@@ -824,9 +906,15 @@
       <c r="F14" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>2825</t>
+      <c r="G14" t="n">
+        <v>2825</v>
+      </c>
+      <c r="H14" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>3158</t>
         </is>
       </c>
     </row>
@@ -855,9 +943,15 @@
       <c r="F15" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>2746</t>
+      <c r="G15" t="n">
+        <v>2746</v>
+      </c>
+      <c r="H15" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>2892</t>
         </is>
       </c>
     </row>
@@ -886,9 +980,15 @@
       <c r="F16" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>2961</t>
+      <c r="G16" t="n">
+        <v>2961</v>
+      </c>
+      <c r="H16" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>3301</t>
         </is>
       </c>
     </row>
@@ -917,9 +1017,15 @@
       <c r="F17" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>2793</t>
+      <c r="G17" t="n">
+        <v>2793</v>
+      </c>
+      <c r="H17" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>3045</t>
         </is>
       </c>
     </row>
@@ -948,9 +1054,15 @@
       <c r="F18" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>2584</t>
+      <c r="G18" t="n">
+        <v>2584</v>
+      </c>
+      <c r="H18" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>2703</t>
         </is>
       </c>
     </row>
@@ -979,9 +1091,15 @@
       <c r="F19" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>2815</t>
+      <c r="G19" t="n">
+        <v>2815</v>
+      </c>
+      <c r="H19" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>3090</t>
         </is>
       </c>
     </row>
@@ -1010,9 +1128,15 @@
       <c r="F20" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>3051</t>
+      <c r="G20" t="n">
+        <v>3051</v>
+      </c>
+      <c r="H20" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>3515</t>
         </is>
       </c>
     </row>
@@ -1041,9 +1165,15 @@
       <c r="F21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="G21" t="n">
+        <v>2500</v>
+      </c>
+      <c r="H21" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>2726</t>
         </is>
       </c>
     </row>
@@ -1072,9 +1202,15 @@
       <c r="F22" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>2919</t>
+      <c r="G22" t="n">
+        <v>2919</v>
+      </c>
+      <c r="H22" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>3189</t>
         </is>
       </c>
     </row>
@@ -1103,9 +1239,15 @@
       <c r="F23" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>2826</t>
+      <c r="G23" t="n">
+        <v>2826</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>2979</t>
         </is>
       </c>
     </row>
@@ -1134,9 +1276,15 @@
       <c r="F24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>2947</t>
+      <c r="G24" t="n">
+        <v>2947</v>
+      </c>
+      <c r="H24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>3197</t>
         </is>
       </c>
     </row>
@@ -1165,7 +1313,13 @@
       <c r="F25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G25" t="inlineStr">
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1196,9 +1350,15 @@
       <c r="F26" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>3091</t>
+      <c r="G26" t="n">
+        <v>3091</v>
+      </c>
+      <c r="H26" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>3465</t>
         </is>
       </c>
     </row>
@@ -1227,9 +1387,15 @@
       <c r="F27" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>2977</t>
+      <c r="G27" t="n">
+        <v>2977</v>
+      </c>
+      <c r="H27" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>3212</t>
         </is>
       </c>
     </row>
@@ -1258,9 +1424,15 @@
       <c r="F28" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>2849</t>
+      <c r="G28" t="n">
+        <v>2849</v>
+      </c>
+      <c r="H28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>2988</t>
         </is>
       </c>
     </row>
@@ -1289,9 +1461,15 @@
       <c r="F29" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>3172</t>
+      <c r="G29" t="n">
+        <v>3172</v>
+      </c>
+      <c r="H29" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>3583</t>
         </is>
       </c>
     </row>
@@ -1320,9 +1498,15 @@
       <c r="F30" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>2814</t>
+      <c r="G30" t="n">
+        <v>2814</v>
+      </c>
+      <c r="H30" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>3153</t>
         </is>
       </c>
     </row>
@@ -1351,9 +1535,15 @@
       <c r="F31" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>2937</t>
+      <c r="G31" t="n">
+        <v>2937</v>
+      </c>
+      <c r="H31" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>3458</t>
         </is>
       </c>
     </row>
@@ -1382,9 +1572,15 @@
       <c r="F32" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>2885</t>
+      <c r="G32" t="n">
+        <v>2885</v>
+      </c>
+      <c r="H32" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>3265</t>
         </is>
       </c>
     </row>
@@ -1413,9 +1609,15 @@
       <c r="F33" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>2781</t>
+      <c r="G33" t="n">
+        <v>2781</v>
+      </c>
+      <c r="H33" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>3195</t>
         </is>
       </c>
     </row>
@@ -1444,9 +1646,15 @@
       <c r="F34" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>2927</t>
+      <c r="G34" t="n">
+        <v>2927</v>
+      </c>
+      <c r="H34" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>3210</t>
         </is>
       </c>
     </row>
@@ -1475,9 +1683,15 @@
       <c r="F35" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>2934</t>
+      <c r="G35" t="n">
+        <v>2934</v>
+      </c>
+      <c r="H35" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>3275</t>
         </is>
       </c>
     </row>
@@ -1506,9 +1720,15 @@
       <c r="F36" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>2788</t>
+      <c r="G36" t="n">
+        <v>2788</v>
+      </c>
+      <c r="H36" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>3061</t>
         </is>
       </c>
     </row>
@@ -1537,9 +1757,15 @@
       <c r="F37" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>2865</t>
+      <c r="G37" t="n">
+        <v>2865</v>
+      </c>
+      <c r="H37" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>3211</t>
         </is>
       </c>
     </row>
@@ -1568,9 +1794,15 @@
       <c r="F38" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>2952</t>
+      <c r="G38" t="n">
+        <v>2952</v>
+      </c>
+      <c r="H38" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>3220</t>
         </is>
       </c>
     </row>
@@ -1599,9 +1831,15 @@
       <c r="F39" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>2941</t>
+      <c r="G39" t="n">
+        <v>2941</v>
+      </c>
+      <c r="H39" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>3284</t>
         </is>
       </c>
     </row>
@@ -1630,9 +1868,15 @@
       <c r="F40" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>2935</t>
+      <c r="G40" t="n">
+        <v>2935</v>
+      </c>
+      <c r="H40" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>3389</t>
         </is>
       </c>
     </row>
@@ -1655,15 +1899,21 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F41" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>2815</t>
+      <c r="G41" t="n">
+        <v>2815</v>
+      </c>
+      <c r="H41" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>3154</t>
         </is>
       </c>
     </row>
@@ -1692,9 +1942,15 @@
       <c r="F42" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>3027</t>
+      <c r="G42" t="n">
+        <v>3027</v>
+      </c>
+      <c r="H42" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>3429</t>
         </is>
       </c>
     </row>
@@ -1723,9 +1979,15 @@
       <c r="F43" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>2869</t>
+      <c r="G43" t="n">
+        <v>2869</v>
+      </c>
+      <c r="H43" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>3210</t>
         </is>
       </c>
     </row>
@@ -1754,9 +2016,15 @@
       <c r="F44" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>2877</t>
+      <c r="G44" t="n">
+        <v>2877</v>
+      </c>
+      <c r="H44" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>3329</t>
         </is>
       </c>
     </row>
@@ -1785,9 +2053,15 @@
       <c r="F45" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>2876</t>
+      <c r="G45" t="n">
+        <v>2876</v>
+      </c>
+      <c r="H45" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>3193</t>
         </is>
       </c>
     </row>
@@ -1816,9 +2090,15 @@
       <c r="F46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>2933</t>
+      <c r="G46" t="n">
+        <v>2933</v>
+      </c>
+      <c r="H46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>3207</t>
         </is>
       </c>
     </row>
@@ -1847,7 +2127,13 @@
       <c r="F47" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G47" t="inlineStr">
+      <c r="G47" t="n">
+        <v>2500</v>
+      </c>
+      <c r="H47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1878,9 +2164,15 @@
       <c r="F48" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>2883</t>
+      <c r="G48" t="n">
+        <v>2883</v>
+      </c>
+      <c r="H48" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>3359</t>
         </is>
       </c>
     </row>
@@ -1909,9 +2201,15 @@
       <c r="F49" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>2691</t>
+      <c r="G49" t="n">
+        <v>2691</v>
+      </c>
+      <c r="H49" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>2949</t>
         </is>
       </c>
     </row>
@@ -1940,9 +2238,15 @@
       <c r="F50" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>2954</t>
+      <c r="G50" t="n">
+        <v>2954</v>
+      </c>
+      <c r="H50" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>3400</t>
         </is>
       </c>
     </row>
@@ -1971,9 +2275,15 @@
       <c r="F51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>2501</t>
+      <c r="G51" t="n">
+        <v>2501</v>
+      </c>
+      <c r="H51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>2522</t>
         </is>
       </c>
     </row>
@@ -2002,7 +2312,13 @@
       <c r="F52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G52" t="inlineStr">
+      <c r="G52" t="n">
+        <v>0</v>
+      </c>
+      <c r="H52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I52" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2033,9 +2349,15 @@
       <c r="F53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>2492</t>
+      <c r="G53" t="n">
+        <v>2492</v>
+      </c>
+      <c r="H53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>2486</t>
         </is>
       </c>
     </row>
@@ -2064,9 +2386,15 @@
       <c r="F54" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>2959</t>
+      <c r="G54" t="n">
+        <v>2959</v>
+      </c>
+      <c r="H54" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>3422</t>
         </is>
       </c>
     </row>
@@ -2095,9 +2423,15 @@
       <c r="F55" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>2733</t>
+      <c r="G55" t="n">
+        <v>2733</v>
+      </c>
+      <c r="H55" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>2870</t>
         </is>
       </c>
     </row>
@@ -2126,9 +2460,15 @@
       <c r="F56" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>2684</t>
+      <c r="G56" t="n">
+        <v>2684</v>
+      </c>
+      <c r="H56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>2918</t>
         </is>
       </c>
     </row>
@@ -2157,9 +2497,15 @@
       <c r="F57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>2813</t>
+      <c r="G57" t="n">
+        <v>2813</v>
+      </c>
+      <c r="H57" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>3163</t>
         </is>
       </c>
     </row>
@@ -2188,9 +2534,15 @@
       <c r="F58" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>2765</t>
+      <c r="G58" t="n">
+        <v>2765</v>
+      </c>
+      <c r="H58" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>2836</t>
         </is>
       </c>
     </row>
@@ -2214,6 +2566,8 @@
       <c r="E59" t="inlineStr"/>
       <c r="F59" s="3" t="inlineStr"/>
       <c r="G59" t="inlineStr"/>
+      <c r="H59" s="3" t="inlineStr"/>
+      <c r="I59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -2235,6 +2589,8 @@
       <c r="E60" t="inlineStr"/>
       <c r="F60" s="3" t="inlineStr"/>
       <c r="G60" t="inlineStr"/>
+      <c r="H60" s="3" t="inlineStr"/>
+      <c r="I60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -2261,9 +2617,15 @@
       <c r="F61" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>2773</t>
+      <c r="G61" t="n">
+        <v>2773</v>
+      </c>
+      <c r="H61" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>3096</t>
         </is>
       </c>
     </row>
@@ -2292,7 +2654,13 @@
       <c r="F62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G62" t="inlineStr">
+      <c r="G62" t="n">
+        <v>0</v>
+      </c>
+      <c r="H62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2323,9 +2691,15 @@
       <c r="F63" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>2876</t>
+      <c r="G63" t="n">
+        <v>2876</v>
+      </c>
+      <c r="H63" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>3204</t>
         </is>
       </c>
     </row>
@@ -2354,9 +2728,15 @@
       <c r="F64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>2494</t>
+      <c r="G64" t="n">
+        <v>2494</v>
+      </c>
+      <c r="H64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>2490</t>
         </is>
       </c>
     </row>
@@ -2380,6 +2760,8 @@
       <c r="E65" t="inlineStr"/>
       <c r="F65" s="3" t="inlineStr"/>
       <c r="G65" t="inlineStr"/>
+      <c r="H65" s="3" t="inlineStr"/>
+      <c r="I65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -2406,9 +2788,15 @@
       <c r="F66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G66" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>2460</t>
         </is>
       </c>
     </row>
@@ -2437,9 +2825,15 @@
       <c r="F67" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>2722</t>
+      <c r="G67" t="n">
+        <v>2722</v>
+      </c>
+      <c r="H67" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>2974</t>
         </is>
       </c>
     </row>
@@ -2468,9 +2862,15 @@
       <c r="F68" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>2856</t>
+      <c r="G68" t="n">
+        <v>2856</v>
+      </c>
+      <c r="H68" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>3272</t>
         </is>
       </c>
     </row>
@@ -2499,9 +2899,15 @@
       <c r="F69" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>2816</t>
+      <c r="G69" t="n">
+        <v>2816</v>
+      </c>
+      <c r="H69" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>2894</t>
         </is>
       </c>
     </row>
@@ -2530,9 +2936,15 @@
       <c r="F70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>2505</t>
+      <c r="G70" t="n">
+        <v>2505</v>
+      </c>
+      <c r="H70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>2521</t>
         </is>
       </c>
     </row>
@@ -2561,9 +2973,15 @@
       <c r="F71" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>2725</t>
+      <c r="G71" t="n">
+        <v>2725</v>
+      </c>
+      <c r="H71" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>2893</t>
         </is>
       </c>
     </row>
@@ -2592,9 +3010,15 @@
       <c r="F72" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>2796</t>
+      <c r="G72" t="n">
+        <v>2796</v>
+      </c>
+      <c r="H72" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>2788</t>
         </is>
       </c>
     </row>
@@ -2623,9 +3047,15 @@
       <c r="F73" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>2722</t>
+      <c r="G73" t="n">
+        <v>2722</v>
+      </c>
+      <c r="H73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>2928</t>
         </is>
       </c>
     </row>
@@ -2654,9 +3084,15 @@
       <c r="F74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>2515</t>
+      <c r="G74" t="n">
+        <v>2515</v>
+      </c>
+      <c r="H74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>2526</t>
         </is>
       </c>
     </row>
@@ -2685,9 +3121,15 @@
       <c r="F75" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>2711</t>
+      <c r="G75" t="n">
+        <v>2711</v>
+      </c>
+      <c r="H75" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>2920</t>
         </is>
       </c>
     </row>
@@ -2716,9 +3158,15 @@
       <c r="F76" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>2786</t>
+      <c r="G76" t="n">
+        <v>2786</v>
+      </c>
+      <c r="H76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>2808</t>
         </is>
       </c>
     </row>
@@ -2747,9 +3195,15 @@
       <c r="F77" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>2808</t>
+      <c r="G77" t="n">
+        <v>2808</v>
+      </c>
+      <c r="H77" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>3120</t>
         </is>
       </c>
     </row>
@@ -2778,9 +3232,15 @@
       <c r="F78" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>2884</t>
+      <c r="G78" t="n">
+        <v>2884</v>
+      </c>
+      <c r="H78" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>3254</t>
         </is>
       </c>
     </row>
@@ -2809,7 +3269,13 @@
       <c r="F79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G79" t="inlineStr">
+      <c r="G79" t="n">
+        <v>0</v>
+      </c>
+      <c r="H79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2840,9 +3306,15 @@
       <c r="F80" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>2750</t>
+      <c r="G80" t="n">
+        <v>2750</v>
+      </c>
+      <c r="H80" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>3015</t>
         </is>
       </c>
     </row>
@@ -2871,9 +3343,15 @@
       <c r="F81" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>2896</t>
+      <c r="G81" t="n">
+        <v>2896</v>
+      </c>
+      <c r="H81" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>3139</t>
         </is>
       </c>
     </row>
@@ -2902,9 +3380,15 @@
       <c r="F82" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>2881</t>
+      <c r="G82" t="n">
+        <v>2881</v>
+      </c>
+      <c r="H82" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>3110</t>
         </is>
       </c>
     </row>
@@ -2933,9 +3417,15 @@
       <c r="F83" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>2802</t>
+      <c r="G83" t="n">
+        <v>2802</v>
+      </c>
+      <c r="H83" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>2973</t>
         </is>
       </c>
     </row>
@@ -2964,9 +3454,15 @@
       <c r="F84" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>2621</t>
+      <c r="G84" t="n">
+        <v>2621</v>
+      </c>
+      <c r="H84" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>2644</t>
         </is>
       </c>
     </row>
@@ -2995,9 +3491,15 @@
       <c r="F85" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>2620</t>
+      <c r="G85" t="n">
+        <v>2620</v>
+      </c>
+      <c r="H85" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>2808</t>
         </is>
       </c>
     </row>
@@ -3026,9 +3528,15 @@
       <c r="F86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>2475</t>
+      <c r="G86" t="n">
+        <v>2475</v>
+      </c>
+      <c r="H86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>2489</t>
         </is>
       </c>
     </row>
@@ -3057,9 +3565,15 @@
       <c r="F87" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>2926</t>
+      <c r="G87" t="n">
+        <v>2926</v>
+      </c>
+      <c r="H87" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>3133</t>
         </is>
       </c>
     </row>
@@ -3088,9 +3602,15 @@
       <c r="F88" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>2574</t>
+      <c r="G88" t="n">
+        <v>2574</v>
+      </c>
+      <c r="H88" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>2582</t>
         </is>
       </c>
     </row>
@@ -3119,9 +3639,15 @@
       <c r="F89" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>2631</t>
+      <c r="G89" t="n">
+        <v>2631</v>
+      </c>
+      <c r="H89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>2554</t>
         </is>
       </c>
     </row>
@@ -3150,9 +3676,15 @@
       <c r="F90" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>2495</t>
+      <c r="G90" t="n">
+        <v>2495</v>
+      </c>
+      <c r="H90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>2460</t>
         </is>
       </c>
     </row>
@@ -3181,9 +3713,15 @@
       <c r="F91" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>2555</t>
+      <c r="G91" t="n">
+        <v>2555</v>
+      </c>
+      <c r="H91" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>2595</t>
         </is>
       </c>
     </row>
@@ -3212,7 +3750,13 @@
       <c r="F92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G92" t="inlineStr">
+      <c r="G92" t="n">
+        <v>0</v>
+      </c>
+      <c r="H92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3243,9 +3787,15 @@
       <c r="F93" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>2486</t>
+      <c r="G93" t="n">
+        <v>2486</v>
+      </c>
+      <c r="H93" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>2431</t>
         </is>
       </c>
     </row>
@@ -3274,9 +3824,15 @@
       <c r="F94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G94" t="n">
+        <v>0</v>
+      </c>
+      <c r="H94" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>2579</t>
         </is>
       </c>
     </row>
@@ -3305,9 +3861,15 @@
       <c r="F95" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>2600</t>
+      <c r="G95" t="n">
+        <v>2600</v>
+      </c>
+      <c r="H95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>2493</t>
         </is>
       </c>
     </row>
@@ -3336,9 +3898,15 @@
       <c r="F96" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>2592</t>
+      <c r="G96" t="n">
+        <v>2592</v>
+      </c>
+      <c r="H96" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>2759</t>
         </is>
       </c>
     </row>
@@ -3367,9 +3935,15 @@
       <c r="F97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>2492</t>
+      <c r="G97" t="n">
+        <v>2492</v>
+      </c>
+      <c r="H97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>2478</t>
         </is>
       </c>
     </row>
@@ -3398,7 +3972,13 @@
       <c r="F98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G98" t="inlineStr">
+      <c r="G98" t="n">
+        <v>0</v>
+      </c>
+      <c r="H98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3429,9 +4009,15 @@
       <c r="F99" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>2574</t>
+      <c r="G99" t="n">
+        <v>2574</v>
+      </c>
+      <c r="H99" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>2730</t>
         </is>
       </c>
     </row>
@@ -3460,9 +4046,15 @@
       <c r="F100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>2454</t>
+      <c r="G100" t="n">
+        <v>2454</v>
+      </c>
+      <c r="H100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>2416</t>
         </is>
       </c>
     </row>
@@ -3491,9 +4083,15 @@
       <c r="F101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>2814</t>
+      <c r="G101" t="n">
+        <v>2814</v>
+      </c>
+      <c r="H101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>3075</t>
         </is>
       </c>
     </row>
@@ -3522,9 +4120,15 @@
       <c r="F102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G102" t="inlineStr">
-        <is>
-          <t>2664</t>
+      <c r="G102" t="n">
+        <v>2664</v>
+      </c>
+      <c r="H102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>2854</t>
         </is>
       </c>
     </row>
@@ -3553,9 +4157,15 @@
       <c r="F103" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="G103" t="inlineStr">
-        <is>
-          <t>2556</t>
+      <c r="G103" t="n">
+        <v>2556</v>
+      </c>
+      <c r="H103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>2521</t>
         </is>
       </c>
     </row>
@@ -3584,9 +4194,15 @@
       <c r="F104" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>2803</t>
+      <c r="G104" t="n">
+        <v>2803</v>
+      </c>
+      <c r="H104" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>2986</t>
         </is>
       </c>
     </row>
@@ -3615,9 +4231,15 @@
       <c r="F105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G105" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="G105" t="n">
+        <v>2500</v>
+      </c>
+      <c r="H105" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>2875</t>
         </is>
       </c>
     </row>
@@ -3646,7 +4268,13 @@
       <c r="F106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G106" t="inlineStr">
+      <c r="G106" t="n">
+        <v>0</v>
+      </c>
+      <c r="H106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3677,9 +4305,15 @@
       <c r="F107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G107" t="inlineStr">
-        <is>
-          <t>2497</t>
+      <c r="G107" t="n">
+        <v>2497</v>
+      </c>
+      <c r="H107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>2544</t>
         </is>
       </c>
     </row>
@@ -3708,7 +4342,13 @@
       <c r="F108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G108" t="inlineStr">
+      <c r="G108" t="n">
+        <v>0</v>
+      </c>
+      <c r="H108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3739,9 +4379,15 @@
       <c r="F109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G109" t="inlineStr">
-        <is>
-          <t>2565</t>
+      <c r="G109" t="n">
+        <v>2565</v>
+      </c>
+      <c r="H109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>2666</t>
         </is>
       </c>
     </row>
@@ -3770,9 +4416,15 @@
       <c r="F110" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G110" t="inlineStr">
-        <is>
-          <t>2599</t>
+      <c r="G110" t="n">
+        <v>2599</v>
+      </c>
+      <c r="H110" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>2743</t>
         </is>
       </c>
     </row>
@@ -3801,9 +4453,15 @@
       <c r="F111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G111" t="inlineStr">
-        <is>
-          <t>2535</t>
+      <c r="G111" t="n">
+        <v>2535</v>
+      </c>
+      <c r="H111" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>2559</t>
         </is>
       </c>
     </row>
@@ -3832,9 +4490,15 @@
       <c r="F112" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="G112" t="inlineStr">
-        <is>
-          <t>2498</t>
+      <c r="G112" t="n">
+        <v>2498</v>
+      </c>
+      <c r="H112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -3863,9 +4527,15 @@
       <c r="F113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G113" t="inlineStr">
-        <is>
-          <t>2557</t>
+      <c r="G113" t="n">
+        <v>2557</v>
+      </c>
+      <c r="H113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>2571</t>
         </is>
       </c>
     </row>
@@ -3894,7 +4564,13 @@
       <c r="F114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G114" t="inlineStr">
+      <c r="G114" t="n">
+        <v>0</v>
+      </c>
+      <c r="H114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I114" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3925,9 +4601,15 @@
       <c r="F115" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="G115" t="inlineStr">
-        <is>
-          <t>2517</t>
+      <c r="G115" t="n">
+        <v>2517</v>
+      </c>
+      <c r="H115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>2488</t>
         </is>
       </c>
     </row>
@@ -3956,9 +4638,15 @@
       <c r="F116" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="G116" t="inlineStr">
-        <is>
-          <t>2508</t>
+      <c r="G116" t="n">
+        <v>2508</v>
+      </c>
+      <c r="H116" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>2579</t>
         </is>
       </c>
     </row>
@@ -3987,9 +4675,15 @@
       <c r="F117" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="G117" t="inlineStr">
-        <is>
-          <t>2694</t>
+      <c r="G117" t="n">
+        <v>2694</v>
+      </c>
+      <c r="H117" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>3029</t>
         </is>
       </c>
     </row>
@@ -4018,7 +4712,13 @@
       <c r="F118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G118" t="inlineStr">
+      <c r="G118" t="n">
+        <v>0</v>
+      </c>
+      <c r="H118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4049,9 +4749,15 @@
       <c r="F119" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G119" t="inlineStr">
-        <is>
-          <t>2738</t>
+      <c r="G119" t="n">
+        <v>2738</v>
+      </c>
+      <c r="H119" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>2762</t>
         </is>
       </c>
     </row>
@@ -4080,9 +4786,15 @@
       <c r="F120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G120" t="inlineStr">
-        <is>
-          <t>2439</t>
+      <c r="G120" t="n">
+        <v>2439</v>
+      </c>
+      <c r="H120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>2417</t>
         </is>
       </c>
     </row>
@@ -4111,9 +4823,15 @@
       <c r="F121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G121" t="inlineStr">
-        <is>
-          <t>2540</t>
+      <c r="G121" t="n">
+        <v>2540</v>
+      </c>
+      <c r="H121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>2578</t>
         </is>
       </c>
     </row>
@@ -4142,7 +4860,13 @@
       <c r="F122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G122" t="inlineStr">
+      <c r="G122" t="n">
+        <v>0</v>
+      </c>
+      <c r="H122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4173,9 +4897,15 @@
       <c r="F123" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G123" t="inlineStr">
-        <is>
-          <t>2619</t>
+      <c r="G123" t="n">
+        <v>2619</v>
+      </c>
+      <c r="H123" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>2711</t>
         </is>
       </c>
     </row>
@@ -4204,9 +4934,15 @@
       <c r="F124" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G124" t="inlineStr">
-        <is>
-          <t>2470</t>
+      <c r="G124" t="n">
+        <v>2470</v>
+      </c>
+      <c r="H124" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>2613</t>
         </is>
       </c>
     </row>
@@ -4235,9 +4971,15 @@
       <c r="F125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G125" t="inlineStr">
-        <is>
-          <t>2501</t>
+      <c r="G125" t="n">
+        <v>2501</v>
+      </c>
+      <c r="H125" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>2716</t>
         </is>
       </c>
     </row>
@@ -4266,9 +5008,15 @@
       <c r="F126" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="G126" t="inlineStr">
-        <is>
-          <t>2560</t>
+      <c r="G126" t="n">
+        <v>2560</v>
+      </c>
+      <c r="H126" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>2715</t>
         </is>
       </c>
     </row>
@@ -4297,9 +5045,15 @@
       <c r="F127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G127" t="inlineStr">
-        <is>
-          <t>2453</t>
+      <c r="G127" t="n">
+        <v>2453</v>
+      </c>
+      <c r="H127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>2450</t>
         </is>
       </c>
     </row>
@@ -4328,7 +5082,13 @@
       <c r="F128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G128" t="inlineStr">
+      <c r="G128" t="n">
+        <v>0</v>
+      </c>
+      <c r="H128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4359,7 +5119,13 @@
       <c r="F129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G129" t="inlineStr">
+      <c r="G129" t="n">
+        <v>0</v>
+      </c>
+      <c r="H129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4390,9 +5156,15 @@
       <c r="F130" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="G130" t="inlineStr">
-        <is>
-          <t>2481</t>
+      <c r="G130" t="n">
+        <v>2481</v>
+      </c>
+      <c r="H130" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>2528</t>
         </is>
       </c>
     </row>
@@ -4421,9 +5193,15 @@
       <c r="F131" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G131" t="inlineStr">
-        <is>
-          <t>2478</t>
+      <c r="G131" t="n">
+        <v>2478</v>
+      </c>
+      <c r="H131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>2437</t>
         </is>
       </c>
     </row>
@@ -4452,9 +5230,15 @@
       <c r="F132" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G132" t="inlineStr">
-        <is>
-          <t>2408</t>
+      <c r="G132" t="n">
+        <v>2408</v>
+      </c>
+      <c r="H132" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>2414</t>
         </is>
       </c>
     </row>
@@ -4483,9 +5267,15 @@
       <c r="F133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G133" t="inlineStr">
-        <is>
-          <t>2458</t>
+      <c r="G133" t="n">
+        <v>2458</v>
+      </c>
+      <c r="H133" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I133" t="inlineStr">
+        <is>
+          <t>2689</t>
         </is>
       </c>
     </row>
@@ -4514,9 +5304,15 @@
       <c r="F134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G134" t="inlineStr">
-        <is>
-          <t>1200</t>
+      <c r="G134" t="n">
+        <v>1200</v>
+      </c>
+      <c r="H134" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>1503</t>
         </is>
       </c>
     </row>
@@ -4545,7 +5341,13 @@
       <c r="F135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G135" t="inlineStr">
+      <c r="G135" t="n">
+        <v>0</v>
+      </c>
+      <c r="H135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I135" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4576,9 +5378,15 @@
       <c r="F136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G136" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G136" t="n">
+        <v>0</v>
+      </c>
+      <c r="H136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>2496</t>
         </is>
       </c>
     </row>
@@ -4607,7 +5415,13 @@
       <c r="F137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G137" t="inlineStr">
+      <c r="G137" t="n">
+        <v>0</v>
+      </c>
+      <c r="H137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4638,7 +5452,13 @@
       <c r="F138" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G138" t="inlineStr">
+      <c r="G138" t="n">
+        <v>0</v>
+      </c>
+      <c r="H138" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I138" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4669,9 +5489,15 @@
       <c r="F139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G139" t="inlineStr">
-        <is>
-          <t>2461</t>
+      <c r="G139" t="n">
+        <v>2461</v>
+      </c>
+      <c r="H139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I139" t="inlineStr">
+        <is>
+          <t>2448</t>
         </is>
       </c>
     </row>
@@ -4700,9 +5526,15 @@
       <c r="F140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G140" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G140" t="n">
+        <v>0</v>
+      </c>
+      <c r="H140" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I140" t="inlineStr">
+        <is>
+          <t>2561</t>
         </is>
       </c>
     </row>
@@ -4731,7 +5563,13 @@
       <c r="F141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G141" t="inlineStr">
+      <c r="G141" t="n">
+        <v>0</v>
+      </c>
+      <c r="H141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4762,9 +5600,15 @@
       <c r="F142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G142" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G142" t="n">
+        <v>0</v>
+      </c>
+      <c r="H142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I142" t="inlineStr">
+        <is>
+          <t>2000</t>
         </is>
       </c>
     </row>
@@ -4793,7 +5637,13 @@
       <c r="F143" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G143" t="inlineStr">
+      <c r="G143" t="n">
+        <v>0</v>
+      </c>
+      <c r="H143" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I143" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4824,7 +5674,13 @@
       <c r="F144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G144" t="inlineStr">
+      <c r="G144" t="n">
+        <v>0</v>
+      </c>
+      <c r="H144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I144" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4855,7 +5711,13 @@
       <c r="F145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G145" t="inlineStr">
+      <c r="G145" t="n">
+        <v>0</v>
+      </c>
+      <c r="H145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4886,7 +5748,13 @@
       <c r="F146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G146" t="inlineStr">
+      <c r="G146" t="n">
+        <v>0</v>
+      </c>
+      <c r="H146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4917,7 +5785,13 @@
       <c r="F147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G147" t="inlineStr">
+      <c r="G147" t="n">
+        <v>0</v>
+      </c>
+      <c r="H147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I147" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4948,7 +5822,13 @@
       <c r="F148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G148" t="inlineStr">
+      <c r="G148" t="n">
+        <v>1500</v>
+      </c>
+      <c r="H148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I148" t="inlineStr">
         <is>
           <t>1500</t>
         </is>
@@ -4979,9 +5859,15 @@
       <c r="F149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G149" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="G149" t="n">
+        <v>2500</v>
+      </c>
+      <c r="H149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I149" t="inlineStr">
+        <is>
+          <t>2496</t>
         </is>
       </c>
     </row>
@@ -5010,7 +5896,13 @@
       <c r="F150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G150" t="inlineStr">
+      <c r="G150" t="n">
+        <v>0</v>
+      </c>
+      <c r="H150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5041,7 +5933,13 @@
       <c r="F151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G151" t="inlineStr">
+      <c r="G151" t="n">
+        <v>0</v>
+      </c>
+      <c r="H151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5072,7 +5970,13 @@
       <c r="F152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G152" t="inlineStr">
+      <c r="G152" t="n">
+        <v>0</v>
+      </c>
+      <c r="H152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5103,7 +6007,13 @@
       <c r="F153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G153" t="inlineStr">
+      <c r="G153" t="n">
+        <v>0</v>
+      </c>
+      <c r="H153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5134,7 +6044,13 @@
       <c r="F154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G154" t="inlineStr">
+      <c r="G154" t="n">
+        <v>0</v>
+      </c>
+      <c r="H154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5165,17 +6081,21 @@
       <c r="F155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G155" t="inlineStr">
+      <c r="G155" t="n">
+        <v>0</v>
+      </c>
+      <c r="H155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I155" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
     </row>
     <row r="156">
-      <c r="A156" t="inlineStr">
-        <is>
-          <t>44789201</t>
-        </is>
+      <c r="A156" t="n">
+        <v>44789201</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
@@ -5192,17 +6112,21 @@
       <c r="F156" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="G156" t="inlineStr">
-        <is>
-          <t>2625</t>
+      <c r="G156" t="n">
+        <v>2625</v>
+      </c>
+      <c r="H156" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="I156" t="inlineStr">
+        <is>
+          <t>2695</t>
         </is>
       </c>
     </row>
     <row r="157">
-      <c r="A157" t="inlineStr">
-        <is>
-          <t>56349880</t>
-        </is>
+      <c r="A157" t="n">
+        <v>56349880</v>
       </c>
       <c r="B157" t="inlineStr">
         <is>
@@ -5219,17 +6143,21 @@
       <c r="F157" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G157" t="inlineStr">
-        <is>
-          <t>2006</t>
+      <c r="G157" t="n">
+        <v>2006</v>
+      </c>
+      <c r="H157" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I157" t="inlineStr">
+        <is>
+          <t>2055</t>
         </is>
       </c>
     </row>
     <row r="158">
-      <c r="A158" t="inlineStr">
-        <is>
-          <t>29355299</t>
-        </is>
+      <c r="A158" t="n">
+        <v>29355299</v>
       </c>
       <c r="B158" t="inlineStr">
         <is>
@@ -5246,17 +6174,21 @@
       <c r="F158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G158" t="inlineStr">
+      <c r="G158" t="n">
+        <v>0</v>
+      </c>
+      <c r="H158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
     </row>
     <row r="159">
-      <c r="A159" t="inlineStr">
-        <is>
-          <t>58839983</t>
-        </is>
+      <c r="A159" t="n">
+        <v>58839983</v>
       </c>
       <c r="B159" t="inlineStr">
         <is>
@@ -5273,9 +6205,44 @@
       <c r="F159" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G159" t="inlineStr">
-        <is>
-          <t>1375</t>
+      <c r="G159" t="n">
+        <v>1375</v>
+      </c>
+      <c r="H159" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I159" t="inlineStr">
+        <is>
+          <t>1751</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>57446384</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>总有刁民想睡朕</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr"/>
+      <c r="D160" t="inlineStr"/>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F160" s="3" t="inlineStr"/>
+      <c r="G160" t="inlineStr"/>
+      <c r="H160" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I160" t="inlineStr">
+        <is>
+          <t>1996</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-02-15 11:30:34
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I160"/>
+  <dimension ref="A1:K160"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,6 +436,16 @@
           <t>02-13_0</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>02-14_A</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>02-14_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -468,9 +478,15 @@
       <c r="H2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>2470</t>
+      <c r="I2" t="n">
+        <v>2470</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>2577</t>
         </is>
       </c>
     </row>
@@ -505,9 +521,15 @@
       <c r="H3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>3098</t>
+      <c r="I3" t="n">
+        <v>3098</v>
+      </c>
+      <c r="J3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>3383</t>
         </is>
       </c>
     </row>
@@ -542,9 +564,15 @@
       <c r="H4" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>3428</t>
+      <c r="I4" t="n">
+        <v>3428</v>
+      </c>
+      <c r="J4" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>3742</t>
         </is>
       </c>
     </row>
@@ -579,9 +607,15 @@
       <c r="H5" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>2903</t>
+      <c r="I5" t="n">
+        <v>2903</v>
+      </c>
+      <c r="J5" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>3031</t>
         </is>
       </c>
     </row>
@@ -616,9 +650,15 @@
       <c r="H6" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>3143</t>
+      <c r="I6" t="n">
+        <v>3143</v>
+      </c>
+      <c r="J6" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>3462</t>
         </is>
       </c>
     </row>
@@ -653,9 +693,15 @@
       <c r="H7" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>3564</t>
+      <c r="I7" t="n">
+        <v>3564</v>
+      </c>
+      <c r="J7" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>3876</t>
         </is>
       </c>
     </row>
@@ -690,9 +736,15 @@
       <c r="H8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>3089</t>
+      <c r="I8" t="n">
+        <v>3089</v>
+      </c>
+      <c r="J8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>3382</t>
         </is>
       </c>
     </row>
@@ -727,9 +779,15 @@
       <c r="H9" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>3118</t>
+      <c r="I9" t="n">
+        <v>3118</v>
+      </c>
+      <c r="J9" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>3388</t>
         </is>
       </c>
     </row>
@@ -764,9 +822,15 @@
       <c r="H10" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>3194</t>
+      <c r="I10" t="n">
+        <v>3194</v>
+      </c>
+      <c r="J10" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>3437</t>
         </is>
       </c>
     </row>
@@ -801,9 +865,15 @@
       <c r="H11" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>3052</t>
+      <c r="I11" t="n">
+        <v>3052</v>
+      </c>
+      <c r="J11" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>3294</t>
         </is>
       </c>
     </row>
@@ -838,7 +908,13 @@
       <c r="H12" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="I12" t="n">
+        <v>2677</v>
+      </c>
+      <c r="J12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="inlineStr">
         <is>
           <t>2677</t>
         </is>
@@ -875,9 +951,15 @@
       <c r="H13" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>3497</t>
+      <c r="I13" t="n">
+        <v>3497</v>
+      </c>
+      <c r="J13" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>3856</t>
         </is>
       </c>
     </row>
@@ -912,9 +994,15 @@
       <c r="H14" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>3158</t>
+      <c r="I14" t="n">
+        <v>3158</v>
+      </c>
+      <c r="J14" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>3450</t>
         </is>
       </c>
     </row>
@@ -949,9 +1037,15 @@
       <c r="H15" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>2892</t>
+      <c r="I15" t="n">
+        <v>2892</v>
+      </c>
+      <c r="J15" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>3078</t>
         </is>
       </c>
     </row>
@@ -986,9 +1080,15 @@
       <c r="H16" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>3301</t>
+      <c r="I16" t="n">
+        <v>3301</v>
+      </c>
+      <c r="J16" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>3602</t>
         </is>
       </c>
     </row>
@@ -1023,9 +1123,15 @@
       <c r="H17" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>3045</t>
+      <c r="I17" t="n">
+        <v>3045</v>
+      </c>
+      <c r="J17" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>3213</t>
         </is>
       </c>
     </row>
@@ -1060,9 +1166,15 @@
       <c r="H18" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>2703</t>
+      <c r="I18" t="n">
+        <v>2703</v>
+      </c>
+      <c r="J18" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>2967</t>
         </is>
       </c>
     </row>
@@ -1097,9 +1209,15 @@
       <c r="H19" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>3090</t>
+      <c r="I19" t="n">
+        <v>3090</v>
+      </c>
+      <c r="J19" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>3408</t>
         </is>
       </c>
     </row>
@@ -1134,9 +1252,15 @@
       <c r="H20" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>3515</t>
+      <c r="I20" t="n">
+        <v>3515</v>
+      </c>
+      <c r="J20" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>3977</t>
         </is>
       </c>
     </row>
@@ -1171,7 +1295,13 @@
       <c r="H21" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="I21" t="inlineStr">
+      <c r="I21" t="n">
+        <v>2726</v>
+      </c>
+      <c r="J21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" t="inlineStr">
         <is>
           <t>2726</t>
         </is>
@@ -1208,9 +1338,15 @@
       <c r="H22" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>3189</t>
+      <c r="I22" t="n">
+        <v>3189</v>
+      </c>
+      <c r="J22" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>3543</t>
         </is>
       </c>
     </row>
@@ -1245,9 +1381,15 @@
       <c r="H23" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>2979</t>
+      <c r="I23" t="n">
+        <v>2979</v>
+      </c>
+      <c r="J23" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>3348</t>
         </is>
       </c>
     </row>
@@ -1282,9 +1424,15 @@
       <c r="H24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>3197</t>
+      <c r="I24" t="n">
+        <v>3197</v>
+      </c>
+      <c r="J24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>3530</t>
         </is>
       </c>
     </row>
@@ -1319,7 +1467,13 @@
       <c r="H25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I25" t="inlineStr">
+      <c r="I25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1356,9 +1510,15 @@
       <c r="H26" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>3465</t>
+      <c r="I26" t="n">
+        <v>3465</v>
+      </c>
+      <c r="J26" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>3727</t>
         </is>
       </c>
     </row>
@@ -1393,9 +1553,15 @@
       <c r="H27" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>3212</t>
+      <c r="I27" t="n">
+        <v>3212</v>
+      </c>
+      <c r="J27" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>3545</t>
         </is>
       </c>
     </row>
@@ -1430,9 +1596,15 @@
       <c r="H28" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>2988</t>
+      <c r="I28" t="n">
+        <v>2988</v>
+      </c>
+      <c r="J28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>3148</t>
         </is>
       </c>
     </row>
@@ -1467,9 +1639,15 @@
       <c r="H29" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>3583</t>
+      <c r="I29" t="n">
+        <v>3583</v>
+      </c>
+      <c r="J29" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>3932</t>
         </is>
       </c>
     </row>
@@ -1504,9 +1682,15 @@
       <c r="H30" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>3153</t>
+      <c r="I30" t="n">
+        <v>3153</v>
+      </c>
+      <c r="J30" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>3401</t>
         </is>
       </c>
     </row>
@@ -1541,9 +1725,15 @@
       <c r="H31" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>3458</t>
+      <c r="I31" t="n">
+        <v>3458</v>
+      </c>
+      <c r="J31" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>3693</t>
         </is>
       </c>
     </row>
@@ -1578,9 +1768,15 @@
       <c r="H32" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>3265</t>
+      <c r="I32" t="n">
+        <v>3265</v>
+      </c>
+      <c r="J32" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>3496</t>
         </is>
       </c>
     </row>
@@ -1615,9 +1811,15 @@
       <c r="H33" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>3195</t>
+      <c r="I33" t="n">
+        <v>3195</v>
+      </c>
+      <c r="J33" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>3437</t>
         </is>
       </c>
     </row>
@@ -1652,9 +1854,15 @@
       <c r="H34" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>3210</t>
+      <c r="I34" t="n">
+        <v>3210</v>
+      </c>
+      <c r="J34" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>3452</t>
         </is>
       </c>
     </row>
@@ -1689,9 +1897,15 @@
       <c r="H35" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>3275</t>
+      <c r="I35" t="n">
+        <v>3275</v>
+      </c>
+      <c r="J35" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>3497</t>
         </is>
       </c>
     </row>
@@ -1726,9 +1940,15 @@
       <c r="H36" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>3061</t>
+      <c r="I36" t="n">
+        <v>3061</v>
+      </c>
+      <c r="J36" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>3410</t>
         </is>
       </c>
     </row>
@@ -1763,9 +1983,15 @@
       <c r="H37" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>3211</t>
+      <c r="I37" t="n">
+        <v>3211</v>
+      </c>
+      <c r="J37" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>3342</t>
         </is>
       </c>
     </row>
@@ -1800,9 +2026,15 @@
       <c r="H38" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>3220</t>
+      <c r="I38" t="n">
+        <v>3220</v>
+      </c>
+      <c r="J38" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>3585</t>
         </is>
       </c>
     </row>
@@ -1837,9 +2069,15 @@
       <c r="H39" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>3284</t>
+      <c r="I39" t="n">
+        <v>3284</v>
+      </c>
+      <c r="J39" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>3589</t>
         </is>
       </c>
     </row>
@@ -1874,9 +2112,15 @@
       <c r="H40" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>3389</t>
+      <c r="I40" t="n">
+        <v>3389</v>
+      </c>
+      <c r="J40" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>3612</t>
         </is>
       </c>
     </row>
@@ -1911,9 +2155,15 @@
       <c r="H41" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>3154</t>
+      <c r="I41" t="n">
+        <v>3154</v>
+      </c>
+      <c r="J41" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>3460</t>
         </is>
       </c>
     </row>
@@ -1948,9 +2198,15 @@
       <c r="H42" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>3429</t>
+      <c r="I42" t="n">
+        <v>3429</v>
+      </c>
+      <c r="J42" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>3796</t>
         </is>
       </c>
     </row>
@@ -1985,9 +2241,15 @@
       <c r="H43" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>3210</t>
+      <c r="I43" t="n">
+        <v>3210</v>
+      </c>
+      <c r="J43" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>3555</t>
         </is>
       </c>
     </row>
@@ -2022,9 +2284,15 @@
       <c r="H44" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>3329</t>
+      <c r="I44" t="n">
+        <v>3329</v>
+      </c>
+      <c r="J44" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>3590</t>
         </is>
       </c>
     </row>
@@ -2059,9 +2327,15 @@
       <c r="H45" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>3193</t>
+      <c r="I45" t="n">
+        <v>3193</v>
+      </c>
+      <c r="J45" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>3407</t>
         </is>
       </c>
     </row>
@@ -2096,9 +2370,15 @@
       <c r="H46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>3207</t>
+      <c r="I46" t="n">
+        <v>3207</v>
+      </c>
+      <c r="J46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>3498</t>
         </is>
       </c>
     </row>
@@ -2133,7 +2413,13 @@
       <c r="H47" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I47" t="inlineStr">
+      <c r="I47" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2170,9 +2456,15 @@
       <c r="H48" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>3359</t>
+      <c r="I48" t="n">
+        <v>3359</v>
+      </c>
+      <c r="J48" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>3698</t>
         </is>
       </c>
     </row>
@@ -2207,9 +2499,15 @@
       <c r="H49" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>2949</t>
+      <c r="I49" t="n">
+        <v>2949</v>
+      </c>
+      <c r="J49" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>3117</t>
         </is>
       </c>
     </row>
@@ -2244,9 +2542,15 @@
       <c r="H50" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>3400</t>
+      <c r="I50" t="n">
+        <v>3400</v>
+      </c>
+      <c r="J50" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>3791</t>
         </is>
       </c>
     </row>
@@ -2281,9 +2585,15 @@
       <c r="H51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t>2522</t>
+      <c r="I51" t="n">
+        <v>2522</v>
+      </c>
+      <c r="J51" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>2782</t>
         </is>
       </c>
     </row>
@@ -2318,9 +2628,15 @@
       <c r="H52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I52" t="n">
+        <v>0</v>
+      </c>
+      <c r="J52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -2355,9 +2671,15 @@
       <c r="H53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I53" t="inlineStr">
-        <is>
-          <t>2486</t>
+      <c r="I53" t="n">
+        <v>2486</v>
+      </c>
+      <c r="J53" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>2555</t>
         </is>
       </c>
     </row>
@@ -2392,9 +2714,15 @@
       <c r="H54" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t>3422</t>
+      <c r="I54" t="n">
+        <v>3422</v>
+      </c>
+      <c r="J54" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>3607</t>
         </is>
       </c>
     </row>
@@ -2429,9 +2757,15 @@
       <c r="H55" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t>2870</t>
+      <c r="I55" t="n">
+        <v>2870</v>
+      </c>
+      <c r="J55" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>3073</t>
         </is>
       </c>
     </row>
@@ -2466,9 +2800,15 @@
       <c r="H56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>2918</t>
+      <c r="I56" t="n">
+        <v>2918</v>
+      </c>
+      <c r="J56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>3094</t>
         </is>
       </c>
     </row>
@@ -2503,9 +2843,15 @@
       <c r="H57" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>3163</t>
+      <c r="I57" t="n">
+        <v>3163</v>
+      </c>
+      <c r="J57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>3436</t>
         </is>
       </c>
     </row>
@@ -2540,9 +2886,15 @@
       <c r="H58" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>2836</t>
+      <c r="I58" t="n">
+        <v>2836</v>
+      </c>
+      <c r="J58" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>3002</t>
         </is>
       </c>
     </row>
@@ -2568,6 +2920,8 @@
       <c r="G59" t="inlineStr"/>
       <c r="H59" s="3" t="inlineStr"/>
       <c r="I59" t="inlineStr"/>
+      <c r="J59" s="3" t="inlineStr"/>
+      <c r="K59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -2591,6 +2945,8 @@
       <c r="G60" t="inlineStr"/>
       <c r="H60" s="3" t="inlineStr"/>
       <c r="I60" t="inlineStr"/>
+      <c r="J60" s="3" t="inlineStr"/>
+      <c r="K60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -2623,9 +2979,15 @@
       <c r="H61" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I61" t="inlineStr">
-        <is>
-          <t>3096</t>
+      <c r="I61" t="n">
+        <v>3096</v>
+      </c>
+      <c r="J61" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>3303</t>
         </is>
       </c>
     </row>
@@ -2660,7 +3022,13 @@
       <c r="H62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I62" t="inlineStr">
+      <c r="I62" t="n">
+        <v>0</v>
+      </c>
+      <c r="J62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2697,9 +3065,15 @@
       <c r="H63" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>3204</t>
+      <c r="I63" t="n">
+        <v>3204</v>
+      </c>
+      <c r="J63" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>3487</t>
         </is>
       </c>
     </row>
@@ -2734,7 +3108,13 @@
       <c r="H64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I64" t="inlineStr">
+      <c r="I64" t="n">
+        <v>2490</v>
+      </c>
+      <c r="J64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K64" t="inlineStr">
         <is>
           <t>2490</t>
         </is>
@@ -2762,6 +3142,8 @@
       <c r="G65" t="inlineStr"/>
       <c r="H65" s="3" t="inlineStr"/>
       <c r="I65" t="inlineStr"/>
+      <c r="J65" s="3" t="inlineStr"/>
+      <c r="K65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -2794,9 +3176,15 @@
       <c r="H66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I66" t="inlineStr">
-        <is>
-          <t>2460</t>
+      <c r="I66" t="n">
+        <v>2460</v>
+      </c>
+      <c r="J66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>2459</t>
         </is>
       </c>
     </row>
@@ -2831,9 +3219,15 @@
       <c r="H67" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I67" t="inlineStr">
-        <is>
-          <t>2974</t>
+      <c r="I67" t="n">
+        <v>2974</v>
+      </c>
+      <c r="J67" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>3290</t>
         </is>
       </c>
     </row>
@@ -2868,9 +3262,15 @@
       <c r="H68" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I68" t="inlineStr">
-        <is>
-          <t>3272</t>
+      <c r="I68" t="n">
+        <v>3272</v>
+      </c>
+      <c r="J68" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>3639</t>
         </is>
       </c>
     </row>
@@ -2905,9 +3305,15 @@
       <c r="H69" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="I69" t="inlineStr">
-        <is>
-          <t>2894</t>
+      <c r="I69" t="n">
+        <v>2894</v>
+      </c>
+      <c r="J69" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>3197</t>
         </is>
       </c>
     </row>
@@ -2942,9 +3348,15 @@
       <c r="H70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I70" t="inlineStr">
-        <is>
-          <t>2521</t>
+      <c r="I70" t="n">
+        <v>2521</v>
+      </c>
+      <c r="J70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>2567</t>
         </is>
       </c>
     </row>
@@ -2979,9 +3391,15 @@
       <c r="H71" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I71" t="inlineStr">
-        <is>
-          <t>2893</t>
+      <c r="I71" t="n">
+        <v>2893</v>
+      </c>
+      <c r="J71" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>3115</t>
         </is>
       </c>
     </row>
@@ -3016,9 +3434,15 @@
       <c r="H72" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="I72" t="inlineStr">
-        <is>
-          <t>2788</t>
+      <c r="I72" t="n">
+        <v>2788</v>
+      </c>
+      <c r="J72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>2790</t>
         </is>
       </c>
     </row>
@@ -3053,9 +3477,15 @@
       <c r="H73" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I73" t="inlineStr">
-        <is>
-          <t>2928</t>
+      <c r="I73" t="n">
+        <v>2928</v>
+      </c>
+      <c r="J73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>3097</t>
         </is>
       </c>
     </row>
@@ -3090,9 +3520,15 @@
       <c r="H74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I74" t="inlineStr">
-        <is>
-          <t>2526</t>
+      <c r="I74" t="n">
+        <v>2526</v>
+      </c>
+      <c r="J74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>2563</t>
         </is>
       </c>
     </row>
@@ -3127,9 +3563,15 @@
       <c r="H75" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I75" t="inlineStr">
-        <is>
-          <t>2920</t>
+      <c r="I75" t="n">
+        <v>2920</v>
+      </c>
+      <c r="J75" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>3071</t>
         </is>
       </c>
     </row>
@@ -3164,9 +3606,15 @@
       <c r="H76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I76" t="inlineStr">
-        <is>
-          <t>2808</t>
+      <c r="I76" t="n">
+        <v>2808</v>
+      </c>
+      <c r="J76" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>3209</t>
         </is>
       </c>
     </row>
@@ -3201,9 +3649,15 @@
       <c r="H77" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I77" t="inlineStr">
-        <is>
-          <t>3120</t>
+      <c r="I77" t="n">
+        <v>3120</v>
+      </c>
+      <c r="J77" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>3321</t>
         </is>
       </c>
     </row>
@@ -3238,9 +3692,15 @@
       <c r="H78" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I78" t="inlineStr">
-        <is>
-          <t>3254</t>
+      <c r="I78" t="n">
+        <v>3254</v>
+      </c>
+      <c r="J78" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>3449</t>
         </is>
       </c>
     </row>
@@ -3275,7 +3735,13 @@
       <c r="H79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I79" t="inlineStr">
+      <c r="I79" t="n">
+        <v>0</v>
+      </c>
+      <c r="J79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3312,9 +3778,15 @@
       <c r="H80" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="I80" t="inlineStr">
-        <is>
-          <t>3015</t>
+      <c r="I80" t="n">
+        <v>3015</v>
+      </c>
+      <c r="J80" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>3310</t>
         </is>
       </c>
     </row>
@@ -3349,9 +3821,15 @@
       <c r="H81" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="I81" t="inlineStr">
-        <is>
-          <t>3139</t>
+      <c r="I81" t="n">
+        <v>3139</v>
+      </c>
+      <c r="J81" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>3310</t>
         </is>
       </c>
     </row>
@@ -3386,9 +3864,15 @@
       <c r="H82" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I82" t="inlineStr">
-        <is>
-          <t>3110</t>
+      <c r="I82" t="n">
+        <v>3110</v>
+      </c>
+      <c r="J82" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>3121</t>
         </is>
       </c>
     </row>
@@ -3423,9 +3907,15 @@
       <c r="H83" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I83" t="inlineStr">
-        <is>
-          <t>2973</t>
+      <c r="I83" t="n">
+        <v>2973</v>
+      </c>
+      <c r="J83" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>3148</t>
         </is>
       </c>
     </row>
@@ -3460,9 +3950,15 @@
       <c r="H84" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="I84" t="inlineStr">
-        <is>
-          <t>2644</t>
+      <c r="I84" t="n">
+        <v>2644</v>
+      </c>
+      <c r="J84" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>2812</t>
         </is>
       </c>
     </row>
@@ -3497,9 +3993,15 @@
       <c r="H85" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I85" t="inlineStr">
-        <is>
-          <t>2808</t>
+      <c r="I85" t="n">
+        <v>2808</v>
+      </c>
+      <c r="J85" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>2982</t>
         </is>
       </c>
     </row>
@@ -3534,9 +4036,15 @@
       <c r="H86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I86" t="inlineStr">
-        <is>
-          <t>2489</t>
+      <c r="I86" t="n">
+        <v>2489</v>
+      </c>
+      <c r="J86" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>2724</t>
         </is>
       </c>
     </row>
@@ -3571,9 +4079,15 @@
       <c r="H87" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I87" t="inlineStr">
-        <is>
-          <t>3133</t>
+      <c r="I87" t="n">
+        <v>3133</v>
+      </c>
+      <c r="J87" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>3513</t>
         </is>
       </c>
     </row>
@@ -3608,9 +4122,15 @@
       <c r="H88" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I88" t="inlineStr">
-        <is>
-          <t>2582</t>
+      <c r="I88" t="n">
+        <v>2582</v>
+      </c>
+      <c r="J88" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>2696</t>
         </is>
       </c>
     </row>
@@ -3645,9 +4165,15 @@
       <c r="H89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I89" t="inlineStr">
-        <is>
-          <t>2554</t>
+      <c r="I89" t="n">
+        <v>2554</v>
+      </c>
+      <c r="J89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>2538</t>
         </is>
       </c>
     </row>
@@ -3682,9 +4208,15 @@
       <c r="H90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I90" t="inlineStr">
-        <is>
-          <t>2460</t>
+      <c r="I90" t="n">
+        <v>2460</v>
+      </c>
+      <c r="J90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>2448</t>
         </is>
       </c>
     </row>
@@ -3719,9 +4251,15 @@
       <c r="H91" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I91" t="inlineStr">
-        <is>
-          <t>2595</t>
+      <c r="I91" t="n">
+        <v>2595</v>
+      </c>
+      <c r="J91" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>2636</t>
         </is>
       </c>
     </row>
@@ -3756,7 +4294,13 @@
       <c r="H92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I92" t="inlineStr">
+      <c r="I92" t="n">
+        <v>0</v>
+      </c>
+      <c r="J92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3793,9 +4337,15 @@
       <c r="H93" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="I93" t="inlineStr">
-        <is>
-          <t>2431</t>
+      <c r="I93" t="n">
+        <v>2431</v>
+      </c>
+      <c r="J93" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>2511</t>
         </is>
       </c>
     </row>
@@ -3830,9 +4380,15 @@
       <c r="H94" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I94" t="inlineStr">
-        <is>
-          <t>2579</t>
+      <c r="I94" t="n">
+        <v>2579</v>
+      </c>
+      <c r="J94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>2544</t>
         </is>
       </c>
     </row>
@@ -3867,9 +4423,15 @@
       <c r="H95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I95" t="inlineStr">
-        <is>
-          <t>2493</t>
+      <c r="I95" t="n">
+        <v>2493</v>
+      </c>
+      <c r="J95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>2445</t>
         </is>
       </c>
     </row>
@@ -3904,9 +4466,15 @@
       <c r="H96" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="I96" t="inlineStr">
-        <is>
-          <t>2759</t>
+      <c r="I96" t="n">
+        <v>2759</v>
+      </c>
+      <c r="J96" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>2849</t>
         </is>
       </c>
     </row>
@@ -3941,9 +4509,15 @@
       <c r="H97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I97" t="inlineStr">
-        <is>
-          <t>2478</t>
+      <c r="I97" t="n">
+        <v>2478</v>
+      </c>
+      <c r="J97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>2499</t>
         </is>
       </c>
     </row>
@@ -3978,7 +4552,13 @@
       <c r="H98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I98" t="inlineStr">
+      <c r="I98" t="n">
+        <v>0</v>
+      </c>
+      <c r="J98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4015,9 +4595,15 @@
       <c r="H99" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I99" t="inlineStr">
-        <is>
-          <t>2730</t>
+      <c r="I99" t="n">
+        <v>2730</v>
+      </c>
+      <c r="J99" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>2832</t>
         </is>
       </c>
     </row>
@@ -4052,9 +4638,15 @@
       <c r="H100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I100" t="inlineStr">
-        <is>
-          <t>2416</t>
+      <c r="I100" t="n">
+        <v>2416</v>
+      </c>
+      <c r="J100" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>2436</t>
         </is>
       </c>
     </row>
@@ -4089,9 +4681,15 @@
       <c r="H101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I101" t="inlineStr">
-        <is>
-          <t>3075</t>
+      <c r="I101" t="n">
+        <v>3075</v>
+      </c>
+      <c r="J101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>3214</t>
         </is>
       </c>
     </row>
@@ -4126,9 +4724,15 @@
       <c r="H102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I102" t="inlineStr">
-        <is>
-          <t>2854</t>
+      <c r="I102" t="n">
+        <v>2854</v>
+      </c>
+      <c r="J102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>3042</t>
         </is>
       </c>
     </row>
@@ -4163,9 +4767,15 @@
       <c r="H103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I103" t="inlineStr">
-        <is>
-          <t>2521</t>
+      <c r="I103" t="n">
+        <v>2521</v>
+      </c>
+      <c r="J103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>2532</t>
         </is>
       </c>
     </row>
@@ -4200,9 +4810,15 @@
       <c r="H104" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="I104" t="inlineStr">
-        <is>
-          <t>2986</t>
+      <c r="I104" t="n">
+        <v>2986</v>
+      </c>
+      <c r="J104" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>3259</t>
         </is>
       </c>
     </row>
@@ -4237,9 +4853,15 @@
       <c r="H105" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I105" t="inlineStr">
-        <is>
-          <t>2875</t>
+      <c r="I105" t="n">
+        <v>2875</v>
+      </c>
+      <c r="J105" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>3118</t>
         </is>
       </c>
     </row>
@@ -4274,7 +4896,13 @@
       <c r="H106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I106" t="inlineStr">
+      <c r="I106" t="n">
+        <v>0</v>
+      </c>
+      <c r="J106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4311,9 +4939,15 @@
       <c r="H107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I107" t="inlineStr">
-        <is>
-          <t>2544</t>
+      <c r="I107" t="n">
+        <v>2544</v>
+      </c>
+      <c r="J107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>2510</t>
         </is>
       </c>
     </row>
@@ -4348,7 +4982,13 @@
       <c r="H108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I108" t="inlineStr">
+      <c r="I108" t="n">
+        <v>0</v>
+      </c>
+      <c r="J108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4385,9 +5025,15 @@
       <c r="H109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I109" t="inlineStr">
-        <is>
-          <t>2666</t>
+      <c r="I109" t="n">
+        <v>2666</v>
+      </c>
+      <c r="J109" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>2841</t>
         </is>
       </c>
     </row>
@@ -4422,9 +5068,15 @@
       <c r="H110" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I110" t="inlineStr">
-        <is>
-          <t>2743</t>
+      <c r="I110" t="n">
+        <v>2743</v>
+      </c>
+      <c r="J110" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>2891</t>
         </is>
       </c>
     </row>
@@ -4459,9 +5111,15 @@
       <c r="H111" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="I111" t="inlineStr">
-        <is>
-          <t>2559</t>
+      <c r="I111" t="n">
+        <v>2559</v>
+      </c>
+      <c r="J111" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>2636</t>
         </is>
       </c>
     </row>
@@ -4496,9 +5154,15 @@
       <c r="H112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I112" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="I112" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>2608</t>
         </is>
       </c>
     </row>
@@ -4533,9 +5197,15 @@
       <c r="H113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I113" t="inlineStr">
-        <is>
-          <t>2571</t>
+      <c r="I113" t="n">
+        <v>2571</v>
+      </c>
+      <c r="J113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>2689</t>
         </is>
       </c>
     </row>
@@ -4570,7 +5240,13 @@
       <c r="H114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I114" t="inlineStr">
+      <c r="I114" t="n">
+        <v>0</v>
+      </c>
+      <c r="J114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K114" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4607,9 +5283,15 @@
       <c r="H115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I115" t="inlineStr">
-        <is>
-          <t>2488</t>
+      <c r="I115" t="n">
+        <v>2488</v>
+      </c>
+      <c r="J115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>2466</t>
         </is>
       </c>
     </row>
@@ -4644,9 +5326,15 @@
       <c r="H116" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="I116" t="inlineStr">
-        <is>
-          <t>2579</t>
+      <c r="I116" t="n">
+        <v>2579</v>
+      </c>
+      <c r="J116" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>2622</t>
         </is>
       </c>
     </row>
@@ -4681,9 +5369,15 @@
       <c r="H117" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I117" t="inlineStr">
-        <is>
-          <t>3029</t>
+      <c r="I117" t="n">
+        <v>3029</v>
+      </c>
+      <c r="J117" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>2938</t>
         </is>
       </c>
     </row>
@@ -4718,7 +5412,13 @@
       <c r="H118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I118" t="inlineStr">
+      <c r="I118" t="n">
+        <v>0</v>
+      </c>
+      <c r="J118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4755,9 +5455,15 @@
       <c r="H119" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I119" t="inlineStr">
-        <is>
-          <t>2762</t>
+      <c r="I119" t="n">
+        <v>2762</v>
+      </c>
+      <c r="J119" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K119" t="inlineStr">
+        <is>
+          <t>3001</t>
         </is>
       </c>
     </row>
@@ -4792,9 +5498,15 @@
       <c r="H120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I120" t="inlineStr">
-        <is>
-          <t>2417</t>
+      <c r="I120" t="n">
+        <v>2417</v>
+      </c>
+      <c r="J120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K120" t="inlineStr">
+        <is>
+          <t>2381</t>
         </is>
       </c>
     </row>
@@ -4829,9 +5541,15 @@
       <c r="H121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I121" t="inlineStr">
-        <is>
-          <t>2578</t>
+      <c r="I121" t="n">
+        <v>2578</v>
+      </c>
+      <c r="J121" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>2715</t>
         </is>
       </c>
     </row>
@@ -4866,7 +5584,13 @@
       <c r="H122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I122" t="inlineStr">
+      <c r="I122" t="n">
+        <v>0</v>
+      </c>
+      <c r="J122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4903,9 +5627,15 @@
       <c r="H123" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="I123" t="inlineStr">
-        <is>
-          <t>2711</t>
+      <c r="I123" t="n">
+        <v>2711</v>
+      </c>
+      <c r="J123" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>2725</t>
         </is>
       </c>
     </row>
@@ -4940,9 +5670,15 @@
       <c r="H124" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="I124" t="inlineStr">
-        <is>
-          <t>2613</t>
+      <c r="I124" t="n">
+        <v>2613</v>
+      </c>
+      <c r="J124" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>2762</t>
         </is>
       </c>
     </row>
@@ -4977,9 +5713,15 @@
       <c r="H125" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I125" t="inlineStr">
-        <is>
-          <t>2716</t>
+      <c r="I125" t="n">
+        <v>2716</v>
+      </c>
+      <c r="J125" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K125" t="inlineStr">
+        <is>
+          <t>2855</t>
         </is>
       </c>
     </row>
@@ -5014,9 +5756,15 @@
       <c r="H126" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I126" t="inlineStr">
-        <is>
-          <t>2715</t>
+      <c r="I126" t="n">
+        <v>2715</v>
+      </c>
+      <c r="J126" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K126" t="inlineStr">
+        <is>
+          <t>2816</t>
         </is>
       </c>
     </row>
@@ -5051,9 +5799,15 @@
       <c r="H127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I127" t="inlineStr">
-        <is>
-          <t>2450</t>
+      <c r="I127" t="n">
+        <v>2450</v>
+      </c>
+      <c r="J127" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="K127" t="inlineStr">
+        <is>
+          <t>2476</t>
         </is>
       </c>
     </row>
@@ -5088,7 +5842,13 @@
       <c r="H128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I128" t="inlineStr">
+      <c r="I128" t="n">
+        <v>0</v>
+      </c>
+      <c r="J128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5125,7 +5885,13 @@
       <c r="H129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I129" t="inlineStr">
+      <c r="I129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5162,9 +5928,15 @@
       <c r="H130" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I130" t="inlineStr">
-        <is>
-          <t>2528</t>
+      <c r="I130" t="n">
+        <v>2528</v>
+      </c>
+      <c r="J130" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K130" t="inlineStr">
+        <is>
+          <t>2509</t>
         </is>
       </c>
     </row>
@@ -5199,9 +5971,15 @@
       <c r="H131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I131" t="inlineStr">
-        <is>
-          <t>2437</t>
+      <c r="I131" t="n">
+        <v>2437</v>
+      </c>
+      <c r="J131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K131" t="inlineStr">
+        <is>
+          <t>2407</t>
         </is>
       </c>
     </row>
@@ -5236,9 +6014,15 @@
       <c r="H132" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I132" t="inlineStr">
-        <is>
-          <t>2414</t>
+      <c r="I132" t="n">
+        <v>2414</v>
+      </c>
+      <c r="J132" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K132" t="inlineStr">
+        <is>
+          <t>2430</t>
         </is>
       </c>
     </row>
@@ -5273,9 +6057,15 @@
       <c r="H133" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I133" t="inlineStr">
-        <is>
-          <t>2689</t>
+      <c r="I133" t="n">
+        <v>2689</v>
+      </c>
+      <c r="J133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K133" t="inlineStr">
+        <is>
+          <t>2669</t>
         </is>
       </c>
     </row>
@@ -5310,9 +6100,15 @@
       <c r="H134" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I134" t="inlineStr">
-        <is>
-          <t>1503</t>
+      <c r="I134" t="n">
+        <v>1503</v>
+      </c>
+      <c r="J134" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="K134" t="inlineStr">
+        <is>
+          <t>1560</t>
         </is>
       </c>
     </row>
@@ -5347,7 +6143,13 @@
       <c r="H135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I135" t="inlineStr">
+      <c r="I135" t="n">
+        <v>0</v>
+      </c>
+      <c r="J135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K135" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5384,9 +6186,15 @@
       <c r="H136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I136" t="inlineStr">
-        <is>
-          <t>2496</t>
+      <c r="I136" t="n">
+        <v>2496</v>
+      </c>
+      <c r="J136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>2543</t>
         </is>
       </c>
     </row>
@@ -5421,7 +6229,13 @@
       <c r="H137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I137" t="inlineStr">
+      <c r="I137" t="n">
+        <v>0</v>
+      </c>
+      <c r="J137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5458,7 +6272,13 @@
       <c r="H138" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I138" t="inlineStr">
+      <c r="I138" t="n">
+        <v>0</v>
+      </c>
+      <c r="J138" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K138" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5495,9 +6315,15 @@
       <c r="H139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I139" t="inlineStr">
-        <is>
-          <t>2448</t>
+      <c r="I139" t="n">
+        <v>2448</v>
+      </c>
+      <c r="J139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K139" t="inlineStr">
+        <is>
+          <t>2413</t>
         </is>
       </c>
     </row>
@@ -5532,9 +6358,15 @@
       <c r="H140" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I140" t="inlineStr">
-        <is>
-          <t>2561</t>
+      <c r="I140" t="n">
+        <v>2561</v>
+      </c>
+      <c r="J140" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="K140" t="inlineStr">
+        <is>
+          <t>2639</t>
         </is>
       </c>
     </row>
@@ -5569,7 +6401,13 @@
       <c r="H141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I141" t="inlineStr">
+      <c r="I141" t="n">
+        <v>0</v>
+      </c>
+      <c r="J141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5606,7 +6444,13 @@
       <c r="H142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I142" t="inlineStr">
+      <c r="I142" t="n">
+        <v>2000</v>
+      </c>
+      <c r="J142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K142" t="inlineStr">
         <is>
           <t>2000</t>
         </is>
@@ -5643,7 +6487,13 @@
       <c r="H143" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I143" t="inlineStr">
+      <c r="I143" t="n">
+        <v>0</v>
+      </c>
+      <c r="J143" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K143" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5680,7 +6530,13 @@
       <c r="H144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I144" t="inlineStr">
+      <c r="I144" t="n">
+        <v>0</v>
+      </c>
+      <c r="J144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K144" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5717,7 +6573,13 @@
       <c r="H145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I145" t="inlineStr">
+      <c r="I145" t="n">
+        <v>0</v>
+      </c>
+      <c r="J145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5754,7 +6616,13 @@
       <c r="H146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I146" t="inlineStr">
+      <c r="I146" t="n">
+        <v>0</v>
+      </c>
+      <c r="J146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5791,7 +6659,13 @@
       <c r="H147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I147" t="inlineStr">
+      <c r="I147" t="n">
+        <v>0</v>
+      </c>
+      <c r="J147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K147" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5828,7 +6702,13 @@
       <c r="H148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I148" t="inlineStr">
+      <c r="I148" t="n">
+        <v>1500</v>
+      </c>
+      <c r="J148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K148" t="inlineStr">
         <is>
           <t>1500</t>
         </is>
@@ -5865,7 +6745,13 @@
       <c r="H149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I149" t="inlineStr">
+      <c r="I149" t="n">
+        <v>2496</v>
+      </c>
+      <c r="J149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K149" t="inlineStr">
         <is>
           <t>2496</t>
         </is>
@@ -5902,7 +6788,13 @@
       <c r="H150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I150" t="inlineStr">
+      <c r="I150" t="n">
+        <v>0</v>
+      </c>
+      <c r="J150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5939,7 +6831,13 @@
       <c r="H151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I151" t="inlineStr">
+      <c r="I151" t="n">
+        <v>0</v>
+      </c>
+      <c r="J151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5976,7 +6874,13 @@
       <c r="H152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I152" t="inlineStr">
+      <c r="I152" t="n">
+        <v>0</v>
+      </c>
+      <c r="J152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6013,7 +6917,13 @@
       <c r="H153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I153" t="inlineStr">
+      <c r="I153" t="n">
+        <v>0</v>
+      </c>
+      <c r="J153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6050,7 +6960,13 @@
       <c r="H154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I154" t="inlineStr">
+      <c r="I154" t="n">
+        <v>0</v>
+      </c>
+      <c r="J154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6087,7 +7003,13 @@
       <c r="H155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I155" t="inlineStr">
+      <c r="I155" t="n">
+        <v>0</v>
+      </c>
+      <c r="J155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K155" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6118,9 +7040,15 @@
       <c r="H156" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="I156" t="inlineStr">
-        <is>
-          <t>2695</t>
+      <c r="I156" t="n">
+        <v>2695</v>
+      </c>
+      <c r="J156" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="K156" t="inlineStr">
+        <is>
+          <t>2809</t>
         </is>
       </c>
     </row>
@@ -6149,9 +7077,15 @@
       <c r="H157" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I157" t="inlineStr">
-        <is>
-          <t>2055</t>
+      <c r="I157" t="n">
+        <v>2055</v>
+      </c>
+      <c r="J157" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="K157" t="inlineStr">
+        <is>
+          <t>2129</t>
         </is>
       </c>
     </row>
@@ -6180,7 +7114,13 @@
       <c r="H158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I158" t="inlineStr">
+      <c r="I158" t="n">
+        <v>0</v>
+      </c>
+      <c r="J158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6192,14 +7132,14 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Player-58839983</t>
+          <t>青龙偃月灯</t>
         </is>
       </c>
       <c r="C159" t="inlineStr"/>
       <c r="D159" t="inlineStr"/>
       <c r="E159" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F159" s="3" t="n">
@@ -6211,17 +7151,21 @@
       <c r="H159" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I159" t="inlineStr">
-        <is>
-          <t>1751</t>
+      <c r="I159" t="n">
+        <v>1751</v>
+      </c>
+      <c r="J159" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="K159" t="inlineStr">
+        <is>
+          <t>2157</t>
         </is>
       </c>
     </row>
     <row r="160">
-      <c r="A160" t="inlineStr">
-        <is>
-          <t>57446384</t>
-        </is>
+      <c r="A160" t="n">
+        <v>57446384</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
@@ -6240,7 +7184,13 @@
       <c r="H160" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I160" t="inlineStr">
+      <c r="I160" t="n">
+        <v>1996</v>
+      </c>
+      <c r="J160" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K160" t="inlineStr">
         <is>
           <t>1996</t>
         </is>

</xml_diff>

<commit_message>
Code updated 23-02-16 11:30:35
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K160"/>
+  <dimension ref="A1:M162"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,6 +446,16 @@
           <t>02-14_0</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>02-15_A</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>02-15_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -484,9 +494,15 @@
       <c r="J2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>2577</t>
+      <c r="K2" t="n">
+        <v>2577</v>
+      </c>
+      <c r="L2" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>2901</t>
         </is>
       </c>
     </row>
@@ -527,9 +543,15 @@
       <c r="J3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>3383</t>
+      <c r="K3" t="n">
+        <v>3383</v>
+      </c>
+      <c r="L3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>3570</t>
         </is>
       </c>
     </row>
@@ -570,9 +592,15 @@
       <c r="J4" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>3742</t>
+      <c r="K4" t="n">
+        <v>3742</v>
+      </c>
+      <c r="L4" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>4020</t>
         </is>
       </c>
     </row>
@@ -613,9 +641,15 @@
       <c r="J5" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>3031</t>
+      <c r="K5" t="n">
+        <v>3031</v>
+      </c>
+      <c r="L5" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>3275</t>
         </is>
       </c>
     </row>
@@ -656,9 +690,15 @@
       <c r="J6" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>3462</t>
+      <c r="K6" t="n">
+        <v>3462</v>
+      </c>
+      <c r="L6" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>3781</t>
         </is>
       </c>
     </row>
@@ -681,7 +721,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F7" s="4" t="n">
@@ -699,9 +739,15 @@
       <c r="J7" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>3876</t>
+      <c r="K7" t="n">
+        <v>3876</v>
+      </c>
+      <c r="L7" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>4201</t>
         </is>
       </c>
     </row>
@@ -742,9 +788,15 @@
       <c r="J8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>3382</t>
+      <c r="K8" t="n">
+        <v>3382</v>
+      </c>
+      <c r="L8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>3607</t>
         </is>
       </c>
     </row>
@@ -785,9 +837,15 @@
       <c r="J9" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>3388</t>
+      <c r="K9" t="n">
+        <v>3388</v>
+      </c>
+      <c r="L9" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>3661</t>
         </is>
       </c>
     </row>
@@ -828,9 +886,15 @@
       <c r="J10" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>3437</t>
+      <c r="K10" t="n">
+        <v>3437</v>
+      </c>
+      <c r="L10" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>3622</t>
         </is>
       </c>
     </row>
@@ -871,9 +935,15 @@
       <c r="J11" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>3294</t>
+      <c r="K11" t="n">
+        <v>3294</v>
+      </c>
+      <c r="L11" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>3473</t>
         </is>
       </c>
     </row>
@@ -914,7 +984,13 @@
       <c r="J12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="K12" t="n">
+        <v>2677</v>
+      </c>
+      <c r="L12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="inlineStr">
         <is>
           <t>2677</t>
         </is>
@@ -939,7 +1015,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F13" s="4" t="n">
@@ -957,9 +1033,15 @@
       <c r="J13" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>3856</t>
+      <c r="K13" t="n">
+        <v>3856</v>
+      </c>
+      <c r="L13" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>4241</t>
         </is>
       </c>
     </row>
@@ -1000,9 +1082,15 @@
       <c r="J14" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>3450</t>
+      <c r="K14" t="n">
+        <v>3450</v>
+      </c>
+      <c r="L14" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>3767</t>
         </is>
       </c>
     </row>
@@ -1043,9 +1131,15 @@
       <c r="J15" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>3078</t>
+      <c r="K15" t="n">
+        <v>3078</v>
+      </c>
+      <c r="L15" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>3319</t>
         </is>
       </c>
     </row>
@@ -1086,9 +1180,15 @@
       <c r="J16" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>3602</t>
+      <c r="K16" t="n">
+        <v>3602</v>
+      </c>
+      <c r="L16" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>3826</t>
         </is>
       </c>
     </row>
@@ -1129,9 +1229,15 @@
       <c r="J17" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>3213</t>
+      <c r="K17" t="n">
+        <v>3213</v>
+      </c>
+      <c r="L17" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>3399</t>
         </is>
       </c>
     </row>
@@ -1172,9 +1278,15 @@
       <c r="J18" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>2967</t>
+      <c r="K18" t="n">
+        <v>2967</v>
+      </c>
+      <c r="L18" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>3229</t>
         </is>
       </c>
     </row>
@@ -1215,9 +1327,15 @@
       <c r="J19" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>3408</t>
+      <c r="K19" t="n">
+        <v>3408</v>
+      </c>
+      <c r="L19" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>3667</t>
         </is>
       </c>
     </row>
@@ -1258,9 +1376,15 @@
       <c r="J20" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>3977</t>
+      <c r="K20" t="n">
+        <v>3977</v>
+      </c>
+      <c r="L20" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>4329</t>
         </is>
       </c>
     </row>
@@ -1301,9 +1425,15 @@
       <c r="J21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>2726</t>
+      <c r="K21" t="n">
+        <v>2726</v>
+      </c>
+      <c r="L21" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>3038</t>
         </is>
       </c>
     </row>
@@ -1344,9 +1474,15 @@
       <c r="J22" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>3543</t>
+      <c r="K22" t="n">
+        <v>3543</v>
+      </c>
+      <c r="L22" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>3772</t>
         </is>
       </c>
     </row>
@@ -1387,9 +1523,15 @@
       <c r="J23" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>3348</t>
+      <c r="K23" t="n">
+        <v>3348</v>
+      </c>
+      <c r="L23" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>3663</t>
         </is>
       </c>
     </row>
@@ -1412,7 +1554,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F24" s="4" t="n">
@@ -1430,9 +1572,15 @@
       <c r="J24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>3530</t>
+      <c r="K24" t="n">
+        <v>3530</v>
+      </c>
+      <c r="L24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>3868</t>
         </is>
       </c>
     </row>
@@ -1473,7 +1621,13 @@
       <c r="J25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K25" t="inlineStr">
+      <c r="K25" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1516,9 +1670,15 @@
       <c r="J26" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>3727</t>
+      <c r="K26" t="n">
+        <v>3727</v>
+      </c>
+      <c r="L26" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>3987</t>
         </is>
       </c>
     </row>
@@ -1559,9 +1719,15 @@
       <c r="J27" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>3545</t>
+      <c r="K27" t="n">
+        <v>3545</v>
+      </c>
+      <c r="L27" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>3848</t>
         </is>
       </c>
     </row>
@@ -1602,9 +1768,15 @@
       <c r="J28" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>3148</t>
+      <c r="K28" t="n">
+        <v>3148</v>
+      </c>
+      <c r="L28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>3283</t>
         </is>
       </c>
     </row>
@@ -1645,9 +1817,15 @@
       <c r="J29" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>3932</t>
+      <c r="K29" t="n">
+        <v>3932</v>
+      </c>
+      <c r="L29" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>4370</t>
         </is>
       </c>
     </row>
@@ -1688,9 +1866,15 @@
       <c r="J30" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>3401</t>
+      <c r="K30" t="n">
+        <v>3401</v>
+      </c>
+      <c r="L30" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>3538</t>
         </is>
       </c>
     </row>
@@ -1731,9 +1915,15 @@
       <c r="J31" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>3693</t>
+      <c r="K31" t="n">
+        <v>3693</v>
+      </c>
+      <c r="L31" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>4215</t>
         </is>
       </c>
     </row>
@@ -1774,9 +1964,15 @@
       <c r="J32" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>3496</t>
+      <c r="K32" t="n">
+        <v>3496</v>
+      </c>
+      <c r="L32" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>3668</t>
         </is>
       </c>
     </row>
@@ -1817,9 +2013,15 @@
       <c r="J33" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>3437</t>
+      <c r="K33" t="n">
+        <v>3437</v>
+      </c>
+      <c r="L33" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>3759</t>
         </is>
       </c>
     </row>
@@ -1860,9 +2062,15 @@
       <c r="J34" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>3452</t>
+      <c r="K34" t="n">
+        <v>3452</v>
+      </c>
+      <c r="L34" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>3799</t>
         </is>
       </c>
     </row>
@@ -1885,7 +2093,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F35" s="4" t="n">
@@ -1903,9 +2111,15 @@
       <c r="J35" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>3497</t>
+      <c r="K35" t="n">
+        <v>3497</v>
+      </c>
+      <c r="L35" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>3837</t>
         </is>
       </c>
     </row>
@@ -1946,9 +2160,15 @@
       <c r="J36" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>3410</t>
+      <c r="K36" t="n">
+        <v>3410</v>
+      </c>
+      <c r="L36" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>3798</t>
         </is>
       </c>
     </row>
@@ -1989,9 +2209,15 @@
       <c r="J37" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>3342</t>
+      <c r="K37" t="n">
+        <v>3342</v>
+      </c>
+      <c r="L37" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>3512</t>
         </is>
       </c>
     </row>
@@ -2032,9 +2258,15 @@
       <c r="J38" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K38" t="inlineStr">
-        <is>
-          <t>3585</t>
+      <c r="K38" t="n">
+        <v>3585</v>
+      </c>
+      <c r="L38" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>3823</t>
         </is>
       </c>
     </row>
@@ -2075,9 +2307,15 @@
       <c r="J39" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>3589</t>
+      <c r="K39" t="n">
+        <v>3589</v>
+      </c>
+      <c r="L39" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>3920</t>
         </is>
       </c>
     </row>
@@ -2118,9 +2356,15 @@
       <c r="J40" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>3612</t>
+      <c r="K40" t="n">
+        <v>3612</v>
+      </c>
+      <c r="L40" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>4047</t>
         </is>
       </c>
     </row>
@@ -2161,9 +2405,15 @@
       <c r="J41" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K41" t="inlineStr">
-        <is>
-          <t>3460</t>
+      <c r="K41" t="n">
+        <v>3460</v>
+      </c>
+      <c r="L41" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>3599</t>
         </is>
       </c>
     </row>
@@ -2204,9 +2454,15 @@
       <c r="J42" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>3796</t>
+      <c r="K42" t="n">
+        <v>3796</v>
+      </c>
+      <c r="L42" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>4155</t>
         </is>
       </c>
     </row>
@@ -2229,7 +2485,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F43" s="4" t="n">
@@ -2247,9 +2503,15 @@
       <c r="J43" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K43" t="inlineStr">
-        <is>
-          <t>3555</t>
+      <c r="K43" t="n">
+        <v>3555</v>
+      </c>
+      <c r="L43" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>3882</t>
         </is>
       </c>
     </row>
@@ -2272,7 +2534,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F44" s="4" t="n">
@@ -2290,9 +2552,15 @@
       <c r="J44" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="K44" t="inlineStr">
-        <is>
-          <t>3590</t>
+      <c r="K44" t="n">
+        <v>3590</v>
+      </c>
+      <c r="L44" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>3882</t>
         </is>
       </c>
     </row>
@@ -2333,9 +2601,15 @@
       <c r="J45" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>3407</t>
+      <c r="K45" t="n">
+        <v>3407</v>
+      </c>
+      <c r="L45" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>3763</t>
         </is>
       </c>
     </row>
@@ -2376,9 +2650,15 @@
       <c r="J46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>3498</t>
+      <c r="K46" t="n">
+        <v>3498</v>
+      </c>
+      <c r="L46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>3684</t>
         </is>
       </c>
     </row>
@@ -2419,7 +2699,13 @@
       <c r="J47" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K47" t="inlineStr">
+      <c r="K47" t="n">
+        <v>2500</v>
+      </c>
+      <c r="L47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M47" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2462,9 +2748,15 @@
       <c r="J48" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>3698</t>
+      <c r="K48" t="n">
+        <v>3698</v>
+      </c>
+      <c r="L48" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>3989</t>
         </is>
       </c>
     </row>
@@ -2505,9 +2797,15 @@
       <c r="J49" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>3117</t>
+      <c r="K49" t="n">
+        <v>3117</v>
+      </c>
+      <c r="L49" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>3263</t>
         </is>
       </c>
     </row>
@@ -2548,9 +2846,15 @@
       <c r="J50" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>3791</t>
+      <c r="K50" t="n">
+        <v>3791</v>
+      </c>
+      <c r="L50" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>4137</t>
         </is>
       </c>
     </row>
@@ -2591,9 +2895,15 @@
       <c r="J51" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>2782</t>
+      <c r="K51" t="n">
+        <v>2782</v>
+      </c>
+      <c r="L51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>2757</t>
         </is>
       </c>
     </row>
@@ -2634,9 +2944,15 @@
       <c r="J52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="K52" t="n">
+        <v>2500</v>
+      </c>
+      <c r="L52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>2498</t>
         </is>
       </c>
     </row>
@@ -2677,9 +2993,15 @@
       <c r="J53" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>2555</t>
+      <c r="K53" t="n">
+        <v>2555</v>
+      </c>
+      <c r="L53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>2584</t>
         </is>
       </c>
     </row>
@@ -2720,9 +3042,15 @@
       <c r="J54" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="K54" t="inlineStr">
-        <is>
-          <t>3607</t>
+      <c r="K54" t="n">
+        <v>3607</v>
+      </c>
+      <c r="L54" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>3834</t>
         </is>
       </c>
     </row>
@@ -2763,9 +3091,15 @@
       <c r="J55" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>3073</t>
+      <c r="K55" t="n">
+        <v>3073</v>
+      </c>
+      <c r="L55" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>3259</t>
         </is>
       </c>
     </row>
@@ -2806,9 +3140,15 @@
       <c r="J56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K56" t="inlineStr">
-        <is>
-          <t>3094</t>
+      <c r="K56" t="n">
+        <v>3094</v>
+      </c>
+      <c r="L56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>3289</t>
         </is>
       </c>
     </row>
@@ -2849,9 +3189,15 @@
       <c r="J57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>3436</t>
+      <c r="K57" t="n">
+        <v>3436</v>
+      </c>
+      <c r="L57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>3639</t>
         </is>
       </c>
     </row>
@@ -2892,9 +3238,15 @@
       <c r="J58" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="K58" t="inlineStr">
-        <is>
-          <t>3002</t>
+      <c r="K58" t="n">
+        <v>3002</v>
+      </c>
+      <c r="L58" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>3263</t>
         </is>
       </c>
     </row>
@@ -2922,6 +3274,8 @@
       <c r="I59" t="inlineStr"/>
       <c r="J59" s="3" t="inlineStr"/>
       <c r="K59" t="inlineStr"/>
+      <c r="L59" s="3" t="inlineStr"/>
+      <c r="M59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -2947,6 +3301,8 @@
       <c r="I60" t="inlineStr"/>
       <c r="J60" s="3" t="inlineStr"/>
       <c r="K60" t="inlineStr"/>
+      <c r="L60" s="3" t="inlineStr"/>
+      <c r="M60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -2985,9 +3341,15 @@
       <c r="J61" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K61" t="inlineStr">
-        <is>
-          <t>3303</t>
+      <c r="K61" t="n">
+        <v>3303</v>
+      </c>
+      <c r="L61" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>3660</t>
         </is>
       </c>
     </row>
@@ -3028,7 +3390,13 @@
       <c r="J62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K62" t="inlineStr">
+      <c r="K62" t="n">
+        <v>0</v>
+      </c>
+      <c r="L62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3071,9 +3439,15 @@
       <c r="J63" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="K63" t="inlineStr">
-        <is>
-          <t>3487</t>
+      <c r="K63" t="n">
+        <v>3487</v>
+      </c>
+      <c r="L63" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>3743</t>
         </is>
       </c>
     </row>
@@ -3114,9 +3488,15 @@
       <c r="J64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K64" t="inlineStr">
-        <is>
-          <t>2490</t>
+      <c r="K64" t="n">
+        <v>2490</v>
+      </c>
+      <c r="L64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>2518</t>
         </is>
       </c>
     </row>
@@ -3144,6 +3524,8 @@
       <c r="I65" t="inlineStr"/>
       <c r="J65" s="3" t="inlineStr"/>
       <c r="K65" t="inlineStr"/>
+      <c r="L65" s="3" t="inlineStr"/>
+      <c r="M65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -3182,9 +3564,15 @@
       <c r="J66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K66" t="inlineStr">
-        <is>
-          <t>2459</t>
+      <c r="K66" t="n">
+        <v>2459</v>
+      </c>
+      <c r="L66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>2422</t>
         </is>
       </c>
     </row>
@@ -3225,9 +3613,15 @@
       <c r="J67" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="K67" t="inlineStr">
-        <is>
-          <t>3290</t>
+      <c r="K67" t="n">
+        <v>3290</v>
+      </c>
+      <c r="L67" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>3488</t>
         </is>
       </c>
     </row>
@@ -3268,9 +3662,15 @@
       <c r="J68" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K68" t="inlineStr">
-        <is>
-          <t>3639</t>
+      <c r="K68" t="n">
+        <v>3639</v>
+      </c>
+      <c r="L68" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>3923</t>
         </is>
       </c>
     </row>
@@ -3311,9 +3711,15 @@
       <c r="J69" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="K69" t="inlineStr">
-        <is>
-          <t>3197</t>
+      <c r="K69" t="n">
+        <v>3197</v>
+      </c>
+      <c r="L69" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>3334</t>
         </is>
       </c>
     </row>
@@ -3354,9 +3760,15 @@
       <c r="J70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K70" t="inlineStr">
-        <is>
-          <t>2567</t>
+      <c r="K70" t="n">
+        <v>2567</v>
+      </c>
+      <c r="L70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>2595</t>
         </is>
       </c>
     </row>
@@ -3397,9 +3809,15 @@
       <c r="J71" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="K71" t="inlineStr">
-        <is>
-          <t>3115</t>
+      <c r="K71" t="n">
+        <v>3115</v>
+      </c>
+      <c r="L71" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>3287</t>
         </is>
       </c>
     </row>
@@ -3440,9 +3858,15 @@
       <c r="J72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K72" t="inlineStr">
-        <is>
-          <t>2790</t>
+      <c r="K72" t="n">
+        <v>2790</v>
+      </c>
+      <c r="L72" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>2863</t>
         </is>
       </c>
     </row>
@@ -3483,9 +3907,15 @@
       <c r="J73" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K73" t="inlineStr">
-        <is>
-          <t>3097</t>
+      <c r="K73" t="n">
+        <v>3097</v>
+      </c>
+      <c r="L73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>3308</t>
         </is>
       </c>
     </row>
@@ -3526,9 +3956,15 @@
       <c r="J74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K74" t="inlineStr">
-        <is>
-          <t>2563</t>
+      <c r="K74" t="n">
+        <v>2563</v>
+      </c>
+      <c r="L74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>2590</t>
         </is>
       </c>
     </row>
@@ -3569,9 +4005,15 @@
       <c r="J75" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="K75" t="inlineStr">
-        <is>
-          <t>3071</t>
+      <c r="K75" t="n">
+        <v>3071</v>
+      </c>
+      <c r="L75" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>3182</t>
         </is>
       </c>
     </row>
@@ -3612,9 +4054,15 @@
       <c r="J76" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K76" t="inlineStr">
-        <is>
-          <t>3209</t>
+      <c r="K76" t="n">
+        <v>3209</v>
+      </c>
+      <c r="L76" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>3486</t>
         </is>
       </c>
     </row>
@@ -3655,9 +4103,15 @@
       <c r="J77" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K77" t="inlineStr">
-        <is>
-          <t>3321</t>
+      <c r="K77" t="n">
+        <v>3321</v>
+      </c>
+      <c r="L77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>3335</t>
         </is>
       </c>
     </row>
@@ -3698,9 +4152,15 @@
       <c r="J78" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K78" t="inlineStr">
-        <is>
-          <t>3449</t>
+      <c r="K78" t="n">
+        <v>3449</v>
+      </c>
+      <c r="L78" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M78" t="inlineStr">
+        <is>
+          <t>3717</t>
         </is>
       </c>
     </row>
@@ -3741,7 +4201,13 @@
       <c r="J79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K79" t="inlineStr">
+      <c r="K79" t="n">
+        <v>0</v>
+      </c>
+      <c r="L79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3784,9 +4250,15 @@
       <c r="J80" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="K80" t="inlineStr">
-        <is>
-          <t>3310</t>
+      <c r="K80" t="n">
+        <v>3310</v>
+      </c>
+      <c r="L80" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M80" t="inlineStr">
+        <is>
+          <t>3524</t>
         </is>
       </c>
     </row>
@@ -3827,9 +4299,15 @@
       <c r="J81" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K81" t="inlineStr">
-        <is>
-          <t>3310</t>
+      <c r="K81" t="n">
+        <v>3310</v>
+      </c>
+      <c r="L81" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="M81" t="inlineStr">
+        <is>
+          <t>3574</t>
         </is>
       </c>
     </row>
@@ -3870,9 +4348,15 @@
       <c r="J82" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="K82" t="inlineStr">
-        <is>
-          <t>3121</t>
+      <c r="K82" t="n">
+        <v>3121</v>
+      </c>
+      <c r="L82" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="M82" t="inlineStr">
+        <is>
+          <t>3381</t>
         </is>
       </c>
     </row>
@@ -3913,9 +4397,15 @@
       <c r="J83" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="K83" t="inlineStr">
-        <is>
-          <t>3148</t>
+      <c r="K83" t="n">
+        <v>3148</v>
+      </c>
+      <c r="L83" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M83" t="inlineStr">
+        <is>
+          <t>3265</t>
         </is>
       </c>
     </row>
@@ -3956,9 +4446,15 @@
       <c r="J84" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="K84" t="inlineStr">
-        <is>
-          <t>2812</t>
+      <c r="K84" t="n">
+        <v>2812</v>
+      </c>
+      <c r="L84" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="M84" t="inlineStr">
+        <is>
+          <t>2758</t>
         </is>
       </c>
     </row>
@@ -3999,9 +4495,15 @@
       <c r="J85" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K85" t="inlineStr">
-        <is>
-          <t>2982</t>
+      <c r="K85" t="n">
+        <v>2982</v>
+      </c>
+      <c r="L85" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M85" t="inlineStr">
+        <is>
+          <t>2998</t>
         </is>
       </c>
     </row>
@@ -4042,9 +4544,15 @@
       <c r="J86" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K86" t="inlineStr">
-        <is>
-          <t>2724</t>
+      <c r="K86" t="n">
+        <v>2724</v>
+      </c>
+      <c r="L86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M86" t="inlineStr">
+        <is>
+          <t>2717</t>
         </is>
       </c>
     </row>
@@ -4085,9 +4593,15 @@
       <c r="J87" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K87" t="inlineStr">
-        <is>
-          <t>3513</t>
+      <c r="K87" t="n">
+        <v>3513</v>
+      </c>
+      <c r="L87" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M87" t="inlineStr">
+        <is>
+          <t>3492</t>
         </is>
       </c>
     </row>
@@ -4128,9 +4642,15 @@
       <c r="J88" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="K88" t="inlineStr">
-        <is>
-          <t>2696</t>
+      <c r="K88" t="n">
+        <v>2696</v>
+      </c>
+      <c r="L88" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M88" t="inlineStr">
+        <is>
+          <t>2721</t>
         </is>
       </c>
     </row>
@@ -4171,9 +4691,15 @@
       <c r="J89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K89" t="inlineStr">
-        <is>
-          <t>2538</t>
+      <c r="K89" t="n">
+        <v>2538</v>
+      </c>
+      <c r="L89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M89" t="inlineStr">
+        <is>
+          <t>2581</t>
         </is>
       </c>
     </row>
@@ -4214,9 +4740,15 @@
       <c r="J90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K90" t="inlineStr">
-        <is>
-          <t>2448</t>
+      <c r="K90" t="n">
+        <v>2448</v>
+      </c>
+      <c r="L90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M90" t="inlineStr">
+        <is>
+          <t>2408</t>
         </is>
       </c>
     </row>
@@ -4257,9 +4789,15 @@
       <c r="J91" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K91" t="inlineStr">
-        <is>
-          <t>2636</t>
+      <c r="K91" t="n">
+        <v>2636</v>
+      </c>
+      <c r="L91" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M91" t="inlineStr">
+        <is>
+          <t>2646</t>
         </is>
       </c>
     </row>
@@ -4300,7 +4838,13 @@
       <c r="J92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K92" t="inlineStr">
+      <c r="K92" t="n">
+        <v>0</v>
+      </c>
+      <c r="L92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4343,9 +4887,15 @@
       <c r="J93" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="K93" t="inlineStr">
-        <is>
-          <t>2511</t>
+      <c r="K93" t="n">
+        <v>2511</v>
+      </c>
+      <c r="L93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M93" t="inlineStr">
+        <is>
+          <t>2454</t>
         </is>
       </c>
     </row>
@@ -4386,9 +4936,15 @@
       <c r="J94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K94" t="inlineStr">
-        <is>
-          <t>2544</t>
+      <c r="K94" t="n">
+        <v>2544</v>
+      </c>
+      <c r="L94" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M94" t="inlineStr">
+        <is>
+          <t>2882</t>
         </is>
       </c>
     </row>
@@ -4429,9 +4985,15 @@
       <c r="J95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K95" t="inlineStr">
-        <is>
-          <t>2445</t>
+      <c r="K95" t="n">
+        <v>2445</v>
+      </c>
+      <c r="L95" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="M95" t="inlineStr">
+        <is>
+          <t>2645</t>
         </is>
       </c>
     </row>
@@ -4472,9 +5034,15 @@
       <c r="J96" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="K96" t="inlineStr">
-        <is>
-          <t>2849</t>
+      <c r="K96" t="n">
+        <v>2849</v>
+      </c>
+      <c r="L96" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M96" t="inlineStr">
+        <is>
+          <t>2927</t>
         </is>
       </c>
     </row>
@@ -4515,9 +5083,15 @@
       <c r="J97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K97" t="inlineStr">
-        <is>
-          <t>2499</t>
+      <c r="K97" t="n">
+        <v>2499</v>
+      </c>
+      <c r="L97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M97" t="inlineStr">
+        <is>
+          <t>2495</t>
         </is>
       </c>
     </row>
@@ -4558,7 +5132,13 @@
       <c r="J98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K98" t="inlineStr">
+      <c r="K98" t="n">
+        <v>0</v>
+      </c>
+      <c r="L98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4601,9 +5181,15 @@
       <c r="J99" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="K99" t="inlineStr">
-        <is>
-          <t>2832</t>
+      <c r="K99" t="n">
+        <v>2832</v>
+      </c>
+      <c r="L99" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="M99" t="inlineStr">
+        <is>
+          <t>2903</t>
         </is>
       </c>
     </row>
@@ -4644,9 +5230,15 @@
       <c r="J100" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="K100" t="inlineStr">
-        <is>
-          <t>2436</t>
+      <c r="K100" t="n">
+        <v>2436</v>
+      </c>
+      <c r="L100" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="M100" t="inlineStr">
+        <is>
+          <t>2435</t>
         </is>
       </c>
     </row>
@@ -4687,9 +5279,15 @@
       <c r="J101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K101" t="inlineStr">
-        <is>
-          <t>3214</t>
+      <c r="K101" t="n">
+        <v>3214</v>
+      </c>
+      <c r="L101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M101" t="inlineStr">
+        <is>
+          <t>3454</t>
         </is>
       </c>
     </row>
@@ -4730,9 +5328,15 @@
       <c r="J102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K102" t="inlineStr">
-        <is>
-          <t>3042</t>
+      <c r="K102" t="n">
+        <v>3042</v>
+      </c>
+      <c r="L102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M102" t="inlineStr">
+        <is>
+          <t>3222</t>
         </is>
       </c>
     </row>
@@ -4773,9 +5377,15 @@
       <c r="J103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K103" t="inlineStr">
-        <is>
-          <t>2532</t>
+      <c r="K103" t="n">
+        <v>2532</v>
+      </c>
+      <c r="L103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M103" t="inlineStr">
+        <is>
+          <t>2523</t>
         </is>
       </c>
     </row>
@@ -4816,9 +5426,15 @@
       <c r="J104" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K104" t="inlineStr">
-        <is>
-          <t>3259</t>
+      <c r="K104" t="n">
+        <v>3259</v>
+      </c>
+      <c r="L104" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="M104" t="inlineStr">
+        <is>
+          <t>3468</t>
         </is>
       </c>
     </row>
@@ -4859,9 +5475,15 @@
       <c r="J105" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="K105" t="inlineStr">
-        <is>
-          <t>3118</t>
+      <c r="K105" t="n">
+        <v>3118</v>
+      </c>
+      <c r="L105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M105" t="inlineStr">
+        <is>
+          <t>3104</t>
         </is>
       </c>
     </row>
@@ -4902,7 +5524,13 @@
       <c r="J106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K106" t="inlineStr">
+      <c r="K106" t="n">
+        <v>0</v>
+      </c>
+      <c r="L106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4945,9 +5573,15 @@
       <c r="J107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K107" t="inlineStr">
-        <is>
-          <t>2510</t>
+      <c r="K107" t="n">
+        <v>2510</v>
+      </c>
+      <c r="L107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M107" t="inlineStr">
+        <is>
+          <t>2513</t>
         </is>
       </c>
     </row>
@@ -4988,7 +5622,13 @@
       <c r="J108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K108" t="inlineStr">
+      <c r="K108" t="n">
+        <v>0</v>
+      </c>
+      <c r="L108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5031,9 +5671,15 @@
       <c r="J109" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="K109" t="inlineStr">
-        <is>
-          <t>2841</t>
+      <c r="K109" t="n">
+        <v>2841</v>
+      </c>
+      <c r="L109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M109" t="inlineStr">
+        <is>
+          <t>2976</t>
         </is>
       </c>
     </row>
@@ -5074,9 +5720,15 @@
       <c r="J110" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="K110" t="inlineStr">
-        <is>
-          <t>2891</t>
+      <c r="K110" t="n">
+        <v>2891</v>
+      </c>
+      <c r="L110" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M110" t="inlineStr">
+        <is>
+          <t>2995</t>
         </is>
       </c>
     </row>
@@ -5117,9 +5769,15 @@
       <c r="J111" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="K111" t="inlineStr">
-        <is>
-          <t>2636</t>
+      <c r="K111" t="n">
+        <v>2636</v>
+      </c>
+      <c r="L111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M111" t="inlineStr">
+        <is>
+          <t>2607</t>
         </is>
       </c>
     </row>
@@ -5160,9 +5818,15 @@
       <c r="J112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K112" t="inlineStr">
-        <is>
-          <t>2608</t>
+      <c r="K112" t="n">
+        <v>2608</v>
+      </c>
+      <c r="L112" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="M112" t="inlineStr">
+        <is>
+          <t>2814</t>
         </is>
       </c>
     </row>
@@ -5203,9 +5867,15 @@
       <c r="J113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K113" t="inlineStr">
-        <is>
-          <t>2689</t>
+      <c r="K113" t="n">
+        <v>2689</v>
+      </c>
+      <c r="L113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M113" t="inlineStr">
+        <is>
+          <t>2732</t>
         </is>
       </c>
     </row>
@@ -5246,7 +5916,13 @@
       <c r="J114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K114" t="inlineStr">
+      <c r="K114" t="n">
+        <v>0</v>
+      </c>
+      <c r="L114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M114" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5289,9 +5965,15 @@
       <c r="J115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K115" t="inlineStr">
-        <is>
-          <t>2466</t>
+      <c r="K115" t="n">
+        <v>2466</v>
+      </c>
+      <c r="L115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M115" t="inlineStr">
+        <is>
+          <t>2440</t>
         </is>
       </c>
     </row>
@@ -5332,9 +6014,15 @@
       <c r="J116" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="K116" t="inlineStr">
-        <is>
-          <t>2622</t>
+      <c r="K116" t="n">
+        <v>2622</v>
+      </c>
+      <c r="L116" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="M116" t="inlineStr">
+        <is>
+          <t>2721</t>
         </is>
       </c>
     </row>
@@ -5375,9 +6063,15 @@
       <c r="J117" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K117" t="inlineStr">
-        <is>
-          <t>2938</t>
+      <c r="K117" t="n">
+        <v>2938</v>
+      </c>
+      <c r="L117" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="M117" t="inlineStr">
+        <is>
+          <t>3065</t>
         </is>
       </c>
     </row>
@@ -5418,7 +6112,13 @@
       <c r="J118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K118" t="inlineStr">
+      <c r="K118" t="n">
+        <v>0</v>
+      </c>
+      <c r="L118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5461,9 +6161,15 @@
       <c r="J119" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K119" t="inlineStr">
-        <is>
-          <t>3001</t>
+      <c r="K119" t="n">
+        <v>3001</v>
+      </c>
+      <c r="L119" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M119" t="inlineStr">
+        <is>
+          <t>3090</t>
         </is>
       </c>
     </row>
@@ -5504,9 +6210,15 @@
       <c r="J120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K120" t="inlineStr">
-        <is>
-          <t>2381</t>
+      <c r="K120" t="n">
+        <v>2381</v>
+      </c>
+      <c r="L120" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="M120" t="inlineStr">
+        <is>
+          <t>2449</t>
         </is>
       </c>
     </row>
@@ -5547,9 +6259,15 @@
       <c r="J121" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="K121" t="inlineStr">
-        <is>
-          <t>2715</t>
+      <c r="K121" t="n">
+        <v>2715</v>
+      </c>
+      <c r="L121" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="M121" t="inlineStr">
+        <is>
+          <t>2875</t>
         </is>
       </c>
     </row>
@@ -5590,7 +6308,13 @@
       <c r="J122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K122" t="inlineStr">
+      <c r="K122" t="n">
+        <v>0</v>
+      </c>
+      <c r="L122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5633,9 +6357,15 @@
       <c r="J123" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K123" t="inlineStr">
-        <is>
-          <t>2725</t>
+      <c r="K123" t="n">
+        <v>2725</v>
+      </c>
+      <c r="L123" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M123" t="inlineStr">
+        <is>
+          <t>2866</t>
         </is>
       </c>
     </row>
@@ -5676,9 +6406,15 @@
       <c r="J124" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="K124" t="inlineStr">
-        <is>
-          <t>2762</t>
+      <c r="K124" t="n">
+        <v>2762</v>
+      </c>
+      <c r="L124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M124" t="inlineStr">
+        <is>
+          <t>2857</t>
         </is>
       </c>
     </row>
@@ -5719,9 +6455,15 @@
       <c r="J125" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K125" t="inlineStr">
-        <is>
-          <t>2855</t>
+      <c r="K125" t="n">
+        <v>2855</v>
+      </c>
+      <c r="L125" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M125" t="inlineStr">
+        <is>
+          <t>2997</t>
         </is>
       </c>
     </row>
@@ -5762,9 +6504,15 @@
       <c r="J126" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K126" t="inlineStr">
-        <is>
-          <t>2816</t>
+      <c r="K126" t="n">
+        <v>2816</v>
+      </c>
+      <c r="L126" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M126" t="inlineStr">
+        <is>
+          <t>2823</t>
         </is>
       </c>
     </row>
@@ -5805,9 +6553,15 @@
       <c r="J127" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="K127" t="inlineStr">
-        <is>
-          <t>2476</t>
+      <c r="K127" t="n">
+        <v>2476</v>
+      </c>
+      <c r="L127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M127" t="inlineStr">
+        <is>
+          <t>2415</t>
         </is>
       </c>
     </row>
@@ -5848,7 +6602,13 @@
       <c r="J128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K128" t="inlineStr">
+      <c r="K128" t="n">
+        <v>0</v>
+      </c>
+      <c r="L128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5891,7 +6651,13 @@
       <c r="J129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K129" t="inlineStr">
+      <c r="K129" t="n">
+        <v>0</v>
+      </c>
+      <c r="L129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5934,9 +6700,15 @@
       <c r="J130" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="K130" t="inlineStr">
-        <is>
-          <t>2509</t>
+      <c r="K130" t="n">
+        <v>2509</v>
+      </c>
+      <c r="L130" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="M130" t="inlineStr">
+        <is>
+          <t>2600</t>
         </is>
       </c>
     </row>
@@ -5977,9 +6749,15 @@
       <c r="J131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K131" t="inlineStr">
-        <is>
-          <t>2407</t>
+      <c r="K131" t="n">
+        <v>2407</v>
+      </c>
+      <c r="L131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M131" t="inlineStr">
+        <is>
+          <t>2439</t>
         </is>
       </c>
     </row>
@@ -6020,9 +6798,15 @@
       <c r="J132" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K132" t="inlineStr">
-        <is>
-          <t>2430</t>
+      <c r="K132" t="n">
+        <v>2430</v>
+      </c>
+      <c r="L132" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M132" t="inlineStr">
+        <is>
+          <t>2442</t>
         </is>
       </c>
     </row>
@@ -6063,9 +6847,15 @@
       <c r="J133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K133" t="inlineStr">
-        <is>
-          <t>2669</t>
+      <c r="K133" t="n">
+        <v>2669</v>
+      </c>
+      <c r="L133" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="M133" t="inlineStr">
+        <is>
+          <t>2755</t>
         </is>
       </c>
     </row>
@@ -6106,9 +6896,15 @@
       <c r="J134" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="K134" t="inlineStr">
-        <is>
-          <t>1560</t>
+      <c r="K134" t="n">
+        <v>1560</v>
+      </c>
+      <c r="L134" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="M134" t="inlineStr">
+        <is>
+          <t>1668</t>
         </is>
       </c>
     </row>
@@ -6149,11 +6945,11 @@
       <c r="J135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K135" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="K135" t="n">
+        <v>0</v>
+      </c>
+      <c r="L135" s="3" t="inlineStr"/>
+      <c r="M135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -6192,9 +6988,15 @@
       <c r="J136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K136" t="inlineStr">
-        <is>
-          <t>2543</t>
+      <c r="K136" t="n">
+        <v>2543</v>
+      </c>
+      <c r="L136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M136" t="inlineStr">
+        <is>
+          <t>2601</t>
         </is>
       </c>
     </row>
@@ -6235,7 +7037,13 @@
       <c r="J137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K137" t="inlineStr">
+      <c r="K137" t="n">
+        <v>0</v>
+      </c>
+      <c r="L137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6278,11 +7086,11 @@
       <c r="J138" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K138" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="K138" t="n">
+        <v>0</v>
+      </c>
+      <c r="L138" s="3" t="inlineStr"/>
+      <c r="M138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -6321,9 +7129,15 @@
       <c r="J139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K139" t="inlineStr">
-        <is>
-          <t>2413</t>
+      <c r="K139" t="n">
+        <v>2413</v>
+      </c>
+      <c r="L139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M139" t="inlineStr">
+        <is>
+          <t>2410</t>
         </is>
       </c>
     </row>
@@ -6364,9 +7178,15 @@
       <c r="J140" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="K140" t="inlineStr">
-        <is>
-          <t>2639</t>
+      <c r="K140" t="n">
+        <v>2639</v>
+      </c>
+      <c r="L140" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M140" t="inlineStr">
+        <is>
+          <t>2663</t>
         </is>
       </c>
     </row>
@@ -6407,11 +7227,11 @@
       <c r="J141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K141" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="K141" t="n">
+        <v>0</v>
+      </c>
+      <c r="L141" s="3" t="inlineStr"/>
+      <c r="M141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -6450,7 +7270,13 @@
       <c r="J142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K142" t="inlineStr">
+      <c r="K142" t="n">
+        <v>2000</v>
+      </c>
+      <c r="L142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M142" t="inlineStr">
         <is>
           <t>2000</t>
         </is>
@@ -6493,11 +7319,11 @@
       <c r="J143" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K143" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="K143" t="n">
+        <v>0</v>
+      </c>
+      <c r="L143" s="3" t="inlineStr"/>
+      <c r="M143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -6536,11 +7362,11 @@
       <c r="J144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K144" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="K144" t="n">
+        <v>0</v>
+      </c>
+      <c r="L144" s="3" t="inlineStr"/>
+      <c r="M144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -6579,11 +7405,11 @@
       <c r="J145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K145" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="K145" t="n">
+        <v>0</v>
+      </c>
+      <c r="L145" s="3" t="inlineStr"/>
+      <c r="M145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -6622,11 +7448,11 @@
       <c r="J146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K146" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="K146" t="n">
+        <v>0</v>
+      </c>
+      <c r="L146" s="3" t="inlineStr"/>
+      <c r="M146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -6665,11 +7491,11 @@
       <c r="J147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K147" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="K147" t="n">
+        <v>0</v>
+      </c>
+      <c r="L147" s="3" t="inlineStr"/>
+      <c r="M147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -6708,7 +7534,13 @@
       <c r="J148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K148" t="inlineStr">
+      <c r="K148" t="n">
+        <v>1500</v>
+      </c>
+      <c r="L148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M148" t="inlineStr">
         <is>
           <t>1500</t>
         </is>
@@ -6751,9 +7583,15 @@
       <c r="J149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K149" t="inlineStr">
-        <is>
-          <t>2496</t>
+      <c r="K149" t="n">
+        <v>2496</v>
+      </c>
+      <c r="L149" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="M149" t="inlineStr">
+        <is>
+          <t>2578</t>
         </is>
       </c>
     </row>
@@ -6794,7 +7632,13 @@
       <c r="J150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K150" t="inlineStr">
+      <c r="K150" t="n">
+        <v>0</v>
+      </c>
+      <c r="L150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6837,7 +7681,13 @@
       <c r="J151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K151" t="inlineStr">
+      <c r="K151" t="n">
+        <v>0</v>
+      </c>
+      <c r="L151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6880,7 +7730,13 @@
       <c r="J152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K152" t="inlineStr">
+      <c r="K152" t="n">
+        <v>0</v>
+      </c>
+      <c r="L152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6923,7 +7779,13 @@
       <c r="J153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K153" t="inlineStr">
+      <c r="K153" t="n">
+        <v>0</v>
+      </c>
+      <c r="L153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6966,7 +7828,13 @@
       <c r="J154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K154" t="inlineStr">
+      <c r="K154" t="n">
+        <v>0</v>
+      </c>
+      <c r="L154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7009,7 +7877,13 @@
       <c r="J155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K155" t="inlineStr">
+      <c r="K155" t="n">
+        <v>0</v>
+      </c>
+      <c r="L155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M155" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7046,9 +7920,15 @@
       <c r="J156" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="K156" t="inlineStr">
-        <is>
-          <t>2809</t>
+      <c r="K156" t="n">
+        <v>2809</v>
+      </c>
+      <c r="L156" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M156" t="inlineStr">
+        <is>
+          <t>2994</t>
         </is>
       </c>
     </row>
@@ -7083,11 +7963,11 @@
       <c r="J157" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="K157" t="inlineStr">
-        <is>
-          <t>2129</t>
-        </is>
-      </c>
+      <c r="K157" t="n">
+        <v>2129</v>
+      </c>
+      <c r="L157" s="3" t="inlineStr"/>
+      <c r="M157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -7120,7 +8000,13 @@
       <c r="J158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K158" t="inlineStr">
+      <c r="K158" t="n">
+        <v>0</v>
+      </c>
+      <c r="L158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7157,9 +8043,15 @@
       <c r="J159" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="K159" t="inlineStr">
-        <is>
-          <t>2157</t>
+      <c r="K159" t="n">
+        <v>2157</v>
+      </c>
+      <c r="L159" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M159" t="inlineStr">
+        <is>
+          <t>2429</t>
         </is>
       </c>
     </row>
@@ -7190,9 +8082,81 @@
       <c r="J160" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K160" t="inlineStr">
-        <is>
-          <t>1996</t>
+      <c r="K160" t="n">
+        <v>1996</v>
+      </c>
+      <c r="L160" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="M160" t="inlineStr">
+        <is>
+          <t>2184</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>58743790</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Ma</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr"/>
+      <c r="D161" t="inlineStr"/>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F161" s="3" t="inlineStr"/>
+      <c r="G161" t="inlineStr"/>
+      <c r="H161" s="3" t="inlineStr"/>
+      <c r="I161" t="inlineStr"/>
+      <c r="J161" s="3" t="inlineStr"/>
+      <c r="K161" t="inlineStr"/>
+      <c r="L161" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="M161" t="inlineStr">
+        <is>
+          <t>2502</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>10636651</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>"Ismail Aflou"</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr"/>
+      <c r="D162" t="inlineStr"/>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="F162" s="3" t="inlineStr"/>
+      <c r="G162" t="inlineStr"/>
+      <c r="H162" s="3" t="inlineStr"/>
+      <c r="I162" t="inlineStr"/>
+      <c r="J162" s="3" t="inlineStr"/>
+      <c r="K162" t="inlineStr"/>
+      <c r="L162" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M162" t="inlineStr">
+        <is>
+          <t>2317</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-02-17 11:30:35
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M162"/>
+  <dimension ref="A1:O163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,6 +456,16 @@
           <t>02-15_0</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>02-16_A</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>02-16_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -500,9 +510,15 @@
       <c r="L2" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>2901</t>
+      <c r="M2" t="n">
+        <v>2901</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>2962</t>
         </is>
       </c>
     </row>
@@ -549,9 +565,15 @@
       <c r="L3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>3570</t>
+      <c r="M3" t="n">
+        <v>3570</v>
+      </c>
+      <c r="N3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>3789</t>
         </is>
       </c>
     </row>
@@ -598,9 +620,15 @@
       <c r="L4" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>4020</t>
+      <c r="M4" t="n">
+        <v>4020</v>
+      </c>
+      <c r="N4" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>4364</t>
         </is>
       </c>
     </row>
@@ -647,9 +675,15 @@
       <c r="L5" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>3275</t>
+      <c r="M5" t="n">
+        <v>3275</v>
+      </c>
+      <c r="N5" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>3365</t>
         </is>
       </c>
     </row>
@@ -696,9 +730,15 @@
       <c r="L6" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>3781</t>
+      <c r="M6" t="n">
+        <v>3781</v>
+      </c>
+      <c r="N6" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>4052</t>
         </is>
       </c>
     </row>
@@ -745,9 +785,15 @@
       <c r="L7" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>4201</t>
+      <c r="M7" t="n">
+        <v>4201</v>
+      </c>
+      <c r="N7" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>4547</t>
         </is>
       </c>
     </row>
@@ -794,9 +840,15 @@
       <c r="L8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>3607</t>
+      <c r="M8" t="n">
+        <v>3607</v>
+      </c>
+      <c r="N8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>3784</t>
         </is>
       </c>
     </row>
@@ -843,9 +895,15 @@
       <c r="L9" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>3661</t>
+      <c r="M9" t="n">
+        <v>3661</v>
+      </c>
+      <c r="N9" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>3885</t>
         </is>
       </c>
     </row>
@@ -892,9 +950,15 @@
       <c r="L10" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>3622</t>
+      <c r="M10" t="n">
+        <v>3622</v>
+      </c>
+      <c r="N10" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>3843</t>
         </is>
       </c>
     </row>
@@ -941,9 +1005,15 @@
       <c r="L11" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>3473</t>
+      <c r="M11" t="n">
+        <v>3473</v>
+      </c>
+      <c r="N11" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>3660</t>
         </is>
       </c>
     </row>
@@ -990,9 +1060,15 @@
       <c r="L12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>2677</t>
+      <c r="M12" t="n">
+        <v>2677</v>
+      </c>
+      <c r="N12" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>2835</t>
         </is>
       </c>
     </row>
@@ -1039,9 +1115,15 @@
       <c r="L13" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>4241</t>
+      <c r="M13" t="n">
+        <v>4241</v>
+      </c>
+      <c r="N13" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>4544</t>
         </is>
       </c>
     </row>
@@ -1088,9 +1170,15 @@
       <c r="L14" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>3767</t>
+      <c r="M14" t="n">
+        <v>3767</v>
+      </c>
+      <c r="N14" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>3996</t>
         </is>
       </c>
     </row>
@@ -1137,9 +1225,15 @@
       <c r="L15" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>3319</t>
+      <c r="M15" t="n">
+        <v>3319</v>
+      </c>
+      <c r="N15" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>3582</t>
         </is>
       </c>
     </row>
@@ -1186,9 +1280,15 @@
       <c r="L16" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>3826</t>
+      <c r="M16" t="n">
+        <v>3826</v>
+      </c>
+      <c r="N16" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>4073</t>
         </is>
       </c>
     </row>
@@ -1235,9 +1335,15 @@
       <c r="L17" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>3399</t>
+      <c r="M17" t="n">
+        <v>3399</v>
+      </c>
+      <c r="N17" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>3594</t>
         </is>
       </c>
     </row>
@@ -1284,9 +1390,15 @@
       <c r="L18" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>3229</t>
+      <c r="M18" t="n">
+        <v>3229</v>
+      </c>
+      <c r="N18" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>3603</t>
         </is>
       </c>
     </row>
@@ -1309,7 +1421,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F19" s="3" t="n">
@@ -1333,9 +1445,15 @@
       <c r="L19" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>3667</t>
+      <c r="M19" t="n">
+        <v>3667</v>
+      </c>
+      <c r="N19" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>3954</t>
         </is>
       </c>
     </row>
@@ -1358,7 +1476,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F20" s="3" t="n">
@@ -1382,9 +1500,15 @@
       <c r="L20" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>4329</t>
+      <c r="M20" t="n">
+        <v>4329</v>
+      </c>
+      <c r="N20" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>4637</t>
         </is>
       </c>
     </row>
@@ -1431,9 +1555,15 @@
       <c r="L21" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>3038</t>
+      <c r="M21" t="n">
+        <v>3038</v>
+      </c>
+      <c r="N21" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>3204</t>
         </is>
       </c>
     </row>
@@ -1480,9 +1610,15 @@
       <c r="L22" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>3772</t>
+      <c r="M22" t="n">
+        <v>3772</v>
+      </c>
+      <c r="N22" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>4118</t>
         </is>
       </c>
     </row>
@@ -1529,9 +1665,15 @@
       <c r="L23" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M23" t="inlineStr">
-        <is>
-          <t>3663</t>
+      <c r="M23" t="n">
+        <v>3663</v>
+      </c>
+      <c r="N23" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>3874</t>
         </is>
       </c>
     </row>
@@ -1578,9 +1720,15 @@
       <c r="L24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>3868</t>
+      <c r="M24" t="n">
+        <v>3868</v>
+      </c>
+      <c r="N24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>4177</t>
         </is>
       </c>
     </row>
@@ -1627,7 +1775,13 @@
       <c r="L25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M25" t="inlineStr">
+      <c r="M25" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1676,9 +1830,15 @@
       <c r="L26" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="M26" t="inlineStr">
-        <is>
-          <t>3987</t>
+      <c r="M26" t="n">
+        <v>3987</v>
+      </c>
+      <c r="N26" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>4232</t>
         </is>
       </c>
     </row>
@@ -1725,9 +1885,15 @@
       <c r="L27" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M27" t="inlineStr">
-        <is>
-          <t>3848</t>
+      <c r="M27" t="n">
+        <v>3848</v>
+      </c>
+      <c r="N27" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>4143</t>
         </is>
       </c>
     </row>
@@ -1774,9 +1940,15 @@
       <c r="L28" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="M28" t="inlineStr">
-        <is>
-          <t>3283</t>
+      <c r="M28" t="n">
+        <v>3283</v>
+      </c>
+      <c r="N28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>3496</t>
         </is>
       </c>
     </row>
@@ -1823,9 +1995,15 @@
       <c r="L29" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="M29" t="inlineStr">
-        <is>
-          <t>4370</t>
+      <c r="M29" t="n">
+        <v>4370</v>
+      </c>
+      <c r="N29" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>4693</t>
         </is>
       </c>
     </row>
@@ -1872,9 +2050,15 @@
       <c r="L30" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M30" t="inlineStr">
-        <is>
-          <t>3538</t>
+      <c r="M30" t="n">
+        <v>3538</v>
+      </c>
+      <c r="N30" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>3712</t>
         </is>
       </c>
     </row>
@@ -1921,9 +2105,15 @@
       <c r="L31" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="M31" t="inlineStr">
-        <is>
-          <t>4215</t>
+      <c r="M31" t="n">
+        <v>4215</v>
+      </c>
+      <c r="N31" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>4605</t>
         </is>
       </c>
     </row>
@@ -1970,7 +2160,13 @@
       <c r="L32" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M32" t="inlineStr">
+      <c r="M32" t="n">
+        <v>3668</v>
+      </c>
+      <c r="N32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O32" t="inlineStr">
         <is>
           <t>3668</t>
         </is>
@@ -2019,9 +2215,15 @@
       <c r="L33" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="M33" t="inlineStr">
-        <is>
-          <t>3759</t>
+      <c r="M33" t="n">
+        <v>3759</v>
+      </c>
+      <c r="N33" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>4061</t>
         </is>
       </c>
     </row>
@@ -2044,7 +2246,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F34" s="3" t="n">
@@ -2068,9 +2270,15 @@
       <c r="L34" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M34" t="inlineStr">
-        <is>
-          <t>3799</t>
+      <c r="M34" t="n">
+        <v>3799</v>
+      </c>
+      <c r="N34" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>4109</t>
         </is>
       </c>
     </row>
@@ -2117,9 +2325,15 @@
       <c r="L35" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M35" t="inlineStr">
-        <is>
-          <t>3837</t>
+      <c r="M35" t="n">
+        <v>3837</v>
+      </c>
+      <c r="N35" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>4020</t>
         </is>
       </c>
     </row>
@@ -2166,9 +2380,15 @@
       <c r="L36" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M36" t="inlineStr">
-        <is>
-          <t>3798</t>
+      <c r="M36" t="n">
+        <v>3798</v>
+      </c>
+      <c r="N36" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>4156</t>
         </is>
       </c>
     </row>
@@ -2215,9 +2435,15 @@
       <c r="L37" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="M37" t="inlineStr">
-        <is>
-          <t>3512</t>
+      <c r="M37" t="n">
+        <v>3512</v>
+      </c>
+      <c r="N37" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>3713</t>
         </is>
       </c>
     </row>
@@ -2264,9 +2490,15 @@
       <c r="L38" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="M38" t="inlineStr">
-        <is>
-          <t>3823</t>
+      <c r="M38" t="n">
+        <v>3823</v>
+      </c>
+      <c r="N38" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>4068</t>
         </is>
       </c>
     </row>
@@ -2313,9 +2545,15 @@
       <c r="L39" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="M39" t="inlineStr">
-        <is>
-          <t>3920</t>
+      <c r="M39" t="n">
+        <v>3920</v>
+      </c>
+      <c r="N39" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>4080</t>
         </is>
       </c>
     </row>
@@ -2362,9 +2600,15 @@
       <c r="L40" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M40" t="inlineStr">
-        <is>
-          <t>4047</t>
+      <c r="M40" t="n">
+        <v>4047</v>
+      </c>
+      <c r="N40" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>4481</t>
         </is>
       </c>
     </row>
@@ -2411,9 +2655,15 @@
       <c r="L41" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="M41" t="inlineStr">
-        <is>
-          <t>3599</t>
+      <c r="M41" t="n">
+        <v>3599</v>
+      </c>
+      <c r="N41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>3632</t>
         </is>
       </c>
     </row>
@@ -2460,9 +2710,15 @@
       <c r="L42" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="M42" t="inlineStr">
-        <is>
-          <t>4155</t>
+      <c r="M42" t="n">
+        <v>4155</v>
+      </c>
+      <c r="N42" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>4516</t>
         </is>
       </c>
     </row>
@@ -2509,9 +2765,15 @@
       <c r="L43" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M43" t="inlineStr">
-        <is>
-          <t>3882</t>
+      <c r="M43" t="n">
+        <v>3882</v>
+      </c>
+      <c r="N43" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>4128</t>
         </is>
       </c>
     </row>
@@ -2558,9 +2820,15 @@
       <c r="L44" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="M44" t="inlineStr">
-        <is>
-          <t>3882</t>
+      <c r="M44" t="n">
+        <v>3882</v>
+      </c>
+      <c r="N44" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>4251</t>
         </is>
       </c>
     </row>
@@ -2607,9 +2875,15 @@
       <c r="L45" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M45" t="inlineStr">
-        <is>
-          <t>3763</t>
+      <c r="M45" t="n">
+        <v>3763</v>
+      </c>
+      <c r="N45" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>3916</t>
         </is>
       </c>
     </row>
@@ -2656,9 +2930,15 @@
       <c r="L46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M46" t="inlineStr">
-        <is>
-          <t>3684</t>
+      <c r="M46" t="n">
+        <v>3684</v>
+      </c>
+      <c r="N46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>3906</t>
         </is>
       </c>
     </row>
@@ -2705,7 +2985,13 @@
       <c r="L47" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M47" t="inlineStr">
+      <c r="M47" t="n">
+        <v>2500</v>
+      </c>
+      <c r="N47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O47" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2730,7 +3016,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F48" s="4" t="n">
@@ -2754,9 +3040,15 @@
       <c r="L48" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="M48" t="inlineStr">
-        <is>
-          <t>3989</t>
+      <c r="M48" t="n">
+        <v>3989</v>
+      </c>
+      <c r="N48" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>4383</t>
         </is>
       </c>
     </row>
@@ -2803,9 +3095,15 @@
       <c r="L49" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M49" t="inlineStr">
-        <is>
-          <t>3263</t>
+      <c r="M49" t="n">
+        <v>3263</v>
+      </c>
+      <c r="N49" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>3452</t>
         </is>
       </c>
     </row>
@@ -2852,9 +3150,15 @@
       <c r="L50" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="M50" t="inlineStr">
-        <is>
-          <t>4137</t>
+      <c r="M50" t="n">
+        <v>4137</v>
+      </c>
+      <c r="N50" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>4419</t>
         </is>
       </c>
     </row>
@@ -2901,9 +3205,15 @@
       <c r="L51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M51" t="inlineStr">
-        <is>
-          <t>2757</t>
+      <c r="M51" t="n">
+        <v>2757</v>
+      </c>
+      <c r="N51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>2786</t>
         </is>
       </c>
     </row>
@@ -2950,9 +3260,15 @@
       <c r="L52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M52" t="inlineStr">
-        <is>
-          <t>2498</t>
+      <c r="M52" t="n">
+        <v>2498</v>
+      </c>
+      <c r="N52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>2511</t>
         </is>
       </c>
     </row>
@@ -2999,7 +3315,13 @@
       <c r="L53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M53" t="inlineStr">
+      <c r="M53" t="n">
+        <v>2584</v>
+      </c>
+      <c r="N53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O53" t="inlineStr">
         <is>
           <t>2584</t>
         </is>
@@ -3048,9 +3370,15 @@
       <c r="L54" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="M54" t="inlineStr">
-        <is>
-          <t>3834</t>
+      <c r="M54" t="n">
+        <v>3834</v>
+      </c>
+      <c r="N54" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>4151</t>
         </is>
       </c>
     </row>
@@ -3097,9 +3425,15 @@
       <c r="L55" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="M55" t="inlineStr">
-        <is>
-          <t>3259</t>
+      <c r="M55" t="n">
+        <v>3259</v>
+      </c>
+      <c r="N55" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>3434</t>
         </is>
       </c>
     </row>
@@ -3146,9 +3480,15 @@
       <c r="L56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M56" t="inlineStr">
-        <is>
-          <t>3289</t>
+      <c r="M56" t="n">
+        <v>3289</v>
+      </c>
+      <c r="N56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>3400</t>
         </is>
       </c>
     </row>
@@ -3195,9 +3535,15 @@
       <c r="L57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M57" t="inlineStr">
-        <is>
-          <t>3639</t>
+      <c r="M57" t="n">
+        <v>3639</v>
+      </c>
+      <c r="N57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>3892</t>
         </is>
       </c>
     </row>
@@ -3244,9 +3590,15 @@
       <c r="L58" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="M58" t="inlineStr">
-        <is>
-          <t>3263</t>
+      <c r="M58" t="n">
+        <v>3263</v>
+      </c>
+      <c r="N58" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>3383</t>
         </is>
       </c>
     </row>
@@ -3276,6 +3628,8 @@
       <c r="K59" t="inlineStr"/>
       <c r="L59" s="3" t="inlineStr"/>
       <c r="M59" t="inlineStr"/>
+      <c r="N59" s="3" t="inlineStr"/>
+      <c r="O59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -3303,6 +3657,8 @@
       <c r="K60" t="inlineStr"/>
       <c r="L60" s="3" t="inlineStr"/>
       <c r="M60" t="inlineStr"/>
+      <c r="N60" s="3" t="inlineStr"/>
+      <c r="O60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -3347,9 +3703,15 @@
       <c r="L61" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M61" t="inlineStr">
-        <is>
-          <t>3660</t>
+      <c r="M61" t="n">
+        <v>3660</v>
+      </c>
+      <c r="N61" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>3855</t>
         </is>
       </c>
     </row>
@@ -3396,7 +3758,13 @@
       <c r="L62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M62" t="inlineStr">
+      <c r="M62" t="n">
+        <v>0</v>
+      </c>
+      <c r="N62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3445,9 +3813,15 @@
       <c r="L63" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="M63" t="inlineStr">
-        <is>
-          <t>3743</t>
+      <c r="M63" t="n">
+        <v>3743</v>
+      </c>
+      <c r="N63" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>3965</t>
         </is>
       </c>
     </row>
@@ -3494,9 +3868,15 @@
       <c r="L64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M64" t="inlineStr">
-        <is>
-          <t>2518</t>
+      <c r="M64" t="n">
+        <v>2518</v>
+      </c>
+      <c r="N64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>2533</t>
         </is>
       </c>
     </row>
@@ -3526,6 +3906,8 @@
       <c r="K65" t="inlineStr"/>
       <c r="L65" s="3" t="inlineStr"/>
       <c r="M65" t="inlineStr"/>
+      <c r="N65" s="3" t="inlineStr"/>
+      <c r="O65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -3570,9 +3952,15 @@
       <c r="L66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M66" t="inlineStr">
-        <is>
-          <t>2422</t>
+      <c r="M66" t="n">
+        <v>2422</v>
+      </c>
+      <c r="N66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>2409</t>
         </is>
       </c>
     </row>
@@ -3619,9 +4007,15 @@
       <c r="L67" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M67" t="inlineStr">
-        <is>
-          <t>3488</t>
+      <c r="M67" t="n">
+        <v>3488</v>
+      </c>
+      <c r="N67" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>3659</t>
         </is>
       </c>
     </row>
@@ -3644,7 +4038,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F68" s="4" t="n">
@@ -3668,9 +4062,15 @@
       <c r="L68" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M68" t="inlineStr">
-        <is>
-          <t>3923</t>
+      <c r="M68" t="n">
+        <v>3923</v>
+      </c>
+      <c r="N68" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>4106</t>
         </is>
       </c>
     </row>
@@ -3717,9 +4117,15 @@
       <c r="L69" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M69" t="inlineStr">
-        <is>
-          <t>3334</t>
+      <c r="M69" t="n">
+        <v>3334</v>
+      </c>
+      <c r="N69" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>3535</t>
         </is>
       </c>
     </row>
@@ -3766,9 +4172,15 @@
       <c r="L70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M70" t="inlineStr">
-        <is>
-          <t>2595</t>
+      <c r="M70" t="n">
+        <v>2595</v>
+      </c>
+      <c r="N70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O70" t="inlineStr">
+        <is>
+          <t>2625</t>
         </is>
       </c>
     </row>
@@ -3815,9 +4227,15 @@
       <c r="L71" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M71" t="inlineStr">
-        <is>
-          <t>3287</t>
+      <c r="M71" t="n">
+        <v>3287</v>
+      </c>
+      <c r="N71" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>3519</t>
         </is>
       </c>
     </row>
@@ -3864,9 +4282,15 @@
       <c r="L72" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="M72" t="inlineStr">
-        <is>
-          <t>2863</t>
+      <c r="M72" t="n">
+        <v>2863</v>
+      </c>
+      <c r="N72" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>2896</t>
         </is>
       </c>
     </row>
@@ -3913,9 +4337,15 @@
       <c r="L73" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M73" t="inlineStr">
-        <is>
-          <t>3308</t>
+      <c r="M73" t="n">
+        <v>3308</v>
+      </c>
+      <c r="N73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>3445</t>
         </is>
       </c>
     </row>
@@ -3962,9 +4392,15 @@
       <c r="L74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M74" t="inlineStr">
-        <is>
-          <t>2590</t>
+      <c r="M74" t="n">
+        <v>2590</v>
+      </c>
+      <c r="N74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>2618</t>
         </is>
       </c>
     </row>
@@ -4011,9 +4447,15 @@
       <c r="L75" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="M75" t="inlineStr">
-        <is>
-          <t>3182</t>
+      <c r="M75" t="n">
+        <v>3182</v>
+      </c>
+      <c r="N75" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>3350</t>
         </is>
       </c>
     </row>
@@ -4060,9 +4502,15 @@
       <c r="L76" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M76" t="inlineStr">
-        <is>
-          <t>3486</t>
+      <c r="M76" t="n">
+        <v>3486</v>
+      </c>
+      <c r="N76" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>3769</t>
         </is>
       </c>
     </row>
@@ -4109,9 +4557,15 @@
       <c r="L77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M77" t="inlineStr">
-        <is>
-          <t>3335</t>
+      <c r="M77" t="n">
+        <v>3335</v>
+      </c>
+      <c r="N77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>3323</t>
         </is>
       </c>
     </row>
@@ -4158,9 +4612,15 @@
       <c r="L78" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M78" t="inlineStr">
-        <is>
-          <t>3717</t>
+      <c r="M78" t="n">
+        <v>3717</v>
+      </c>
+      <c r="N78" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>3953</t>
         </is>
       </c>
     </row>
@@ -4207,7 +4667,13 @@
       <c r="L79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M79" t="inlineStr">
+      <c r="M79" t="n">
+        <v>0</v>
+      </c>
+      <c r="N79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4256,9 +4722,15 @@
       <c r="L80" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M80" t="inlineStr">
-        <is>
-          <t>3524</t>
+      <c r="M80" t="n">
+        <v>3524</v>
+      </c>
+      <c r="N80" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>3721</t>
         </is>
       </c>
     </row>
@@ -4305,9 +4777,15 @@
       <c r="L81" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="M81" t="inlineStr">
-        <is>
-          <t>3574</t>
+      <c r="M81" t="n">
+        <v>3574</v>
+      </c>
+      <c r="N81" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>3858</t>
         </is>
       </c>
     </row>
@@ -4354,9 +4832,15 @@
       <c r="L82" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="M82" t="inlineStr">
-        <is>
-          <t>3381</t>
+      <c r="M82" t="n">
+        <v>3381</v>
+      </c>
+      <c r="N82" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>3637</t>
         </is>
       </c>
     </row>
@@ -4403,9 +4887,15 @@
       <c r="L83" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M83" t="inlineStr">
-        <is>
-          <t>3265</t>
+      <c r="M83" t="n">
+        <v>3265</v>
+      </c>
+      <c r="N83" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>3432</t>
         </is>
       </c>
     </row>
@@ -4452,9 +4942,15 @@
       <c r="L84" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="M84" t="inlineStr">
-        <is>
-          <t>2758</t>
+      <c r="M84" t="n">
+        <v>2758</v>
+      </c>
+      <c r="N84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>2785</t>
         </is>
       </c>
     </row>
@@ -4501,9 +4997,15 @@
       <c r="L85" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M85" t="inlineStr">
-        <is>
-          <t>2998</t>
+      <c r="M85" t="n">
+        <v>2998</v>
+      </c>
+      <c r="N85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>3003</t>
         </is>
       </c>
     </row>
@@ -4550,9 +5052,15 @@
       <c r="L86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M86" t="inlineStr">
-        <is>
-          <t>2717</t>
+      <c r="M86" t="n">
+        <v>2717</v>
+      </c>
+      <c r="N86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>2750</t>
         </is>
       </c>
     </row>
@@ -4599,9 +5107,15 @@
       <c r="L87" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M87" t="inlineStr">
-        <is>
-          <t>3492</t>
+      <c r="M87" t="n">
+        <v>3492</v>
+      </c>
+      <c r="N87" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>3816</t>
         </is>
       </c>
     </row>
@@ -4648,9 +5162,15 @@
       <c r="L88" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M88" t="inlineStr">
-        <is>
-          <t>2721</t>
+      <c r="M88" t="n">
+        <v>2721</v>
+      </c>
+      <c r="N88" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>2789</t>
         </is>
       </c>
     </row>
@@ -4697,9 +5217,15 @@
       <c r="L89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M89" t="inlineStr">
-        <is>
-          <t>2581</t>
+      <c r="M89" t="n">
+        <v>2581</v>
+      </c>
+      <c r="N89" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>2790</t>
         </is>
       </c>
     </row>
@@ -4746,9 +5272,15 @@
       <c r="L90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M90" t="inlineStr">
-        <is>
-          <t>2408</t>
+      <c r="M90" t="n">
+        <v>2408</v>
+      </c>
+      <c r="N90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>2390</t>
         </is>
       </c>
     </row>
@@ -4795,9 +5327,15 @@
       <c r="L91" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M91" t="inlineStr">
-        <is>
-          <t>2646</t>
+      <c r="M91" t="n">
+        <v>2646</v>
+      </c>
+      <c r="N91" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>2672</t>
         </is>
       </c>
     </row>
@@ -4844,7 +5382,13 @@
       <c r="L92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M92" t="inlineStr">
+      <c r="M92" t="n">
+        <v>0</v>
+      </c>
+      <c r="N92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4893,9 +5437,15 @@
       <c r="L93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M93" t="inlineStr">
-        <is>
-          <t>2454</t>
+      <c r="M93" t="n">
+        <v>2454</v>
+      </c>
+      <c r="N93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O93" t="inlineStr">
+        <is>
+          <t>2441</t>
         </is>
       </c>
     </row>
@@ -4942,9 +5492,15 @@
       <c r="L94" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M94" t="inlineStr">
-        <is>
-          <t>2882</t>
+      <c r="M94" t="n">
+        <v>2882</v>
+      </c>
+      <c r="N94" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O94" t="inlineStr">
+        <is>
+          <t>2948</t>
         </is>
       </c>
     </row>
@@ -4991,9 +5547,15 @@
       <c r="L95" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="M95" t="inlineStr">
-        <is>
-          <t>2645</t>
+      <c r="M95" t="n">
+        <v>2645</v>
+      </c>
+      <c r="N95" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>2729</t>
         </is>
       </c>
     </row>
@@ -5040,9 +5602,15 @@
       <c r="L96" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M96" t="inlineStr">
-        <is>
-          <t>2927</t>
+      <c r="M96" t="n">
+        <v>2927</v>
+      </c>
+      <c r="N96" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O96" t="inlineStr">
+        <is>
+          <t>3147</t>
         </is>
       </c>
     </row>
@@ -5089,9 +5657,15 @@
       <c r="L97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M97" t="inlineStr">
-        <is>
-          <t>2495</t>
+      <c r="M97" t="n">
+        <v>2495</v>
+      </c>
+      <c r="N97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O97" t="inlineStr">
+        <is>
+          <t>2519</t>
         </is>
       </c>
     </row>
@@ -5138,7 +5712,13 @@
       <c r="L98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M98" t="inlineStr">
+      <c r="M98" t="n">
+        <v>0</v>
+      </c>
+      <c r="N98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5187,9 +5767,15 @@
       <c r="L99" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="M99" t="inlineStr">
-        <is>
-          <t>2903</t>
+      <c r="M99" t="n">
+        <v>2903</v>
+      </c>
+      <c r="N99" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O99" t="inlineStr">
+        <is>
+          <t>3120</t>
         </is>
       </c>
     </row>
@@ -5236,9 +5822,15 @@
       <c r="L100" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="M100" t="inlineStr">
-        <is>
-          <t>2435</t>
+      <c r="M100" t="n">
+        <v>2435</v>
+      </c>
+      <c r="N100" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="O100" t="inlineStr">
+        <is>
+          <t>2453</t>
         </is>
       </c>
     </row>
@@ -5285,9 +5877,15 @@
       <c r="L101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M101" t="inlineStr">
-        <is>
-          <t>3454</t>
+      <c r="M101" t="n">
+        <v>3454</v>
+      </c>
+      <c r="N101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O101" t="inlineStr">
+        <is>
+          <t>3640</t>
         </is>
       </c>
     </row>
@@ -5334,9 +5932,15 @@
       <c r="L102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M102" t="inlineStr">
-        <is>
-          <t>3222</t>
+      <c r="M102" t="n">
+        <v>3222</v>
+      </c>
+      <c r="N102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O102" t="inlineStr">
+        <is>
+          <t>3322</t>
         </is>
       </c>
     </row>
@@ -5383,9 +5987,15 @@
       <c r="L103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M103" t="inlineStr">
-        <is>
-          <t>2523</t>
+      <c r="M103" t="n">
+        <v>2523</v>
+      </c>
+      <c r="N103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O103" t="inlineStr">
+        <is>
+          <t>2518</t>
         </is>
       </c>
     </row>
@@ -5432,9 +6042,15 @@
       <c r="L104" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="M104" t="inlineStr">
-        <is>
-          <t>3468</t>
+      <c r="M104" t="n">
+        <v>3468</v>
+      </c>
+      <c r="N104" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O104" t="inlineStr">
+        <is>
+          <t>3627</t>
         </is>
       </c>
     </row>
@@ -5481,9 +6097,15 @@
       <c r="L105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M105" t="inlineStr">
-        <is>
-          <t>3104</t>
+      <c r="M105" t="n">
+        <v>3104</v>
+      </c>
+      <c r="N105" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="O105" t="inlineStr">
+        <is>
+          <t>3398</t>
         </is>
       </c>
     </row>
@@ -5530,7 +6152,13 @@
       <c r="L106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M106" t="inlineStr">
+      <c r="M106" t="n">
+        <v>0</v>
+      </c>
+      <c r="N106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5579,9 +6207,15 @@
       <c r="L107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M107" t="inlineStr">
-        <is>
-          <t>2513</t>
+      <c r="M107" t="n">
+        <v>2513</v>
+      </c>
+      <c r="N107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O107" t="inlineStr">
+        <is>
+          <t>2479</t>
         </is>
       </c>
     </row>
@@ -5628,7 +6262,13 @@
       <c r="L108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M108" t="inlineStr">
+      <c r="M108" t="n">
+        <v>0</v>
+      </c>
+      <c r="N108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5677,9 +6317,15 @@
       <c r="L109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M109" t="inlineStr">
-        <is>
-          <t>2976</t>
+      <c r="M109" t="n">
+        <v>2976</v>
+      </c>
+      <c r="N109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O109" t="inlineStr">
+        <is>
+          <t>3055</t>
         </is>
       </c>
     </row>
@@ -5726,9 +6372,15 @@
       <c r="L110" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M110" t="inlineStr">
-        <is>
-          <t>2995</t>
+      <c r="M110" t="n">
+        <v>2995</v>
+      </c>
+      <c r="N110" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="O110" t="inlineStr">
+        <is>
+          <t>3188</t>
         </is>
       </c>
     </row>
@@ -5775,9 +6427,15 @@
       <c r="L111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M111" t="inlineStr">
-        <is>
-          <t>2607</t>
+      <c r="M111" t="n">
+        <v>2607</v>
+      </c>
+      <c r="N111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O111" t="inlineStr">
+        <is>
+          <t>2590</t>
         </is>
       </c>
     </row>
@@ -5824,9 +6482,15 @@
       <c r="L112" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="M112" t="inlineStr">
-        <is>
-          <t>2814</t>
+      <c r="M112" t="n">
+        <v>2814</v>
+      </c>
+      <c r="N112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O112" t="inlineStr">
+        <is>
+          <t>2787</t>
         </is>
       </c>
     </row>
@@ -5873,9 +6537,15 @@
       <c r="L113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M113" t="inlineStr">
-        <is>
-          <t>2732</t>
+      <c r="M113" t="n">
+        <v>2732</v>
+      </c>
+      <c r="N113" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="O113" t="inlineStr">
+        <is>
+          <t>2891</t>
         </is>
       </c>
     </row>
@@ -5922,9 +6592,15 @@
       <c r="L114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M114" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M114" t="n">
+        <v>0</v>
+      </c>
+      <c r="N114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O114" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -5971,9 +6647,15 @@
       <c r="L115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M115" t="inlineStr">
-        <is>
-          <t>2440</t>
+      <c r="M115" t="n">
+        <v>2440</v>
+      </c>
+      <c r="N115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O115" t="inlineStr">
+        <is>
+          <t>2416</t>
         </is>
       </c>
     </row>
@@ -6020,9 +6702,15 @@
       <c r="L116" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="M116" t="inlineStr">
-        <is>
-          <t>2721</t>
+      <c r="M116" t="n">
+        <v>2721</v>
+      </c>
+      <c r="N116" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="O116" t="inlineStr">
+        <is>
+          <t>2891</t>
         </is>
       </c>
     </row>
@@ -6069,9 +6757,15 @@
       <c r="L117" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="M117" t="inlineStr">
-        <is>
-          <t>3065</t>
+      <c r="M117" t="n">
+        <v>3065</v>
+      </c>
+      <c r="N117" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="O117" t="inlineStr">
+        <is>
+          <t>3142</t>
         </is>
       </c>
     </row>
@@ -6118,7 +6812,13 @@
       <c r="L118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M118" t="inlineStr">
+      <c r="M118" t="n">
+        <v>0</v>
+      </c>
+      <c r="N118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6167,9 +6867,15 @@
       <c r="L119" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M119" t="inlineStr">
-        <is>
-          <t>3090</t>
+      <c r="M119" t="n">
+        <v>3090</v>
+      </c>
+      <c r="N119" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O119" t="inlineStr">
+        <is>
+          <t>3176</t>
         </is>
       </c>
     </row>
@@ -6216,9 +6922,15 @@
       <c r="L120" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="M120" t="inlineStr">
-        <is>
-          <t>2449</t>
+      <c r="M120" t="n">
+        <v>2449</v>
+      </c>
+      <c r="N120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O120" t="inlineStr">
+        <is>
+          <t>2443</t>
         </is>
       </c>
     </row>
@@ -6265,9 +6977,15 @@
       <c r="L121" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="M121" t="inlineStr">
-        <is>
-          <t>2875</t>
+      <c r="M121" t="n">
+        <v>2875</v>
+      </c>
+      <c r="N121" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="O121" t="inlineStr">
+        <is>
+          <t>3033</t>
         </is>
       </c>
     </row>
@@ -6314,7 +7032,13 @@
       <c r="L122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M122" t="inlineStr">
+      <c r="M122" t="n">
+        <v>0</v>
+      </c>
+      <c r="N122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6363,9 +7087,15 @@
       <c r="L123" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M123" t="inlineStr">
-        <is>
-          <t>2866</t>
+      <c r="M123" t="n">
+        <v>2866</v>
+      </c>
+      <c r="N123" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="O123" t="inlineStr">
+        <is>
+          <t>2871</t>
         </is>
       </c>
     </row>
@@ -6412,9 +7142,15 @@
       <c r="L124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M124" t="inlineStr">
-        <is>
-          <t>2857</t>
+      <c r="M124" t="n">
+        <v>2857</v>
+      </c>
+      <c r="N124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O124" t="inlineStr">
+        <is>
+          <t>2850</t>
         </is>
       </c>
     </row>
@@ -6461,9 +7197,15 @@
       <c r="L125" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M125" t="inlineStr">
-        <is>
-          <t>2997</t>
+      <c r="M125" t="n">
+        <v>2997</v>
+      </c>
+      <c r="N125" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="O125" t="inlineStr">
+        <is>
+          <t>3135</t>
         </is>
       </c>
     </row>
@@ -6510,9 +7252,15 @@
       <c r="L126" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M126" t="inlineStr">
-        <is>
-          <t>2823</t>
+      <c r="M126" t="n">
+        <v>2823</v>
+      </c>
+      <c r="N126" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O126" t="inlineStr">
+        <is>
+          <t>2954</t>
         </is>
       </c>
     </row>
@@ -6559,9 +7307,15 @@
       <c r="L127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M127" t="inlineStr">
-        <is>
-          <t>2415</t>
+      <c r="M127" t="n">
+        <v>2415</v>
+      </c>
+      <c r="N127" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O127" t="inlineStr">
+        <is>
+          <t>2412</t>
         </is>
       </c>
     </row>
@@ -6608,7 +7362,13 @@
       <c r="L128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M128" t="inlineStr">
+      <c r="M128" t="n">
+        <v>0</v>
+      </c>
+      <c r="N128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6657,7 +7417,13 @@
       <c r="L129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M129" t="inlineStr">
+      <c r="M129" t="n">
+        <v>0</v>
+      </c>
+      <c r="N129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6706,9 +7472,15 @@
       <c r="L130" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="M130" t="inlineStr">
-        <is>
-          <t>2600</t>
+      <c r="M130" t="n">
+        <v>2600</v>
+      </c>
+      <c r="N130" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="O130" t="inlineStr">
+        <is>
+          <t>2683</t>
         </is>
       </c>
     </row>
@@ -6755,9 +7527,15 @@
       <c r="L131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M131" t="inlineStr">
-        <is>
-          <t>2439</t>
+      <c r="M131" t="n">
+        <v>2439</v>
+      </c>
+      <c r="N131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O131" t="inlineStr">
+        <is>
+          <t>2429</t>
         </is>
       </c>
     </row>
@@ -6804,9 +7582,15 @@
       <c r="L132" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M132" t="inlineStr">
-        <is>
-          <t>2442</t>
+      <c r="M132" t="n">
+        <v>2442</v>
+      </c>
+      <c r="N132" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O132" t="inlineStr">
+        <is>
+          <t>2410</t>
         </is>
       </c>
     </row>
@@ -6853,9 +7637,15 @@
       <c r="L133" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="M133" t="inlineStr">
-        <is>
-          <t>2755</t>
+      <c r="M133" t="n">
+        <v>2755</v>
+      </c>
+      <c r="N133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O133" t="inlineStr">
+        <is>
+          <t>2742</t>
         </is>
       </c>
     </row>
@@ -6902,9 +7692,15 @@
       <c r="L134" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="M134" t="inlineStr">
-        <is>
-          <t>1668</t>
+      <c r="M134" t="n">
+        <v>1668</v>
+      </c>
+      <c r="N134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O134" t="inlineStr">
+        <is>
+          <t>1693</t>
         </is>
       </c>
     </row>
@@ -6950,6 +7746,8 @@
       </c>
       <c r="L135" s="3" t="inlineStr"/>
       <c r="M135" t="inlineStr"/>
+      <c r="N135" s="3" t="inlineStr"/>
+      <c r="O135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -6994,9 +7792,15 @@
       <c r="L136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M136" t="inlineStr">
-        <is>
-          <t>2601</t>
+      <c r="M136" t="n">
+        <v>2601</v>
+      </c>
+      <c r="N136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O136" t="inlineStr">
+        <is>
+          <t>2607</t>
         </is>
       </c>
     </row>
@@ -7043,7 +7847,13 @@
       <c r="L137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M137" t="inlineStr">
+      <c r="M137" t="n">
+        <v>0</v>
+      </c>
+      <c r="N137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7091,6 +7901,8 @@
       </c>
       <c r="L138" s="3" t="inlineStr"/>
       <c r="M138" t="inlineStr"/>
+      <c r="N138" s="3" t="inlineStr"/>
+      <c r="O138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -7135,9 +7947,15 @@
       <c r="L139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M139" t="inlineStr">
-        <is>
-          <t>2410</t>
+      <c r="M139" t="n">
+        <v>2410</v>
+      </c>
+      <c r="N139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O139" t="inlineStr">
+        <is>
+          <t>2390</t>
         </is>
       </c>
     </row>
@@ -7184,9 +8002,15 @@
       <c r="L140" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M140" t="inlineStr">
-        <is>
-          <t>2663</t>
+      <c r="M140" t="n">
+        <v>2663</v>
+      </c>
+      <c r="N140" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O140" t="inlineStr">
+        <is>
+          <t>2677</t>
         </is>
       </c>
     </row>
@@ -7232,6 +8056,8 @@
       </c>
       <c r="L141" s="3" t="inlineStr"/>
       <c r="M141" t="inlineStr"/>
+      <c r="N141" s="3" t="inlineStr"/>
+      <c r="O141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -7276,9 +8102,15 @@
       <c r="L142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M142" t="inlineStr">
-        <is>
-          <t>2000</t>
+      <c r="M142" t="n">
+        <v>2000</v>
+      </c>
+      <c r="N142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O142" t="inlineStr">
+        <is>
+          <t>2034</t>
         </is>
       </c>
     </row>
@@ -7324,6 +8156,8 @@
       </c>
       <c r="L143" s="3" t="inlineStr"/>
       <c r="M143" t="inlineStr"/>
+      <c r="N143" s="3" t="inlineStr"/>
+      <c r="O143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -7367,6 +8201,8 @@
       </c>
       <c r="L144" s="3" t="inlineStr"/>
       <c r="M144" t="inlineStr"/>
+      <c r="N144" s="3" t="inlineStr"/>
+      <c r="O144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -7410,6 +8246,8 @@
       </c>
       <c r="L145" s="3" t="inlineStr"/>
       <c r="M145" t="inlineStr"/>
+      <c r="N145" s="3" t="inlineStr"/>
+      <c r="O145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -7453,6 +8291,8 @@
       </c>
       <c r="L146" s="3" t="inlineStr"/>
       <c r="M146" t="inlineStr"/>
+      <c r="N146" s="3" t="inlineStr"/>
+      <c r="O146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -7496,6 +8336,8 @@
       </c>
       <c r="L147" s="3" t="inlineStr"/>
       <c r="M147" t="inlineStr"/>
+      <c r="N147" s="3" t="inlineStr"/>
+      <c r="O147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -7540,9 +8382,15 @@
       <c r="L148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M148" t="inlineStr">
-        <is>
-          <t>1500</t>
+      <c r="M148" t="n">
+        <v>1500</v>
+      </c>
+      <c r="N148" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="O148" t="inlineStr">
+        <is>
+          <t>1530</t>
         </is>
       </c>
     </row>
@@ -7589,9 +8437,15 @@
       <c r="L149" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="M149" t="inlineStr">
-        <is>
-          <t>2578</t>
+      <c r="M149" t="n">
+        <v>2578</v>
+      </c>
+      <c r="N149" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="O149" t="inlineStr">
+        <is>
+          <t>2685</t>
         </is>
       </c>
     </row>
@@ -7638,7 +8492,13 @@
       <c r="L150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M150" t="inlineStr">
+      <c r="M150" t="n">
+        <v>0</v>
+      </c>
+      <c r="N150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7687,7 +8547,13 @@
       <c r="L151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M151" t="inlineStr">
+      <c r="M151" t="n">
+        <v>0</v>
+      </c>
+      <c r="N151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7736,7 +8602,13 @@
       <c r="L152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M152" t="inlineStr">
+      <c r="M152" t="n">
+        <v>0</v>
+      </c>
+      <c r="N152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7785,7 +8657,13 @@
       <c r="L153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M153" t="inlineStr">
+      <c r="M153" t="n">
+        <v>0</v>
+      </c>
+      <c r="N153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7834,7 +8712,13 @@
       <c r="L154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M154" t="inlineStr">
+      <c r="M154" t="n">
+        <v>0</v>
+      </c>
+      <c r="N154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7883,7 +8767,13 @@
       <c r="L155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M155" t="inlineStr">
+      <c r="M155" t="n">
+        <v>0</v>
+      </c>
+      <c r="N155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O155" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7926,9 +8816,15 @@
       <c r="L156" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M156" t="inlineStr">
-        <is>
-          <t>2994</t>
+      <c r="M156" t="n">
+        <v>2994</v>
+      </c>
+      <c r="N156" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="O156" t="inlineStr">
+        <is>
+          <t>3068</t>
         </is>
       </c>
     </row>
@@ -7968,6 +8864,8 @@
       </c>
       <c r="L157" s="3" t="inlineStr"/>
       <c r="M157" t="inlineStr"/>
+      <c r="N157" s="3" t="inlineStr"/>
+      <c r="O157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -8006,7 +8904,13 @@
       <c r="L158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M158" t="inlineStr">
+      <c r="M158" t="n">
+        <v>0</v>
+      </c>
+      <c r="N158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8049,9 +8953,15 @@
       <c r="L159" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M159" t="inlineStr">
-        <is>
-          <t>2429</t>
+      <c r="M159" t="n">
+        <v>2429</v>
+      </c>
+      <c r="N159" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O159" t="inlineStr">
+        <is>
+          <t>2499</t>
         </is>
       </c>
     </row>
@@ -8088,17 +8998,15 @@
       <c r="L160" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="M160" t="inlineStr">
-        <is>
-          <t>2184</t>
-        </is>
-      </c>
+      <c r="M160" t="n">
+        <v>2184</v>
+      </c>
+      <c r="N160" s="3" t="inlineStr"/>
+      <c r="O160" t="inlineStr"/>
     </row>
     <row r="161">
-      <c r="A161" t="inlineStr">
-        <is>
-          <t>58743790</t>
-        </is>
+      <c r="A161" t="n">
+        <v>58743790</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>
@@ -8121,17 +9029,21 @@
       <c r="L161" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="M161" t="inlineStr">
-        <is>
-          <t>2502</t>
+      <c r="M161" t="n">
+        <v>2502</v>
+      </c>
+      <c r="N161" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="O161" t="inlineStr">
+        <is>
+          <t>2580</t>
         </is>
       </c>
     </row>
     <row r="162">
-      <c r="A162" t="inlineStr">
-        <is>
-          <t>10636651</t>
-        </is>
+      <c r="A162" t="n">
+        <v>10636651</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>
@@ -8154,9 +9066,50 @@
       <c r="L162" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M162" t="inlineStr">
-        <is>
-          <t>2317</t>
+      <c r="M162" t="n">
+        <v>2317</v>
+      </c>
+      <c r="N162" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="O162" t="inlineStr">
+        <is>
+          <t>2382</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>47244896</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Dropthebeat</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr"/>
+      <c r="D163" t="inlineStr"/>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F163" s="3" t="inlineStr"/>
+      <c r="G163" t="inlineStr"/>
+      <c r="H163" s="3" t="inlineStr"/>
+      <c r="I163" t="inlineStr"/>
+      <c r="J163" s="3" t="inlineStr"/>
+      <c r="K163" t="inlineStr"/>
+      <c r="L163" s="3" t="inlineStr"/>
+      <c r="M163" t="inlineStr"/>
+      <c r="N163" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O163" t="inlineStr">
+        <is>
+          <t>2712</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-02-18 13:20:59
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O163"/>
+  <dimension ref="A1:Q163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,6 +466,16 @@
           <t>02-16_0</t>
         </is>
       </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>02-17_A</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>02-17_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -516,9 +526,15 @@
       <c r="N2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>2962</t>
+      <c r="O2" t="n">
+        <v>2962</v>
+      </c>
+      <c r="P2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>3046</t>
         </is>
       </c>
     </row>
@@ -571,9 +587,15 @@
       <c r="N3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>3789</t>
+      <c r="O3" t="n">
+        <v>3789</v>
+      </c>
+      <c r="P3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>3977</t>
         </is>
       </c>
     </row>
@@ -626,9 +648,15 @@
       <c r="N4" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>4364</t>
+      <c r="O4" t="n">
+        <v>4364</v>
+      </c>
+      <c r="P4" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>4677</t>
         </is>
       </c>
     </row>
@@ -681,9 +709,15 @@
       <c r="N5" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>3365</t>
+      <c r="O5" t="n">
+        <v>3365</v>
+      </c>
+      <c r="P5" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>3498</t>
         </is>
       </c>
     </row>
@@ -736,9 +770,15 @@
       <c r="N6" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>4052</t>
+      <c r="O6" t="n">
+        <v>4052</v>
+      </c>
+      <c r="P6" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>4388</t>
         </is>
       </c>
     </row>
@@ -791,9 +831,15 @@
       <c r="N7" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>4547</t>
+      <c r="O7" t="n">
+        <v>4547</v>
+      </c>
+      <c r="P7" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>4881</t>
         </is>
       </c>
     </row>
@@ -846,9 +892,15 @@
       <c r="N8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>3784</t>
+      <c r="O8" t="n">
+        <v>3784</v>
+      </c>
+      <c r="P8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>4055</t>
         </is>
       </c>
     </row>
@@ -901,9 +953,15 @@
       <c r="N9" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>3885</t>
+      <c r="O9" t="n">
+        <v>3885</v>
+      </c>
+      <c r="P9" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>4040</t>
         </is>
       </c>
     </row>
@@ -956,9 +1014,15 @@
       <c r="N10" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>3843</t>
+      <c r="O10" t="n">
+        <v>3843</v>
+      </c>
+      <c r="P10" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>4265</t>
         </is>
       </c>
     </row>
@@ -1011,9 +1075,15 @@
       <c r="N11" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>3660</t>
+      <c r="O11" t="n">
+        <v>3660</v>
+      </c>
+      <c r="P11" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>3850</t>
         </is>
       </c>
     </row>
@@ -1066,7 +1136,13 @@
       <c r="N12" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="O12" t="inlineStr">
+      <c r="O12" t="n">
+        <v>2835</v>
+      </c>
+      <c r="P12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="inlineStr">
         <is>
           <t>2835</t>
         </is>
@@ -1121,9 +1197,15 @@
       <c r="N13" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>4544</t>
+      <c r="O13" t="n">
+        <v>4544</v>
+      </c>
+      <c r="P13" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>4925</t>
         </is>
       </c>
     </row>
@@ -1176,9 +1258,15 @@
       <c r="N14" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>3996</t>
+      <c r="O14" t="n">
+        <v>3996</v>
+      </c>
+      <c r="P14" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>4230</t>
         </is>
       </c>
     </row>
@@ -1231,9 +1319,15 @@
       <c r="N15" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>3582</t>
+      <c r="O15" t="n">
+        <v>3582</v>
+      </c>
+      <c r="P15" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>3729</t>
         </is>
       </c>
     </row>
@@ -1286,9 +1380,15 @@
       <c r="N16" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>4073</t>
+      <c r="O16" t="n">
+        <v>4073</v>
+      </c>
+      <c r="P16" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>4308</t>
         </is>
       </c>
     </row>
@@ -1341,9 +1441,15 @@
       <c r="N17" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t>3594</t>
+      <c r="O17" t="n">
+        <v>3594</v>
+      </c>
+      <c r="P17" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>3714</t>
         </is>
       </c>
     </row>
@@ -1396,9 +1502,15 @@
       <c r="N18" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>3603</t>
+      <c r="O18" t="n">
+        <v>3603</v>
+      </c>
+      <c r="P18" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>3789</t>
         </is>
       </c>
     </row>
@@ -1451,9 +1563,15 @@
       <c r="N19" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="O19" t="inlineStr">
-        <is>
-          <t>3954</t>
+      <c r="O19" t="n">
+        <v>3954</v>
+      </c>
+      <c r="P19" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>4254</t>
         </is>
       </c>
     </row>
@@ -1506,9 +1624,15 @@
       <c r="N20" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="O20" t="inlineStr">
-        <is>
-          <t>4637</t>
+      <c r="O20" t="n">
+        <v>4637</v>
+      </c>
+      <c r="P20" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>5090</t>
         </is>
       </c>
     </row>
@@ -1561,9 +1685,15 @@
       <c r="N21" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>3204</t>
+      <c r="O21" t="n">
+        <v>3204</v>
+      </c>
+      <c r="P21" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>3490</t>
         </is>
       </c>
     </row>
@@ -1616,9 +1746,15 @@
       <c r="N22" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="O22" t="inlineStr">
-        <is>
-          <t>4118</t>
+      <c r="O22" t="n">
+        <v>4118</v>
+      </c>
+      <c r="P22" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>4364</t>
         </is>
       </c>
     </row>
@@ -1671,9 +1807,15 @@
       <c r="N23" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>3874</t>
+      <c r="O23" t="n">
+        <v>3874</v>
+      </c>
+      <c r="P23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>3897</t>
         </is>
       </c>
     </row>
@@ -1726,9 +1868,15 @@
       <c r="N24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>4177</t>
+      <c r="O24" t="n">
+        <v>4177</v>
+      </c>
+      <c r="P24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>4389</t>
         </is>
       </c>
     </row>
@@ -1781,7 +1929,13 @@
       <c r="N25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O25" t="inlineStr">
+      <c r="O25" t="n">
+        <v>0</v>
+      </c>
+      <c r="P25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1836,9 +1990,15 @@
       <c r="N26" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="O26" t="inlineStr">
-        <is>
-          <t>4232</t>
+      <c r="O26" t="n">
+        <v>4232</v>
+      </c>
+      <c r="P26" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>4478</t>
         </is>
       </c>
     </row>
@@ -1891,9 +2051,15 @@
       <c r="N27" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="O27" t="inlineStr">
-        <is>
-          <t>4143</t>
+      <c r="O27" t="n">
+        <v>4143</v>
+      </c>
+      <c r="P27" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>4348</t>
         </is>
       </c>
     </row>
@@ -1946,9 +2112,15 @@
       <c r="N28" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="O28" t="inlineStr">
-        <is>
-          <t>3496</t>
+      <c r="O28" t="n">
+        <v>3496</v>
+      </c>
+      <c r="P28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>3663</t>
         </is>
       </c>
     </row>
@@ -2001,9 +2173,15 @@
       <c r="N29" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="O29" t="inlineStr">
-        <is>
-          <t>4693</t>
+      <c r="O29" t="n">
+        <v>4693</v>
+      </c>
+      <c r="P29" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>5046</t>
         </is>
       </c>
     </row>
@@ -2056,9 +2234,15 @@
       <c r="N30" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="O30" t="inlineStr">
-        <is>
-          <t>3712</t>
+      <c r="O30" t="n">
+        <v>3712</v>
+      </c>
+      <c r="P30" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>3889</t>
         </is>
       </c>
     </row>
@@ -2111,9 +2295,15 @@
       <c r="N31" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="O31" t="inlineStr">
-        <is>
-          <t>4605</t>
+      <c r="O31" t="n">
+        <v>4605</v>
+      </c>
+      <c r="P31" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>4682</t>
         </is>
       </c>
     </row>
@@ -2166,9 +2356,15 @@
       <c r="N32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O32" t="inlineStr">
-        <is>
-          <t>3668</t>
+      <c r="O32" t="n">
+        <v>3668</v>
+      </c>
+      <c r="P32" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>3962</t>
         </is>
       </c>
     </row>
@@ -2221,9 +2417,15 @@
       <c r="N33" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="O33" t="inlineStr">
-        <is>
-          <t>4061</t>
+      <c r="O33" t="n">
+        <v>4061</v>
+      </c>
+      <c r="P33" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>4274</t>
         </is>
       </c>
     </row>
@@ -2276,9 +2478,15 @@
       <c r="N34" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O34" t="inlineStr">
-        <is>
-          <t>4109</t>
+      <c r="O34" t="n">
+        <v>4109</v>
+      </c>
+      <c r="P34" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>4263</t>
         </is>
       </c>
     </row>
@@ -2331,9 +2539,15 @@
       <c r="N35" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="O35" t="inlineStr">
-        <is>
-          <t>4020</t>
+      <c r="O35" t="n">
+        <v>4020</v>
+      </c>
+      <c r="P35" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>4320</t>
         </is>
       </c>
     </row>
@@ -2386,9 +2600,15 @@
       <c r="N36" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O36" t="inlineStr">
-        <is>
-          <t>4156</t>
+      <c r="O36" t="n">
+        <v>4156</v>
+      </c>
+      <c r="P36" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>4431</t>
         </is>
       </c>
     </row>
@@ -2441,9 +2661,15 @@
       <c r="N37" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="O37" t="inlineStr">
-        <is>
-          <t>3713</t>
+      <c r="O37" t="n">
+        <v>3713</v>
+      </c>
+      <c r="P37" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>3878</t>
         </is>
       </c>
     </row>
@@ -2496,9 +2722,15 @@
       <c r="N38" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O38" t="inlineStr">
-        <is>
-          <t>4068</t>
+      <c r="O38" t="n">
+        <v>4068</v>
+      </c>
+      <c r="P38" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>4325</t>
         </is>
       </c>
     </row>
@@ -2551,9 +2783,15 @@
       <c r="N39" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="O39" t="inlineStr">
-        <is>
-          <t>4080</t>
+      <c r="O39" t="n">
+        <v>4080</v>
+      </c>
+      <c r="P39" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>4451</t>
         </is>
       </c>
     </row>
@@ -2606,9 +2844,15 @@
       <c r="N40" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="O40" t="inlineStr">
-        <is>
-          <t>4481</t>
+      <c r="O40" t="n">
+        <v>4481</v>
+      </c>
+      <c r="P40" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>4767</t>
         </is>
       </c>
     </row>
@@ -2661,7 +2905,13 @@
       <c r="N41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O41" t="inlineStr">
+      <c r="O41" t="n">
+        <v>3632</v>
+      </c>
+      <c r="P41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q41" t="inlineStr">
         <is>
           <t>3632</t>
         </is>
@@ -2716,9 +2966,15 @@
       <c r="N42" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="O42" t="inlineStr">
-        <is>
-          <t>4516</t>
+      <c r="O42" t="n">
+        <v>4516</v>
+      </c>
+      <c r="P42" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>4744</t>
         </is>
       </c>
     </row>
@@ -2771,9 +3027,15 @@
       <c r="N43" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="O43" t="inlineStr">
-        <is>
-          <t>4128</t>
+      <c r="O43" t="n">
+        <v>4128</v>
+      </c>
+      <c r="P43" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>4465</t>
         </is>
       </c>
     </row>
@@ -2826,9 +3088,15 @@
       <c r="N44" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="O44" t="inlineStr">
-        <is>
-          <t>4251</t>
+      <c r="O44" t="n">
+        <v>4251</v>
+      </c>
+      <c r="P44" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>4573</t>
         </is>
       </c>
     </row>
@@ -2881,9 +3149,15 @@
       <c r="N45" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="O45" t="inlineStr">
-        <is>
-          <t>3916</t>
+      <c r="O45" t="n">
+        <v>3916</v>
+      </c>
+      <c r="P45" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>4112</t>
         </is>
       </c>
     </row>
@@ -2936,9 +3210,15 @@
       <c r="N46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O46" t="inlineStr">
-        <is>
-          <t>3906</t>
+      <c r="O46" t="n">
+        <v>3906</v>
+      </c>
+      <c r="P46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>4085</t>
         </is>
       </c>
     </row>
@@ -2991,7 +3271,13 @@
       <c r="N47" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O47" t="inlineStr">
+      <c r="O47" t="n">
+        <v>2500</v>
+      </c>
+      <c r="P47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q47" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -3046,9 +3332,15 @@
       <c r="N48" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="O48" t="inlineStr">
-        <is>
-          <t>4383</t>
+      <c r="O48" t="n">
+        <v>4383</v>
+      </c>
+      <c r="P48" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>4674</t>
         </is>
       </c>
     </row>
@@ -3101,9 +3393,15 @@
       <c r="N49" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="O49" t="inlineStr">
-        <is>
-          <t>3452</t>
+      <c r="O49" t="n">
+        <v>3452</v>
+      </c>
+      <c r="P49" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>3599</t>
         </is>
       </c>
     </row>
@@ -3156,9 +3454,15 @@
       <c r="N50" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="O50" t="inlineStr">
-        <is>
-          <t>4419</t>
+      <c r="O50" t="n">
+        <v>4419</v>
+      </c>
+      <c r="P50" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>4800</t>
         </is>
       </c>
     </row>
@@ -3211,9 +3515,15 @@
       <c r="N51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O51" t="inlineStr">
-        <is>
-          <t>2786</t>
+      <c r="O51" t="n">
+        <v>2786</v>
+      </c>
+      <c r="P51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>2835</t>
         </is>
       </c>
     </row>
@@ -3266,9 +3576,15 @@
       <c r="N52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O52" t="inlineStr">
-        <is>
-          <t>2511</t>
+      <c r="O52" t="n">
+        <v>2511</v>
+      </c>
+      <c r="P52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q52" t="inlineStr">
+        <is>
+          <t>2526</t>
         </is>
       </c>
     </row>
@@ -3321,9 +3637,15 @@
       <c r="N53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O53" t="inlineStr">
-        <is>
-          <t>2584</t>
+      <c r="O53" t="n">
+        <v>2584</v>
+      </c>
+      <c r="P53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>2599</t>
         </is>
       </c>
     </row>
@@ -3376,9 +3698,15 @@
       <c r="N54" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="O54" t="inlineStr">
-        <is>
-          <t>4151</t>
+      <c r="O54" t="n">
+        <v>4151</v>
+      </c>
+      <c r="P54" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>4413</t>
         </is>
       </c>
     </row>
@@ -3431,9 +3759,15 @@
       <c r="N55" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="O55" t="inlineStr">
-        <is>
-          <t>3434</t>
+      <c r="O55" t="n">
+        <v>3434</v>
+      </c>
+      <c r="P55" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>3526</t>
         </is>
       </c>
     </row>
@@ -3486,9 +3820,15 @@
       <c r="N56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O56" t="inlineStr">
-        <is>
-          <t>3400</t>
+      <c r="O56" t="n">
+        <v>3400</v>
+      </c>
+      <c r="P56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>3656</t>
         </is>
       </c>
     </row>
@@ -3541,9 +3881,15 @@
       <c r="N57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O57" t="inlineStr">
-        <is>
-          <t>3892</t>
+      <c r="O57" t="n">
+        <v>3892</v>
+      </c>
+      <c r="P57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q57" t="inlineStr">
+        <is>
+          <t>4156</t>
         </is>
       </c>
     </row>
@@ -3596,9 +3942,15 @@
       <c r="N58" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="O58" t="inlineStr">
-        <is>
-          <t>3383</t>
+      <c r="O58" t="n">
+        <v>3383</v>
+      </c>
+      <c r="P58" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q58" t="inlineStr">
+        <is>
+          <t>3573</t>
         </is>
       </c>
     </row>
@@ -3630,6 +3982,8 @@
       <c r="M59" t="inlineStr"/>
       <c r="N59" s="3" t="inlineStr"/>
       <c r="O59" t="inlineStr"/>
+      <c r="P59" s="3" t="inlineStr"/>
+      <c r="Q59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -3659,6 +4013,8 @@
       <c r="M60" t="inlineStr"/>
       <c r="N60" s="3" t="inlineStr"/>
       <c r="O60" t="inlineStr"/>
+      <c r="P60" s="3" t="inlineStr"/>
+      <c r="Q60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -3709,9 +4065,15 @@
       <c r="N61" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O61" t="inlineStr">
-        <is>
-          <t>3855</t>
+      <c r="O61" t="n">
+        <v>3855</v>
+      </c>
+      <c r="P61" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q61" t="inlineStr">
+        <is>
+          <t>4023</t>
         </is>
       </c>
     </row>
@@ -3764,7 +4126,13 @@
       <c r="N62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O62" t="inlineStr">
+      <c r="O62" t="n">
+        <v>0</v>
+      </c>
+      <c r="P62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3819,9 +4187,15 @@
       <c r="N63" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="O63" t="inlineStr">
-        <is>
-          <t>3965</t>
+      <c r="O63" t="n">
+        <v>3965</v>
+      </c>
+      <c r="P63" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="Q63" t="inlineStr">
+        <is>
+          <t>4150</t>
         </is>
       </c>
     </row>
@@ -3874,7 +4248,13 @@
       <c r="N64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O64" t="inlineStr">
+      <c r="O64" t="n">
+        <v>2533</v>
+      </c>
+      <c r="P64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q64" t="inlineStr">
         <is>
           <t>2533</t>
         </is>
@@ -3908,6 +4288,8 @@
       <c r="M65" t="inlineStr"/>
       <c r="N65" s="3" t="inlineStr"/>
       <c r="O65" t="inlineStr"/>
+      <c r="P65" s="3" t="inlineStr"/>
+      <c r="Q65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -3958,9 +4340,15 @@
       <c r="N66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O66" t="inlineStr">
-        <is>
-          <t>2409</t>
+      <c r="O66" t="n">
+        <v>2409</v>
+      </c>
+      <c r="P66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q66" t="inlineStr">
+        <is>
+          <t>2401</t>
         </is>
       </c>
     </row>
@@ -4013,9 +4401,15 @@
       <c r="N67" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="O67" t="inlineStr">
-        <is>
-          <t>3659</t>
+      <c r="O67" t="n">
+        <v>3659</v>
+      </c>
+      <c r="P67" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q67" t="inlineStr">
+        <is>
+          <t>3906</t>
         </is>
       </c>
     </row>
@@ -4068,9 +4462,15 @@
       <c r="N68" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="O68" t="inlineStr">
-        <is>
-          <t>4106</t>
+      <c r="O68" t="n">
+        <v>4106</v>
+      </c>
+      <c r="P68" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q68" t="inlineStr">
+        <is>
+          <t>4401</t>
         </is>
       </c>
     </row>
@@ -4123,9 +4523,15 @@
       <c r="N69" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="O69" t="inlineStr">
-        <is>
-          <t>3535</t>
+      <c r="O69" t="n">
+        <v>3535</v>
+      </c>
+      <c r="P69" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q69" t="inlineStr">
+        <is>
+          <t>3717</t>
         </is>
       </c>
     </row>
@@ -4178,9 +4584,15 @@
       <c r="N70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O70" t="inlineStr">
-        <is>
-          <t>2625</t>
+      <c r="O70" t="n">
+        <v>2625</v>
+      </c>
+      <c r="P70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q70" t="inlineStr">
+        <is>
+          <t>2654</t>
         </is>
       </c>
     </row>
@@ -4233,9 +4645,15 @@
       <c r="N71" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="O71" t="inlineStr">
-        <is>
-          <t>3519</t>
+      <c r="O71" t="n">
+        <v>3519</v>
+      </c>
+      <c r="P71" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q71" t="inlineStr">
+        <is>
+          <t>3747</t>
         </is>
       </c>
     </row>
@@ -4288,9 +4706,15 @@
       <c r="N72" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="O72" t="inlineStr">
-        <is>
-          <t>2896</t>
+      <c r="O72" t="n">
+        <v>2896</v>
+      </c>
+      <c r="P72" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q72" t="inlineStr">
+        <is>
+          <t>3172</t>
         </is>
       </c>
     </row>
@@ -4343,9 +4767,15 @@
       <c r="N73" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O73" t="inlineStr">
-        <is>
-          <t>3445</t>
+      <c r="O73" t="n">
+        <v>3445</v>
+      </c>
+      <c r="P73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q73" t="inlineStr">
+        <is>
+          <t>3616</t>
         </is>
       </c>
     </row>
@@ -4398,9 +4828,15 @@
       <c r="N74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O74" t="inlineStr">
-        <is>
-          <t>2618</t>
+      <c r="O74" t="n">
+        <v>2618</v>
+      </c>
+      <c r="P74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q74" t="inlineStr">
+        <is>
+          <t>2671</t>
         </is>
       </c>
     </row>
@@ -4453,9 +4889,15 @@
       <c r="N75" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="O75" t="inlineStr">
-        <is>
-          <t>3350</t>
+      <c r="O75" t="n">
+        <v>3350</v>
+      </c>
+      <c r="P75" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q75" t="inlineStr">
+        <is>
+          <t>3487</t>
         </is>
       </c>
     </row>
@@ -4508,9 +4950,15 @@
       <c r="N76" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O76" t="inlineStr">
-        <is>
-          <t>3769</t>
+      <c r="O76" t="n">
+        <v>3769</v>
+      </c>
+      <c r="P76" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q76" t="inlineStr">
+        <is>
+          <t>4026</t>
         </is>
       </c>
     </row>
@@ -4563,9 +5011,15 @@
       <c r="N77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O77" t="inlineStr">
-        <is>
-          <t>3323</t>
+      <c r="O77" t="n">
+        <v>3323</v>
+      </c>
+      <c r="P77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q77" t="inlineStr">
+        <is>
+          <t>3355</t>
         </is>
       </c>
     </row>
@@ -4618,9 +5072,15 @@
       <c r="N78" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O78" t="inlineStr">
-        <is>
-          <t>3953</t>
+      <c r="O78" t="n">
+        <v>3953</v>
+      </c>
+      <c r="P78" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q78" t="inlineStr">
+        <is>
+          <t>4169</t>
         </is>
       </c>
     </row>
@@ -4673,7 +5133,13 @@
       <c r="N79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O79" t="inlineStr">
+      <c r="O79" t="n">
+        <v>0</v>
+      </c>
+      <c r="P79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4728,9 +5194,15 @@
       <c r="N80" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="O80" t="inlineStr">
-        <is>
-          <t>3721</t>
+      <c r="O80" t="n">
+        <v>3721</v>
+      </c>
+      <c r="P80" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="Q80" t="inlineStr">
+        <is>
+          <t>3884</t>
         </is>
       </c>
     </row>
@@ -4783,9 +5255,15 @@
       <c r="N81" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="O81" t="inlineStr">
-        <is>
-          <t>3858</t>
+      <c r="O81" t="n">
+        <v>3858</v>
+      </c>
+      <c r="P81" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q81" t="inlineStr">
+        <is>
+          <t>3987</t>
         </is>
       </c>
     </row>
@@ -4838,9 +5316,15 @@
       <c r="N82" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="O82" t="inlineStr">
-        <is>
-          <t>3637</t>
+      <c r="O82" t="n">
+        <v>3637</v>
+      </c>
+      <c r="P82" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="Q82" t="inlineStr">
+        <is>
+          <t>3777</t>
         </is>
       </c>
     </row>
@@ -4893,9 +5377,15 @@
       <c r="N83" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="O83" t="inlineStr">
-        <is>
-          <t>3432</t>
+      <c r="O83" t="n">
+        <v>3432</v>
+      </c>
+      <c r="P83" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q83" t="inlineStr">
+        <is>
+          <t>3722</t>
         </is>
       </c>
     </row>
@@ -4948,9 +5438,15 @@
       <c r="N84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O84" t="inlineStr">
-        <is>
-          <t>2785</t>
+      <c r="O84" t="n">
+        <v>2785</v>
+      </c>
+      <c r="P84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q84" t="inlineStr">
+        <is>
+          <t>2767</t>
         </is>
       </c>
     </row>
@@ -5003,9 +5499,15 @@
       <c r="N85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O85" t="inlineStr">
-        <is>
-          <t>3003</t>
+      <c r="O85" t="n">
+        <v>3003</v>
+      </c>
+      <c r="P85" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q85" t="inlineStr">
+        <is>
+          <t>3136</t>
         </is>
       </c>
     </row>
@@ -5058,9 +5560,15 @@
       <c r="N86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O86" t="inlineStr">
-        <is>
-          <t>2750</t>
+      <c r="O86" t="n">
+        <v>2750</v>
+      </c>
+      <c r="P86" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q86" t="inlineStr">
+        <is>
+          <t>2927</t>
         </is>
       </c>
     </row>
@@ -5113,9 +5621,15 @@
       <c r="N87" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O87" t="inlineStr">
-        <is>
-          <t>3816</t>
+      <c r="O87" t="n">
+        <v>3816</v>
+      </c>
+      <c r="P87" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q87" t="inlineStr">
+        <is>
+          <t>3795</t>
         </is>
       </c>
     </row>
@@ -5168,9 +5682,15 @@
       <c r="N88" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O88" t="inlineStr">
-        <is>
-          <t>2789</t>
+      <c r="O88" t="n">
+        <v>2789</v>
+      </c>
+      <c r="P88" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q88" t="inlineStr">
+        <is>
+          <t>2790</t>
         </is>
       </c>
     </row>
@@ -5223,9 +5743,15 @@
       <c r="N89" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O89" t="inlineStr">
-        <is>
-          <t>2790</t>
+      <c r="O89" t="n">
+        <v>2790</v>
+      </c>
+      <c r="P89" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q89" t="inlineStr">
+        <is>
+          <t>2939</t>
         </is>
       </c>
     </row>
@@ -5278,9 +5804,15 @@
       <c r="N90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O90" t="inlineStr">
-        <is>
-          <t>2390</t>
+      <c r="O90" t="n">
+        <v>2390</v>
+      </c>
+      <c r="P90" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q90" t="inlineStr">
+        <is>
+          <t>2655</t>
         </is>
       </c>
     </row>
@@ -5333,9 +5865,15 @@
       <c r="N91" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O91" t="inlineStr">
-        <is>
-          <t>2672</t>
+      <c r="O91" t="n">
+        <v>2672</v>
+      </c>
+      <c r="P91" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q91" t="inlineStr">
+        <is>
+          <t>2732</t>
         </is>
       </c>
     </row>
@@ -5388,7 +5926,13 @@
       <c r="N92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O92" t="inlineStr">
+      <c r="O92" t="n">
+        <v>0</v>
+      </c>
+      <c r="P92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5443,9 +5987,15 @@
       <c r="N93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O93" t="inlineStr">
-        <is>
-          <t>2441</t>
+      <c r="O93" t="n">
+        <v>2441</v>
+      </c>
+      <c r="P93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q93" t="inlineStr">
+        <is>
+          <t>2393</t>
         </is>
       </c>
     </row>
@@ -5498,9 +6048,15 @@
       <c r="N94" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O94" t="inlineStr">
-        <is>
-          <t>2948</t>
+      <c r="O94" t="n">
+        <v>2948</v>
+      </c>
+      <c r="P94" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q94" t="inlineStr">
+        <is>
+          <t>2984</t>
         </is>
       </c>
     </row>
@@ -5553,9 +6109,15 @@
       <c r="N95" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="O95" t="inlineStr">
-        <is>
-          <t>2729</t>
+      <c r="O95" t="n">
+        <v>2729</v>
+      </c>
+      <c r="P95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q95" t="inlineStr">
+        <is>
+          <t>2671</t>
         </is>
       </c>
     </row>
@@ -5608,9 +6170,15 @@
       <c r="N96" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O96" t="inlineStr">
-        <is>
-          <t>3147</t>
+      <c r="O96" t="n">
+        <v>3147</v>
+      </c>
+      <c r="P96" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q96" t="inlineStr">
+        <is>
+          <t>3308</t>
         </is>
       </c>
     </row>
@@ -5663,9 +6231,15 @@
       <c r="N97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O97" t="inlineStr">
-        <is>
-          <t>2519</t>
+      <c r="O97" t="n">
+        <v>2519</v>
+      </c>
+      <c r="P97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q97" t="inlineStr">
+        <is>
+          <t>2546</t>
         </is>
       </c>
     </row>
@@ -5718,7 +6292,13 @@
       <c r="N98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O98" t="inlineStr">
+      <c r="O98" t="n">
+        <v>0</v>
+      </c>
+      <c r="P98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5773,9 +6353,15 @@
       <c r="N99" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O99" t="inlineStr">
-        <is>
-          <t>3120</t>
+      <c r="O99" t="n">
+        <v>3120</v>
+      </c>
+      <c r="P99" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q99" t="inlineStr">
+        <is>
+          <t>3211</t>
         </is>
       </c>
     </row>
@@ -5828,9 +6414,15 @@
       <c r="N100" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="O100" t="inlineStr">
-        <is>
-          <t>2453</t>
+      <c r="O100" t="n">
+        <v>2453</v>
+      </c>
+      <c r="P100" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q100" t="inlineStr">
+        <is>
+          <t>2497</t>
         </is>
       </c>
     </row>
@@ -5883,9 +6475,15 @@
       <c r="N101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O101" t="inlineStr">
-        <is>
-          <t>3640</t>
+      <c r="O101" t="n">
+        <v>3640</v>
+      </c>
+      <c r="P101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q101" t="inlineStr">
+        <is>
+          <t>3731</t>
         </is>
       </c>
     </row>
@@ -5938,9 +6536,15 @@
       <c r="N102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O102" t="inlineStr">
-        <is>
-          <t>3322</t>
+      <c r="O102" t="n">
+        <v>3322</v>
+      </c>
+      <c r="P102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q102" t="inlineStr">
+        <is>
+          <t>3442</t>
         </is>
       </c>
     </row>
@@ -5993,9 +6597,15 @@
       <c r="N103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O103" t="inlineStr">
-        <is>
-          <t>2518</t>
+      <c r="O103" t="n">
+        <v>2518</v>
+      </c>
+      <c r="P103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q103" t="inlineStr">
+        <is>
+          <t>2512</t>
         </is>
       </c>
     </row>
@@ -6048,9 +6658,15 @@
       <c r="N104" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O104" t="inlineStr">
-        <is>
-          <t>3627</t>
+      <c r="O104" t="n">
+        <v>3627</v>
+      </c>
+      <c r="P104" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q104" t="inlineStr">
+        <is>
+          <t>3768</t>
         </is>
       </c>
     </row>
@@ -6103,9 +6719,15 @@
       <c r="N105" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="O105" t="inlineStr">
-        <is>
-          <t>3398</t>
+      <c r="O105" t="n">
+        <v>3398</v>
+      </c>
+      <c r="P105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q105" t="inlineStr">
+        <is>
+          <t>3407</t>
         </is>
       </c>
     </row>
@@ -6158,7 +6780,13 @@
       <c r="N106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O106" t="inlineStr">
+      <c r="O106" t="n">
+        <v>0</v>
+      </c>
+      <c r="P106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6213,9 +6841,15 @@
       <c r="N107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O107" t="inlineStr">
-        <is>
-          <t>2479</t>
+      <c r="O107" t="n">
+        <v>2479</v>
+      </c>
+      <c r="P107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q107" t="inlineStr">
+        <is>
+          <t>2485</t>
         </is>
       </c>
     </row>
@@ -6268,7 +6902,13 @@
       <c r="N108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O108" t="inlineStr">
+      <c r="O108" t="n">
+        <v>0</v>
+      </c>
+      <c r="P108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6323,9 +6963,15 @@
       <c r="N109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O109" t="inlineStr">
-        <is>
-          <t>3055</t>
+      <c r="O109" t="n">
+        <v>3055</v>
+      </c>
+      <c r="P109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q109" t="inlineStr">
+        <is>
+          <t>3123</t>
         </is>
       </c>
     </row>
@@ -6378,9 +7024,15 @@
       <c r="N110" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="O110" t="inlineStr">
-        <is>
-          <t>3188</t>
+      <c r="O110" t="n">
+        <v>3188</v>
+      </c>
+      <c r="P110" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="Q110" t="inlineStr">
+        <is>
+          <t>3250</t>
         </is>
       </c>
     </row>
@@ -6433,9 +7085,15 @@
       <c r="N111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O111" t="inlineStr">
-        <is>
-          <t>2590</t>
+      <c r="O111" t="n">
+        <v>2590</v>
+      </c>
+      <c r="P111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q111" t="inlineStr">
+        <is>
+          <t>2565</t>
         </is>
       </c>
     </row>
@@ -6488,9 +7146,15 @@
       <c r="N112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O112" t="inlineStr">
-        <is>
-          <t>2787</t>
+      <c r="O112" t="n">
+        <v>2787</v>
+      </c>
+      <c r="P112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q112" t="inlineStr">
+        <is>
+          <t>2826</t>
         </is>
       </c>
     </row>
@@ -6543,9 +7207,15 @@
       <c r="N113" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="O113" t="inlineStr">
-        <is>
-          <t>2891</t>
+      <c r="O113" t="n">
+        <v>2891</v>
+      </c>
+      <c r="P113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q113" t="inlineStr">
+        <is>
+          <t>3052</t>
         </is>
       </c>
     </row>
@@ -6598,9 +7268,15 @@
       <c r="N114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O114" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="O114" t="n">
+        <v>2500</v>
+      </c>
+      <c r="P114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q114" t="inlineStr">
+        <is>
+          <t>2554</t>
         </is>
       </c>
     </row>
@@ -6653,9 +7329,15 @@
       <c r="N115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O115" t="inlineStr">
-        <is>
-          <t>2416</t>
+      <c r="O115" t="n">
+        <v>2416</v>
+      </c>
+      <c r="P115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q115" t="inlineStr">
+        <is>
+          <t>2402</t>
         </is>
       </c>
     </row>
@@ -6708,9 +7390,15 @@
       <c r="N116" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="O116" t="inlineStr">
-        <is>
-          <t>2891</t>
+      <c r="O116" t="n">
+        <v>2891</v>
+      </c>
+      <c r="P116" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q116" t="inlineStr">
+        <is>
+          <t>2906</t>
         </is>
       </c>
     </row>
@@ -6763,9 +7451,15 @@
       <c r="N117" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="O117" t="inlineStr">
-        <is>
-          <t>3142</t>
+      <c r="O117" t="n">
+        <v>3142</v>
+      </c>
+      <c r="P117" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q117" t="inlineStr">
+        <is>
+          <t>3225</t>
         </is>
       </c>
     </row>
@@ -6818,7 +7512,13 @@
       <c r="N118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O118" t="inlineStr">
+      <c r="O118" t="n">
+        <v>0</v>
+      </c>
+      <c r="P118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6873,9 +7573,15 @@
       <c r="N119" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O119" t="inlineStr">
-        <is>
-          <t>3176</t>
+      <c r="O119" t="n">
+        <v>3176</v>
+      </c>
+      <c r="P119" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q119" t="inlineStr">
+        <is>
+          <t>3384</t>
         </is>
       </c>
     </row>
@@ -6928,9 +7634,15 @@
       <c r="N120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O120" t="inlineStr">
-        <is>
-          <t>2443</t>
+      <c r="O120" t="n">
+        <v>2443</v>
+      </c>
+      <c r="P120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q120" t="inlineStr">
+        <is>
+          <t>2452</t>
         </is>
       </c>
     </row>
@@ -6983,9 +7695,15 @@
       <c r="N121" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="O121" t="inlineStr">
-        <is>
-          <t>3033</t>
+      <c r="O121" t="n">
+        <v>3033</v>
+      </c>
+      <c r="P121" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q121" t="inlineStr">
+        <is>
+          <t>3039</t>
         </is>
       </c>
     </row>
@@ -7038,7 +7756,13 @@
       <c r="N122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O122" t="inlineStr">
+      <c r="O122" t="n">
+        <v>0</v>
+      </c>
+      <c r="P122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7093,9 +7817,15 @@
       <c r="N123" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="O123" t="inlineStr">
-        <is>
-          <t>2871</t>
+      <c r="O123" t="n">
+        <v>2871</v>
+      </c>
+      <c r="P123" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q123" t="inlineStr">
+        <is>
+          <t>2923</t>
         </is>
       </c>
     </row>
@@ -7148,9 +7878,15 @@
       <c r="N124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O124" t="inlineStr">
-        <is>
-          <t>2850</t>
+      <c r="O124" t="n">
+        <v>2850</v>
+      </c>
+      <c r="P124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q124" t="inlineStr">
+        <is>
+          <t>2993</t>
         </is>
       </c>
     </row>
@@ -7203,9 +7939,15 @@
       <c r="N125" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="O125" t="inlineStr">
-        <is>
-          <t>3135</t>
+      <c r="O125" t="n">
+        <v>3135</v>
+      </c>
+      <c r="P125" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q125" t="inlineStr">
+        <is>
+          <t>3165</t>
         </is>
       </c>
     </row>
@@ -7258,9 +8000,15 @@
       <c r="N126" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O126" t="inlineStr">
-        <is>
-          <t>2954</t>
+      <c r="O126" t="n">
+        <v>2954</v>
+      </c>
+      <c r="P126" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q126" t="inlineStr">
+        <is>
+          <t>2990</t>
         </is>
       </c>
     </row>
@@ -7313,9 +8061,15 @@
       <c r="N127" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="O127" t="inlineStr">
-        <is>
-          <t>2412</t>
+      <c r="O127" t="n">
+        <v>2412</v>
+      </c>
+      <c r="P127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q127" t="inlineStr">
+        <is>
+          <t>2386</t>
         </is>
       </c>
     </row>
@@ -7368,7 +8122,13 @@
       <c r="N128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O128" t="inlineStr">
+      <c r="O128" t="n">
+        <v>0</v>
+      </c>
+      <c r="P128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7423,7 +8183,13 @@
       <c r="N129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O129" t="inlineStr">
+      <c r="O129" t="n">
+        <v>0</v>
+      </c>
+      <c r="P129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7478,9 +8244,15 @@
       <c r="N130" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="O130" t="inlineStr">
-        <is>
-          <t>2683</t>
+      <c r="O130" t="n">
+        <v>2683</v>
+      </c>
+      <c r="P130" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q130" t="inlineStr">
+        <is>
+          <t>2695</t>
         </is>
       </c>
     </row>
@@ -7533,9 +8305,15 @@
       <c r="N131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O131" t="inlineStr">
-        <is>
-          <t>2429</t>
+      <c r="O131" t="n">
+        <v>2429</v>
+      </c>
+      <c r="P131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q131" t="inlineStr">
+        <is>
+          <t>2446</t>
         </is>
       </c>
     </row>
@@ -7588,9 +8366,15 @@
       <c r="N132" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O132" t="inlineStr">
-        <is>
-          <t>2410</t>
+      <c r="O132" t="n">
+        <v>2410</v>
+      </c>
+      <c r="P132" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q132" t="inlineStr">
+        <is>
+          <t>2451</t>
         </is>
       </c>
     </row>
@@ -7643,9 +8427,15 @@
       <c r="N133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O133" t="inlineStr">
-        <is>
-          <t>2742</t>
+      <c r="O133" t="n">
+        <v>2742</v>
+      </c>
+      <c r="P133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q133" t="inlineStr">
+        <is>
+          <t>2729</t>
         </is>
       </c>
     </row>
@@ -7698,11 +8488,11 @@
       <c r="N134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O134" t="inlineStr">
-        <is>
-          <t>1693</t>
-        </is>
-      </c>
+      <c r="O134" t="n">
+        <v>1693</v>
+      </c>
+      <c r="P134" s="3" t="inlineStr"/>
+      <c r="Q134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -7748,6 +8538,8 @@
       <c r="M135" t="inlineStr"/>
       <c r="N135" s="3" t="inlineStr"/>
       <c r="O135" t="inlineStr"/>
+      <c r="P135" s="3" t="inlineStr"/>
+      <c r="Q135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -7798,9 +8590,15 @@
       <c r="N136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O136" t="inlineStr">
-        <is>
-          <t>2607</t>
+      <c r="O136" t="n">
+        <v>2607</v>
+      </c>
+      <c r="P136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q136" t="inlineStr">
+        <is>
+          <t>2618</t>
         </is>
       </c>
     </row>
@@ -7853,7 +8651,13 @@
       <c r="N137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O137" t="inlineStr">
+      <c r="O137" t="n">
+        <v>0</v>
+      </c>
+      <c r="P137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7903,6 +8707,8 @@
       <c r="M138" t="inlineStr"/>
       <c r="N138" s="3" t="inlineStr"/>
       <c r="O138" t="inlineStr"/>
+      <c r="P138" s="3" t="inlineStr"/>
+      <c r="Q138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -7953,9 +8759,15 @@
       <c r="N139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O139" t="inlineStr">
-        <is>
-          <t>2390</t>
+      <c r="O139" t="n">
+        <v>2390</v>
+      </c>
+      <c r="P139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q139" t="inlineStr">
+        <is>
+          <t>2365</t>
         </is>
       </c>
     </row>
@@ -8008,9 +8820,15 @@
       <c r="N140" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O140" t="inlineStr">
-        <is>
-          <t>2677</t>
+      <c r="O140" t="n">
+        <v>2677</v>
+      </c>
+      <c r="P140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q140" t="inlineStr">
+        <is>
+          <t>2621</t>
         </is>
       </c>
     </row>
@@ -8058,6 +8876,8 @@
       <c r="M141" t="inlineStr"/>
       <c r="N141" s="3" t="inlineStr"/>
       <c r="O141" t="inlineStr"/>
+      <c r="P141" s="3" t="inlineStr"/>
+      <c r="Q141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -8108,9 +8928,15 @@
       <c r="N142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O142" t="inlineStr">
-        <is>
-          <t>2034</t>
+      <c r="O142" t="n">
+        <v>2034</v>
+      </c>
+      <c r="P142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q142" t="inlineStr">
+        <is>
+          <t>2020</t>
         </is>
       </c>
     </row>
@@ -8158,6 +8984,8 @@
       <c r="M143" t="inlineStr"/>
       <c r="N143" s="3" t="inlineStr"/>
       <c r="O143" t="inlineStr"/>
+      <c r="P143" s="3" t="inlineStr"/>
+      <c r="Q143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -8203,6 +9031,8 @@
       <c r="M144" t="inlineStr"/>
       <c r="N144" s="3" t="inlineStr"/>
       <c r="O144" t="inlineStr"/>
+      <c r="P144" s="3" t="inlineStr"/>
+      <c r="Q144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -8248,6 +9078,8 @@
       <c r="M145" t="inlineStr"/>
       <c r="N145" s="3" t="inlineStr"/>
       <c r="O145" t="inlineStr"/>
+      <c r="P145" s="3" t="inlineStr"/>
+      <c r="Q145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -8293,6 +9125,8 @@
       <c r="M146" t="inlineStr"/>
       <c r="N146" s="3" t="inlineStr"/>
       <c r="O146" t="inlineStr"/>
+      <c r="P146" s="3" t="inlineStr"/>
+      <c r="Q146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -8338,6 +9172,8 @@
       <c r="M147" t="inlineStr"/>
       <c r="N147" s="3" t="inlineStr"/>
       <c r="O147" t="inlineStr"/>
+      <c r="P147" s="3" t="inlineStr"/>
+      <c r="Q147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -8388,9 +9224,15 @@
       <c r="N148" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="O148" t="inlineStr">
-        <is>
-          <t>1530</t>
+      <c r="O148" t="n">
+        <v>1530</v>
+      </c>
+      <c r="P148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q148" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -8443,9 +9285,15 @@
       <c r="N149" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="O149" t="inlineStr">
-        <is>
-          <t>2685</t>
+      <c r="O149" t="n">
+        <v>2685</v>
+      </c>
+      <c r="P149" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q149" t="inlineStr">
+        <is>
+          <t>2875</t>
         </is>
       </c>
     </row>
@@ -8498,7 +9346,13 @@
       <c r="N150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O150" t="inlineStr">
+      <c r="O150" t="n">
+        <v>0</v>
+      </c>
+      <c r="P150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8553,7 +9407,13 @@
       <c r="N151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O151" t="inlineStr">
+      <c r="O151" t="n">
+        <v>0</v>
+      </c>
+      <c r="P151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8608,7 +9468,13 @@
       <c r="N152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O152" t="inlineStr">
+      <c r="O152" t="n">
+        <v>0</v>
+      </c>
+      <c r="P152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8663,7 +9529,13 @@
       <c r="N153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O153" t="inlineStr">
+      <c r="O153" t="n">
+        <v>0</v>
+      </c>
+      <c r="P153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8718,7 +9590,13 @@
       <c r="N154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O154" t="inlineStr">
+      <c r="O154" t="n">
+        <v>0</v>
+      </c>
+      <c r="P154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8773,7 +9651,13 @@
       <c r="N155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O155" t="inlineStr">
+      <c r="O155" t="n">
+        <v>0</v>
+      </c>
+      <c r="P155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q155" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8822,9 +9706,15 @@
       <c r="N156" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="O156" t="inlineStr">
-        <is>
-          <t>3068</t>
+      <c r="O156" t="n">
+        <v>3068</v>
+      </c>
+      <c r="P156" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q156" t="inlineStr">
+        <is>
+          <t>3149</t>
         </is>
       </c>
     </row>
@@ -8866,6 +9756,8 @@
       <c r="M157" t="inlineStr"/>
       <c r="N157" s="3" t="inlineStr"/>
       <c r="O157" t="inlineStr"/>
+      <c r="P157" s="3" t="inlineStr"/>
+      <c r="Q157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -8910,7 +9802,13 @@
       <c r="N158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O158" t="inlineStr">
+      <c r="O158" t="n">
+        <v>0</v>
+      </c>
+      <c r="P158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8959,9 +9857,15 @@
       <c r="N159" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O159" t="inlineStr">
-        <is>
-          <t>2499</t>
+      <c r="O159" t="n">
+        <v>2499</v>
+      </c>
+      <c r="P159" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q159" t="inlineStr">
+        <is>
+          <t>2708</t>
         </is>
       </c>
     </row>
@@ -9003,6 +9907,8 @@
       </c>
       <c r="N160" s="3" t="inlineStr"/>
       <c r="O160" t="inlineStr"/>
+      <c r="P160" s="3" t="inlineStr"/>
+      <c r="Q160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -9035,9 +9941,15 @@
       <c r="N161" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="O161" t="inlineStr">
-        <is>
-          <t>2580</t>
+      <c r="O161" t="n">
+        <v>2580</v>
+      </c>
+      <c r="P161" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="Q161" t="inlineStr">
+        <is>
+          <t>2593</t>
         </is>
       </c>
     </row>
@@ -9072,17 +9984,21 @@
       <c r="N162" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="O162" t="inlineStr">
-        <is>
-          <t>2382</t>
+      <c r="O162" t="n">
+        <v>2382</v>
+      </c>
+      <c r="P162" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q162" t="inlineStr">
+        <is>
+          <t>2432</t>
         </is>
       </c>
     </row>
     <row r="163">
-      <c r="A163" t="inlineStr">
-        <is>
-          <t>47244896</t>
-        </is>
+      <c r="A163" t="n">
+        <v>47244896</v>
       </c>
       <c r="B163" t="inlineStr">
         <is>
@@ -9107,9 +10023,15 @@
       <c r="N163" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O163" t="inlineStr">
-        <is>
-          <t>2712</t>
+      <c r="O163" t="n">
+        <v>2712</v>
+      </c>
+      <c r="P163" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q163" t="inlineStr">
+        <is>
+          <t>2987</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-02-19 11:30:35
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q163"/>
+  <dimension ref="A1:S163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,6 +476,16 @@
           <t>02-17_0</t>
         </is>
       </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>02-18_A</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>02-18_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -532,9 +542,15 @@
       <c r="P2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>3046</t>
+      <c r="Q2" t="n">
+        <v>3046</v>
+      </c>
+      <c r="R2" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>3429</t>
         </is>
       </c>
     </row>
@@ -593,9 +609,15 @@
       <c r="P3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>3977</t>
+      <c r="Q3" t="n">
+        <v>3977</v>
+      </c>
+      <c r="R3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>4196</t>
         </is>
       </c>
     </row>
@@ -654,9 +676,15 @@
       <c r="P4" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>4677</t>
+      <c r="Q4" t="n">
+        <v>4677</v>
+      </c>
+      <c r="R4" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>4934</t>
         </is>
       </c>
     </row>
@@ -715,9 +743,15 @@
       <c r="P5" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>3498</t>
+      <c r="Q5" t="n">
+        <v>3498</v>
+      </c>
+      <c r="R5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>3964</t>
         </is>
       </c>
     </row>
@@ -776,9 +810,15 @@
       <c r="P6" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>4388</t>
+      <c r="Q6" t="n">
+        <v>4388</v>
+      </c>
+      <c r="R6" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>4592</t>
         </is>
       </c>
     </row>
@@ -837,9 +877,15 @@
       <c r="P7" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>4881</t>
+      <c r="Q7" t="n">
+        <v>4881</v>
+      </c>
+      <c r="R7" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>5032</t>
         </is>
       </c>
     </row>
@@ -898,9 +944,15 @@
       <c r="P8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>4055</t>
+      <c r="Q8" t="n">
+        <v>4055</v>
+      </c>
+      <c r="R8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>4300</t>
         </is>
       </c>
     </row>
@@ -959,9 +1011,15 @@
       <c r="P9" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>4040</t>
+      <c r="Q9" t="n">
+        <v>4040</v>
+      </c>
+      <c r="R9" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>4279</t>
         </is>
       </c>
     </row>
@@ -1020,9 +1078,15 @@
       <c r="P10" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>4265</t>
+      <c r="Q10" t="n">
+        <v>4265</v>
+      </c>
+      <c r="R10" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>4556</t>
         </is>
       </c>
     </row>
@@ -1081,9 +1145,15 @@
       <c r="P11" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>3850</t>
+      <c r="Q11" t="n">
+        <v>3850</v>
+      </c>
+      <c r="R11" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>4048</t>
         </is>
       </c>
     </row>
@@ -1142,7 +1212,13 @@
       <c r="P12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q12" t="inlineStr">
+      <c r="Q12" t="n">
+        <v>2835</v>
+      </c>
+      <c r="R12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" t="inlineStr">
         <is>
           <t>2835</t>
         </is>
@@ -1203,9 +1279,15 @@
       <c r="P13" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>4925</t>
+      <c r="Q13" t="n">
+        <v>4925</v>
+      </c>
+      <c r="R13" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>5370</t>
         </is>
       </c>
     </row>
@@ -1264,9 +1346,15 @@
       <c r="P14" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>4230</t>
+      <c r="Q14" t="n">
+        <v>4230</v>
+      </c>
+      <c r="R14" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>4482</t>
         </is>
       </c>
     </row>
@@ -1325,9 +1413,15 @@
       <c r="P15" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t>3729</t>
+      <c r="Q15" t="n">
+        <v>3729</v>
+      </c>
+      <c r="R15" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>4002</t>
         </is>
       </c>
     </row>
@@ -1386,9 +1480,15 @@
       <c r="P16" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>4308</t>
+      <c r="Q16" t="n">
+        <v>4308</v>
+      </c>
+      <c r="R16" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>4454</t>
         </is>
       </c>
     </row>
@@ -1447,9 +1547,15 @@
       <c r="P17" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="Q17" t="inlineStr">
-        <is>
-          <t>3714</t>
+      <c r="Q17" t="n">
+        <v>3714</v>
+      </c>
+      <c r="R17" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>3863</t>
         </is>
       </c>
     </row>
@@ -1508,9 +1614,15 @@
       <c r="P18" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>3789</t>
+      <c r="Q18" t="n">
+        <v>3789</v>
+      </c>
+      <c r="R18" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>3805</t>
         </is>
       </c>
     </row>
@@ -1569,9 +1681,15 @@
       <c r="P19" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>4254</t>
+      <c r="Q19" t="n">
+        <v>4254</v>
+      </c>
+      <c r="R19" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>4466</t>
         </is>
       </c>
     </row>
@@ -1630,9 +1748,15 @@
       <c r="P20" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>5090</t>
+      <c r="Q20" t="n">
+        <v>5090</v>
+      </c>
+      <c r="R20" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>5324</t>
         </is>
       </c>
     </row>
@@ -1691,9 +1815,15 @@
       <c r="P21" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q21" t="inlineStr">
-        <is>
-          <t>3490</t>
+      <c r="Q21" t="n">
+        <v>3490</v>
+      </c>
+      <c r="R21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>3509</t>
         </is>
       </c>
     </row>
@@ -1752,9 +1882,15 @@
       <c r="P22" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>4364</t>
+      <c r="Q22" t="n">
+        <v>4364</v>
+      </c>
+      <c r="R22" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>4555</t>
         </is>
       </c>
     </row>
@@ -1813,9 +1949,15 @@
       <c r="P23" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>3897</t>
+      <c r="Q23" t="n">
+        <v>3897</v>
+      </c>
+      <c r="R23" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>4203</t>
         </is>
       </c>
     </row>
@@ -1874,9 +2016,15 @@
       <c r="P24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>4389</t>
+      <c r="Q24" t="n">
+        <v>4389</v>
+      </c>
+      <c r="R24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>4533</t>
         </is>
       </c>
     </row>
@@ -1935,7 +2083,13 @@
       <c r="P25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q25" t="inlineStr">
+      <c r="Q25" t="n">
+        <v>0</v>
+      </c>
+      <c r="R25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1996,9 +2150,15 @@
       <c r="P26" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="Q26" t="inlineStr">
-        <is>
-          <t>4478</t>
+      <c r="Q26" t="n">
+        <v>4478</v>
+      </c>
+      <c r="R26" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>4661</t>
         </is>
       </c>
     </row>
@@ -2057,9 +2217,15 @@
       <c r="P27" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q27" t="inlineStr">
-        <is>
-          <t>4348</t>
+      <c r="Q27" t="n">
+        <v>4348</v>
+      </c>
+      <c r="R27" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>4675</t>
         </is>
       </c>
     </row>
@@ -2118,9 +2284,15 @@
       <c r="P28" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="Q28" t="inlineStr">
-        <is>
-          <t>3663</t>
+      <c r="Q28" t="n">
+        <v>3663</v>
+      </c>
+      <c r="R28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>3766</t>
         </is>
       </c>
     </row>
@@ -2179,9 +2351,15 @@
       <c r="P29" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="Q29" t="inlineStr">
-        <is>
-          <t>5046</t>
+      <c r="Q29" t="n">
+        <v>5046</v>
+      </c>
+      <c r="R29" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>5294</t>
         </is>
       </c>
     </row>
@@ -2240,9 +2418,15 @@
       <c r="P30" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q30" t="inlineStr">
-        <is>
-          <t>3889</t>
+      <c r="Q30" t="n">
+        <v>3889</v>
+      </c>
+      <c r="R30" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S30" t="inlineStr">
+        <is>
+          <t>4103</t>
         </is>
       </c>
     </row>
@@ -2301,9 +2485,15 @@
       <c r="P31" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="Q31" t="inlineStr">
-        <is>
-          <t>4682</t>
+      <c r="Q31" t="n">
+        <v>4682</v>
+      </c>
+      <c r="R31" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>4797</t>
         </is>
       </c>
     </row>
@@ -2362,9 +2552,15 @@
       <c r="P32" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q32" t="inlineStr">
-        <is>
-          <t>3962</t>
+      <c r="Q32" t="n">
+        <v>3962</v>
+      </c>
+      <c r="R32" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S32" t="inlineStr">
+        <is>
+          <t>4182</t>
         </is>
       </c>
     </row>
@@ -2423,9 +2619,15 @@
       <c r="P33" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="Q33" t="inlineStr">
-        <is>
-          <t>4274</t>
+      <c r="Q33" t="n">
+        <v>4274</v>
+      </c>
+      <c r="R33" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="S33" t="inlineStr">
+        <is>
+          <t>4487</t>
         </is>
       </c>
     </row>
@@ -2484,9 +2686,15 @@
       <c r="P34" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q34" t="inlineStr">
-        <is>
-          <t>4263</t>
+      <c r="Q34" t="n">
+        <v>4263</v>
+      </c>
+      <c r="R34" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S34" t="inlineStr">
+        <is>
+          <t>4614</t>
         </is>
       </c>
     </row>
@@ -2545,9 +2753,15 @@
       <c r="P35" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q35" t="inlineStr">
-        <is>
-          <t>4320</t>
+      <c r="Q35" t="n">
+        <v>4320</v>
+      </c>
+      <c r="R35" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="S35" t="inlineStr">
+        <is>
+          <t>4546</t>
         </is>
       </c>
     </row>
@@ -2606,9 +2820,15 @@
       <c r="P36" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q36" t="inlineStr">
-        <is>
-          <t>4431</t>
+      <c r="Q36" t="n">
+        <v>4431</v>
+      </c>
+      <c r="R36" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S36" t="inlineStr">
+        <is>
+          <t>4609</t>
         </is>
       </c>
     </row>
@@ -2667,9 +2887,15 @@
       <c r="P37" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q37" t="inlineStr">
-        <is>
-          <t>3878</t>
+      <c r="Q37" t="n">
+        <v>3878</v>
+      </c>
+      <c r="R37" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S37" t="inlineStr">
+        <is>
+          <t>4035</t>
         </is>
       </c>
     </row>
@@ -2728,9 +2954,15 @@
       <c r="P38" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q38" t="inlineStr">
-        <is>
-          <t>4325</t>
+      <c r="Q38" t="n">
+        <v>4325</v>
+      </c>
+      <c r="R38" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="S38" t="inlineStr">
+        <is>
+          <t>4509</t>
         </is>
       </c>
     </row>
@@ -2789,9 +3021,15 @@
       <c r="P39" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="Q39" t="inlineStr">
-        <is>
-          <t>4451</t>
+      <c r="Q39" t="n">
+        <v>4451</v>
+      </c>
+      <c r="R39" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="S39" t="inlineStr">
+        <is>
+          <t>4568</t>
         </is>
       </c>
     </row>
@@ -2850,9 +3088,15 @@
       <c r="P40" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q40" t="inlineStr">
-        <is>
-          <t>4767</t>
+      <c r="Q40" t="n">
+        <v>4767</v>
+      </c>
+      <c r="R40" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="S40" t="inlineStr">
+        <is>
+          <t>5064</t>
         </is>
       </c>
     </row>
@@ -2911,7 +3155,13 @@
       <c r="P41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q41" t="inlineStr">
+      <c r="Q41" t="n">
+        <v>3632</v>
+      </c>
+      <c r="R41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S41" t="inlineStr">
         <is>
           <t>3632</t>
         </is>
@@ -2972,9 +3222,15 @@
       <c r="P42" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="Q42" t="inlineStr">
-        <is>
-          <t>4744</t>
+      <c r="Q42" t="n">
+        <v>4744</v>
+      </c>
+      <c r="R42" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="S42" t="inlineStr">
+        <is>
+          <t>4996</t>
         </is>
       </c>
     </row>
@@ -3033,9 +3289,15 @@
       <c r="P43" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q43" t="inlineStr">
-        <is>
-          <t>4465</t>
+      <c r="Q43" t="n">
+        <v>4465</v>
+      </c>
+      <c r="R43" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="S43" t="inlineStr">
+        <is>
+          <t>4792</t>
         </is>
       </c>
     </row>
@@ -3094,9 +3356,15 @@
       <c r="P44" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="Q44" t="inlineStr">
-        <is>
-          <t>4573</t>
+      <c r="Q44" t="n">
+        <v>4573</v>
+      </c>
+      <c r="R44" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="S44" t="inlineStr">
+        <is>
+          <t>4735</t>
         </is>
       </c>
     </row>
@@ -3155,9 +3423,15 @@
       <c r="P45" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q45" t="inlineStr">
-        <is>
-          <t>4112</t>
+      <c r="Q45" t="n">
+        <v>4112</v>
+      </c>
+      <c r="R45" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="S45" t="inlineStr">
+        <is>
+          <t>4240</t>
         </is>
       </c>
     </row>
@@ -3216,9 +3490,15 @@
       <c r="P46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q46" t="inlineStr">
-        <is>
-          <t>4085</t>
+      <c r="Q46" t="n">
+        <v>4085</v>
+      </c>
+      <c r="R46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S46" t="inlineStr">
+        <is>
+          <t>4243</t>
         </is>
       </c>
     </row>
@@ -3277,7 +3557,13 @@
       <c r="P47" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q47" t="inlineStr">
+      <c r="Q47" t="n">
+        <v>2500</v>
+      </c>
+      <c r="R47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S47" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -3338,9 +3624,15 @@
       <c r="P48" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="Q48" t="inlineStr">
-        <is>
-          <t>4674</t>
+      <c r="Q48" t="n">
+        <v>4674</v>
+      </c>
+      <c r="R48" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="S48" t="inlineStr">
+        <is>
+          <t>4765</t>
         </is>
       </c>
     </row>
@@ -3399,9 +3691,15 @@
       <c r="P49" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="Q49" t="inlineStr">
-        <is>
-          <t>3599</t>
+      <c r="Q49" t="n">
+        <v>3599</v>
+      </c>
+      <c r="R49" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S49" t="inlineStr">
+        <is>
+          <t>3720</t>
         </is>
       </c>
     </row>
@@ -3460,9 +3758,15 @@
       <c r="P50" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="Q50" t="inlineStr">
-        <is>
-          <t>4800</t>
+      <c r="Q50" t="n">
+        <v>4800</v>
+      </c>
+      <c r="R50" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="S50" t="inlineStr">
+        <is>
+          <t>4934</t>
         </is>
       </c>
     </row>
@@ -3521,9 +3825,15 @@
       <c r="P51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q51" t="inlineStr">
-        <is>
-          <t>2835</t>
+      <c r="Q51" t="n">
+        <v>2835</v>
+      </c>
+      <c r="R51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S51" t="inlineStr">
+        <is>
+          <t>2833</t>
         </is>
       </c>
     </row>
@@ -3582,9 +3892,15 @@
       <c r="P52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q52" t="inlineStr">
-        <is>
-          <t>2526</t>
+      <c r="Q52" t="n">
+        <v>2526</v>
+      </c>
+      <c r="R52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S52" t="inlineStr">
+        <is>
+          <t>2660</t>
         </is>
       </c>
     </row>
@@ -3643,9 +3959,15 @@
       <c r="P53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q53" t="inlineStr">
-        <is>
-          <t>2599</t>
+      <c r="Q53" t="n">
+        <v>2599</v>
+      </c>
+      <c r="R53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S53" t="inlineStr">
+        <is>
+          <t>2628</t>
         </is>
       </c>
     </row>
@@ -3704,9 +4026,15 @@
       <c r="P54" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="Q54" t="inlineStr">
-        <is>
-          <t>4413</t>
+      <c r="Q54" t="n">
+        <v>4413</v>
+      </c>
+      <c r="R54" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="S54" t="inlineStr">
+        <is>
+          <t>4685</t>
         </is>
       </c>
     </row>
@@ -3765,9 +4093,15 @@
       <c r="P55" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="Q55" t="inlineStr">
-        <is>
-          <t>3526</t>
+      <c r="Q55" t="n">
+        <v>3526</v>
+      </c>
+      <c r="R55" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="S55" t="inlineStr">
+        <is>
+          <t>3676</t>
         </is>
       </c>
     </row>
@@ -3826,9 +4160,15 @@
       <c r="P56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q56" t="inlineStr">
-        <is>
-          <t>3656</t>
+      <c r="Q56" t="n">
+        <v>3656</v>
+      </c>
+      <c r="R56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S56" t="inlineStr">
+        <is>
+          <t>3740</t>
         </is>
       </c>
     </row>
@@ -3887,9 +4227,15 @@
       <c r="P57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q57" t="inlineStr">
-        <is>
-          <t>4156</t>
+      <c r="Q57" t="n">
+        <v>4156</v>
+      </c>
+      <c r="R57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S57" t="inlineStr">
+        <is>
+          <t>4443</t>
         </is>
       </c>
     </row>
@@ -3948,9 +4294,15 @@
       <c r="P58" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q58" t="inlineStr">
-        <is>
-          <t>3573</t>
+      <c r="Q58" t="n">
+        <v>3573</v>
+      </c>
+      <c r="R58" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="S58" t="inlineStr">
+        <is>
+          <t>3733</t>
         </is>
       </c>
     </row>
@@ -3984,6 +4336,8 @@
       <c r="O59" t="inlineStr"/>
       <c r="P59" s="3" t="inlineStr"/>
       <c r="Q59" t="inlineStr"/>
+      <c r="R59" s="3" t="inlineStr"/>
+      <c r="S59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -4015,6 +4369,8 @@
       <c r="O60" t="inlineStr"/>
       <c r="P60" s="3" t="inlineStr"/>
       <c r="Q60" t="inlineStr"/>
+      <c r="R60" s="3" t="inlineStr"/>
+      <c r="S60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -4071,9 +4427,15 @@
       <c r="P61" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q61" t="inlineStr">
-        <is>
-          <t>4023</t>
+      <c r="Q61" t="n">
+        <v>4023</v>
+      </c>
+      <c r="R61" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S61" t="inlineStr">
+        <is>
+          <t>4289</t>
         </is>
       </c>
     </row>
@@ -4132,7 +4494,13 @@
       <c r="P62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q62" t="inlineStr">
+      <c r="Q62" t="n">
+        <v>0</v>
+      </c>
+      <c r="R62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4193,9 +4561,15 @@
       <c r="P63" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="Q63" t="inlineStr">
-        <is>
-          <t>4150</t>
+      <c r="Q63" t="n">
+        <v>4150</v>
+      </c>
+      <c r="R63" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="S63" t="inlineStr">
+        <is>
+          <t>4381</t>
         </is>
       </c>
     </row>
@@ -4254,7 +4628,13 @@
       <c r="P64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q64" t="inlineStr">
+      <c r="Q64" t="n">
+        <v>2533</v>
+      </c>
+      <c r="R64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S64" t="inlineStr">
         <is>
           <t>2533</t>
         </is>
@@ -4290,6 +4670,8 @@
       <c r="O65" t="inlineStr"/>
       <c r="P65" s="3" t="inlineStr"/>
       <c r="Q65" t="inlineStr"/>
+      <c r="R65" s="3" t="inlineStr"/>
+      <c r="S65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -4346,9 +4728,15 @@
       <c r="P66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q66" t="inlineStr">
-        <is>
-          <t>2401</t>
+      <c r="Q66" t="n">
+        <v>2401</v>
+      </c>
+      <c r="R66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S66" t="inlineStr">
+        <is>
+          <t>2397</t>
         </is>
       </c>
     </row>
@@ -4407,9 +4795,15 @@
       <c r="P67" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q67" t="inlineStr">
-        <is>
-          <t>3906</t>
+      <c r="Q67" t="n">
+        <v>3906</v>
+      </c>
+      <c r="R67" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S67" t="inlineStr">
+        <is>
+          <t>4153</t>
         </is>
       </c>
     </row>
@@ -4468,9 +4862,15 @@
       <c r="P68" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q68" t="inlineStr">
-        <is>
-          <t>4401</t>
+      <c r="Q68" t="n">
+        <v>4401</v>
+      </c>
+      <c r="R68" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="S68" t="inlineStr">
+        <is>
+          <t>4652</t>
         </is>
       </c>
     </row>
@@ -4529,9 +4929,15 @@
       <c r="P69" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q69" t="inlineStr">
-        <is>
-          <t>3717</t>
+      <c r="Q69" t="n">
+        <v>3717</v>
+      </c>
+      <c r="R69" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="S69" t="inlineStr">
+        <is>
+          <t>3830</t>
         </is>
       </c>
     </row>
@@ -4590,9 +4996,15 @@
       <c r="P70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q70" t="inlineStr">
-        <is>
-          <t>2654</t>
+      <c r="Q70" t="n">
+        <v>2654</v>
+      </c>
+      <c r="R70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S70" t="inlineStr">
+        <is>
+          <t>2645</t>
         </is>
       </c>
     </row>
@@ -4651,9 +5063,15 @@
       <c r="P71" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q71" t="inlineStr">
-        <is>
-          <t>3747</t>
+      <c r="Q71" t="n">
+        <v>3747</v>
+      </c>
+      <c r="R71" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S71" t="inlineStr">
+        <is>
+          <t>3889</t>
         </is>
       </c>
     </row>
@@ -4712,9 +5130,15 @@
       <c r="P72" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="Q72" t="inlineStr">
-        <is>
-          <t>3172</t>
+      <c r="Q72" t="n">
+        <v>3172</v>
+      </c>
+      <c r="R72" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="S72" t="inlineStr">
+        <is>
+          <t>3282</t>
         </is>
       </c>
     </row>
@@ -4773,9 +5197,15 @@
       <c r="P73" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q73" t="inlineStr">
-        <is>
-          <t>3616</t>
+      <c r="Q73" t="n">
+        <v>3616</v>
+      </c>
+      <c r="R73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S73" t="inlineStr">
+        <is>
+          <t>3765</t>
         </is>
       </c>
     </row>
@@ -4834,9 +5264,15 @@
       <c r="P74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q74" t="inlineStr">
-        <is>
-          <t>2671</t>
+      <c r="Q74" t="n">
+        <v>2671</v>
+      </c>
+      <c r="R74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S74" t="inlineStr">
+        <is>
+          <t>2769</t>
         </is>
       </c>
     </row>
@@ -4895,9 +5331,15 @@
       <c r="P75" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q75" t="inlineStr">
-        <is>
-          <t>3487</t>
+      <c r="Q75" t="n">
+        <v>3487</v>
+      </c>
+      <c r="R75" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="S75" t="inlineStr">
+        <is>
+          <t>3591</t>
         </is>
       </c>
     </row>
@@ -4956,9 +5398,15 @@
       <c r="P76" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q76" t="inlineStr">
-        <is>
-          <t>4026</t>
+      <c r="Q76" t="n">
+        <v>4026</v>
+      </c>
+      <c r="R76" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S76" t="inlineStr">
+        <is>
+          <t>4259</t>
         </is>
       </c>
     </row>
@@ -5017,9 +5465,15 @@
       <c r="P77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q77" t="inlineStr">
-        <is>
-          <t>3355</t>
+      <c r="Q77" t="n">
+        <v>3355</v>
+      </c>
+      <c r="R77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S77" t="inlineStr">
+        <is>
+          <t>3353</t>
         </is>
       </c>
     </row>
@@ -5078,9 +5532,15 @@
       <c r="P78" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q78" t="inlineStr">
-        <is>
-          <t>4169</t>
+      <c r="Q78" t="n">
+        <v>4169</v>
+      </c>
+      <c r="R78" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S78" t="inlineStr">
+        <is>
+          <t>4426</t>
         </is>
       </c>
     </row>
@@ -5139,7 +5599,13 @@
       <c r="P79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q79" t="inlineStr">
+      <c r="Q79" t="n">
+        <v>0</v>
+      </c>
+      <c r="R79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5200,9 +5666,15 @@
       <c r="P80" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="Q80" t="inlineStr">
-        <is>
-          <t>3884</t>
+      <c r="Q80" t="n">
+        <v>3884</v>
+      </c>
+      <c r="R80" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S80" t="inlineStr">
+        <is>
+          <t>4153</t>
         </is>
       </c>
     </row>
@@ -5261,9 +5733,15 @@
       <c r="P81" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q81" t="inlineStr">
-        <is>
-          <t>3987</t>
+      <c r="Q81" t="n">
+        <v>3987</v>
+      </c>
+      <c r="R81" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="S81" t="inlineStr">
+        <is>
+          <t>4137</t>
         </is>
       </c>
     </row>
@@ -5322,9 +5800,15 @@
       <c r="P82" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="Q82" t="inlineStr">
-        <is>
-          <t>3777</t>
+      <c r="Q82" t="n">
+        <v>3777</v>
+      </c>
+      <c r="R82" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="S82" t="inlineStr">
+        <is>
+          <t>3923</t>
         </is>
       </c>
     </row>
@@ -5383,9 +5867,15 @@
       <c r="P83" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q83" t="inlineStr">
-        <is>
-          <t>3722</t>
+      <c r="Q83" t="n">
+        <v>3722</v>
+      </c>
+      <c r="R83" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S83" t="inlineStr">
+        <is>
+          <t>3841</t>
         </is>
       </c>
     </row>
@@ -5444,9 +5934,15 @@
       <c r="P84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q84" t="inlineStr">
-        <is>
-          <t>2767</t>
+      <c r="Q84" t="n">
+        <v>2767</v>
+      </c>
+      <c r="R84" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="S84" t="inlineStr">
+        <is>
+          <t>2906</t>
         </is>
       </c>
     </row>
@@ -5505,9 +6001,15 @@
       <c r="P85" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="Q85" t="inlineStr">
-        <is>
-          <t>3136</t>
+      <c r="Q85" t="n">
+        <v>3136</v>
+      </c>
+      <c r="R85" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="S85" t="inlineStr">
+        <is>
+          <t>3308</t>
         </is>
       </c>
     </row>
@@ -5566,9 +6068,15 @@
       <c r="P86" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="Q86" t="inlineStr">
-        <is>
-          <t>2927</t>
+      <c r="Q86" t="n">
+        <v>2927</v>
+      </c>
+      <c r="R86" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="S86" t="inlineStr">
+        <is>
+          <t>3033</t>
         </is>
       </c>
     </row>
@@ -5627,9 +6135,15 @@
       <c r="P87" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q87" t="inlineStr">
-        <is>
-          <t>3795</t>
+      <c r="Q87" t="n">
+        <v>3795</v>
+      </c>
+      <c r="R87" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S87" t="inlineStr">
+        <is>
+          <t>4032</t>
         </is>
       </c>
     </row>
@@ -5688,9 +6202,15 @@
       <c r="P88" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q88" t="inlineStr">
-        <is>
-          <t>2790</t>
+      <c r="Q88" t="n">
+        <v>2790</v>
+      </c>
+      <c r="R88" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S88" t="inlineStr">
+        <is>
+          <t>2894</t>
         </is>
       </c>
     </row>
@@ -5749,9 +6269,15 @@
       <c r="P89" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q89" t="inlineStr">
-        <is>
-          <t>2939</t>
+      <c r="Q89" t="n">
+        <v>2939</v>
+      </c>
+      <c r="R89" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S89" t="inlineStr">
+        <is>
+          <t>2993</t>
         </is>
       </c>
     </row>
@@ -5810,9 +6336,15 @@
       <c r="P90" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q90" t="inlineStr">
-        <is>
-          <t>2655</t>
+      <c r="Q90" t="n">
+        <v>2655</v>
+      </c>
+      <c r="R90" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S90" t="inlineStr">
+        <is>
+          <t>2785</t>
         </is>
       </c>
     </row>
@@ -5871,9 +6403,15 @@
       <c r="P91" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q91" t="inlineStr">
-        <is>
-          <t>2732</t>
+      <c r="Q91" t="n">
+        <v>2732</v>
+      </c>
+      <c r="R91" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S91" t="inlineStr">
+        <is>
+          <t>2792</t>
         </is>
       </c>
     </row>
@@ -5932,7 +6470,13 @@
       <c r="P92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q92" t="inlineStr">
+      <c r="Q92" t="n">
+        <v>0</v>
+      </c>
+      <c r="R92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5993,9 +6537,15 @@
       <c r="P93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q93" t="inlineStr">
-        <is>
-          <t>2393</t>
+      <c r="Q93" t="n">
+        <v>2393</v>
+      </c>
+      <c r="R93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S93" t="inlineStr">
+        <is>
+          <t>2397</t>
         </is>
       </c>
     </row>
@@ -6054,9 +6604,15 @@
       <c r="P94" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q94" t="inlineStr">
-        <is>
-          <t>2984</t>
+      <c r="Q94" t="n">
+        <v>2984</v>
+      </c>
+      <c r="R94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S94" t="inlineStr">
+        <is>
+          <t>3012</t>
         </is>
       </c>
     </row>
@@ -6115,9 +6671,15 @@
       <c r="P95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q95" t="inlineStr">
-        <is>
-          <t>2671</t>
+      <c r="Q95" t="n">
+        <v>2671</v>
+      </c>
+      <c r="R95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S95" t="inlineStr">
+        <is>
+          <t>2619</t>
         </is>
       </c>
     </row>
@@ -6176,9 +6738,15 @@
       <c r="P96" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q96" t="inlineStr">
-        <is>
-          <t>3308</t>
+      <c r="Q96" t="n">
+        <v>3308</v>
+      </c>
+      <c r="R96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S96" t="inlineStr">
+        <is>
+          <t>3245</t>
         </is>
       </c>
     </row>
@@ -6237,9 +6805,15 @@
       <c r="P97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q97" t="inlineStr">
-        <is>
-          <t>2546</t>
+      <c r="Q97" t="n">
+        <v>2546</v>
+      </c>
+      <c r="R97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S97" t="inlineStr">
+        <is>
+          <t>2545</t>
         </is>
       </c>
     </row>
@@ -6298,7 +6872,13 @@
       <c r="P98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q98" t="inlineStr">
+      <c r="Q98" t="n">
+        <v>0</v>
+      </c>
+      <c r="R98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6359,9 +6939,15 @@
       <c r="P99" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="Q99" t="inlineStr">
-        <is>
-          <t>3211</t>
+      <c r="Q99" t="n">
+        <v>3211</v>
+      </c>
+      <c r="R99" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="S99" t="inlineStr">
+        <is>
+          <t>3415</t>
         </is>
       </c>
     </row>
@@ -6371,7 +6957,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Player-20372140</t>
+          <t>人山即是仙</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -6420,9 +7006,15 @@
       <c r="P100" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="Q100" t="inlineStr">
-        <is>
-          <t>2497</t>
+      <c r="Q100" t="n">
+        <v>2497</v>
+      </c>
+      <c r="R100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S100" t="inlineStr">
+        <is>
+          <t>2458</t>
         </is>
       </c>
     </row>
@@ -6481,9 +7073,15 @@
       <c r="P101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q101" t="inlineStr">
-        <is>
-          <t>3731</t>
+      <c r="Q101" t="n">
+        <v>3731</v>
+      </c>
+      <c r="R101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S101" t="inlineStr">
+        <is>
+          <t>3893</t>
         </is>
       </c>
     </row>
@@ -6542,9 +7140,15 @@
       <c r="P102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q102" t="inlineStr">
-        <is>
-          <t>3442</t>
+      <c r="Q102" t="n">
+        <v>3442</v>
+      </c>
+      <c r="R102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S102" t="inlineStr">
+        <is>
+          <t>3535</t>
         </is>
       </c>
     </row>
@@ -6603,9 +7207,15 @@
       <c r="P103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q103" t="inlineStr">
-        <is>
-          <t>2512</t>
+      <c r="Q103" t="n">
+        <v>2512</v>
+      </c>
+      <c r="R103" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="S103" t="inlineStr">
+        <is>
+          <t>2527</t>
         </is>
       </c>
     </row>
@@ -6664,9 +7274,15 @@
       <c r="P104" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q104" t="inlineStr">
-        <is>
-          <t>3768</t>
+      <c r="Q104" t="n">
+        <v>3768</v>
+      </c>
+      <c r="R104" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S104" t="inlineStr">
+        <is>
+          <t>3873</t>
         </is>
       </c>
     </row>
@@ -6725,9 +7341,15 @@
       <c r="P105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q105" t="inlineStr">
-        <is>
-          <t>3407</t>
+      <c r="Q105" t="n">
+        <v>3407</v>
+      </c>
+      <c r="R105" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="S105" t="inlineStr">
+        <is>
+          <t>3600</t>
         </is>
       </c>
     </row>
@@ -6786,7 +7408,13 @@
       <c r="P106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q106" t="inlineStr">
+      <c r="Q106" t="n">
+        <v>0</v>
+      </c>
+      <c r="R106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6847,9 +7475,15 @@
       <c r="P107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q107" t="inlineStr">
-        <is>
-          <t>2485</t>
+      <c r="Q107" t="n">
+        <v>2485</v>
+      </c>
+      <c r="R107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S107" t="inlineStr">
+        <is>
+          <t>2495</t>
         </is>
       </c>
     </row>
@@ -6908,7 +7542,13 @@
       <c r="P108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q108" t="inlineStr">
+      <c r="Q108" t="n">
+        <v>0</v>
+      </c>
+      <c r="R108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6969,9 +7609,15 @@
       <c r="P109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q109" t="inlineStr">
-        <is>
-          <t>3123</t>
+      <c r="Q109" t="n">
+        <v>3123</v>
+      </c>
+      <c r="R109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S109" t="inlineStr">
+        <is>
+          <t>3274</t>
         </is>
       </c>
     </row>
@@ -7030,9 +7676,15 @@
       <c r="P110" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="Q110" t="inlineStr">
-        <is>
-          <t>3250</t>
+      <c r="Q110" t="n">
+        <v>3250</v>
+      </c>
+      <c r="R110" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="S110" t="inlineStr">
+        <is>
+          <t>3364</t>
         </is>
       </c>
     </row>
@@ -7091,9 +7743,15 @@
       <c r="P111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q111" t="inlineStr">
-        <is>
-          <t>2565</t>
+      <c r="Q111" t="n">
+        <v>2565</v>
+      </c>
+      <c r="R111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S111" t="inlineStr">
+        <is>
+          <t>2555</t>
         </is>
       </c>
     </row>
@@ -7152,9 +7810,15 @@
       <c r="P112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q112" t="inlineStr">
-        <is>
-          <t>2826</t>
+      <c r="Q112" t="n">
+        <v>2826</v>
+      </c>
+      <c r="R112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S112" t="inlineStr">
+        <is>
+          <t>2818</t>
         </is>
       </c>
     </row>
@@ -7213,9 +7877,15 @@
       <c r="P113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q113" t="inlineStr">
-        <is>
-          <t>3052</t>
+      <c r="Q113" t="n">
+        <v>3052</v>
+      </c>
+      <c r="R113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S113" t="inlineStr">
+        <is>
+          <t>3004</t>
         </is>
       </c>
     </row>
@@ -7274,9 +7944,15 @@
       <c r="P114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q114" t="inlineStr">
-        <is>
-          <t>2554</t>
+      <c r="Q114" t="n">
+        <v>2554</v>
+      </c>
+      <c r="R114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S114" t="inlineStr">
+        <is>
+          <t>2628</t>
         </is>
       </c>
     </row>
@@ -7335,9 +8011,15 @@
       <c r="P115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q115" t="inlineStr">
-        <is>
-          <t>2402</t>
+      <c r="Q115" t="n">
+        <v>2402</v>
+      </c>
+      <c r="R115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S115" t="inlineStr">
+        <is>
+          <t>2368</t>
         </is>
       </c>
     </row>
@@ -7396,9 +8078,15 @@
       <c r="P116" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="Q116" t="inlineStr">
-        <is>
-          <t>2906</t>
+      <c r="Q116" t="n">
+        <v>2906</v>
+      </c>
+      <c r="R116" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="S116" t="inlineStr">
+        <is>
+          <t>2978</t>
         </is>
       </c>
     </row>
@@ -7457,9 +8145,15 @@
       <c r="P117" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q117" t="inlineStr">
-        <is>
-          <t>3225</t>
+      <c r="Q117" t="n">
+        <v>3225</v>
+      </c>
+      <c r="R117" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S117" t="inlineStr">
+        <is>
+          <t>3356</t>
         </is>
       </c>
     </row>
@@ -7518,7 +8212,13 @@
       <c r="P118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q118" t="inlineStr">
+      <c r="Q118" t="n">
+        <v>0</v>
+      </c>
+      <c r="R118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7579,9 +8279,15 @@
       <c r="P119" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q119" t="inlineStr">
-        <is>
-          <t>3384</t>
+      <c r="Q119" t="n">
+        <v>3384</v>
+      </c>
+      <c r="R119" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S119" t="inlineStr">
+        <is>
+          <t>3660</t>
         </is>
       </c>
     </row>
@@ -7640,9 +8346,15 @@
       <c r="P120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q120" t="inlineStr">
-        <is>
-          <t>2452</t>
+      <c r="Q120" t="n">
+        <v>2452</v>
+      </c>
+      <c r="R120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S120" t="inlineStr">
+        <is>
+          <t>2443</t>
         </is>
       </c>
     </row>
@@ -7701,9 +8413,15 @@
       <c r="P121" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="Q121" t="inlineStr">
-        <is>
-          <t>3039</t>
+      <c r="Q121" t="n">
+        <v>3039</v>
+      </c>
+      <c r="R121" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="S121" t="inlineStr">
+        <is>
+          <t>3182</t>
         </is>
       </c>
     </row>
@@ -7762,7 +8480,13 @@
       <c r="P122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q122" t="inlineStr">
+      <c r="Q122" t="n">
+        <v>0</v>
+      </c>
+      <c r="R122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7823,9 +8547,15 @@
       <c r="P123" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q123" t="inlineStr">
-        <is>
-          <t>2923</t>
+      <c r="Q123" t="n">
+        <v>2923</v>
+      </c>
+      <c r="R123" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S123" t="inlineStr">
+        <is>
+          <t>2997</t>
         </is>
       </c>
     </row>
@@ -7884,9 +8614,15 @@
       <c r="P124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q124" t="inlineStr">
-        <is>
-          <t>2993</t>
+      <c r="Q124" t="n">
+        <v>2993</v>
+      </c>
+      <c r="R124" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="S124" t="inlineStr">
+        <is>
+          <t>2985</t>
         </is>
       </c>
     </row>
@@ -7945,9 +8681,15 @@
       <c r="P125" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q125" t="inlineStr">
-        <is>
-          <t>3165</t>
+      <c r="Q125" t="n">
+        <v>3165</v>
+      </c>
+      <c r="R125" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S125" t="inlineStr">
+        <is>
+          <t>3227</t>
         </is>
       </c>
     </row>
@@ -8006,9 +8748,15 @@
       <c r="P126" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q126" t="inlineStr">
-        <is>
-          <t>2990</t>
+      <c r="Q126" t="n">
+        <v>2990</v>
+      </c>
+      <c r="R126" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S126" t="inlineStr">
+        <is>
+          <t>3077</t>
         </is>
       </c>
     </row>
@@ -8067,9 +8815,15 @@
       <c r="P127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q127" t="inlineStr">
-        <is>
-          <t>2386</t>
+      <c r="Q127" t="n">
+        <v>2386</v>
+      </c>
+      <c r="R127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S127" t="inlineStr">
+        <is>
+          <t>2377</t>
         </is>
       </c>
     </row>
@@ -8128,7 +8882,13 @@
       <c r="P128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q128" t="inlineStr">
+      <c r="Q128" t="n">
+        <v>0</v>
+      </c>
+      <c r="R128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8189,7 +8949,13 @@
       <c r="P129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q129" t="inlineStr">
+      <c r="Q129" t="n">
+        <v>0</v>
+      </c>
+      <c r="R129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8250,9 +9016,15 @@
       <c r="P130" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q130" t="inlineStr">
-        <is>
-          <t>2695</t>
+      <c r="Q130" t="n">
+        <v>2695</v>
+      </c>
+      <c r="R130" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S130" t="inlineStr">
+        <is>
+          <t>2756</t>
         </is>
       </c>
     </row>
@@ -8311,9 +9083,15 @@
       <c r="P131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q131" t="inlineStr">
-        <is>
-          <t>2446</t>
+      <c r="Q131" t="n">
+        <v>2446</v>
+      </c>
+      <c r="R131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S131" t="inlineStr">
+        <is>
+          <t>2435</t>
         </is>
       </c>
     </row>
@@ -8372,9 +9150,15 @@
       <c r="P132" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q132" t="inlineStr">
-        <is>
-          <t>2451</t>
+      <c r="Q132" t="n">
+        <v>2451</v>
+      </c>
+      <c r="R132" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S132" t="inlineStr">
+        <is>
+          <t>2629</t>
         </is>
       </c>
     </row>
@@ -8433,9 +9217,15 @@
       <c r="P133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q133" t="inlineStr">
-        <is>
-          <t>2729</t>
+      <c r="Q133" t="n">
+        <v>2729</v>
+      </c>
+      <c r="R133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S133" t="inlineStr">
+        <is>
+          <t>2748</t>
         </is>
       </c>
     </row>
@@ -8493,6 +9283,8 @@
       </c>
       <c r="P134" s="3" t="inlineStr"/>
       <c r="Q134" t="inlineStr"/>
+      <c r="R134" s="3" t="inlineStr"/>
+      <c r="S134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -8540,6 +9332,8 @@
       <c r="O135" t="inlineStr"/>
       <c r="P135" s="3" t="inlineStr"/>
       <c r="Q135" t="inlineStr"/>
+      <c r="R135" s="3" t="inlineStr"/>
+      <c r="S135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -8596,9 +9390,15 @@
       <c r="P136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q136" t="inlineStr">
-        <is>
-          <t>2618</t>
+      <c r="Q136" t="n">
+        <v>2618</v>
+      </c>
+      <c r="R136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S136" t="inlineStr">
+        <is>
+          <t>2660</t>
         </is>
       </c>
     </row>
@@ -8657,7 +9457,13 @@
       <c r="P137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q137" t="inlineStr">
+      <c r="Q137" t="n">
+        <v>0</v>
+      </c>
+      <c r="R137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8709,6 +9515,8 @@
       <c r="O138" t="inlineStr"/>
       <c r="P138" s="3" t="inlineStr"/>
       <c r="Q138" t="inlineStr"/>
+      <c r="R138" s="3" t="inlineStr"/>
+      <c r="S138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -8765,9 +9573,15 @@
       <c r="P139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q139" t="inlineStr">
-        <is>
-          <t>2365</t>
+      <c r="Q139" t="n">
+        <v>2365</v>
+      </c>
+      <c r="R139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S139" t="inlineStr">
+        <is>
+          <t>2346</t>
         </is>
       </c>
     </row>
@@ -8826,9 +9640,15 @@
       <c r="P140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q140" t="inlineStr">
-        <is>
-          <t>2621</t>
+      <c r="Q140" t="n">
+        <v>2621</v>
+      </c>
+      <c r="R140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S140" t="inlineStr">
+        <is>
+          <t>2571</t>
         </is>
       </c>
     </row>
@@ -8878,6 +9698,8 @@
       <c r="O141" t="inlineStr"/>
       <c r="P141" s="3" t="inlineStr"/>
       <c r="Q141" t="inlineStr"/>
+      <c r="R141" s="3" t="inlineStr"/>
+      <c r="S141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -8934,9 +9756,15 @@
       <c r="P142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q142" t="inlineStr">
-        <is>
-          <t>2020</t>
+      <c r="Q142" t="n">
+        <v>2020</v>
+      </c>
+      <c r="R142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S142" t="inlineStr">
+        <is>
+          <t>2096</t>
         </is>
       </c>
     </row>
@@ -8986,6 +9814,8 @@
       <c r="O143" t="inlineStr"/>
       <c r="P143" s="3" t="inlineStr"/>
       <c r="Q143" t="inlineStr"/>
+      <c r="R143" s="3" t="inlineStr"/>
+      <c r="S143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -9033,6 +9863,8 @@
       <c r="O144" t="inlineStr"/>
       <c r="P144" s="3" t="inlineStr"/>
       <c r="Q144" t="inlineStr"/>
+      <c r="R144" s="3" t="inlineStr"/>
+      <c r="S144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -9080,6 +9912,8 @@
       <c r="O145" t="inlineStr"/>
       <c r="P145" s="3" t="inlineStr"/>
       <c r="Q145" t="inlineStr"/>
+      <c r="R145" s="3" t="inlineStr"/>
+      <c r="S145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -9127,6 +9961,8 @@
       <c r="O146" t="inlineStr"/>
       <c r="P146" s="3" t="inlineStr"/>
       <c r="Q146" t="inlineStr"/>
+      <c r="R146" s="3" t="inlineStr"/>
+      <c r="S146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -9174,6 +10010,8 @@
       <c r="O147" t="inlineStr"/>
       <c r="P147" s="3" t="inlineStr"/>
       <c r="Q147" t="inlineStr"/>
+      <c r="R147" s="3" t="inlineStr"/>
+      <c r="S147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -9230,9 +10068,15 @@
       <c r="P148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q148" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="Q148" t="n">
+        <v>0</v>
+      </c>
+      <c r="R148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S148" t="inlineStr">
+        <is>
+          <t>1522</t>
         </is>
       </c>
     </row>
@@ -9291,9 +10135,15 @@
       <c r="P149" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="Q149" t="inlineStr">
-        <is>
-          <t>2875</t>
+      <c r="Q149" t="n">
+        <v>2875</v>
+      </c>
+      <c r="R149" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S149" t="inlineStr">
+        <is>
+          <t>3638</t>
         </is>
       </c>
     </row>
@@ -9352,7 +10202,13 @@
       <c r="P150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q150" t="inlineStr">
+      <c r="Q150" t="n">
+        <v>0</v>
+      </c>
+      <c r="R150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9413,7 +10269,13 @@
       <c r="P151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q151" t="inlineStr">
+      <c r="Q151" t="n">
+        <v>0</v>
+      </c>
+      <c r="R151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9474,7 +10336,13 @@
       <c r="P152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q152" t="inlineStr">
+      <c r="Q152" t="n">
+        <v>0</v>
+      </c>
+      <c r="R152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9535,7 +10403,13 @@
       <c r="P153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q153" t="inlineStr">
+      <c r="Q153" t="n">
+        <v>0</v>
+      </c>
+      <c r="R153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9596,7 +10470,13 @@
       <c r="P154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q154" t="inlineStr">
+      <c r="Q154" t="n">
+        <v>0</v>
+      </c>
+      <c r="R154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9657,9 +10537,15 @@
       <c r="P155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q155" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="Q155" t="n">
+        <v>0</v>
+      </c>
+      <c r="R155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S155" t="inlineStr">
+        <is>
+          <t>2528</t>
         </is>
       </c>
     </row>
@@ -9712,9 +10598,15 @@
       <c r="P156" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q156" t="inlineStr">
-        <is>
-          <t>3149</t>
+      <c r="Q156" t="n">
+        <v>3149</v>
+      </c>
+      <c r="R156" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S156" t="inlineStr">
+        <is>
+          <t>3228</t>
         </is>
       </c>
     </row>
@@ -9758,6 +10650,8 @@
       <c r="O157" t="inlineStr"/>
       <c r="P157" s="3" t="inlineStr"/>
       <c r="Q157" t="inlineStr"/>
+      <c r="R157" s="3" t="inlineStr"/>
+      <c r="S157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -9808,7 +10702,13 @@
       <c r="P158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q158" t="inlineStr">
+      <c r="Q158" t="n">
+        <v>0</v>
+      </c>
+      <c r="R158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9863,9 +10763,15 @@
       <c r="P159" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q159" t="inlineStr">
-        <is>
-          <t>2708</t>
+      <c r="Q159" t="n">
+        <v>2708</v>
+      </c>
+      <c r="R159" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S159" t="inlineStr">
+        <is>
+          <t>2779</t>
         </is>
       </c>
     </row>
@@ -9909,6 +10815,8 @@
       <c r="O160" t="inlineStr"/>
       <c r="P160" s="3" t="inlineStr"/>
       <c r="Q160" t="inlineStr"/>
+      <c r="R160" s="3" t="inlineStr"/>
+      <c r="S160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -9947,9 +10855,15 @@
       <c r="P161" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="Q161" t="inlineStr">
-        <is>
-          <t>2593</t>
+      <c r="Q161" t="n">
+        <v>2593</v>
+      </c>
+      <c r="R161" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="S161" t="inlineStr">
+        <is>
+          <t>2666</t>
         </is>
       </c>
     </row>
@@ -9990,9 +10904,15 @@
       <c r="P162" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="Q162" t="inlineStr">
-        <is>
-          <t>2432</t>
+      <c r="Q162" t="n">
+        <v>2432</v>
+      </c>
+      <c r="R162" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="S162" t="inlineStr">
+        <is>
+          <t>2430</t>
         </is>
       </c>
     </row>
@@ -10029,9 +10949,15 @@
       <c r="P163" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q163" t="inlineStr">
-        <is>
-          <t>2987</t>
+      <c r="Q163" t="n">
+        <v>2987</v>
+      </c>
+      <c r="R163" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S163" t="inlineStr">
+        <is>
+          <t>2965</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-02-20 11:30:33
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S163"/>
+  <dimension ref="A1:U165"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,6 +486,16 @@
           <t>02-18_0</t>
         </is>
       </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>02-19_A</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>02-19_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -548,9 +558,15 @@
       <c r="R2" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>3429</t>
+      <c r="S2" t="n">
+        <v>3429</v>
+      </c>
+      <c r="T2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>3461</t>
         </is>
       </c>
     </row>
@@ -615,9 +631,15 @@
       <c r="R3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>4196</t>
+      <c r="S3" t="n">
+        <v>4196</v>
+      </c>
+      <c r="T3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>4551</t>
         </is>
       </c>
     </row>
@@ -682,9 +704,15 @@
       <c r="R4" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>4934</t>
+      <c r="S4" t="n">
+        <v>4934</v>
+      </c>
+      <c r="T4" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>5201</t>
         </is>
       </c>
     </row>
@@ -749,9 +777,15 @@
       <c r="R5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>3964</t>
+      <c r="S5" t="n">
+        <v>3964</v>
+      </c>
+      <c r="T5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>4456</t>
         </is>
       </c>
     </row>
@@ -816,9 +850,15 @@
       <c r="R6" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>4592</t>
+      <c r="S6" t="n">
+        <v>4592</v>
+      </c>
+      <c r="T6" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>4836</t>
         </is>
       </c>
     </row>
@@ -883,9 +923,15 @@
       <c r="R7" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>5032</t>
+      <c r="S7" t="n">
+        <v>5032</v>
+      </c>
+      <c r="T7" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>5392</t>
         </is>
       </c>
     </row>
@@ -950,9 +996,15 @@
       <c r="R8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>4300</t>
+      <c r="S8" t="n">
+        <v>4300</v>
+      </c>
+      <c r="T8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>4548</t>
         </is>
       </c>
     </row>
@@ -1017,9 +1069,15 @@
       <c r="R9" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>4279</t>
+      <c r="S9" t="n">
+        <v>4279</v>
+      </c>
+      <c r="T9" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>4660</t>
         </is>
       </c>
     </row>
@@ -1084,9 +1142,15 @@
       <c r="R10" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>4556</t>
+      <c r="S10" t="n">
+        <v>4556</v>
+      </c>
+      <c r="T10" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>5078</t>
         </is>
       </c>
     </row>
@@ -1151,9 +1215,15 @@
       <c r="R11" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>4048</t>
+      <c r="S11" t="n">
+        <v>4048</v>
+      </c>
+      <c r="T11" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>4156</t>
         </is>
       </c>
     </row>
@@ -1218,7 +1288,13 @@
       <c r="R12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S12" t="inlineStr">
+      <c r="S12" t="n">
+        <v>2835</v>
+      </c>
+      <c r="T12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U12" t="inlineStr">
         <is>
           <t>2835</t>
         </is>
@@ -1285,9 +1361,15 @@
       <c r="R13" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>5370</t>
+      <c r="S13" t="n">
+        <v>5370</v>
+      </c>
+      <c r="T13" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>5592</t>
         </is>
       </c>
     </row>
@@ -1352,9 +1434,15 @@
       <c r="R14" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>4482</t>
+      <c r="S14" t="n">
+        <v>4482</v>
+      </c>
+      <c r="T14" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>4755</t>
         </is>
       </c>
     </row>
@@ -1419,9 +1507,15 @@
       <c r="R15" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="S15" t="inlineStr">
-        <is>
-          <t>4002</t>
+      <c r="S15" t="n">
+        <v>4002</v>
+      </c>
+      <c r="T15" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>4302</t>
         </is>
       </c>
     </row>
@@ -1486,9 +1580,15 @@
       <c r="R16" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="S16" t="inlineStr">
-        <is>
-          <t>4454</t>
+      <c r="S16" t="n">
+        <v>4454</v>
+      </c>
+      <c r="T16" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>4727</t>
         </is>
       </c>
     </row>
@@ -1553,9 +1653,15 @@
       <c r="R17" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="S17" t="inlineStr">
-        <is>
-          <t>3863</t>
+      <c r="S17" t="n">
+        <v>3863</v>
+      </c>
+      <c r="T17" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>4085</t>
         </is>
       </c>
     </row>
@@ -1620,9 +1726,15 @@
       <c r="R18" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>3805</t>
+      <c r="S18" t="n">
+        <v>3805</v>
+      </c>
+      <c r="T18" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>3874</t>
         </is>
       </c>
     </row>
@@ -1687,9 +1799,15 @@
       <c r="R19" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S19" t="inlineStr">
-        <is>
-          <t>4466</t>
+      <c r="S19" t="n">
+        <v>4466</v>
+      </c>
+      <c r="T19" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>4747</t>
         </is>
       </c>
     </row>
@@ -1754,9 +1872,15 @@
       <c r="R20" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="S20" t="inlineStr">
-        <is>
-          <t>5324</t>
+      <c r="S20" t="n">
+        <v>5324</v>
+      </c>
+      <c r="T20" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>5634</t>
         </is>
       </c>
     </row>
@@ -1821,9 +1945,15 @@
       <c r="R21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S21" t="inlineStr">
-        <is>
-          <t>3509</t>
+      <c r="S21" t="n">
+        <v>3509</v>
+      </c>
+      <c r="T21" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>3920</t>
         </is>
       </c>
     </row>
@@ -1888,9 +2018,15 @@
       <c r="R22" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="S22" t="inlineStr">
-        <is>
-          <t>4555</t>
+      <c r="S22" t="n">
+        <v>4555</v>
+      </c>
+      <c r="T22" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>4612</t>
         </is>
       </c>
     </row>
@@ -1955,9 +2091,15 @@
       <c r="R23" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="S23" t="inlineStr">
-        <is>
-          <t>4203</t>
+      <c r="S23" t="n">
+        <v>4203</v>
+      </c>
+      <c r="T23" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>4389</t>
         </is>
       </c>
     </row>
@@ -2022,9 +2164,15 @@
       <c r="R24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="S24" t="inlineStr">
-        <is>
-          <t>4533</t>
+      <c r="S24" t="n">
+        <v>4533</v>
+      </c>
+      <c r="T24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>4970</t>
         </is>
       </c>
     </row>
@@ -2089,7 +2237,13 @@
       <c r="R25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S25" t="inlineStr">
+      <c r="S25" t="n">
+        <v>0</v>
+      </c>
+      <c r="T25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2156,9 +2310,15 @@
       <c r="R26" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="S26" t="inlineStr">
-        <is>
-          <t>4661</t>
+      <c r="S26" t="n">
+        <v>4661</v>
+      </c>
+      <c r="T26" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>4880</t>
         </is>
       </c>
     </row>
@@ -2223,9 +2383,15 @@
       <c r="R27" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="S27" t="inlineStr">
-        <is>
-          <t>4675</t>
+      <c r="S27" t="n">
+        <v>4675</v>
+      </c>
+      <c r="T27" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>4994</t>
         </is>
       </c>
     </row>
@@ -2290,9 +2456,15 @@
       <c r="R28" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="S28" t="inlineStr">
-        <is>
-          <t>3766</t>
+      <c r="S28" t="n">
+        <v>3766</v>
+      </c>
+      <c r="T28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>3967</t>
         </is>
       </c>
     </row>
@@ -2357,9 +2529,15 @@
       <c r="R29" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="S29" t="inlineStr">
-        <is>
-          <t>5294</t>
+      <c r="S29" t="n">
+        <v>5294</v>
+      </c>
+      <c r="T29" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>5566</t>
         </is>
       </c>
     </row>
@@ -2424,9 +2602,15 @@
       <c r="R30" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="S30" t="inlineStr">
-        <is>
-          <t>4103</t>
+      <c r="S30" t="n">
+        <v>4103</v>
+      </c>
+      <c r="T30" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>4222</t>
         </is>
       </c>
     </row>
@@ -2491,9 +2675,15 @@
       <c r="R31" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="S31" t="inlineStr">
-        <is>
-          <t>4797</t>
+      <c r="S31" t="n">
+        <v>4797</v>
+      </c>
+      <c r="T31" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>5211</t>
         </is>
       </c>
     </row>
@@ -2516,7 +2706,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F32" s="4" t="n">
@@ -2558,7 +2748,13 @@
       <c r="R32" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S32" t="inlineStr">
+      <c r="S32" t="n">
+        <v>4182</v>
+      </c>
+      <c r="T32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U32" t="inlineStr">
         <is>
           <t>4182</t>
         </is>
@@ -2625,9 +2821,15 @@
       <c r="R33" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="S33" t="inlineStr">
-        <is>
-          <t>4487</t>
+      <c r="S33" t="n">
+        <v>4487</v>
+      </c>
+      <c r="T33" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="U33" t="inlineStr">
+        <is>
+          <t>4674</t>
         </is>
       </c>
     </row>
@@ -2692,9 +2894,15 @@
       <c r="R34" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S34" t="inlineStr">
-        <is>
-          <t>4614</t>
+      <c r="S34" t="n">
+        <v>4614</v>
+      </c>
+      <c r="T34" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U34" t="inlineStr">
+        <is>
+          <t>4760</t>
         </is>
       </c>
     </row>
@@ -2717,7 +2925,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F35" s="4" t="n">
@@ -2759,9 +2967,15 @@
       <c r="R35" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="S35" t="inlineStr">
-        <is>
-          <t>4546</t>
+      <c r="S35" t="n">
+        <v>4546</v>
+      </c>
+      <c r="T35" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="U35" t="inlineStr">
+        <is>
+          <t>4769</t>
         </is>
       </c>
     </row>
@@ -2826,9 +3040,15 @@
       <c r="R36" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S36" t="inlineStr">
-        <is>
-          <t>4609</t>
+      <c r="S36" t="n">
+        <v>4609</v>
+      </c>
+      <c r="T36" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U36" t="inlineStr">
+        <is>
+          <t>4746</t>
         </is>
       </c>
     </row>
@@ -2893,9 +3113,15 @@
       <c r="R37" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S37" t="inlineStr">
-        <is>
-          <t>4035</t>
+      <c r="S37" t="n">
+        <v>4035</v>
+      </c>
+      <c r="T37" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U37" t="inlineStr">
+        <is>
+          <t>4180</t>
         </is>
       </c>
     </row>
@@ -2960,9 +3186,15 @@
       <c r="R38" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="S38" t="inlineStr">
-        <is>
-          <t>4509</t>
+      <c r="S38" t="n">
+        <v>4509</v>
+      </c>
+      <c r="T38" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="U38" t="inlineStr">
+        <is>
+          <t>4542</t>
         </is>
       </c>
     </row>
@@ -3027,9 +3259,15 @@
       <c r="R39" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="S39" t="inlineStr">
-        <is>
-          <t>4568</t>
+      <c r="S39" t="n">
+        <v>4568</v>
+      </c>
+      <c r="T39" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="U39" t="inlineStr">
+        <is>
+          <t>4831</t>
         </is>
       </c>
     </row>
@@ -3094,9 +3332,15 @@
       <c r="R40" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="S40" t="inlineStr">
-        <is>
-          <t>5064</t>
+      <c r="S40" t="n">
+        <v>5064</v>
+      </c>
+      <c r="T40" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U40" t="inlineStr">
+        <is>
+          <t>5381</t>
         </is>
       </c>
     </row>
@@ -3161,7 +3405,13 @@
       <c r="R41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S41" t="inlineStr">
+      <c r="S41" t="n">
+        <v>3632</v>
+      </c>
+      <c r="T41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U41" t="inlineStr">
         <is>
           <t>3632</t>
         </is>
@@ -3228,9 +3478,15 @@
       <c r="R42" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="S42" t="inlineStr">
-        <is>
-          <t>4996</t>
+      <c r="S42" t="n">
+        <v>4996</v>
+      </c>
+      <c r="T42" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="U42" t="inlineStr">
+        <is>
+          <t>5329</t>
         </is>
       </c>
     </row>
@@ -3295,9 +3551,15 @@
       <c r="R43" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="S43" t="inlineStr">
-        <is>
-          <t>4792</t>
+      <c r="S43" t="n">
+        <v>4792</v>
+      </c>
+      <c r="T43" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U43" t="inlineStr">
+        <is>
+          <t>5058</t>
         </is>
       </c>
     </row>
@@ -3362,9 +3624,15 @@
       <c r="R44" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="S44" t="inlineStr">
-        <is>
-          <t>4735</t>
+      <c r="S44" t="n">
+        <v>4735</v>
+      </c>
+      <c r="T44" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="U44" t="inlineStr">
+        <is>
+          <t>4862</t>
         </is>
       </c>
     </row>
@@ -3429,9 +3697,15 @@
       <c r="R45" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="S45" t="inlineStr">
-        <is>
-          <t>4240</t>
+      <c r="S45" t="n">
+        <v>4240</v>
+      </c>
+      <c r="T45" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U45" t="inlineStr">
+        <is>
+          <t>4391</t>
         </is>
       </c>
     </row>
@@ -3496,9 +3770,15 @@
       <c r="R46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S46" t="inlineStr">
-        <is>
-          <t>4243</t>
+      <c r="S46" t="n">
+        <v>4243</v>
+      </c>
+      <c r="T46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U46" t="inlineStr">
+        <is>
+          <t>4362</t>
         </is>
       </c>
     </row>
@@ -3563,7 +3843,13 @@
       <c r="R47" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S47" t="inlineStr">
+      <c r="S47" t="n">
+        <v>2500</v>
+      </c>
+      <c r="T47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U47" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -3630,9 +3916,15 @@
       <c r="R48" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="S48" t="inlineStr">
-        <is>
-          <t>4765</t>
+      <c r="S48" t="n">
+        <v>4765</v>
+      </c>
+      <c r="T48" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="U48" t="inlineStr">
+        <is>
+          <t>4992</t>
         </is>
       </c>
     </row>
@@ -3697,9 +3989,15 @@
       <c r="R49" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S49" t="inlineStr">
-        <is>
-          <t>3720</t>
+      <c r="S49" t="n">
+        <v>3720</v>
+      </c>
+      <c r="T49" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U49" t="inlineStr">
+        <is>
+          <t>3803</t>
         </is>
       </c>
     </row>
@@ -3764,9 +4062,15 @@
       <c r="R50" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="S50" t="inlineStr">
-        <is>
-          <t>4934</t>
+      <c r="S50" t="n">
+        <v>4934</v>
+      </c>
+      <c r="T50" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="U50" t="inlineStr">
+        <is>
+          <t>5228</t>
         </is>
       </c>
     </row>
@@ -3831,9 +4135,15 @@
       <c r="R51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S51" t="inlineStr">
-        <is>
-          <t>2833</t>
+      <c r="S51" t="n">
+        <v>2833</v>
+      </c>
+      <c r="T51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U51" t="inlineStr">
+        <is>
+          <t>2845</t>
         </is>
       </c>
     </row>
@@ -3898,9 +4208,15 @@
       <c r="R52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S52" t="inlineStr">
-        <is>
-          <t>2660</t>
+      <c r="S52" t="n">
+        <v>2660</v>
+      </c>
+      <c r="T52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U52" t="inlineStr">
+        <is>
+          <t>2720</t>
         </is>
       </c>
     </row>
@@ -3965,9 +4281,15 @@
       <c r="R53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S53" t="inlineStr">
-        <is>
-          <t>2628</t>
+      <c r="S53" t="n">
+        <v>2628</v>
+      </c>
+      <c r="T53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U53" t="inlineStr">
+        <is>
+          <t>2658</t>
         </is>
       </c>
     </row>
@@ -4032,9 +4354,15 @@
       <c r="R54" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="S54" t="inlineStr">
-        <is>
-          <t>4685</t>
+      <c r="S54" t="n">
+        <v>4685</v>
+      </c>
+      <c r="T54" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="U54" t="inlineStr">
+        <is>
+          <t>4945</t>
         </is>
       </c>
     </row>
@@ -4099,9 +4427,15 @@
       <c r="R55" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="S55" t="inlineStr">
-        <is>
-          <t>3676</t>
+      <c r="S55" t="n">
+        <v>3676</v>
+      </c>
+      <c r="T55" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="U55" t="inlineStr">
+        <is>
+          <t>3848</t>
         </is>
       </c>
     </row>
@@ -4166,9 +4500,15 @@
       <c r="R56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S56" t="inlineStr">
-        <is>
-          <t>3740</t>
+      <c r="S56" t="n">
+        <v>3740</v>
+      </c>
+      <c r="T56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U56" t="inlineStr">
+        <is>
+          <t>3901</t>
         </is>
       </c>
     </row>
@@ -4233,9 +4573,15 @@
       <c r="R57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S57" t="inlineStr">
-        <is>
-          <t>4443</t>
+      <c r="S57" t="n">
+        <v>4443</v>
+      </c>
+      <c r="T57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U57" t="inlineStr">
+        <is>
+          <t>4644</t>
         </is>
       </c>
     </row>
@@ -4300,9 +4646,15 @@
       <c r="R58" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="S58" t="inlineStr">
-        <is>
-          <t>3733</t>
+      <c r="S58" t="n">
+        <v>3733</v>
+      </c>
+      <c r="T58" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U58" t="inlineStr">
+        <is>
+          <t>3872</t>
         </is>
       </c>
     </row>
@@ -4338,6 +4690,8 @@
       <c r="Q59" t="inlineStr"/>
       <c r="R59" s="3" t="inlineStr"/>
       <c r="S59" t="inlineStr"/>
+      <c r="T59" s="3" t="inlineStr"/>
+      <c r="U59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -4371,6 +4725,8 @@
       <c r="Q60" t="inlineStr"/>
       <c r="R60" s="3" t="inlineStr"/>
       <c r="S60" t="inlineStr"/>
+      <c r="T60" s="3" t="inlineStr"/>
+      <c r="U60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -4433,9 +4789,15 @@
       <c r="R61" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S61" t="inlineStr">
-        <is>
-          <t>4289</t>
+      <c r="S61" t="n">
+        <v>4289</v>
+      </c>
+      <c r="T61" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U61" t="inlineStr">
+        <is>
+          <t>4422</t>
         </is>
       </c>
     </row>
@@ -4500,7 +4862,13 @@
       <c r="R62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S62" t="inlineStr">
+      <c r="S62" t="n">
+        <v>0</v>
+      </c>
+      <c r="T62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4567,9 +4935,15 @@
       <c r="R63" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="S63" t="inlineStr">
-        <is>
-          <t>4381</t>
+      <c r="S63" t="n">
+        <v>4381</v>
+      </c>
+      <c r="T63" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="U63" t="inlineStr">
+        <is>
+          <t>4606</t>
         </is>
       </c>
     </row>
@@ -4634,9 +5008,15 @@
       <c r="R64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S64" t="inlineStr">
-        <is>
-          <t>2533</t>
+      <c r="S64" t="n">
+        <v>2533</v>
+      </c>
+      <c r="T64" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="U64" t="inlineStr">
+        <is>
+          <t>2887</t>
         </is>
       </c>
     </row>
@@ -4672,6 +5052,8 @@
       <c r="Q65" t="inlineStr"/>
       <c r="R65" s="3" t="inlineStr"/>
       <c r="S65" t="inlineStr"/>
+      <c r="T65" s="3" t="inlineStr"/>
+      <c r="U65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -4734,9 +5116,15 @@
       <c r="R66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S66" t="inlineStr">
-        <is>
-          <t>2397</t>
+      <c r="S66" t="n">
+        <v>2397</v>
+      </c>
+      <c r="T66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U66" t="inlineStr">
+        <is>
+          <t>2393</t>
         </is>
       </c>
     </row>
@@ -4801,9 +5189,15 @@
       <c r="R67" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="S67" t="inlineStr">
-        <is>
-          <t>4153</t>
+      <c r="S67" t="n">
+        <v>4153</v>
+      </c>
+      <c r="T67" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="U67" t="inlineStr">
+        <is>
+          <t>4367</t>
         </is>
       </c>
     </row>
@@ -4868,9 +5262,15 @@
       <c r="R68" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="S68" t="inlineStr">
-        <is>
-          <t>4652</t>
+      <c r="S68" t="n">
+        <v>4652</v>
+      </c>
+      <c r="T68" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U68" t="inlineStr">
+        <is>
+          <t>4869</t>
         </is>
       </c>
     </row>
@@ -4935,9 +5335,15 @@
       <c r="R69" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="S69" t="inlineStr">
-        <is>
-          <t>3830</t>
+      <c r="S69" t="n">
+        <v>3830</v>
+      </c>
+      <c r="T69" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U69" t="inlineStr">
+        <is>
+          <t>4009</t>
         </is>
       </c>
     </row>
@@ -5002,7 +5408,13 @@
       <c r="R70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S70" t="inlineStr">
+      <c r="S70" t="n">
+        <v>2645</v>
+      </c>
+      <c r="T70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U70" t="inlineStr">
         <is>
           <t>2645</t>
         </is>
@@ -5069,9 +5481,15 @@
       <c r="R71" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="S71" t="inlineStr">
-        <is>
-          <t>3889</t>
+      <c r="S71" t="n">
+        <v>3889</v>
+      </c>
+      <c r="T71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U71" t="inlineStr">
+        <is>
+          <t>3900</t>
         </is>
       </c>
     </row>
@@ -5136,9 +5554,15 @@
       <c r="R72" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="S72" t="inlineStr">
-        <is>
-          <t>3282</t>
+      <c r="S72" t="n">
+        <v>3282</v>
+      </c>
+      <c r="T72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U72" t="inlineStr">
+        <is>
+          <t>3271</t>
         </is>
       </c>
     </row>
@@ -5203,9 +5627,15 @@
       <c r="R73" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S73" t="inlineStr">
-        <is>
-          <t>3765</t>
+      <c r="S73" t="n">
+        <v>3765</v>
+      </c>
+      <c r="T73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U73" t="inlineStr">
+        <is>
+          <t>3876</t>
         </is>
       </c>
     </row>
@@ -5270,9 +5700,15 @@
       <c r="R74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S74" t="inlineStr">
-        <is>
-          <t>2769</t>
+      <c r="S74" t="n">
+        <v>2769</v>
+      </c>
+      <c r="T74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U74" t="inlineStr">
+        <is>
+          <t>2768</t>
         </is>
       </c>
     </row>
@@ -5337,9 +5773,15 @@
       <c r="R75" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="S75" t="inlineStr">
-        <is>
-          <t>3591</t>
+      <c r="S75" t="n">
+        <v>3591</v>
+      </c>
+      <c r="T75" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="U75" t="inlineStr">
+        <is>
+          <t>3679</t>
         </is>
       </c>
     </row>
@@ -5404,9 +5846,15 @@
       <c r="R76" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="S76" t="inlineStr">
-        <is>
-          <t>4259</t>
+      <c r="S76" t="n">
+        <v>4259</v>
+      </c>
+      <c r="T76" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="U76" t="inlineStr">
+        <is>
+          <t>4450</t>
         </is>
       </c>
     </row>
@@ -5471,7 +5919,13 @@
       <c r="R77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S77" t="inlineStr">
+      <c r="S77" t="n">
+        <v>3353</v>
+      </c>
+      <c r="T77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U77" t="inlineStr">
         <is>
           <t>3353</t>
         </is>
@@ -5538,9 +5992,15 @@
       <c r="R78" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S78" t="inlineStr">
-        <is>
-          <t>4426</t>
+      <c r="S78" t="n">
+        <v>4426</v>
+      </c>
+      <c r="T78" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U78" t="inlineStr">
+        <is>
+          <t>4545</t>
         </is>
       </c>
     </row>
@@ -5605,7 +6065,13 @@
       <c r="R79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S79" t="inlineStr">
+      <c r="S79" t="n">
+        <v>0</v>
+      </c>
+      <c r="T79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5672,9 +6138,15 @@
       <c r="R80" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S80" t="inlineStr">
-        <is>
-          <t>4153</t>
+      <c r="S80" t="n">
+        <v>4153</v>
+      </c>
+      <c r="T80" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="U80" t="inlineStr">
+        <is>
+          <t>4302</t>
         </is>
       </c>
     </row>
@@ -5739,9 +6211,15 @@
       <c r="R81" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="S81" t="inlineStr">
-        <is>
-          <t>4137</t>
+      <c r="S81" t="n">
+        <v>4137</v>
+      </c>
+      <c r="T81" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U81" t="inlineStr">
+        <is>
+          <t>4334</t>
         </is>
       </c>
     </row>
@@ -5806,9 +6284,15 @@
       <c r="R82" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="S82" t="inlineStr">
-        <is>
-          <t>3923</t>
+      <c r="S82" t="n">
+        <v>3923</v>
+      </c>
+      <c r="T82" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="U82" t="inlineStr">
+        <is>
+          <t>4154</t>
         </is>
       </c>
     </row>
@@ -5873,9 +6357,15 @@
       <c r="R83" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="S83" t="inlineStr">
-        <is>
-          <t>3841</t>
+      <c r="S83" t="n">
+        <v>3841</v>
+      </c>
+      <c r="T83" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="U83" t="inlineStr">
+        <is>
+          <t>3995</t>
         </is>
       </c>
     </row>
@@ -5940,9 +6430,15 @@
       <c r="R84" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="S84" t="inlineStr">
-        <is>
-          <t>2906</t>
+      <c r="S84" t="n">
+        <v>2906</v>
+      </c>
+      <c r="T84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U84" t="inlineStr">
+        <is>
+          <t>2975</t>
         </is>
       </c>
     </row>
@@ -6007,9 +6503,15 @@
       <c r="R85" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="S85" t="inlineStr">
-        <is>
-          <t>3308</t>
+      <c r="S85" t="n">
+        <v>3308</v>
+      </c>
+      <c r="T85" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U85" t="inlineStr">
+        <is>
+          <t>3412</t>
         </is>
       </c>
     </row>
@@ -6074,9 +6576,15 @@
       <c r="R86" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="S86" t="inlineStr">
-        <is>
-          <t>3033</t>
+      <c r="S86" t="n">
+        <v>3033</v>
+      </c>
+      <c r="T86" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="U86" t="inlineStr">
+        <is>
+          <t>3178</t>
         </is>
       </c>
     </row>
@@ -6141,9 +6649,15 @@
       <c r="R87" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S87" t="inlineStr">
-        <is>
-          <t>4032</t>
+      <c r="S87" t="n">
+        <v>4032</v>
+      </c>
+      <c r="T87" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U87" t="inlineStr">
+        <is>
+          <t>4268</t>
         </is>
       </c>
     </row>
@@ -6208,9 +6722,15 @@
       <c r="R88" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S88" t="inlineStr">
-        <is>
-          <t>2894</t>
+      <c r="S88" t="n">
+        <v>2894</v>
+      </c>
+      <c r="T88" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U88" t="inlineStr">
+        <is>
+          <t>2869</t>
         </is>
       </c>
     </row>
@@ -6275,9 +6795,15 @@
       <c r="R89" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S89" t="inlineStr">
-        <is>
-          <t>2993</t>
+      <c r="S89" t="n">
+        <v>2993</v>
+      </c>
+      <c r="T89" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="U89" t="inlineStr">
+        <is>
+          <t>3098</t>
         </is>
       </c>
     </row>
@@ -6342,9 +6868,15 @@
       <c r="R90" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S90" t="inlineStr">
-        <is>
-          <t>2785</t>
+      <c r="S90" t="n">
+        <v>2785</v>
+      </c>
+      <c r="T90" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="U90" t="inlineStr">
+        <is>
+          <t>2801</t>
         </is>
       </c>
     </row>
@@ -6409,9 +6941,15 @@
       <c r="R91" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S91" t="inlineStr">
-        <is>
-          <t>2792</t>
+      <c r="S91" t="n">
+        <v>2792</v>
+      </c>
+      <c r="T91" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U91" t="inlineStr">
+        <is>
+          <t>2800</t>
         </is>
       </c>
     </row>
@@ -6476,7 +7014,13 @@
       <c r="R92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S92" t="inlineStr">
+      <c r="S92" t="n">
+        <v>0</v>
+      </c>
+      <c r="T92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6543,9 +7087,15 @@
       <c r="R93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S93" t="inlineStr">
-        <is>
-          <t>2397</t>
+      <c r="S93" t="n">
+        <v>2397</v>
+      </c>
+      <c r="T93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U93" t="inlineStr">
+        <is>
+          <t>2396</t>
         </is>
       </c>
     </row>
@@ -6610,9 +7160,15 @@
       <c r="R94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S94" t="inlineStr">
-        <is>
-          <t>3012</t>
+      <c r="S94" t="n">
+        <v>3012</v>
+      </c>
+      <c r="T94" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U94" t="inlineStr">
+        <is>
+          <t>3217</t>
         </is>
       </c>
     </row>
@@ -6677,9 +7233,15 @@
       <c r="R95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S95" t="inlineStr">
-        <is>
-          <t>2619</t>
+      <c r="S95" t="n">
+        <v>2619</v>
+      </c>
+      <c r="T95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U95" t="inlineStr">
+        <is>
+          <t>2576</t>
         </is>
       </c>
     </row>
@@ -6744,9 +7306,15 @@
       <c r="R96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S96" t="inlineStr">
-        <is>
-          <t>3245</t>
+      <c r="S96" t="n">
+        <v>3245</v>
+      </c>
+      <c r="T96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U96" t="inlineStr">
+        <is>
+          <t>3182</t>
         </is>
       </c>
     </row>
@@ -6811,7 +7379,13 @@
       <c r="R97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S97" t="inlineStr">
+      <c r="S97" t="n">
+        <v>2545</v>
+      </c>
+      <c r="T97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U97" t="inlineStr">
         <is>
           <t>2545</t>
         </is>
@@ -6878,7 +7452,13 @@
       <c r="R98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S98" t="inlineStr">
+      <c r="S98" t="n">
+        <v>0</v>
+      </c>
+      <c r="T98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6945,9 +7525,15 @@
       <c r="R99" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="S99" t="inlineStr">
-        <is>
-          <t>3415</t>
+      <c r="S99" t="n">
+        <v>3415</v>
+      </c>
+      <c r="T99" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U99" t="inlineStr">
+        <is>
+          <t>3517</t>
         </is>
       </c>
     </row>
@@ -7012,9 +7598,15 @@
       <c r="R100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S100" t="inlineStr">
-        <is>
-          <t>2458</t>
+      <c r="S100" t="n">
+        <v>2458</v>
+      </c>
+      <c r="T100" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="U100" t="inlineStr">
+        <is>
+          <t>2463</t>
         </is>
       </c>
     </row>
@@ -7079,9 +7671,15 @@
       <c r="R101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S101" t="inlineStr">
-        <is>
-          <t>3893</t>
+      <c r="S101" t="n">
+        <v>3893</v>
+      </c>
+      <c r="T101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U101" t="inlineStr">
+        <is>
+          <t>4010</t>
         </is>
       </c>
     </row>
@@ -7146,9 +7744,15 @@
       <c r="R102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S102" t="inlineStr">
-        <is>
-          <t>3535</t>
+      <c r="S102" t="n">
+        <v>3535</v>
+      </c>
+      <c r="T102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U102" t="inlineStr">
+        <is>
+          <t>3593</t>
         </is>
       </c>
     </row>
@@ -7213,9 +7817,15 @@
       <c r="R103" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="S103" t="inlineStr">
-        <is>
-          <t>2527</t>
+      <c r="S103" t="n">
+        <v>2527</v>
+      </c>
+      <c r="T103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U103" t="inlineStr">
+        <is>
+          <t>2537</t>
         </is>
       </c>
     </row>
@@ -7280,9 +7890,15 @@
       <c r="R104" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S104" t="inlineStr">
-        <is>
-          <t>3873</t>
+      <c r="S104" t="n">
+        <v>3873</v>
+      </c>
+      <c r="T104" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U104" t="inlineStr">
+        <is>
+          <t>4031</t>
         </is>
       </c>
     </row>
@@ -7347,9 +7963,15 @@
       <c r="R105" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="S105" t="inlineStr">
-        <is>
-          <t>3600</t>
+      <c r="S105" t="n">
+        <v>3600</v>
+      </c>
+      <c r="T105" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="U105" t="inlineStr">
+        <is>
+          <t>3728</t>
         </is>
       </c>
     </row>
@@ -7414,7 +8036,13 @@
       <c r="R106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S106" t="inlineStr">
+      <c r="S106" t="n">
+        <v>0</v>
+      </c>
+      <c r="T106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7481,9 +8109,15 @@
       <c r="R107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S107" t="inlineStr">
-        <is>
-          <t>2495</t>
+      <c r="S107" t="n">
+        <v>2495</v>
+      </c>
+      <c r="T107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U107" t="inlineStr">
+        <is>
+          <t>2487</t>
         </is>
       </c>
     </row>
@@ -7548,7 +8182,13 @@
       <c r="R108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S108" t="inlineStr">
+      <c r="S108" t="n">
+        <v>0</v>
+      </c>
+      <c r="T108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7615,9 +8255,15 @@
       <c r="R109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S109" t="inlineStr">
-        <is>
-          <t>3274</t>
+      <c r="S109" t="n">
+        <v>3274</v>
+      </c>
+      <c r="T109" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="U109" t="inlineStr">
+        <is>
+          <t>3419</t>
         </is>
       </c>
     </row>
@@ -7682,9 +8328,15 @@
       <c r="R110" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="S110" t="inlineStr">
-        <is>
-          <t>3364</t>
+      <c r="S110" t="n">
+        <v>3364</v>
+      </c>
+      <c r="T110" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="U110" t="inlineStr">
+        <is>
+          <t>3509</t>
         </is>
       </c>
     </row>
@@ -7749,9 +8401,15 @@
       <c r="R111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S111" t="inlineStr">
-        <is>
-          <t>2555</t>
+      <c r="S111" t="n">
+        <v>2555</v>
+      </c>
+      <c r="T111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U111" t="inlineStr">
+        <is>
+          <t>2585</t>
         </is>
       </c>
     </row>
@@ -7816,9 +8474,15 @@
       <c r="R112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S112" t="inlineStr">
-        <is>
-          <t>2818</t>
+      <c r="S112" t="n">
+        <v>2818</v>
+      </c>
+      <c r="T112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U112" t="inlineStr">
+        <is>
+          <t>2804</t>
         </is>
       </c>
     </row>
@@ -7883,9 +8547,15 @@
       <c r="R113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S113" t="inlineStr">
-        <is>
-          <t>3004</t>
+      <c r="S113" t="n">
+        <v>3004</v>
+      </c>
+      <c r="T113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U113" t="inlineStr">
+        <is>
+          <t>3082</t>
         </is>
       </c>
     </row>
@@ -7950,9 +8620,15 @@
       <c r="R114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S114" t="inlineStr">
-        <is>
-          <t>2628</t>
+      <c r="S114" t="n">
+        <v>2628</v>
+      </c>
+      <c r="T114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U114" t="inlineStr">
+        <is>
+          <t>2671</t>
         </is>
       </c>
     </row>
@@ -8017,9 +8693,15 @@
       <c r="R115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S115" t="inlineStr">
-        <is>
-          <t>2368</t>
+      <c r="S115" t="n">
+        <v>2368</v>
+      </c>
+      <c r="T115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U115" t="inlineStr">
+        <is>
+          <t>2356</t>
         </is>
       </c>
     </row>
@@ -8084,9 +8766,15 @@
       <c r="R116" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="S116" t="inlineStr">
-        <is>
-          <t>2978</t>
+      <c r="S116" t="n">
+        <v>2978</v>
+      </c>
+      <c r="T116" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="U116" t="inlineStr">
+        <is>
+          <t>3036</t>
         </is>
       </c>
     </row>
@@ -8151,9 +8839,15 @@
       <c r="R117" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S117" t="inlineStr">
-        <is>
-          <t>3356</t>
+      <c r="S117" t="n">
+        <v>3356</v>
+      </c>
+      <c r="T117" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U117" t="inlineStr">
+        <is>
+          <t>3446</t>
         </is>
       </c>
     </row>
@@ -8218,7 +8912,13 @@
       <c r="R118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S118" t="inlineStr">
+      <c r="S118" t="n">
+        <v>0</v>
+      </c>
+      <c r="T118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8285,9 +8985,15 @@
       <c r="R119" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S119" t="inlineStr">
-        <is>
-          <t>3660</t>
+      <c r="S119" t="n">
+        <v>3660</v>
+      </c>
+      <c r="T119" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U119" t="inlineStr">
+        <is>
+          <t>3765</t>
         </is>
       </c>
     </row>
@@ -8352,9 +9058,15 @@
       <c r="R120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S120" t="inlineStr">
-        <is>
-          <t>2443</t>
+      <c r="S120" t="n">
+        <v>2443</v>
+      </c>
+      <c r="T120" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="U120" t="inlineStr">
+        <is>
+          <t>2595</t>
         </is>
       </c>
     </row>
@@ -8419,9 +9131,15 @@
       <c r="R121" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="S121" t="inlineStr">
-        <is>
-          <t>3182</t>
+      <c r="S121" t="n">
+        <v>3182</v>
+      </c>
+      <c r="T121" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="U121" t="inlineStr">
+        <is>
+          <t>3225</t>
         </is>
       </c>
     </row>
@@ -8486,7 +9204,13 @@
       <c r="R122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S122" t="inlineStr">
+      <c r="S122" t="n">
+        <v>0</v>
+      </c>
+      <c r="T122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8553,9 +9277,15 @@
       <c r="R123" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S123" t="inlineStr">
-        <is>
-          <t>2997</t>
+      <c r="S123" t="n">
+        <v>2997</v>
+      </c>
+      <c r="T123" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U123" t="inlineStr">
+        <is>
+          <t>3118</t>
         </is>
       </c>
     </row>
@@ -8620,9 +9350,15 @@
       <c r="R124" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="S124" t="inlineStr">
-        <is>
-          <t>2985</t>
+      <c r="S124" t="n">
+        <v>2985</v>
+      </c>
+      <c r="T124" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="U124" t="inlineStr">
+        <is>
+          <t>3022</t>
         </is>
       </c>
     </row>
@@ -8687,9 +9423,15 @@
       <c r="R125" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S125" t="inlineStr">
-        <is>
-          <t>3227</t>
+      <c r="S125" t="n">
+        <v>3227</v>
+      </c>
+      <c r="T125" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U125" t="inlineStr">
+        <is>
+          <t>3385</t>
         </is>
       </c>
     </row>
@@ -8754,9 +9496,15 @@
       <c r="R126" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S126" t="inlineStr">
-        <is>
-          <t>3077</t>
+      <c r="S126" t="n">
+        <v>3077</v>
+      </c>
+      <c r="T126" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U126" t="inlineStr">
+        <is>
+          <t>3089</t>
         </is>
       </c>
     </row>
@@ -8821,9 +9569,15 @@
       <c r="R127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S127" t="inlineStr">
-        <is>
-          <t>2377</t>
+      <c r="S127" t="n">
+        <v>2377</v>
+      </c>
+      <c r="T127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U127" t="inlineStr">
+        <is>
+          <t>2372</t>
         </is>
       </c>
     </row>
@@ -8888,7 +9642,13 @@
       <c r="R128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S128" t="inlineStr">
+      <c r="S128" t="n">
+        <v>0</v>
+      </c>
+      <c r="T128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8955,7 +9715,13 @@
       <c r="R129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S129" t="inlineStr">
+      <c r="S129" t="n">
+        <v>0</v>
+      </c>
+      <c r="T129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9022,9 +9788,15 @@
       <c r="R130" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="S130" t="inlineStr">
-        <is>
-          <t>2756</t>
+      <c r="S130" t="n">
+        <v>2756</v>
+      </c>
+      <c r="T130" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="U130" t="inlineStr">
+        <is>
+          <t>2803</t>
         </is>
       </c>
     </row>
@@ -9089,9 +9861,15 @@
       <c r="R131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S131" t="inlineStr">
-        <is>
-          <t>2435</t>
+      <c r="S131" t="n">
+        <v>2435</v>
+      </c>
+      <c r="T131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U131" t="inlineStr">
+        <is>
+          <t>2464</t>
         </is>
       </c>
     </row>
@@ -9156,9 +9934,15 @@
       <c r="R132" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S132" t="inlineStr">
-        <is>
-          <t>2629</t>
+      <c r="S132" t="n">
+        <v>2629</v>
+      </c>
+      <c r="T132" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U132" t="inlineStr">
+        <is>
+          <t>2632</t>
         </is>
       </c>
     </row>
@@ -9223,9 +10007,15 @@
       <c r="R133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S133" t="inlineStr">
-        <is>
-          <t>2748</t>
+      <c r="S133" t="n">
+        <v>2748</v>
+      </c>
+      <c r="T133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U133" t="inlineStr">
+        <is>
+          <t>2749</t>
         </is>
       </c>
     </row>
@@ -9285,6 +10075,8 @@
       <c r="Q134" t="inlineStr"/>
       <c r="R134" s="3" t="inlineStr"/>
       <c r="S134" t="inlineStr"/>
+      <c r="T134" s="3" t="inlineStr"/>
+      <c r="U134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -9334,6 +10126,8 @@
       <c r="Q135" t="inlineStr"/>
       <c r="R135" s="3" t="inlineStr"/>
       <c r="S135" t="inlineStr"/>
+      <c r="T135" s="3" t="inlineStr"/>
+      <c r="U135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -9396,9 +10190,15 @@
       <c r="R136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S136" t="inlineStr">
-        <is>
-          <t>2660</t>
+      <c r="S136" t="n">
+        <v>2660</v>
+      </c>
+      <c r="T136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U136" t="inlineStr">
+        <is>
+          <t>2686</t>
         </is>
       </c>
     </row>
@@ -9463,7 +10263,13 @@
       <c r="R137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S137" t="inlineStr">
+      <c r="S137" t="n">
+        <v>0</v>
+      </c>
+      <c r="T137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9517,6 +10323,8 @@
       <c r="Q138" t="inlineStr"/>
       <c r="R138" s="3" t="inlineStr"/>
       <c r="S138" t="inlineStr"/>
+      <c r="T138" s="3" t="inlineStr"/>
+      <c r="U138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -9579,9 +10387,15 @@
       <c r="R139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S139" t="inlineStr">
-        <is>
-          <t>2346</t>
+      <c r="S139" t="n">
+        <v>2346</v>
+      </c>
+      <c r="T139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U139" t="inlineStr">
+        <is>
+          <t>2337</t>
         </is>
       </c>
     </row>
@@ -9646,9 +10460,15 @@
       <c r="R140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S140" t="inlineStr">
-        <is>
-          <t>2571</t>
+      <c r="S140" t="n">
+        <v>2571</v>
+      </c>
+      <c r="T140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U140" t="inlineStr">
+        <is>
+          <t>2561</t>
         </is>
       </c>
     </row>
@@ -9700,6 +10520,8 @@
       <c r="Q141" t="inlineStr"/>
       <c r="R141" s="3" t="inlineStr"/>
       <c r="S141" t="inlineStr"/>
+      <c r="T141" s="3" t="inlineStr"/>
+      <c r="U141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -9762,9 +10584,15 @@
       <c r="R142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S142" t="inlineStr">
-        <is>
-          <t>2096</t>
+      <c r="S142" t="n">
+        <v>2096</v>
+      </c>
+      <c r="T142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U142" t="inlineStr">
+        <is>
+          <t>2142</t>
         </is>
       </c>
     </row>
@@ -9816,6 +10644,8 @@
       <c r="Q143" t="inlineStr"/>
       <c r="R143" s="3" t="inlineStr"/>
       <c r="S143" t="inlineStr"/>
+      <c r="T143" s="3" t="inlineStr"/>
+      <c r="U143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -9865,6 +10695,8 @@
       <c r="Q144" t="inlineStr"/>
       <c r="R144" s="3" t="inlineStr"/>
       <c r="S144" t="inlineStr"/>
+      <c r="T144" s="3" t="inlineStr"/>
+      <c r="U144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -9914,6 +10746,8 @@
       <c r="Q145" t="inlineStr"/>
       <c r="R145" s="3" t="inlineStr"/>
       <c r="S145" t="inlineStr"/>
+      <c r="T145" s="3" t="inlineStr"/>
+      <c r="U145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -9963,6 +10797,8 @@
       <c r="Q146" t="inlineStr"/>
       <c r="R146" s="3" t="inlineStr"/>
       <c r="S146" t="inlineStr"/>
+      <c r="T146" s="3" t="inlineStr"/>
+      <c r="U146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -10012,6 +10848,8 @@
       <c r="Q147" t="inlineStr"/>
       <c r="R147" s="3" t="inlineStr"/>
       <c r="S147" t="inlineStr"/>
+      <c r="T147" s="3" t="inlineStr"/>
+      <c r="U147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -10074,9 +10912,15 @@
       <c r="R148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S148" t="inlineStr">
-        <is>
-          <t>1522</t>
+      <c r="S148" t="n">
+        <v>1522</v>
+      </c>
+      <c r="T148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U148" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -10141,9 +10985,15 @@
       <c r="R149" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S149" t="inlineStr">
-        <is>
-          <t>3638</t>
+      <c r="S149" t="n">
+        <v>3638</v>
+      </c>
+      <c r="T149" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="U149" t="inlineStr">
+        <is>
+          <t>3849</t>
         </is>
       </c>
     </row>
@@ -10208,7 +11058,13 @@
       <c r="R150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S150" t="inlineStr">
+      <c r="S150" t="n">
+        <v>0</v>
+      </c>
+      <c r="T150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10275,9 +11131,15 @@
       <c r="R151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S151" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="S151" t="n">
+        <v>0</v>
+      </c>
+      <c r="T151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U151" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -10342,7 +11204,13 @@
       <c r="R152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S152" t="inlineStr">
+      <c r="S152" t="n">
+        <v>0</v>
+      </c>
+      <c r="T152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10409,7 +11277,13 @@
       <c r="R153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S153" t="inlineStr">
+      <c r="S153" t="n">
+        <v>0</v>
+      </c>
+      <c r="T153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10476,7 +11350,13 @@
       <c r="R154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S154" t="inlineStr">
+      <c r="S154" t="n">
+        <v>0</v>
+      </c>
+      <c r="T154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10543,9 +11423,15 @@
       <c r="R155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S155" t="inlineStr">
-        <is>
-          <t>2528</t>
+      <c r="S155" t="n">
+        <v>2528</v>
+      </c>
+      <c r="T155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U155" t="inlineStr">
+        <is>
+          <t>2554</t>
         </is>
       </c>
     </row>
@@ -10604,9 +11490,15 @@
       <c r="R156" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S156" t="inlineStr">
-        <is>
-          <t>3228</t>
+      <c r="S156" t="n">
+        <v>3228</v>
+      </c>
+      <c r="T156" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="U156" t="inlineStr">
+        <is>
+          <t>3355</t>
         </is>
       </c>
     </row>
@@ -10652,6 +11544,8 @@
       <c r="Q157" t="inlineStr"/>
       <c r="R157" s="3" t="inlineStr"/>
       <c r="S157" t="inlineStr"/>
+      <c r="T157" s="3" t="inlineStr"/>
+      <c r="U157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -10708,7 +11602,13 @@
       <c r="R158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S158" t="inlineStr">
+      <c r="S158" t="n">
+        <v>0</v>
+      </c>
+      <c r="T158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10769,9 +11669,15 @@
       <c r="R159" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S159" t="inlineStr">
-        <is>
-          <t>2779</t>
+      <c r="S159" t="n">
+        <v>2779</v>
+      </c>
+      <c r="T159" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U159" t="inlineStr">
+        <is>
+          <t>2894</t>
         </is>
       </c>
     </row>
@@ -10817,6 +11723,8 @@
       <c r="Q160" t="inlineStr"/>
       <c r="R160" s="3" t="inlineStr"/>
       <c r="S160" t="inlineStr"/>
+      <c r="T160" s="3" t="inlineStr"/>
+      <c r="U160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -10861,9 +11769,15 @@
       <c r="R161" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="S161" t="inlineStr">
-        <is>
-          <t>2666</t>
+      <c r="S161" t="n">
+        <v>2666</v>
+      </c>
+      <c r="T161" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="U161" t="inlineStr">
+        <is>
+          <t>2697</t>
         </is>
       </c>
     </row>
@@ -10910,9 +11824,15 @@
       <c r="R162" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="S162" t="inlineStr">
-        <is>
-          <t>2430</t>
+      <c r="S162" t="n">
+        <v>2430</v>
+      </c>
+      <c r="T162" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U162" t="inlineStr">
+        <is>
+          <t>2524</t>
         </is>
       </c>
     </row>
@@ -10955,9 +11875,97 @@
       <c r="R163" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S163" t="inlineStr">
-        <is>
-          <t>2965</t>
+      <c r="S163" t="n">
+        <v>2965</v>
+      </c>
+      <c r="T163" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U163" t="inlineStr">
+        <is>
+          <t>2958</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>3649043</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>"慶頴 謝"</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr"/>
+      <c r="D164" t="inlineStr"/>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F164" s="3" t="inlineStr"/>
+      <c r="G164" t="inlineStr"/>
+      <c r="H164" s="3" t="inlineStr"/>
+      <c r="I164" t="inlineStr"/>
+      <c r="J164" s="3" t="inlineStr"/>
+      <c r="K164" t="inlineStr"/>
+      <c r="L164" s="3" t="inlineStr"/>
+      <c r="M164" t="inlineStr"/>
+      <c r="N164" s="3" t="inlineStr"/>
+      <c r="O164" t="inlineStr"/>
+      <c r="P164" s="3" t="inlineStr"/>
+      <c r="Q164" t="inlineStr"/>
+      <c r="R164" s="3" t="inlineStr"/>
+      <c r="S164" t="inlineStr"/>
+      <c r="T164" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="U164" t="inlineStr">
+        <is>
+          <t>3360</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>50837459</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>NINE日</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr"/>
+      <c r="D165" t="inlineStr"/>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F165" s="3" t="inlineStr"/>
+      <c r="G165" t="inlineStr"/>
+      <c r="H165" s="3" t="inlineStr"/>
+      <c r="I165" t="inlineStr"/>
+      <c r="J165" s="3" t="inlineStr"/>
+      <c r="K165" t="inlineStr"/>
+      <c r="L165" s="3" t="inlineStr"/>
+      <c r="M165" t="inlineStr"/>
+      <c r="N165" s="3" t="inlineStr"/>
+      <c r="O165" t="inlineStr"/>
+      <c r="P165" s="3" t="inlineStr"/>
+      <c r="Q165" t="inlineStr"/>
+      <c r="R165" s="3" t="inlineStr"/>
+      <c r="S165" t="inlineStr"/>
+      <c r="T165" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="U165" t="inlineStr">
+        <is>
+          <t>2535</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-02-20 14:21:00
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -11888,10 +11888,8 @@
       </c>
     </row>
     <row r="164">
-      <c r="A164" t="inlineStr">
-        <is>
-          <t>3649043</t>
-        </is>
+      <c r="A164" t="n">
+        <v>3649043</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
@@ -11929,10 +11927,8 @@
       </c>
     </row>
     <row r="165">
-      <c r="A165" t="inlineStr">
-        <is>
-          <t>50837459</t>
-        </is>
+      <c r="A165" t="n">
+        <v>50837459</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Code updated 23-02-21 12:56:03
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U165"/>
+  <dimension ref="A1:W165"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,6 +496,16 @@
           <t>02-19_0</t>
         </is>
       </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>02-20_A</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>02-20_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -564,9 +574,15 @@
       <c r="T2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>3461</t>
+      <c r="U2" t="n">
+        <v>3461</v>
+      </c>
+      <c r="V2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>3564</t>
         </is>
       </c>
     </row>
@@ -637,9 +653,15 @@
       <c r="T3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>4551</t>
+      <c r="U3" t="n">
+        <v>4551</v>
+      </c>
+      <c r="V3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>4969</t>
         </is>
       </c>
     </row>
@@ -710,9 +732,15 @@
       <c r="T4" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>5201</t>
+      <c r="U4" t="n">
+        <v>5201</v>
+      </c>
+      <c r="V4" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>5508</t>
         </is>
       </c>
     </row>
@@ -783,9 +811,15 @@
       <c r="T5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>4456</t>
+      <c r="U5" t="n">
+        <v>4456</v>
+      </c>
+      <c r="V5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>4731</t>
         </is>
       </c>
     </row>
@@ -856,9 +890,15 @@
       <c r="T6" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>4836</t>
+      <c r="U6" t="n">
+        <v>4836</v>
+      </c>
+      <c r="V6" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>5043</t>
         </is>
       </c>
     </row>
@@ -881,7 +921,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F7" s="4" t="n">
@@ -929,9 +969,15 @@
       <c r="T7" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>5392</t>
+      <c r="U7" t="n">
+        <v>5392</v>
+      </c>
+      <c r="V7" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>5712</t>
         </is>
       </c>
     </row>
@@ -1002,9 +1048,15 @@
       <c r="T8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U8" t="inlineStr">
-        <is>
-          <t>4548</t>
+      <c r="U8" t="n">
+        <v>4548</v>
+      </c>
+      <c r="V8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>4703</t>
         </is>
       </c>
     </row>
@@ -1075,9 +1127,15 @@
       <c r="T9" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="U9" t="inlineStr">
-        <is>
-          <t>4660</t>
+      <c r="U9" t="n">
+        <v>4660</v>
+      </c>
+      <c r="V9" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>4763</t>
         </is>
       </c>
     </row>
@@ -1148,9 +1206,15 @@
       <c r="T10" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U10" t="inlineStr">
-        <is>
-          <t>5078</t>
+      <c r="U10" t="n">
+        <v>5078</v>
+      </c>
+      <c r="V10" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>5327</t>
         </is>
       </c>
     </row>
@@ -1221,9 +1285,15 @@
       <c r="T11" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U11" t="inlineStr">
-        <is>
-          <t>4156</t>
+      <c r="U11" t="n">
+        <v>4156</v>
+      </c>
+      <c r="V11" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>4384</t>
         </is>
       </c>
     </row>
@@ -1294,7 +1364,13 @@
       <c r="T12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U12" t="inlineStr">
+      <c r="U12" t="n">
+        <v>2835</v>
+      </c>
+      <c r="V12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" t="inlineStr">
         <is>
           <t>2835</t>
         </is>
@@ -1367,9 +1443,15 @@
       <c r="T13" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="U13" t="inlineStr">
-        <is>
-          <t>5592</t>
+      <c r="U13" t="n">
+        <v>5592</v>
+      </c>
+      <c r="V13" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>5736</t>
         </is>
       </c>
     </row>
@@ -1440,9 +1522,15 @@
       <c r="T14" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="U14" t="inlineStr">
-        <is>
-          <t>4755</t>
+      <c r="U14" t="n">
+        <v>4755</v>
+      </c>
+      <c r="V14" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>4992</t>
         </is>
       </c>
     </row>
@@ -1513,9 +1601,15 @@
       <c r="T15" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="U15" t="inlineStr">
-        <is>
-          <t>4302</t>
+      <c r="U15" t="n">
+        <v>4302</v>
+      </c>
+      <c r="V15" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>4524</t>
         </is>
       </c>
     </row>
@@ -1586,9 +1680,15 @@
       <c r="T16" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U16" t="inlineStr">
-        <is>
-          <t>4727</t>
+      <c r="U16" t="n">
+        <v>4727</v>
+      </c>
+      <c r="V16" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>5025</t>
         </is>
       </c>
     </row>
@@ -1659,9 +1759,15 @@
       <c r="T17" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="U17" t="inlineStr">
-        <is>
-          <t>4085</t>
+      <c r="U17" t="n">
+        <v>4085</v>
+      </c>
+      <c r="V17" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>4172</t>
         </is>
       </c>
     </row>
@@ -1732,9 +1838,15 @@
       <c r="T18" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="U18" t="inlineStr">
-        <is>
-          <t>3874</t>
+      <c r="U18" t="n">
+        <v>3874</v>
+      </c>
+      <c r="V18" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>3923</t>
         </is>
       </c>
     </row>
@@ -1805,9 +1917,15 @@
       <c r="T19" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="U19" t="inlineStr">
-        <is>
-          <t>4747</t>
+      <c r="U19" t="n">
+        <v>4747</v>
+      </c>
+      <c r="V19" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>4907</t>
         </is>
       </c>
     </row>
@@ -1878,9 +1996,15 @@
       <c r="T20" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="U20" t="inlineStr">
-        <is>
-          <t>5634</t>
+      <c r="U20" t="n">
+        <v>5634</v>
+      </c>
+      <c r="V20" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>5910</t>
         </is>
       </c>
     </row>
@@ -1951,9 +2075,15 @@
       <c r="T21" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U21" t="inlineStr">
-        <is>
-          <t>3920</t>
+      <c r="U21" t="n">
+        <v>3920</v>
+      </c>
+      <c r="V21" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>4376</t>
         </is>
       </c>
     </row>
@@ -2024,9 +2154,15 @@
       <c r="T22" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="U22" t="inlineStr">
-        <is>
-          <t>4612</t>
+      <c r="U22" t="n">
+        <v>4612</v>
+      </c>
+      <c r="V22" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="W22" t="inlineStr">
+        <is>
+          <t>4886</t>
         </is>
       </c>
     </row>
@@ -2097,9 +2233,15 @@
       <c r="T23" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U23" t="inlineStr">
-        <is>
-          <t>4389</t>
+      <c r="U23" t="n">
+        <v>4389</v>
+      </c>
+      <c r="V23" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="W23" t="inlineStr">
+        <is>
+          <t>4647</t>
         </is>
       </c>
     </row>
@@ -2122,7 +2264,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F24" s="4" t="n">
@@ -2170,9 +2312,15 @@
       <c r="T24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U24" t="inlineStr">
-        <is>
-          <t>4970</t>
+      <c r="U24" t="n">
+        <v>4970</v>
+      </c>
+      <c r="V24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="W24" t="inlineStr">
+        <is>
+          <t>5306</t>
         </is>
       </c>
     </row>
@@ -2243,7 +2391,13 @@
       <c r="T25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U25" t="inlineStr">
+      <c r="U25" t="n">
+        <v>0</v>
+      </c>
+      <c r="V25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2316,9 +2470,15 @@
       <c r="T26" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="U26" t="inlineStr">
-        <is>
-          <t>4880</t>
+      <c r="U26" t="n">
+        <v>4880</v>
+      </c>
+      <c r="V26" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="W26" t="inlineStr">
+        <is>
+          <t>5066</t>
         </is>
       </c>
     </row>
@@ -2389,9 +2549,15 @@
       <c r="T27" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="U27" t="inlineStr">
-        <is>
-          <t>4994</t>
+      <c r="U27" t="n">
+        <v>4994</v>
+      </c>
+      <c r="V27" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="W27" t="inlineStr">
+        <is>
+          <t>5164</t>
         </is>
       </c>
     </row>
@@ -2462,9 +2628,15 @@
       <c r="T28" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="U28" t="inlineStr">
-        <is>
-          <t>3967</t>
+      <c r="U28" t="n">
+        <v>3967</v>
+      </c>
+      <c r="V28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="W28" t="inlineStr">
+        <is>
+          <t>4099</t>
         </is>
       </c>
     </row>
@@ -2535,9 +2707,15 @@
       <c r="T29" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="U29" t="inlineStr">
-        <is>
-          <t>5566</t>
+      <c r="U29" t="n">
+        <v>5566</v>
+      </c>
+      <c r="V29" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="W29" t="inlineStr">
+        <is>
+          <t>5911</t>
         </is>
       </c>
     </row>
@@ -2608,9 +2786,15 @@
       <c r="T30" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="U30" t="inlineStr">
-        <is>
-          <t>4222</t>
+      <c r="U30" t="n">
+        <v>4222</v>
+      </c>
+      <c r="V30" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="W30" t="inlineStr">
+        <is>
+          <t>4588</t>
         </is>
       </c>
     </row>
@@ -2681,9 +2865,15 @@
       <c r="T31" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="U31" t="inlineStr">
-        <is>
-          <t>5211</t>
+      <c r="U31" t="n">
+        <v>5211</v>
+      </c>
+      <c r="V31" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="W31" t="inlineStr">
+        <is>
+          <t>5554</t>
         </is>
       </c>
     </row>
@@ -2754,9 +2944,15 @@
       <c r="T32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U32" t="inlineStr">
-        <is>
-          <t>4182</t>
+      <c r="U32" t="n">
+        <v>4182</v>
+      </c>
+      <c r="V32" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="W32" t="inlineStr">
+        <is>
+          <t>4528</t>
         </is>
       </c>
     </row>
@@ -2827,9 +3023,15 @@
       <c r="T33" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="U33" t="inlineStr">
-        <is>
-          <t>4674</t>
+      <c r="U33" t="n">
+        <v>4674</v>
+      </c>
+      <c r="V33" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="W33" t="inlineStr">
+        <is>
+          <t>4978</t>
         </is>
       </c>
     </row>
@@ -2900,9 +3102,15 @@
       <c r="T34" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U34" t="inlineStr">
-        <is>
-          <t>4760</t>
+      <c r="U34" t="n">
+        <v>4760</v>
+      </c>
+      <c r="V34" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W34" t="inlineStr">
+        <is>
+          <t>4927</t>
         </is>
       </c>
     </row>
@@ -2973,9 +3181,15 @@
       <c r="T35" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="U35" t="inlineStr">
-        <is>
-          <t>4769</t>
+      <c r="U35" t="n">
+        <v>4769</v>
+      </c>
+      <c r="V35" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="W35" t="inlineStr">
+        <is>
+          <t>5162</t>
         </is>
       </c>
     </row>
@@ -3046,9 +3260,15 @@
       <c r="T36" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U36" t="inlineStr">
-        <is>
-          <t>4746</t>
+      <c r="U36" t="n">
+        <v>4746</v>
+      </c>
+      <c r="V36" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W36" t="inlineStr">
+        <is>
+          <t>4990</t>
         </is>
       </c>
     </row>
@@ -3119,9 +3339,15 @@
       <c r="T37" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U37" t="inlineStr">
-        <is>
-          <t>4180</t>
+      <c r="U37" t="n">
+        <v>4180</v>
+      </c>
+      <c r="V37" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="W37" t="inlineStr">
+        <is>
+          <t>4277</t>
         </is>
       </c>
     </row>
@@ -3192,9 +3418,15 @@
       <c r="T38" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="U38" t="inlineStr">
-        <is>
-          <t>4542</t>
+      <c r="U38" t="n">
+        <v>4542</v>
+      </c>
+      <c r="V38" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="W38" t="inlineStr">
+        <is>
+          <t>4809</t>
         </is>
       </c>
     </row>
@@ -3265,9 +3497,15 @@
       <c r="T39" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="U39" t="inlineStr">
-        <is>
-          <t>4831</t>
+      <c r="U39" t="n">
+        <v>4831</v>
+      </c>
+      <c r="V39" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="W39" t="inlineStr">
+        <is>
+          <t>5136</t>
         </is>
       </c>
     </row>
@@ -3338,9 +3576,15 @@
       <c r="T40" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U40" t="inlineStr">
-        <is>
-          <t>5381</t>
+      <c r="U40" t="n">
+        <v>5381</v>
+      </c>
+      <c r="V40" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="W40" t="inlineStr">
+        <is>
+          <t>5687</t>
         </is>
       </c>
     </row>
@@ -3411,7 +3655,13 @@
       <c r="T41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U41" t="inlineStr">
+      <c r="U41" t="n">
+        <v>3632</v>
+      </c>
+      <c r="V41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W41" t="inlineStr">
         <is>
           <t>3632</t>
         </is>
@@ -3484,9 +3734,15 @@
       <c r="T42" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="U42" t="inlineStr">
-        <is>
-          <t>5329</t>
+      <c r="U42" t="n">
+        <v>5329</v>
+      </c>
+      <c r="V42" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="W42" t="inlineStr">
+        <is>
+          <t>5654</t>
         </is>
       </c>
     </row>
@@ -3509,7 +3765,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F43" s="4" t="n">
@@ -3557,9 +3813,15 @@
       <c r="T43" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U43" t="inlineStr">
-        <is>
-          <t>5058</t>
+      <c r="U43" t="n">
+        <v>5058</v>
+      </c>
+      <c r="V43" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="W43" t="inlineStr">
+        <is>
+          <t>5247</t>
         </is>
       </c>
     </row>
@@ -3582,7 +3844,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F44" s="4" t="n">
@@ -3630,9 +3892,15 @@
       <c r="T44" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="U44" t="inlineStr">
-        <is>
-          <t>4862</t>
+      <c r="U44" t="n">
+        <v>4862</v>
+      </c>
+      <c r="V44" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="W44" t="inlineStr">
+        <is>
+          <t>5183</t>
         </is>
       </c>
     </row>
@@ -3703,9 +3971,15 @@
       <c r="T45" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U45" t="inlineStr">
-        <is>
-          <t>4391</t>
+      <c r="U45" t="n">
+        <v>4391</v>
+      </c>
+      <c r="V45" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="W45" t="inlineStr">
+        <is>
+          <t>4537</t>
         </is>
       </c>
     </row>
@@ -3776,9 +4050,15 @@
       <c r="T46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U46" t="inlineStr">
-        <is>
-          <t>4362</t>
+      <c r="U46" t="n">
+        <v>4362</v>
+      </c>
+      <c r="V46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W46" t="inlineStr">
+        <is>
+          <t>4511</t>
         </is>
       </c>
     </row>
@@ -3849,7 +4129,13 @@
       <c r="T47" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U47" t="inlineStr">
+      <c r="U47" t="n">
+        <v>2500</v>
+      </c>
+      <c r="V47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W47" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -3874,7 +4160,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F48" s="4" t="n">
@@ -3922,9 +4208,15 @@
       <c r="T48" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="U48" t="inlineStr">
-        <is>
-          <t>4992</t>
+      <c r="U48" t="n">
+        <v>4992</v>
+      </c>
+      <c r="V48" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="W48" t="inlineStr">
+        <is>
+          <t>5345</t>
         </is>
       </c>
     </row>
@@ -3995,9 +4287,15 @@
       <c r="T49" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U49" t="inlineStr">
-        <is>
-          <t>3803</t>
+      <c r="U49" t="n">
+        <v>3803</v>
+      </c>
+      <c r="V49" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="W49" t="inlineStr">
+        <is>
+          <t>3967</t>
         </is>
       </c>
     </row>
@@ -4068,9 +4366,15 @@
       <c r="T50" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="U50" t="inlineStr">
-        <is>
-          <t>5228</t>
+      <c r="U50" t="n">
+        <v>5228</v>
+      </c>
+      <c r="V50" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="W50" t="inlineStr">
+        <is>
+          <t>5622</t>
         </is>
       </c>
     </row>
@@ -4141,9 +4445,15 @@
       <c r="T51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U51" t="inlineStr">
-        <is>
-          <t>2845</t>
+      <c r="U51" t="n">
+        <v>2845</v>
+      </c>
+      <c r="V51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W51" t="inlineStr">
+        <is>
+          <t>2841</t>
         </is>
       </c>
     </row>
@@ -4214,9 +4524,15 @@
       <c r="T52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U52" t="inlineStr">
-        <is>
-          <t>2720</t>
+      <c r="U52" t="n">
+        <v>2720</v>
+      </c>
+      <c r="V52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W52" t="inlineStr">
+        <is>
+          <t>2732</t>
         </is>
       </c>
     </row>
@@ -4287,9 +4603,15 @@
       <c r="T53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U53" t="inlineStr">
-        <is>
-          <t>2658</t>
+      <c r="U53" t="n">
+        <v>2658</v>
+      </c>
+      <c r="V53" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="W53" t="inlineStr">
+        <is>
+          <t>2850</t>
         </is>
       </c>
     </row>
@@ -4360,9 +4682,15 @@
       <c r="T54" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="U54" t="inlineStr">
-        <is>
-          <t>4945</t>
+      <c r="U54" t="n">
+        <v>4945</v>
+      </c>
+      <c r="V54" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W54" t="inlineStr">
+        <is>
+          <t>5108</t>
         </is>
       </c>
     </row>
@@ -4433,9 +4761,15 @@
       <c r="T55" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="U55" t="inlineStr">
-        <is>
-          <t>3848</t>
+      <c r="U55" t="n">
+        <v>3848</v>
+      </c>
+      <c r="V55" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="W55" t="inlineStr">
+        <is>
+          <t>3982</t>
         </is>
       </c>
     </row>
@@ -4506,9 +4840,15 @@
       <c r="T56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U56" t="inlineStr">
-        <is>
-          <t>3901</t>
+      <c r="U56" t="n">
+        <v>3901</v>
+      </c>
+      <c r="V56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W56" t="inlineStr">
+        <is>
+          <t>4041</t>
         </is>
       </c>
     </row>
@@ -4579,9 +4919,15 @@
       <c r="T57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U57" t="inlineStr">
-        <is>
-          <t>4644</t>
+      <c r="U57" t="n">
+        <v>4644</v>
+      </c>
+      <c r="V57" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="W57" t="inlineStr">
+        <is>
+          <t>4763</t>
         </is>
       </c>
     </row>
@@ -4652,9 +4998,15 @@
       <c r="T58" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U58" t="inlineStr">
-        <is>
-          <t>3872</t>
+      <c r="U58" t="n">
+        <v>3872</v>
+      </c>
+      <c r="V58" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="W58" t="inlineStr">
+        <is>
+          <t>4084</t>
         </is>
       </c>
     </row>
@@ -4692,6 +5044,8 @@
       <c r="S59" t="inlineStr"/>
       <c r="T59" s="3" t="inlineStr"/>
       <c r="U59" t="inlineStr"/>
+      <c r="V59" s="3" t="inlineStr"/>
+      <c r="W59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -4727,6 +5081,8 @@
       <c r="S60" t="inlineStr"/>
       <c r="T60" s="3" t="inlineStr"/>
       <c r="U60" t="inlineStr"/>
+      <c r="V60" s="3" t="inlineStr"/>
+      <c r="W60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -4795,9 +5151,15 @@
       <c r="T61" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U61" t="inlineStr">
-        <is>
-          <t>4422</t>
+      <c r="U61" t="n">
+        <v>4422</v>
+      </c>
+      <c r="V61" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W61" t="inlineStr">
+        <is>
+          <t>4581</t>
         </is>
       </c>
     </row>
@@ -4868,7 +5230,13 @@
       <c r="T62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U62" t="inlineStr">
+      <c r="U62" t="n">
+        <v>0</v>
+      </c>
+      <c r="V62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4941,9 +5309,15 @@
       <c r="T63" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="U63" t="inlineStr">
-        <is>
-          <t>4606</t>
+      <c r="U63" t="n">
+        <v>4606</v>
+      </c>
+      <c r="V63" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="W63" t="inlineStr">
+        <is>
+          <t>4816</t>
         </is>
       </c>
     </row>
@@ -5014,9 +5388,15 @@
       <c r="T64" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="U64" t="inlineStr">
-        <is>
-          <t>2887</t>
+      <c r="U64" t="n">
+        <v>2887</v>
+      </c>
+      <c r="V64" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="W64" t="inlineStr">
+        <is>
+          <t>3031</t>
         </is>
       </c>
     </row>
@@ -5054,6 +5434,8 @@
       <c r="S65" t="inlineStr"/>
       <c r="T65" s="3" t="inlineStr"/>
       <c r="U65" t="inlineStr"/>
+      <c r="V65" s="3" t="inlineStr"/>
+      <c r="W65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -5122,9 +5504,15 @@
       <c r="T66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U66" t="inlineStr">
-        <is>
-          <t>2393</t>
+      <c r="U66" t="n">
+        <v>2393</v>
+      </c>
+      <c r="V66" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="W66" t="inlineStr">
+        <is>
+          <t>2631</t>
         </is>
       </c>
     </row>
@@ -5195,9 +5583,15 @@
       <c r="T67" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="U67" t="inlineStr">
-        <is>
-          <t>4367</t>
+      <c r="U67" t="n">
+        <v>4367</v>
+      </c>
+      <c r="V67" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="W67" t="inlineStr">
+        <is>
+          <t>4581</t>
         </is>
       </c>
     </row>
@@ -5220,7 +5614,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F68" s="4" t="n">
@@ -5268,9 +5662,15 @@
       <c r="T68" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U68" t="inlineStr">
-        <is>
-          <t>4869</t>
+      <c r="U68" t="n">
+        <v>4869</v>
+      </c>
+      <c r="V68" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="W68" t="inlineStr">
+        <is>
+          <t>5224</t>
         </is>
       </c>
     </row>
@@ -5341,9 +5741,15 @@
       <c r="T69" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U69" t="inlineStr">
-        <is>
-          <t>4009</t>
+      <c r="U69" t="n">
+        <v>4009</v>
+      </c>
+      <c r="V69" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="W69" t="inlineStr">
+        <is>
+          <t>4135</t>
         </is>
       </c>
     </row>
@@ -5414,7 +5820,13 @@
       <c r="T70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U70" t="inlineStr">
+      <c r="U70" t="n">
+        <v>2645</v>
+      </c>
+      <c r="V70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W70" t="inlineStr">
         <is>
           <t>2645</t>
         </is>
@@ -5487,9 +5899,15 @@
       <c r="T71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U71" t="inlineStr">
-        <is>
-          <t>3900</t>
+      <c r="U71" t="n">
+        <v>3900</v>
+      </c>
+      <c r="V71" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="W71" t="inlineStr">
+        <is>
+          <t>4022</t>
         </is>
       </c>
     </row>
@@ -5560,9 +5978,15 @@
       <c r="T72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U72" t="inlineStr">
-        <is>
-          <t>3271</t>
+      <c r="U72" t="n">
+        <v>3271</v>
+      </c>
+      <c r="V72" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="W72" t="inlineStr">
+        <is>
+          <t>3503</t>
         </is>
       </c>
     </row>
@@ -5633,9 +6057,15 @@
       <c r="T73" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U73" t="inlineStr">
-        <is>
-          <t>3876</t>
+      <c r="U73" t="n">
+        <v>3876</v>
+      </c>
+      <c r="V73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W73" t="inlineStr">
+        <is>
+          <t>4028</t>
         </is>
       </c>
     </row>
@@ -5706,9 +6136,15 @@
       <c r="T74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U74" t="inlineStr">
-        <is>
-          <t>2768</t>
+      <c r="U74" t="n">
+        <v>2768</v>
+      </c>
+      <c r="V74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W74" t="inlineStr">
+        <is>
+          <t>2765</t>
         </is>
       </c>
     </row>
@@ -5779,9 +6215,15 @@
       <c r="T75" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="U75" t="inlineStr">
-        <is>
-          <t>3679</t>
+      <c r="U75" t="n">
+        <v>3679</v>
+      </c>
+      <c r="V75" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="W75" t="inlineStr">
+        <is>
+          <t>3816</t>
         </is>
       </c>
     </row>
@@ -5852,9 +6294,15 @@
       <c r="T76" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="U76" t="inlineStr">
-        <is>
-          <t>4450</t>
+      <c r="U76" t="n">
+        <v>4450</v>
+      </c>
+      <c r="V76" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="W76" t="inlineStr">
+        <is>
+          <t>4664</t>
         </is>
       </c>
     </row>
@@ -5925,9 +6373,15 @@
       <c r="T77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U77" t="inlineStr">
-        <is>
-          <t>3353</t>
+      <c r="U77" t="n">
+        <v>3353</v>
+      </c>
+      <c r="V77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W77" t="inlineStr">
+        <is>
+          <t>3383</t>
         </is>
       </c>
     </row>
@@ -5998,9 +6452,15 @@
       <c r="T78" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U78" t="inlineStr">
-        <is>
-          <t>4545</t>
+      <c r="U78" t="n">
+        <v>4545</v>
+      </c>
+      <c r="V78" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W78" t="inlineStr">
+        <is>
+          <t>4699</t>
         </is>
       </c>
     </row>
@@ -6071,7 +6531,13 @@
       <c r="T79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U79" t="inlineStr">
+      <c r="U79" t="n">
+        <v>0</v>
+      </c>
+      <c r="V79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6144,9 +6610,15 @@
       <c r="T80" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="U80" t="inlineStr">
-        <is>
-          <t>4302</t>
+      <c r="U80" t="n">
+        <v>4302</v>
+      </c>
+      <c r="V80" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="W80" t="inlineStr">
+        <is>
+          <t>4551</t>
         </is>
       </c>
     </row>
@@ -6217,9 +6689,15 @@
       <c r="T81" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U81" t="inlineStr">
-        <is>
-          <t>4334</t>
+      <c r="U81" t="n">
+        <v>4334</v>
+      </c>
+      <c r="V81" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="W81" t="inlineStr">
+        <is>
+          <t>4469</t>
         </is>
       </c>
     </row>
@@ -6290,9 +6768,15 @@
       <c r="T82" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="U82" t="inlineStr">
-        <is>
-          <t>4154</t>
+      <c r="U82" t="n">
+        <v>4154</v>
+      </c>
+      <c r="V82" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="W82" t="inlineStr">
+        <is>
+          <t>4275</t>
         </is>
       </c>
     </row>
@@ -6363,9 +6847,15 @@
       <c r="T83" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="U83" t="inlineStr">
-        <is>
-          <t>3995</t>
+      <c r="U83" t="n">
+        <v>3995</v>
+      </c>
+      <c r="V83" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="W83" t="inlineStr">
+        <is>
+          <t>4209</t>
         </is>
       </c>
     </row>
@@ -6436,9 +6926,15 @@
       <c r="T84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U84" t="inlineStr">
-        <is>
-          <t>2975</t>
+      <c r="U84" t="n">
+        <v>2975</v>
+      </c>
+      <c r="V84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W84" t="inlineStr">
+        <is>
+          <t>2990</t>
         </is>
       </c>
     </row>
@@ -6509,9 +7005,15 @@
       <c r="T85" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U85" t="inlineStr">
-        <is>
-          <t>3412</t>
+      <c r="U85" t="n">
+        <v>3412</v>
+      </c>
+      <c r="V85" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="W85" t="inlineStr">
+        <is>
+          <t>3513</t>
         </is>
       </c>
     </row>
@@ -6582,9 +7084,15 @@
       <c r="T86" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="U86" t="inlineStr">
-        <is>
-          <t>3178</t>
+      <c r="U86" t="n">
+        <v>3178</v>
+      </c>
+      <c r="V86" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="W86" t="inlineStr">
+        <is>
+          <t>3186</t>
         </is>
       </c>
     </row>
@@ -6655,9 +7163,15 @@
       <c r="T87" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U87" t="inlineStr">
-        <is>
-          <t>4268</t>
+      <c r="U87" t="n">
+        <v>4268</v>
+      </c>
+      <c r="V87" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W87" t="inlineStr">
+        <is>
+          <t>4303</t>
         </is>
       </c>
     </row>
@@ -6728,9 +7242,15 @@
       <c r="T88" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U88" t="inlineStr">
-        <is>
-          <t>2869</t>
+      <c r="U88" t="n">
+        <v>2869</v>
+      </c>
+      <c r="V88" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W88" t="inlineStr">
+        <is>
+          <t>2928</t>
         </is>
       </c>
     </row>
@@ -6801,9 +7321,15 @@
       <c r="T89" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="U89" t="inlineStr">
-        <is>
-          <t>3098</t>
+      <c r="U89" t="n">
+        <v>3098</v>
+      </c>
+      <c r="V89" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W89" t="inlineStr">
+        <is>
+          <t>3223</t>
         </is>
       </c>
     </row>
@@ -6874,9 +7400,15 @@
       <c r="T90" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="U90" t="inlineStr">
-        <is>
-          <t>2801</t>
+      <c r="U90" t="n">
+        <v>2801</v>
+      </c>
+      <c r="V90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W90" t="inlineStr">
+        <is>
+          <t>2759</t>
         </is>
       </c>
     </row>
@@ -6947,9 +7479,15 @@
       <c r="T91" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U91" t="inlineStr">
-        <is>
-          <t>2800</t>
+      <c r="U91" t="n">
+        <v>2800</v>
+      </c>
+      <c r="V91" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W91" t="inlineStr">
+        <is>
+          <t>2794</t>
         </is>
       </c>
     </row>
@@ -7020,7 +7558,13 @@
       <c r="T92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U92" t="inlineStr">
+      <c r="U92" t="n">
+        <v>0</v>
+      </c>
+      <c r="V92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7093,9 +7637,15 @@
       <c r="T93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U93" t="inlineStr">
-        <is>
-          <t>2396</t>
+      <c r="U93" t="n">
+        <v>2396</v>
+      </c>
+      <c r="V93" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W93" t="inlineStr">
+        <is>
+          <t>2673</t>
         </is>
       </c>
     </row>
@@ -7166,9 +7716,15 @@
       <c r="T94" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U94" t="inlineStr">
-        <is>
-          <t>3217</t>
+      <c r="U94" t="n">
+        <v>3217</v>
+      </c>
+      <c r="V94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W94" t="inlineStr">
+        <is>
+          <t>3227</t>
         </is>
       </c>
     </row>
@@ -7239,9 +7795,15 @@
       <c r="T95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U95" t="inlineStr">
-        <is>
-          <t>2576</t>
+      <c r="U95" t="n">
+        <v>2576</v>
+      </c>
+      <c r="V95" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="W95" t="inlineStr">
+        <is>
+          <t>2551</t>
         </is>
       </c>
     </row>
@@ -7312,9 +7874,15 @@
       <c r="T96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U96" t="inlineStr">
-        <is>
-          <t>3182</t>
+      <c r="U96" t="n">
+        <v>3182</v>
+      </c>
+      <c r="V96" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W96" t="inlineStr">
+        <is>
+          <t>3435</t>
         </is>
       </c>
     </row>
@@ -7385,9 +7953,15 @@
       <c r="T97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U97" t="inlineStr">
-        <is>
-          <t>2545</t>
+      <c r="U97" t="n">
+        <v>2545</v>
+      </c>
+      <c r="V97" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="W97" t="inlineStr">
+        <is>
+          <t>2586</t>
         </is>
       </c>
     </row>
@@ -7458,7 +8032,13 @@
       <c r="T98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U98" t="inlineStr">
+      <c r="U98" t="n">
+        <v>0</v>
+      </c>
+      <c r="V98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7531,9 +8111,15 @@
       <c r="T99" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U99" t="inlineStr">
-        <is>
-          <t>3517</t>
+      <c r="U99" t="n">
+        <v>3517</v>
+      </c>
+      <c r="V99" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W99" t="inlineStr">
+        <is>
+          <t>3688</t>
         </is>
       </c>
     </row>
@@ -7604,9 +8190,15 @@
       <c r="T100" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="U100" t="inlineStr">
-        <is>
-          <t>2463</t>
+      <c r="U100" t="n">
+        <v>2463</v>
+      </c>
+      <c r="V100" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="W100" t="inlineStr">
+        <is>
+          <t>2579</t>
         </is>
       </c>
     </row>
@@ -7677,9 +8269,15 @@
       <c r="T101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U101" t="inlineStr">
-        <is>
-          <t>4010</t>
+      <c r="U101" t="n">
+        <v>4010</v>
+      </c>
+      <c r="V101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W101" t="inlineStr">
+        <is>
+          <t>4113</t>
         </is>
       </c>
     </row>
@@ -7750,9 +8348,15 @@
       <c r="T102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U102" t="inlineStr">
-        <is>
-          <t>3593</t>
+      <c r="U102" t="n">
+        <v>3593</v>
+      </c>
+      <c r="V102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W102" t="inlineStr">
+        <is>
+          <t>3763</t>
         </is>
       </c>
     </row>
@@ -7823,9 +8427,15 @@
       <c r="T103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U103" t="inlineStr">
-        <is>
-          <t>2537</t>
+      <c r="U103" t="n">
+        <v>2537</v>
+      </c>
+      <c r="V103" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="W103" t="inlineStr">
+        <is>
+          <t>2580</t>
         </is>
       </c>
     </row>
@@ -7896,9 +8506,15 @@
       <c r="T104" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U104" t="inlineStr">
-        <is>
-          <t>4031</t>
+      <c r="U104" t="n">
+        <v>4031</v>
+      </c>
+      <c r="V104" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="W104" t="inlineStr">
+        <is>
+          <t>4161</t>
         </is>
       </c>
     </row>
@@ -7969,9 +8585,15 @@
       <c r="T105" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="U105" t="inlineStr">
-        <is>
-          <t>3728</t>
+      <c r="U105" t="n">
+        <v>3728</v>
+      </c>
+      <c r="V105" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="W105" t="inlineStr">
+        <is>
+          <t>3836</t>
         </is>
       </c>
     </row>
@@ -8042,7 +8664,13 @@
       <c r="T106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U106" t="inlineStr">
+      <c r="U106" t="n">
+        <v>0</v>
+      </c>
+      <c r="V106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8115,9 +8743,15 @@
       <c r="T107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U107" t="inlineStr">
-        <is>
-          <t>2487</t>
+      <c r="U107" t="n">
+        <v>2487</v>
+      </c>
+      <c r="V107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W107" t="inlineStr">
+        <is>
+          <t>2516</t>
         </is>
       </c>
     </row>
@@ -8188,7 +8822,13 @@
       <c r="T108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U108" t="inlineStr">
+      <c r="U108" t="n">
+        <v>0</v>
+      </c>
+      <c r="V108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8261,9 +8901,15 @@
       <c r="T109" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="U109" t="inlineStr">
-        <is>
-          <t>3419</t>
+      <c r="U109" t="n">
+        <v>3419</v>
+      </c>
+      <c r="V109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W109" t="inlineStr">
+        <is>
+          <t>3587</t>
         </is>
       </c>
     </row>
@@ -8334,9 +8980,15 @@
       <c r="T110" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="U110" t="inlineStr">
-        <is>
-          <t>3509</t>
+      <c r="U110" t="n">
+        <v>3509</v>
+      </c>
+      <c r="V110" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W110" t="inlineStr">
+        <is>
+          <t>3627</t>
         </is>
       </c>
     </row>
@@ -8407,9 +9059,15 @@
       <c r="T111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U111" t="inlineStr">
-        <is>
-          <t>2585</t>
+      <c r="U111" t="n">
+        <v>2585</v>
+      </c>
+      <c r="V111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W111" t="inlineStr">
+        <is>
+          <t>2578</t>
         </is>
       </c>
     </row>
@@ -8480,9 +9138,15 @@
       <c r="T112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U112" t="inlineStr">
-        <is>
-          <t>2804</t>
+      <c r="U112" t="n">
+        <v>2804</v>
+      </c>
+      <c r="V112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W112" t="inlineStr">
+        <is>
+          <t>2888</t>
         </is>
       </c>
     </row>
@@ -8553,9 +9217,15 @@
       <c r="T113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U113" t="inlineStr">
-        <is>
-          <t>3082</t>
+      <c r="U113" t="n">
+        <v>3082</v>
+      </c>
+      <c r="V113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W113" t="inlineStr">
+        <is>
+          <t>3298</t>
         </is>
       </c>
     </row>
@@ -8626,9 +9296,15 @@
       <c r="T114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U114" t="inlineStr">
-        <is>
-          <t>2671</t>
+      <c r="U114" t="n">
+        <v>2671</v>
+      </c>
+      <c r="V114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W114" t="inlineStr">
+        <is>
+          <t>2833</t>
         </is>
       </c>
     </row>
@@ -8699,9 +9375,15 @@
       <c r="T115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U115" t="inlineStr">
-        <is>
-          <t>2356</t>
+      <c r="U115" t="n">
+        <v>2356</v>
+      </c>
+      <c r="V115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W115" t="inlineStr">
+        <is>
+          <t>2349</t>
         </is>
       </c>
     </row>
@@ -8772,9 +9454,15 @@
       <c r="T116" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="U116" t="inlineStr">
-        <is>
-          <t>3036</t>
+      <c r="U116" t="n">
+        <v>3036</v>
+      </c>
+      <c r="V116" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="W116" t="inlineStr">
+        <is>
+          <t>3121</t>
         </is>
       </c>
     </row>
@@ -8845,9 +9533,15 @@
       <c r="T117" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U117" t="inlineStr">
-        <is>
-          <t>3446</t>
+      <c r="U117" t="n">
+        <v>3446</v>
+      </c>
+      <c r="V117" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W117" t="inlineStr">
+        <is>
+          <t>3566</t>
         </is>
       </c>
     </row>
@@ -8918,7 +9612,13 @@
       <c r="T118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U118" t="inlineStr">
+      <c r="U118" t="n">
+        <v>0</v>
+      </c>
+      <c r="V118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8991,9 +9691,15 @@
       <c r="T119" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U119" t="inlineStr">
-        <is>
-          <t>3765</t>
+      <c r="U119" t="n">
+        <v>3765</v>
+      </c>
+      <c r="V119" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W119" t="inlineStr">
+        <is>
+          <t>3819</t>
         </is>
       </c>
     </row>
@@ -9064,9 +9770,15 @@
       <c r="T120" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="U120" t="inlineStr">
-        <is>
-          <t>2595</t>
+      <c r="U120" t="n">
+        <v>2595</v>
+      </c>
+      <c r="V120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W120" t="inlineStr">
+        <is>
+          <t>2580</t>
         </is>
       </c>
     </row>
@@ -9137,9 +9849,15 @@
       <c r="T121" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="U121" t="inlineStr">
-        <is>
-          <t>3225</t>
+      <c r="U121" t="n">
+        <v>3225</v>
+      </c>
+      <c r="V121" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="W121" t="inlineStr">
+        <is>
+          <t>3308</t>
         </is>
       </c>
     </row>
@@ -9210,7 +9928,13 @@
       <c r="T122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U122" t="inlineStr">
+      <c r="U122" t="n">
+        <v>0</v>
+      </c>
+      <c r="V122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9283,9 +10007,15 @@
       <c r="T123" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U123" t="inlineStr">
-        <is>
-          <t>3118</t>
+      <c r="U123" t="n">
+        <v>3118</v>
+      </c>
+      <c r="V123" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W123" t="inlineStr">
+        <is>
+          <t>3159</t>
         </is>
       </c>
     </row>
@@ -9356,9 +10086,15 @@
       <c r="T124" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="U124" t="inlineStr">
-        <is>
-          <t>3022</t>
+      <c r="U124" t="n">
+        <v>3022</v>
+      </c>
+      <c r="V124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W124" t="inlineStr">
+        <is>
+          <t>3132</t>
         </is>
       </c>
     </row>
@@ -9429,9 +10165,15 @@
       <c r="T125" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U125" t="inlineStr">
-        <is>
-          <t>3385</t>
+      <c r="U125" t="n">
+        <v>3385</v>
+      </c>
+      <c r="V125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W125" t="inlineStr">
+        <is>
+          <t>3377</t>
         </is>
       </c>
     </row>
@@ -9502,9 +10244,15 @@
       <c r="T126" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U126" t="inlineStr">
-        <is>
-          <t>3089</t>
+      <c r="U126" t="n">
+        <v>3089</v>
+      </c>
+      <c r="V126" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W126" t="inlineStr">
+        <is>
+          <t>3171</t>
         </is>
       </c>
     </row>
@@ -9575,9 +10323,15 @@
       <c r="T127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U127" t="inlineStr">
-        <is>
-          <t>2372</t>
+      <c r="U127" t="n">
+        <v>2372</v>
+      </c>
+      <c r="V127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W127" t="inlineStr">
+        <is>
+          <t>2364</t>
         </is>
       </c>
     </row>
@@ -9648,7 +10402,13 @@
       <c r="T128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U128" t="inlineStr">
+      <c r="U128" t="n">
+        <v>0</v>
+      </c>
+      <c r="V128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9721,7 +10481,13 @@
       <c r="T129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U129" t="inlineStr">
+      <c r="U129" t="n">
+        <v>0</v>
+      </c>
+      <c r="V129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9794,9 +10560,15 @@
       <c r="T130" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="U130" t="inlineStr">
-        <is>
-          <t>2803</t>
+      <c r="U130" t="n">
+        <v>2803</v>
+      </c>
+      <c r="V130" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="W130" t="inlineStr">
+        <is>
+          <t>2832</t>
         </is>
       </c>
     </row>
@@ -9867,7 +10639,13 @@
       <c r="T131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U131" t="inlineStr">
+      <c r="U131" t="n">
+        <v>2464</v>
+      </c>
+      <c r="V131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W131" t="inlineStr">
         <is>
           <t>2464</t>
         </is>
@@ -9940,9 +10718,15 @@
       <c r="T132" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U132" t="inlineStr">
-        <is>
-          <t>2632</t>
+      <c r="U132" t="n">
+        <v>2632</v>
+      </c>
+      <c r="V132" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W132" t="inlineStr">
+        <is>
+          <t>2678</t>
         </is>
       </c>
     </row>
@@ -10013,9 +10797,15 @@
       <c r="T133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U133" t="inlineStr">
-        <is>
-          <t>2749</t>
+      <c r="U133" t="n">
+        <v>2749</v>
+      </c>
+      <c r="V133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W133" t="inlineStr">
+        <is>
+          <t>2784</t>
         </is>
       </c>
     </row>
@@ -10077,6 +10867,8 @@
       <c r="S134" t="inlineStr"/>
       <c r="T134" s="3" t="inlineStr"/>
       <c r="U134" t="inlineStr"/>
+      <c r="V134" s="3" t="inlineStr"/>
+      <c r="W134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -10128,6 +10920,8 @@
       <c r="S135" t="inlineStr"/>
       <c r="T135" s="3" t="inlineStr"/>
       <c r="U135" t="inlineStr"/>
+      <c r="V135" s="3" t="inlineStr"/>
+      <c r="W135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -10196,9 +10990,15 @@
       <c r="T136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U136" t="inlineStr">
-        <is>
-          <t>2686</t>
+      <c r="U136" t="n">
+        <v>2686</v>
+      </c>
+      <c r="V136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W136" t="inlineStr">
+        <is>
+          <t>2679</t>
         </is>
       </c>
     </row>
@@ -10269,7 +11069,13 @@
       <c r="T137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U137" t="inlineStr">
+      <c r="U137" t="n">
+        <v>0</v>
+      </c>
+      <c r="V137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10325,6 +11131,8 @@
       <c r="S138" t="inlineStr"/>
       <c r="T138" s="3" t="inlineStr"/>
       <c r="U138" t="inlineStr"/>
+      <c r="V138" s="3" t="inlineStr"/>
+      <c r="W138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -10393,9 +11201,15 @@
       <c r="T139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U139" t="inlineStr">
-        <is>
-          <t>2337</t>
+      <c r="U139" t="n">
+        <v>2337</v>
+      </c>
+      <c r="V139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W139" t="inlineStr">
+        <is>
+          <t>2386</t>
         </is>
       </c>
     </row>
@@ -10466,9 +11280,15 @@
       <c r="T140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U140" t="inlineStr">
-        <is>
-          <t>2561</t>
+      <c r="U140" t="n">
+        <v>2561</v>
+      </c>
+      <c r="V140" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W140" t="inlineStr">
+        <is>
+          <t>2784</t>
         </is>
       </c>
     </row>
@@ -10522,6 +11342,8 @@
       <c r="S141" t="inlineStr"/>
       <c r="T141" s="3" t="inlineStr"/>
       <c r="U141" t="inlineStr"/>
+      <c r="V141" s="3" t="inlineStr"/>
+      <c r="W141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -10590,9 +11412,15 @@
       <c r="T142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U142" t="inlineStr">
-        <is>
-          <t>2142</t>
+      <c r="U142" t="n">
+        <v>2142</v>
+      </c>
+      <c r="V142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W142" t="inlineStr">
+        <is>
+          <t>2178</t>
         </is>
       </c>
     </row>
@@ -10646,6 +11474,8 @@
       <c r="S143" t="inlineStr"/>
       <c r="T143" s="3" t="inlineStr"/>
       <c r="U143" t="inlineStr"/>
+      <c r="V143" s="3" t="inlineStr"/>
+      <c r="W143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -10697,6 +11527,8 @@
       <c r="S144" t="inlineStr"/>
       <c r="T144" s="3" t="inlineStr"/>
       <c r="U144" t="inlineStr"/>
+      <c r="V144" s="3" t="inlineStr"/>
+      <c r="W144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -10748,6 +11580,8 @@
       <c r="S145" t="inlineStr"/>
       <c r="T145" s="3" t="inlineStr"/>
       <c r="U145" t="inlineStr"/>
+      <c r="V145" s="3" t="inlineStr"/>
+      <c r="W145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -10799,6 +11633,8 @@
       <c r="S146" t="inlineStr"/>
       <c r="T146" s="3" t="inlineStr"/>
       <c r="U146" t="inlineStr"/>
+      <c r="V146" s="3" t="inlineStr"/>
+      <c r="W146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -10850,6 +11686,8 @@
       <c r="S147" t="inlineStr"/>
       <c r="T147" s="3" t="inlineStr"/>
       <c r="U147" t="inlineStr"/>
+      <c r="V147" s="3" t="inlineStr"/>
+      <c r="W147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -10918,9 +11756,15 @@
       <c r="T148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U148" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="U148" t="n">
+        <v>0</v>
+      </c>
+      <c r="V148" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="W148" t="inlineStr">
+        <is>
+          <t>1516</t>
         </is>
       </c>
     </row>
@@ -10991,7 +11835,13 @@
       <c r="T149" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="U149" t="inlineStr">
+      <c r="U149" t="n">
+        <v>3849</v>
+      </c>
+      <c r="V149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W149" t="inlineStr">
         <is>
           <t>3849</t>
         </is>
@@ -11064,7 +11914,13 @@
       <c r="T150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U150" t="inlineStr">
+      <c r="U150" t="n">
+        <v>0</v>
+      </c>
+      <c r="V150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11137,7 +11993,13 @@
       <c r="T151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U151" t="inlineStr">
+      <c r="U151" t="n">
+        <v>2500</v>
+      </c>
+      <c r="V151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W151" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -11210,7 +12072,13 @@
       <c r="T152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U152" t="inlineStr">
+      <c r="U152" t="n">
+        <v>0</v>
+      </c>
+      <c r="V152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11283,7 +12151,13 @@
       <c r="T153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U153" t="inlineStr">
+      <c r="U153" t="n">
+        <v>0</v>
+      </c>
+      <c r="V153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11356,7 +12230,13 @@
       <c r="T154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U154" t="inlineStr">
+      <c r="U154" t="n">
+        <v>0</v>
+      </c>
+      <c r="V154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11429,9 +12309,15 @@
       <c r="T155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U155" t="inlineStr">
-        <is>
-          <t>2554</t>
+      <c r="U155" t="n">
+        <v>2554</v>
+      </c>
+      <c r="V155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W155" t="inlineStr">
+        <is>
+          <t>2614</t>
         </is>
       </c>
     </row>
@@ -11496,9 +12382,15 @@
       <c r="T156" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="U156" t="inlineStr">
-        <is>
-          <t>3355</t>
+      <c r="U156" t="n">
+        <v>3355</v>
+      </c>
+      <c r="V156" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="W156" t="inlineStr">
+        <is>
+          <t>3451</t>
         </is>
       </c>
     </row>
@@ -11546,6 +12438,8 @@
       <c r="S157" t="inlineStr"/>
       <c r="T157" s="3" t="inlineStr"/>
       <c r="U157" t="inlineStr"/>
+      <c r="V157" s="3" t="inlineStr"/>
+      <c r="W157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -11608,7 +12502,13 @@
       <c r="T158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U158" t="inlineStr">
+      <c r="U158" t="n">
+        <v>0</v>
+      </c>
+      <c r="V158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11675,9 +12575,15 @@
       <c r="T159" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U159" t="inlineStr">
-        <is>
-          <t>2894</t>
+      <c r="U159" t="n">
+        <v>2894</v>
+      </c>
+      <c r="V159" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W159" t="inlineStr">
+        <is>
+          <t>2921</t>
         </is>
       </c>
     </row>
@@ -11725,6 +12631,8 @@
       <c r="S160" t="inlineStr"/>
       <c r="T160" s="3" t="inlineStr"/>
       <c r="U160" t="inlineStr"/>
+      <c r="V160" s="3" t="inlineStr"/>
+      <c r="W160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -11775,9 +12683,15 @@
       <c r="T161" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="U161" t="inlineStr">
-        <is>
-          <t>2697</t>
+      <c r="U161" t="n">
+        <v>2697</v>
+      </c>
+      <c r="V161" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="W161" t="inlineStr">
+        <is>
+          <t>2773</t>
         </is>
       </c>
     </row>
@@ -11830,9 +12744,15 @@
       <c r="T162" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U162" t="inlineStr">
-        <is>
-          <t>2524</t>
+      <c r="U162" t="n">
+        <v>2524</v>
+      </c>
+      <c r="V162" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="W162" t="inlineStr">
+        <is>
+          <t>2532</t>
         </is>
       </c>
     </row>
@@ -11881,9 +12801,15 @@
       <c r="T163" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U163" t="inlineStr">
-        <is>
-          <t>2958</t>
+      <c r="U163" t="n">
+        <v>2958</v>
+      </c>
+      <c r="V163" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W163" t="inlineStr">
+        <is>
+          <t>2953</t>
         </is>
       </c>
     </row>
@@ -11920,9 +12846,15 @@
       <c r="T164" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="U164" t="inlineStr">
-        <is>
-          <t>3360</t>
+      <c r="U164" t="n">
+        <v>3360</v>
+      </c>
+      <c r="V164" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W164" t="inlineStr">
+        <is>
+          <t>3418</t>
         </is>
       </c>
     </row>
@@ -11959,9 +12891,15 @@
       <c r="T165" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="U165" t="inlineStr">
-        <is>
-          <t>2535</t>
+      <c r="U165" t="n">
+        <v>2535</v>
+      </c>
+      <c r="V165" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="W165" t="inlineStr">
+        <is>
+          <t>2809</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-02-22 10:26:46
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W165"/>
+  <dimension ref="A1:Y166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,6 +506,16 @@
           <t>02-20_0</t>
         </is>
       </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>02-21_A</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>02-21_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -580,9 +590,15 @@
       <c r="V2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>3564</t>
+      <c r="W2" t="n">
+        <v>3564</v>
+      </c>
+      <c r="X2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>3656</t>
         </is>
       </c>
     </row>
@@ -659,9 +675,15 @@
       <c r="V3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>4969</t>
+      <c r="W3" t="n">
+        <v>4969</v>
+      </c>
+      <c r="X3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>5395</t>
         </is>
       </c>
     </row>
@@ -738,9 +760,15 @@
       <c r="V4" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>5508</t>
+      <c r="W4" t="n">
+        <v>5508</v>
+      </c>
+      <c r="X4" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>5777</t>
         </is>
       </c>
     </row>
@@ -817,9 +845,15 @@
       <c r="V5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>4731</t>
+      <c r="W5" t="n">
+        <v>4731</v>
+      </c>
+      <c r="X5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>5029</t>
         </is>
       </c>
     </row>
@@ -896,9 +930,15 @@
       <c r="V6" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="W6" t="inlineStr">
-        <is>
-          <t>5043</t>
+      <c r="W6" t="n">
+        <v>5043</v>
+      </c>
+      <c r="X6" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>5254</t>
         </is>
       </c>
     </row>
@@ -975,9 +1015,15 @@
       <c r="V7" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>5712</t>
+      <c r="W7" t="n">
+        <v>5712</v>
+      </c>
+      <c r="X7" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>6064</t>
         </is>
       </c>
     </row>
@@ -1054,9 +1100,15 @@
       <c r="V8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W8" t="inlineStr">
-        <is>
-          <t>4703</t>
+      <c r="W8" t="n">
+        <v>4703</v>
+      </c>
+      <c r="X8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>4871</t>
         </is>
       </c>
     </row>
@@ -1133,9 +1185,15 @@
       <c r="V9" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="W9" t="inlineStr">
-        <is>
-          <t>4763</t>
+      <c r="W9" t="n">
+        <v>4763</v>
+      </c>
+      <c r="X9" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>4919</t>
         </is>
       </c>
     </row>
@@ -1212,9 +1270,15 @@
       <c r="V10" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W10" t="inlineStr">
-        <is>
-          <t>5327</t>
+      <c r="W10" t="n">
+        <v>5327</v>
+      </c>
+      <c r="X10" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>5828</t>
         </is>
       </c>
     </row>
@@ -1291,9 +1355,15 @@
       <c r="V11" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W11" t="inlineStr">
-        <is>
-          <t>4384</t>
+      <c r="W11" t="n">
+        <v>4384</v>
+      </c>
+      <c r="X11" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y11" t="inlineStr">
+        <is>
+          <t>4826</t>
         </is>
       </c>
     </row>
@@ -1370,9 +1440,15 @@
       <c r="V12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W12" t="inlineStr">
-        <is>
-          <t>2835</t>
+      <c r="W12" t="n">
+        <v>2835</v>
+      </c>
+      <c r="X12" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y12" t="inlineStr">
+        <is>
+          <t>2914</t>
         </is>
       </c>
     </row>
@@ -1449,9 +1525,15 @@
       <c r="V13" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="W13" t="inlineStr">
-        <is>
-          <t>5736</t>
+      <c r="W13" t="n">
+        <v>5736</v>
+      </c>
+      <c r="X13" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="Y13" t="inlineStr">
+        <is>
+          <t>6094</t>
         </is>
       </c>
     </row>
@@ -1528,9 +1610,15 @@
       <c r="V14" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="W14" t="inlineStr">
-        <is>
-          <t>4992</t>
+      <c r="W14" t="n">
+        <v>4992</v>
+      </c>
+      <c r="X14" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y14" t="inlineStr">
+        <is>
+          <t>5157</t>
         </is>
       </c>
     </row>
@@ -1607,9 +1695,15 @@
       <c r="V15" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="W15" t="inlineStr">
-        <is>
-          <t>4524</t>
+      <c r="W15" t="n">
+        <v>4524</v>
+      </c>
+      <c r="X15" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="Y15" t="inlineStr">
+        <is>
+          <t>4785</t>
         </is>
       </c>
     </row>
@@ -1686,9 +1780,15 @@
       <c r="V16" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W16" t="inlineStr">
-        <is>
-          <t>5025</t>
+      <c r="W16" t="n">
+        <v>5025</v>
+      </c>
+      <c r="X16" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y16" t="inlineStr">
+        <is>
+          <t>5398</t>
         </is>
       </c>
     </row>
@@ -1765,9 +1865,15 @@
       <c r="V17" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="W17" t="inlineStr">
-        <is>
-          <t>4172</t>
+      <c r="W17" t="n">
+        <v>4172</v>
+      </c>
+      <c r="X17" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>4245</t>
         </is>
       </c>
     </row>
@@ -1844,9 +1950,15 @@
       <c r="V18" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="W18" t="inlineStr">
-        <is>
-          <t>3923</t>
+      <c r="W18" t="n">
+        <v>3923</v>
+      </c>
+      <c r="X18" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y18" t="inlineStr">
+        <is>
+          <t>4274</t>
         </is>
       </c>
     </row>
@@ -1923,9 +2035,15 @@
       <c r="V19" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="W19" t="inlineStr">
-        <is>
-          <t>4907</t>
+      <c r="W19" t="n">
+        <v>4907</v>
+      </c>
+      <c r="X19" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="Y19" t="inlineStr">
+        <is>
+          <t>5205</t>
         </is>
       </c>
     </row>
@@ -2002,9 +2120,15 @@
       <c r="V20" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="W20" t="inlineStr">
-        <is>
-          <t>5910</t>
+      <c r="W20" t="n">
+        <v>5910</v>
+      </c>
+      <c r="X20" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="Y20" t="inlineStr">
+        <is>
+          <t>6250</t>
         </is>
       </c>
     </row>
@@ -2081,9 +2205,15 @@
       <c r="V21" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="W21" t="inlineStr">
-        <is>
-          <t>4376</t>
+      <c r="W21" t="n">
+        <v>4376</v>
+      </c>
+      <c r="X21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y21" t="inlineStr">
+        <is>
+          <t>4374</t>
         </is>
       </c>
     </row>
@@ -2160,9 +2290,15 @@
       <c r="V22" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="W22" t="inlineStr">
-        <is>
-          <t>4886</t>
+      <c r="W22" t="n">
+        <v>4886</v>
+      </c>
+      <c r="X22" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y22" t="inlineStr">
+        <is>
+          <t>4944</t>
         </is>
       </c>
     </row>
@@ -2239,9 +2375,15 @@
       <c r="V23" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="W23" t="inlineStr">
-        <is>
-          <t>4647</t>
+      <c r="W23" t="n">
+        <v>4647</v>
+      </c>
+      <c r="X23" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="Y23" t="inlineStr">
+        <is>
+          <t>4838</t>
         </is>
       </c>
     </row>
@@ -2318,9 +2460,15 @@
       <c r="V24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="W24" t="inlineStr">
-        <is>
-          <t>5306</t>
+      <c r="W24" t="n">
+        <v>5306</v>
+      </c>
+      <c r="X24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y24" t="inlineStr">
+        <is>
+          <t>5604</t>
         </is>
       </c>
     </row>
@@ -2397,7 +2545,13 @@
       <c r="V25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W25" t="inlineStr">
+      <c r="W25" t="n">
+        <v>0</v>
+      </c>
+      <c r="X25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2476,9 +2630,15 @@
       <c r="V26" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="W26" t="inlineStr">
-        <is>
-          <t>5066</t>
+      <c r="W26" t="n">
+        <v>5066</v>
+      </c>
+      <c r="X26" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="Y26" t="inlineStr">
+        <is>
+          <t>5329</t>
         </is>
       </c>
     </row>
@@ -2555,9 +2715,15 @@
       <c r="V27" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="W27" t="inlineStr">
-        <is>
-          <t>5164</t>
+      <c r="W27" t="n">
+        <v>5164</v>
+      </c>
+      <c r="X27" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="Y27" t="inlineStr">
+        <is>
+          <t>5455</t>
         </is>
       </c>
     </row>
@@ -2634,9 +2800,15 @@
       <c r="V28" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="W28" t="inlineStr">
-        <is>
-          <t>4099</t>
+      <c r="W28" t="n">
+        <v>4099</v>
+      </c>
+      <c r="X28" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="Y28" t="inlineStr">
+        <is>
+          <t>4713</t>
         </is>
       </c>
     </row>
@@ -2713,9 +2885,15 @@
       <c r="V29" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="W29" t="inlineStr">
-        <is>
-          <t>5911</t>
+      <c r="W29" t="n">
+        <v>5911</v>
+      </c>
+      <c r="X29" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Y29" t="inlineStr">
+        <is>
+          <t>6245</t>
         </is>
       </c>
     </row>
@@ -2792,9 +2970,15 @@
       <c r="V30" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="W30" t="inlineStr">
-        <is>
-          <t>4588</t>
+      <c r="W30" t="n">
+        <v>4588</v>
+      </c>
+      <c r="X30" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y30" t="inlineStr">
+        <is>
+          <t>4854</t>
         </is>
       </c>
     </row>
@@ -2871,9 +3055,15 @@
       <c r="V31" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="W31" t="inlineStr">
-        <is>
-          <t>5554</t>
+      <c r="W31" t="n">
+        <v>5554</v>
+      </c>
+      <c r="X31" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="Y31" t="inlineStr">
+        <is>
+          <t>5905</t>
         </is>
       </c>
     </row>
@@ -2950,9 +3140,15 @@
       <c r="V32" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="W32" t="inlineStr">
-        <is>
-          <t>4528</t>
+      <c r="W32" t="n">
+        <v>4528</v>
+      </c>
+      <c r="X32" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="Y32" t="inlineStr">
+        <is>
+          <t>4821</t>
         </is>
       </c>
     </row>
@@ -3029,9 +3225,15 @@
       <c r="V33" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="W33" t="inlineStr">
-        <is>
-          <t>4978</t>
+      <c r="W33" t="n">
+        <v>4978</v>
+      </c>
+      <c r="X33" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="Y33" t="inlineStr">
+        <is>
+          <t>5281</t>
         </is>
       </c>
     </row>
@@ -3108,9 +3310,15 @@
       <c r="V34" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W34" t="inlineStr">
-        <is>
-          <t>4927</t>
+      <c r="W34" t="n">
+        <v>4927</v>
+      </c>
+      <c r="X34" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y34" t="inlineStr">
+        <is>
+          <t>5205</t>
         </is>
       </c>
     </row>
@@ -3187,9 +3395,15 @@
       <c r="V35" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="W35" t="inlineStr">
-        <is>
-          <t>5162</t>
+      <c r="W35" t="n">
+        <v>5162</v>
+      </c>
+      <c r="X35" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="Y35" t="inlineStr">
+        <is>
+          <t>5417</t>
         </is>
       </c>
     </row>
@@ -3266,9 +3480,15 @@
       <c r="V36" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W36" t="inlineStr">
-        <is>
-          <t>4990</t>
+      <c r="W36" t="n">
+        <v>4990</v>
+      </c>
+      <c r="X36" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y36" t="inlineStr">
+        <is>
+          <t>5243</t>
         </is>
       </c>
     </row>
@@ -3345,9 +3565,15 @@
       <c r="V37" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="W37" t="inlineStr">
-        <is>
-          <t>4277</t>
+      <c r="W37" t="n">
+        <v>4277</v>
+      </c>
+      <c r="X37" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y37" t="inlineStr">
+        <is>
+          <t>4400</t>
         </is>
       </c>
     </row>
@@ -3424,9 +3650,15 @@
       <c r="V38" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="W38" t="inlineStr">
-        <is>
-          <t>4809</t>
+      <c r="W38" t="n">
+        <v>4809</v>
+      </c>
+      <c r="X38" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y38" t="inlineStr">
+        <is>
+          <t>5090</t>
         </is>
       </c>
     </row>
@@ -3503,9 +3735,15 @@
       <c r="V39" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="W39" t="inlineStr">
-        <is>
-          <t>5136</t>
+      <c r="W39" t="n">
+        <v>5136</v>
+      </c>
+      <c r="X39" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="Y39" t="inlineStr">
+        <is>
+          <t>5214</t>
         </is>
       </c>
     </row>
@@ -3582,9 +3820,15 @@
       <c r="V40" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="W40" t="inlineStr">
-        <is>
-          <t>5687</t>
+      <c r="W40" t="n">
+        <v>5687</v>
+      </c>
+      <c r="X40" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="Y40" t="inlineStr">
+        <is>
+          <t>5994</t>
         </is>
       </c>
     </row>
@@ -3661,7 +3905,13 @@
       <c r="V41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W41" t="inlineStr">
+      <c r="W41" t="n">
+        <v>3632</v>
+      </c>
+      <c r="X41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y41" t="inlineStr">
         <is>
           <t>3632</t>
         </is>
@@ -3740,9 +3990,15 @@
       <c r="V42" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="W42" t="inlineStr">
-        <is>
-          <t>5654</t>
+      <c r="W42" t="n">
+        <v>5654</v>
+      </c>
+      <c r="X42" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="Y42" t="inlineStr">
+        <is>
+          <t>6001</t>
         </is>
       </c>
     </row>
@@ -3819,9 +4075,15 @@
       <c r="V43" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="W43" t="inlineStr">
-        <is>
-          <t>5247</t>
+      <c r="W43" t="n">
+        <v>5247</v>
+      </c>
+      <c r="X43" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y43" t="inlineStr">
+        <is>
+          <t>5422</t>
         </is>
       </c>
     </row>
@@ -3898,9 +4160,15 @@
       <c r="V44" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="W44" t="inlineStr">
-        <is>
-          <t>5183</t>
+      <c r="W44" t="n">
+        <v>5183</v>
+      </c>
+      <c r="X44" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Y44" t="inlineStr">
+        <is>
+          <t>5437</t>
         </is>
       </c>
     </row>
@@ -3977,9 +4245,15 @@
       <c r="V45" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="W45" t="inlineStr">
-        <is>
-          <t>4537</t>
+      <c r="W45" t="n">
+        <v>4537</v>
+      </c>
+      <c r="X45" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="Y45" t="inlineStr">
+        <is>
+          <t>4719</t>
         </is>
       </c>
     </row>
@@ -4056,9 +4330,15 @@
       <c r="V46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W46" t="inlineStr">
-        <is>
-          <t>4511</t>
+      <c r="W46" t="n">
+        <v>4511</v>
+      </c>
+      <c r="X46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y46" t="inlineStr">
+        <is>
+          <t>4633</t>
         </is>
       </c>
     </row>
@@ -4135,9 +4415,15 @@
       <c r="V47" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W47" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="W47" t="n">
+        <v>2500</v>
+      </c>
+      <c r="X47" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="Y47" t="inlineStr">
+        <is>
+          <t>2870</t>
         </is>
       </c>
     </row>
@@ -4214,9 +4500,15 @@
       <c r="V48" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="W48" t="inlineStr">
-        <is>
-          <t>5345</t>
+      <c r="W48" t="n">
+        <v>5345</v>
+      </c>
+      <c r="X48" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="Y48" t="inlineStr">
+        <is>
+          <t>5627</t>
         </is>
       </c>
     </row>
@@ -4293,9 +4585,15 @@
       <c r="V49" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="W49" t="inlineStr">
-        <is>
-          <t>3967</t>
+      <c r="W49" t="n">
+        <v>3967</v>
+      </c>
+      <c r="X49" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="Y49" t="inlineStr">
+        <is>
+          <t>4247</t>
         </is>
       </c>
     </row>
@@ -4372,9 +4670,15 @@
       <c r="V50" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="W50" t="inlineStr">
-        <is>
-          <t>5622</t>
+      <c r="W50" t="n">
+        <v>5622</v>
+      </c>
+      <c r="X50" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Y50" t="inlineStr">
+        <is>
+          <t>5909</t>
         </is>
       </c>
     </row>
@@ -4451,9 +4755,15 @@
       <c r="V51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W51" t="inlineStr">
-        <is>
-          <t>2841</t>
+      <c r="W51" t="n">
+        <v>2841</v>
+      </c>
+      <c r="X51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y51" t="inlineStr">
+        <is>
+          <t>2857</t>
         </is>
       </c>
     </row>
@@ -4530,9 +4840,15 @@
       <c r="V52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W52" t="inlineStr">
-        <is>
-          <t>2732</t>
+      <c r="W52" t="n">
+        <v>2732</v>
+      </c>
+      <c r="X52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y52" t="inlineStr">
+        <is>
+          <t>2758</t>
         </is>
       </c>
     </row>
@@ -4609,7 +4925,13 @@
       <c r="V53" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="W53" t="inlineStr">
+      <c r="W53" t="n">
+        <v>2850</v>
+      </c>
+      <c r="X53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y53" t="inlineStr">
         <is>
           <t>2850</t>
         </is>
@@ -4688,9 +5010,15 @@
       <c r="V54" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W54" t="inlineStr">
-        <is>
-          <t>5108</t>
+      <c r="W54" t="n">
+        <v>5108</v>
+      </c>
+      <c r="X54" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="Y54" t="inlineStr">
+        <is>
+          <t>5357</t>
         </is>
       </c>
     </row>
@@ -4767,9 +5095,15 @@
       <c r="V55" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="W55" t="inlineStr">
-        <is>
-          <t>3982</t>
+      <c r="W55" t="n">
+        <v>3982</v>
+      </c>
+      <c r="X55" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Y55" t="inlineStr">
+        <is>
+          <t>4167</t>
         </is>
       </c>
     </row>
@@ -4846,9 +5180,15 @@
       <c r="V56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W56" t="inlineStr">
-        <is>
-          <t>4041</t>
+      <c r="W56" t="n">
+        <v>4041</v>
+      </c>
+      <c r="X56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y56" t="inlineStr">
+        <is>
+          <t>4202</t>
         </is>
       </c>
     </row>
@@ -4925,9 +5265,15 @@
       <c r="V57" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="W57" t="inlineStr">
-        <is>
-          <t>4763</t>
+      <c r="W57" t="n">
+        <v>4763</v>
+      </c>
+      <c r="X57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y57" t="inlineStr">
+        <is>
+          <t>5043</t>
         </is>
       </c>
     </row>
@@ -5004,9 +5350,15 @@
       <c r="V58" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="W58" t="inlineStr">
-        <is>
-          <t>4084</t>
+      <c r="W58" t="n">
+        <v>4084</v>
+      </c>
+      <c r="X58" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="Y58" t="inlineStr">
+        <is>
+          <t>4199</t>
         </is>
       </c>
     </row>
@@ -5046,6 +5398,8 @@
       <c r="U59" t="inlineStr"/>
       <c r="V59" s="3" t="inlineStr"/>
       <c r="W59" t="inlineStr"/>
+      <c r="X59" s="3" t="inlineStr"/>
+      <c r="Y59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -5083,6 +5437,8 @@
       <c r="U60" t="inlineStr"/>
       <c r="V60" s="3" t="inlineStr"/>
       <c r="W60" t="inlineStr"/>
+      <c r="X60" s="3" t="inlineStr"/>
+      <c r="Y60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -5157,9 +5513,15 @@
       <c r="V61" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W61" t="inlineStr">
-        <is>
-          <t>4581</t>
+      <c r="W61" t="n">
+        <v>4581</v>
+      </c>
+      <c r="X61" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y61" t="inlineStr">
+        <is>
+          <t>4611</t>
         </is>
       </c>
     </row>
@@ -5236,7 +5598,13 @@
       <c r="V62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W62" t="inlineStr">
+      <c r="W62" t="n">
+        <v>0</v>
+      </c>
+      <c r="X62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5315,9 +5683,15 @@
       <c r="V63" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="W63" t="inlineStr">
-        <is>
-          <t>4816</t>
+      <c r="W63" t="n">
+        <v>4816</v>
+      </c>
+      <c r="X63" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="Y63" t="inlineStr">
+        <is>
+          <t>4928</t>
         </is>
       </c>
     </row>
@@ -5394,9 +5768,15 @@
       <c r="V64" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="W64" t="inlineStr">
-        <is>
-          <t>3031</t>
+      <c r="W64" t="n">
+        <v>3031</v>
+      </c>
+      <c r="X64" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y64" t="inlineStr">
+        <is>
+          <t>3088</t>
         </is>
       </c>
     </row>
@@ -5436,6 +5816,8 @@
       <c r="U65" t="inlineStr"/>
       <c r="V65" s="3" t="inlineStr"/>
       <c r="W65" t="inlineStr"/>
+      <c r="X65" s="3" t="inlineStr"/>
+      <c r="Y65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -5510,9 +5892,15 @@
       <c r="V66" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="W66" t="inlineStr">
-        <is>
-          <t>2631</t>
+      <c r="W66" t="n">
+        <v>2631</v>
+      </c>
+      <c r="X66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y66" t="inlineStr">
+        <is>
+          <t>2642</t>
         </is>
       </c>
     </row>
@@ -5589,9 +5977,15 @@
       <c r="V67" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="W67" t="inlineStr">
-        <is>
-          <t>4581</t>
+      <c r="W67" t="n">
+        <v>4581</v>
+      </c>
+      <c r="X67" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y67" t="inlineStr">
+        <is>
+          <t>4741</t>
         </is>
       </c>
     </row>
@@ -5668,9 +6062,15 @@
       <c r="V68" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="W68" t="inlineStr">
-        <is>
-          <t>5224</t>
+      <c r="W68" t="n">
+        <v>5224</v>
+      </c>
+      <c r="X68" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y68" t="inlineStr">
+        <is>
+          <t>5542</t>
         </is>
       </c>
     </row>
@@ -5747,9 +6147,15 @@
       <c r="V69" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="W69" t="inlineStr">
-        <is>
-          <t>4135</t>
+      <c r="W69" t="n">
+        <v>4135</v>
+      </c>
+      <c r="X69" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="Y69" t="inlineStr">
+        <is>
+          <t>4281</t>
         </is>
       </c>
     </row>
@@ -5826,9 +6232,15 @@
       <c r="V70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W70" t="inlineStr">
-        <is>
-          <t>2645</t>
+      <c r="W70" t="n">
+        <v>2645</v>
+      </c>
+      <c r="X70" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="Y70" t="inlineStr">
+        <is>
+          <t>3026</t>
         </is>
       </c>
     </row>
@@ -5905,9 +6317,15 @@
       <c r="V71" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="W71" t="inlineStr">
-        <is>
-          <t>4022</t>
+      <c r="W71" t="n">
+        <v>4022</v>
+      </c>
+      <c r="X71" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y71" t="inlineStr">
+        <is>
+          <t>4224</t>
         </is>
       </c>
     </row>
@@ -5984,7 +6402,13 @@
       <c r="V72" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="W72" t="inlineStr">
+      <c r="W72" t="n">
+        <v>3503</v>
+      </c>
+      <c r="X72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y72" t="inlineStr">
         <is>
           <t>3503</t>
         </is>
@@ -6063,9 +6487,15 @@
       <c r="V73" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W73" t="inlineStr">
-        <is>
-          <t>4028</t>
+      <c r="W73" t="n">
+        <v>4028</v>
+      </c>
+      <c r="X73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y73" t="inlineStr">
+        <is>
+          <t>4230</t>
         </is>
       </c>
     </row>
@@ -6142,9 +6572,15 @@
       <c r="V74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W74" t="inlineStr">
-        <is>
-          <t>2765</t>
+      <c r="W74" t="n">
+        <v>2765</v>
+      </c>
+      <c r="X74" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="Y74" t="inlineStr">
+        <is>
+          <t>3180</t>
         </is>
       </c>
     </row>
@@ -6221,9 +6657,15 @@
       <c r="V75" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="W75" t="inlineStr">
-        <is>
-          <t>3816</t>
+      <c r="W75" t="n">
+        <v>3816</v>
+      </c>
+      <c r="X75" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y75" t="inlineStr">
+        <is>
+          <t>3993</t>
         </is>
       </c>
     </row>
@@ -6300,9 +6742,15 @@
       <c r="V76" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="W76" t="inlineStr">
-        <is>
-          <t>4664</t>
+      <c r="W76" t="n">
+        <v>4664</v>
+      </c>
+      <c r="X76" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y76" t="inlineStr">
+        <is>
+          <t>4820</t>
         </is>
       </c>
     </row>
@@ -6379,7 +6827,13 @@
       <c r="V77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W77" t="inlineStr">
+      <c r="W77" t="n">
+        <v>3383</v>
+      </c>
+      <c r="X77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y77" t="inlineStr">
         <is>
           <t>3383</t>
         </is>
@@ -6458,9 +6912,15 @@
       <c r="V78" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W78" t="inlineStr">
-        <is>
-          <t>4699</t>
+      <c r="W78" t="n">
+        <v>4699</v>
+      </c>
+      <c r="X78" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y78" t="inlineStr">
+        <is>
+          <t>4843</t>
         </is>
       </c>
     </row>
@@ -6537,7 +6997,13 @@
       <c r="V79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W79" t="inlineStr">
+      <c r="W79" t="n">
+        <v>0</v>
+      </c>
+      <c r="X79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6616,9 +7082,15 @@
       <c r="V80" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="W80" t="inlineStr">
-        <is>
-          <t>4551</t>
+      <c r="W80" t="n">
+        <v>4551</v>
+      </c>
+      <c r="X80" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="Y80" t="inlineStr">
+        <is>
+          <t>4722</t>
         </is>
       </c>
     </row>
@@ -6695,9 +7167,15 @@
       <c r="V81" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="W81" t="inlineStr">
-        <is>
-          <t>4469</t>
+      <c r="W81" t="n">
+        <v>4469</v>
+      </c>
+      <c r="X81" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y81" t="inlineStr">
+        <is>
+          <t>4717</t>
         </is>
       </c>
     </row>
@@ -6774,9 +7252,15 @@
       <c r="V82" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="W82" t="inlineStr">
-        <is>
-          <t>4275</t>
+      <c r="W82" t="n">
+        <v>4275</v>
+      </c>
+      <c r="X82" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y82" t="inlineStr">
+        <is>
+          <t>4468</t>
         </is>
       </c>
     </row>
@@ -6853,9 +7337,15 @@
       <c r="V83" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="W83" t="inlineStr">
-        <is>
-          <t>4209</t>
+      <c r="W83" t="n">
+        <v>4209</v>
+      </c>
+      <c r="X83" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="Y83" t="inlineStr">
+        <is>
+          <t>4285</t>
         </is>
       </c>
     </row>
@@ -6932,9 +7422,15 @@
       <c r="V84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W84" t="inlineStr">
-        <is>
-          <t>2990</t>
+      <c r="W84" t="n">
+        <v>2990</v>
+      </c>
+      <c r="X84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y84" t="inlineStr">
+        <is>
+          <t>3008</t>
         </is>
       </c>
     </row>
@@ -7011,9 +7507,15 @@
       <c r="V85" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="W85" t="inlineStr">
-        <is>
-          <t>3513</t>
+      <c r="W85" t="n">
+        <v>3513</v>
+      </c>
+      <c r="X85" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y85" t="inlineStr">
+        <is>
+          <t>3641</t>
         </is>
       </c>
     </row>
@@ -7090,9 +7592,15 @@
       <c r="V86" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="W86" t="inlineStr">
-        <is>
-          <t>3186</t>
+      <c r="W86" t="n">
+        <v>3186</v>
+      </c>
+      <c r="X86" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y86" t="inlineStr">
+        <is>
+          <t>3193</t>
         </is>
       </c>
     </row>
@@ -7169,9 +7677,15 @@
       <c r="V87" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W87" t="inlineStr">
-        <is>
-          <t>4303</t>
+      <c r="W87" t="n">
+        <v>4303</v>
+      </c>
+      <c r="X87" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y87" t="inlineStr">
+        <is>
+          <t>4570</t>
         </is>
       </c>
     </row>
@@ -7248,9 +7762,15 @@
       <c r="V88" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W88" t="inlineStr">
-        <is>
-          <t>2928</t>
+      <c r="W88" t="n">
+        <v>2928</v>
+      </c>
+      <c r="X88" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y88" t="inlineStr">
+        <is>
+          <t>2986</t>
         </is>
       </c>
     </row>
@@ -7327,9 +7847,15 @@
       <c r="V89" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W89" t="inlineStr">
-        <is>
-          <t>3223</t>
+      <c r="W89" t="n">
+        <v>3223</v>
+      </c>
+      <c r="X89" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y89" t="inlineStr">
+        <is>
+          <t>3301</t>
         </is>
       </c>
     </row>
@@ -7406,9 +7932,15 @@
       <c r="V90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W90" t="inlineStr">
-        <is>
-          <t>2759</t>
+      <c r="W90" t="n">
+        <v>2759</v>
+      </c>
+      <c r="X90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y90" t="inlineStr">
+        <is>
+          <t>2720</t>
         </is>
       </c>
     </row>
@@ -7485,9 +8017,15 @@
       <c r="V91" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W91" t="inlineStr">
-        <is>
-          <t>2794</t>
+      <c r="W91" t="n">
+        <v>2794</v>
+      </c>
+      <c r="X91" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y91" t="inlineStr">
+        <is>
+          <t>2836</t>
         </is>
       </c>
     </row>
@@ -7564,7 +8102,13 @@
       <c r="V92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W92" t="inlineStr">
+      <c r="W92" t="n">
+        <v>0</v>
+      </c>
+      <c r="X92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7643,9 +8187,15 @@
       <c r="V93" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W93" t="inlineStr">
-        <is>
-          <t>2673</t>
+      <c r="W93" t="n">
+        <v>2673</v>
+      </c>
+      <c r="X93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y93" t="inlineStr">
+        <is>
+          <t>2667</t>
         </is>
       </c>
     </row>
@@ -7722,9 +8272,15 @@
       <c r="V94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W94" t="inlineStr">
-        <is>
-          <t>3227</t>
+      <c r="W94" t="n">
+        <v>3227</v>
+      </c>
+      <c r="X94" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y94" t="inlineStr">
+        <is>
+          <t>3250</t>
         </is>
       </c>
     </row>
@@ -7801,9 +8357,15 @@
       <c r="V95" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="W95" t="inlineStr">
-        <is>
-          <t>2551</t>
+      <c r="W95" t="n">
+        <v>2551</v>
+      </c>
+      <c r="X95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y95" t="inlineStr">
+        <is>
+          <t>2535</t>
         </is>
       </c>
     </row>
@@ -7880,9 +8442,15 @@
       <c r="V96" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W96" t="inlineStr">
-        <is>
-          <t>3435</t>
+      <c r="W96" t="n">
+        <v>3435</v>
+      </c>
+      <c r="X96" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="Y96" t="inlineStr">
+        <is>
+          <t>3605</t>
         </is>
       </c>
     </row>
@@ -7959,9 +8527,15 @@
       <c r="V97" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="W97" t="inlineStr">
-        <is>
-          <t>2586</t>
+      <c r="W97" t="n">
+        <v>2586</v>
+      </c>
+      <c r="X97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y97" t="inlineStr">
+        <is>
+          <t>2585</t>
         </is>
       </c>
     </row>
@@ -8038,7 +8612,13 @@
       <c r="V98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W98" t="inlineStr">
+      <c r="W98" t="n">
+        <v>0</v>
+      </c>
+      <c r="X98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8117,9 +8697,15 @@
       <c r="V99" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W99" t="inlineStr">
-        <is>
-          <t>3688</t>
+      <c r="W99" t="n">
+        <v>3688</v>
+      </c>
+      <c r="X99" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y99" t="inlineStr">
+        <is>
+          <t>3693</t>
         </is>
       </c>
     </row>
@@ -8196,9 +8782,15 @@
       <c r="V100" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="W100" t="inlineStr">
-        <is>
-          <t>2579</t>
+      <c r="W100" t="n">
+        <v>2579</v>
+      </c>
+      <c r="X100" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="Y100" t="inlineStr">
+        <is>
+          <t>2794</t>
         </is>
       </c>
     </row>
@@ -8275,9 +8867,15 @@
       <c r="V101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W101" t="inlineStr">
-        <is>
-          <t>4113</t>
+      <c r="W101" t="n">
+        <v>4113</v>
+      </c>
+      <c r="X101" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="Y101" t="inlineStr">
+        <is>
+          <t>4173</t>
         </is>
       </c>
     </row>
@@ -8354,9 +8952,15 @@
       <c r="V102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W102" t="inlineStr">
-        <is>
-          <t>3763</t>
+      <c r="W102" t="n">
+        <v>3763</v>
+      </c>
+      <c r="X102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y102" t="inlineStr">
+        <is>
+          <t>3860</t>
         </is>
       </c>
     </row>
@@ -8433,9 +9037,15 @@
       <c r="V103" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="W103" t="inlineStr">
-        <is>
-          <t>2580</t>
+      <c r="W103" t="n">
+        <v>2580</v>
+      </c>
+      <c r="X103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y103" t="inlineStr">
+        <is>
+          <t>2607</t>
         </is>
       </c>
     </row>
@@ -8512,9 +9122,15 @@
       <c r="V104" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="W104" t="inlineStr">
-        <is>
-          <t>4161</t>
+      <c r="W104" t="n">
+        <v>4161</v>
+      </c>
+      <c r="X104" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="Y104" t="inlineStr">
+        <is>
+          <t>4349</t>
         </is>
       </c>
     </row>
@@ -8591,9 +9207,15 @@
       <c r="V105" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="W105" t="inlineStr">
-        <is>
-          <t>3836</t>
+      <c r="W105" t="n">
+        <v>3836</v>
+      </c>
+      <c r="X105" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="Y105" t="inlineStr">
+        <is>
+          <t>3985</t>
         </is>
       </c>
     </row>
@@ -8670,7 +9292,13 @@
       <c r="V106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W106" t="inlineStr">
+      <c r="W106" t="n">
+        <v>0</v>
+      </c>
+      <c r="X106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8749,9 +9377,15 @@
       <c r="V107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W107" t="inlineStr">
-        <is>
-          <t>2516</t>
+      <c r="W107" t="n">
+        <v>2516</v>
+      </c>
+      <c r="X107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y107" t="inlineStr">
+        <is>
+          <t>2502</t>
         </is>
       </c>
     </row>
@@ -8828,7 +9462,13 @@
       <c r="V108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W108" t="inlineStr">
+      <c r="W108" t="n">
+        <v>0</v>
+      </c>
+      <c r="X108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8907,9 +9547,15 @@
       <c r="V109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W109" t="inlineStr">
-        <is>
-          <t>3587</t>
+      <c r="W109" t="n">
+        <v>3587</v>
+      </c>
+      <c r="X109" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y109" t="inlineStr">
+        <is>
+          <t>3645</t>
         </is>
       </c>
     </row>
@@ -8986,9 +9632,15 @@
       <c r="V110" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W110" t="inlineStr">
-        <is>
-          <t>3627</t>
+      <c r="W110" t="n">
+        <v>3627</v>
+      </c>
+      <c r="X110" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="Y110" t="inlineStr">
+        <is>
+          <t>3617</t>
         </is>
       </c>
     </row>
@@ -9065,9 +9717,15 @@
       <c r="V111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W111" t="inlineStr">
-        <is>
-          <t>2578</t>
+      <c r="W111" t="n">
+        <v>2578</v>
+      </c>
+      <c r="X111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y111" t="inlineStr">
+        <is>
+          <t>2594</t>
         </is>
       </c>
     </row>
@@ -9144,9 +9802,15 @@
       <c r="V112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W112" t="inlineStr">
-        <is>
-          <t>2888</t>
+      <c r="W112" t="n">
+        <v>2888</v>
+      </c>
+      <c r="X112" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y112" t="inlineStr">
+        <is>
+          <t>2938</t>
         </is>
       </c>
     </row>
@@ -9223,9 +9887,15 @@
       <c r="V113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W113" t="inlineStr">
-        <is>
-          <t>3298</t>
+      <c r="W113" t="n">
+        <v>3298</v>
+      </c>
+      <c r="X113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y113" t="inlineStr">
+        <is>
+          <t>3423</t>
         </is>
       </c>
     </row>
@@ -9302,9 +9972,15 @@
       <c r="V114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W114" t="inlineStr">
-        <is>
-          <t>2833</t>
+      <c r="W114" t="n">
+        <v>2833</v>
+      </c>
+      <c r="X114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y114" t="inlineStr">
+        <is>
+          <t>2980</t>
         </is>
       </c>
     </row>
@@ -9381,9 +10057,15 @@
       <c r="V115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W115" t="inlineStr">
-        <is>
-          <t>2349</t>
+      <c r="W115" t="n">
+        <v>2349</v>
+      </c>
+      <c r="X115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y115" t="inlineStr">
+        <is>
+          <t>2341</t>
         </is>
       </c>
     </row>
@@ -9460,9 +10142,15 @@
       <c r="V116" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="W116" t="inlineStr">
-        <is>
-          <t>3121</t>
+      <c r="W116" t="n">
+        <v>3121</v>
+      </c>
+      <c r="X116" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="Y116" t="inlineStr">
+        <is>
+          <t>3261</t>
         </is>
       </c>
     </row>
@@ -9539,9 +10227,15 @@
       <c r="V117" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W117" t="inlineStr">
-        <is>
-          <t>3566</t>
+      <c r="W117" t="n">
+        <v>3566</v>
+      </c>
+      <c r="X117" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y117" t="inlineStr">
+        <is>
+          <t>3572</t>
         </is>
       </c>
     </row>
@@ -9618,7 +10312,13 @@
       <c r="V118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W118" t="inlineStr">
+      <c r="W118" t="n">
+        <v>0</v>
+      </c>
+      <c r="X118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9697,9 +10397,15 @@
       <c r="V119" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W119" t="inlineStr">
-        <is>
-          <t>3819</t>
+      <c r="W119" t="n">
+        <v>3819</v>
+      </c>
+      <c r="X119" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y119" t="inlineStr">
+        <is>
+          <t>3879</t>
         </is>
       </c>
     </row>
@@ -9776,9 +10482,15 @@
       <c r="V120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W120" t="inlineStr">
-        <is>
-          <t>2580</t>
+      <c r="W120" t="n">
+        <v>2580</v>
+      </c>
+      <c r="X120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y120" t="inlineStr">
+        <is>
+          <t>2572</t>
         </is>
       </c>
     </row>
@@ -9855,9 +10567,15 @@
       <c r="V121" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="W121" t="inlineStr">
-        <is>
-          <t>3308</t>
+      <c r="W121" t="n">
+        <v>3308</v>
+      </c>
+      <c r="X121" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y121" t="inlineStr">
+        <is>
+          <t>3408</t>
         </is>
       </c>
     </row>
@@ -9934,7 +10652,13 @@
       <c r="V122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W122" t="inlineStr">
+      <c r="W122" t="n">
+        <v>0</v>
+      </c>
+      <c r="X122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10013,9 +10737,15 @@
       <c r="V123" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W123" t="inlineStr">
-        <is>
-          <t>3159</t>
+      <c r="W123" t="n">
+        <v>3159</v>
+      </c>
+      <c r="X123" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y123" t="inlineStr">
+        <is>
+          <t>3265</t>
         </is>
       </c>
     </row>
@@ -10092,9 +10822,15 @@
       <c r="V124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W124" t="inlineStr">
-        <is>
-          <t>3132</t>
+      <c r="W124" t="n">
+        <v>3132</v>
+      </c>
+      <c r="X124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y124" t="inlineStr">
+        <is>
+          <t>3205</t>
         </is>
       </c>
     </row>
@@ -10171,9 +10907,15 @@
       <c r="V125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W125" t="inlineStr">
-        <is>
-          <t>3377</t>
+      <c r="W125" t="n">
+        <v>3377</v>
+      </c>
+      <c r="X125" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y125" t="inlineStr">
+        <is>
+          <t>3552</t>
         </is>
       </c>
     </row>
@@ -10250,9 +10992,15 @@
       <c r="V126" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W126" t="inlineStr">
-        <is>
-          <t>3171</t>
+      <c r="W126" t="n">
+        <v>3171</v>
+      </c>
+      <c r="X126" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y126" t="inlineStr">
+        <is>
+          <t>3262</t>
         </is>
       </c>
     </row>
@@ -10329,9 +11077,15 @@
       <c r="V127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W127" t="inlineStr">
-        <is>
-          <t>2364</t>
+      <c r="W127" t="n">
+        <v>2364</v>
+      </c>
+      <c r="X127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y127" t="inlineStr">
+        <is>
+          <t>2352</t>
         </is>
       </c>
     </row>
@@ -10408,7 +11162,13 @@
       <c r="V128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W128" t="inlineStr">
+      <c r="W128" t="n">
+        <v>0</v>
+      </c>
+      <c r="X128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10487,7 +11247,13 @@
       <c r="V129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W129" t="inlineStr">
+      <c r="W129" t="n">
+        <v>0</v>
+      </c>
+      <c r="X129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10566,9 +11332,15 @@
       <c r="V130" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="W130" t="inlineStr">
-        <is>
-          <t>2832</t>
+      <c r="W130" t="n">
+        <v>2832</v>
+      </c>
+      <c r="X130" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="Y130" t="inlineStr">
+        <is>
+          <t>2822</t>
         </is>
       </c>
     </row>
@@ -10645,9 +11417,15 @@
       <c r="V131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W131" t="inlineStr">
-        <is>
-          <t>2464</t>
+      <c r="W131" t="n">
+        <v>2464</v>
+      </c>
+      <c r="X131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y131" t="inlineStr">
+        <is>
+          <t>2550</t>
         </is>
       </c>
     </row>
@@ -10724,9 +11502,15 @@
       <c r="V132" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W132" t="inlineStr">
-        <is>
-          <t>2678</t>
+      <c r="W132" t="n">
+        <v>2678</v>
+      </c>
+      <c r="X132" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y132" t="inlineStr">
+        <is>
+          <t>2690</t>
         </is>
       </c>
     </row>
@@ -10803,9 +11587,15 @@
       <c r="V133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W133" t="inlineStr">
-        <is>
-          <t>2784</t>
+      <c r="W133" t="n">
+        <v>2784</v>
+      </c>
+      <c r="X133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y133" t="inlineStr">
+        <is>
+          <t>2796</t>
         </is>
       </c>
     </row>
@@ -10869,6 +11659,8 @@
       <c r="U134" t="inlineStr"/>
       <c r="V134" s="3" t="inlineStr"/>
       <c r="W134" t="inlineStr"/>
+      <c r="X134" s="3" t="inlineStr"/>
+      <c r="Y134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -10922,6 +11714,8 @@
       <c r="U135" t="inlineStr"/>
       <c r="V135" s="3" t="inlineStr"/>
       <c r="W135" t="inlineStr"/>
+      <c r="X135" s="3" t="inlineStr"/>
+      <c r="Y135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -10996,9 +11790,15 @@
       <c r="V136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W136" t="inlineStr">
-        <is>
-          <t>2679</t>
+      <c r="W136" t="n">
+        <v>2679</v>
+      </c>
+      <c r="X136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y136" t="inlineStr">
+        <is>
+          <t>2677</t>
         </is>
       </c>
     </row>
@@ -11075,9 +11875,15 @@
       <c r="V137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W137" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="W137" t="n">
+        <v>0</v>
+      </c>
+      <c r="X137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y137" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -11133,6 +11939,8 @@
       <c r="U138" t="inlineStr"/>
       <c r="V138" s="3" t="inlineStr"/>
       <c r="W138" t="inlineStr"/>
+      <c r="X138" s="3" t="inlineStr"/>
+      <c r="Y138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -11207,9 +12015,15 @@
       <c r="V139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W139" t="inlineStr">
-        <is>
-          <t>2386</t>
+      <c r="W139" t="n">
+        <v>2386</v>
+      </c>
+      <c r="X139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y139" t="inlineStr">
+        <is>
+          <t>2377</t>
         </is>
       </c>
     </row>
@@ -11286,9 +12100,15 @@
       <c r="V140" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W140" t="inlineStr">
-        <is>
-          <t>2784</t>
+      <c r="W140" t="n">
+        <v>2784</v>
+      </c>
+      <c r="X140" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y140" t="inlineStr">
+        <is>
+          <t>2906</t>
         </is>
       </c>
     </row>
@@ -11344,6 +12164,8 @@
       <c r="U141" t="inlineStr"/>
       <c r="V141" s="3" t="inlineStr"/>
       <c r="W141" t="inlineStr"/>
+      <c r="X141" s="3" t="inlineStr"/>
+      <c r="Y141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -11418,9 +12240,15 @@
       <c r="V142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W142" t="inlineStr">
-        <is>
-          <t>2178</t>
+      <c r="W142" t="n">
+        <v>2178</v>
+      </c>
+      <c r="X142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y142" t="inlineStr">
+        <is>
+          <t>2173</t>
         </is>
       </c>
     </row>
@@ -11476,6 +12304,8 @@
       <c r="U143" t="inlineStr"/>
       <c r="V143" s="3" t="inlineStr"/>
       <c r="W143" t="inlineStr"/>
+      <c r="X143" s="3" t="inlineStr"/>
+      <c r="Y143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -11529,6 +12359,8 @@
       <c r="U144" t="inlineStr"/>
       <c r="V144" s="3" t="inlineStr"/>
       <c r="W144" t="inlineStr"/>
+      <c r="X144" s="3" t="inlineStr"/>
+      <c r="Y144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -11582,6 +12414,8 @@
       <c r="U145" t="inlineStr"/>
       <c r="V145" s="3" t="inlineStr"/>
       <c r="W145" t="inlineStr"/>
+      <c r="X145" s="3" t="inlineStr"/>
+      <c r="Y145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -11635,6 +12469,8 @@
       <c r="U146" t="inlineStr"/>
       <c r="V146" s="3" t="inlineStr"/>
       <c r="W146" t="inlineStr"/>
+      <c r="X146" s="3" t="inlineStr"/>
+      <c r="Y146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -11688,6 +12524,8 @@
       <c r="U147" t="inlineStr"/>
       <c r="V147" s="3" t="inlineStr"/>
       <c r="W147" t="inlineStr"/>
+      <c r="X147" s="3" t="inlineStr"/>
+      <c r="Y147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -11762,9 +12600,15 @@
       <c r="V148" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="W148" t="inlineStr">
-        <is>
-          <t>1516</t>
+      <c r="W148" t="n">
+        <v>1516</v>
+      </c>
+      <c r="X148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y148" t="inlineStr">
+        <is>
+          <t>1514</t>
         </is>
       </c>
     </row>
@@ -11841,7 +12685,13 @@
       <c r="V149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W149" t="inlineStr">
+      <c r="W149" t="n">
+        <v>3849</v>
+      </c>
+      <c r="X149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y149" t="inlineStr">
         <is>
           <t>3849</t>
         </is>
@@ -11920,7 +12770,13 @@
       <c r="V150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W150" t="inlineStr">
+      <c r="W150" t="n">
+        <v>0</v>
+      </c>
+      <c r="X150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11999,9 +12855,15 @@
       <c r="V151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W151" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="W151" t="n">
+        <v>2500</v>
+      </c>
+      <c r="X151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y151" t="inlineStr">
+        <is>
+          <t>2511</t>
         </is>
       </c>
     </row>
@@ -12078,7 +12940,13 @@
       <c r="V152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W152" t="inlineStr">
+      <c r="W152" t="n">
+        <v>0</v>
+      </c>
+      <c r="X152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12157,7 +13025,13 @@
       <c r="V153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W153" t="inlineStr">
+      <c r="W153" t="n">
+        <v>0</v>
+      </c>
+      <c r="X153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12236,7 +13110,13 @@
       <c r="V154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W154" t="inlineStr">
+      <c r="W154" t="n">
+        <v>0</v>
+      </c>
+      <c r="X154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12315,9 +13195,15 @@
       <c r="V155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W155" t="inlineStr">
-        <is>
-          <t>2614</t>
+      <c r="W155" t="n">
+        <v>2614</v>
+      </c>
+      <c r="X155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y155" t="inlineStr">
+        <is>
+          <t>2694</t>
         </is>
       </c>
     </row>
@@ -12388,9 +13274,15 @@
       <c r="V156" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="W156" t="inlineStr">
-        <is>
-          <t>3451</t>
+      <c r="W156" t="n">
+        <v>3451</v>
+      </c>
+      <c r="X156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y156" t="inlineStr">
+        <is>
+          <t>3449</t>
         </is>
       </c>
     </row>
@@ -12440,6 +13332,8 @@
       <c r="U157" t="inlineStr"/>
       <c r="V157" s="3" t="inlineStr"/>
       <c r="W157" t="inlineStr"/>
+      <c r="X157" s="3" t="inlineStr"/>
+      <c r="Y157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -12508,7 +13402,13 @@
       <c r="V158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W158" t="inlineStr">
+      <c r="W158" t="n">
+        <v>0</v>
+      </c>
+      <c r="X158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12581,9 +13481,15 @@
       <c r="V159" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W159" t="inlineStr">
-        <is>
-          <t>2921</t>
+      <c r="W159" t="n">
+        <v>2921</v>
+      </c>
+      <c r="X159" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y159" t="inlineStr">
+        <is>
+          <t>2937</t>
         </is>
       </c>
     </row>
@@ -12633,6 +13539,8 @@
       <c r="U160" t="inlineStr"/>
       <c r="V160" s="3" t="inlineStr"/>
       <c r="W160" t="inlineStr"/>
+      <c r="X160" s="3" t="inlineStr"/>
+      <c r="Y160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -12689,9 +13597,15 @@
       <c r="V161" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="W161" t="inlineStr">
-        <is>
-          <t>2773</t>
+      <c r="W161" t="n">
+        <v>2773</v>
+      </c>
+      <c r="X161" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Y161" t="inlineStr">
+        <is>
+          <t>2915</t>
         </is>
       </c>
     </row>
@@ -12750,9 +13664,15 @@
       <c r="V162" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="W162" t="inlineStr">
-        <is>
-          <t>2532</t>
+      <c r="W162" t="n">
+        <v>2532</v>
+      </c>
+      <c r="X162" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="Y162" t="inlineStr">
+        <is>
+          <t>2632</t>
         </is>
       </c>
     </row>
@@ -12807,9 +13727,15 @@
       <c r="V163" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W163" t="inlineStr">
-        <is>
-          <t>2953</t>
+      <c r="W163" t="n">
+        <v>2953</v>
+      </c>
+      <c r="X163" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y163" t="inlineStr">
+        <is>
+          <t>2942</t>
         </is>
       </c>
     </row>
@@ -12852,9 +13778,15 @@
       <c r="V164" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W164" t="inlineStr">
-        <is>
-          <t>3418</t>
+      <c r="W164" t="n">
+        <v>3418</v>
+      </c>
+      <c r="X164" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y164" t="inlineStr">
+        <is>
+          <t>3370</t>
         </is>
       </c>
     </row>
@@ -12897,9 +13829,60 @@
       <c r="V165" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="W165" t="inlineStr">
-        <is>
-          <t>2809</t>
+      <c r="W165" t="n">
+        <v>2809</v>
+      </c>
+      <c r="X165" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="Y165" t="inlineStr">
+        <is>
+          <t>2786</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>31401481</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Player-31401481</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr"/>
+      <c r="D166" t="inlineStr"/>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F166" s="3" t="inlineStr"/>
+      <c r="G166" t="inlineStr"/>
+      <c r="H166" s="3" t="inlineStr"/>
+      <c r="I166" t="inlineStr"/>
+      <c r="J166" s="3" t="inlineStr"/>
+      <c r="K166" t="inlineStr"/>
+      <c r="L166" s="3" t="inlineStr"/>
+      <c r="M166" t="inlineStr"/>
+      <c r="N166" s="3" t="inlineStr"/>
+      <c r="O166" t="inlineStr"/>
+      <c r="P166" s="3" t="inlineStr"/>
+      <c r="Q166" t="inlineStr"/>
+      <c r="R166" s="3" t="inlineStr"/>
+      <c r="S166" t="inlineStr"/>
+      <c r="T166" s="3" t="inlineStr"/>
+      <c r="U166" t="inlineStr"/>
+      <c r="V166" s="3" t="inlineStr"/>
+      <c r="W166" t="inlineStr"/>
+      <c r="X166" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y166" t="inlineStr">
+        <is>
+          <t>2567</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-02-22 11:30:35
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -13842,10 +13842,8 @@
       </c>
     </row>
     <row r="166">
-      <c r="A166" t="inlineStr">
-        <is>
-          <t>31401481</t>
-        </is>
+      <c r="A166" t="n">
+        <v>31401481</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Code updated 23-02-24 11:30:34
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA166"/>
+  <dimension ref="A1:AC166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,6 +526,16 @@
           <t>02-22_0</t>
         </is>
       </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>02-23_A</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>02-23_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -612,9 +622,15 @@
       <c r="Z2" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>3916</t>
+      <c r="AA2" t="n">
+        <v>3916</v>
+      </c>
+      <c r="AB2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>3926</t>
         </is>
       </c>
     </row>
@@ -703,9 +719,15 @@
       <c r="Z3" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t>5721</t>
+      <c r="AA3" t="n">
+        <v>5721</v>
+      </c>
+      <c r="AB3" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>6141</t>
         </is>
       </c>
     </row>
@@ -794,9 +816,15 @@
       <c r="Z4" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t>5973</t>
+      <c r="AA4" t="n">
+        <v>5973</v>
+      </c>
+      <c r="AB4" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>6313</t>
         </is>
       </c>
     </row>
@@ -885,9 +913,15 @@
       <c r="Z5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA5" t="inlineStr">
-        <is>
-          <t>5355</t>
+      <c r="AA5" t="n">
+        <v>5355</v>
+      </c>
+      <c r="AB5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>5653</t>
         </is>
       </c>
     </row>
@@ -976,9 +1010,15 @@
       <c r="Z6" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AA6" t="inlineStr">
-        <is>
-          <t>5606</t>
+      <c r="AA6" t="n">
+        <v>5606</v>
+      </c>
+      <c r="AB6" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>5856</t>
         </is>
       </c>
     </row>
@@ -1067,9 +1107,15 @@
       <c r="Z7" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AA7" t="inlineStr">
-        <is>
-          <t>6405</t>
+      <c r="AA7" t="n">
+        <v>6405</v>
+      </c>
+      <c r="AB7" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>6669</t>
         </is>
       </c>
     </row>
@@ -1158,9 +1204,15 @@
       <c r="Z8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA8" t="inlineStr">
-        <is>
-          <t>4944</t>
+      <c r="AA8" t="n">
+        <v>4944</v>
+      </c>
+      <c r="AB8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t>5165</t>
         </is>
       </c>
     </row>
@@ -1249,9 +1301,15 @@
       <c r="Z9" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AA9" t="inlineStr">
-        <is>
-          <t>5252</t>
+      <c r="AA9" t="n">
+        <v>5252</v>
+      </c>
+      <c r="AB9" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>5337</t>
         </is>
       </c>
     </row>
@@ -1340,9 +1398,15 @@
       <c r="Z10" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="AA10" t="inlineStr">
-        <is>
-          <t>6225</t>
+      <c r="AA10" t="n">
+        <v>6225</v>
+      </c>
+      <c r="AB10" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AC10" t="inlineStr">
+        <is>
+          <t>6591</t>
         </is>
       </c>
     </row>
@@ -1431,9 +1495,15 @@
       <c r="Z11" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA11" t="inlineStr">
-        <is>
-          <t>5211</t>
+      <c r="AA11" t="n">
+        <v>5211</v>
+      </c>
+      <c r="AB11" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC11" t="inlineStr">
+        <is>
+          <t>5569</t>
         </is>
       </c>
     </row>
@@ -1522,7 +1592,13 @@
       <c r="Z12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA12" t="inlineStr">
+      <c r="AA12" t="n">
+        <v>2914</v>
+      </c>
+      <c r="AB12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC12" t="inlineStr">
         <is>
           <t>2914</t>
         </is>
@@ -1613,9 +1689,15 @@
       <c r="Z13" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AA13" t="inlineStr">
-        <is>
-          <t>6319</t>
+      <c r="AA13" t="n">
+        <v>6319</v>
+      </c>
+      <c r="AB13" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC13" t="inlineStr">
+        <is>
+          <t>6493</t>
         </is>
       </c>
     </row>
@@ -1704,9 +1786,15 @@
       <c r="Z14" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AA14" t="inlineStr">
-        <is>
-          <t>5461</t>
+      <c r="AA14" t="n">
+        <v>5461</v>
+      </c>
+      <c r="AB14" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AC14" t="inlineStr">
+        <is>
+          <t>5680</t>
         </is>
       </c>
     </row>
@@ -1795,9 +1883,15 @@
       <c r="Z15" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA15" t="inlineStr">
-        <is>
-          <t>5165</t>
+      <c r="AA15" t="n">
+        <v>5165</v>
+      </c>
+      <c r="AB15" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC15" t="inlineStr">
+        <is>
+          <t>5430</t>
         </is>
       </c>
     </row>
@@ -1886,9 +1980,15 @@
       <c r="Z16" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA16" t="inlineStr">
-        <is>
-          <t>5607</t>
+      <c r="AA16" t="n">
+        <v>5607</v>
+      </c>
+      <c r="AB16" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AC16" t="inlineStr">
+        <is>
+          <t>6002</t>
         </is>
       </c>
     </row>
@@ -1977,9 +2077,15 @@
       <c r="Z17" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AA17" t="inlineStr">
-        <is>
-          <t>4421</t>
+      <c r="AA17" t="n">
+        <v>4421</v>
+      </c>
+      <c r="AB17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC17" t="inlineStr">
+        <is>
+          <t>4463</t>
         </is>
       </c>
     </row>
@@ -2068,9 +2174,15 @@
       <c r="Z18" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA18" t="inlineStr">
-        <is>
-          <t>4274</t>
+      <c r="AA18" t="n">
+        <v>4274</v>
+      </c>
+      <c r="AB18" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC18" t="inlineStr">
+        <is>
+          <t>4594</t>
         </is>
       </c>
     </row>
@@ -2159,9 +2271,15 @@
       <c r="Z19" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="AA19" t="inlineStr">
-        <is>
-          <t>5477</t>
+      <c r="AA19" t="n">
+        <v>5477</v>
+      </c>
+      <c r="AB19" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC19" t="inlineStr">
+        <is>
+          <t>5786</t>
         </is>
       </c>
     </row>
@@ -2250,9 +2368,15 @@
       <c r="Z20" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AA20" t="inlineStr">
-        <is>
-          <t>6473</t>
+      <c r="AA20" t="n">
+        <v>6473</v>
+      </c>
+      <c r="AB20" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AC20" t="inlineStr">
+        <is>
+          <t>6836</t>
         </is>
       </c>
     </row>
@@ -2341,9 +2465,15 @@
       <c r="Z21" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="AA21" t="inlineStr">
-        <is>
-          <t>4950</t>
+      <c r="AA21" t="n">
+        <v>4950</v>
+      </c>
+      <c r="AB21" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC21" t="inlineStr">
+        <is>
+          <t>5361</t>
         </is>
       </c>
     </row>
@@ -2432,9 +2562,15 @@
       <c r="Z22" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AA22" t="inlineStr">
-        <is>
-          <t>5224</t>
+      <c r="AA22" t="n">
+        <v>5224</v>
+      </c>
+      <c r="AB22" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC22" t="inlineStr">
+        <is>
+          <t>5376</t>
         </is>
       </c>
     </row>
@@ -2523,9 +2659,15 @@
       <c r="Z23" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AA23" t="inlineStr">
-        <is>
-          <t>5114</t>
+      <c r="AA23" t="n">
+        <v>5114</v>
+      </c>
+      <c r="AB23" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AC23" t="inlineStr">
+        <is>
+          <t>5600</t>
         </is>
       </c>
     </row>
@@ -2614,9 +2756,15 @@
       <c r="Z24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AA24" t="inlineStr">
-        <is>
-          <t>5760</t>
+      <c r="AA24" t="n">
+        <v>5760</v>
+      </c>
+      <c r="AB24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC24" t="inlineStr">
+        <is>
+          <t>6110</t>
         </is>
       </c>
     </row>
@@ -2705,7 +2853,13 @@
       <c r="Z25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA25" t="inlineStr">
+      <c r="AA25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2796,9 +2950,15 @@
       <c r="Z26" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="AA26" t="inlineStr">
-        <is>
-          <t>5732</t>
+      <c r="AA26" t="n">
+        <v>5732</v>
+      </c>
+      <c r="AB26" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC26" t="inlineStr">
+        <is>
+          <t>5947</t>
         </is>
       </c>
     </row>
@@ -2887,9 +3047,15 @@
       <c r="Z27" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AA27" t="inlineStr">
-        <is>
-          <t>5910</t>
+      <c r="AA27" t="n">
+        <v>5910</v>
+      </c>
+      <c r="AB27" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC27" t="inlineStr">
+        <is>
+          <t>6467</t>
         </is>
       </c>
     </row>
@@ -2978,9 +3144,15 @@
       <c r="Z28" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="AA28" t="inlineStr">
-        <is>
-          <t>5153</t>
+      <c r="AA28" t="n">
+        <v>5153</v>
+      </c>
+      <c r="AB28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="AC28" t="inlineStr">
+        <is>
+          <t>5613</t>
         </is>
       </c>
     </row>
@@ -3069,9 +3241,15 @@
       <c r="Z29" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AA29" t="inlineStr">
-        <is>
-          <t>6591</t>
+      <c r="AA29" t="n">
+        <v>6591</v>
+      </c>
+      <c r="AB29" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC29" t="inlineStr">
+        <is>
+          <t>6737</t>
         </is>
       </c>
     </row>
@@ -3160,9 +3338,15 @@
       <c r="Z30" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AA30" t="inlineStr">
-        <is>
-          <t>5164</t>
+      <c r="AA30" t="n">
+        <v>5164</v>
+      </c>
+      <c r="AB30" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC30" t="inlineStr">
+        <is>
+          <t>5484</t>
         </is>
       </c>
     </row>
@@ -3251,9 +3435,15 @@
       <c r="Z31" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AA31" t="inlineStr">
-        <is>
-          <t>6080</t>
+      <c r="AA31" t="n">
+        <v>6080</v>
+      </c>
+      <c r="AB31" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AC31" t="inlineStr">
+        <is>
+          <t>6243</t>
         </is>
       </c>
     </row>
@@ -3342,9 +3532,15 @@
       <c r="Z32" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AA32" t="inlineStr">
-        <is>
-          <t>5074</t>
+      <c r="AA32" t="n">
+        <v>5074</v>
+      </c>
+      <c r="AB32" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC32" t="inlineStr">
+        <is>
+          <t>5242</t>
         </is>
       </c>
     </row>
@@ -3433,9 +3629,15 @@
       <c r="Z33" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AA33" t="inlineStr">
-        <is>
-          <t>5478</t>
+      <c r="AA33" t="n">
+        <v>5478</v>
+      </c>
+      <c r="AB33" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC33" t="inlineStr">
+        <is>
+          <t>5664</t>
         </is>
       </c>
     </row>
@@ -3524,9 +3726,15 @@
       <c r="Z34" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA34" t="inlineStr">
-        <is>
-          <t>5439</t>
+      <c r="AA34" t="n">
+        <v>5439</v>
+      </c>
+      <c r="AB34" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC34" t="inlineStr">
+        <is>
+          <t>5746</t>
         </is>
       </c>
     </row>
@@ -3615,9 +3823,15 @@
       <c r="Z35" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="AA35" t="inlineStr">
-        <is>
-          <t>5715</t>
+      <c r="AA35" t="n">
+        <v>5715</v>
+      </c>
+      <c r="AB35" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC35" t="inlineStr">
+        <is>
+          <t>5989</t>
         </is>
       </c>
     </row>
@@ -3706,9 +3920,15 @@
       <c r="Z36" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA36" t="inlineStr">
-        <is>
-          <t>5425</t>
+      <c r="AA36" t="n">
+        <v>5425</v>
+      </c>
+      <c r="AB36" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC36" t="inlineStr">
+        <is>
+          <t>5582</t>
         </is>
       </c>
     </row>
@@ -3797,9 +4017,15 @@
       <c r="Z37" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AA37" t="inlineStr">
-        <is>
-          <t>4509</t>
+      <c r="AA37" t="n">
+        <v>4509</v>
+      </c>
+      <c r="AB37" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC37" t="inlineStr">
+        <is>
+          <t>4516</t>
         </is>
       </c>
     </row>
@@ -3888,9 +4114,15 @@
       <c r="Z38" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA38" t="inlineStr">
-        <is>
-          <t>5359</t>
+      <c r="AA38" t="n">
+        <v>5359</v>
+      </c>
+      <c r="AB38" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AC38" t="inlineStr">
+        <is>
+          <t>5611</t>
         </is>
       </c>
     </row>
@@ -3979,9 +4211,15 @@
       <c r="Z39" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AA39" t="inlineStr">
-        <is>
-          <t>5502</t>
+      <c r="AA39" t="n">
+        <v>5502</v>
+      </c>
+      <c r="AB39" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AC39" t="inlineStr">
+        <is>
+          <t>6008</t>
         </is>
       </c>
     </row>
@@ -4070,9 +4308,15 @@
       <c r="Z40" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AA40" t="inlineStr">
-        <is>
-          <t>6225</t>
+      <c r="AA40" t="n">
+        <v>6225</v>
+      </c>
+      <c r="AB40" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC40" t="inlineStr">
+        <is>
+          <t>6487</t>
         </is>
       </c>
     </row>
@@ -4161,7 +4405,13 @@
       <c r="Z41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA41" t="inlineStr">
+      <c r="AA41" t="n">
+        <v>3648</v>
+      </c>
+      <c r="AB41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC41" t="inlineStr">
         <is>
           <t>3648</t>
         </is>
@@ -4252,9 +4502,15 @@
       <c r="Z42" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AA42" t="inlineStr">
-        <is>
-          <t>6253</t>
+      <c r="AA42" t="n">
+        <v>6253</v>
+      </c>
+      <c r="AB42" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AC42" t="inlineStr">
+        <is>
+          <t>6633</t>
         </is>
       </c>
     </row>
@@ -4343,9 +4599,15 @@
       <c r="Z43" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AA43" t="inlineStr">
-        <is>
-          <t>5718</t>
+      <c r="AA43" t="n">
+        <v>5718</v>
+      </c>
+      <c r="AB43" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC43" t="inlineStr">
+        <is>
+          <t>5902</t>
         </is>
       </c>
     </row>
@@ -4434,9 +4696,15 @@
       <c r="Z44" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AA44" t="inlineStr">
-        <is>
-          <t>5670</t>
+      <c r="AA44" t="n">
+        <v>5670</v>
+      </c>
+      <c r="AB44" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC44" t="inlineStr">
+        <is>
+          <t>5993</t>
         </is>
       </c>
     </row>
@@ -4525,9 +4793,15 @@
       <c r="Z45" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AA45" t="inlineStr">
-        <is>
-          <t>4892</t>
+      <c r="AA45" t="n">
+        <v>4892</v>
+      </c>
+      <c r="AB45" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC45" t="inlineStr">
+        <is>
+          <t>5233</t>
         </is>
       </c>
     </row>
@@ -4616,9 +4890,15 @@
       <c r="Z46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA46" t="inlineStr">
-        <is>
-          <t>5108</t>
+      <c r="AA46" t="n">
+        <v>5108</v>
+      </c>
+      <c r="AB46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC46" t="inlineStr">
+        <is>
+          <t>5621</t>
         </is>
       </c>
     </row>
@@ -4707,7 +4987,13 @@
       <c r="Z47" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA47" t="inlineStr">
+      <c r="AA47" t="n">
+        <v>3199</v>
+      </c>
+      <c r="AB47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC47" t="inlineStr">
         <is>
           <t>3199</t>
         </is>
@@ -4798,9 +5084,15 @@
       <c r="Z48" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="AA48" t="inlineStr">
-        <is>
-          <t>5864</t>
+      <c r="AA48" t="n">
+        <v>5864</v>
+      </c>
+      <c r="AB48" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AC48" t="inlineStr">
+        <is>
+          <t>6167</t>
         </is>
       </c>
     </row>
@@ -4889,9 +5181,15 @@
       <c r="Z49" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="AA49" t="inlineStr">
-        <is>
-          <t>4486</t>
+      <c r="AA49" t="n">
+        <v>4486</v>
+      </c>
+      <c r="AB49" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AC49" t="inlineStr">
+        <is>
+          <t>4742</t>
         </is>
       </c>
     </row>
@@ -4980,9 +5278,15 @@
       <c r="Z50" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AA50" t="inlineStr">
-        <is>
-          <t>6273</t>
+      <c r="AA50" t="n">
+        <v>6273</v>
+      </c>
+      <c r="AB50" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC50" t="inlineStr">
+        <is>
+          <t>6413</t>
         </is>
       </c>
     </row>
@@ -5071,9 +5375,15 @@
       <c r="Z51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA51" t="inlineStr">
-        <is>
-          <t>2885</t>
+      <c r="AA51" t="n">
+        <v>2885</v>
+      </c>
+      <c r="AB51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC51" t="inlineStr">
+        <is>
+          <t>2893</t>
         </is>
       </c>
     </row>
@@ -5162,9 +5472,15 @@
       <c r="Z52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA52" t="inlineStr">
-        <is>
-          <t>2860</t>
+      <c r="AA52" t="n">
+        <v>2860</v>
+      </c>
+      <c r="AB52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC52" t="inlineStr">
+        <is>
+          <t>2907</t>
         </is>
       </c>
     </row>
@@ -5253,9 +5569,15 @@
       <c r="Z53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA53" t="inlineStr">
-        <is>
-          <t>2858</t>
+      <c r="AA53" t="n">
+        <v>2858</v>
+      </c>
+      <c r="AB53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC53" t="inlineStr">
+        <is>
+          <t>2908</t>
         </is>
       </c>
     </row>
@@ -5344,9 +5666,15 @@
       <c r="Z54" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AA54" t="inlineStr">
-        <is>
-          <t>5528</t>
+      <c r="AA54" t="n">
+        <v>5528</v>
+      </c>
+      <c r="AB54" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC54" t="inlineStr">
+        <is>
+          <t>5734</t>
         </is>
       </c>
     </row>
@@ -5435,9 +5763,15 @@
       <c r="Z55" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AA55" t="inlineStr">
-        <is>
-          <t>4209</t>
+      <c r="AA55" t="n">
+        <v>4209</v>
+      </c>
+      <c r="AB55" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC55" t="inlineStr">
+        <is>
+          <t>4434</t>
         </is>
       </c>
     </row>
@@ -5526,9 +5860,15 @@
       <c r="Z56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA56" t="inlineStr">
-        <is>
-          <t>4414</t>
+      <c r="AA56" t="n">
+        <v>4414</v>
+      </c>
+      <c r="AB56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC56" t="inlineStr">
+        <is>
+          <t>4549</t>
         </is>
       </c>
     </row>
@@ -5617,9 +5957,15 @@
       <c r="Z57" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AA57" t="inlineStr">
-        <is>
-          <t>5236</t>
+      <c r="AA57" t="n">
+        <v>5236</v>
+      </c>
+      <c r="AB57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC57" t="inlineStr">
+        <is>
+          <t>5378</t>
         </is>
       </c>
     </row>
@@ -5708,9 +6054,15 @@
       <c r="Z58" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AA58" t="inlineStr">
-        <is>
-          <t>4381</t>
+      <c r="AA58" t="n">
+        <v>4381</v>
+      </c>
+      <c r="AB58" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC58" t="inlineStr">
+        <is>
+          <t>4600</t>
         </is>
       </c>
     </row>
@@ -5754,6 +6106,8 @@
       <c r="Y59" t="inlineStr"/>
       <c r="Z59" s="3" t="inlineStr"/>
       <c r="AA59" t="inlineStr"/>
+      <c r="AB59" s="3" t="inlineStr"/>
+      <c r="AC59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -5795,6 +6149,8 @@
       <c r="Y60" t="inlineStr"/>
       <c r="Z60" s="3" t="inlineStr"/>
       <c r="AA60" t="inlineStr"/>
+      <c r="AB60" s="3" t="inlineStr"/>
+      <c r="AC60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -5881,9 +6237,15 @@
       <c r="Z61" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA61" t="inlineStr">
-        <is>
-          <t>4896</t>
+      <c r="AA61" t="n">
+        <v>4896</v>
+      </c>
+      <c r="AB61" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC61" t="inlineStr">
+        <is>
+          <t>5180</t>
         </is>
       </c>
     </row>
@@ -5972,7 +6334,13 @@
       <c r="Z62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA62" t="inlineStr">
+      <c r="AA62" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6063,9 +6431,15 @@
       <c r="Z63" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AA63" t="inlineStr">
-        <is>
-          <t>5196</t>
+      <c r="AA63" t="n">
+        <v>5196</v>
+      </c>
+      <c r="AB63" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AC63" t="inlineStr">
+        <is>
+          <t>5353</t>
         </is>
       </c>
     </row>
@@ -6154,7 +6528,13 @@
       <c r="Z64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA64" t="inlineStr">
+      <c r="AA64" t="n">
+        <v>3088</v>
+      </c>
+      <c r="AB64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC64" t="inlineStr">
         <is>
           <t>3088</t>
         </is>
@@ -6200,6 +6580,8 @@
       <c r="Y65" t="inlineStr"/>
       <c r="Z65" s="3" t="inlineStr"/>
       <c r="AA65" t="inlineStr"/>
+      <c r="AB65" s="3" t="inlineStr"/>
+      <c r="AC65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -6286,9 +6668,15 @@
       <c r="Z66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA66" t="inlineStr">
-        <is>
-          <t>2635</t>
+      <c r="AA66" t="n">
+        <v>2635</v>
+      </c>
+      <c r="AB66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC66" t="inlineStr">
+        <is>
+          <t>2632</t>
         </is>
       </c>
     </row>
@@ -6377,9 +6765,15 @@
       <c r="Z67" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AA67" t="inlineStr">
-        <is>
-          <t>4840</t>
+      <c r="AA67" t="n">
+        <v>4840</v>
+      </c>
+      <c r="AB67" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC67" t="inlineStr">
+        <is>
+          <t>4986</t>
         </is>
       </c>
     </row>
@@ -6468,9 +6862,15 @@
       <c r="Z68" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AA68" t="inlineStr">
-        <is>
-          <t>5645</t>
+      <c r="AA68" t="n">
+        <v>5645</v>
+      </c>
+      <c r="AB68" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC68" t="inlineStr">
+        <is>
+          <t>5878</t>
         </is>
       </c>
     </row>
@@ -6559,9 +6959,15 @@
       <c r="Z69" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AA69" t="inlineStr">
-        <is>
-          <t>4306</t>
+      <c r="AA69" t="n">
+        <v>4306</v>
+      </c>
+      <c r="AB69" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AC69" t="inlineStr">
+        <is>
+          <t>4378</t>
         </is>
       </c>
     </row>
@@ -6650,9 +7056,15 @@
       <c r="Z70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA70" t="inlineStr">
-        <is>
-          <t>3041</t>
+      <c r="AA70" t="n">
+        <v>3041</v>
+      </c>
+      <c r="AB70" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC70" t="inlineStr">
+        <is>
+          <t>3537</t>
         </is>
       </c>
     </row>
@@ -6741,9 +7153,15 @@
       <c r="Z71" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA71" t="inlineStr">
-        <is>
-          <t>4364</t>
+      <c r="AA71" t="n">
+        <v>4364</v>
+      </c>
+      <c r="AB71" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC71" t="inlineStr">
+        <is>
+          <t>4768</t>
         </is>
       </c>
     </row>
@@ -6832,9 +7250,15 @@
       <c r="Z72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA72" t="inlineStr">
-        <is>
-          <t>3515</t>
+      <c r="AA72" t="n">
+        <v>3515</v>
+      </c>
+      <c r="AB72" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="AC72" t="inlineStr">
+        <is>
+          <t>3745</t>
         </is>
       </c>
     </row>
@@ -6923,9 +7347,15 @@
       <c r="Z73" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA73" t="inlineStr">
-        <is>
-          <t>4354</t>
+      <c r="AA73" t="n">
+        <v>4354</v>
+      </c>
+      <c r="AB73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC73" t="inlineStr">
+        <is>
+          <t>4397</t>
         </is>
       </c>
     </row>
@@ -7014,9 +7444,15 @@
       <c r="Z74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA74" t="inlineStr">
-        <is>
-          <t>3226</t>
+      <c r="AA74" t="n">
+        <v>3226</v>
+      </c>
+      <c r="AB74" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC74" t="inlineStr">
+        <is>
+          <t>3637</t>
         </is>
       </c>
     </row>
@@ -7105,9 +7541,15 @@
       <c r="Z75" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AA75" t="inlineStr">
-        <is>
-          <t>4037</t>
+      <c r="AA75" t="n">
+        <v>4037</v>
+      </c>
+      <c r="AB75" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AC75" t="inlineStr">
+        <is>
+          <t>4219</t>
         </is>
       </c>
     </row>
@@ -7196,9 +7638,15 @@
       <c r="Z76" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA76" t="inlineStr">
-        <is>
-          <t>4994</t>
+      <c r="AA76" t="n">
+        <v>4994</v>
+      </c>
+      <c r="AB76" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC76" t="inlineStr">
+        <is>
+          <t>5205</t>
         </is>
       </c>
     </row>
@@ -7287,7 +7735,13 @@
       <c r="Z77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA77" t="inlineStr">
+      <c r="AA77" t="n">
+        <v>3383</v>
+      </c>
+      <c r="AB77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC77" t="inlineStr">
         <is>
           <t>3383</t>
         </is>
@@ -7378,9 +7832,15 @@
       <c r="Z78" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA78" t="inlineStr">
-        <is>
-          <t>5020</t>
+      <c r="AA78" t="n">
+        <v>5020</v>
+      </c>
+      <c r="AB78" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC78" t="inlineStr">
+        <is>
+          <t>5192</t>
         </is>
       </c>
     </row>
@@ -7469,7 +7929,13 @@
       <c r="Z79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA79" t="inlineStr">
+      <c r="AA79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7560,9 +8026,15 @@
       <c r="Z80" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="AA80" t="inlineStr">
-        <is>
-          <t>4883</t>
+      <c r="AA80" t="n">
+        <v>4883</v>
+      </c>
+      <c r="AB80" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="AC80" t="inlineStr">
+        <is>
+          <t>5084</t>
         </is>
       </c>
     </row>
@@ -7651,9 +8123,15 @@
       <c r="Z81" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AA81" t="inlineStr">
-        <is>
-          <t>4945</t>
+      <c r="AA81" t="n">
+        <v>4945</v>
+      </c>
+      <c r="AB81" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC81" t="inlineStr">
+        <is>
+          <t>4983</t>
         </is>
       </c>
     </row>
@@ -7742,9 +8220,15 @@
       <c r="Z82" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA82" t="inlineStr">
-        <is>
-          <t>4605</t>
+      <c r="AA82" t="n">
+        <v>4605</v>
+      </c>
+      <c r="AB82" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC82" t="inlineStr">
+        <is>
+          <t>4837</t>
         </is>
       </c>
     </row>
@@ -7833,9 +8317,15 @@
       <c r="Z83" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="AA83" t="inlineStr">
-        <is>
-          <t>4470</t>
+      <c r="AA83" t="n">
+        <v>4470</v>
+      </c>
+      <c r="AB83" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AC83" t="inlineStr">
+        <is>
+          <t>4593</t>
         </is>
       </c>
     </row>
@@ -7924,9 +8414,15 @@
       <c r="Z84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA84" t="inlineStr">
-        <is>
-          <t>2945</t>
+      <c r="AA84" t="n">
+        <v>2945</v>
+      </c>
+      <c r="AB84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC84" t="inlineStr">
+        <is>
+          <t>2956</t>
         </is>
       </c>
     </row>
@@ -8015,9 +8511,15 @@
       <c r="Z85" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AA85" t="inlineStr">
-        <is>
-          <t>3657</t>
+      <c r="AA85" t="n">
+        <v>3657</v>
+      </c>
+      <c r="AB85" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC85" t="inlineStr">
+        <is>
+          <t>3779</t>
         </is>
       </c>
     </row>
@@ -8106,9 +8608,15 @@
       <c r="Z86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA86" t="inlineStr">
-        <is>
-          <t>3199</t>
+      <c r="AA86" t="n">
+        <v>3199</v>
+      </c>
+      <c r="AB86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC86" t="inlineStr">
+        <is>
+          <t>3247</t>
         </is>
       </c>
     </row>
@@ -8197,9 +8705,15 @@
       <c r="Z87" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AA87" t="inlineStr">
-        <is>
-          <t>4754</t>
+      <c r="AA87" t="n">
+        <v>4754</v>
+      </c>
+      <c r="AB87" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC87" t="inlineStr">
+        <is>
+          <t>4811</t>
         </is>
       </c>
     </row>
@@ -8288,9 +8802,15 @@
       <c r="Z88" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA88" t="inlineStr">
-        <is>
-          <t>2994</t>
+      <c r="AA88" t="n">
+        <v>2994</v>
+      </c>
+      <c r="AB88" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC88" t="inlineStr">
+        <is>
+          <t>2973</t>
         </is>
       </c>
     </row>
@@ -8379,9 +8899,15 @@
       <c r="Z89" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA89" t="inlineStr">
-        <is>
-          <t>3275</t>
+      <c r="AA89" t="n">
+        <v>3275</v>
+      </c>
+      <c r="AB89" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC89" t="inlineStr">
+        <is>
+          <t>3305</t>
         </is>
       </c>
     </row>
@@ -8470,9 +8996,15 @@
       <c r="Z90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA90" t="inlineStr">
-        <is>
-          <t>2688</t>
+      <c r="AA90" t="n">
+        <v>2688</v>
+      </c>
+      <c r="AB90" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC90" t="inlineStr">
+        <is>
+          <t>2683</t>
         </is>
       </c>
     </row>
@@ -8561,9 +9093,15 @@
       <c r="Z91" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA91" t="inlineStr">
-        <is>
-          <t>2864</t>
+      <c r="AA91" t="n">
+        <v>2864</v>
+      </c>
+      <c r="AB91" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC91" t="inlineStr">
+        <is>
+          <t>2891</t>
         </is>
       </c>
     </row>
@@ -8652,7 +9190,13 @@
       <c r="Z92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA92" t="inlineStr">
+      <c r="AA92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8743,9 +9287,15 @@
       <c r="Z93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA93" t="inlineStr">
-        <is>
-          <t>2625</t>
+      <c r="AA93" t="n">
+        <v>2625</v>
+      </c>
+      <c r="AB93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC93" t="inlineStr">
+        <is>
+          <t>2609</t>
         </is>
       </c>
     </row>
@@ -8834,9 +9384,15 @@
       <c r="Z94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA94" t="inlineStr">
-        <is>
-          <t>3258</t>
+      <c r="AA94" t="n">
+        <v>3258</v>
+      </c>
+      <c r="AB94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC94" t="inlineStr">
+        <is>
+          <t>3286</t>
         </is>
       </c>
     </row>
@@ -8925,9 +9481,15 @@
       <c r="Z95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA95" t="inlineStr">
-        <is>
-          <t>2525</t>
+      <c r="AA95" t="n">
+        <v>2525</v>
+      </c>
+      <c r="AB95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC95" t="inlineStr">
+        <is>
+          <t>2504</t>
         </is>
       </c>
     </row>
@@ -9016,9 +9578,15 @@
       <c r="Z96" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="AA96" t="inlineStr">
-        <is>
-          <t>3733</t>
+      <c r="AA96" t="n">
+        <v>3733</v>
+      </c>
+      <c r="AB96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC96" t="inlineStr">
+        <is>
+          <t>3704</t>
         </is>
       </c>
     </row>
@@ -9107,9 +9675,15 @@
       <c r="Z97" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AA97" t="inlineStr">
-        <is>
-          <t>3082</t>
+      <c r="AA97" t="n">
+        <v>3082</v>
+      </c>
+      <c r="AB97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC97" t="inlineStr">
+        <is>
+          <t>3081</t>
         </is>
       </c>
     </row>
@@ -9198,7 +9772,13 @@
       <c r="Z98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA98" t="inlineStr">
+      <c r="AA98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9289,9 +9869,15 @@
       <c r="Z99" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA99" t="inlineStr">
-        <is>
-          <t>3889</t>
+      <c r="AA99" t="n">
+        <v>3889</v>
+      </c>
+      <c r="AB99" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="AC99" t="inlineStr">
+        <is>
+          <t>3967</t>
         </is>
       </c>
     </row>
@@ -9380,9 +9966,15 @@
       <c r="Z100" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="AA100" t="inlineStr">
-        <is>
-          <t>2805</t>
+      <c r="AA100" t="n">
+        <v>2805</v>
+      </c>
+      <c r="AB100" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC100" t="inlineStr">
+        <is>
+          <t>2806</t>
         </is>
       </c>
     </row>
@@ -9471,9 +10063,15 @@
       <c r="Z101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA101" t="inlineStr">
-        <is>
-          <t>4334</t>
+      <c r="AA101" t="n">
+        <v>4334</v>
+      </c>
+      <c r="AB101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC101" t="inlineStr">
+        <is>
+          <t>4558</t>
         </is>
       </c>
     </row>
@@ -9562,9 +10160,15 @@
       <c r="Z102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA102" t="inlineStr">
-        <is>
-          <t>3930</t>
+      <c r="AA102" t="n">
+        <v>3930</v>
+      </c>
+      <c r="AB102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC102" t="inlineStr">
+        <is>
+          <t>4000</t>
         </is>
       </c>
     </row>
@@ -9653,9 +10257,15 @@
       <c r="Z103" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA103" t="inlineStr">
-        <is>
-          <t>2936</t>
+      <c r="AA103" t="n">
+        <v>2936</v>
+      </c>
+      <c r="AB103" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC103" t="inlineStr">
+        <is>
+          <t>3257</t>
         </is>
       </c>
     </row>
@@ -9744,9 +10354,15 @@
       <c r="Z104" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA104" t="inlineStr">
-        <is>
-          <t>4454</t>
+      <c r="AA104" t="n">
+        <v>4454</v>
+      </c>
+      <c r="AB104" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC104" t="inlineStr">
+        <is>
+          <t>4587</t>
         </is>
       </c>
     </row>
@@ -9835,9 +10451,15 @@
       <c r="Z105" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AA105" t="inlineStr">
-        <is>
-          <t>4238</t>
+      <c r="AA105" t="n">
+        <v>4238</v>
+      </c>
+      <c r="AB105" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC105" t="inlineStr">
+        <is>
+          <t>4155</t>
         </is>
       </c>
     </row>
@@ -9926,7 +10548,13 @@
       <c r="Z106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA106" t="inlineStr">
+      <c r="AA106" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10017,9 +10645,15 @@
       <c r="Z107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA107" t="inlineStr">
-        <is>
-          <t>2498</t>
+      <c r="AA107" t="n">
+        <v>2498</v>
+      </c>
+      <c r="AB107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC107" t="inlineStr">
+        <is>
+          <t>2515</t>
         </is>
       </c>
     </row>
@@ -10108,7 +10742,13 @@
       <c r="Z108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA108" t="inlineStr">
+      <c r="AA108" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10199,9 +10839,15 @@
       <c r="Z109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA109" t="inlineStr">
-        <is>
-          <t>3819</t>
+      <c r="AA109" t="n">
+        <v>3819</v>
+      </c>
+      <c r="AB109" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC109" t="inlineStr">
+        <is>
+          <t>3850</t>
         </is>
       </c>
     </row>
@@ -10290,9 +10936,15 @@
       <c r="Z110" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="AA110" t="inlineStr">
-        <is>
-          <t>3679</t>
+      <c r="AA110" t="n">
+        <v>3679</v>
+      </c>
+      <c r="AB110" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AC110" t="inlineStr">
+        <is>
+          <t>3722</t>
         </is>
       </c>
     </row>
@@ -10381,9 +11033,15 @@
       <c r="Z111" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AA111" t="inlineStr">
-        <is>
-          <t>2658</t>
+      <c r="AA111" t="n">
+        <v>2658</v>
+      </c>
+      <c r="AB111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC111" t="inlineStr">
+        <is>
+          <t>2655</t>
         </is>
       </c>
     </row>
@@ -10472,9 +11130,15 @@
       <c r="Z112" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA112" t="inlineStr">
-        <is>
-          <t>3286</t>
+      <c r="AA112" t="n">
+        <v>3286</v>
+      </c>
+      <c r="AB112" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="AC112" t="inlineStr">
+        <is>
+          <t>3452</t>
         </is>
       </c>
     </row>
@@ -10563,9 +11227,15 @@
       <c r="Z113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA113" t="inlineStr">
-        <is>
-          <t>3476</t>
+      <c r="AA113" t="n">
+        <v>3476</v>
+      </c>
+      <c r="AB113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC113" t="inlineStr">
+        <is>
+          <t>3588</t>
         </is>
       </c>
     </row>
@@ -10654,9 +11324,15 @@
       <c r="Z114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA114" t="inlineStr">
-        <is>
-          <t>3052</t>
+      <c r="AA114" t="n">
+        <v>3052</v>
+      </c>
+      <c r="AB114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC114" t="inlineStr">
+        <is>
+          <t>3124</t>
         </is>
       </c>
     </row>
@@ -10745,9 +11421,15 @@
       <c r="Z115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA115" t="inlineStr">
-        <is>
-          <t>2318</t>
+      <c r="AA115" t="n">
+        <v>2318</v>
+      </c>
+      <c r="AB115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC115" t="inlineStr">
+        <is>
+          <t>2316</t>
         </is>
       </c>
     </row>
@@ -10836,9 +11518,15 @@
       <c r="Z116" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AA116" t="inlineStr">
-        <is>
-          <t>3292</t>
+      <c r="AA116" t="n">
+        <v>3292</v>
+      </c>
+      <c r="AB116" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC116" t="inlineStr">
+        <is>
+          <t>3339</t>
         </is>
       </c>
     </row>
@@ -10927,9 +11615,15 @@
       <c r="Z117" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA117" t="inlineStr">
-        <is>
-          <t>3690</t>
+      <c r="AA117" t="n">
+        <v>3690</v>
+      </c>
+      <c r="AB117" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC117" t="inlineStr">
+        <is>
+          <t>3771</t>
         </is>
       </c>
     </row>
@@ -11018,7 +11712,13 @@
       <c r="Z118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA118" t="inlineStr">
+      <c r="AA118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11109,9 +11809,15 @@
       <c r="Z119" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AA119" t="inlineStr">
-        <is>
-          <t>4024</t>
+      <c r="AA119" t="n">
+        <v>4024</v>
+      </c>
+      <c r="AB119" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AC119" t="inlineStr">
+        <is>
+          <t>4068</t>
         </is>
       </c>
     </row>
@@ -11200,9 +11906,15 @@
       <c r="Z120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA120" t="inlineStr">
-        <is>
-          <t>2577</t>
+      <c r="AA120" t="n">
+        <v>2577</v>
+      </c>
+      <c r="AB120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC120" t="inlineStr">
+        <is>
+          <t>2567</t>
         </is>
       </c>
     </row>
@@ -11291,9 +12003,15 @@
       <c r="Z121" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="AA121" t="inlineStr">
-        <is>
-          <t>3531</t>
+      <c r="AA121" t="n">
+        <v>3531</v>
+      </c>
+      <c r="AB121" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC121" t="inlineStr">
+        <is>
+          <t>3665</t>
         </is>
       </c>
     </row>
@@ -11382,7 +12100,13 @@
       <c r="Z122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA122" t="inlineStr">
+      <c r="AA122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11473,9 +12197,15 @@
       <c r="Z123" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="AA123" t="inlineStr">
-        <is>
-          <t>3283</t>
+      <c r="AA123" t="n">
+        <v>3283</v>
+      </c>
+      <c r="AB123" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="AC123" t="inlineStr">
+        <is>
+          <t>3303</t>
         </is>
       </c>
     </row>
@@ -11564,9 +12294,15 @@
       <c r="Z124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA124" t="inlineStr">
-        <is>
-          <t>3342</t>
+      <c r="AA124" t="n">
+        <v>3342</v>
+      </c>
+      <c r="AB124" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="AC124" t="inlineStr">
+        <is>
+          <t>3364</t>
         </is>
       </c>
     </row>
@@ -11655,9 +12391,15 @@
       <c r="Z125" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA125" t="inlineStr">
-        <is>
-          <t>3665</t>
+      <c r="AA125" t="n">
+        <v>3665</v>
+      </c>
+      <c r="AB125" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC125" t="inlineStr">
+        <is>
+          <t>3807</t>
         </is>
       </c>
     </row>
@@ -11746,9 +12488,15 @@
       <c r="Z126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA126" t="inlineStr">
-        <is>
-          <t>3239</t>
+      <c r="AA126" t="n">
+        <v>3239</v>
+      </c>
+      <c r="AB126" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC126" t="inlineStr">
+        <is>
+          <t>3340</t>
         </is>
       </c>
     </row>
@@ -11837,9 +12585,15 @@
       <c r="Z127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA127" t="inlineStr">
-        <is>
-          <t>2361</t>
+      <c r="AA127" t="n">
+        <v>2361</v>
+      </c>
+      <c r="AB127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC127" t="inlineStr">
+        <is>
+          <t>2350</t>
         </is>
       </c>
     </row>
@@ -11928,7 +12682,13 @@
       <c r="Z128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA128" t="inlineStr">
+      <c r="AA128" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12019,7 +12779,13 @@
       <c r="Z129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA129" t="inlineStr">
+      <c r="AA129" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12110,9 +12876,15 @@
       <c r="Z130" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA130" t="inlineStr">
-        <is>
-          <t>2999</t>
+      <c r="AA130" t="n">
+        <v>2999</v>
+      </c>
+      <c r="AB130" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AC130" t="inlineStr">
+        <is>
+          <t>2968</t>
         </is>
       </c>
     </row>
@@ -12201,9 +12973,15 @@
       <c r="Z131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA131" t="inlineStr">
-        <is>
-          <t>2556</t>
+      <c r="AA131" t="n">
+        <v>2556</v>
+      </c>
+      <c r="AB131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC131" t="inlineStr">
+        <is>
+          <t>2567</t>
         </is>
       </c>
     </row>
@@ -12292,9 +13070,15 @@
       <c r="Z132" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA132" t="inlineStr">
-        <is>
-          <t>2716</t>
+      <c r="AA132" t="n">
+        <v>2716</v>
+      </c>
+      <c r="AB132" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC132" t="inlineStr">
+        <is>
+          <t>2729</t>
         </is>
       </c>
     </row>
@@ -12383,9 +13167,15 @@
       <c r="Z133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA133" t="inlineStr">
-        <is>
-          <t>2866</t>
+      <c r="AA133" t="n">
+        <v>2866</v>
+      </c>
+      <c r="AB133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC133" t="inlineStr">
+        <is>
+          <t>2900</t>
         </is>
       </c>
     </row>
@@ -12453,6 +13243,8 @@
       <c r="Y134" t="inlineStr"/>
       <c r="Z134" s="3" t="inlineStr"/>
       <c r="AA134" t="inlineStr"/>
+      <c r="AB134" s="3" t="inlineStr"/>
+      <c r="AC134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -12510,6 +13302,8 @@
       <c r="Y135" t="inlineStr"/>
       <c r="Z135" s="3" t="inlineStr"/>
       <c r="AA135" t="inlineStr"/>
+      <c r="AB135" s="3" t="inlineStr"/>
+      <c r="AC135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -12596,9 +13390,15 @@
       <c r="Z136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA136" t="inlineStr">
-        <is>
-          <t>2699</t>
+      <c r="AA136" t="n">
+        <v>2699</v>
+      </c>
+      <c r="AB136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC136" t="inlineStr">
+        <is>
+          <t>2692</t>
         </is>
       </c>
     </row>
@@ -12687,9 +13487,15 @@
       <c r="Z137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA137" t="inlineStr">
-        <is>
-          <t>2531</t>
+      <c r="AA137" t="n">
+        <v>2531</v>
+      </c>
+      <c r="AB137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC137" t="inlineStr">
+        <is>
+          <t>2556</t>
         </is>
       </c>
     </row>
@@ -12749,6 +13555,8 @@
       <c r="Y138" t="inlineStr"/>
       <c r="Z138" s="3" t="inlineStr"/>
       <c r="AA138" t="inlineStr"/>
+      <c r="AB138" s="3" t="inlineStr"/>
+      <c r="AC138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -12835,9 +13643,15 @@
       <c r="Z139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA139" t="inlineStr">
-        <is>
-          <t>2410</t>
+      <c r="AA139" t="n">
+        <v>2410</v>
+      </c>
+      <c r="AB139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC139" t="inlineStr">
+        <is>
+          <t>2404</t>
         </is>
       </c>
     </row>
@@ -12926,9 +13740,15 @@
       <c r="Z140" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="AA140" t="inlineStr">
-        <is>
-          <t>3018</t>
+      <c r="AA140" t="n">
+        <v>3018</v>
+      </c>
+      <c r="AB140" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC140" t="inlineStr">
+        <is>
+          <t>3030</t>
         </is>
       </c>
     </row>
@@ -12988,6 +13808,8 @@
       <c r="Y141" t="inlineStr"/>
       <c r="Z141" s="3" t="inlineStr"/>
       <c r="AA141" t="inlineStr"/>
+      <c r="AB141" s="3" t="inlineStr"/>
+      <c r="AC141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -13074,9 +13896,15 @@
       <c r="Z142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA142" t="inlineStr">
-        <is>
-          <t>2189</t>
+      <c r="AA142" t="n">
+        <v>2189</v>
+      </c>
+      <c r="AB142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC142" t="inlineStr">
+        <is>
+          <t>2227</t>
         </is>
       </c>
     </row>
@@ -13136,6 +13964,8 @@
       <c r="Y143" t="inlineStr"/>
       <c r="Z143" s="3" t="inlineStr"/>
       <c r="AA143" t="inlineStr"/>
+      <c r="AB143" s="3" t="inlineStr"/>
+      <c r="AC143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -13193,6 +14023,8 @@
       <c r="Y144" t="inlineStr"/>
       <c r="Z144" s="3" t="inlineStr"/>
       <c r="AA144" t="inlineStr"/>
+      <c r="AB144" s="3" t="inlineStr"/>
+      <c r="AC144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -13250,6 +14082,8 @@
       <c r="Y145" t="inlineStr"/>
       <c r="Z145" s="3" t="inlineStr"/>
       <c r="AA145" t="inlineStr"/>
+      <c r="AB145" s="3" t="inlineStr"/>
+      <c r="AC145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -13307,6 +14141,8 @@
       <c r="Y146" t="inlineStr"/>
       <c r="Z146" s="3" t="inlineStr"/>
       <c r="AA146" t="inlineStr"/>
+      <c r="AB146" s="3" t="inlineStr"/>
+      <c r="AC146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -13364,6 +14200,8 @@
       <c r="Y147" t="inlineStr"/>
       <c r="Z147" s="3" t="inlineStr"/>
       <c r="AA147" t="inlineStr"/>
+      <c r="AB147" s="3" t="inlineStr"/>
+      <c r="AC147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -13450,9 +14288,15 @@
       <c r="Z148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA148" t="inlineStr">
-        <is>
-          <t>1506</t>
+      <c r="AA148" t="n">
+        <v>1506</v>
+      </c>
+      <c r="AB148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC148" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -13541,7 +14385,13 @@
       <c r="Z149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA149" t="inlineStr">
+      <c r="AA149" t="n">
+        <v>3849</v>
+      </c>
+      <c r="AB149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC149" t="inlineStr">
         <is>
           <t>3849</t>
         </is>
@@ -13632,7 +14482,13 @@
       <c r="Z150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA150" t="inlineStr">
+      <c r="AA150" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13723,7 +14579,13 @@
       <c r="Z151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA151" t="inlineStr">
+      <c r="AA151" t="n">
+        <v>2511</v>
+      </c>
+      <c r="AB151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC151" t="inlineStr">
         <is>
           <t>2511</t>
         </is>
@@ -13814,7 +14676,13 @@
       <c r="Z152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA152" t="inlineStr">
+      <c r="AA152" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13905,7 +14773,13 @@
       <c r="Z153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA153" t="inlineStr">
+      <c r="AA153" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13996,7 +14870,13 @@
       <c r="Z154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA154" t="inlineStr">
+      <c r="AA154" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14087,9 +14967,15 @@
       <c r="Z155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA155" t="inlineStr">
-        <is>
-          <t>2747</t>
+      <c r="AA155" t="n">
+        <v>2747</v>
+      </c>
+      <c r="AB155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC155" t="inlineStr">
+        <is>
+          <t>2797</t>
         </is>
       </c>
     </row>
@@ -14172,9 +15058,15 @@
       <c r="Z156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA156" t="inlineStr">
-        <is>
-          <t>3458</t>
+      <c r="AA156" t="n">
+        <v>3458</v>
+      </c>
+      <c r="AB156" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="AC156" t="inlineStr">
+        <is>
+          <t>3577</t>
         </is>
       </c>
     </row>
@@ -14228,6 +15120,8 @@
       <c r="Y157" t="inlineStr"/>
       <c r="Z157" s="3" t="inlineStr"/>
       <c r="AA157" t="inlineStr"/>
+      <c r="AB157" s="3" t="inlineStr"/>
+      <c r="AC157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -14308,7 +15202,13 @@
       <c r="Z158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA158" t="inlineStr">
+      <c r="AA158" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14393,9 +15293,15 @@
       <c r="Z159" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA159" t="inlineStr">
-        <is>
-          <t>3010</t>
+      <c r="AA159" t="n">
+        <v>3010</v>
+      </c>
+      <c r="AB159" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC159" t="inlineStr">
+        <is>
+          <t>2999</t>
         </is>
       </c>
     </row>
@@ -14449,6 +15355,8 @@
       <c r="Y160" t="inlineStr"/>
       <c r="Z160" s="3" t="inlineStr"/>
       <c r="AA160" t="inlineStr"/>
+      <c r="AB160" s="3" t="inlineStr"/>
+      <c r="AC160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -14517,9 +15425,15 @@
       <c r="Z161" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AA161" t="inlineStr">
-        <is>
-          <t>3001</t>
+      <c r="AA161" t="n">
+        <v>3001</v>
+      </c>
+      <c r="AB161" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC161" t="inlineStr">
+        <is>
+          <t>3055</t>
         </is>
       </c>
     </row>
@@ -14590,9 +15504,15 @@
       <c r="Z162" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="AA162" t="inlineStr">
-        <is>
-          <t>2633</t>
+      <c r="AA162" t="n">
+        <v>2633</v>
+      </c>
+      <c r="AB162" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC162" t="inlineStr">
+        <is>
+          <t>2672</t>
         </is>
       </c>
     </row>
@@ -14659,9 +15579,15 @@
       <c r="Z163" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA163" t="inlineStr">
-        <is>
-          <t>3218</t>
+      <c r="AA163" t="n">
+        <v>3218</v>
+      </c>
+      <c r="AB163" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC163" t="inlineStr">
+        <is>
+          <t>3213</t>
         </is>
       </c>
     </row>
@@ -14716,9 +15642,15 @@
       <c r="Z164" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="AA164" t="inlineStr">
-        <is>
-          <t>3592</t>
+      <c r="AA164" t="n">
+        <v>3592</v>
+      </c>
+      <c r="AB164" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC164" t="inlineStr">
+        <is>
+          <t>3557</t>
         </is>
       </c>
     </row>
@@ -14773,9 +15705,15 @@
       <c r="Z165" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AA165" t="inlineStr">
-        <is>
-          <t>2783</t>
+      <c r="AA165" t="n">
+        <v>2783</v>
+      </c>
+      <c r="AB165" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="AC165" t="inlineStr">
+        <is>
+          <t>2853</t>
         </is>
       </c>
     </row>
@@ -14822,9 +15760,15 @@
       <c r="Z166" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA166" t="inlineStr">
-        <is>
-          <t>2565</t>
+      <c r="AA166" t="n">
+        <v>2565</v>
+      </c>
+      <c r="AB166" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC166" t="inlineStr">
+        <is>
+          <t>2561</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-02-25 11:19:53
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC166"/>
+  <dimension ref="A1:AE167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,6 +536,16 @@
           <t>02-23_0</t>
         </is>
       </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>02-24_A</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>02-24_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -628,9 +638,15 @@
       <c r="AB2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t>3926</t>
+      <c r="AC2" t="n">
+        <v>3926</v>
+      </c>
+      <c r="AD2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>3995</t>
         </is>
       </c>
     </row>
@@ -725,9 +741,15 @@
       <c r="AB3" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>6141</t>
+      <c r="AC3" t="n">
+        <v>6141</v>
+      </c>
+      <c r="AD3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>6488</t>
         </is>
       </c>
     </row>
@@ -822,9 +844,15 @@
       <c r="AB4" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AC4" t="inlineStr">
-        <is>
-          <t>6313</t>
+      <c r="AC4" t="n">
+        <v>6313</v>
+      </c>
+      <c r="AD4" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>6513</t>
         </is>
       </c>
     </row>
@@ -919,9 +947,15 @@
       <c r="AB5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC5" t="inlineStr">
-        <is>
-          <t>5653</t>
+      <c r="AC5" t="n">
+        <v>5653</v>
+      </c>
+      <c r="AD5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t>6013</t>
         </is>
       </c>
     </row>
@@ -1016,9 +1050,15 @@
       <c r="AB6" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AC6" t="inlineStr">
-        <is>
-          <t>5856</t>
+      <c r="AC6" t="n">
+        <v>5856</v>
+      </c>
+      <c r="AD6" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t>6115</t>
         </is>
       </c>
     </row>
@@ -1113,9 +1153,15 @@
       <c r="AB7" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AC7" t="inlineStr">
-        <is>
-          <t>6669</t>
+      <c r="AC7" t="n">
+        <v>6669</v>
+      </c>
+      <c r="AD7" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AE7" t="inlineStr">
+        <is>
+          <t>6772</t>
         </is>
       </c>
     </row>
@@ -1210,9 +1256,15 @@
       <c r="AB8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC8" t="inlineStr">
-        <is>
-          <t>5165</t>
+      <c r="AC8" t="n">
+        <v>5165</v>
+      </c>
+      <c r="AD8" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AE8" t="inlineStr">
+        <is>
+          <t>5310</t>
         </is>
       </c>
     </row>
@@ -1307,9 +1359,15 @@
       <c r="AB9" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AC9" t="inlineStr">
-        <is>
-          <t>5337</t>
+      <c r="AC9" t="n">
+        <v>5337</v>
+      </c>
+      <c r="AD9" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AE9" t="inlineStr">
+        <is>
+          <t>5810</t>
         </is>
       </c>
     </row>
@@ -1404,9 +1462,15 @@
       <c r="AB10" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AC10" t="inlineStr">
-        <is>
-          <t>6591</t>
+      <c r="AC10" t="n">
+        <v>6591</v>
+      </c>
+      <c r="AD10" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AE10" t="inlineStr">
+        <is>
+          <t>6944</t>
         </is>
       </c>
     </row>
@@ -1501,9 +1565,15 @@
       <c r="AB11" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC11" t="inlineStr">
-        <is>
-          <t>5569</t>
+      <c r="AC11" t="n">
+        <v>5569</v>
+      </c>
+      <c r="AD11" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="AE11" t="inlineStr">
+        <is>
+          <t>5566</t>
         </is>
       </c>
     </row>
@@ -1598,7 +1668,13 @@
       <c r="AB12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC12" t="inlineStr">
+      <c r="AC12" t="n">
+        <v>2914</v>
+      </c>
+      <c r="AD12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE12" t="inlineStr">
         <is>
           <t>2914</t>
         </is>
@@ -1695,9 +1771,15 @@
       <c r="AB13" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AC13" t="inlineStr">
-        <is>
-          <t>6493</t>
+      <c r="AC13" t="n">
+        <v>6493</v>
+      </c>
+      <c r="AD13" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE13" t="inlineStr">
+        <is>
+          <t>6804</t>
         </is>
       </c>
     </row>
@@ -1792,9 +1874,15 @@
       <c r="AB14" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="AC14" t="inlineStr">
-        <is>
-          <t>5680</t>
+      <c r="AC14" t="n">
+        <v>5680</v>
+      </c>
+      <c r="AD14" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AE14" t="inlineStr">
+        <is>
+          <t>5938</t>
         </is>
       </c>
     </row>
@@ -1889,9 +1977,15 @@
       <c r="AB15" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AC15" t="inlineStr">
-        <is>
-          <t>5430</t>
+      <c r="AC15" t="n">
+        <v>5430</v>
+      </c>
+      <c r="AD15" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AE15" t="inlineStr">
+        <is>
+          <t>5697</t>
         </is>
       </c>
     </row>
@@ -1986,9 +2080,15 @@
       <c r="AB16" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AC16" t="inlineStr">
-        <is>
-          <t>6002</t>
+      <c r="AC16" t="n">
+        <v>6002</v>
+      </c>
+      <c r="AD16" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE16" t="inlineStr">
+        <is>
+          <t>6360</t>
         </is>
       </c>
     </row>
@@ -2083,9 +2183,15 @@
       <c r="AB17" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC17" t="inlineStr">
-        <is>
-          <t>4463</t>
+      <c r="AC17" t="n">
+        <v>4463</v>
+      </c>
+      <c r="AD17" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AE17" t="inlineStr">
+        <is>
+          <t>4707</t>
         </is>
       </c>
     </row>
@@ -2180,9 +2286,15 @@
       <c r="AB18" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AC18" t="inlineStr">
-        <is>
-          <t>4594</t>
+      <c r="AC18" t="n">
+        <v>4594</v>
+      </c>
+      <c r="AD18" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AE18" t="inlineStr">
+        <is>
+          <t>4827</t>
         </is>
       </c>
     </row>
@@ -2277,9 +2389,15 @@
       <c r="AB19" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC19" t="inlineStr">
-        <is>
-          <t>5786</t>
+      <c r="AC19" t="n">
+        <v>5786</v>
+      </c>
+      <c r="AD19" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AE19" t="inlineStr">
+        <is>
+          <t>6005</t>
         </is>
       </c>
     </row>
@@ -2374,9 +2492,15 @@
       <c r="AB20" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AC20" t="inlineStr">
-        <is>
-          <t>6836</t>
+      <c r="AC20" t="n">
+        <v>6836</v>
+      </c>
+      <c r="AD20" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="AE20" t="inlineStr">
+        <is>
+          <t>7128</t>
         </is>
       </c>
     </row>
@@ -2471,9 +2595,15 @@
       <c r="AB21" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AC21" t="inlineStr">
-        <is>
-          <t>5361</t>
+      <c r="AC21" t="n">
+        <v>5361</v>
+      </c>
+      <c r="AD21" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AE21" t="inlineStr">
+        <is>
+          <t>5710</t>
         </is>
       </c>
     </row>
@@ -2568,9 +2698,15 @@
       <c r="AB22" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AC22" t="inlineStr">
-        <is>
-          <t>5376</t>
+      <c r="AC22" t="n">
+        <v>5376</v>
+      </c>
+      <c r="AD22" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AE22" t="inlineStr">
+        <is>
+          <t>5648</t>
         </is>
       </c>
     </row>
@@ -2665,9 +2801,15 @@
       <c r="AB23" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AC23" t="inlineStr">
-        <is>
-          <t>5600</t>
+      <c r="AC23" t="n">
+        <v>5600</v>
+      </c>
+      <c r="AD23" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE23" t="inlineStr">
+        <is>
+          <t>5632</t>
         </is>
       </c>
     </row>
@@ -2762,9 +2904,15 @@
       <c r="AB24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AC24" t="inlineStr">
-        <is>
-          <t>6110</t>
+      <c r="AC24" t="n">
+        <v>6110</v>
+      </c>
+      <c r="AD24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AE24" t="inlineStr">
+        <is>
+          <t>6443</t>
         </is>
       </c>
     </row>
@@ -2859,7 +3007,13 @@
       <c r="AB25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC25" t="inlineStr">
+      <c r="AC25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2956,9 +3110,15 @@
       <c r="AB26" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AC26" t="inlineStr">
-        <is>
-          <t>5947</t>
+      <c r="AC26" t="n">
+        <v>5947</v>
+      </c>
+      <c r="AD26" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="AE26" t="inlineStr">
+        <is>
+          <t>6090</t>
         </is>
       </c>
     </row>
@@ -3053,9 +3213,15 @@
       <c r="AB27" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AC27" t="inlineStr">
-        <is>
-          <t>6467</t>
+      <c r="AC27" t="n">
+        <v>6467</v>
+      </c>
+      <c r="AD27" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AE27" t="inlineStr">
+        <is>
+          <t>6928</t>
         </is>
       </c>
     </row>
@@ -3150,9 +3316,15 @@
       <c r="AB28" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="AC28" t="inlineStr">
-        <is>
-          <t>5613</t>
+      <c r="AC28" t="n">
+        <v>5613</v>
+      </c>
+      <c r="AD28" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AE28" t="inlineStr">
+        <is>
+          <t>6040</t>
         </is>
       </c>
     </row>
@@ -3247,9 +3419,15 @@
       <c r="AB29" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AC29" t="inlineStr">
-        <is>
-          <t>6737</t>
+      <c r="AC29" t="n">
+        <v>6737</v>
+      </c>
+      <c r="AD29" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AE29" t="inlineStr">
+        <is>
+          <t>6924</t>
         </is>
       </c>
     </row>
@@ -3344,9 +3522,15 @@
       <c r="AB30" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AC30" t="inlineStr">
-        <is>
-          <t>5484</t>
+      <c r="AC30" t="n">
+        <v>5484</v>
+      </c>
+      <c r="AD30" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="AE30" t="inlineStr">
+        <is>
+          <t>5703</t>
         </is>
       </c>
     </row>
@@ -3441,9 +3625,15 @@
       <c r="AB31" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AC31" t="inlineStr">
-        <is>
-          <t>6243</t>
+      <c r="AC31" t="n">
+        <v>6243</v>
+      </c>
+      <c r="AD31" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AE31" t="inlineStr">
+        <is>
+          <t>6744</t>
         </is>
       </c>
     </row>
@@ -3538,9 +3728,15 @@
       <c r="AB32" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AC32" t="inlineStr">
-        <is>
-          <t>5242</t>
+      <c r="AC32" t="n">
+        <v>5242</v>
+      </c>
+      <c r="AD32" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AE32" t="inlineStr">
+        <is>
+          <t>6061</t>
         </is>
       </c>
     </row>
@@ -3635,9 +3831,15 @@
       <c r="AB33" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AC33" t="inlineStr">
-        <is>
-          <t>5664</t>
+      <c r="AC33" t="n">
+        <v>5664</v>
+      </c>
+      <c r="AD33" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AE33" t="inlineStr">
+        <is>
+          <t>6019</t>
         </is>
       </c>
     </row>
@@ -3732,9 +3934,15 @@
       <c r="AB34" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AC34" t="inlineStr">
-        <is>
-          <t>5746</t>
+      <c r="AC34" t="n">
+        <v>5746</v>
+      </c>
+      <c r="AD34" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE34" t="inlineStr">
+        <is>
+          <t>5961</t>
         </is>
       </c>
     </row>
@@ -3829,9 +4037,15 @@
       <c r="AB35" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AC35" t="inlineStr">
-        <is>
-          <t>5989</t>
+      <c r="AC35" t="n">
+        <v>5989</v>
+      </c>
+      <c r="AD35" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AE35" t="inlineStr">
+        <is>
+          <t>6340</t>
         </is>
       </c>
     </row>
@@ -3926,9 +4140,15 @@
       <c r="AB36" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AC36" t="inlineStr">
-        <is>
-          <t>5582</t>
+      <c r="AC36" t="n">
+        <v>5582</v>
+      </c>
+      <c r="AD36" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AE36" t="inlineStr">
+        <is>
+          <t>5779</t>
         </is>
       </c>
     </row>
@@ -4023,9 +4243,15 @@
       <c r="AB37" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="AC37" t="inlineStr">
-        <is>
-          <t>4516</t>
+      <c r="AC37" t="n">
+        <v>4516</v>
+      </c>
+      <c r="AD37" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AE37" t="inlineStr">
+        <is>
+          <t>4623</t>
         </is>
       </c>
     </row>
@@ -4120,9 +4346,15 @@
       <c r="AB38" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AC38" t="inlineStr">
-        <is>
-          <t>5611</t>
+      <c r="AC38" t="n">
+        <v>5611</v>
+      </c>
+      <c r="AD38" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AE38" t="inlineStr">
+        <is>
+          <t>5990</t>
         </is>
       </c>
     </row>
@@ -4217,9 +4449,15 @@
       <c r="AB39" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AC39" t="inlineStr">
-        <is>
-          <t>6008</t>
+      <c r="AC39" t="n">
+        <v>6008</v>
+      </c>
+      <c r="AD39" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AE39" t="inlineStr">
+        <is>
+          <t>6069</t>
         </is>
       </c>
     </row>
@@ -4314,9 +4552,15 @@
       <c r="AB40" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AC40" t="inlineStr">
-        <is>
-          <t>6487</t>
+      <c r="AC40" t="n">
+        <v>6487</v>
+      </c>
+      <c r="AD40" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AE40" t="inlineStr">
+        <is>
+          <t>6888</t>
         </is>
       </c>
     </row>
@@ -4411,7 +4655,13 @@
       <c r="AB41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC41" t="inlineStr">
+      <c r="AC41" t="n">
+        <v>3648</v>
+      </c>
+      <c r="AD41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE41" t="inlineStr">
         <is>
           <t>3648</t>
         </is>
@@ -4508,9 +4758,15 @@
       <c r="AB42" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AC42" t="inlineStr">
-        <is>
-          <t>6633</t>
+      <c r="AC42" t="n">
+        <v>6633</v>
+      </c>
+      <c r="AD42" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AE42" t="inlineStr">
+        <is>
+          <t>7008</t>
         </is>
       </c>
     </row>
@@ -4605,9 +4861,15 @@
       <c r="AB43" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AC43" t="inlineStr">
-        <is>
-          <t>5902</t>
+      <c r="AC43" t="n">
+        <v>5902</v>
+      </c>
+      <c r="AD43" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AE43" t="inlineStr">
+        <is>
+          <t>6246</t>
         </is>
       </c>
     </row>
@@ -4702,9 +4964,15 @@
       <c r="AB44" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AC44" t="inlineStr">
-        <is>
-          <t>5993</t>
+      <c r="AC44" t="n">
+        <v>5993</v>
+      </c>
+      <c r="AD44" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AE44" t="inlineStr">
+        <is>
+          <t>6225</t>
         </is>
       </c>
     </row>
@@ -4799,9 +5067,15 @@
       <c r="AB45" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AC45" t="inlineStr">
-        <is>
-          <t>5233</t>
+      <c r="AC45" t="n">
+        <v>5233</v>
+      </c>
+      <c r="AD45" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="AE45" t="inlineStr">
+        <is>
+          <t>5610</t>
         </is>
       </c>
     </row>
@@ -4896,9 +5170,15 @@
       <c r="AB46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AC46" t="inlineStr">
-        <is>
-          <t>5621</t>
+      <c r="AC46" t="n">
+        <v>5621</v>
+      </c>
+      <c r="AD46" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AE46" t="inlineStr">
+        <is>
+          <t>5917</t>
         </is>
       </c>
     </row>
@@ -4993,9 +5273,15 @@
       <c r="AB47" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC47" t="inlineStr">
-        <is>
-          <t>3199</t>
+      <c r="AC47" t="n">
+        <v>3199</v>
+      </c>
+      <c r="AD47" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE47" t="inlineStr">
+        <is>
+          <t>3526</t>
         </is>
       </c>
     </row>
@@ -5090,9 +5376,15 @@
       <c r="AB48" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AC48" t="inlineStr">
-        <is>
-          <t>6167</t>
+      <c r="AC48" t="n">
+        <v>6167</v>
+      </c>
+      <c r="AD48" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="AE48" t="inlineStr">
+        <is>
+          <t>6450</t>
         </is>
       </c>
     </row>
@@ -5187,9 +5479,15 @@
       <c r="AB49" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AC49" t="inlineStr">
-        <is>
-          <t>4742</t>
+      <c r="AC49" t="n">
+        <v>4742</v>
+      </c>
+      <c r="AD49" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AE49" t="inlineStr">
+        <is>
+          <t>5060</t>
         </is>
       </c>
     </row>
@@ -5284,9 +5582,15 @@
       <c r="AB50" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AC50" t="inlineStr">
-        <is>
-          <t>6413</t>
+      <c r="AC50" t="n">
+        <v>6413</v>
+      </c>
+      <c r="AD50" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AE50" t="inlineStr">
+        <is>
+          <t>6842</t>
         </is>
       </c>
     </row>
@@ -5381,9 +5685,15 @@
       <c r="AB51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC51" t="inlineStr">
-        <is>
-          <t>2893</t>
+      <c r="AC51" t="n">
+        <v>2893</v>
+      </c>
+      <c r="AD51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE51" t="inlineStr">
+        <is>
+          <t>2924</t>
         </is>
       </c>
     </row>
@@ -5478,7 +5788,13 @@
       <c r="AB52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC52" t="inlineStr">
+      <c r="AC52" t="n">
+        <v>2907</v>
+      </c>
+      <c r="AD52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE52" t="inlineStr">
         <is>
           <t>2907</t>
         </is>
@@ -5575,9 +5891,15 @@
       <c r="AB53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC53" t="inlineStr">
-        <is>
-          <t>2908</t>
+      <c r="AC53" t="n">
+        <v>2908</v>
+      </c>
+      <c r="AD53" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AE53" t="inlineStr">
+        <is>
+          <t>3074</t>
         </is>
       </c>
     </row>
@@ -5672,9 +5994,15 @@
       <c r="AB54" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AC54" t="inlineStr">
-        <is>
-          <t>5734</t>
+      <c r="AC54" t="n">
+        <v>5734</v>
+      </c>
+      <c r="AD54" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE54" t="inlineStr">
+        <is>
+          <t>5930</t>
         </is>
       </c>
     </row>
@@ -5769,9 +6097,15 @@
       <c r="AB55" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AC55" t="inlineStr">
-        <is>
-          <t>4434</t>
+      <c r="AC55" t="n">
+        <v>4434</v>
+      </c>
+      <c r="AD55" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AE55" t="inlineStr">
+        <is>
+          <t>4601</t>
         </is>
       </c>
     </row>
@@ -5866,9 +6200,15 @@
       <c r="AB56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC56" t="inlineStr">
-        <is>
-          <t>4549</t>
+      <c r="AC56" t="n">
+        <v>4549</v>
+      </c>
+      <c r="AD56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE56" t="inlineStr">
+        <is>
+          <t>4640</t>
         </is>
       </c>
     </row>
@@ -5963,9 +6303,15 @@
       <c r="AB57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC57" t="inlineStr">
-        <is>
-          <t>5378</t>
+      <c r="AC57" t="n">
+        <v>5378</v>
+      </c>
+      <c r="AD57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE57" t="inlineStr">
+        <is>
+          <t>5551</t>
         </is>
       </c>
     </row>
@@ -6060,9 +6406,15 @@
       <c r="AB58" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AC58" t="inlineStr">
-        <is>
-          <t>4600</t>
+      <c r="AC58" t="n">
+        <v>4600</v>
+      </c>
+      <c r="AD58" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AE58" t="inlineStr">
+        <is>
+          <t>4762</t>
         </is>
       </c>
     </row>
@@ -6108,6 +6460,8 @@
       <c r="AA59" t="inlineStr"/>
       <c r="AB59" s="3" t="inlineStr"/>
       <c r="AC59" t="inlineStr"/>
+      <c r="AD59" s="3" t="inlineStr"/>
+      <c r="AE59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -6151,6 +6505,8 @@
       <c r="AA60" t="inlineStr"/>
       <c r="AB60" s="3" t="inlineStr"/>
       <c r="AC60" t="inlineStr"/>
+      <c r="AD60" s="3" t="inlineStr"/>
+      <c r="AE60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -6243,9 +6599,15 @@
       <c r="AB61" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AC61" t="inlineStr">
-        <is>
-          <t>5180</t>
+      <c r="AC61" t="n">
+        <v>5180</v>
+      </c>
+      <c r="AD61" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE61" t="inlineStr">
+        <is>
+          <t>5267</t>
         </is>
       </c>
     </row>
@@ -6340,7 +6702,13 @@
       <c r="AB62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC62" t="inlineStr">
+      <c r="AC62" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6437,9 +6805,15 @@
       <c r="AB63" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AC63" t="inlineStr">
-        <is>
-          <t>5353</t>
+      <c r="AC63" t="n">
+        <v>5353</v>
+      </c>
+      <c r="AD63" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AE63" t="inlineStr">
+        <is>
+          <t>5570</t>
         </is>
       </c>
     </row>
@@ -6534,9 +6908,15 @@
       <c r="AB64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC64" t="inlineStr">
-        <is>
-          <t>3088</t>
+      <c r="AC64" t="n">
+        <v>3088</v>
+      </c>
+      <c r="AD64" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="AE64" t="inlineStr">
+        <is>
+          <t>3258</t>
         </is>
       </c>
     </row>
@@ -6582,6 +6962,8 @@
       <c r="AA65" t="inlineStr"/>
       <c r="AB65" s="3" t="inlineStr"/>
       <c r="AC65" t="inlineStr"/>
+      <c r="AD65" s="3" t="inlineStr"/>
+      <c r="AE65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -6674,9 +7056,15 @@
       <c r="AB66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC66" t="inlineStr">
-        <is>
-          <t>2632</t>
+      <c r="AC66" t="n">
+        <v>2632</v>
+      </c>
+      <c r="AD66" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AE66" t="inlineStr">
+        <is>
+          <t>2704</t>
         </is>
       </c>
     </row>
@@ -6771,9 +7159,15 @@
       <c r="AB67" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AC67" t="inlineStr">
-        <is>
-          <t>4986</t>
+      <c r="AC67" t="n">
+        <v>4986</v>
+      </c>
+      <c r="AD67" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AE67" t="inlineStr">
+        <is>
+          <t>5202</t>
         </is>
       </c>
     </row>
@@ -6868,9 +7262,15 @@
       <c r="AB68" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AC68" t="inlineStr">
-        <is>
-          <t>5878</t>
+      <c r="AC68" t="n">
+        <v>5878</v>
+      </c>
+      <c r="AD68" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="AE68" t="inlineStr">
+        <is>
+          <t>6187</t>
         </is>
       </c>
     </row>
@@ -6965,9 +7365,15 @@
       <c r="AB69" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AC69" t="inlineStr">
-        <is>
-          <t>4378</t>
+      <c r="AC69" t="n">
+        <v>4378</v>
+      </c>
+      <c r="AD69" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AE69" t="inlineStr">
+        <is>
+          <t>4523</t>
         </is>
       </c>
     </row>
@@ -7062,9 +7468,15 @@
       <c r="AB70" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC70" t="inlineStr">
-        <is>
-          <t>3537</t>
+      <c r="AC70" t="n">
+        <v>3537</v>
+      </c>
+      <c r="AD70" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="AE70" t="inlineStr">
+        <is>
+          <t>4208</t>
         </is>
       </c>
     </row>
@@ -7159,9 +7571,15 @@
       <c r="AB71" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AC71" t="inlineStr">
-        <is>
-          <t>4768</t>
+      <c r="AC71" t="n">
+        <v>4768</v>
+      </c>
+      <c r="AD71" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="AE71" t="inlineStr">
+        <is>
+          <t>5094</t>
         </is>
       </c>
     </row>
@@ -7256,9 +7674,15 @@
       <c r="AB72" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="AC72" t="inlineStr">
-        <is>
-          <t>3745</t>
+      <c r="AC72" t="n">
+        <v>3745</v>
+      </c>
+      <c r="AD72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE72" t="inlineStr">
+        <is>
+          <t>3832</t>
         </is>
       </c>
     </row>
@@ -7353,9 +7777,15 @@
       <c r="AB73" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC73" t="inlineStr">
-        <is>
-          <t>4397</t>
+      <c r="AC73" t="n">
+        <v>4397</v>
+      </c>
+      <c r="AD73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE73" t="inlineStr">
+        <is>
+          <t>4520</t>
         </is>
       </c>
     </row>
@@ -7450,9 +7880,15 @@
       <c r="AB74" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC74" t="inlineStr">
-        <is>
-          <t>3637</t>
+      <c r="AC74" t="n">
+        <v>3637</v>
+      </c>
+      <c r="AD74" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="AE74" t="inlineStr">
+        <is>
+          <t>4229</t>
         </is>
       </c>
     </row>
@@ -7547,9 +7983,15 @@
       <c r="AB75" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="AC75" t="inlineStr">
-        <is>
-          <t>4219</t>
+      <c r="AC75" t="n">
+        <v>4219</v>
+      </c>
+      <c r="AD75" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE75" t="inlineStr">
+        <is>
+          <t>4384</t>
         </is>
       </c>
     </row>
@@ -7644,9 +8086,15 @@
       <c r="AB76" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AC76" t="inlineStr">
-        <is>
-          <t>5205</t>
+      <c r="AC76" t="n">
+        <v>5205</v>
+      </c>
+      <c r="AD76" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE76" t="inlineStr">
+        <is>
+          <t>5333</t>
         </is>
       </c>
     </row>
@@ -7741,7 +8189,13 @@
       <c r="AB77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC77" t="inlineStr">
+      <c r="AC77" t="n">
+        <v>3383</v>
+      </c>
+      <c r="AD77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE77" t="inlineStr">
         <is>
           <t>3383</t>
         </is>
@@ -7838,9 +8292,15 @@
       <c r="AB78" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AC78" t="inlineStr">
-        <is>
-          <t>5192</t>
+      <c r="AC78" t="n">
+        <v>5192</v>
+      </c>
+      <c r="AD78" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE78" t="inlineStr">
+        <is>
+          <t>5301</t>
         </is>
       </c>
     </row>
@@ -7935,7 +8395,13 @@
       <c r="AB79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC79" t="inlineStr">
+      <c r="AC79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8032,9 +8498,15 @@
       <c r="AB80" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="AC80" t="inlineStr">
-        <is>
-          <t>5084</t>
+      <c r="AC80" t="n">
+        <v>5084</v>
+      </c>
+      <c r="AD80" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AE80" t="inlineStr">
+        <is>
+          <t>5142</t>
         </is>
       </c>
     </row>
@@ -8129,9 +8601,15 @@
       <c r="AB81" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AC81" t="inlineStr">
-        <is>
-          <t>4983</t>
+      <c r="AC81" t="n">
+        <v>4983</v>
+      </c>
+      <c r="AD81" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AE81" t="inlineStr">
+        <is>
+          <t>5115</t>
         </is>
       </c>
     </row>
@@ -8226,9 +8704,15 @@
       <c r="AB82" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AC82" t="inlineStr">
-        <is>
-          <t>4837</t>
+      <c r="AC82" t="n">
+        <v>4837</v>
+      </c>
+      <c r="AD82" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE82" t="inlineStr">
+        <is>
+          <t>4945</t>
         </is>
       </c>
     </row>
@@ -8323,9 +8807,15 @@
       <c r="AB83" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="AC83" t="inlineStr">
-        <is>
-          <t>4593</t>
+      <c r="AC83" t="n">
+        <v>4593</v>
+      </c>
+      <c r="AD83" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AE83" t="inlineStr">
+        <is>
+          <t>4680</t>
         </is>
       </c>
     </row>
@@ -8420,9 +8910,15 @@
       <c r="AB84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC84" t="inlineStr">
-        <is>
-          <t>2956</t>
+      <c r="AC84" t="n">
+        <v>2956</v>
+      </c>
+      <c r="AD84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE84" t="inlineStr">
+        <is>
+          <t>2968</t>
         </is>
       </c>
     </row>
@@ -8517,9 +9013,15 @@
       <c r="AB85" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="AC85" t="inlineStr">
-        <is>
-          <t>3779</t>
+      <c r="AC85" t="n">
+        <v>3779</v>
+      </c>
+      <c r="AD85" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE85" t="inlineStr">
+        <is>
+          <t>3949</t>
         </is>
       </c>
     </row>
@@ -8614,9 +9116,15 @@
       <c r="AB86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC86" t="inlineStr">
-        <is>
-          <t>3247</t>
+      <c r="AC86" t="n">
+        <v>3247</v>
+      </c>
+      <c r="AD86" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE86" t="inlineStr">
+        <is>
+          <t>3550</t>
         </is>
       </c>
     </row>
@@ -8711,9 +9219,15 @@
       <c r="AB87" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AC87" t="inlineStr">
-        <is>
-          <t>4811</t>
+      <c r="AC87" t="n">
+        <v>4811</v>
+      </c>
+      <c r="AD87" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AE87" t="inlineStr">
+        <is>
+          <t>4962</t>
         </is>
       </c>
     </row>
@@ -8808,9 +9322,15 @@
       <c r="AB88" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC88" t="inlineStr">
-        <is>
-          <t>2973</t>
+      <c r="AC88" t="n">
+        <v>2973</v>
+      </c>
+      <c r="AD88" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE88" t="inlineStr">
+        <is>
+          <t>3048</t>
         </is>
       </c>
     </row>
@@ -8905,9 +9425,15 @@
       <c r="AB89" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC89" t="inlineStr">
-        <is>
-          <t>3305</t>
+      <c r="AC89" t="n">
+        <v>3305</v>
+      </c>
+      <c r="AD89" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE89" t="inlineStr">
+        <is>
+          <t>3453</t>
         </is>
       </c>
     </row>
@@ -9002,9 +9528,15 @@
       <c r="AB90" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="AC90" t="inlineStr">
-        <is>
-          <t>2683</t>
+      <c r="AC90" t="n">
+        <v>2683</v>
+      </c>
+      <c r="AD90" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE90" t="inlineStr">
+        <is>
+          <t>2815</t>
         </is>
       </c>
     </row>
@@ -9099,9 +9631,15 @@
       <c r="AB91" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC91" t="inlineStr">
-        <is>
-          <t>2891</t>
+      <c r="AC91" t="n">
+        <v>2891</v>
+      </c>
+      <c r="AD91" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE91" t="inlineStr">
+        <is>
+          <t>2943</t>
         </is>
       </c>
     </row>
@@ -9196,7 +9734,13 @@
       <c r="AB92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC92" t="inlineStr">
+      <c r="AC92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9293,9 +9837,15 @@
       <c r="AB93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC93" t="inlineStr">
-        <is>
-          <t>2609</t>
+      <c r="AC93" t="n">
+        <v>2609</v>
+      </c>
+      <c r="AD93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE93" t="inlineStr">
+        <is>
+          <t>2586</t>
         </is>
       </c>
     </row>
@@ -9390,9 +9940,15 @@
       <c r="AB94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC94" t="inlineStr">
-        <is>
-          <t>3286</t>
+      <c r="AC94" t="n">
+        <v>3286</v>
+      </c>
+      <c r="AD94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE94" t="inlineStr">
+        <is>
+          <t>3265</t>
         </is>
       </c>
     </row>
@@ -9487,9 +10043,15 @@
       <c r="AB95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC95" t="inlineStr">
-        <is>
-          <t>2504</t>
+      <c r="AC95" t="n">
+        <v>2504</v>
+      </c>
+      <c r="AD95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE95" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -9584,9 +10146,15 @@
       <c r="AB96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC96" t="inlineStr">
-        <is>
-          <t>3704</t>
+      <c r="AC96" t="n">
+        <v>3704</v>
+      </c>
+      <c r="AD96" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="AE96" t="inlineStr">
+        <is>
+          <t>3877</t>
         </is>
       </c>
     </row>
@@ -9681,9 +10249,15 @@
       <c r="AB97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC97" t="inlineStr">
-        <is>
-          <t>3081</t>
+      <c r="AC97" t="n">
+        <v>3081</v>
+      </c>
+      <c r="AD97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE97" t="inlineStr">
+        <is>
+          <t>3111</t>
         </is>
       </c>
     </row>
@@ -9778,7 +10352,13 @@
       <c r="AB98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC98" t="inlineStr">
+      <c r="AC98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9875,9 +10455,15 @@
       <c r="AB99" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="AC99" t="inlineStr">
-        <is>
-          <t>3967</t>
+      <c r="AC99" t="n">
+        <v>3967</v>
+      </c>
+      <c r="AD99" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AE99" t="inlineStr">
+        <is>
+          <t>4130</t>
         </is>
       </c>
     </row>
@@ -9972,9 +10558,15 @@
       <c r="AB100" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="AC100" t="inlineStr">
-        <is>
-          <t>2806</t>
+      <c r="AC100" t="n">
+        <v>2806</v>
+      </c>
+      <c r="AD100" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE100" t="inlineStr">
+        <is>
+          <t>2781</t>
         </is>
       </c>
     </row>
@@ -10069,9 +10661,15 @@
       <c r="AB101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AC101" t="inlineStr">
-        <is>
-          <t>4558</t>
+      <c r="AC101" t="n">
+        <v>4558</v>
+      </c>
+      <c r="AD101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE101" t="inlineStr">
+        <is>
+          <t>4725</t>
         </is>
       </c>
     </row>
@@ -10166,9 +10764,15 @@
       <c r="AB102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC102" t="inlineStr">
-        <is>
-          <t>4000</t>
+      <c r="AC102" t="n">
+        <v>4000</v>
+      </c>
+      <c r="AD102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE102" t="inlineStr">
+        <is>
+          <t>4155</t>
         </is>
       </c>
     </row>
@@ -10263,9 +10867,15 @@
       <c r="AB103" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC103" t="inlineStr">
-        <is>
-          <t>3257</t>
+      <c r="AC103" t="n">
+        <v>3257</v>
+      </c>
+      <c r="AD103" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE103" t="inlineStr">
+        <is>
+          <t>3596</t>
         </is>
       </c>
     </row>
@@ -10360,9 +10970,15 @@
       <c r="AB104" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AC104" t="inlineStr">
-        <is>
-          <t>4587</t>
+      <c r="AC104" t="n">
+        <v>4587</v>
+      </c>
+      <c r="AD104" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AE104" t="inlineStr">
+        <is>
+          <t>4721</t>
         </is>
       </c>
     </row>
@@ -10457,9 +11073,15 @@
       <c r="AB105" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="AC105" t="inlineStr">
-        <is>
-          <t>4155</t>
+      <c r="AC105" t="n">
+        <v>4155</v>
+      </c>
+      <c r="AD105" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AE105" t="inlineStr">
+        <is>
+          <t>4347</t>
         </is>
       </c>
     </row>
@@ -10554,7 +11176,13 @@
       <c r="AB106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC106" t="inlineStr">
+      <c r="AC106" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10651,9 +11279,15 @@
       <c r="AB107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC107" t="inlineStr">
-        <is>
-          <t>2515</t>
+      <c r="AC107" t="n">
+        <v>2515</v>
+      </c>
+      <c r="AD107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE107" t="inlineStr">
+        <is>
+          <t>2529</t>
         </is>
       </c>
     </row>
@@ -10748,7 +11382,13 @@
       <c r="AB108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC108" t="inlineStr">
+      <c r="AC108" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10845,9 +11485,15 @@
       <c r="AB109" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="AC109" t="inlineStr">
-        <is>
-          <t>3850</t>
+      <c r="AC109" t="n">
+        <v>3850</v>
+      </c>
+      <c r="AD109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE109" t="inlineStr">
+        <is>
+          <t>3916</t>
         </is>
       </c>
     </row>
@@ -10942,9 +11588,15 @@
       <c r="AB110" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="AC110" t="inlineStr">
-        <is>
-          <t>3722</t>
+      <c r="AC110" t="n">
+        <v>3722</v>
+      </c>
+      <c r="AD110" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE110" t="inlineStr">
+        <is>
+          <t>3765</t>
         </is>
       </c>
     </row>
@@ -11039,9 +11691,15 @@
       <c r="AB111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC111" t="inlineStr">
-        <is>
-          <t>2655</t>
+      <c r="AC111" t="n">
+        <v>2655</v>
+      </c>
+      <c r="AD111" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AE111" t="inlineStr">
+        <is>
+          <t>2781</t>
         </is>
       </c>
     </row>
@@ -11136,9 +11794,15 @@
       <c r="AB112" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="AC112" t="inlineStr">
-        <is>
-          <t>3452</t>
+      <c r="AC112" t="n">
+        <v>3452</v>
+      </c>
+      <c r="AD112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE112" t="inlineStr">
+        <is>
+          <t>3513</t>
         </is>
       </c>
     </row>
@@ -11233,9 +11897,15 @@
       <c r="AB113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC113" t="inlineStr">
-        <is>
-          <t>3588</t>
+      <c r="AC113" t="n">
+        <v>3588</v>
+      </c>
+      <c r="AD113" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="AE113" t="inlineStr">
+        <is>
+          <t>3727</t>
         </is>
       </c>
     </row>
@@ -11330,9 +12000,15 @@
       <c r="AB114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC114" t="inlineStr">
-        <is>
-          <t>3124</t>
+      <c r="AC114" t="n">
+        <v>3124</v>
+      </c>
+      <c r="AD114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE114" t="inlineStr">
+        <is>
+          <t>3259</t>
         </is>
       </c>
     </row>
@@ -11427,9 +12103,15 @@
       <c r="AB115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC115" t="inlineStr">
-        <is>
-          <t>2316</t>
+      <c r="AC115" t="n">
+        <v>2316</v>
+      </c>
+      <c r="AD115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE115" t="inlineStr">
+        <is>
+          <t>2303</t>
         </is>
       </c>
     </row>
@@ -11524,9 +12206,15 @@
       <c r="AB116" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AC116" t="inlineStr">
-        <is>
-          <t>3339</t>
+      <c r="AC116" t="n">
+        <v>3339</v>
+      </c>
+      <c r="AD116" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AE116" t="inlineStr">
+        <is>
+          <t>3333</t>
         </is>
       </c>
     </row>
@@ -11621,9 +12309,15 @@
       <c r="AB117" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AC117" t="inlineStr">
-        <is>
-          <t>3771</t>
+      <c r="AC117" t="n">
+        <v>3771</v>
+      </c>
+      <c r="AD117" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE117" t="inlineStr">
+        <is>
+          <t>3638</t>
         </is>
       </c>
     </row>
@@ -11718,7 +12412,13 @@
       <c r="AB118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC118" t="inlineStr">
+      <c r="AC118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11815,9 +12515,15 @@
       <c r="AB119" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AC119" t="inlineStr">
-        <is>
-          <t>4068</t>
+      <c r="AC119" t="n">
+        <v>4068</v>
+      </c>
+      <c r="AD119" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AE119" t="inlineStr">
+        <is>
+          <t>4239</t>
         </is>
       </c>
     </row>
@@ -11912,9 +12618,15 @@
       <c r="AB120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC120" t="inlineStr">
-        <is>
-          <t>2567</t>
+      <c r="AC120" t="n">
+        <v>2567</v>
+      </c>
+      <c r="AD120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE120" t="inlineStr">
+        <is>
+          <t>2556</t>
         </is>
       </c>
     </row>
@@ -12009,9 +12721,15 @@
       <c r="AB121" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="AC121" t="inlineStr">
-        <is>
-          <t>3665</t>
+      <c r="AC121" t="n">
+        <v>3665</v>
+      </c>
+      <c r="AD121" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AE121" t="inlineStr">
+        <is>
+          <t>3807</t>
         </is>
       </c>
     </row>
@@ -12106,7 +12824,13 @@
       <c r="AB122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC122" t="inlineStr">
+      <c r="AC122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12203,9 +12927,15 @@
       <c r="AB123" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="AC123" t="inlineStr">
-        <is>
-          <t>3303</t>
+      <c r="AC123" t="n">
+        <v>3303</v>
+      </c>
+      <c r="AD123" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE123" t="inlineStr">
+        <is>
+          <t>3426</t>
         </is>
       </c>
     </row>
@@ -12300,9 +13030,15 @@
       <c r="AB124" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="AC124" t="inlineStr">
-        <is>
-          <t>3364</t>
+      <c r="AC124" t="n">
+        <v>3364</v>
+      </c>
+      <c r="AD124" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="AE124" t="inlineStr">
+        <is>
+          <t>3445</t>
         </is>
       </c>
     </row>
@@ -12397,9 +13133,15 @@
       <c r="AB125" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC125" t="inlineStr">
-        <is>
-          <t>3807</t>
+      <c r="AC125" t="n">
+        <v>3807</v>
+      </c>
+      <c r="AD125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE125" t="inlineStr">
+        <is>
+          <t>3805</t>
         </is>
       </c>
     </row>
@@ -12494,9 +13236,15 @@
       <c r="AB126" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC126" t="inlineStr">
-        <is>
-          <t>3340</t>
+      <c r="AC126" t="n">
+        <v>3340</v>
+      </c>
+      <c r="AD126" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AE126" t="inlineStr">
+        <is>
+          <t>3519</t>
         </is>
       </c>
     </row>
@@ -12591,9 +13339,15 @@
       <c r="AB127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC127" t="inlineStr">
-        <is>
-          <t>2350</t>
+      <c r="AC127" t="n">
+        <v>2350</v>
+      </c>
+      <c r="AD127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE127" t="inlineStr">
+        <is>
+          <t>2341</t>
         </is>
       </c>
     </row>
@@ -12688,7 +13442,13 @@
       <c r="AB128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC128" t="inlineStr">
+      <c r="AC128" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12785,7 +13545,13 @@
       <c r="AB129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC129" t="inlineStr">
+      <c r="AC129" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12882,9 +13648,15 @@
       <c r="AB130" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="AC130" t="inlineStr">
-        <is>
-          <t>2968</t>
+      <c r="AC130" t="n">
+        <v>2968</v>
+      </c>
+      <c r="AD130" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AE130" t="inlineStr">
+        <is>
+          <t>2981</t>
         </is>
       </c>
     </row>
@@ -12979,9 +13751,15 @@
       <c r="AB131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC131" t="inlineStr">
-        <is>
-          <t>2567</t>
+      <c r="AC131" t="n">
+        <v>2567</v>
+      </c>
+      <c r="AD131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE131" t="inlineStr">
+        <is>
+          <t>2575</t>
         </is>
       </c>
     </row>
@@ -13076,9 +13854,15 @@
       <c r="AB132" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC132" t="inlineStr">
-        <is>
-          <t>2729</t>
+      <c r="AC132" t="n">
+        <v>2729</v>
+      </c>
+      <c r="AD132" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE132" t="inlineStr">
+        <is>
+          <t>2754</t>
         </is>
       </c>
     </row>
@@ -13173,9 +13957,15 @@
       <c r="AB133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC133" t="inlineStr">
-        <is>
-          <t>2900</t>
+      <c r="AC133" t="n">
+        <v>2900</v>
+      </c>
+      <c r="AD133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE133" t="inlineStr">
+        <is>
+          <t>2901</t>
         </is>
       </c>
     </row>
@@ -13245,6 +14035,8 @@
       <c r="AA134" t="inlineStr"/>
       <c r="AB134" s="3" t="inlineStr"/>
       <c r="AC134" t="inlineStr"/>
+      <c r="AD134" s="3" t="inlineStr"/>
+      <c r="AE134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -13304,6 +14096,8 @@
       <c r="AA135" t="inlineStr"/>
       <c r="AB135" s="3" t="inlineStr"/>
       <c r="AC135" t="inlineStr"/>
+      <c r="AD135" s="3" t="inlineStr"/>
+      <c r="AE135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -13396,9 +14190,15 @@
       <c r="AB136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC136" t="inlineStr">
-        <is>
-          <t>2692</t>
+      <c r="AC136" t="n">
+        <v>2692</v>
+      </c>
+      <c r="AD136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE136" t="inlineStr">
+        <is>
+          <t>2681</t>
         </is>
       </c>
     </row>
@@ -13493,7 +14293,13 @@
       <c r="AB137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC137" t="inlineStr">
+      <c r="AC137" t="n">
+        <v>2556</v>
+      </c>
+      <c r="AD137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE137" t="inlineStr">
         <is>
           <t>2556</t>
         </is>
@@ -13557,6 +14363,8 @@
       <c r="AA138" t="inlineStr"/>
       <c r="AB138" s="3" t="inlineStr"/>
       <c r="AC138" t="inlineStr"/>
+      <c r="AD138" s="3" t="inlineStr"/>
+      <c r="AE138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -13649,9 +14457,15 @@
       <c r="AB139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC139" t="inlineStr">
-        <is>
-          <t>2404</t>
+      <c r="AC139" t="n">
+        <v>2404</v>
+      </c>
+      <c r="AD139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE139" t="inlineStr">
+        <is>
+          <t>2395</t>
         </is>
       </c>
     </row>
@@ -13746,9 +14560,15 @@
       <c r="AB140" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC140" t="inlineStr">
-        <is>
-          <t>3030</t>
+      <c r="AC140" t="n">
+        <v>3030</v>
+      </c>
+      <c r="AD140" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="AE140" t="inlineStr">
+        <is>
+          <t>3045</t>
         </is>
       </c>
     </row>
@@ -13810,6 +14630,8 @@
       <c r="AA141" t="inlineStr"/>
       <c r="AB141" s="3" t="inlineStr"/>
       <c r="AC141" t="inlineStr"/>
+      <c r="AD141" s="3" t="inlineStr"/>
+      <c r="AE141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -13902,9 +14724,15 @@
       <c r="AB142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC142" t="inlineStr">
-        <is>
-          <t>2227</t>
+      <c r="AC142" t="n">
+        <v>2227</v>
+      </c>
+      <c r="AD142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE142" t="inlineStr">
+        <is>
+          <t>2255</t>
         </is>
       </c>
     </row>
@@ -13966,6 +14794,8 @@
       <c r="AA143" t="inlineStr"/>
       <c r="AB143" s="3" t="inlineStr"/>
       <c r="AC143" t="inlineStr"/>
+      <c r="AD143" s="3" t="inlineStr"/>
+      <c r="AE143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -14025,6 +14855,8 @@
       <c r="AA144" t="inlineStr"/>
       <c r="AB144" s="3" t="inlineStr"/>
       <c r="AC144" t="inlineStr"/>
+      <c r="AD144" s="3" t="inlineStr"/>
+      <c r="AE144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -14084,6 +14916,8 @@
       <c r="AA145" t="inlineStr"/>
       <c r="AB145" s="3" t="inlineStr"/>
       <c r="AC145" t="inlineStr"/>
+      <c r="AD145" s="3" t="inlineStr"/>
+      <c r="AE145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -14143,6 +14977,8 @@
       <c r="AA146" t="inlineStr"/>
       <c r="AB146" s="3" t="inlineStr"/>
       <c r="AC146" t="inlineStr"/>
+      <c r="AD146" s="3" t="inlineStr"/>
+      <c r="AE146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -14202,6 +15038,8 @@
       <c r="AA147" t="inlineStr"/>
       <c r="AB147" s="3" t="inlineStr"/>
       <c r="AC147" t="inlineStr"/>
+      <c r="AD147" s="3" t="inlineStr"/>
+      <c r="AE147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -14294,9 +15132,15 @@
       <c r="AB148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC148" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="AC148" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE148" t="inlineStr">
+        <is>
+          <t>1524</t>
         </is>
       </c>
     </row>
@@ -14391,7 +15235,13 @@
       <c r="AB149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC149" t="inlineStr">
+      <c r="AC149" t="n">
+        <v>3849</v>
+      </c>
+      <c r="AD149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE149" t="inlineStr">
         <is>
           <t>3849</t>
         </is>
@@ -14488,7 +15338,13 @@
       <c r="AB150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC150" t="inlineStr">
+      <c r="AC150" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14585,7 +15441,13 @@
       <c r="AB151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC151" t="inlineStr">
+      <c r="AC151" t="n">
+        <v>2511</v>
+      </c>
+      <c r="AD151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE151" t="inlineStr">
         <is>
           <t>2511</t>
         </is>
@@ -14682,7 +15544,13 @@
       <c r="AB152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC152" t="inlineStr">
+      <c r="AC152" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14779,7 +15647,13 @@
       <c r="AB153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC153" t="inlineStr">
+      <c r="AC153" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14876,7 +15750,13 @@
       <c r="AB154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC154" t="inlineStr">
+      <c r="AC154" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14973,9 +15853,15 @@
       <c r="AB155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC155" t="inlineStr">
-        <is>
-          <t>2797</t>
+      <c r="AC155" t="n">
+        <v>2797</v>
+      </c>
+      <c r="AD155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE155" t="inlineStr">
+        <is>
+          <t>2918</t>
         </is>
       </c>
     </row>
@@ -15064,9 +15950,15 @@
       <c r="AB156" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="AC156" t="inlineStr">
-        <is>
-          <t>3577</t>
+      <c r="AC156" t="n">
+        <v>3577</v>
+      </c>
+      <c r="AD156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE156" t="inlineStr">
+        <is>
+          <t>3607</t>
         </is>
       </c>
     </row>
@@ -15122,6 +16014,8 @@
       <c r="AA157" t="inlineStr"/>
       <c r="AB157" s="3" t="inlineStr"/>
       <c r="AC157" t="inlineStr"/>
+      <c r="AD157" s="3" t="inlineStr"/>
+      <c r="AE157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -15208,7 +16102,13 @@
       <c r="AB158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC158" t="inlineStr">
+      <c r="AC158" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15299,9 +16199,15 @@
       <c r="AB159" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC159" t="inlineStr">
-        <is>
-          <t>2999</t>
+      <c r="AC159" t="n">
+        <v>2999</v>
+      </c>
+      <c r="AD159" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AE159" t="inlineStr">
+        <is>
+          <t>3070</t>
         </is>
       </c>
     </row>
@@ -15357,6 +16263,8 @@
       <c r="AA160" t="inlineStr"/>
       <c r="AB160" s="3" t="inlineStr"/>
       <c r="AC160" t="inlineStr"/>
+      <c r="AD160" s="3" t="inlineStr"/>
+      <c r="AE160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -15431,9 +16339,15 @@
       <c r="AB161" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AC161" t="inlineStr">
-        <is>
-          <t>3055</t>
+      <c r="AC161" t="n">
+        <v>3055</v>
+      </c>
+      <c r="AD161" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AE161" t="inlineStr">
+        <is>
+          <t>3147</t>
         </is>
       </c>
     </row>
@@ -15510,9 +16424,15 @@
       <c r="AB162" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="AC162" t="inlineStr">
-        <is>
-          <t>2672</t>
+      <c r="AC162" t="n">
+        <v>2672</v>
+      </c>
+      <c r="AD162" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="AE162" t="inlineStr">
+        <is>
+          <t>2713</t>
         </is>
       </c>
     </row>
@@ -15585,9 +16505,15 @@
       <c r="AB163" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC163" t="inlineStr">
-        <is>
-          <t>3213</t>
+      <c r="AC163" t="n">
+        <v>3213</v>
+      </c>
+      <c r="AD163" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE163" t="inlineStr">
+        <is>
+          <t>3489</t>
         </is>
       </c>
     </row>
@@ -15648,11 +16574,11 @@
       <c r="AB164" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC164" t="inlineStr">
-        <is>
-          <t>3557</t>
-        </is>
-      </c>
+      <c r="AC164" t="n">
+        <v>3557</v>
+      </c>
+      <c r="AD164" s="3" t="inlineStr"/>
+      <c r="AE164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="n">
@@ -15711,9 +16637,15 @@
       <c r="AB165" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="AC165" t="inlineStr">
-        <is>
-          <t>2853</t>
+      <c r="AC165" t="n">
+        <v>2853</v>
+      </c>
+      <c r="AD165" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AE165" t="inlineStr">
+        <is>
+          <t>2856</t>
         </is>
       </c>
     </row>
@@ -15766,9 +16698,66 @@
       <c r="AB166" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC166" t="inlineStr">
-        <is>
-          <t>2561</t>
+      <c r="AC166" t="n">
+        <v>2561</v>
+      </c>
+      <c r="AD166" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AE166" t="inlineStr">
+        <is>
+          <t>3013</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>58910668</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>BrittleAuthor33</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr"/>
+      <c r="D167" t="inlineStr"/>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F167" s="3" t="inlineStr"/>
+      <c r="G167" t="inlineStr"/>
+      <c r="H167" s="3" t="inlineStr"/>
+      <c r="I167" t="inlineStr"/>
+      <c r="J167" s="3" t="inlineStr"/>
+      <c r="K167" t="inlineStr"/>
+      <c r="L167" s="3" t="inlineStr"/>
+      <c r="M167" t="inlineStr"/>
+      <c r="N167" s="3" t="inlineStr"/>
+      <c r="O167" t="inlineStr"/>
+      <c r="P167" s="3" t="inlineStr"/>
+      <c r="Q167" t="inlineStr"/>
+      <c r="R167" s="3" t="inlineStr"/>
+      <c r="S167" t="inlineStr"/>
+      <c r="T167" s="3" t="inlineStr"/>
+      <c r="U167" t="inlineStr"/>
+      <c r="V167" s="3" t="inlineStr"/>
+      <c r="W167" t="inlineStr"/>
+      <c r="X167" s="3" t="inlineStr"/>
+      <c r="Y167" t="inlineStr"/>
+      <c r="Z167" s="3" t="inlineStr"/>
+      <c r="AA167" t="inlineStr"/>
+      <c r="AB167" s="3" t="inlineStr"/>
+      <c r="AC167" t="inlineStr"/>
+      <c r="AD167" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE167" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-02-25 11:30:47
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -16711,10 +16711,8 @@
       </c>
     </row>
     <row r="167">
-      <c r="A167" t="inlineStr">
-        <is>
-          <t>58910668</t>
-        </is>
+      <c r="A167" t="n">
+        <v>58910668</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Code updated 23-02-26 01:22:54
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -644,10 +644,8 @@
       <c r="AD2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE2" t="inlineStr">
-        <is>
-          <t>3995</t>
-        </is>
+      <c r="AE2" t="n">
+        <v>3995</v>
       </c>
     </row>
     <row r="3">
@@ -747,10 +745,8 @@
       <c r="AD3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AE3" t="inlineStr">
-        <is>
-          <t>6488</t>
-        </is>
+      <c r="AE3" t="n">
+        <v>6488</v>
       </c>
     </row>
     <row r="4">
@@ -850,10 +846,8 @@
       <c r="AD4" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AE4" t="inlineStr">
-        <is>
-          <t>6513</t>
-        </is>
+      <c r="AE4" t="n">
+        <v>6513</v>
       </c>
     </row>
     <row r="5">
@@ -953,10 +947,8 @@
       <c r="AD5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AE5" t="inlineStr">
-        <is>
-          <t>6013</t>
-        </is>
+      <c r="AE5" t="n">
+        <v>6013</v>
       </c>
     </row>
     <row r="6">
@@ -1056,10 +1048,8 @@
       <c r="AD6" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AE6" t="inlineStr">
-        <is>
-          <t>6115</t>
-        </is>
+      <c r="AE6" t="n">
+        <v>6115</v>
       </c>
     </row>
     <row r="7">
@@ -1159,10 +1149,8 @@
       <c r="AD7" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AE7" t="inlineStr">
-        <is>
-          <t>6772</t>
-        </is>
+      <c r="AE7" t="n">
+        <v>6772</v>
       </c>
     </row>
     <row r="8">
@@ -1262,10 +1250,8 @@
       <c r="AD8" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AE8" t="inlineStr">
-        <is>
-          <t>5310</t>
-        </is>
+      <c r="AE8" t="n">
+        <v>5310</v>
       </c>
     </row>
     <row r="9">
@@ -1365,10 +1351,8 @@
       <c r="AD9" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AE9" t="inlineStr">
-        <is>
-          <t>5810</t>
-        </is>
+      <c r="AE9" t="n">
+        <v>5810</v>
       </c>
     </row>
     <row r="10">
@@ -1468,10 +1452,8 @@
       <c r="AD10" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AE10" t="inlineStr">
-        <is>
-          <t>6944</t>
-        </is>
+      <c r="AE10" t="n">
+        <v>6944</v>
       </c>
     </row>
     <row r="11">
@@ -1571,10 +1553,8 @@
       <c r="AD11" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="AE11" t="inlineStr">
-        <is>
-          <t>5566</t>
-        </is>
+      <c r="AE11" t="n">
+        <v>5566</v>
       </c>
     </row>
     <row r="12">
@@ -1674,10 +1654,8 @@
       <c r="AD12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE12" t="inlineStr">
-        <is>
-          <t>2914</t>
-        </is>
+      <c r="AE12" t="n">
+        <v>2914</v>
       </c>
     </row>
     <row r="13">
@@ -1777,10 +1755,8 @@
       <c r="AD13" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AE13" t="inlineStr">
-        <is>
-          <t>6804</t>
-        </is>
+      <c r="AE13" t="n">
+        <v>6804</v>
       </c>
     </row>
     <row r="14">
@@ -1880,10 +1856,8 @@
       <c r="AD14" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="AE14" t="inlineStr">
-        <is>
-          <t>5938</t>
-        </is>
+      <c r="AE14" t="n">
+        <v>5938</v>
       </c>
     </row>
     <row r="15">
@@ -1983,10 +1957,8 @@
       <c r="AD15" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AE15" t="inlineStr">
-        <is>
-          <t>5697</t>
-        </is>
+      <c r="AE15" t="n">
+        <v>5697</v>
       </c>
     </row>
     <row r="16">
@@ -2086,10 +2058,8 @@
       <c r="AD16" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AE16" t="inlineStr">
-        <is>
-          <t>6360</t>
-        </is>
+      <c r="AE16" t="n">
+        <v>6360</v>
       </c>
     </row>
     <row r="17">
@@ -2189,10 +2159,8 @@
       <c r="AD17" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AE17" t="inlineStr">
-        <is>
-          <t>4707</t>
-        </is>
+      <c r="AE17" t="n">
+        <v>4707</v>
       </c>
     </row>
     <row r="18">
@@ -2292,10 +2260,8 @@
       <c r="AD18" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AE18" t="inlineStr">
-        <is>
-          <t>4827</t>
-        </is>
+      <c r="AE18" t="n">
+        <v>4827</v>
       </c>
     </row>
     <row r="19">
@@ -2395,10 +2361,8 @@
       <c r="AD19" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AE19" t="inlineStr">
-        <is>
-          <t>6005</t>
-        </is>
+      <c r="AE19" t="n">
+        <v>6005</v>
       </c>
     </row>
     <row r="20">
@@ -2498,10 +2462,8 @@
       <c r="AD20" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="AE20" t="inlineStr">
-        <is>
-          <t>7128</t>
-        </is>
+      <c r="AE20" t="n">
+        <v>7128</v>
       </c>
     </row>
     <row r="21">
@@ -2601,10 +2563,8 @@
       <c r="AD21" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="AE21" t="inlineStr">
-        <is>
-          <t>5710</t>
-        </is>
+      <c r="AE21" t="n">
+        <v>5710</v>
       </c>
     </row>
     <row r="22">
@@ -2704,10 +2664,8 @@
       <c r="AD22" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AE22" t="inlineStr">
-        <is>
-          <t>5648</t>
-        </is>
+      <c r="AE22" t="n">
+        <v>5648</v>
       </c>
     </row>
     <row r="23">
@@ -2807,10 +2765,8 @@
       <c r="AD23" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="AE23" t="inlineStr">
-        <is>
-          <t>5632</t>
-        </is>
+      <c r="AE23" t="n">
+        <v>5632</v>
       </c>
     </row>
     <row r="24">
@@ -2910,10 +2866,8 @@
       <c r="AD24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AE24" t="inlineStr">
-        <is>
-          <t>6443</t>
-        </is>
+      <c r="AE24" t="n">
+        <v>6443</v>
       </c>
     </row>
     <row r="25">
@@ -3013,10 +2967,8 @@
       <c r="AD25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE25" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="AE25" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -3116,10 +3068,8 @@
       <c r="AD26" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="AE26" t="inlineStr">
-        <is>
-          <t>6090</t>
-        </is>
+      <c r="AE26" t="n">
+        <v>6090</v>
       </c>
     </row>
     <row r="27">
@@ -3219,10 +3169,8 @@
       <c r="AD27" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AE27" t="inlineStr">
-        <is>
-          <t>6928</t>
-        </is>
+      <c r="AE27" t="n">
+        <v>6928</v>
       </c>
     </row>
     <row r="28">
@@ -3322,10 +3270,8 @@
       <c r="AD28" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="AE28" t="inlineStr">
-        <is>
-          <t>6040</t>
-        </is>
+      <c r="AE28" t="n">
+        <v>6040</v>
       </c>
     </row>
     <row r="29">
@@ -3425,10 +3371,8 @@
       <c r="AD29" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AE29" t="inlineStr">
-        <is>
-          <t>6924</t>
-        </is>
+      <c r="AE29" t="n">
+        <v>6924</v>
       </c>
     </row>
     <row r="30">
@@ -3528,10 +3472,8 @@
       <c r="AD30" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="AE30" t="inlineStr">
-        <is>
-          <t>5703</t>
-        </is>
+      <c r="AE30" t="n">
+        <v>5703</v>
       </c>
     </row>
     <row r="31">
@@ -3631,10 +3573,8 @@
       <c r="AD31" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AE31" t="inlineStr">
-        <is>
-          <t>6744</t>
-        </is>
+      <c r="AE31" t="n">
+        <v>6744</v>
       </c>
     </row>
     <row r="32">
@@ -3734,10 +3674,8 @@
       <c r="AD32" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AE32" t="inlineStr">
-        <is>
-          <t>6061</t>
-        </is>
+      <c r="AE32" t="n">
+        <v>6061</v>
       </c>
     </row>
     <row r="33">
@@ -3837,10 +3775,8 @@
       <c r="AD33" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AE33" t="inlineStr">
-        <is>
-          <t>6019</t>
-        </is>
+      <c r="AE33" t="n">
+        <v>6019</v>
       </c>
     </row>
     <row r="34">
@@ -3940,10 +3876,8 @@
       <c r="AD34" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AE34" t="inlineStr">
-        <is>
-          <t>5961</t>
-        </is>
+      <c r="AE34" t="n">
+        <v>5961</v>
       </c>
     </row>
     <row r="35">
@@ -4043,10 +3977,8 @@
       <c r="AD35" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AE35" t="inlineStr">
-        <is>
-          <t>6340</t>
-        </is>
+      <c r="AE35" t="n">
+        <v>6340</v>
       </c>
     </row>
     <row r="36">
@@ -4146,10 +4078,8 @@
       <c r="AD36" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AE36" t="inlineStr">
-        <is>
-          <t>5779</t>
-        </is>
+      <c r="AE36" t="n">
+        <v>5779</v>
       </c>
     </row>
     <row r="37">
@@ -4249,10 +4179,8 @@
       <c r="AD37" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AE37" t="inlineStr">
-        <is>
-          <t>4623</t>
-        </is>
+      <c r="AE37" t="n">
+        <v>4623</v>
       </c>
     </row>
     <row r="38">
@@ -4352,10 +4280,8 @@
       <c r="AD38" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AE38" t="inlineStr">
-        <is>
-          <t>5990</t>
-        </is>
+      <c r="AE38" t="n">
+        <v>5990</v>
       </c>
     </row>
     <row r="39">
@@ -4455,10 +4381,8 @@
       <c r="AD39" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AE39" t="inlineStr">
-        <is>
-          <t>6069</t>
-        </is>
+      <c r="AE39" t="n">
+        <v>6069</v>
       </c>
     </row>
     <row r="40">
@@ -4558,10 +4482,8 @@
       <c r="AD40" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AE40" t="inlineStr">
-        <is>
-          <t>6888</t>
-        </is>
+      <c r="AE40" t="n">
+        <v>6888</v>
       </c>
     </row>
     <row r="41">
@@ -4661,10 +4583,8 @@
       <c r="AD41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE41" t="inlineStr">
-        <is>
-          <t>3648</t>
-        </is>
+      <c r="AE41" t="n">
+        <v>3648</v>
       </c>
     </row>
     <row r="42">
@@ -4764,10 +4684,8 @@
       <c r="AD42" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AE42" t="inlineStr">
-        <is>
-          <t>7008</t>
-        </is>
+      <c r="AE42" t="n">
+        <v>7008</v>
       </c>
     </row>
     <row r="43">
@@ -4867,10 +4785,8 @@
       <c r="AD43" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AE43" t="inlineStr">
-        <is>
-          <t>6246</t>
-        </is>
+      <c r="AE43" t="n">
+        <v>6246</v>
       </c>
     </row>
     <row r="44">
@@ -4970,10 +4886,8 @@
       <c r="AD44" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AE44" t="inlineStr">
-        <is>
-          <t>6225</t>
-        </is>
+      <c r="AE44" t="n">
+        <v>6225</v>
       </c>
     </row>
     <row r="45">
@@ -5073,10 +4987,8 @@
       <c r="AD45" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="AE45" t="inlineStr">
-        <is>
-          <t>5610</t>
-        </is>
+      <c r="AE45" t="n">
+        <v>5610</v>
       </c>
     </row>
     <row r="46">
@@ -5176,10 +5088,8 @@
       <c r="AD46" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AE46" t="inlineStr">
-        <is>
-          <t>5917</t>
-        </is>
+      <c r="AE46" t="n">
+        <v>5917</v>
       </c>
     </row>
     <row r="47">
@@ -5279,10 +5189,8 @@
       <c r="AD47" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AE47" t="inlineStr">
-        <is>
-          <t>3526</t>
-        </is>
+      <c r="AE47" t="n">
+        <v>3526</v>
       </c>
     </row>
     <row r="48">
@@ -5382,10 +5290,8 @@
       <c r="AD48" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="AE48" t="inlineStr">
-        <is>
-          <t>6450</t>
-        </is>
+      <c r="AE48" t="n">
+        <v>6450</v>
       </c>
     </row>
     <row r="49">
@@ -5485,10 +5391,8 @@
       <c r="AD49" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AE49" t="inlineStr">
-        <is>
-          <t>5060</t>
-        </is>
+      <c r="AE49" t="n">
+        <v>5060</v>
       </c>
     </row>
     <row r="50">
@@ -5588,10 +5492,8 @@
       <c r="AD50" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AE50" t="inlineStr">
-        <is>
-          <t>6842</t>
-        </is>
+      <c r="AE50" t="n">
+        <v>6842</v>
       </c>
     </row>
     <row r="51">
@@ -5691,10 +5593,8 @@
       <c r="AD51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE51" t="inlineStr">
-        <is>
-          <t>2924</t>
-        </is>
+      <c r="AE51" t="n">
+        <v>2924</v>
       </c>
     </row>
     <row r="52">
@@ -5794,10 +5694,8 @@
       <c r="AD52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE52" t="inlineStr">
-        <is>
-          <t>2907</t>
-        </is>
+      <c r="AE52" t="n">
+        <v>2907</v>
       </c>
     </row>
     <row r="53">
@@ -5897,10 +5795,8 @@
       <c r="AD53" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="AE53" t="inlineStr">
-        <is>
-          <t>3074</t>
-        </is>
+      <c r="AE53" t="n">
+        <v>3074</v>
       </c>
     </row>
     <row r="54">
@@ -6000,10 +5896,8 @@
       <c r="AD54" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AE54" t="inlineStr">
-        <is>
-          <t>5930</t>
-        </is>
+      <c r="AE54" t="n">
+        <v>5930</v>
       </c>
     </row>
     <row r="55">
@@ -6103,10 +5997,8 @@
       <c r="AD55" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AE55" t="inlineStr">
-        <is>
-          <t>4601</t>
-        </is>
+      <c r="AE55" t="n">
+        <v>4601</v>
       </c>
     </row>
     <row r="56">
@@ -6206,10 +6098,8 @@
       <c r="AD56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AE56" t="inlineStr">
-        <is>
-          <t>4640</t>
-        </is>
+      <c r="AE56" t="n">
+        <v>4640</v>
       </c>
     </row>
     <row r="57">
@@ -6309,10 +6199,8 @@
       <c r="AD57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AE57" t="inlineStr">
-        <is>
-          <t>5551</t>
-        </is>
+      <c r="AE57" t="n">
+        <v>5551</v>
       </c>
     </row>
     <row r="58">
@@ -6412,10 +6300,8 @@
       <c r="AD58" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AE58" t="inlineStr">
-        <is>
-          <t>4762</t>
-        </is>
+      <c r="AE58" t="n">
+        <v>4762</v>
       </c>
     </row>
     <row r="59">
@@ -6605,10 +6491,8 @@
       <c r="AD61" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AE61" t="inlineStr">
-        <is>
-          <t>5267</t>
-        </is>
+      <c r="AE61" t="n">
+        <v>5267</v>
       </c>
     </row>
     <row r="62">
@@ -6708,10 +6592,8 @@
       <c r="AD62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE62" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="AE62" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -6811,10 +6693,8 @@
       <c r="AD63" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AE63" t="inlineStr">
-        <is>
-          <t>5570</t>
-        </is>
+      <c r="AE63" t="n">
+        <v>5570</v>
       </c>
     </row>
     <row r="64">
@@ -6914,10 +6794,8 @@
       <c r="AD64" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="AE64" t="inlineStr">
-        <is>
-          <t>3258</t>
-        </is>
+      <c r="AE64" t="n">
+        <v>3258</v>
       </c>
     </row>
     <row r="65">
@@ -7062,10 +6940,8 @@
       <c r="AD66" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AE66" t="inlineStr">
-        <is>
-          <t>2704</t>
-        </is>
+      <c r="AE66" t="n">
+        <v>2704</v>
       </c>
     </row>
     <row r="67">
@@ -7165,10 +7041,8 @@
       <c r="AD67" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AE67" t="inlineStr">
-        <is>
-          <t>5202</t>
-        </is>
+      <c r="AE67" t="n">
+        <v>5202</v>
       </c>
     </row>
     <row r="68">
@@ -7268,10 +7142,8 @@
       <c r="AD68" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="AE68" t="inlineStr">
-        <is>
-          <t>6187</t>
-        </is>
+      <c r="AE68" t="n">
+        <v>6187</v>
       </c>
     </row>
     <row r="69">
@@ -7371,10 +7243,8 @@
       <c r="AD69" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AE69" t="inlineStr">
-        <is>
-          <t>4523</t>
-        </is>
+      <c r="AE69" t="n">
+        <v>4523</v>
       </c>
     </row>
     <row r="70">
@@ -7474,10 +7344,8 @@
       <c r="AD70" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="AE70" t="inlineStr">
-        <is>
-          <t>4208</t>
-        </is>
+      <c r="AE70" t="n">
+        <v>4208</v>
       </c>
     </row>
     <row r="71">
@@ -7577,10 +7445,8 @@
       <c r="AD71" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="AE71" t="inlineStr">
-        <is>
-          <t>5094</t>
-        </is>
+      <c r="AE71" t="n">
+        <v>5094</v>
       </c>
     </row>
     <row r="72">
@@ -7680,10 +7546,8 @@
       <c r="AD72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE72" t="inlineStr">
-        <is>
-          <t>3832</t>
-        </is>
+      <c r="AE72" t="n">
+        <v>3832</v>
       </c>
     </row>
     <row r="73">
@@ -7783,10 +7647,8 @@
       <c r="AD73" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AE73" t="inlineStr">
-        <is>
-          <t>4520</t>
-        </is>
+      <c r="AE73" t="n">
+        <v>4520</v>
       </c>
     </row>
     <row r="74">
@@ -7886,10 +7748,8 @@
       <c r="AD74" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="AE74" t="inlineStr">
-        <is>
-          <t>4229</t>
-        </is>
+      <c r="AE74" t="n">
+        <v>4229</v>
       </c>
     </row>
     <row r="75">
@@ -7989,10 +7849,8 @@
       <c r="AD75" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AE75" t="inlineStr">
-        <is>
-          <t>4384</t>
-        </is>
+      <c r="AE75" t="n">
+        <v>4384</v>
       </c>
     </row>
     <row r="76">
@@ -8092,10 +7950,8 @@
       <c r="AD76" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AE76" t="inlineStr">
-        <is>
-          <t>5333</t>
-        </is>
+      <c r="AE76" t="n">
+        <v>5333</v>
       </c>
     </row>
     <row r="77">
@@ -8195,10 +8051,8 @@
       <c r="AD77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE77" t="inlineStr">
-        <is>
-          <t>3383</t>
-        </is>
+      <c r="AE77" t="n">
+        <v>3383</v>
       </c>
     </row>
     <row r="78">
@@ -8298,10 +8152,8 @@
       <c r="AD78" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AE78" t="inlineStr">
-        <is>
-          <t>5301</t>
-        </is>
+      <c r="AE78" t="n">
+        <v>5301</v>
       </c>
     </row>
     <row r="79">
@@ -8401,10 +8253,8 @@
       <c r="AD79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE79" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="AE79" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="80">
@@ -8504,10 +8354,8 @@
       <c r="AD80" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="AE80" t="inlineStr">
-        <is>
-          <t>5142</t>
-        </is>
+      <c r="AE80" t="n">
+        <v>5142</v>
       </c>
     </row>
     <row r="81">
@@ -8607,10 +8455,8 @@
       <c r="AD81" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AE81" t="inlineStr">
-        <is>
-          <t>5115</t>
-        </is>
+      <c r="AE81" t="n">
+        <v>5115</v>
       </c>
     </row>
     <row r="82">
@@ -8710,10 +8556,8 @@
       <c r="AD82" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AE82" t="inlineStr">
-        <is>
-          <t>4945</t>
-        </is>
+      <c r="AE82" t="n">
+        <v>4945</v>
       </c>
     </row>
     <row r="83">
@@ -8813,10 +8657,8 @@
       <c r="AD83" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AE83" t="inlineStr">
-        <is>
-          <t>4680</t>
-        </is>
+      <c r="AE83" t="n">
+        <v>4680</v>
       </c>
     </row>
     <row r="84">
@@ -8916,10 +8758,8 @@
       <c r="AD84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE84" t="inlineStr">
-        <is>
-          <t>2968</t>
-        </is>
+      <c r="AE84" t="n">
+        <v>2968</v>
       </c>
     </row>
     <row r="85">
@@ -9019,10 +8859,8 @@
       <c r="AD85" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AE85" t="inlineStr">
-        <is>
-          <t>3949</t>
-        </is>
+      <c r="AE85" t="n">
+        <v>3949</v>
       </c>
     </row>
     <row r="86">
@@ -9122,10 +8960,8 @@
       <c r="AD86" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AE86" t="inlineStr">
-        <is>
-          <t>3550</t>
-        </is>
+      <c r="AE86" t="n">
+        <v>3550</v>
       </c>
     </row>
     <row r="87">
@@ -9225,10 +9061,8 @@
       <c r="AD87" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AE87" t="inlineStr">
-        <is>
-          <t>4962</t>
-        </is>
+      <c r="AE87" t="n">
+        <v>4962</v>
       </c>
     </row>
     <row r="88">
@@ -9328,10 +9162,8 @@
       <c r="AD88" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AE88" t="inlineStr">
-        <is>
-          <t>3048</t>
-        </is>
+      <c r="AE88" t="n">
+        <v>3048</v>
       </c>
     </row>
     <row r="89">
@@ -9431,10 +9263,8 @@
       <c r="AD89" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AE89" t="inlineStr">
-        <is>
-          <t>3453</t>
-        </is>
+      <c r="AE89" t="n">
+        <v>3453</v>
       </c>
     </row>
     <row r="90">
@@ -9534,10 +9364,8 @@
       <c r="AD90" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AE90" t="inlineStr">
-        <is>
-          <t>2815</t>
-        </is>
+      <c r="AE90" t="n">
+        <v>2815</v>
       </c>
     </row>
     <row r="91">
@@ -9637,10 +9465,8 @@
       <c r="AD91" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AE91" t="inlineStr">
-        <is>
-          <t>2943</t>
-        </is>
+      <c r="AE91" t="n">
+        <v>2943</v>
       </c>
     </row>
     <row r="92">
@@ -9740,10 +9566,8 @@
       <c r="AD92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE92" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="AE92" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="93">
@@ -9843,10 +9667,8 @@
       <c r="AD93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE93" t="inlineStr">
-        <is>
-          <t>2586</t>
-        </is>
+      <c r="AE93" t="n">
+        <v>2586</v>
       </c>
     </row>
     <row r="94">
@@ -9946,10 +9768,8 @@
       <c r="AD94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE94" t="inlineStr">
-        <is>
-          <t>3265</t>
-        </is>
+      <c r="AE94" t="n">
+        <v>3265</v>
       </c>
     </row>
     <row r="95">
@@ -10049,10 +9869,8 @@
       <c r="AD95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE95" t="inlineStr">
-        <is>
-          <t>2500</t>
-        </is>
+      <c r="AE95" t="n">
+        <v>2500</v>
       </c>
     </row>
     <row r="96">
@@ -10152,10 +9970,8 @@
       <c r="AD96" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="AE96" t="inlineStr">
-        <is>
-          <t>3877</t>
-        </is>
+      <c r="AE96" t="n">
+        <v>3877</v>
       </c>
     </row>
     <row r="97">
@@ -10255,10 +10071,8 @@
       <c r="AD97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE97" t="inlineStr">
-        <is>
-          <t>3111</t>
-        </is>
+      <c r="AE97" t="n">
+        <v>3111</v>
       </c>
     </row>
     <row r="98">
@@ -10358,10 +10172,8 @@
       <c r="AD98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE98" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="AE98" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="99">
@@ -10461,10 +10273,8 @@
       <c r="AD99" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AE99" t="inlineStr">
-        <is>
-          <t>4130</t>
-        </is>
+      <c r="AE99" t="n">
+        <v>4130</v>
       </c>
     </row>
     <row r="100">
@@ -10564,10 +10374,8 @@
       <c r="AD100" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="AE100" t="inlineStr">
-        <is>
-          <t>2781</t>
-        </is>
+      <c r="AE100" t="n">
+        <v>2781</v>
       </c>
     </row>
     <row r="101">
@@ -10667,10 +10475,8 @@
       <c r="AD101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AE101" t="inlineStr">
-        <is>
-          <t>4725</t>
-        </is>
+      <c r="AE101" t="n">
+        <v>4725</v>
       </c>
     </row>
     <row r="102">
@@ -10770,10 +10576,8 @@
       <c r="AD102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AE102" t="inlineStr">
-        <is>
-          <t>4155</t>
-        </is>
+      <c r="AE102" t="n">
+        <v>4155</v>
       </c>
     </row>
     <row r="103">
@@ -10873,10 +10677,8 @@
       <c r="AD103" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AE103" t="inlineStr">
-        <is>
-          <t>3596</t>
-        </is>
+      <c r="AE103" t="n">
+        <v>3596</v>
       </c>
     </row>
     <row r="104">
@@ -10976,10 +10778,8 @@
       <c r="AD104" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AE104" t="inlineStr">
-        <is>
-          <t>4721</t>
-        </is>
+      <c r="AE104" t="n">
+        <v>4721</v>
       </c>
     </row>
     <row r="105">
@@ -11079,10 +10879,8 @@
       <c r="AD105" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AE105" t="inlineStr">
-        <is>
-          <t>4347</t>
-        </is>
+      <c r="AE105" t="n">
+        <v>4347</v>
       </c>
     </row>
     <row r="106">
@@ -11182,10 +10980,8 @@
       <c r="AD106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE106" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="AE106" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="107">
@@ -11285,10 +11081,8 @@
       <c r="AD107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE107" t="inlineStr">
-        <is>
-          <t>2529</t>
-        </is>
+      <c r="AE107" t="n">
+        <v>2529</v>
       </c>
     </row>
     <row r="108">
@@ -11388,10 +11182,8 @@
       <c r="AD108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE108" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="AE108" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="109">
@@ -11491,10 +11283,8 @@
       <c r="AD109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE109" t="inlineStr">
-        <is>
-          <t>3916</t>
-        </is>
+      <c r="AE109" t="n">
+        <v>3916</v>
       </c>
     </row>
     <row r="110">
@@ -11594,10 +11384,8 @@
       <c r="AD110" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AE110" t="inlineStr">
-        <is>
-          <t>3765</t>
-        </is>
+      <c r="AE110" t="n">
+        <v>3765</v>
       </c>
     </row>
     <row r="111">
@@ -11697,10 +11485,8 @@
       <c r="AD111" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AE111" t="inlineStr">
-        <is>
-          <t>2781</t>
-        </is>
+      <c r="AE111" t="n">
+        <v>2781</v>
       </c>
     </row>
     <row r="112">
@@ -11800,10 +11586,8 @@
       <c r="AD112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE112" t="inlineStr">
-        <is>
-          <t>3513</t>
-        </is>
+      <c r="AE112" t="n">
+        <v>3513</v>
       </c>
     </row>
     <row r="113">
@@ -11903,10 +11687,8 @@
       <c r="AD113" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="AE113" t="inlineStr">
-        <is>
-          <t>3727</t>
-        </is>
+      <c r="AE113" t="n">
+        <v>3727</v>
       </c>
     </row>
     <row r="114">
@@ -12006,10 +11788,8 @@
       <c r="AD114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE114" t="inlineStr">
-        <is>
-          <t>3259</t>
-        </is>
+      <c r="AE114" t="n">
+        <v>3259</v>
       </c>
     </row>
     <row r="115">
@@ -12109,10 +11889,8 @@
       <c r="AD115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE115" t="inlineStr">
-        <is>
-          <t>2303</t>
-        </is>
+      <c r="AE115" t="n">
+        <v>2303</v>
       </c>
     </row>
     <row r="116">
@@ -12212,10 +11990,8 @@
       <c r="AD116" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AE116" t="inlineStr">
-        <is>
-          <t>3333</t>
-        </is>
+      <c r="AE116" t="n">
+        <v>3333</v>
       </c>
     </row>
     <row r="117">
@@ -12315,10 +12091,8 @@
       <c r="AD117" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE117" t="inlineStr">
-        <is>
-          <t>3638</t>
-        </is>
+      <c r="AE117" t="n">
+        <v>3638</v>
       </c>
     </row>
     <row r="118">
@@ -12418,10 +12192,8 @@
       <c r="AD118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE118" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="AE118" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="119">
@@ -12521,10 +12293,8 @@
       <c r="AD119" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AE119" t="inlineStr">
-        <is>
-          <t>4239</t>
-        </is>
+      <c r="AE119" t="n">
+        <v>4239</v>
       </c>
     </row>
     <row r="120">
@@ -12624,10 +12394,8 @@
       <c r="AD120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE120" t="inlineStr">
-        <is>
-          <t>2556</t>
-        </is>
+      <c r="AE120" t="n">
+        <v>2556</v>
       </c>
     </row>
     <row r="121">
@@ -12727,10 +12495,8 @@
       <c r="AD121" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AE121" t="inlineStr">
-        <is>
-          <t>3807</t>
-        </is>
+      <c r="AE121" t="n">
+        <v>3807</v>
       </c>
     </row>
     <row r="122">
@@ -12830,10 +12596,8 @@
       <c r="AD122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE122" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="AE122" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="123">
@@ -12933,10 +12697,8 @@
       <c r="AD123" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AE123" t="inlineStr">
-        <is>
-          <t>3426</t>
-        </is>
+      <c r="AE123" t="n">
+        <v>3426</v>
       </c>
     </row>
     <row r="124">
@@ -13036,10 +12798,8 @@
       <c r="AD124" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="AE124" t="inlineStr">
-        <is>
-          <t>3445</t>
-        </is>
+      <c r="AE124" t="n">
+        <v>3445</v>
       </c>
     </row>
     <row r="125">
@@ -13139,10 +12899,8 @@
       <c r="AD125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE125" t="inlineStr">
-        <is>
-          <t>3805</t>
-        </is>
+      <c r="AE125" t="n">
+        <v>3805</v>
       </c>
     </row>
     <row r="126">
@@ -13242,10 +13000,8 @@
       <c r="AD126" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AE126" t="inlineStr">
-        <is>
-          <t>3519</t>
-        </is>
+      <c r="AE126" t="n">
+        <v>3519</v>
       </c>
     </row>
     <row r="127">
@@ -13345,10 +13101,8 @@
       <c r="AD127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE127" t="inlineStr">
-        <is>
-          <t>2341</t>
-        </is>
+      <c r="AE127" t="n">
+        <v>2341</v>
       </c>
     </row>
     <row r="128">
@@ -13448,10 +13202,8 @@
       <c r="AD128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE128" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="AE128" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="129">
@@ -13551,10 +13303,8 @@
       <c r="AD129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE129" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="AE129" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="130">
@@ -13654,10 +13404,8 @@
       <c r="AD130" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AE130" t="inlineStr">
-        <is>
-          <t>2981</t>
-        </is>
+      <c r="AE130" t="n">
+        <v>2981</v>
       </c>
     </row>
     <row r="131">
@@ -13757,10 +13505,8 @@
       <c r="AD131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE131" t="inlineStr">
-        <is>
-          <t>2575</t>
-        </is>
+      <c r="AE131" t="n">
+        <v>2575</v>
       </c>
     </row>
     <row r="132">
@@ -13860,10 +13606,8 @@
       <c r="AD132" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AE132" t="inlineStr">
-        <is>
-          <t>2754</t>
-        </is>
+      <c r="AE132" t="n">
+        <v>2754</v>
       </c>
     </row>
     <row r="133">
@@ -13963,10 +13707,8 @@
       <c r="AD133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE133" t="inlineStr">
-        <is>
-          <t>2901</t>
-        </is>
+      <c r="AE133" t="n">
+        <v>2901</v>
       </c>
     </row>
     <row r="134">
@@ -14196,10 +13938,8 @@
       <c r="AD136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE136" t="inlineStr">
-        <is>
-          <t>2681</t>
-        </is>
+      <c r="AE136" t="n">
+        <v>2681</v>
       </c>
     </row>
     <row r="137">
@@ -14299,10 +14039,8 @@
       <c r="AD137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE137" t="inlineStr">
-        <is>
-          <t>2556</t>
-        </is>
+      <c r="AE137" t="n">
+        <v>2556</v>
       </c>
     </row>
     <row r="138">
@@ -14463,10 +14201,8 @@
       <c r="AD139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE139" t="inlineStr">
-        <is>
-          <t>2395</t>
-        </is>
+      <c r="AE139" t="n">
+        <v>2395</v>
       </c>
     </row>
     <row r="140">
@@ -14566,10 +14302,8 @@
       <c r="AD140" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="AE140" t="inlineStr">
-        <is>
-          <t>3045</t>
-        </is>
+      <c r="AE140" t="n">
+        <v>3045</v>
       </c>
     </row>
     <row r="141">
@@ -14730,10 +14464,8 @@
       <c r="AD142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE142" t="inlineStr">
-        <is>
-          <t>2255</t>
-        </is>
+      <c r="AE142" t="n">
+        <v>2255</v>
       </c>
     </row>
     <row r="143">
@@ -15138,10 +14870,8 @@
       <c r="AD148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE148" t="inlineStr">
-        <is>
-          <t>1524</t>
-        </is>
+      <c r="AE148" t="n">
+        <v>1524</v>
       </c>
     </row>
     <row r="149">
@@ -15241,10 +14971,8 @@
       <c r="AD149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE149" t="inlineStr">
-        <is>
-          <t>3849</t>
-        </is>
+      <c r="AE149" t="n">
+        <v>3849</v>
       </c>
     </row>
     <row r="150">
@@ -15344,10 +15072,8 @@
       <c r="AD150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE150" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="AE150" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="151">
@@ -15447,10 +15173,8 @@
       <c r="AD151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE151" t="inlineStr">
-        <is>
-          <t>2511</t>
-        </is>
+      <c r="AE151" t="n">
+        <v>2511</v>
       </c>
     </row>
     <row r="152">
@@ -15550,10 +15274,8 @@
       <c r="AD152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE152" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="AE152" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="153">
@@ -15653,10 +15375,8 @@
       <c r="AD153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE153" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="AE153" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="154">
@@ -15756,10 +15476,8 @@
       <c r="AD154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE154" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="AE154" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="155">
@@ -15859,10 +15577,8 @@
       <c r="AD155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE155" t="inlineStr">
-        <is>
-          <t>2918</t>
-        </is>
+      <c r="AE155" t="n">
+        <v>2918</v>
       </c>
     </row>
     <row r="156">
@@ -15956,10 +15672,8 @@
       <c r="AD156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE156" t="inlineStr">
-        <is>
-          <t>3607</t>
-        </is>
+      <c r="AE156" t="n">
+        <v>3607</v>
       </c>
     </row>
     <row r="157">
@@ -16108,10 +15822,8 @@
       <c r="AD158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE158" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="AE158" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="159">
@@ -16205,10 +15917,8 @@
       <c r="AD159" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="AE159" t="inlineStr">
-        <is>
-          <t>3070</t>
-        </is>
+      <c r="AE159" t="n">
+        <v>3070</v>
       </c>
     </row>
     <row r="160">
@@ -16345,10 +16055,8 @@
       <c r="AD161" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AE161" t="inlineStr">
-        <is>
-          <t>3147</t>
-        </is>
+      <c r="AE161" t="n">
+        <v>3147</v>
       </c>
     </row>
     <row r="162">
@@ -16430,10 +16138,8 @@
       <c r="AD162" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="AE162" t="inlineStr">
-        <is>
-          <t>2713</t>
-        </is>
+      <c r="AE162" t="n">
+        <v>2713</v>
       </c>
     </row>
     <row r="163">
@@ -16511,10 +16217,8 @@
       <c r="AD163" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AE163" t="inlineStr">
-        <is>
-          <t>3489</t>
-        </is>
+      <c r="AE163" t="n">
+        <v>3489</v>
       </c>
     </row>
     <row r="164">
@@ -16643,10 +16347,8 @@
       <c r="AD165" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="AE165" t="inlineStr">
-        <is>
-          <t>2856</t>
-        </is>
+      <c r="AE165" t="n">
+        <v>2856</v>
       </c>
     </row>
     <row r="166">
@@ -16704,10 +16406,8 @@
       <c r="AD166" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="AE166" t="inlineStr">
-        <is>
-          <t>3013</t>
-        </is>
+      <c r="AE166" t="n">
+        <v>3013</v>
       </c>
     </row>
     <row r="167">
@@ -16753,10 +16453,8 @@
       <c r="AD167" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE167" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="AE167" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code updated 23-02-26 11:30:34
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE167"/>
+  <dimension ref="A1:AG168"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -546,6 +546,16 @@
           <t>02-24_0</t>
         </is>
       </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>02-25_A</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>02-25_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -646,6 +656,14 @@
       </c>
       <c r="AE2" t="n">
         <v>3995</v>
+      </c>
+      <c r="AF2" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>4203</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -748,6 +766,14 @@
       <c r="AE3" t="n">
         <v>6488</v>
       </c>
+      <c r="AF3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>6828</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -849,6 +875,14 @@
       <c r="AE4" t="n">
         <v>6513</v>
       </c>
+      <c r="AF4" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>6717</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -950,6 +984,14 @@
       <c r="AE5" t="n">
         <v>6013</v>
       </c>
+      <c r="AF5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t>6303</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -1051,6 +1093,14 @@
       <c r="AE6" t="n">
         <v>6115</v>
       </c>
+      <c r="AF6" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>6374</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -1152,6 +1202,14 @@
       <c r="AE7" t="n">
         <v>6772</v>
       </c>
+      <c r="AF7" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="AG7" t="inlineStr">
+        <is>
+          <t>6879</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1253,6 +1311,14 @@
       <c r="AE8" t="n">
         <v>5310</v>
       </c>
+      <c r="AF8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG8" t="inlineStr">
+        <is>
+          <t>5488</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1354,6 +1420,14 @@
       <c r="AE9" t="n">
         <v>5810</v>
       </c>
+      <c r="AF9" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AG9" t="inlineStr">
+        <is>
+          <t>5851</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1455,6 +1529,14 @@
       <c r="AE10" t="n">
         <v>6944</v>
       </c>
+      <c r="AF10" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AG10" t="inlineStr">
+        <is>
+          <t>7171</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1556,6 +1638,14 @@
       <c r="AE11" t="n">
         <v>5566</v>
       </c>
+      <c r="AF11" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AG11" t="inlineStr">
+        <is>
+          <t>6091</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1657,6 +1747,14 @@
       <c r="AE12" t="n">
         <v>2914</v>
       </c>
+      <c r="AF12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1677,7 +1775,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F13" s="5" t="n">
@@ -1757,6 +1855,14 @@
       </c>
       <c r="AE13" t="n">
         <v>6804</v>
+      </c>
+      <c r="AF13" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AG13" t="inlineStr">
+        <is>
+          <t>7163</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -1859,6 +1965,14 @@
       <c r="AE14" t="n">
         <v>5938</v>
       </c>
+      <c r="AF14" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG14" t="inlineStr">
+        <is>
+          <t>6165</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1960,6 +2074,14 @@
       <c r="AE15" t="n">
         <v>5697</v>
       </c>
+      <c r="AF15" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AG15" t="inlineStr">
+        <is>
+          <t>6052</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -2061,6 +2183,14 @@
       <c r="AE16" t="n">
         <v>6360</v>
       </c>
+      <c r="AF16" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AG16" t="inlineStr">
+        <is>
+          <t>6606</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -2162,6 +2292,14 @@
       <c r="AE17" t="n">
         <v>4707</v>
       </c>
+      <c r="AF17" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AG17" t="inlineStr">
+        <is>
+          <t>4798</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -2263,6 +2401,14 @@
       <c r="AE18" t="n">
         <v>4827</v>
       </c>
+      <c r="AF18" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="AG18" t="inlineStr">
+        <is>
+          <t>5186</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -2283,7 +2429,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F19" s="3" t="n">
@@ -2363,6 +2509,14 @@
       </c>
       <c r="AE19" t="n">
         <v>6005</v>
+      </c>
+      <c r="AF19" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG19" t="inlineStr">
+        <is>
+          <t>6238</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -2384,7 +2538,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F20" s="3" t="n">
@@ -2464,6 +2618,14 @@
       </c>
       <c r="AE20" t="n">
         <v>7128</v>
+      </c>
+      <c r="AF20" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AG20" t="inlineStr">
+        <is>
+          <t>7340</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -2566,6 +2728,14 @@
       <c r="AE21" t="n">
         <v>5710</v>
       </c>
+      <c r="AF21" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG21" t="inlineStr">
+        <is>
+          <t>6059</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -2667,6 +2837,14 @@
       <c r="AE22" t="n">
         <v>5648</v>
       </c>
+      <c r="AF22" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AG22" t="inlineStr">
+        <is>
+          <t>5968</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -2768,6 +2946,14 @@
       <c r="AE23" t="n">
         <v>5632</v>
       </c>
+      <c r="AF23" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AG23" t="inlineStr">
+        <is>
+          <t>6067</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -2869,6 +3055,14 @@
       <c r="AE24" t="n">
         <v>6443</v>
       </c>
+      <c r="AF24" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AG24" t="inlineStr">
+        <is>
+          <t>6509</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -2970,6 +3164,14 @@
       <c r="AE25" t="n">
         <v>0</v>
       </c>
+      <c r="AF25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -3071,6 +3273,14 @@
       <c r="AE26" t="n">
         <v>6090</v>
       </c>
+      <c r="AF26" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="AG26" t="inlineStr">
+        <is>
+          <t>6238</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -3172,6 +3382,14 @@
       <c r="AE27" t="n">
         <v>6928</v>
       </c>
+      <c r="AF27" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AG27" t="inlineStr">
+        <is>
+          <t>7162</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -3273,6 +3491,14 @@
       <c r="AE28" t="n">
         <v>6040</v>
       </c>
+      <c r="AF28" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AG28" t="inlineStr">
+        <is>
+          <t>6385</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -3374,6 +3600,14 @@
       <c r="AE29" t="n">
         <v>6924</v>
       </c>
+      <c r="AF29" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AG29" t="inlineStr">
+        <is>
+          <t>7222</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -3475,6 +3709,14 @@
       <c r="AE30" t="n">
         <v>5703</v>
       </c>
+      <c r="AF30" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AG30" t="inlineStr">
+        <is>
+          <t>6157</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -3576,6 +3818,14 @@
       <c r="AE31" t="n">
         <v>6744</v>
       </c>
+      <c r="AF31" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="AG31" t="inlineStr">
+        <is>
+          <t>6670</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -3677,6 +3927,14 @@
       <c r="AE32" t="n">
         <v>6061</v>
       </c>
+      <c r="AF32" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="AG32" t="inlineStr">
+        <is>
+          <t>6647</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -3778,6 +4036,14 @@
       <c r="AE33" t="n">
         <v>6019</v>
       </c>
+      <c r="AF33" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AG33" t="inlineStr">
+        <is>
+          <t>6201</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -3798,7 +4064,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F34" s="3" t="n">
@@ -3878,6 +4144,14 @@
       </c>
       <c r="AE34" t="n">
         <v>5961</v>
+      </c>
+      <c r="AF34" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG34" t="inlineStr">
+        <is>
+          <t>6239</t>
+        </is>
       </c>
     </row>
     <row r="35">
@@ -3980,6 +4254,14 @@
       <c r="AE35" t="n">
         <v>6340</v>
       </c>
+      <c r="AF35" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AG35" t="inlineStr">
+        <is>
+          <t>6503</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -4081,6 +4363,14 @@
       <c r="AE36" t="n">
         <v>5779</v>
       </c>
+      <c r="AF36" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AG36" t="inlineStr">
+        <is>
+          <t>6040</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -4182,6 +4472,14 @@
       <c r="AE37" t="n">
         <v>4623</v>
       </c>
+      <c r="AF37" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="AG37" t="inlineStr">
+        <is>
+          <t>4689</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -4283,6 +4581,14 @@
       <c r="AE38" t="n">
         <v>5990</v>
       </c>
+      <c r="AF38" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AG38" t="inlineStr">
+        <is>
+          <t>6401</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -4384,6 +4690,14 @@
       <c r="AE39" t="n">
         <v>6069</v>
       </c>
+      <c r="AF39" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG39" t="inlineStr">
+        <is>
+          <t>6188</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -4485,6 +4799,14 @@
       <c r="AE40" t="n">
         <v>6888</v>
       </c>
+      <c r="AF40" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="AG40" t="inlineStr">
+        <is>
+          <t>7207</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -4586,6 +4908,14 @@
       <c r="AE41" t="n">
         <v>3648</v>
       </c>
+      <c r="AF41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG41" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -4687,6 +5017,14 @@
       <c r="AE42" t="n">
         <v>7008</v>
       </c>
+      <c r="AF42" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AG42" t="inlineStr">
+        <is>
+          <t>7251</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -4788,6 +5126,14 @@
       <c r="AE43" t="n">
         <v>6246</v>
       </c>
+      <c r="AF43" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AG43" t="inlineStr">
+        <is>
+          <t>6491</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -4889,6 +5235,14 @@
       <c r="AE44" t="n">
         <v>6225</v>
       </c>
+      <c r="AF44" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AG44" t="inlineStr">
+        <is>
+          <t>6306</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -4990,6 +5344,14 @@
       <c r="AE45" t="n">
         <v>5610</v>
       </c>
+      <c r="AF45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG45" t="inlineStr">
+        <is>
+          <t>5624</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -5091,6 +5453,14 @@
       <c r="AE46" t="n">
         <v>5917</v>
       </c>
+      <c r="AF46" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AG46" t="inlineStr">
+        <is>
+          <t>6162</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -5192,6 +5562,14 @@
       <c r="AE47" t="n">
         <v>3526</v>
       </c>
+      <c r="AF47" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG47" t="inlineStr">
+        <is>
+          <t>3859</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -5293,6 +5671,14 @@
       <c r="AE48" t="n">
         <v>6450</v>
       </c>
+      <c r="AF48" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG48" t="inlineStr">
+        <is>
+          <t>6578</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -5394,6 +5780,14 @@
       <c r="AE49" t="n">
         <v>5060</v>
       </c>
+      <c r="AF49" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG49" t="inlineStr">
+        <is>
+          <t>5288</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -5495,6 +5889,14 @@
       <c r="AE50" t="n">
         <v>6842</v>
       </c>
+      <c r="AF50" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AG50" t="inlineStr">
+        <is>
+          <t>6992</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -5596,6 +5998,14 @@
       <c r="AE51" t="n">
         <v>2924</v>
       </c>
+      <c r="AF51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG51" t="inlineStr">
+        <is>
+          <t>2938</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -5697,6 +6107,14 @@
       <c r="AE52" t="n">
         <v>2907</v>
       </c>
+      <c r="AF52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG52" t="inlineStr">
+        <is>
+          <t>3028</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -5798,6 +6216,14 @@
       <c r="AE53" t="n">
         <v>3074</v>
       </c>
+      <c r="AF53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG53" t="inlineStr">
+        <is>
+          <t>3105</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -5899,6 +6325,14 @@
       <c r="AE54" t="n">
         <v>5930</v>
       </c>
+      <c r="AF54" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="AG54" t="inlineStr">
+        <is>
+          <t>6088</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -6000,6 +6434,14 @@
       <c r="AE55" t="n">
         <v>4601</v>
       </c>
+      <c r="AF55" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AG55" t="inlineStr">
+        <is>
+          <t>4613</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -6101,6 +6543,14 @@
       <c r="AE56" t="n">
         <v>4640</v>
       </c>
+      <c r="AF56" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AG56" t="inlineStr">
+        <is>
+          <t>4855</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -6202,6 +6652,14 @@
       <c r="AE57" t="n">
         <v>5551</v>
       </c>
+      <c r="AF57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG57" t="inlineStr">
+        <is>
+          <t>5779</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -6302,6 +6760,14 @@
       </c>
       <c r="AE58" t="n">
         <v>4762</v>
+      </c>
+      <c r="AF58" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AG58" t="inlineStr">
+        <is>
+          <t>4932</t>
+        </is>
       </c>
     </row>
     <row r="59">
@@ -6348,6 +6814,8 @@
       <c r="AC59" t="inlineStr"/>
       <c r="AD59" s="3" t="inlineStr"/>
       <c r="AE59" t="inlineStr"/>
+      <c r="AF59" s="3" t="inlineStr"/>
+      <c r="AG59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -6393,6 +6861,8 @@
       <c r="AC60" t="inlineStr"/>
       <c r="AD60" s="3" t="inlineStr"/>
       <c r="AE60" t="inlineStr"/>
+      <c r="AF60" s="3" t="inlineStr"/>
+      <c r="AG60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -6494,6 +6964,14 @@
       <c r="AE61" t="n">
         <v>5267</v>
       </c>
+      <c r="AF61" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG61" t="inlineStr">
+        <is>
+          <t>5397</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -6595,6 +7073,14 @@
       <c r="AE62" t="n">
         <v>0</v>
       </c>
+      <c r="AF62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG62" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -6696,6 +7182,14 @@
       <c r="AE63" t="n">
         <v>5570</v>
       </c>
+      <c r="AF63" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AG63" t="inlineStr">
+        <is>
+          <t>5720</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -6796,6 +7290,14 @@
       </c>
       <c r="AE64" t="n">
         <v>3258</v>
+      </c>
+      <c r="AF64" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AG64" t="inlineStr">
+        <is>
+          <t>3840</t>
+        </is>
       </c>
     </row>
     <row r="65">
@@ -6842,6 +7344,8 @@
       <c r="AC65" t="inlineStr"/>
       <c r="AD65" s="3" t="inlineStr"/>
       <c r="AE65" t="inlineStr"/>
+      <c r="AF65" s="3" t="inlineStr"/>
+      <c r="AG65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -6943,6 +7447,14 @@
       <c r="AE66" t="n">
         <v>2704</v>
       </c>
+      <c r="AF66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG66" t="inlineStr">
+        <is>
+          <t>2715</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -7044,6 +7556,14 @@
       <c r="AE67" t="n">
         <v>5202</v>
       </c>
+      <c r="AF67" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG67" t="inlineStr">
+        <is>
+          <t>5367</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -7064,7 +7584,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F68" s="5" t="n">
@@ -7144,6 +7664,14 @@
       </c>
       <c r="AE68" t="n">
         <v>6187</v>
+      </c>
+      <c r="AF68" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="AG68" t="inlineStr">
+        <is>
+          <t>6273</t>
+        </is>
       </c>
     </row>
     <row r="69">
@@ -7246,6 +7774,14 @@
       <c r="AE69" t="n">
         <v>4523</v>
       </c>
+      <c r="AF69" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG69" t="inlineStr">
+        <is>
+          <t>4704</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -7347,6 +7883,14 @@
       <c r="AE70" t="n">
         <v>4208</v>
       </c>
+      <c r="AF70" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG70" t="inlineStr">
+        <is>
+          <t>4534</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -7448,6 +7992,14 @@
       <c r="AE71" t="n">
         <v>5094</v>
       </c>
+      <c r="AF71" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="AG71" t="inlineStr">
+        <is>
+          <t>5307</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -7549,6 +8101,14 @@
       <c r="AE72" t="n">
         <v>3832</v>
       </c>
+      <c r="AF72" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG72" t="inlineStr">
+        <is>
+          <t>3938</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -7650,6 +8210,14 @@
       <c r="AE73" t="n">
         <v>4520</v>
       </c>
+      <c r="AF73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG73" t="inlineStr">
+        <is>
+          <t>4670</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -7751,6 +8319,14 @@
       <c r="AE74" t="n">
         <v>4229</v>
       </c>
+      <c r="AF74" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="AG74" t="inlineStr">
+        <is>
+          <t>4510</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -7852,6 +8428,14 @@
       <c r="AE75" t="n">
         <v>4384</v>
       </c>
+      <c r="AF75" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG75" t="inlineStr">
+        <is>
+          <t>4560</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -7953,6 +8537,14 @@
       <c r="AE76" t="n">
         <v>5333</v>
       </c>
+      <c r="AF76" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG76" t="inlineStr">
+        <is>
+          <t>5556</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -8054,6 +8646,14 @@
       <c r="AE77" t="n">
         <v>3383</v>
       </c>
+      <c r="AF77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG77" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -8155,6 +8755,14 @@
       <c r="AE78" t="n">
         <v>5301</v>
       </c>
+      <c r="AF78" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="AG78" t="inlineStr">
+        <is>
+          <t>5402</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -8256,6 +8864,14 @@
       <c r="AE79" t="n">
         <v>0</v>
       </c>
+      <c r="AF79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG79" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -8357,6 +8973,14 @@
       <c r="AE80" t="n">
         <v>5142</v>
       </c>
+      <c r="AF80" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG80" t="inlineStr">
+        <is>
+          <t>5395</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -8458,6 +9082,14 @@
       <c r="AE81" t="n">
         <v>5115</v>
       </c>
+      <c r="AF81" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AG81" t="inlineStr">
+        <is>
+          <t>5191</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -8559,6 +9191,14 @@
       <c r="AE82" t="n">
         <v>4945</v>
       </c>
+      <c r="AF82" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG82" t="inlineStr">
+        <is>
+          <t>5195</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -8660,6 +9300,14 @@
       <c r="AE83" t="n">
         <v>4680</v>
       </c>
+      <c r="AF83" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG83" t="inlineStr">
+        <is>
+          <t>4834</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -8761,6 +9409,14 @@
       <c r="AE84" t="n">
         <v>2968</v>
       </c>
+      <c r="AF84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG84" t="inlineStr">
+        <is>
+          <t>2991</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -8862,6 +9518,14 @@
       <c r="AE85" t="n">
         <v>3949</v>
       </c>
+      <c r="AF85" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AG85" t="inlineStr">
+        <is>
+          <t>4081</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -8963,6 +9627,14 @@
       <c r="AE86" t="n">
         <v>3550</v>
       </c>
+      <c r="AF86" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG86" t="inlineStr">
+        <is>
+          <t>3852</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -9064,6 +9736,14 @@
       <c r="AE87" t="n">
         <v>4962</v>
       </c>
+      <c r="AF87" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG87" t="inlineStr">
+        <is>
+          <t>5123</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -9165,6 +9845,14 @@
       <c r="AE88" t="n">
         <v>3048</v>
       </c>
+      <c r="AF88" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG88" t="inlineStr">
+        <is>
+          <t>3077</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -9266,6 +9954,14 @@
       <c r="AE89" t="n">
         <v>3453</v>
       </c>
+      <c r="AF89" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="AG89" t="inlineStr">
+        <is>
+          <t>3552</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -9367,6 +10063,14 @@
       <c r="AE90" t="n">
         <v>2815</v>
       </c>
+      <c r="AF90" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG90" t="inlineStr">
+        <is>
+          <t>2976</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -9468,6 +10172,14 @@
       <c r="AE91" t="n">
         <v>2943</v>
       </c>
+      <c r="AF91" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="AG91" t="inlineStr">
+        <is>
+          <t>3006</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -9569,6 +10281,14 @@
       <c r="AE92" t="n">
         <v>0</v>
       </c>
+      <c r="AF92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG92" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -9670,6 +10390,14 @@
       <c r="AE93" t="n">
         <v>2586</v>
       </c>
+      <c r="AF93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG93" t="inlineStr">
+        <is>
+          <t>2562</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -9771,6 +10499,14 @@
       <c r="AE94" t="n">
         <v>3265</v>
       </c>
+      <c r="AF94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG94" t="inlineStr">
+        <is>
+          <t>3284</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -9872,6 +10608,14 @@
       <c r="AE95" t="n">
         <v>2500</v>
       </c>
+      <c r="AF95" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AG95" t="inlineStr">
+        <is>
+          <t>2578</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -9973,6 +10717,14 @@
       <c r="AE96" t="n">
         <v>3877</v>
       </c>
+      <c r="AF96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG96" t="inlineStr">
+        <is>
+          <t>3853</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -10074,6 +10826,14 @@
       <c r="AE97" t="n">
         <v>3111</v>
       </c>
+      <c r="AF97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG97" t="inlineStr">
+        <is>
+          <t>3108</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -10175,6 +10935,14 @@
       <c r="AE98" t="n">
         <v>0</v>
       </c>
+      <c r="AF98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG98" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -10276,6 +11044,14 @@
       <c r="AE99" t="n">
         <v>4130</v>
       </c>
+      <c r="AF99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG99" t="inlineStr">
+        <is>
+          <t>4113</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -10377,6 +11153,14 @@
       <c r="AE100" t="n">
         <v>2781</v>
       </c>
+      <c r="AF100" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="AG100" t="inlineStr">
+        <is>
+          <t>2869</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
@@ -10478,6 +11262,14 @@
       <c r="AE101" t="n">
         <v>4725</v>
       </c>
+      <c r="AF101" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AG101" t="inlineStr">
+        <is>
+          <t>4817</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
@@ -10579,6 +11371,14 @@
       <c r="AE102" t="n">
         <v>4155</v>
       </c>
+      <c r="AF102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG102" t="inlineStr">
+        <is>
+          <t>4227</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
@@ -10680,6 +11480,14 @@
       <c r="AE103" t="n">
         <v>3596</v>
       </c>
+      <c r="AF103" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG103" t="inlineStr">
+        <is>
+          <t>3884</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
@@ -10781,6 +11589,14 @@
       <c r="AE104" t="n">
         <v>4721</v>
       </c>
+      <c r="AF104" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="AG104" t="inlineStr">
+        <is>
+          <t>4732</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -10882,6 +11698,14 @@
       <c r="AE105" t="n">
         <v>4347</v>
       </c>
+      <c r="AF105" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG105" t="inlineStr">
+        <is>
+          <t>4481</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -10983,6 +11807,14 @@
       <c r="AE106" t="n">
         <v>0</v>
       </c>
+      <c r="AF106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG106" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -11084,6 +11916,14 @@
       <c r="AE107" t="n">
         <v>2529</v>
       </c>
+      <c r="AF107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG107" t="inlineStr">
+        <is>
+          <t>2553</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -11185,6 +12025,14 @@
       <c r="AE108" t="n">
         <v>0</v>
       </c>
+      <c r="AF108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG108" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -11286,6 +12134,14 @@
       <c r="AE109" t="n">
         <v>3916</v>
       </c>
+      <c r="AF109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG109" t="inlineStr">
+        <is>
+          <t>4134</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -11387,6 +12243,14 @@
       <c r="AE110" t="n">
         <v>3765</v>
       </c>
+      <c r="AF110" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AG110" t="inlineStr">
+        <is>
+          <t>3767</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -11488,6 +12352,14 @@
       <c r="AE111" t="n">
         <v>2781</v>
       </c>
+      <c r="AF111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG111" t="inlineStr">
+        <is>
+          <t>2803</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -11589,6 +12461,14 @@
       <c r="AE112" t="n">
         <v>3513</v>
       </c>
+      <c r="AF112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG112" t="inlineStr">
+        <is>
+          <t>3505</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -11690,6 +12570,14 @@
       <c r="AE113" t="n">
         <v>3727</v>
       </c>
+      <c r="AF113" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="AG113" t="inlineStr">
+        <is>
+          <t>3700</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -11791,6 +12679,14 @@
       <c r="AE114" t="n">
         <v>3259</v>
       </c>
+      <c r="AF114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG114" t="inlineStr">
+        <is>
+          <t>3301</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -11892,6 +12788,14 @@
       <c r="AE115" t="n">
         <v>2303</v>
       </c>
+      <c r="AF115" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG115" t="inlineStr">
+        <is>
+          <t>2306</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -11993,6 +12897,14 @@
       <c r="AE116" t="n">
         <v>3333</v>
       </c>
+      <c r="AF116" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="AG116" t="inlineStr">
+        <is>
+          <t>3427</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -12094,6 +13006,14 @@
       <c r="AE117" t="n">
         <v>3638</v>
       </c>
+      <c r="AF117" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG117" t="inlineStr">
+        <is>
+          <t>3939</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -12195,6 +13115,14 @@
       <c r="AE118" t="n">
         <v>0</v>
       </c>
+      <c r="AF118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG118" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -12296,6 +13224,14 @@
       <c r="AE119" t="n">
         <v>4239</v>
       </c>
+      <c r="AF119" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AG119" t="inlineStr">
+        <is>
+          <t>4345</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
@@ -12397,6 +13333,14 @@
       <c r="AE120" t="n">
         <v>2556</v>
       </c>
+      <c r="AF120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG120" t="inlineStr">
+        <is>
+          <t>2550</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
@@ -12498,6 +13442,14 @@
       <c r="AE121" t="n">
         <v>3807</v>
       </c>
+      <c r="AF121" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AG121" t="inlineStr">
+        <is>
+          <t>3920</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
@@ -12599,6 +13551,14 @@
       <c r="AE122" t="n">
         <v>0</v>
       </c>
+      <c r="AF122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG122" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
@@ -12700,6 +13660,14 @@
       <c r="AE123" t="n">
         <v>3426</v>
       </c>
+      <c r="AF123" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG123" t="inlineStr">
+        <is>
+          <t>3564</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -12801,6 +13769,14 @@
       <c r="AE124" t="n">
         <v>3445</v>
       </c>
+      <c r="AF124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG124" t="inlineStr">
+        <is>
+          <t>3463</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -12902,6 +13878,14 @@
       <c r="AE125" t="n">
         <v>3805</v>
       </c>
+      <c r="AF125" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG125" t="inlineStr">
+        <is>
+          <t>3856</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
@@ -13003,6 +13987,14 @@
       <c r="AE126" t="n">
         <v>3519</v>
       </c>
+      <c r="AF126" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG126" t="inlineStr">
+        <is>
+          <t>3517</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
@@ -13104,6 +14096,14 @@
       <c r="AE127" t="n">
         <v>2341</v>
       </c>
+      <c r="AF127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG127" t="inlineStr">
+        <is>
+          <t>2336</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -13205,6 +14205,14 @@
       <c r="AE128" t="n">
         <v>0</v>
       </c>
+      <c r="AF128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG128" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -13306,6 +14314,14 @@
       <c r="AE129" t="n">
         <v>0</v>
       </c>
+      <c r="AF129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG129" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -13407,6 +14423,14 @@
       <c r="AE130" t="n">
         <v>2981</v>
       </c>
+      <c r="AF130" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG130" t="inlineStr">
+        <is>
+          <t>3037</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
@@ -13508,6 +14532,14 @@
       <c r="AE131" t="n">
         <v>2575</v>
       </c>
+      <c r="AF131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG131" t="inlineStr">
+        <is>
+          <t>2586</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
@@ -13609,6 +14641,14 @@
       <c r="AE132" t="n">
         <v>2754</v>
       </c>
+      <c r="AF132" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG132" t="inlineStr">
+        <is>
+          <t>2822</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
@@ -13709,6 +14749,14 @@
       </c>
       <c r="AE133" t="n">
         <v>2901</v>
+      </c>
+      <c r="AF133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG133" t="inlineStr">
+        <is>
+          <t>2935</t>
+        </is>
       </c>
     </row>
     <row r="134">
@@ -13779,6 +14827,8 @@
       <c r="AC134" t="inlineStr"/>
       <c r="AD134" s="3" t="inlineStr"/>
       <c r="AE134" t="inlineStr"/>
+      <c r="AF134" s="3" t="inlineStr"/>
+      <c r="AG134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -13840,6 +14890,8 @@
       <c r="AC135" t="inlineStr"/>
       <c r="AD135" s="3" t="inlineStr"/>
       <c r="AE135" t="inlineStr"/>
+      <c r="AF135" s="3" t="inlineStr"/>
+      <c r="AG135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -13941,6 +14993,14 @@
       <c r="AE136" t="n">
         <v>2681</v>
       </c>
+      <c r="AF136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG136" t="inlineStr">
+        <is>
+          <t>2676</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
@@ -14041,6 +15101,14 @@
       </c>
       <c r="AE137" t="n">
         <v>2556</v>
+      </c>
+      <c r="AF137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG137" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="138">
@@ -14103,6 +15171,8 @@
       <c r="AC138" t="inlineStr"/>
       <c r="AD138" s="3" t="inlineStr"/>
       <c r="AE138" t="inlineStr"/>
+      <c r="AF138" s="3" t="inlineStr"/>
+      <c r="AG138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -14204,6 +15274,14 @@
       <c r="AE139" t="n">
         <v>2395</v>
       </c>
+      <c r="AF139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG139" t="inlineStr">
+        <is>
+          <t>2432</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -14304,6 +15382,14 @@
       </c>
       <c r="AE140" t="n">
         <v>3045</v>
+      </c>
+      <c r="AF140" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG140" t="inlineStr">
+        <is>
+          <t>3167</t>
+        </is>
       </c>
     </row>
     <row r="141">
@@ -14366,6 +15452,8 @@
       <c r="AC141" t="inlineStr"/>
       <c r="AD141" s="3" t="inlineStr"/>
       <c r="AE141" t="inlineStr"/>
+      <c r="AF141" s="3" t="inlineStr"/>
+      <c r="AG141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -14466,6 +15554,14 @@
       </c>
       <c r="AE142" t="n">
         <v>2255</v>
+      </c>
+      <c r="AF142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG142" t="inlineStr">
+        <is>
+          <t>2303</t>
+        </is>
       </c>
     </row>
     <row r="143">
@@ -14528,6 +15624,8 @@
       <c r="AC143" t="inlineStr"/>
       <c r="AD143" s="3" t="inlineStr"/>
       <c r="AE143" t="inlineStr"/>
+      <c r="AF143" s="3" t="inlineStr"/>
+      <c r="AG143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -14589,6 +15687,8 @@
       <c r="AC144" t="inlineStr"/>
       <c r="AD144" s="3" t="inlineStr"/>
       <c r="AE144" t="inlineStr"/>
+      <c r="AF144" s="3" t="inlineStr"/>
+      <c r="AG144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -14650,6 +15750,8 @@
       <c r="AC145" t="inlineStr"/>
       <c r="AD145" s="3" t="inlineStr"/>
       <c r="AE145" t="inlineStr"/>
+      <c r="AF145" s="3" t="inlineStr"/>
+      <c r="AG145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -14711,6 +15813,8 @@
       <c r="AC146" t="inlineStr"/>
       <c r="AD146" s="3" t="inlineStr"/>
       <c r="AE146" t="inlineStr"/>
+      <c r="AF146" s="3" t="inlineStr"/>
+      <c r="AG146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -14772,6 +15876,8 @@
       <c r="AC147" t="inlineStr"/>
       <c r="AD147" s="3" t="inlineStr"/>
       <c r="AE147" t="inlineStr"/>
+      <c r="AF147" s="3" t="inlineStr"/>
+      <c r="AG147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -14873,6 +15979,14 @@
       <c r="AE148" t="n">
         <v>1524</v>
       </c>
+      <c r="AF148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG148" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -14974,6 +16088,14 @@
       <c r="AE149" t="n">
         <v>3849</v>
       </c>
+      <c r="AF149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG149" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -15075,6 +16197,14 @@
       <c r="AE150" t="n">
         <v>0</v>
       </c>
+      <c r="AF150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG150" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
@@ -15176,6 +16306,14 @@
       <c r="AE151" t="n">
         <v>2511</v>
       </c>
+      <c r="AF151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG151" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
@@ -15277,6 +16415,14 @@
       <c r="AE152" t="n">
         <v>0</v>
       </c>
+      <c r="AF152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG152" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
@@ -15378,6 +16524,14 @@
       <c r="AE153" t="n">
         <v>0</v>
       </c>
+      <c r="AF153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG153" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
@@ -15479,6 +16633,14 @@
       <c r="AE154" t="n">
         <v>0</v>
       </c>
+      <c r="AF154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG154" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
@@ -15580,6 +16742,14 @@
       <c r="AE155" t="n">
         <v>2918</v>
       </c>
+      <c r="AF155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG155" t="inlineStr">
+        <is>
+          <t>2917</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
@@ -15674,6 +16844,14 @@
       </c>
       <c r="AE156" t="n">
         <v>3607</v>
+      </c>
+      <c r="AF156" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG156" t="inlineStr">
+        <is>
+          <t>3773</t>
+        </is>
       </c>
     </row>
     <row r="157">
@@ -15730,6 +16908,8 @@
       <c r="AC157" t="inlineStr"/>
       <c r="AD157" s="3" t="inlineStr"/>
       <c r="AE157" t="inlineStr"/>
+      <c r="AF157" s="3" t="inlineStr"/>
+      <c r="AG157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -15825,6 +17005,14 @@
       <c r="AE158" t="n">
         <v>0</v>
       </c>
+      <c r="AF158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG158" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="n">
@@ -15919,6 +17107,14 @@
       </c>
       <c r="AE159" t="n">
         <v>3070</v>
+      </c>
+      <c r="AF159" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AG159" t="inlineStr">
+        <is>
+          <t>3110</t>
+        </is>
       </c>
     </row>
     <row r="160">
@@ -15975,6 +17171,8 @@
       <c r="AC160" t="inlineStr"/>
       <c r="AD160" s="3" t="inlineStr"/>
       <c r="AE160" t="inlineStr"/>
+      <c r="AF160" s="3" t="inlineStr"/>
+      <c r="AG160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -16058,6 +17256,14 @@
       <c r="AE161" t="n">
         <v>3147</v>
       </c>
+      <c r="AF161" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="AG161" t="inlineStr">
+        <is>
+          <t>3226</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="n">
@@ -16140,6 +17346,14 @@
       </c>
       <c r="AE162" t="n">
         <v>2713</v>
+      </c>
+      <c r="AF162" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="AG162" t="inlineStr">
+        <is>
+          <t>2820</t>
+        </is>
       </c>
     </row>
     <row r="163">
@@ -16220,6 +17434,14 @@
       <c r="AE163" t="n">
         <v>3489</v>
       </c>
+      <c r="AF163" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG163" t="inlineStr">
+        <is>
+          <t>3764</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="n">
@@ -16234,7 +17456,7 @@
       <c r="D164" t="inlineStr"/>
       <c r="E164" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F164" s="3" t="inlineStr"/>
@@ -16283,6 +17505,14 @@
       </c>
       <c r="AD164" s="3" t="inlineStr"/>
       <c r="AE164" t="inlineStr"/>
+      <c r="AF164" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AG164" t="inlineStr">
+        <is>
+          <t>3798</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="n">
@@ -16349,6 +17579,14 @@
       </c>
       <c r="AE165" t="n">
         <v>2856</v>
+      </c>
+      <c r="AF165" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG165" t="inlineStr">
+        <is>
+          <t>2846</t>
+        </is>
       </c>
     </row>
     <row r="166">
@@ -16408,6 +17646,14 @@
       </c>
       <c r="AE166" t="n">
         <v>3013</v>
+      </c>
+      <c r="AF166" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG166" t="inlineStr">
+        <is>
+          <t>3325</t>
+        </is>
       </c>
     </row>
     <row r="167">
@@ -16456,6 +17702,67 @@
       <c r="AE167" t="n">
         <v>0</v>
       </c>
+      <c r="AF167" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG167" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>55745105</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>eldeniz</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr"/>
+      <c r="D168" t="inlineStr"/>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F168" s="3" t="inlineStr"/>
+      <c r="G168" t="inlineStr"/>
+      <c r="H168" s="3" t="inlineStr"/>
+      <c r="I168" t="inlineStr"/>
+      <c r="J168" s="3" t="inlineStr"/>
+      <c r="K168" t="inlineStr"/>
+      <c r="L168" s="3" t="inlineStr"/>
+      <c r="M168" t="inlineStr"/>
+      <c r="N168" s="3" t="inlineStr"/>
+      <c r="O168" t="inlineStr"/>
+      <c r="P168" s="3" t="inlineStr"/>
+      <c r="Q168" t="inlineStr"/>
+      <c r="R168" s="3" t="inlineStr"/>
+      <c r="S168" t="inlineStr"/>
+      <c r="T168" s="3" t="inlineStr"/>
+      <c r="U168" t="inlineStr"/>
+      <c r="V168" s="3" t="inlineStr"/>
+      <c r="W168" t="inlineStr"/>
+      <c r="X168" s="3" t="inlineStr"/>
+      <c r="Y168" t="inlineStr"/>
+      <c r="Z168" s="3" t="inlineStr"/>
+      <c r="AA168" t="inlineStr"/>
+      <c r="AB168" s="3" t="inlineStr"/>
+      <c r="AC168" t="inlineStr"/>
+      <c r="AD168" s="3" t="inlineStr"/>
+      <c r="AE168" t="inlineStr"/>
+      <c r="AF168" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG168" t="inlineStr">
+        <is>
+          <t>1438</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Code updated 23-02-27 11:30:39
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG168"/>
+  <dimension ref="A1:AI170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -556,6 +556,16 @@
           <t>02-25_0</t>
         </is>
       </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>02-26_A</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>02-26_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -660,9 +670,15 @@
       <c r="AF2" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AG2" t="inlineStr">
-        <is>
-          <t>4203</t>
+      <c r="AG2" t="n">
+        <v>4203</v>
+      </c>
+      <c r="AH2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI2" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -769,9 +785,15 @@
       <c r="AF3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AG3" t="inlineStr">
-        <is>
-          <t>6828</t>
+      <c r="AG3" t="n">
+        <v>6828</v>
+      </c>
+      <c r="AH3" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t>2747</t>
         </is>
       </c>
     </row>
@@ -878,9 +900,15 @@
       <c r="AF4" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AG4" t="inlineStr">
-        <is>
-          <t>6717</t>
+      <c r="AG4" t="n">
+        <v>6717</v>
+      </c>
+      <c r="AH4" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AI4" t="inlineStr">
+        <is>
+          <t>2996</t>
         </is>
       </c>
     </row>
@@ -987,9 +1015,15 @@
       <c r="AF5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AG5" t="inlineStr">
-        <is>
-          <t>6303</t>
+      <c r="AG5" t="n">
+        <v>6303</v>
+      </c>
+      <c r="AH5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI5" t="inlineStr">
+        <is>
+          <t>2762</t>
         </is>
       </c>
     </row>
@@ -1096,9 +1130,15 @@
       <c r="AF6" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AG6" t="inlineStr">
-        <is>
-          <t>6374</t>
+      <c r="AG6" t="n">
+        <v>6374</v>
+      </c>
+      <c r="AH6" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI6" t="inlineStr">
+        <is>
+          <t>2808</t>
         </is>
       </c>
     </row>
@@ -1205,9 +1245,15 @@
       <c r="AF7" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="AG7" t="inlineStr">
-        <is>
-          <t>6879</t>
+      <c r="AG7" t="n">
+        <v>6879</v>
+      </c>
+      <c r="AH7" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AI7" t="inlineStr">
+        <is>
+          <t>3002</t>
         </is>
       </c>
     </row>
@@ -1314,9 +1360,15 @@
       <c r="AF8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AG8" t="inlineStr">
-        <is>
-          <t>5488</t>
+      <c r="AG8" t="n">
+        <v>5488</v>
+      </c>
+      <c r="AH8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI8" t="inlineStr">
+        <is>
+          <t>2694</t>
         </is>
       </c>
     </row>
@@ -1423,9 +1475,15 @@
       <c r="AF9" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AG9" t="inlineStr">
-        <is>
-          <t>5851</t>
+      <c r="AG9" t="n">
+        <v>5851</v>
+      </c>
+      <c r="AH9" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AI9" t="inlineStr">
+        <is>
+          <t>2912</t>
         </is>
       </c>
     </row>
@@ -1532,9 +1590,15 @@
       <c r="AF10" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AG10" t="inlineStr">
-        <is>
-          <t>7171</t>
+      <c r="AG10" t="n">
+        <v>7171</v>
+      </c>
+      <c r="AH10" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AI10" t="inlineStr">
+        <is>
+          <t>2897</t>
         </is>
       </c>
     </row>
@@ -1641,9 +1705,15 @@
       <c r="AF11" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AG11" t="inlineStr">
-        <is>
-          <t>6091</t>
+      <c r="AG11" t="n">
+        <v>6091</v>
+      </c>
+      <c r="AH11" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI11" t="inlineStr">
+        <is>
+          <t>2799</t>
         </is>
       </c>
     </row>
@@ -1750,9 +1820,15 @@
       <c r="AF12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG12" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="AG12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI12" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -1859,9 +1935,15 @@
       <c r="AF13" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AG13" t="inlineStr">
-        <is>
-          <t>7163</t>
+      <c r="AG13" t="n">
+        <v>7163</v>
+      </c>
+      <c r="AH13" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AI13" t="inlineStr">
+        <is>
+          <t>3027</t>
         </is>
       </c>
     </row>
@@ -1968,9 +2050,15 @@
       <c r="AF14" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AG14" t="inlineStr">
-        <is>
-          <t>6165</t>
+      <c r="AG14" t="n">
+        <v>6165</v>
+      </c>
+      <c r="AH14" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AI14" t="inlineStr">
+        <is>
+          <t>2835</t>
         </is>
       </c>
     </row>
@@ -2077,9 +2165,15 @@
       <c r="AF15" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="AG15" t="inlineStr">
-        <is>
-          <t>6052</t>
+      <c r="AG15" t="n">
+        <v>6052</v>
+      </c>
+      <c r="AH15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI15" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -2186,9 +2280,15 @@
       <c r="AF16" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AG16" t="inlineStr">
-        <is>
-          <t>6606</t>
+      <c r="AG16" t="n">
+        <v>6606</v>
+      </c>
+      <c r="AH16" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="AI16" t="inlineStr">
+        <is>
+          <t>2938</t>
         </is>
       </c>
     </row>
@@ -2295,9 +2395,15 @@
       <c r="AF17" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AG17" t="inlineStr">
-        <is>
-          <t>4798</t>
+      <c r="AG17" t="n">
+        <v>4798</v>
+      </c>
+      <c r="AH17" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AI17" t="inlineStr">
+        <is>
+          <t>2742</t>
         </is>
       </c>
     </row>
@@ -2404,9 +2510,15 @@
       <c r="AF18" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="AG18" t="inlineStr">
-        <is>
-          <t>5186</t>
+      <c r="AG18" t="n">
+        <v>5186</v>
+      </c>
+      <c r="AH18" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AI18" t="inlineStr">
+        <is>
+          <t>2764</t>
         </is>
       </c>
     </row>
@@ -2513,9 +2625,15 @@
       <c r="AF19" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AG19" t="inlineStr">
-        <is>
-          <t>6238</t>
+      <c r="AG19" t="n">
+        <v>6238</v>
+      </c>
+      <c r="AH19" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AI19" t="inlineStr">
+        <is>
+          <t>2926</t>
         </is>
       </c>
     </row>
@@ -2622,9 +2740,15 @@
       <c r="AF20" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AG20" t="inlineStr">
-        <is>
-          <t>7340</t>
+      <c r="AG20" t="n">
+        <v>7340</v>
+      </c>
+      <c r="AH20" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AI20" t="inlineStr">
+        <is>
+          <t>3107</t>
         </is>
       </c>
     </row>
@@ -2731,9 +2855,15 @@
       <c r="AF21" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AG21" t="inlineStr">
-        <is>
-          <t>6059</t>
+      <c r="AG21" t="n">
+        <v>6059</v>
+      </c>
+      <c r="AH21" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI21" t="inlineStr">
+        <is>
+          <t>2781</t>
         </is>
       </c>
     </row>
@@ -2840,9 +2970,15 @@
       <c r="AF22" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AG22" t="inlineStr">
-        <is>
-          <t>5968</t>
+      <c r="AG22" t="n">
+        <v>5968</v>
+      </c>
+      <c r="AH22" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="AI22" t="inlineStr">
+        <is>
+          <t>2714</t>
         </is>
       </c>
     </row>
@@ -2949,9 +3085,15 @@
       <c r="AF23" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AG23" t="inlineStr">
-        <is>
-          <t>6067</t>
+      <c r="AG23" t="n">
+        <v>6067</v>
+      </c>
+      <c r="AH23" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="AI23" t="inlineStr">
+        <is>
+          <t>2667</t>
         </is>
       </c>
     </row>
@@ -3058,9 +3200,15 @@
       <c r="AF24" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AG24" t="inlineStr">
-        <is>
-          <t>6509</t>
+      <c r="AG24" t="n">
+        <v>6509</v>
+      </c>
+      <c r="AH24" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AI24" t="inlineStr">
+        <is>
+          <t>2924</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3315,13 @@
       <c r="AF25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG25" t="inlineStr">
+      <c r="AG25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3276,9 +3430,15 @@
       <c r="AF26" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="AG26" t="inlineStr">
-        <is>
-          <t>6238</t>
+      <c r="AG26" t="n">
+        <v>6238</v>
+      </c>
+      <c r="AH26" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="AI26" t="inlineStr">
+        <is>
+          <t>3019</t>
         </is>
       </c>
     </row>
@@ -3385,9 +3545,15 @@
       <c r="AF27" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AG27" t="inlineStr">
-        <is>
-          <t>7162</t>
+      <c r="AG27" t="n">
+        <v>7162</v>
+      </c>
+      <c r="AH27" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="AI27" t="inlineStr">
+        <is>
+          <t>2900</t>
         </is>
       </c>
     </row>
@@ -3494,9 +3660,15 @@
       <c r="AF28" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="AG28" t="inlineStr">
-        <is>
-          <t>6385</t>
+      <c r="AG28" t="n">
+        <v>6385</v>
+      </c>
+      <c r="AH28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="AI28" t="inlineStr">
+        <is>
+          <t>2802</t>
         </is>
       </c>
     </row>
@@ -3603,9 +3775,15 @@
       <c r="AF29" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AG29" t="inlineStr">
-        <is>
-          <t>7222</t>
+      <c r="AG29" t="n">
+        <v>7222</v>
+      </c>
+      <c r="AH29" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AI29" t="inlineStr">
+        <is>
+          <t>3227</t>
         </is>
       </c>
     </row>
@@ -3712,9 +3890,15 @@
       <c r="AF30" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AG30" t="inlineStr">
-        <is>
-          <t>6157</t>
+      <c r="AG30" t="n">
+        <v>6157</v>
+      </c>
+      <c r="AH30" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AI30" t="inlineStr">
+        <is>
+          <t>2796</t>
         </is>
       </c>
     </row>
@@ -3821,9 +4005,15 @@
       <c r="AF31" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="AG31" t="inlineStr">
-        <is>
-          <t>6670</t>
+      <c r="AG31" t="n">
+        <v>6670</v>
+      </c>
+      <c r="AH31" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AI31" t="inlineStr">
+        <is>
+          <t>2993</t>
         </is>
       </c>
     </row>
@@ -3846,7 +4036,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F32" s="5" t="n">
@@ -3930,9 +4120,15 @@
       <c r="AF32" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="AG32" t="inlineStr">
-        <is>
-          <t>6647</t>
+      <c r="AG32" t="n">
+        <v>6647</v>
+      </c>
+      <c r="AH32" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AI32" t="inlineStr">
+        <is>
+          <t>2916</t>
         </is>
       </c>
     </row>
@@ -4039,9 +4235,15 @@
       <c r="AF33" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="AG33" t="inlineStr">
-        <is>
-          <t>6201</t>
+      <c r="AG33" t="n">
+        <v>6201</v>
+      </c>
+      <c r="AH33" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI33" t="inlineStr">
+        <is>
+          <t>2783</t>
         </is>
       </c>
     </row>
@@ -4148,9 +4350,15 @@
       <c r="AF34" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AG34" t="inlineStr">
-        <is>
-          <t>6239</t>
+      <c r="AG34" t="n">
+        <v>6239</v>
+      </c>
+      <c r="AH34" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AI34" t="inlineStr">
+        <is>
+          <t>2956</t>
         </is>
       </c>
     </row>
@@ -4257,9 +4465,15 @@
       <c r="AF35" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AG35" t="inlineStr">
-        <is>
-          <t>6503</t>
+      <c r="AG35" t="n">
+        <v>6503</v>
+      </c>
+      <c r="AH35" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AI35" t="inlineStr">
+        <is>
+          <t>2964</t>
         </is>
       </c>
     </row>
@@ -4366,9 +4580,15 @@
       <c r="AF36" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="AG36" t="inlineStr">
-        <is>
-          <t>6040</t>
+      <c r="AG36" t="n">
+        <v>6040</v>
+      </c>
+      <c r="AH36" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="AI36" t="inlineStr">
+        <is>
+          <t>2700</t>
         </is>
       </c>
     </row>
@@ -4475,9 +4695,15 @@
       <c r="AF37" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="AG37" t="inlineStr">
-        <is>
-          <t>4689</t>
+      <c r="AG37" t="n">
+        <v>4689</v>
+      </c>
+      <c r="AH37" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AI37" t="inlineStr">
+        <is>
+          <t>2916</t>
         </is>
       </c>
     </row>
@@ -4584,9 +4810,15 @@
       <c r="AF38" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AG38" t="inlineStr">
-        <is>
-          <t>6401</t>
+      <c r="AG38" t="n">
+        <v>6401</v>
+      </c>
+      <c r="AH38" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AI38" t="inlineStr">
+        <is>
+          <t>2901</t>
         </is>
       </c>
     </row>
@@ -4693,9 +4925,15 @@
       <c r="AF39" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AG39" t="inlineStr">
-        <is>
-          <t>6188</t>
+      <c r="AG39" t="n">
+        <v>6188</v>
+      </c>
+      <c r="AH39" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AI39" t="inlineStr">
+        <is>
+          <t>2900</t>
         </is>
       </c>
     </row>
@@ -4802,9 +5040,15 @@
       <c r="AF40" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="AG40" t="inlineStr">
-        <is>
-          <t>7207</t>
+      <c r="AG40" t="n">
+        <v>7207</v>
+      </c>
+      <c r="AH40" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AI40" t="inlineStr">
+        <is>
+          <t>3048</t>
         </is>
       </c>
     </row>
@@ -4911,7 +5155,13 @@
       <c r="AF41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG41" t="inlineStr">
+      <c r="AG41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI41" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5020,9 +5270,15 @@
       <c r="AF42" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AG42" t="inlineStr">
-        <is>
-          <t>7251</t>
+      <c r="AG42" t="n">
+        <v>7251</v>
+      </c>
+      <c r="AH42" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="AI42" t="inlineStr">
+        <is>
+          <t>2939</t>
         </is>
       </c>
     </row>
@@ -5129,9 +5385,15 @@
       <c r="AF43" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AG43" t="inlineStr">
-        <is>
-          <t>6491</t>
+      <c r="AG43" t="n">
+        <v>6491</v>
+      </c>
+      <c r="AH43" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AI43" t="inlineStr">
+        <is>
+          <t>2959</t>
         </is>
       </c>
     </row>
@@ -5238,9 +5500,15 @@
       <c r="AF44" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AG44" t="inlineStr">
-        <is>
-          <t>6306</t>
+      <c r="AG44" t="n">
+        <v>6306</v>
+      </c>
+      <c r="AH44" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AI44" t="inlineStr">
+        <is>
+          <t>2859</t>
         </is>
       </c>
     </row>
@@ -5347,9 +5615,15 @@
       <c r="AF45" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG45" t="inlineStr">
-        <is>
-          <t>5624</t>
+      <c r="AG45" t="n">
+        <v>5624</v>
+      </c>
+      <c r="AH45" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AI45" t="inlineStr">
+        <is>
+          <t>2834</t>
         </is>
       </c>
     </row>
@@ -5456,9 +5730,15 @@
       <c r="AF46" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AG46" t="inlineStr">
-        <is>
-          <t>6162</t>
+      <c r="AG46" t="n">
+        <v>6162</v>
+      </c>
+      <c r="AH46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AI46" t="inlineStr">
+        <is>
+          <t>2861</t>
         </is>
       </c>
     </row>
@@ -5565,9 +5845,15 @@
       <c r="AF47" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AG47" t="inlineStr">
-        <is>
-          <t>3859</t>
+      <c r="AG47" t="n">
+        <v>3859</v>
+      </c>
+      <c r="AH47" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AI47" t="inlineStr">
+        <is>
+          <t>2829</t>
         </is>
       </c>
     </row>
@@ -5674,9 +5960,15 @@
       <c r="AF48" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AG48" t="inlineStr">
-        <is>
-          <t>6578</t>
+      <c r="AG48" t="n">
+        <v>6578</v>
+      </c>
+      <c r="AH48" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AI48" t="inlineStr">
+        <is>
+          <t>3033</t>
         </is>
       </c>
     </row>
@@ -5783,9 +6075,15 @@
       <c r="AF49" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AG49" t="inlineStr">
-        <is>
-          <t>5288</t>
+      <c r="AG49" t="n">
+        <v>5288</v>
+      </c>
+      <c r="AH49" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI49" t="inlineStr">
+        <is>
+          <t>2758</t>
         </is>
       </c>
     </row>
@@ -5892,9 +6190,15 @@
       <c r="AF50" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AG50" t="inlineStr">
-        <is>
-          <t>6992</t>
+      <c r="AG50" t="n">
+        <v>6992</v>
+      </c>
+      <c r="AH50" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AI50" t="inlineStr">
+        <is>
+          <t>2836</t>
         </is>
       </c>
     </row>
@@ -6001,9 +6305,15 @@
       <c r="AF51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG51" t="inlineStr">
-        <is>
-          <t>2938</t>
+      <c r="AG51" t="n">
+        <v>2938</v>
+      </c>
+      <c r="AH51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI51" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -6110,9 +6420,15 @@
       <c r="AF52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG52" t="inlineStr">
-        <is>
-          <t>3028</t>
+      <c r="AG52" t="n">
+        <v>3028</v>
+      </c>
+      <c r="AH52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI52" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -6219,9 +6535,15 @@
       <c r="AF53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG53" t="inlineStr">
-        <is>
-          <t>3105</t>
+      <c r="AG53" t="n">
+        <v>3105</v>
+      </c>
+      <c r="AH53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI53" t="inlineStr">
+        <is>
+          <t>2511</t>
         </is>
       </c>
     </row>
@@ -6328,9 +6650,15 @@
       <c r="AF54" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="AG54" t="inlineStr">
-        <is>
-          <t>6088</t>
+      <c r="AG54" t="n">
+        <v>6088</v>
+      </c>
+      <c r="AH54" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AI54" t="inlineStr">
+        <is>
+          <t>3005</t>
         </is>
       </c>
     </row>
@@ -6437,9 +6765,15 @@
       <c r="AF55" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AG55" t="inlineStr">
-        <is>
-          <t>4613</t>
+      <c r="AG55" t="n">
+        <v>4613</v>
+      </c>
+      <c r="AH55" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AI55" t="inlineStr">
+        <is>
+          <t>2701</t>
         </is>
       </c>
     </row>
@@ -6546,9 +6880,15 @@
       <c r="AF56" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AG56" t="inlineStr">
-        <is>
-          <t>4855</t>
+      <c r="AG56" t="n">
+        <v>4855</v>
+      </c>
+      <c r="AH56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI56" t="inlineStr">
+        <is>
+          <t>2701</t>
         </is>
       </c>
     </row>
@@ -6655,9 +6995,15 @@
       <c r="AF57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AG57" t="inlineStr">
-        <is>
-          <t>5779</t>
+      <c r="AG57" t="n">
+        <v>5779</v>
+      </c>
+      <c r="AH57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI57" t="inlineStr">
+        <is>
+          <t>2787</t>
         </is>
       </c>
     </row>
@@ -6764,9 +7110,15 @@
       <c r="AF58" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AG58" t="inlineStr">
-        <is>
-          <t>4932</t>
+      <c r="AG58" t="n">
+        <v>4932</v>
+      </c>
+      <c r="AH58" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AI58" t="inlineStr">
+        <is>
+          <t>2826</t>
         </is>
       </c>
     </row>
@@ -6816,6 +7168,8 @@
       <c r="AE59" t="inlineStr"/>
       <c r="AF59" s="3" t="inlineStr"/>
       <c r="AG59" t="inlineStr"/>
+      <c r="AH59" s="3" t="inlineStr"/>
+      <c r="AI59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -6863,6 +7217,8 @@
       <c r="AE60" t="inlineStr"/>
       <c r="AF60" s="3" t="inlineStr"/>
       <c r="AG60" t="inlineStr"/>
+      <c r="AH60" s="3" t="inlineStr"/>
+      <c r="AI60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -6967,9 +7323,15 @@
       <c r="AF61" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AG61" t="inlineStr">
-        <is>
-          <t>5397</t>
+      <c r="AG61" t="n">
+        <v>5397</v>
+      </c>
+      <c r="AH61" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AI61" t="inlineStr">
+        <is>
+          <t>2836</t>
         </is>
       </c>
     </row>
@@ -7076,7 +7438,13 @@
       <c r="AF62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG62" t="inlineStr">
+      <c r="AG62" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7185,9 +7553,15 @@
       <c r="AF63" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="AG63" t="inlineStr">
-        <is>
-          <t>5720</t>
+      <c r="AG63" t="n">
+        <v>5720</v>
+      </c>
+      <c r="AH63" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AI63" t="inlineStr">
+        <is>
+          <t>2885</t>
         </is>
       </c>
     </row>
@@ -7294,9 +7668,15 @@
       <c r="AF64" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AG64" t="inlineStr">
-        <is>
-          <t>3840</t>
+      <c r="AG64" t="n">
+        <v>3840</v>
+      </c>
+      <c r="AH64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI64" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -7346,6 +7726,8 @@
       <c r="AE65" t="inlineStr"/>
       <c r="AF65" s="3" t="inlineStr"/>
       <c r="AG65" t="inlineStr"/>
+      <c r="AH65" s="3" t="inlineStr"/>
+      <c r="AI65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -7450,9 +7832,15 @@
       <c r="AF66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG66" t="inlineStr">
-        <is>
-          <t>2715</t>
+      <c r="AG66" t="n">
+        <v>2715</v>
+      </c>
+      <c r="AH66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI66" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -7559,9 +7947,15 @@
       <c r="AF67" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AG67" t="inlineStr">
-        <is>
-          <t>5367</t>
+      <c r="AG67" t="n">
+        <v>5367</v>
+      </c>
+      <c r="AH67" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AI67" t="inlineStr">
+        <is>
+          <t>2797</t>
         </is>
       </c>
     </row>
@@ -7668,9 +8062,15 @@
       <c r="AF68" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="AG68" t="inlineStr">
-        <is>
-          <t>6273</t>
+      <c r="AG68" t="n">
+        <v>6273</v>
+      </c>
+      <c r="AH68" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AI68" t="inlineStr">
+        <is>
+          <t>2956</t>
         </is>
       </c>
     </row>
@@ -7777,9 +8177,15 @@
       <c r="AF69" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AG69" t="inlineStr">
-        <is>
-          <t>4704</t>
+      <c r="AG69" t="n">
+        <v>4704</v>
+      </c>
+      <c r="AH69" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AI69" t="inlineStr">
+        <is>
+          <t>2777</t>
         </is>
       </c>
     </row>
@@ -7886,9 +8292,15 @@
       <c r="AF70" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AG70" t="inlineStr">
-        <is>
-          <t>4534</t>
+      <c r="AG70" t="n">
+        <v>4534</v>
+      </c>
+      <c r="AH70" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI70" t="inlineStr">
+        <is>
+          <t>2494</t>
         </is>
       </c>
     </row>
@@ -7995,9 +8407,15 @@
       <c r="AF71" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="AG71" t="inlineStr">
-        <is>
-          <t>5307</t>
+      <c r="AG71" t="n">
+        <v>5307</v>
+      </c>
+      <c r="AH71" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="AI71" t="inlineStr">
+        <is>
+          <t>2705</t>
         </is>
       </c>
     </row>
@@ -8104,9 +8522,15 @@
       <c r="AF72" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="AG72" t="inlineStr">
-        <is>
-          <t>3938</t>
+      <c r="AG72" t="n">
+        <v>3938</v>
+      </c>
+      <c r="AH72" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AI72" t="inlineStr">
+        <is>
+          <t>2510</t>
         </is>
       </c>
     </row>
@@ -8213,9 +8637,15 @@
       <c r="AF73" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AG73" t="inlineStr">
-        <is>
-          <t>4670</t>
+      <c r="AG73" t="n">
+        <v>4670</v>
+      </c>
+      <c r="AH73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI73" t="inlineStr">
+        <is>
+          <t>2712</t>
         </is>
       </c>
     </row>
@@ -8322,9 +8752,15 @@
       <c r="AF74" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="AG74" t="inlineStr">
-        <is>
-          <t>4510</t>
+      <c r="AG74" t="n">
+        <v>4510</v>
+      </c>
+      <c r="AH74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI74" t="inlineStr">
+        <is>
+          <t>2508</t>
         </is>
       </c>
     </row>
@@ -8431,9 +8867,15 @@
       <c r="AF75" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AG75" t="inlineStr">
-        <is>
-          <t>4560</t>
+      <c r="AG75" t="n">
+        <v>4560</v>
+      </c>
+      <c r="AH75" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AI75" t="inlineStr">
+        <is>
+          <t>2749</t>
         </is>
       </c>
     </row>
@@ -8540,9 +8982,15 @@
       <c r="AF76" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AG76" t="inlineStr">
-        <is>
-          <t>5556</t>
+      <c r="AG76" t="n">
+        <v>5556</v>
+      </c>
+      <c r="AH76" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="AI76" t="inlineStr">
+        <is>
+          <t>2797</t>
         </is>
       </c>
     </row>
@@ -8649,7 +9097,13 @@
       <c r="AF77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG77" t="inlineStr">
+      <c r="AG77" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI77" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8758,9 +9212,15 @@
       <c r="AF78" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="AG78" t="inlineStr">
-        <is>
-          <t>5402</t>
+      <c r="AG78" t="n">
+        <v>5402</v>
+      </c>
+      <c r="AH78" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AI78" t="inlineStr">
+        <is>
+          <t>2866</t>
         </is>
       </c>
     </row>
@@ -8867,7 +9327,13 @@
       <c r="AF79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG79" t="inlineStr">
+      <c r="AG79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8976,9 +9442,15 @@
       <c r="AF80" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AG80" t="inlineStr">
-        <is>
-          <t>5395</t>
+      <c r="AG80" t="n">
+        <v>5395</v>
+      </c>
+      <c r="AH80" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="AI80" t="inlineStr">
+        <is>
+          <t>2794</t>
         </is>
       </c>
     </row>
@@ -9085,9 +9557,15 @@
       <c r="AF81" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AG81" t="inlineStr">
-        <is>
-          <t>5191</t>
+      <c r="AG81" t="n">
+        <v>5191</v>
+      </c>
+      <c r="AH81" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AI81" t="inlineStr">
+        <is>
+          <t>2942</t>
         </is>
       </c>
     </row>
@@ -9194,9 +9672,15 @@
       <c r="AF82" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AG82" t="inlineStr">
-        <is>
-          <t>5195</t>
+      <c r="AG82" t="n">
+        <v>5195</v>
+      </c>
+      <c r="AH82" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AI82" t="inlineStr">
+        <is>
+          <t>2845</t>
         </is>
       </c>
     </row>
@@ -9303,9 +9787,15 @@
       <c r="AF83" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AG83" t="inlineStr">
-        <is>
-          <t>4834</t>
+      <c r="AG83" t="n">
+        <v>4834</v>
+      </c>
+      <c r="AH83" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AI83" t="inlineStr">
+        <is>
+          <t>2863</t>
         </is>
       </c>
     </row>
@@ -9412,11 +9902,11 @@
       <c r="AF84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG84" t="inlineStr">
-        <is>
-          <t>2991</t>
-        </is>
-      </c>
+      <c r="AG84" t="n">
+        <v>2991</v>
+      </c>
+      <c r="AH84" s="3" t="inlineStr"/>
+      <c r="AI84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -9521,9 +10011,15 @@
       <c r="AF85" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AG85" t="inlineStr">
-        <is>
-          <t>4081</t>
+      <c r="AG85" t="n">
+        <v>4081</v>
+      </c>
+      <c r="AH85" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI85" t="inlineStr">
+        <is>
+          <t>2805</t>
         </is>
       </c>
     </row>
@@ -9630,9 +10126,15 @@
       <c r="AF86" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AG86" t="inlineStr">
-        <is>
-          <t>3852</t>
+      <c r="AG86" t="n">
+        <v>3852</v>
+      </c>
+      <c r="AH86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI86" t="inlineStr">
+        <is>
+          <t>2485</t>
         </is>
       </c>
     </row>
@@ -9739,9 +10241,15 @@
       <c r="AF87" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AG87" t="inlineStr">
-        <is>
-          <t>5123</t>
+      <c r="AG87" t="n">
+        <v>5123</v>
+      </c>
+      <c r="AH87" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI87" t="inlineStr">
+        <is>
+          <t>2856</t>
         </is>
       </c>
     </row>
@@ -9848,9 +10356,15 @@
       <c r="AF88" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AG88" t="inlineStr">
-        <is>
-          <t>3077</t>
+      <c r="AG88" t="n">
+        <v>3077</v>
+      </c>
+      <c r="AH88" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI88" t="inlineStr">
+        <is>
+          <t>2525</t>
         </is>
       </c>
     </row>
@@ -9957,9 +10471,15 @@
       <c r="AF89" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="AG89" t="inlineStr">
-        <is>
-          <t>3552</t>
+      <c r="AG89" t="n">
+        <v>3552</v>
+      </c>
+      <c r="AH89" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI89" t="inlineStr">
+        <is>
+          <t>2683</t>
         </is>
       </c>
     </row>
@@ -10066,9 +10586,15 @@
       <c r="AF90" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AG90" t="inlineStr">
-        <is>
-          <t>2976</t>
+      <c r="AG90" t="n">
+        <v>2976</v>
+      </c>
+      <c r="AH90" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI90" t="inlineStr">
+        <is>
+          <t>2531</t>
         </is>
       </c>
     </row>
@@ -10175,9 +10701,15 @@
       <c r="AF91" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="AG91" t="inlineStr">
-        <is>
-          <t>3006</t>
+      <c r="AG91" t="n">
+        <v>3006</v>
+      </c>
+      <c r="AH91" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI91" t="inlineStr">
+        <is>
+          <t>2495</t>
         </is>
       </c>
     </row>
@@ -10284,7 +10816,13 @@
       <c r="AF92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG92" t="inlineStr">
+      <c r="AG92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10393,9 +10931,15 @@
       <c r="AF93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG93" t="inlineStr">
-        <is>
-          <t>2562</t>
+      <c r="AG93" t="n">
+        <v>2562</v>
+      </c>
+      <c r="AH93" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI93" t="inlineStr">
+        <is>
+          <t>2437</t>
         </is>
       </c>
     </row>
@@ -10502,9 +11046,15 @@
       <c r="AF94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG94" t="inlineStr">
-        <is>
-          <t>3284</t>
+      <c r="AG94" t="n">
+        <v>3284</v>
+      </c>
+      <c r="AH94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI94" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -10611,9 +11161,15 @@
       <c r="AF95" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="AG95" t="inlineStr">
-        <is>
-          <t>2578</t>
+      <c r="AG95" t="n">
+        <v>2578</v>
+      </c>
+      <c r="AH95" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AI95" t="inlineStr">
+        <is>
+          <t>2502</t>
         </is>
       </c>
     </row>
@@ -10720,9 +11276,15 @@
       <c r="AF96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG96" t="inlineStr">
-        <is>
-          <t>3853</t>
+      <c r="AG96" t="n">
+        <v>3853</v>
+      </c>
+      <c r="AH96" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="AI96" t="inlineStr">
+        <is>
+          <t>2606</t>
         </is>
       </c>
     </row>
@@ -10829,9 +11391,15 @@
       <c r="AF97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG97" t="inlineStr">
-        <is>
-          <t>3108</t>
+      <c r="AG97" t="n">
+        <v>3108</v>
+      </c>
+      <c r="AH97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI97" t="inlineStr">
+        <is>
+          <t>2505</t>
         </is>
       </c>
     </row>
@@ -10938,7 +11506,13 @@
       <c r="AF98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG98" t="inlineStr">
+      <c r="AG98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11047,9 +11621,15 @@
       <c r="AF99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG99" t="inlineStr">
-        <is>
-          <t>4113</t>
+      <c r="AG99" t="n">
+        <v>4113</v>
+      </c>
+      <c r="AH99" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="AI99" t="inlineStr">
+        <is>
+          <t>2631</t>
         </is>
       </c>
     </row>
@@ -11156,9 +11736,15 @@
       <c r="AF100" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="AG100" t="inlineStr">
-        <is>
-          <t>2869</t>
+      <c r="AG100" t="n">
+        <v>2869</v>
+      </c>
+      <c r="AH100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI100" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -11265,9 +11851,15 @@
       <c r="AF101" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="AG101" t="inlineStr">
-        <is>
-          <t>4817</t>
+      <c r="AG101" t="n">
+        <v>4817</v>
+      </c>
+      <c r="AH101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AI101" t="inlineStr">
+        <is>
+          <t>2838</t>
         </is>
       </c>
     </row>
@@ -11374,9 +11966,15 @@
       <c r="AF102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AG102" t="inlineStr">
-        <is>
-          <t>4227</t>
+      <c r="AG102" t="n">
+        <v>4227</v>
+      </c>
+      <c r="AH102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI102" t="inlineStr">
+        <is>
+          <t>2691</t>
         </is>
       </c>
     </row>
@@ -11483,9 +12081,15 @@
       <c r="AF103" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AG103" t="inlineStr">
-        <is>
-          <t>3884</t>
+      <c r="AG103" t="n">
+        <v>3884</v>
+      </c>
+      <c r="AH103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI103" t="inlineStr">
+        <is>
+          <t>2481</t>
         </is>
       </c>
     </row>
@@ -11592,9 +12196,15 @@
       <c r="AF104" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="AG104" t="inlineStr">
-        <is>
-          <t>4732</t>
+      <c r="AG104" t="n">
+        <v>4732</v>
+      </c>
+      <c r="AH104" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AI104" t="inlineStr">
+        <is>
+          <t>2814</t>
         </is>
       </c>
     </row>
@@ -11701,9 +12311,15 @@
       <c r="AF105" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AG105" t="inlineStr">
-        <is>
-          <t>4481</t>
+      <c r="AG105" t="n">
+        <v>4481</v>
+      </c>
+      <c r="AH105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI105" t="inlineStr">
+        <is>
+          <t>2629</t>
         </is>
       </c>
     </row>
@@ -11810,7 +12426,13 @@
       <c r="AF106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG106" t="inlineStr">
+      <c r="AG106" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11919,9 +12541,15 @@
       <c r="AF107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG107" t="inlineStr">
-        <is>
-          <t>2553</t>
+      <c r="AG107" t="n">
+        <v>2553</v>
+      </c>
+      <c r="AH107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI107" t="inlineStr">
+        <is>
+          <t>2469</t>
         </is>
       </c>
     </row>
@@ -12028,7 +12656,13 @@
       <c r="AF108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG108" t="inlineStr">
+      <c r="AG108" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12137,9 +12771,15 @@
       <c r="AF109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG109" t="inlineStr">
-        <is>
-          <t>4134</t>
+      <c r="AG109" t="n">
+        <v>4134</v>
+      </c>
+      <c r="AH109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI109" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -12246,9 +12886,15 @@
       <c r="AF110" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="AG110" t="inlineStr">
-        <is>
-          <t>3767</t>
+      <c r="AG110" t="n">
+        <v>3767</v>
+      </c>
+      <c r="AH110" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AI110" t="inlineStr">
+        <is>
+          <t>2645</t>
         </is>
       </c>
     </row>
@@ -12355,9 +13001,15 @@
       <c r="AF111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG111" t="inlineStr">
-        <is>
-          <t>2803</t>
+      <c r="AG111" t="n">
+        <v>2803</v>
+      </c>
+      <c r="AH111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI111" t="inlineStr">
+        <is>
+          <t>2463</t>
         </is>
       </c>
     </row>
@@ -12464,9 +13116,15 @@
       <c r="AF112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG112" t="inlineStr">
-        <is>
-          <t>3505</t>
+      <c r="AG112" t="n">
+        <v>3505</v>
+      </c>
+      <c r="AH112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI112" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -12573,9 +13231,15 @@
       <c r="AF113" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="AG113" t="inlineStr">
-        <is>
-          <t>3700</t>
+      <c r="AG113" t="n">
+        <v>3700</v>
+      </c>
+      <c r="AH113" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="AI113" t="inlineStr">
+        <is>
+          <t>2526</t>
         </is>
       </c>
     </row>
@@ -12682,9 +13346,15 @@
       <c r="AF114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG114" t="inlineStr">
-        <is>
-          <t>3301</t>
+      <c r="AG114" t="n">
+        <v>3301</v>
+      </c>
+      <c r="AH114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI114" t="inlineStr">
+        <is>
+          <t>2537</t>
         </is>
       </c>
     </row>
@@ -12791,9 +13461,15 @@
       <c r="AF115" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="AG115" t="inlineStr">
-        <is>
-          <t>2306</t>
+      <c r="AG115" t="n">
+        <v>2306</v>
+      </c>
+      <c r="AH115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI115" t="inlineStr">
+        <is>
+          <t>2010</t>
         </is>
       </c>
     </row>
@@ -12900,9 +13576,15 @@
       <c r="AF116" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="AG116" t="inlineStr">
-        <is>
-          <t>3427</t>
+      <c r="AG116" t="n">
+        <v>3427</v>
+      </c>
+      <c r="AH116" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AI116" t="inlineStr">
+        <is>
+          <t>2467</t>
         </is>
       </c>
     </row>
@@ -13009,9 +13691,15 @@
       <c r="AF117" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AG117" t="inlineStr">
-        <is>
-          <t>3939</t>
+      <c r="AG117" t="n">
+        <v>3939</v>
+      </c>
+      <c r="AH117" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AI117" t="inlineStr">
+        <is>
+          <t>2722</t>
         </is>
       </c>
     </row>
@@ -13118,7 +13806,13 @@
       <c r="AF118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG118" t="inlineStr">
+      <c r="AG118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13143,7 +13837,7 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F119" s="3" t="n">
@@ -13227,9 +13921,15 @@
       <c r="AF119" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AG119" t="inlineStr">
-        <is>
-          <t>4345</t>
+      <c r="AG119" t="n">
+        <v>4345</v>
+      </c>
+      <c r="AH119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI119" t="inlineStr">
+        <is>
+          <t>2544</t>
         </is>
       </c>
     </row>
@@ -13336,9 +14036,15 @@
       <c r="AF120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG120" t="inlineStr">
-        <is>
-          <t>2550</t>
+      <c r="AG120" t="n">
+        <v>2550</v>
+      </c>
+      <c r="AH120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI120" t="inlineStr">
+        <is>
+          <t>2460</t>
         </is>
       </c>
     </row>
@@ -13445,9 +14151,15 @@
       <c r="AF121" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="AG121" t="inlineStr">
-        <is>
-          <t>3920</t>
+      <c r="AG121" t="n">
+        <v>3920</v>
+      </c>
+      <c r="AH121" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AI121" t="inlineStr">
+        <is>
+          <t>2523</t>
         </is>
       </c>
     </row>
@@ -13554,7 +14266,13 @@
       <c r="AF122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG122" t="inlineStr">
+      <c r="AG122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13663,9 +14381,15 @@
       <c r="AF123" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AG123" t="inlineStr">
-        <is>
-          <t>3564</t>
+      <c r="AG123" t="n">
+        <v>3564</v>
+      </c>
+      <c r="AH123" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI123" t="inlineStr">
+        <is>
+          <t>2556</t>
         </is>
       </c>
     </row>
@@ -13772,9 +14496,15 @@
       <c r="AF124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AG124" t="inlineStr">
-        <is>
-          <t>3463</t>
+      <c r="AG124" t="n">
+        <v>3463</v>
+      </c>
+      <c r="AH124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI124" t="inlineStr">
+        <is>
+          <t>2573</t>
         </is>
       </c>
     </row>
@@ -13881,9 +14611,15 @@
       <c r="AF125" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AG125" t="inlineStr">
-        <is>
-          <t>3856</t>
+      <c r="AG125" t="n">
+        <v>3856</v>
+      </c>
+      <c r="AH125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI125" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -13990,9 +14726,15 @@
       <c r="AF126" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AG126" t="inlineStr">
-        <is>
-          <t>3517</t>
+      <c r="AG126" t="n">
+        <v>3517</v>
+      </c>
+      <c r="AH126" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI126" t="inlineStr">
+        <is>
+          <t>2685</t>
         </is>
       </c>
     </row>
@@ -14099,9 +14841,15 @@
       <c r="AF127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG127" t="inlineStr">
-        <is>
-          <t>2336</t>
+      <c r="AG127" t="n">
+        <v>2336</v>
+      </c>
+      <c r="AH127" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="AI127" t="inlineStr">
+        <is>
+          <t>2103</t>
         </is>
       </c>
     </row>
@@ -14208,7 +14956,13 @@
       <c r="AF128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG128" t="inlineStr">
+      <c r="AG128" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14317,7 +15071,13 @@
       <c r="AF129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG129" t="inlineStr">
+      <c r="AG129" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14426,9 +15186,15 @@
       <c r="AF130" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AG130" t="inlineStr">
-        <is>
-          <t>3037</t>
+      <c r="AG130" t="n">
+        <v>3037</v>
+      </c>
+      <c r="AH130" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AI130" t="inlineStr">
+        <is>
+          <t>2463</t>
         </is>
       </c>
     </row>
@@ -14535,9 +15301,15 @@
       <c r="AF131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG131" t="inlineStr">
-        <is>
-          <t>2586</t>
+      <c r="AG131" t="n">
+        <v>2586</v>
+      </c>
+      <c r="AH131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI131" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -14644,9 +15416,15 @@
       <c r="AF132" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AG132" t="inlineStr">
-        <is>
-          <t>2822</t>
+      <c r="AG132" t="n">
+        <v>2822</v>
+      </c>
+      <c r="AH132" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI132" t="inlineStr">
+        <is>
+          <t>2457</t>
         </is>
       </c>
     </row>
@@ -14753,9 +15531,15 @@
       <c r="AF133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG133" t="inlineStr">
-        <is>
-          <t>2935</t>
+      <c r="AG133" t="n">
+        <v>2935</v>
+      </c>
+      <c r="AH133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI133" t="inlineStr">
+        <is>
+          <t>2481</t>
         </is>
       </c>
     </row>
@@ -14829,6 +15613,8 @@
       <c r="AE134" t="inlineStr"/>
       <c r="AF134" s="3" t="inlineStr"/>
       <c r="AG134" t="inlineStr"/>
+      <c r="AH134" s="3" t="inlineStr"/>
+      <c r="AI134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -14892,6 +15678,8 @@
       <c r="AE135" t="inlineStr"/>
       <c r="AF135" s="3" t="inlineStr"/>
       <c r="AG135" t="inlineStr"/>
+      <c r="AH135" s="3" t="inlineStr"/>
+      <c r="AI135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -14996,9 +15784,15 @@
       <c r="AF136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG136" t="inlineStr">
-        <is>
-          <t>2676</t>
+      <c r="AG136" t="n">
+        <v>2676</v>
+      </c>
+      <c r="AH136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI136" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -15105,7 +15899,13 @@
       <c r="AF137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG137" t="inlineStr">
+      <c r="AG137" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15173,6 +15973,8 @@
       <c r="AE138" t="inlineStr"/>
       <c r="AF138" s="3" t="inlineStr"/>
       <c r="AG138" t="inlineStr"/>
+      <c r="AH138" s="3" t="inlineStr"/>
+      <c r="AI138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -15277,9 +16079,15 @@
       <c r="AF139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG139" t="inlineStr">
-        <is>
-          <t>2432</t>
+      <c r="AG139" t="n">
+        <v>2432</v>
+      </c>
+      <c r="AH139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI139" t="inlineStr">
+        <is>
+          <t>1986</t>
         </is>
       </c>
     </row>
@@ -15386,9 +16194,15 @@
       <c r="AF140" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AG140" t="inlineStr">
-        <is>
-          <t>3167</t>
+      <c r="AG140" t="n">
+        <v>3167</v>
+      </c>
+      <c r="AH140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI140" t="inlineStr">
+        <is>
+          <t>2445</t>
         </is>
       </c>
     </row>
@@ -15454,6 +16268,8 @@
       <c r="AE141" t="inlineStr"/>
       <c r="AF141" s="3" t="inlineStr"/>
       <c r="AG141" t="inlineStr"/>
+      <c r="AH141" s="3" t="inlineStr"/>
+      <c r="AI141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -15558,9 +16374,15 @@
       <c r="AF142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG142" t="inlineStr">
-        <is>
-          <t>2303</t>
+      <c r="AG142" t="n">
+        <v>2303</v>
+      </c>
+      <c r="AH142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI142" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -15626,6 +16448,8 @@
       <c r="AE143" t="inlineStr"/>
       <c r="AF143" s="3" t="inlineStr"/>
       <c r="AG143" t="inlineStr"/>
+      <c r="AH143" s="3" t="inlineStr"/>
+      <c r="AI143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -15689,6 +16513,8 @@
       <c r="AE144" t="inlineStr"/>
       <c r="AF144" s="3" t="inlineStr"/>
       <c r="AG144" t="inlineStr"/>
+      <c r="AH144" s="3" t="inlineStr"/>
+      <c r="AI144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -15752,6 +16578,8 @@
       <c r="AE145" t="inlineStr"/>
       <c r="AF145" s="3" t="inlineStr"/>
       <c r="AG145" t="inlineStr"/>
+      <c r="AH145" s="3" t="inlineStr"/>
+      <c r="AI145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -15815,6 +16643,8 @@
       <c r="AE146" t="inlineStr"/>
       <c r="AF146" s="3" t="inlineStr"/>
       <c r="AG146" t="inlineStr"/>
+      <c r="AH146" s="3" t="inlineStr"/>
+      <c r="AI146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -15878,6 +16708,8 @@
       <c r="AE147" t="inlineStr"/>
       <c r="AF147" s="3" t="inlineStr"/>
       <c r="AG147" t="inlineStr"/>
+      <c r="AH147" s="3" t="inlineStr"/>
+      <c r="AI147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -15982,7 +16814,13 @@
       <c r="AF148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG148" t="inlineStr">
+      <c r="AG148" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16091,9 +16929,15 @@
       <c r="AF149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG149" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="AG149" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI149" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -16200,7 +17044,13 @@
       <c r="AF150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG150" t="inlineStr">
+      <c r="AG150" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16309,7 +17159,13 @@
       <c r="AF151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG151" t="inlineStr">
+      <c r="AG151" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16418,7 +17274,13 @@
       <c r="AF152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG152" t="inlineStr">
+      <c r="AG152" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16527,7 +17389,13 @@
       <c r="AF153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG153" t="inlineStr">
+      <c r="AG153" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16636,7 +17504,13 @@
       <c r="AF154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG154" t="inlineStr">
+      <c r="AG154" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16745,9 +17619,15 @@
       <c r="AF155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG155" t="inlineStr">
-        <is>
-          <t>2917</t>
+      <c r="AG155" t="n">
+        <v>2917</v>
+      </c>
+      <c r="AH155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI155" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -16848,9 +17728,15 @@
       <c r="AF156" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AG156" t="inlineStr">
-        <is>
-          <t>3773</t>
+      <c r="AG156" t="n">
+        <v>3773</v>
+      </c>
+      <c r="AH156" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AI156" t="inlineStr">
+        <is>
+          <t>2628</t>
         </is>
       </c>
     </row>
@@ -16910,6 +17796,8 @@
       <c r="AE157" t="inlineStr"/>
       <c r="AF157" s="3" t="inlineStr"/>
       <c r="AG157" t="inlineStr"/>
+      <c r="AH157" s="3" t="inlineStr"/>
+      <c r="AI157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -17008,7 +17896,13 @@
       <c r="AF158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG158" t="inlineStr">
+      <c r="AG158" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -17111,9 +18005,15 @@
       <c r="AF159" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="AG159" t="inlineStr">
-        <is>
-          <t>3110</t>
+      <c r="AG159" t="n">
+        <v>3110</v>
+      </c>
+      <c r="AH159" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI159" t="inlineStr">
+        <is>
+          <t>2527</t>
         </is>
       </c>
     </row>
@@ -17173,6 +18073,8 @@
       <c r="AE160" t="inlineStr"/>
       <c r="AF160" s="3" t="inlineStr"/>
       <c r="AG160" t="inlineStr"/>
+      <c r="AH160" s="3" t="inlineStr"/>
+      <c r="AI160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -17259,9 +18161,15 @@
       <c r="AF161" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="AG161" t="inlineStr">
-        <is>
-          <t>3226</t>
+      <c r="AG161" t="n">
+        <v>3226</v>
+      </c>
+      <c r="AH161" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AI161" t="inlineStr">
+        <is>
+          <t>2489</t>
         </is>
       </c>
     </row>
@@ -17350,9 +18258,15 @@
       <c r="AF162" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="AG162" t="inlineStr">
-        <is>
-          <t>2820</t>
+      <c r="AG162" t="n">
+        <v>2820</v>
+      </c>
+      <c r="AH162" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="AI162" t="inlineStr">
+        <is>
+          <t>2496</t>
         </is>
       </c>
     </row>
@@ -17437,9 +18351,15 @@
       <c r="AF163" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AG163" t="inlineStr">
-        <is>
-          <t>3764</t>
+      <c r="AG163" t="n">
+        <v>3764</v>
+      </c>
+      <c r="AH163" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AI163" t="inlineStr">
+        <is>
+          <t>2599</t>
         </is>
       </c>
     </row>
@@ -17508,9 +18428,15 @@
       <c r="AF164" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AG164" t="inlineStr">
-        <is>
-          <t>3798</t>
+      <c r="AG164" t="n">
+        <v>3798</v>
+      </c>
+      <c r="AH164" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AI164" t="inlineStr">
+        <is>
+          <t>2505</t>
         </is>
       </c>
     </row>
@@ -17583,9 +18509,15 @@
       <c r="AF165" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="AG165" t="inlineStr">
-        <is>
-          <t>2846</t>
+      <c r="AG165" t="n">
+        <v>2846</v>
+      </c>
+      <c r="AH165" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI165" t="inlineStr">
+        <is>
+          <t>2493</t>
         </is>
       </c>
     </row>
@@ -17650,9 +18582,15 @@
       <c r="AF166" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AG166" t="inlineStr">
-        <is>
-          <t>3325</t>
+      <c r="AG166" t="n">
+        <v>3325</v>
+      </c>
+      <c r="AH166" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI166" t="inlineStr">
+        <is>
+          <t>2464</t>
         </is>
       </c>
     </row>
@@ -17705,17 +18643,21 @@
       <c r="AF167" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG167" t="inlineStr">
+      <c r="AG167" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH167" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI167" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
     </row>
     <row r="168">
-      <c r="A168" t="inlineStr">
-        <is>
-          <t>55745105</t>
-        </is>
+      <c r="A168" t="n">
+        <v>55745105</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
@@ -17758,9 +18700,125 @@
       <c r="AF168" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AG168" t="inlineStr">
-        <is>
-          <t>1438</t>
+      <c r="AG168" t="n">
+        <v>1438</v>
+      </c>
+      <c r="AH168" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI168" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>50337435</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>HornedWarrior291</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr"/>
+      <c r="D169" t="inlineStr"/>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F169" s="3" t="inlineStr"/>
+      <c r="G169" t="inlineStr"/>
+      <c r="H169" s="3" t="inlineStr"/>
+      <c r="I169" t="inlineStr"/>
+      <c r="J169" s="3" t="inlineStr"/>
+      <c r="K169" t="inlineStr"/>
+      <c r="L169" s="3" t="inlineStr"/>
+      <c r="M169" t="inlineStr"/>
+      <c r="N169" s="3" t="inlineStr"/>
+      <c r="O169" t="inlineStr"/>
+      <c r="P169" s="3" t="inlineStr"/>
+      <c r="Q169" t="inlineStr"/>
+      <c r="R169" s="3" t="inlineStr"/>
+      <c r="S169" t="inlineStr"/>
+      <c r="T169" s="3" t="inlineStr"/>
+      <c r="U169" t="inlineStr"/>
+      <c r="V169" s="3" t="inlineStr"/>
+      <c r="W169" t="inlineStr"/>
+      <c r="X169" s="3" t="inlineStr"/>
+      <c r="Y169" t="inlineStr"/>
+      <c r="Z169" s="3" t="inlineStr"/>
+      <c r="AA169" t="inlineStr"/>
+      <c r="AB169" s="3" t="inlineStr"/>
+      <c r="AC169" t="inlineStr"/>
+      <c r="AD169" s="3" t="inlineStr"/>
+      <c r="AE169" t="inlineStr"/>
+      <c r="AF169" s="3" t="inlineStr"/>
+      <c r="AG169" t="inlineStr"/>
+      <c r="AH169" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI169" t="inlineStr">
+        <is>
+          <t>2477</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>54941706</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>AlexMenjivar20</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr"/>
+      <c r="D170" t="inlineStr"/>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F170" s="3" t="inlineStr"/>
+      <c r="G170" t="inlineStr"/>
+      <c r="H170" s="3" t="inlineStr"/>
+      <c r="I170" t="inlineStr"/>
+      <c r="J170" s="3" t="inlineStr"/>
+      <c r="K170" t="inlineStr"/>
+      <c r="L170" s="3" t="inlineStr"/>
+      <c r="M170" t="inlineStr"/>
+      <c r="N170" s="3" t="inlineStr"/>
+      <c r="O170" t="inlineStr"/>
+      <c r="P170" s="3" t="inlineStr"/>
+      <c r="Q170" t="inlineStr"/>
+      <c r="R170" s="3" t="inlineStr"/>
+      <c r="S170" t="inlineStr"/>
+      <c r="T170" s="3" t="inlineStr"/>
+      <c r="U170" t="inlineStr"/>
+      <c r="V170" s="3" t="inlineStr"/>
+      <c r="W170" t="inlineStr"/>
+      <c r="X170" s="3" t="inlineStr"/>
+      <c r="Y170" t="inlineStr"/>
+      <c r="Z170" s="3" t="inlineStr"/>
+      <c r="AA170" t="inlineStr"/>
+      <c r="AB170" s="3" t="inlineStr"/>
+      <c r="AC170" t="inlineStr"/>
+      <c r="AD170" s="3" t="inlineStr"/>
+      <c r="AE170" t="inlineStr"/>
+      <c r="AF170" s="3" t="inlineStr"/>
+      <c r="AG170" t="inlineStr"/>
+      <c r="AH170" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AI170" t="inlineStr">
+        <is>
+          <t>1469</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-02-27 15:29:30
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -18713,10 +18713,8 @@
       </c>
     </row>
     <row r="169">
-      <c r="A169" t="inlineStr">
-        <is>
-          <t>50337435</t>
-        </is>
+      <c r="A169" t="n">
+        <v>50337435</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
@@ -18768,10 +18766,8 @@
       </c>
     </row>
     <row r="170">
-      <c r="A170" t="inlineStr">
-        <is>
-          <t>54941706</t>
-        </is>
+      <c r="A170" t="n">
+        <v>54941706</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Code updated 23-02-28 11:30:34
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI170"/>
+  <dimension ref="A1:AK170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -566,6 +566,16 @@
           <t>02-26_0</t>
         </is>
       </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>02-27_A</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>02-27_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -676,9 +686,15 @@
       <c r="AH2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI2" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="AI2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK2" t="inlineStr">
+        <is>
+          <t>2512</t>
         </is>
       </c>
     </row>
@@ -791,9 +807,15 @@
       <c r="AH3" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="AI3" t="inlineStr">
-        <is>
-          <t>2747</t>
+      <c r="AI3" t="n">
+        <v>2747</v>
+      </c>
+      <c r="AJ3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK3" t="inlineStr">
+        <is>
+          <t>3094</t>
         </is>
       </c>
     </row>
@@ -906,9 +928,15 @@
       <c r="AH4" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AI4" t="inlineStr">
-        <is>
-          <t>2996</t>
+      <c r="AI4" t="n">
+        <v>2996</v>
+      </c>
+      <c r="AJ4" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AK4" t="inlineStr">
+        <is>
+          <t>3406</t>
         </is>
       </c>
     </row>
@@ -1021,9 +1049,15 @@
       <c r="AH5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AI5" t="inlineStr">
-        <is>
-          <t>2762</t>
+      <c r="AI5" t="n">
+        <v>2762</v>
+      </c>
+      <c r="AJ5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK5" t="inlineStr">
+        <is>
+          <t>3102</t>
         </is>
       </c>
     </row>
@@ -1136,9 +1170,15 @@
       <c r="AH6" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AI6" t="inlineStr">
-        <is>
-          <t>2808</t>
+      <c r="AI6" t="n">
+        <v>2808</v>
+      </c>
+      <c r="AJ6" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK6" t="inlineStr">
+        <is>
+          <t>3141</t>
         </is>
       </c>
     </row>
@@ -1251,9 +1291,15 @@
       <c r="AH7" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AI7" t="inlineStr">
-        <is>
-          <t>3002</t>
+      <c r="AI7" t="n">
+        <v>3002</v>
+      </c>
+      <c r="AJ7" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AK7" t="inlineStr">
+        <is>
+          <t>3466</t>
         </is>
       </c>
     </row>
@@ -1366,9 +1412,15 @@
       <c r="AH8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AI8" t="inlineStr">
-        <is>
-          <t>2694</t>
+      <c r="AI8" t="n">
+        <v>2694</v>
+      </c>
+      <c r="AJ8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK8" t="inlineStr">
+        <is>
+          <t>2984</t>
         </is>
       </c>
     </row>
@@ -1481,9 +1533,15 @@
       <c r="AH9" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AI9" t="inlineStr">
-        <is>
-          <t>2912</t>
+      <c r="AI9" t="n">
+        <v>2912</v>
+      </c>
+      <c r="AJ9" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AK9" t="inlineStr">
+        <is>
+          <t>3095</t>
         </is>
       </c>
     </row>
@@ -1596,9 +1654,15 @@
       <c r="AH10" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AI10" t="inlineStr">
-        <is>
-          <t>2897</t>
+      <c r="AI10" t="n">
+        <v>2897</v>
+      </c>
+      <c r="AJ10" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AK10" t="inlineStr">
+        <is>
+          <t>3188</t>
         </is>
       </c>
     </row>
@@ -1711,9 +1775,15 @@
       <c r="AH11" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AI11" t="inlineStr">
-        <is>
-          <t>2799</t>
+      <c r="AI11" t="n">
+        <v>2799</v>
+      </c>
+      <c r="AJ11" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK11" t="inlineStr">
+        <is>
+          <t>3105</t>
         </is>
       </c>
     </row>
@@ -1826,7 +1896,13 @@
       <c r="AH12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI12" t="inlineStr">
+      <c r="AI12" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AJ12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK12" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1941,9 +2017,15 @@
       <c r="AH13" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AI13" t="inlineStr">
-        <is>
-          <t>3027</t>
+      <c r="AI13" t="n">
+        <v>3027</v>
+      </c>
+      <c r="AJ13" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="AK13" t="inlineStr">
+        <is>
+          <t>3458</t>
         </is>
       </c>
     </row>
@@ -2056,9 +2138,15 @@
       <c r="AH14" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AI14" t="inlineStr">
-        <is>
-          <t>2835</t>
+      <c r="AI14" t="n">
+        <v>2835</v>
+      </c>
+      <c r="AJ14" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AK14" t="inlineStr">
+        <is>
+          <t>3150</t>
         </is>
       </c>
     </row>
@@ -2171,7 +2259,13 @@
       <c r="AH15" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI15" t="inlineStr">
+      <c r="AI15" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AJ15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK15" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2286,9 +2380,15 @@
       <c r="AH16" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="AI16" t="inlineStr">
-        <is>
-          <t>2938</t>
+      <c r="AI16" t="n">
+        <v>2938</v>
+      </c>
+      <c r="AJ16" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="AK16" t="inlineStr">
+        <is>
+          <t>3289</t>
         </is>
       </c>
     </row>
@@ -2401,9 +2501,15 @@
       <c r="AH17" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AI17" t="inlineStr">
-        <is>
-          <t>2742</t>
+      <c r="AI17" t="n">
+        <v>2742</v>
+      </c>
+      <c r="AJ17" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AK17" t="inlineStr">
+        <is>
+          <t>3111</t>
         </is>
       </c>
     </row>
@@ -2516,9 +2622,15 @@
       <c r="AH18" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AI18" t="inlineStr">
-        <is>
-          <t>2764</t>
+      <c r="AI18" t="n">
+        <v>2764</v>
+      </c>
+      <c r="AJ18" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK18" t="inlineStr">
+        <is>
+          <t>2919</t>
         </is>
       </c>
     </row>
@@ -2631,9 +2743,15 @@
       <c r="AH19" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AI19" t="inlineStr">
-        <is>
-          <t>2926</t>
+      <c r="AI19" t="n">
+        <v>2926</v>
+      </c>
+      <c r="AJ19" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AK19" t="inlineStr">
+        <is>
+          <t>3257</t>
         </is>
       </c>
     </row>
@@ -2746,9 +2864,15 @@
       <c r="AH20" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AI20" t="inlineStr">
-        <is>
-          <t>3107</t>
+      <c r="AI20" t="n">
+        <v>3107</v>
+      </c>
+      <c r="AJ20" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AK20" t="inlineStr">
+        <is>
+          <t>3604</t>
         </is>
       </c>
     </row>
@@ -2861,7 +2985,13 @@
       <c r="AH21" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AI21" t="inlineStr">
+      <c r="AI21" t="n">
+        <v>2781</v>
+      </c>
+      <c r="AJ21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK21" t="inlineStr">
         <is>
           <t>2781</t>
         </is>
@@ -2976,9 +3106,15 @@
       <c r="AH22" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="AI22" t="inlineStr">
-        <is>
-          <t>2714</t>
+      <c r="AI22" t="n">
+        <v>2714</v>
+      </c>
+      <c r="AJ22" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AK22" t="inlineStr">
+        <is>
+          <t>3132</t>
         </is>
       </c>
     </row>
@@ -3091,9 +3227,15 @@
       <c r="AH23" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="AI23" t="inlineStr">
-        <is>
-          <t>2667</t>
+      <c r="AI23" t="n">
+        <v>2667</v>
+      </c>
+      <c r="AJ23" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK23" t="inlineStr">
+        <is>
+          <t>2990</t>
         </is>
       </c>
     </row>
@@ -3206,9 +3348,15 @@
       <c r="AH24" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AI24" t="inlineStr">
-        <is>
-          <t>2924</t>
+      <c r="AI24" t="n">
+        <v>2924</v>
+      </c>
+      <c r="AJ24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AK24" t="inlineStr">
+        <is>
+          <t>3276</t>
         </is>
       </c>
     </row>
@@ -3321,7 +3469,13 @@
       <c r="AH25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI25" t="inlineStr">
+      <c r="AI25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3436,9 +3590,15 @@
       <c r="AH26" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="AI26" t="inlineStr">
-        <is>
-          <t>3019</t>
+      <c r="AI26" t="n">
+        <v>3019</v>
+      </c>
+      <c r="AJ26" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AK26" t="inlineStr">
+        <is>
+          <t>3330</t>
         </is>
       </c>
     </row>
@@ -3551,9 +3711,15 @@
       <c r="AH27" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="AI27" t="inlineStr">
-        <is>
-          <t>2900</t>
+      <c r="AI27" t="n">
+        <v>2900</v>
+      </c>
+      <c r="AJ27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK27" t="inlineStr">
+        <is>
+          <t>2891</t>
         </is>
       </c>
     </row>
@@ -3666,9 +3832,15 @@
       <c r="AH28" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="AI28" t="inlineStr">
-        <is>
-          <t>2802</t>
+      <c r="AI28" t="n">
+        <v>2802</v>
+      </c>
+      <c r="AJ28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="AK28" t="inlineStr">
+        <is>
+          <t>3000</t>
         </is>
       </c>
     </row>
@@ -3781,9 +3953,15 @@
       <c r="AH29" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AI29" t="inlineStr">
-        <is>
-          <t>3227</t>
+      <c r="AI29" t="n">
+        <v>3227</v>
+      </c>
+      <c r="AJ29" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AK29" t="inlineStr">
+        <is>
+          <t>3599</t>
         </is>
       </c>
     </row>
@@ -3896,9 +4074,15 @@
       <c r="AH30" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AI30" t="inlineStr">
-        <is>
-          <t>2796</t>
+      <c r="AI30" t="n">
+        <v>2796</v>
+      </c>
+      <c r="AJ30" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AK30" t="inlineStr">
+        <is>
+          <t>3089</t>
         </is>
       </c>
     </row>
@@ -4011,9 +4195,15 @@
       <c r="AH31" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AI31" t="inlineStr">
-        <is>
-          <t>2993</t>
+      <c r="AI31" t="n">
+        <v>2993</v>
+      </c>
+      <c r="AJ31" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AK31" t="inlineStr">
+        <is>
+          <t>3384</t>
         </is>
       </c>
     </row>
@@ -4126,9 +4316,15 @@
       <c r="AH32" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AI32" t="inlineStr">
-        <is>
-          <t>2916</t>
+      <c r="AI32" t="n">
+        <v>2916</v>
+      </c>
+      <c r="AJ32" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="AK32" t="inlineStr">
+        <is>
+          <t>3312</t>
         </is>
       </c>
     </row>
@@ -4241,9 +4437,15 @@
       <c r="AH33" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AI33" t="inlineStr">
-        <is>
-          <t>2783</t>
+      <c r="AI33" t="n">
+        <v>2783</v>
+      </c>
+      <c r="AJ33" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="AK33" t="inlineStr">
+        <is>
+          <t>3023</t>
         </is>
       </c>
     </row>
@@ -4356,9 +4558,15 @@
       <c r="AH34" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AI34" t="inlineStr">
-        <is>
-          <t>2956</t>
+      <c r="AI34" t="n">
+        <v>2956</v>
+      </c>
+      <c r="AJ34" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AK34" t="inlineStr">
+        <is>
+          <t>3179</t>
         </is>
       </c>
     </row>
@@ -4471,9 +4679,15 @@
       <c r="AH35" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AI35" t="inlineStr">
-        <is>
-          <t>2964</t>
+      <c r="AI35" t="n">
+        <v>2964</v>
+      </c>
+      <c r="AJ35" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AK35" t="inlineStr">
+        <is>
+          <t>3313</t>
         </is>
       </c>
     </row>
@@ -4586,9 +4800,15 @@
       <c r="AH36" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="AI36" t="inlineStr">
-        <is>
-          <t>2700</t>
+      <c r="AI36" t="n">
+        <v>2700</v>
+      </c>
+      <c r="AJ36" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK36" t="inlineStr">
+        <is>
+          <t>3061</t>
         </is>
       </c>
     </row>
@@ -4701,9 +4921,15 @@
       <c r="AH37" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AI37" t="inlineStr">
-        <is>
-          <t>2916</t>
+      <c r="AI37" t="n">
+        <v>2916</v>
+      </c>
+      <c r="AJ37" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AK37" t="inlineStr">
+        <is>
+          <t>3114</t>
         </is>
       </c>
     </row>
@@ -4816,9 +5042,15 @@
       <c r="AH38" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AI38" t="inlineStr">
-        <is>
-          <t>2901</t>
+      <c r="AI38" t="n">
+        <v>2901</v>
+      </c>
+      <c r="AJ38" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AK38" t="inlineStr">
+        <is>
+          <t>3205</t>
         </is>
       </c>
     </row>
@@ -4931,9 +5163,15 @@
       <c r="AH39" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AI39" t="inlineStr">
-        <is>
-          <t>2900</t>
+      <c r="AI39" t="n">
+        <v>2900</v>
+      </c>
+      <c r="AJ39" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AK39" t="inlineStr">
+        <is>
+          <t>3200</t>
         </is>
       </c>
     </row>
@@ -5046,9 +5284,15 @@
       <c r="AH40" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AI40" t="inlineStr">
-        <is>
-          <t>3048</t>
+      <c r="AI40" t="n">
+        <v>3048</v>
+      </c>
+      <c r="AJ40" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AK40" t="inlineStr">
+        <is>
+          <t>3382</t>
         </is>
       </c>
     </row>
@@ -5161,7 +5405,13 @@
       <c r="AH41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI41" t="inlineStr">
+      <c r="AI41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK41" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5276,9 +5526,15 @@
       <c r="AH42" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="AI42" t="inlineStr">
-        <is>
-          <t>2939</t>
+      <c r="AI42" t="n">
+        <v>2939</v>
+      </c>
+      <c r="AJ42" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AK42" t="inlineStr">
+        <is>
+          <t>3512</t>
         </is>
       </c>
     </row>
@@ -5391,9 +5647,15 @@
       <c r="AH43" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AI43" t="inlineStr">
-        <is>
-          <t>2959</t>
+      <c r="AI43" t="n">
+        <v>2959</v>
+      </c>
+      <c r="AJ43" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AK43" t="inlineStr">
+        <is>
+          <t>3371</t>
         </is>
       </c>
     </row>
@@ -5506,9 +5768,15 @@
       <c r="AH44" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AI44" t="inlineStr">
-        <is>
-          <t>2859</t>
+      <c r="AI44" t="n">
+        <v>2859</v>
+      </c>
+      <c r="AJ44" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AK44" t="inlineStr">
+        <is>
+          <t>3147</t>
         </is>
       </c>
     </row>
@@ -5621,9 +5889,15 @@
       <c r="AH45" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AI45" t="inlineStr">
-        <is>
-          <t>2834</t>
+      <c r="AI45" t="n">
+        <v>2834</v>
+      </c>
+      <c r="AJ45" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AK45" t="inlineStr">
+        <is>
+          <t>3115</t>
         </is>
       </c>
     </row>
@@ -5736,9 +6010,15 @@
       <c r="AH46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AI46" t="inlineStr">
-        <is>
-          <t>2861</t>
+      <c r="AI46" t="n">
+        <v>2861</v>
+      </c>
+      <c r="AJ46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AK46" t="inlineStr">
+        <is>
+          <t>3161</t>
         </is>
       </c>
     </row>
@@ -5851,9 +6131,15 @@
       <c r="AH47" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AI47" t="inlineStr">
-        <is>
-          <t>2829</t>
+      <c r="AI47" t="n">
+        <v>2829</v>
+      </c>
+      <c r="AJ47" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK47" t="inlineStr">
+        <is>
+          <t>3103</t>
         </is>
       </c>
     </row>
@@ -5966,9 +6252,15 @@
       <c r="AH48" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AI48" t="inlineStr">
-        <is>
-          <t>3033</t>
+      <c r="AI48" t="n">
+        <v>3033</v>
+      </c>
+      <c r="AJ48" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AK48" t="inlineStr">
+        <is>
+          <t>3372</t>
         </is>
       </c>
     </row>
@@ -6081,9 +6373,15 @@
       <c r="AH49" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AI49" t="inlineStr">
-        <is>
-          <t>2758</t>
+      <c r="AI49" t="n">
+        <v>2758</v>
+      </c>
+      <c r="AJ49" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK49" t="inlineStr">
+        <is>
+          <t>2769</t>
         </is>
       </c>
     </row>
@@ -6196,9 +6494,15 @@
       <c r="AH50" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AI50" t="inlineStr">
-        <is>
-          <t>2836</t>
+      <c r="AI50" t="n">
+        <v>2836</v>
+      </c>
+      <c r="AJ50" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AK50" t="inlineStr">
+        <is>
+          <t>3233</t>
         </is>
       </c>
     </row>
@@ -6311,9 +6615,15 @@
       <c r="AH51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI51" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="AI51" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK51" t="inlineStr">
+        <is>
+          <t>2481</t>
         </is>
       </c>
     </row>
@@ -6426,7 +6736,13 @@
       <c r="AH52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI52" t="inlineStr">
+      <c r="AI52" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK52" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6541,9 +6857,15 @@
       <c r="AH53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI53" t="inlineStr">
-        <is>
-          <t>2511</t>
+      <c r="AI53" t="n">
+        <v>2511</v>
+      </c>
+      <c r="AJ53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK53" t="inlineStr">
+        <is>
+          <t>2567</t>
         </is>
       </c>
     </row>
@@ -6656,9 +6978,15 @@
       <c r="AH54" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AI54" t="inlineStr">
-        <is>
-          <t>3005</t>
+      <c r="AI54" t="n">
+        <v>3005</v>
+      </c>
+      <c r="AJ54" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AK54" t="inlineStr">
+        <is>
+          <t>3336</t>
         </is>
       </c>
     </row>
@@ -6771,9 +7099,15 @@
       <c r="AH55" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AI55" t="inlineStr">
-        <is>
-          <t>2701</t>
+      <c r="AI55" t="n">
+        <v>2701</v>
+      </c>
+      <c r="AJ55" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AK55" t="inlineStr">
+        <is>
+          <t>2924</t>
         </is>
       </c>
     </row>
@@ -6886,9 +7220,15 @@
       <c r="AH56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AI56" t="inlineStr">
-        <is>
-          <t>2701</t>
+      <c r="AI56" t="n">
+        <v>2701</v>
+      </c>
+      <c r="AJ56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK56" t="inlineStr">
+        <is>
+          <t>2915</t>
         </is>
       </c>
     </row>
@@ -7001,9 +7341,15 @@
       <c r="AH57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AI57" t="inlineStr">
-        <is>
-          <t>2787</t>
+      <c r="AI57" t="n">
+        <v>2787</v>
+      </c>
+      <c r="AJ57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK57" t="inlineStr">
+        <is>
+          <t>3108</t>
         </is>
       </c>
     </row>
@@ -7116,9 +7462,15 @@
       <c r="AH58" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AI58" t="inlineStr">
-        <is>
-          <t>2826</t>
+      <c r="AI58" t="n">
+        <v>2826</v>
+      </c>
+      <c r="AJ58" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AK58" t="inlineStr">
+        <is>
+          <t>2892</t>
         </is>
       </c>
     </row>
@@ -7170,6 +7522,8 @@
       <c r="AG59" t="inlineStr"/>
       <c r="AH59" s="3" t="inlineStr"/>
       <c r="AI59" t="inlineStr"/>
+      <c r="AJ59" s="3" t="inlineStr"/>
+      <c r="AK59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -7219,6 +7573,8 @@
       <c r="AG60" t="inlineStr"/>
       <c r="AH60" s="3" t="inlineStr"/>
       <c r="AI60" t="inlineStr"/>
+      <c r="AJ60" s="3" t="inlineStr"/>
+      <c r="AK60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -7329,9 +7685,15 @@
       <c r="AH61" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AI61" t="inlineStr">
-        <is>
-          <t>2836</t>
+      <c r="AI61" t="n">
+        <v>2836</v>
+      </c>
+      <c r="AJ61" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="AK61" t="inlineStr">
+        <is>
+          <t>2978</t>
         </is>
       </c>
     </row>
@@ -7444,7 +7806,13 @@
       <c r="AH62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI62" t="inlineStr">
+      <c r="AI62" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7559,9 +7927,15 @@
       <c r="AH63" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AI63" t="inlineStr">
-        <is>
-          <t>2885</t>
+      <c r="AI63" t="n">
+        <v>2885</v>
+      </c>
+      <c r="AJ63" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AK63" t="inlineStr">
+        <is>
+          <t>3181</t>
         </is>
       </c>
     </row>
@@ -7674,7 +8048,13 @@
       <c r="AH64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI64" t="inlineStr">
+      <c r="AI64" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AJ64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK64" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -7728,6 +8108,8 @@
       <c r="AG65" t="inlineStr"/>
       <c r="AH65" s="3" t="inlineStr"/>
       <c r="AI65" t="inlineStr"/>
+      <c r="AJ65" s="3" t="inlineStr"/>
+      <c r="AK65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -7838,9 +8220,15 @@
       <c r="AH66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI66" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="AI66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK66" t="inlineStr">
+        <is>
+          <t>2495</t>
         </is>
       </c>
     </row>
@@ -7953,9 +8341,15 @@
       <c r="AH67" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AI67" t="inlineStr">
-        <is>
-          <t>2797</t>
+      <c r="AI67" t="n">
+        <v>2797</v>
+      </c>
+      <c r="AJ67" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AK67" t="inlineStr">
+        <is>
+          <t>3101</t>
         </is>
       </c>
     </row>
@@ -7978,7 +8372,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F68" s="5" t="n">
@@ -8068,9 +8462,15 @@
       <c r="AH68" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AI68" t="inlineStr">
-        <is>
-          <t>2956</t>
+      <c r="AI68" t="n">
+        <v>2956</v>
+      </c>
+      <c r="AJ68" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AK68" t="inlineStr">
+        <is>
+          <t>3233</t>
         </is>
       </c>
     </row>
@@ -8183,9 +8583,15 @@
       <c r="AH69" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AI69" t="inlineStr">
-        <is>
-          <t>2777</t>
+      <c r="AI69" t="n">
+        <v>2777</v>
+      </c>
+      <c r="AJ69" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AK69" t="inlineStr">
+        <is>
+          <t>2895</t>
         </is>
       </c>
     </row>
@@ -8298,7 +8704,13 @@
       <c r="AH70" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="AI70" t="inlineStr">
+      <c r="AI70" t="n">
+        <v>2494</v>
+      </c>
+      <c r="AJ70" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK70" t="inlineStr">
         <is>
           <t>2494</t>
         </is>
@@ -8413,9 +8825,15 @@
       <c r="AH71" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="AI71" t="inlineStr">
-        <is>
-          <t>2705</t>
+      <c r="AI71" t="n">
+        <v>2705</v>
+      </c>
+      <c r="AJ71" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AK71" t="inlineStr">
+        <is>
+          <t>2945</t>
         </is>
       </c>
     </row>
@@ -8528,9 +8946,15 @@
       <c r="AH72" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="AI72" t="inlineStr">
-        <is>
-          <t>2510</t>
+      <c r="AI72" t="n">
+        <v>2510</v>
+      </c>
+      <c r="AJ72" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="AK72" t="inlineStr">
+        <is>
+          <t>2643</t>
         </is>
       </c>
     </row>
@@ -8643,9 +9067,15 @@
       <c r="AH73" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AI73" t="inlineStr">
-        <is>
-          <t>2712</t>
+      <c r="AI73" t="n">
+        <v>2712</v>
+      </c>
+      <c r="AJ73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK73" t="inlineStr">
+        <is>
+          <t>2990</t>
         </is>
       </c>
     </row>
@@ -8758,9 +9188,15 @@
       <c r="AH74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI74" t="inlineStr">
-        <is>
-          <t>2508</t>
+      <c r="AI74" t="n">
+        <v>2508</v>
+      </c>
+      <c r="AJ74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK74" t="inlineStr">
+        <is>
+          <t>2597</t>
         </is>
       </c>
     </row>
@@ -8873,9 +9309,15 @@
       <c r="AH75" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AI75" t="inlineStr">
-        <is>
-          <t>2749</t>
+      <c r="AI75" t="n">
+        <v>2749</v>
+      </c>
+      <c r="AJ75" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="AK75" t="inlineStr">
+        <is>
+          <t>2905</t>
         </is>
       </c>
     </row>
@@ -8988,9 +9430,15 @@
       <c r="AH76" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="AI76" t="inlineStr">
-        <is>
-          <t>2797</t>
+      <c r="AI76" t="n">
+        <v>2797</v>
+      </c>
+      <c r="AJ76" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AK76" t="inlineStr">
+        <is>
+          <t>3215</t>
         </is>
       </c>
     </row>
@@ -9103,7 +9551,13 @@
       <c r="AH77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI77" t="inlineStr">
+      <c r="AI77" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK77" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9218,9 +9672,15 @@
       <c r="AH78" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AI78" t="inlineStr">
-        <is>
-          <t>2866</t>
+      <c r="AI78" t="n">
+        <v>2866</v>
+      </c>
+      <c r="AJ78" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AK78" t="inlineStr">
+        <is>
+          <t>3168</t>
         </is>
       </c>
     </row>
@@ -9333,7 +9793,13 @@
       <c r="AH79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI79" t="inlineStr">
+      <c r="AI79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9448,9 +9914,15 @@
       <c r="AH80" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="AI80" t="inlineStr">
-        <is>
-          <t>2794</t>
+      <c r="AI80" t="n">
+        <v>2794</v>
+      </c>
+      <c r="AJ80" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="AK80" t="inlineStr">
+        <is>
+          <t>3045</t>
         </is>
       </c>
     </row>
@@ -9563,9 +10035,15 @@
       <c r="AH81" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AI81" t="inlineStr">
-        <is>
-          <t>2942</t>
+      <c r="AI81" t="n">
+        <v>2942</v>
+      </c>
+      <c r="AJ81" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AK81" t="inlineStr">
+        <is>
+          <t>3067</t>
         </is>
       </c>
     </row>
@@ -9678,9 +10156,15 @@
       <c r="AH82" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AI82" t="inlineStr">
-        <is>
-          <t>2845</t>
+      <c r="AI82" t="n">
+        <v>2845</v>
+      </c>
+      <c r="AJ82" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK82" t="inlineStr">
+        <is>
+          <t>3132</t>
         </is>
       </c>
     </row>
@@ -9793,9 +10277,15 @@
       <c r="AH83" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AI83" t="inlineStr">
-        <is>
-          <t>2863</t>
+      <c r="AI83" t="n">
+        <v>2863</v>
+      </c>
+      <c r="AJ83" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AK83" t="inlineStr">
+        <is>
+          <t>2936</t>
         </is>
       </c>
     </row>
@@ -9907,6 +10397,8 @@
       </c>
       <c r="AH84" s="3" t="inlineStr"/>
       <c r="AI84" t="inlineStr"/>
+      <c r="AJ84" s="3" t="inlineStr"/>
+      <c r="AK84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -10017,9 +10509,15 @@
       <c r="AH85" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AI85" t="inlineStr">
-        <is>
-          <t>2805</t>
+      <c r="AI85" t="n">
+        <v>2805</v>
+      </c>
+      <c r="AJ85" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK85" t="inlineStr">
+        <is>
+          <t>2856</t>
         </is>
       </c>
     </row>
@@ -10132,9 +10630,15 @@
       <c r="AH86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI86" t="inlineStr">
-        <is>
-          <t>2485</t>
+      <c r="AI86" t="n">
+        <v>2485</v>
+      </c>
+      <c r="AJ86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK86" t="inlineStr">
+        <is>
+          <t>2467</t>
         </is>
       </c>
     </row>
@@ -10247,9 +10751,15 @@
       <c r="AH87" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AI87" t="inlineStr">
-        <is>
-          <t>2856</t>
+      <c r="AI87" t="n">
+        <v>2856</v>
+      </c>
+      <c r="AJ87" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AK87" t="inlineStr">
+        <is>
+          <t>3176</t>
         </is>
       </c>
     </row>
@@ -10362,9 +10872,15 @@
       <c r="AH88" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AI88" t="inlineStr">
-        <is>
-          <t>2525</t>
+      <c r="AI88" t="n">
+        <v>2525</v>
+      </c>
+      <c r="AJ88" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK88" t="inlineStr">
+        <is>
+          <t>2557</t>
         </is>
       </c>
     </row>
@@ -10477,9 +10993,15 @@
       <c r="AH89" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AI89" t="inlineStr">
-        <is>
-          <t>2683</t>
+      <c r="AI89" t="n">
+        <v>2683</v>
+      </c>
+      <c r="AJ89" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK89" t="inlineStr">
+        <is>
+          <t>2766</t>
         </is>
       </c>
     </row>
@@ -10592,9 +11114,15 @@
       <c r="AH90" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AI90" t="inlineStr">
-        <is>
-          <t>2531</t>
+      <c r="AI90" t="n">
+        <v>2531</v>
+      </c>
+      <c r="AJ90" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK90" t="inlineStr">
+        <is>
+          <t>2580</t>
         </is>
       </c>
     </row>
@@ -10707,9 +11235,15 @@
       <c r="AH91" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AI91" t="inlineStr">
-        <is>
-          <t>2495</t>
+      <c r="AI91" t="n">
+        <v>2495</v>
+      </c>
+      <c r="AJ91" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK91" t="inlineStr">
+        <is>
+          <t>2515</t>
         </is>
       </c>
     </row>
@@ -10822,7 +11356,13 @@
       <c r="AH92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI92" t="inlineStr">
+      <c r="AI92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10937,9 +11477,15 @@
       <c r="AH93" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="AI93" t="inlineStr">
-        <is>
-          <t>2437</t>
+      <c r="AI93" t="n">
+        <v>2437</v>
+      </c>
+      <c r="AJ93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK93" t="inlineStr">
+        <is>
+          <t>2395</t>
         </is>
       </c>
     </row>
@@ -11052,7 +11598,13 @@
       <c r="AH94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI94" t="inlineStr">
+      <c r="AI94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11167,9 +11719,15 @@
       <c r="AH95" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AI95" t="inlineStr">
-        <is>
-          <t>2502</t>
+      <c r="AI95" t="n">
+        <v>2502</v>
+      </c>
+      <c r="AJ95" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AK95" t="inlineStr">
+        <is>
+          <t>2496</t>
         </is>
       </c>
     </row>
@@ -11282,9 +11840,15 @@
       <c r="AH96" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="AI96" t="inlineStr">
-        <is>
-          <t>2606</t>
+      <c r="AI96" t="n">
+        <v>2606</v>
+      </c>
+      <c r="AJ96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK96" t="inlineStr">
+        <is>
+          <t>2545</t>
         </is>
       </c>
     </row>
@@ -11397,9 +11961,15 @@
       <c r="AH97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI97" t="inlineStr">
-        <is>
-          <t>2505</t>
+      <c r="AI97" t="n">
+        <v>2505</v>
+      </c>
+      <c r="AJ97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK97" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -11512,7 +12082,13 @@
       <c r="AH98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI98" t="inlineStr">
+      <c r="AI98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11627,9 +12203,15 @@
       <c r="AH99" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="AI99" t="inlineStr">
-        <is>
-          <t>2631</t>
+      <c r="AI99" t="n">
+        <v>2631</v>
+      </c>
+      <c r="AJ99" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AK99" t="inlineStr">
+        <is>
+          <t>2690</t>
         </is>
       </c>
     </row>
@@ -11742,9 +12324,15 @@
       <c r="AH100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI100" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="AI100" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK100" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -11857,9 +12445,15 @@
       <c r="AH101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AI101" t="inlineStr">
-        <is>
-          <t>2838</t>
+      <c r="AI101" t="n">
+        <v>2838</v>
+      </c>
+      <c r="AJ101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AK101" t="inlineStr">
+        <is>
+          <t>3075</t>
         </is>
       </c>
     </row>
@@ -11972,9 +12566,15 @@
       <c r="AH102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AI102" t="inlineStr">
-        <is>
-          <t>2691</t>
+      <c r="AI102" t="n">
+        <v>2691</v>
+      </c>
+      <c r="AJ102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK102" t="inlineStr">
+        <is>
+          <t>2851</t>
         </is>
       </c>
     </row>
@@ -12087,9 +12687,15 @@
       <c r="AH103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI103" t="inlineStr">
-        <is>
-          <t>2481</t>
+      <c r="AI103" t="n">
+        <v>2481</v>
+      </c>
+      <c r="AJ103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK103" t="inlineStr">
+        <is>
+          <t>2475</t>
         </is>
       </c>
     </row>
@@ -12202,9 +12808,15 @@
       <c r="AH104" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AI104" t="inlineStr">
-        <is>
-          <t>2814</t>
+      <c r="AI104" t="n">
+        <v>2814</v>
+      </c>
+      <c r="AJ104" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AK104" t="inlineStr">
+        <is>
+          <t>3068</t>
         </is>
       </c>
     </row>
@@ -12317,9 +12929,15 @@
       <c r="AH105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI105" t="inlineStr">
-        <is>
-          <t>2629</t>
+      <c r="AI105" t="n">
+        <v>2629</v>
+      </c>
+      <c r="AJ105" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AK105" t="inlineStr">
+        <is>
+          <t>2932</t>
         </is>
       </c>
     </row>
@@ -12432,7 +13050,13 @@
       <c r="AH106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI106" t="inlineStr">
+      <c r="AI106" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12547,9 +13171,15 @@
       <c r="AH107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI107" t="inlineStr">
-        <is>
-          <t>2469</t>
+      <c r="AI107" t="n">
+        <v>2469</v>
+      </c>
+      <c r="AJ107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK107" t="inlineStr">
+        <is>
+          <t>2506</t>
         </is>
       </c>
     </row>
@@ -12662,7 +13292,13 @@
       <c r="AH108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI108" t="inlineStr">
+      <c r="AI108" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12777,9 +13413,15 @@
       <c r="AH109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI109" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="AI109" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ109" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="AK109" t="inlineStr">
+        <is>
+          <t>2713</t>
         </is>
       </c>
     </row>
@@ -12892,9 +13534,15 @@
       <c r="AH110" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AI110" t="inlineStr">
-        <is>
-          <t>2645</t>
+      <c r="AI110" t="n">
+        <v>2645</v>
+      </c>
+      <c r="AJ110" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AK110" t="inlineStr">
+        <is>
+          <t>2796</t>
         </is>
       </c>
     </row>
@@ -13007,9 +13655,15 @@
       <c r="AH111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI111" t="inlineStr">
-        <is>
-          <t>2463</t>
+      <c r="AI111" t="n">
+        <v>2463</v>
+      </c>
+      <c r="AJ111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK111" t="inlineStr">
+        <is>
+          <t>2497</t>
         </is>
       </c>
     </row>
@@ -13122,9 +13776,15 @@
       <c r="AH112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI112" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="AI112" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK112" t="inlineStr">
+        <is>
+          <t>2508</t>
         </is>
       </c>
     </row>
@@ -13237,9 +13897,15 @@
       <c r="AH113" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="AI113" t="inlineStr">
-        <is>
-          <t>2526</t>
+      <c r="AI113" t="n">
+        <v>2526</v>
+      </c>
+      <c r="AJ113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK113" t="inlineStr">
+        <is>
+          <t>2611</t>
         </is>
       </c>
     </row>
@@ -13352,9 +14018,15 @@
       <c r="AH114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI114" t="inlineStr">
-        <is>
-          <t>2537</t>
+      <c r="AI114" t="n">
+        <v>2537</v>
+      </c>
+      <c r="AJ114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK114" t="inlineStr">
+        <is>
+          <t>2690</t>
         </is>
       </c>
     </row>
@@ -13467,9 +14139,15 @@
       <c r="AH115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI115" t="inlineStr">
-        <is>
-          <t>2010</t>
+      <c r="AI115" t="n">
+        <v>2010</v>
+      </c>
+      <c r="AJ115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK115" t="inlineStr">
+        <is>
+          <t>2027</t>
         </is>
       </c>
     </row>
@@ -13582,9 +14260,15 @@
       <c r="AH116" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="AI116" t="inlineStr">
-        <is>
-          <t>2467</t>
+      <c r="AI116" t="n">
+        <v>2467</v>
+      </c>
+      <c r="AJ116" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK116" t="inlineStr">
+        <is>
+          <t>2665</t>
         </is>
       </c>
     </row>
@@ -13697,9 +14381,15 @@
       <c r="AH117" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AI117" t="inlineStr">
-        <is>
-          <t>2722</t>
+      <c r="AI117" t="n">
+        <v>2722</v>
+      </c>
+      <c r="AJ117" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AK117" t="inlineStr">
+        <is>
+          <t>2791</t>
         </is>
       </c>
     </row>
@@ -13812,7 +14502,13 @@
       <c r="AH118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI118" t="inlineStr">
+      <c r="AI118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13927,9 +14623,15 @@
       <c r="AH119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI119" t="inlineStr">
-        <is>
-          <t>2544</t>
+      <c r="AI119" t="n">
+        <v>2544</v>
+      </c>
+      <c r="AJ119" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AK119" t="inlineStr">
+        <is>
+          <t>2866</t>
         </is>
       </c>
     </row>
@@ -14042,9 +14744,15 @@
       <c r="AH120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI120" t="inlineStr">
-        <is>
-          <t>2460</t>
+      <c r="AI120" t="n">
+        <v>2460</v>
+      </c>
+      <c r="AJ120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK120" t="inlineStr">
+        <is>
+          <t>2421</t>
         </is>
       </c>
     </row>
@@ -14157,9 +14865,15 @@
       <c r="AH121" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="AI121" t="inlineStr">
-        <is>
-          <t>2523</t>
+      <c r="AI121" t="n">
+        <v>2523</v>
+      </c>
+      <c r="AJ121" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AK121" t="inlineStr">
+        <is>
+          <t>2651</t>
         </is>
       </c>
     </row>
@@ -14272,7 +14986,13 @@
       <c r="AH122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI122" t="inlineStr">
+      <c r="AI122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14387,9 +15107,15 @@
       <c r="AH123" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AI123" t="inlineStr">
-        <is>
-          <t>2556</t>
+      <c r="AI123" t="n">
+        <v>2556</v>
+      </c>
+      <c r="AJ123" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="AK123" t="inlineStr">
+        <is>
+          <t>2622</t>
         </is>
       </c>
     </row>
@@ -14502,9 +15228,15 @@
       <c r="AH124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AI124" t="inlineStr">
-        <is>
-          <t>2573</t>
+      <c r="AI124" t="n">
+        <v>2573</v>
+      </c>
+      <c r="AJ124" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="AK124" t="inlineStr">
+        <is>
+          <t>2565</t>
         </is>
       </c>
     </row>
@@ -14617,7 +15349,13 @@
       <c r="AH125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI125" t="inlineStr">
+      <c r="AI125" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK125" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14732,9 +15470,15 @@
       <c r="AH126" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AI126" t="inlineStr">
-        <is>
-          <t>2685</t>
+      <c r="AI126" t="n">
+        <v>2685</v>
+      </c>
+      <c r="AJ126" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AK126" t="inlineStr">
+        <is>
+          <t>2632</t>
         </is>
       </c>
     </row>
@@ -14847,9 +15591,15 @@
       <c r="AH127" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="AI127" t="inlineStr">
-        <is>
-          <t>2103</t>
+      <c r="AI127" t="n">
+        <v>2103</v>
+      </c>
+      <c r="AJ127" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK127" t="inlineStr">
+        <is>
+          <t>2395</t>
         </is>
       </c>
     </row>
@@ -14962,7 +15712,13 @@
       <c r="AH128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI128" t="inlineStr">
+      <c r="AI128" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15077,7 +15833,13 @@
       <c r="AH129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI129" t="inlineStr">
+      <c r="AI129" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15192,9 +15954,15 @@
       <c r="AH130" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AI130" t="inlineStr">
-        <is>
-          <t>2463</t>
+      <c r="AI130" t="n">
+        <v>2463</v>
+      </c>
+      <c r="AJ130" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AK130" t="inlineStr">
+        <is>
+          <t>2492</t>
         </is>
       </c>
     </row>
@@ -15307,7 +16075,13 @@
       <c r="AH131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI131" t="inlineStr">
+      <c r="AI131" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15422,9 +16196,15 @@
       <c r="AH132" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AI132" t="inlineStr">
-        <is>
-          <t>2457</t>
+      <c r="AI132" t="n">
+        <v>2457</v>
+      </c>
+      <c r="AJ132" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK132" t="inlineStr">
+        <is>
+          <t>2470</t>
         </is>
       </c>
     </row>
@@ -15537,9 +16317,15 @@
       <c r="AH133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI133" t="inlineStr">
-        <is>
-          <t>2481</t>
+      <c r="AI133" t="n">
+        <v>2481</v>
+      </c>
+      <c r="AJ133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK133" t="inlineStr">
+        <is>
+          <t>2424</t>
         </is>
       </c>
     </row>
@@ -15615,6 +16401,8 @@
       <c r="AG134" t="inlineStr"/>
       <c r="AH134" s="3" t="inlineStr"/>
       <c r="AI134" t="inlineStr"/>
+      <c r="AJ134" s="3" t="inlineStr"/>
+      <c r="AK134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -15680,6 +16468,8 @@
       <c r="AG135" t="inlineStr"/>
       <c r="AH135" s="3" t="inlineStr"/>
       <c r="AI135" t="inlineStr"/>
+      <c r="AJ135" s="3" t="inlineStr"/>
+      <c r="AK135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -15790,7 +16580,13 @@
       <c r="AH136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI136" t="inlineStr">
+      <c r="AI136" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK136" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15905,7 +16701,13 @@
       <c r="AH137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI137" t="inlineStr">
+      <c r="AI137" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15975,6 +16777,8 @@
       <c r="AG138" t="inlineStr"/>
       <c r="AH138" s="3" t="inlineStr"/>
       <c r="AI138" t="inlineStr"/>
+      <c r="AJ138" s="3" t="inlineStr"/>
+      <c r="AK138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -16085,9 +16889,15 @@
       <c r="AH139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI139" t="inlineStr">
-        <is>
-          <t>1986</t>
+      <c r="AI139" t="n">
+        <v>1986</v>
+      </c>
+      <c r="AJ139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK139" t="inlineStr">
+        <is>
+          <t>1997</t>
         </is>
       </c>
     </row>
@@ -16200,9 +17010,15 @@
       <c r="AH140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI140" t="inlineStr">
-        <is>
-          <t>2445</t>
+      <c r="AI140" t="n">
+        <v>2445</v>
+      </c>
+      <c r="AJ140" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AK140" t="inlineStr">
+        <is>
+          <t>2475</t>
         </is>
       </c>
     </row>
@@ -16270,6 +17086,8 @@
       <c r="AG141" t="inlineStr"/>
       <c r="AH141" s="3" t="inlineStr"/>
       <c r="AI141" t="inlineStr"/>
+      <c r="AJ141" s="3" t="inlineStr"/>
+      <c r="AK141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -16380,7 +17198,13 @@
       <c r="AH142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI142" t="inlineStr">
+      <c r="AI142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK142" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16450,6 +17274,8 @@
       <c r="AG143" t="inlineStr"/>
       <c r="AH143" s="3" t="inlineStr"/>
       <c r="AI143" t="inlineStr"/>
+      <c r="AJ143" s="3" t="inlineStr"/>
+      <c r="AK143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -16515,6 +17341,8 @@
       <c r="AG144" t="inlineStr"/>
       <c r="AH144" s="3" t="inlineStr"/>
       <c r="AI144" t="inlineStr"/>
+      <c r="AJ144" s="3" t="inlineStr"/>
+      <c r="AK144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -16580,6 +17408,8 @@
       <c r="AG145" t="inlineStr"/>
       <c r="AH145" s="3" t="inlineStr"/>
       <c r="AI145" t="inlineStr"/>
+      <c r="AJ145" s="3" t="inlineStr"/>
+      <c r="AK145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -16645,6 +17475,8 @@
       <c r="AG146" t="inlineStr"/>
       <c r="AH146" s="3" t="inlineStr"/>
       <c r="AI146" t="inlineStr"/>
+      <c r="AJ146" s="3" t="inlineStr"/>
+      <c r="AK146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -16710,6 +17542,8 @@
       <c r="AG147" t="inlineStr"/>
       <c r="AH147" s="3" t="inlineStr"/>
       <c r="AI147" t="inlineStr"/>
+      <c r="AJ147" s="3" t="inlineStr"/>
+      <c r="AK147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -16820,7 +17654,13 @@
       <c r="AH148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI148" t="inlineStr">
+      <c r="AI148" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16935,7 +17775,13 @@
       <c r="AH149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI149" t="inlineStr">
+      <c r="AI149" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AJ149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK149" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -17050,7 +17896,13 @@
       <c r="AH150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI150" t="inlineStr">
+      <c r="AI150" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -17165,7 +18017,13 @@
       <c r="AH151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI151" t="inlineStr">
+      <c r="AI151" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -17280,7 +18138,13 @@
       <c r="AH152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI152" t="inlineStr">
+      <c r="AI152" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -17395,7 +18259,13 @@
       <c r="AH153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI153" t="inlineStr">
+      <c r="AI153" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -17510,7 +18380,13 @@
       <c r="AH154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI154" t="inlineStr">
+      <c r="AI154" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -17625,9 +18501,15 @@
       <c r="AH155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI155" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="AI155" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK155" t="inlineStr">
+        <is>
+          <t>2490</t>
         </is>
       </c>
     </row>
@@ -17734,9 +18616,15 @@
       <c r="AH156" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AI156" t="inlineStr">
-        <is>
-          <t>2628</t>
+      <c r="AI156" t="n">
+        <v>2628</v>
+      </c>
+      <c r="AJ156" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AK156" t="inlineStr">
+        <is>
+          <t>2712</t>
         </is>
       </c>
     </row>
@@ -17798,6 +18686,8 @@
       <c r="AG157" t="inlineStr"/>
       <c r="AH157" s="3" t="inlineStr"/>
       <c r="AI157" t="inlineStr"/>
+      <c r="AJ157" s="3" t="inlineStr"/>
+      <c r="AK157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -17902,7 +18792,13 @@
       <c r="AH158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI158" t="inlineStr">
+      <c r="AI158" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18011,9 +18907,15 @@
       <c r="AH159" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AI159" t="inlineStr">
-        <is>
-          <t>2527</t>
+      <c r="AI159" t="n">
+        <v>2527</v>
+      </c>
+      <c r="AJ159" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK159" t="inlineStr">
+        <is>
+          <t>2551</t>
         </is>
       </c>
     </row>
@@ -18075,6 +18977,8 @@
       <c r="AG160" t="inlineStr"/>
       <c r="AH160" s="3" t="inlineStr"/>
       <c r="AI160" t="inlineStr"/>
+      <c r="AJ160" s="3" t="inlineStr"/>
+      <c r="AK160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -18167,9 +19071,15 @@
       <c r="AH161" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AI161" t="inlineStr">
-        <is>
-          <t>2489</t>
+      <c r="AI161" t="n">
+        <v>2489</v>
+      </c>
+      <c r="AJ161" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="AK161" t="inlineStr">
+        <is>
+          <t>2632</t>
         </is>
       </c>
     </row>
@@ -18264,9 +19174,15 @@
       <c r="AH162" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="AI162" t="inlineStr">
-        <is>
-          <t>2496</t>
+      <c r="AI162" t="n">
+        <v>2496</v>
+      </c>
+      <c r="AJ162" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK162" t="inlineStr">
+        <is>
+          <t>2570</t>
         </is>
       </c>
     </row>
@@ -18357,9 +19273,15 @@
       <c r="AH163" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AI163" t="inlineStr">
-        <is>
-          <t>2599</t>
+      <c r="AI163" t="n">
+        <v>2599</v>
+      </c>
+      <c r="AJ163" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK163" t="inlineStr">
+        <is>
+          <t>2548</t>
         </is>
       </c>
     </row>
@@ -18434,9 +19356,15 @@
       <c r="AH164" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AI164" t="inlineStr">
-        <is>
-          <t>2505</t>
+      <c r="AI164" t="n">
+        <v>2505</v>
+      </c>
+      <c r="AJ164" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK164" t="inlineStr">
+        <is>
+          <t>2473</t>
         </is>
       </c>
     </row>
@@ -18515,9 +19443,15 @@
       <c r="AH165" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AI165" t="inlineStr">
-        <is>
-          <t>2493</t>
+      <c r="AI165" t="n">
+        <v>2493</v>
+      </c>
+      <c r="AJ165" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="AK165" t="inlineStr">
+        <is>
+          <t>2530</t>
         </is>
       </c>
     </row>
@@ -18588,9 +19522,15 @@
       <c r="AH166" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI166" t="inlineStr">
-        <is>
-          <t>2464</t>
+      <c r="AI166" t="n">
+        <v>2464</v>
+      </c>
+      <c r="AJ166" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK166" t="inlineStr">
+        <is>
+          <t>2448</t>
         </is>
       </c>
     </row>
@@ -18649,7 +19589,13 @@
       <c r="AH167" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI167" t="inlineStr">
+      <c r="AI167" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ167" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK167" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18706,9 +19652,15 @@
       <c r="AH168" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI168" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="AI168" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ168" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AK168" t="inlineStr">
+        <is>
+          <t>1421</t>
         </is>
       </c>
     </row>
@@ -18759,11 +19711,11 @@
       <c r="AH169" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI169" t="inlineStr">
-        <is>
-          <t>2477</t>
-        </is>
-      </c>
+      <c r="AI169" t="n">
+        <v>2477</v>
+      </c>
+      <c r="AJ169" s="3" t="inlineStr"/>
+      <c r="AK169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="n">
@@ -18812,9 +19764,15 @@
       <c r="AH170" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="AI170" t="inlineStr">
-        <is>
-          <t>1469</t>
+      <c r="AI170" t="n">
+        <v>1469</v>
+      </c>
+      <c r="AJ170" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK170" t="inlineStr">
+        <is>
+          <t>1489</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-03-01 10:05:13
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK170"/>
+  <dimension ref="A1:AM170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -576,6 +576,16 @@
           <t>02-27_0</t>
         </is>
       </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>02-28_A</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>02-28_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -692,7 +702,13 @@
       <c r="AJ2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK2" t="inlineStr">
+      <c r="AK2" t="n">
+        <v>2512</v>
+      </c>
+      <c r="AL2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM2" t="inlineStr">
         <is>
           <t>2512</t>
         </is>
@@ -813,7 +829,13 @@
       <c r="AJ3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AK3" t="inlineStr">
+      <c r="AK3" t="n">
+        <v>3094</v>
+      </c>
+      <c r="AL3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM3" t="inlineStr">
         <is>
           <t>3094</t>
         </is>
@@ -934,7 +956,13 @@
       <c r="AJ4" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AK4" t="inlineStr">
+      <c r="AK4" t="n">
+        <v>3406</v>
+      </c>
+      <c r="AL4" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AM4" t="inlineStr">
         <is>
           <t>3406</t>
         </is>
@@ -1055,7 +1083,13 @@
       <c r="AJ5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AK5" t="inlineStr">
+      <c r="AK5" t="n">
+        <v>3102</v>
+      </c>
+      <c r="AL5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM5" t="inlineStr">
         <is>
           <t>3102</t>
         </is>
@@ -1176,7 +1210,13 @@
       <c r="AJ6" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AK6" t="inlineStr">
+      <c r="AK6" t="n">
+        <v>3141</v>
+      </c>
+      <c r="AL6" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM6" t="inlineStr">
         <is>
           <t>3141</t>
         </is>
@@ -1297,7 +1337,13 @@
       <c r="AJ7" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AK7" t="inlineStr">
+      <c r="AK7" t="n">
+        <v>3466</v>
+      </c>
+      <c r="AL7" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AM7" t="inlineStr">
         <is>
           <t>3466</t>
         </is>
@@ -1418,7 +1464,13 @@
       <c r="AJ8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AK8" t="inlineStr">
+      <c r="AK8" t="n">
+        <v>2984</v>
+      </c>
+      <c r="AL8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM8" t="inlineStr">
         <is>
           <t>2984</t>
         </is>
@@ -1539,7 +1591,13 @@
       <c r="AJ9" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AK9" t="inlineStr">
+      <c r="AK9" t="n">
+        <v>3095</v>
+      </c>
+      <c r="AL9" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AM9" t="inlineStr">
         <is>
           <t>3095</t>
         </is>
@@ -1660,7 +1718,13 @@
       <c r="AJ10" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AK10" t="inlineStr">
+      <c r="AK10" t="n">
+        <v>3188</v>
+      </c>
+      <c r="AL10" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AM10" t="inlineStr">
         <is>
           <t>3188</t>
         </is>
@@ -1781,7 +1845,13 @@
       <c r="AJ11" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AK11" t="inlineStr">
+      <c r="AK11" t="n">
+        <v>3105</v>
+      </c>
+      <c r="AL11" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM11" t="inlineStr">
         <is>
           <t>3105</t>
         </is>
@@ -1902,7 +1972,13 @@
       <c r="AJ12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK12" t="inlineStr">
+      <c r="AK12" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AL12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM12" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2023,7 +2099,13 @@
       <c r="AJ13" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="AK13" t="inlineStr">
+      <c r="AK13" t="n">
+        <v>3458</v>
+      </c>
+      <c r="AL13" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="AM13" t="inlineStr">
         <is>
           <t>3458</t>
         </is>
@@ -2144,7 +2226,13 @@
       <c r="AJ14" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AK14" t="inlineStr">
+      <c r="AK14" t="n">
+        <v>3150</v>
+      </c>
+      <c r="AL14" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AM14" t="inlineStr">
         <is>
           <t>3150</t>
         </is>
@@ -2265,7 +2353,13 @@
       <c r="AJ15" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK15" t="inlineStr">
+      <c r="AK15" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AL15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM15" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2386,7 +2480,13 @@
       <c r="AJ16" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="AK16" t="inlineStr">
+      <c r="AK16" t="n">
+        <v>3289</v>
+      </c>
+      <c r="AL16" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="AM16" t="inlineStr">
         <is>
           <t>3289</t>
         </is>
@@ -2507,7 +2607,13 @@
       <c r="AJ17" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AK17" t="inlineStr">
+      <c r="AK17" t="n">
+        <v>3111</v>
+      </c>
+      <c r="AL17" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AM17" t="inlineStr">
         <is>
           <t>3111</t>
         </is>
@@ -2628,7 +2734,13 @@
       <c r="AJ18" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AK18" t="inlineStr">
+      <c r="AK18" t="n">
+        <v>2919</v>
+      </c>
+      <c r="AL18" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM18" t="inlineStr">
         <is>
           <t>2919</t>
         </is>
@@ -2749,7 +2861,13 @@
       <c r="AJ19" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AK19" t="inlineStr">
+      <c r="AK19" t="n">
+        <v>3257</v>
+      </c>
+      <c r="AL19" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AM19" t="inlineStr">
         <is>
           <t>3257</t>
         </is>
@@ -2870,7 +2988,13 @@
       <c r="AJ20" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AK20" t="inlineStr">
+      <c r="AK20" t="n">
+        <v>3604</v>
+      </c>
+      <c r="AL20" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AM20" t="inlineStr">
         <is>
           <t>3604</t>
         </is>
@@ -2991,7 +3115,13 @@
       <c r="AJ21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK21" t="inlineStr">
+      <c r="AK21" t="n">
+        <v>2781</v>
+      </c>
+      <c r="AL21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM21" t="inlineStr">
         <is>
           <t>2781</t>
         </is>
@@ -3112,7 +3242,13 @@
       <c r="AJ22" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AK22" t="inlineStr">
+      <c r="AK22" t="n">
+        <v>3132</v>
+      </c>
+      <c r="AL22" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AM22" t="inlineStr">
         <is>
           <t>3132</t>
         </is>
@@ -3233,7 +3369,13 @@
       <c r="AJ23" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AK23" t="inlineStr">
+      <c r="AK23" t="n">
+        <v>2990</v>
+      </c>
+      <c r="AL23" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM23" t="inlineStr">
         <is>
           <t>2990</t>
         </is>
@@ -3354,7 +3496,13 @@
       <c r="AJ24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AK24" t="inlineStr">
+      <c r="AK24" t="n">
+        <v>3276</v>
+      </c>
+      <c r="AL24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AM24" t="inlineStr">
         <is>
           <t>3276</t>
         </is>
@@ -3475,7 +3623,13 @@
       <c r="AJ25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK25" t="inlineStr">
+      <c r="AK25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3596,7 +3750,13 @@
       <c r="AJ26" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AK26" t="inlineStr">
+      <c r="AK26" t="n">
+        <v>3330</v>
+      </c>
+      <c r="AL26" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AM26" t="inlineStr">
         <is>
           <t>3330</t>
         </is>
@@ -3717,7 +3877,13 @@
       <c r="AJ27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK27" t="inlineStr">
+      <c r="AK27" t="n">
+        <v>2891</v>
+      </c>
+      <c r="AL27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM27" t="inlineStr">
         <is>
           <t>2891</t>
         </is>
@@ -3838,7 +4004,13 @@
       <c r="AJ28" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="AK28" t="inlineStr">
+      <c r="AK28" t="n">
+        <v>3000</v>
+      </c>
+      <c r="AL28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="AM28" t="inlineStr">
         <is>
           <t>3000</t>
         </is>
@@ -3959,7 +4131,13 @@
       <c r="AJ29" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AK29" t="inlineStr">
+      <c r="AK29" t="n">
+        <v>3599</v>
+      </c>
+      <c r="AL29" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AM29" t="inlineStr">
         <is>
           <t>3599</t>
         </is>
@@ -4080,7 +4258,13 @@
       <c r="AJ30" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AK30" t="inlineStr">
+      <c r="AK30" t="n">
+        <v>3089</v>
+      </c>
+      <c r="AL30" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AM30" t="inlineStr">
         <is>
           <t>3089</t>
         </is>
@@ -4201,7 +4385,13 @@
       <c r="AJ31" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AK31" t="inlineStr">
+      <c r="AK31" t="n">
+        <v>3384</v>
+      </c>
+      <c r="AL31" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AM31" t="inlineStr">
         <is>
           <t>3384</t>
         </is>
@@ -4322,7 +4512,13 @@
       <c r="AJ32" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="AK32" t="inlineStr">
+      <c r="AK32" t="n">
+        <v>3312</v>
+      </c>
+      <c r="AL32" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="AM32" t="inlineStr">
         <is>
           <t>3312</t>
         </is>
@@ -4443,7 +4639,13 @@
       <c r="AJ33" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="AK33" t="inlineStr">
+      <c r="AK33" t="n">
+        <v>3023</v>
+      </c>
+      <c r="AL33" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="AM33" t="inlineStr">
         <is>
           <t>3023</t>
         </is>
@@ -4564,7 +4766,13 @@
       <c r="AJ34" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AK34" t="inlineStr">
+      <c r="AK34" t="n">
+        <v>3179</v>
+      </c>
+      <c r="AL34" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AM34" t="inlineStr">
         <is>
           <t>3179</t>
         </is>
@@ -4685,7 +4893,13 @@
       <c r="AJ35" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AK35" t="inlineStr">
+      <c r="AK35" t="n">
+        <v>3313</v>
+      </c>
+      <c r="AL35" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AM35" t="inlineStr">
         <is>
           <t>3313</t>
         </is>
@@ -4806,7 +5020,13 @@
       <c r="AJ36" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AK36" t="inlineStr">
+      <c r="AK36" t="n">
+        <v>3061</v>
+      </c>
+      <c r="AL36" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM36" t="inlineStr">
         <is>
           <t>3061</t>
         </is>
@@ -4927,7 +5147,13 @@
       <c r="AJ37" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AK37" t="inlineStr">
+      <c r="AK37" t="n">
+        <v>3114</v>
+      </c>
+      <c r="AL37" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AM37" t="inlineStr">
         <is>
           <t>3114</t>
         </is>
@@ -5048,7 +5274,13 @@
       <c r="AJ38" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AK38" t="inlineStr">
+      <c r="AK38" t="n">
+        <v>3205</v>
+      </c>
+      <c r="AL38" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AM38" t="inlineStr">
         <is>
           <t>3205</t>
         </is>
@@ -5169,7 +5401,13 @@
       <c r="AJ39" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AK39" t="inlineStr">
+      <c r="AK39" t="n">
+        <v>3200</v>
+      </c>
+      <c r="AL39" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AM39" t="inlineStr">
         <is>
           <t>3200</t>
         </is>
@@ -5290,7 +5528,13 @@
       <c r="AJ40" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AK40" t="inlineStr">
+      <c r="AK40" t="n">
+        <v>3382</v>
+      </c>
+      <c r="AL40" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AM40" t="inlineStr">
         <is>
           <t>3382</t>
         </is>
@@ -5411,7 +5655,13 @@
       <c r="AJ41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK41" t="inlineStr">
+      <c r="AK41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM41" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5532,7 +5782,13 @@
       <c r="AJ42" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AK42" t="inlineStr">
+      <c r="AK42" t="n">
+        <v>3512</v>
+      </c>
+      <c r="AL42" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AM42" t="inlineStr">
         <is>
           <t>3512</t>
         </is>
@@ -5653,7 +5909,13 @@
       <c r="AJ43" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AK43" t="inlineStr">
+      <c r="AK43" t="n">
+        <v>3371</v>
+      </c>
+      <c r="AL43" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AM43" t="inlineStr">
         <is>
           <t>3371</t>
         </is>
@@ -5774,7 +6036,13 @@
       <c r="AJ44" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AK44" t="inlineStr">
+      <c r="AK44" t="n">
+        <v>3147</v>
+      </c>
+      <c r="AL44" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AM44" t="inlineStr">
         <is>
           <t>3147</t>
         </is>
@@ -5895,7 +6163,13 @@
       <c r="AJ45" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AK45" t="inlineStr">
+      <c r="AK45" t="n">
+        <v>3115</v>
+      </c>
+      <c r="AL45" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AM45" t="inlineStr">
         <is>
           <t>3115</t>
         </is>
@@ -6016,7 +6290,13 @@
       <c r="AJ46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AK46" t="inlineStr">
+      <c r="AK46" t="n">
+        <v>3161</v>
+      </c>
+      <c r="AL46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AM46" t="inlineStr">
         <is>
           <t>3161</t>
         </is>
@@ -6137,7 +6417,13 @@
       <c r="AJ47" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AK47" t="inlineStr">
+      <c r="AK47" t="n">
+        <v>3103</v>
+      </c>
+      <c r="AL47" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM47" t="inlineStr">
         <is>
           <t>3103</t>
         </is>
@@ -6258,7 +6544,13 @@
       <c r="AJ48" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AK48" t="inlineStr">
+      <c r="AK48" t="n">
+        <v>3372</v>
+      </c>
+      <c r="AL48" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AM48" t="inlineStr">
         <is>
           <t>3372</t>
         </is>
@@ -6379,7 +6671,13 @@
       <c r="AJ49" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AK49" t="inlineStr">
+      <c r="AK49" t="n">
+        <v>2769</v>
+      </c>
+      <c r="AL49" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM49" t="inlineStr">
         <is>
           <t>2769</t>
         </is>
@@ -6500,7 +6798,13 @@
       <c r="AJ50" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AK50" t="inlineStr">
+      <c r="AK50" t="n">
+        <v>3233</v>
+      </c>
+      <c r="AL50" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AM50" t="inlineStr">
         <is>
           <t>3233</t>
         </is>
@@ -6621,7 +6925,13 @@
       <c r="AJ51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK51" t="inlineStr">
+      <c r="AK51" t="n">
+        <v>2481</v>
+      </c>
+      <c r="AL51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM51" t="inlineStr">
         <is>
           <t>2481</t>
         </is>
@@ -6742,7 +7052,13 @@
       <c r="AJ52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK52" t="inlineStr">
+      <c r="AK52" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM52" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6863,7 +7179,13 @@
       <c r="AJ53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK53" t="inlineStr">
+      <c r="AK53" t="n">
+        <v>2567</v>
+      </c>
+      <c r="AL53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM53" t="inlineStr">
         <is>
           <t>2567</t>
         </is>
@@ -6984,7 +7306,13 @@
       <c r="AJ54" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AK54" t="inlineStr">
+      <c r="AK54" t="n">
+        <v>3336</v>
+      </c>
+      <c r="AL54" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AM54" t="inlineStr">
         <is>
           <t>3336</t>
         </is>
@@ -7105,7 +7433,13 @@
       <c r="AJ55" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AK55" t="inlineStr">
+      <c r="AK55" t="n">
+        <v>2924</v>
+      </c>
+      <c r="AL55" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AM55" t="inlineStr">
         <is>
           <t>2924</t>
         </is>
@@ -7226,7 +7560,13 @@
       <c r="AJ56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AK56" t="inlineStr">
+      <c r="AK56" t="n">
+        <v>2915</v>
+      </c>
+      <c r="AL56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM56" t="inlineStr">
         <is>
           <t>2915</t>
         </is>
@@ -7347,7 +7687,13 @@
       <c r="AJ57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AK57" t="inlineStr">
+      <c r="AK57" t="n">
+        <v>3108</v>
+      </c>
+      <c r="AL57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM57" t="inlineStr">
         <is>
           <t>3108</t>
         </is>
@@ -7468,7 +7814,13 @@
       <c r="AJ58" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AK58" t="inlineStr">
+      <c r="AK58" t="n">
+        <v>2892</v>
+      </c>
+      <c r="AL58" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AM58" t="inlineStr">
         <is>
           <t>2892</t>
         </is>
@@ -7524,6 +7876,8 @@
       <c r="AI59" t="inlineStr"/>
       <c r="AJ59" s="3" t="inlineStr"/>
       <c r="AK59" t="inlineStr"/>
+      <c r="AL59" s="3" t="inlineStr"/>
+      <c r="AM59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -7575,6 +7929,8 @@
       <c r="AI60" t="inlineStr"/>
       <c r="AJ60" s="3" t="inlineStr"/>
       <c r="AK60" t="inlineStr"/>
+      <c r="AL60" s="3" t="inlineStr"/>
+      <c r="AM60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -7691,7 +8047,13 @@
       <c r="AJ61" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="AK61" t="inlineStr">
+      <c r="AK61" t="n">
+        <v>2978</v>
+      </c>
+      <c r="AL61" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="AM61" t="inlineStr">
         <is>
           <t>2978</t>
         </is>
@@ -7812,7 +8174,13 @@
       <c r="AJ62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK62" t="inlineStr">
+      <c r="AK62" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7933,7 +8301,13 @@
       <c r="AJ63" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="AK63" t="inlineStr">
+      <c r="AK63" t="n">
+        <v>3181</v>
+      </c>
+      <c r="AL63" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AM63" t="inlineStr">
         <is>
           <t>3181</t>
         </is>
@@ -8054,7 +8428,13 @@
       <c r="AJ64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK64" t="inlineStr">
+      <c r="AK64" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AL64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM64" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -8110,6 +8490,8 @@
       <c r="AI65" t="inlineStr"/>
       <c r="AJ65" s="3" t="inlineStr"/>
       <c r="AK65" t="inlineStr"/>
+      <c r="AL65" s="3" t="inlineStr"/>
+      <c r="AM65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -8226,7 +8608,13 @@
       <c r="AJ66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK66" t="inlineStr">
+      <c r="AK66" t="n">
+        <v>2495</v>
+      </c>
+      <c r="AL66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM66" t="inlineStr">
         <is>
           <t>2495</t>
         </is>
@@ -8347,7 +8735,13 @@
       <c r="AJ67" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AK67" t="inlineStr">
+      <c r="AK67" t="n">
+        <v>3101</v>
+      </c>
+      <c r="AL67" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AM67" t="inlineStr">
         <is>
           <t>3101</t>
         </is>
@@ -8468,7 +8862,13 @@
       <c r="AJ68" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AK68" t="inlineStr">
+      <c r="AK68" t="n">
+        <v>3233</v>
+      </c>
+      <c r="AL68" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AM68" t="inlineStr">
         <is>
           <t>3233</t>
         </is>
@@ -8589,7 +8989,13 @@
       <c r="AJ69" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AK69" t="inlineStr">
+      <c r="AK69" t="n">
+        <v>2895</v>
+      </c>
+      <c r="AL69" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AM69" t="inlineStr">
         <is>
           <t>2895</t>
         </is>
@@ -8710,7 +9116,13 @@
       <c r="AJ70" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="AK70" t="inlineStr">
+      <c r="AK70" t="n">
+        <v>2494</v>
+      </c>
+      <c r="AL70" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM70" t="inlineStr">
         <is>
           <t>2494</t>
         </is>
@@ -8831,7 +9243,13 @@
       <c r="AJ71" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AK71" t="inlineStr">
+      <c r="AK71" t="n">
+        <v>2945</v>
+      </c>
+      <c r="AL71" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AM71" t="inlineStr">
         <is>
           <t>2945</t>
         </is>
@@ -8952,7 +9370,13 @@
       <c r="AJ72" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="AK72" t="inlineStr">
+      <c r="AK72" t="n">
+        <v>2643</v>
+      </c>
+      <c r="AL72" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="AM72" t="inlineStr">
         <is>
           <t>2643</t>
         </is>
@@ -9073,7 +9497,13 @@
       <c r="AJ73" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AK73" t="inlineStr">
+      <c r="AK73" t="n">
+        <v>2990</v>
+      </c>
+      <c r="AL73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM73" t="inlineStr">
         <is>
           <t>2990</t>
         </is>
@@ -9194,7 +9624,13 @@
       <c r="AJ74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK74" t="inlineStr">
+      <c r="AK74" t="n">
+        <v>2597</v>
+      </c>
+      <c r="AL74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM74" t="inlineStr">
         <is>
           <t>2597</t>
         </is>
@@ -9315,7 +9751,13 @@
       <c r="AJ75" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="AK75" t="inlineStr">
+      <c r="AK75" t="n">
+        <v>2905</v>
+      </c>
+      <c r="AL75" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="AM75" t="inlineStr">
         <is>
           <t>2905</t>
         </is>
@@ -9436,7 +9878,13 @@
       <c r="AJ76" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AK76" t="inlineStr">
+      <c r="AK76" t="n">
+        <v>3215</v>
+      </c>
+      <c r="AL76" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AM76" t="inlineStr">
         <is>
           <t>3215</t>
         </is>
@@ -9557,7 +10005,13 @@
       <c r="AJ77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK77" t="inlineStr">
+      <c r="AK77" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM77" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9678,7 +10132,13 @@
       <c r="AJ78" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AK78" t="inlineStr">
+      <c r="AK78" t="n">
+        <v>3168</v>
+      </c>
+      <c r="AL78" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AM78" t="inlineStr">
         <is>
           <t>3168</t>
         </is>
@@ -9799,7 +10259,13 @@
       <c r="AJ79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK79" t="inlineStr">
+      <c r="AK79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9920,7 +10386,13 @@
       <c r="AJ80" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="AK80" t="inlineStr">
+      <c r="AK80" t="n">
+        <v>3045</v>
+      </c>
+      <c r="AL80" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="AM80" t="inlineStr">
         <is>
           <t>3045</t>
         </is>
@@ -10041,7 +10513,13 @@
       <c r="AJ81" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AK81" t="inlineStr">
+      <c r="AK81" t="n">
+        <v>3067</v>
+      </c>
+      <c r="AL81" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AM81" t="inlineStr">
         <is>
           <t>3067</t>
         </is>
@@ -10162,7 +10640,13 @@
       <c r="AJ82" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AK82" t="inlineStr">
+      <c r="AK82" t="n">
+        <v>3132</v>
+      </c>
+      <c r="AL82" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM82" t="inlineStr">
         <is>
           <t>3132</t>
         </is>
@@ -10283,7 +10767,13 @@
       <c r="AJ83" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AK83" t="inlineStr">
+      <c r="AK83" t="n">
+        <v>2936</v>
+      </c>
+      <c r="AL83" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AM83" t="inlineStr">
         <is>
           <t>2936</t>
         </is>
@@ -10399,6 +10889,8 @@
       <c r="AI84" t="inlineStr"/>
       <c r="AJ84" s="3" t="inlineStr"/>
       <c r="AK84" t="inlineStr"/>
+      <c r="AL84" s="3" t="inlineStr"/>
+      <c r="AM84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -10515,7 +11007,13 @@
       <c r="AJ85" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AK85" t="inlineStr">
+      <c r="AK85" t="n">
+        <v>2856</v>
+      </c>
+      <c r="AL85" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM85" t="inlineStr">
         <is>
           <t>2856</t>
         </is>
@@ -10636,7 +11134,13 @@
       <c r="AJ86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK86" t="inlineStr">
+      <c r="AK86" t="n">
+        <v>2467</v>
+      </c>
+      <c r="AL86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM86" t="inlineStr">
         <is>
           <t>2467</t>
         </is>
@@ -10757,7 +11261,13 @@
       <c r="AJ87" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AK87" t="inlineStr">
+      <c r="AK87" t="n">
+        <v>3176</v>
+      </c>
+      <c r="AL87" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AM87" t="inlineStr">
         <is>
           <t>3176</t>
         </is>
@@ -10878,7 +11388,13 @@
       <c r="AJ88" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AK88" t="inlineStr">
+      <c r="AK88" t="n">
+        <v>2557</v>
+      </c>
+      <c r="AL88" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM88" t="inlineStr">
         <is>
           <t>2557</t>
         </is>
@@ -10999,7 +11515,13 @@
       <c r="AJ89" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AK89" t="inlineStr">
+      <c r="AK89" t="n">
+        <v>2766</v>
+      </c>
+      <c r="AL89" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM89" t="inlineStr">
         <is>
           <t>2766</t>
         </is>
@@ -11120,7 +11642,13 @@
       <c r="AJ90" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AK90" t="inlineStr">
+      <c r="AK90" t="n">
+        <v>2580</v>
+      </c>
+      <c r="AL90" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM90" t="inlineStr">
         <is>
           <t>2580</t>
         </is>
@@ -11241,7 +11769,13 @@
       <c r="AJ91" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AK91" t="inlineStr">
+      <c r="AK91" t="n">
+        <v>2515</v>
+      </c>
+      <c r="AL91" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM91" t="inlineStr">
         <is>
           <t>2515</t>
         </is>
@@ -11362,7 +11896,13 @@
       <c r="AJ92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK92" t="inlineStr">
+      <c r="AK92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11483,7 +12023,13 @@
       <c r="AJ93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK93" t="inlineStr">
+      <c r="AK93" t="n">
+        <v>2395</v>
+      </c>
+      <c r="AL93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM93" t="inlineStr">
         <is>
           <t>2395</t>
         </is>
@@ -11604,7 +12150,13 @@
       <c r="AJ94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK94" t="inlineStr">
+      <c r="AK94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11725,7 +12277,13 @@
       <c r="AJ95" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AK95" t="inlineStr">
+      <c r="AK95" t="n">
+        <v>2496</v>
+      </c>
+      <c r="AL95" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM95" t="inlineStr">
         <is>
           <t>2496</t>
         </is>
@@ -11846,7 +12404,13 @@
       <c r="AJ96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK96" t="inlineStr">
+      <c r="AK96" t="n">
+        <v>2545</v>
+      </c>
+      <c r="AL96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM96" t="inlineStr">
         <is>
           <t>2545</t>
         </is>
@@ -11967,7 +12531,13 @@
       <c r="AJ97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK97" t="inlineStr">
+      <c r="AK97" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AL97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM97" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -12088,7 +12658,13 @@
       <c r="AJ98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK98" t="inlineStr">
+      <c r="AK98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12209,7 +12785,13 @@
       <c r="AJ99" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="AK99" t="inlineStr">
+      <c r="AK99" t="n">
+        <v>2690</v>
+      </c>
+      <c r="AL99" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AM99" t="inlineStr">
         <is>
           <t>2690</t>
         </is>
@@ -12330,7 +12912,13 @@
       <c r="AJ100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK100" t="inlineStr">
+      <c r="AK100" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AL100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM100" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -12451,7 +13039,13 @@
       <c r="AJ101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AK101" t="inlineStr">
+      <c r="AK101" t="n">
+        <v>3075</v>
+      </c>
+      <c r="AL101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AM101" t="inlineStr">
         <is>
           <t>3075</t>
         </is>
@@ -12572,7 +13166,13 @@
       <c r="AJ102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AK102" t="inlineStr">
+      <c r="AK102" t="n">
+        <v>2851</v>
+      </c>
+      <c r="AL102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM102" t="inlineStr">
         <is>
           <t>2851</t>
         </is>
@@ -12693,7 +13293,13 @@
       <c r="AJ103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK103" t="inlineStr">
+      <c r="AK103" t="n">
+        <v>2475</v>
+      </c>
+      <c r="AL103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM103" t="inlineStr">
         <is>
           <t>2475</t>
         </is>
@@ -12814,7 +13420,13 @@
       <c r="AJ104" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AK104" t="inlineStr">
+      <c r="AK104" t="n">
+        <v>3068</v>
+      </c>
+      <c r="AL104" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AM104" t="inlineStr">
         <is>
           <t>3068</t>
         </is>
@@ -12935,7 +13547,13 @@
       <c r="AJ105" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="AK105" t="inlineStr">
+      <c r="AK105" t="n">
+        <v>2932</v>
+      </c>
+      <c r="AL105" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AM105" t="inlineStr">
         <is>
           <t>2932</t>
         </is>
@@ -13056,7 +13674,13 @@
       <c r="AJ106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK106" t="inlineStr">
+      <c r="AK106" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13177,7 +13801,13 @@
       <c r="AJ107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK107" t="inlineStr">
+      <c r="AK107" t="n">
+        <v>2506</v>
+      </c>
+      <c r="AL107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM107" t="inlineStr">
         <is>
           <t>2506</t>
         </is>
@@ -13298,7 +13928,13 @@
       <c r="AJ108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK108" t="inlineStr">
+      <c r="AK108" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13419,7 +14055,13 @@
       <c r="AJ109" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="AK109" t="inlineStr">
+      <c r="AK109" t="n">
+        <v>2713</v>
+      </c>
+      <c r="AL109" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="AM109" t="inlineStr">
         <is>
           <t>2713</t>
         </is>
@@ -13540,7 +14182,13 @@
       <c r="AJ110" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AK110" t="inlineStr">
+      <c r="AK110" t="n">
+        <v>2796</v>
+      </c>
+      <c r="AL110" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AM110" t="inlineStr">
         <is>
           <t>2796</t>
         </is>
@@ -13661,7 +14309,13 @@
       <c r="AJ111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK111" t="inlineStr">
+      <c r="AK111" t="n">
+        <v>2497</v>
+      </c>
+      <c r="AL111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM111" t="inlineStr">
         <is>
           <t>2497</t>
         </is>
@@ -13782,7 +14436,13 @@
       <c r="AJ112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK112" t="inlineStr">
+      <c r="AK112" t="n">
+        <v>2508</v>
+      </c>
+      <c r="AL112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM112" t="inlineStr">
         <is>
           <t>2508</t>
         </is>
@@ -13903,7 +14563,13 @@
       <c r="AJ113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK113" t="inlineStr">
+      <c r="AK113" t="n">
+        <v>2611</v>
+      </c>
+      <c r="AL113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM113" t="inlineStr">
         <is>
           <t>2611</t>
         </is>
@@ -14024,7 +14690,13 @@
       <c r="AJ114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK114" t="inlineStr">
+      <c r="AK114" t="n">
+        <v>2690</v>
+      </c>
+      <c r="AL114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM114" t="inlineStr">
         <is>
           <t>2690</t>
         </is>
@@ -14145,7 +14817,13 @@
       <c r="AJ115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK115" t="inlineStr">
+      <c r="AK115" t="n">
+        <v>2027</v>
+      </c>
+      <c r="AL115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM115" t="inlineStr">
         <is>
           <t>2027</t>
         </is>
@@ -14266,7 +14944,13 @@
       <c r="AJ116" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AK116" t="inlineStr">
+      <c r="AK116" t="n">
+        <v>2665</v>
+      </c>
+      <c r="AL116" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM116" t="inlineStr">
         <is>
           <t>2665</t>
         </is>
@@ -14387,7 +15071,13 @@
       <c r="AJ117" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AK117" t="inlineStr">
+      <c r="AK117" t="n">
+        <v>2791</v>
+      </c>
+      <c r="AL117" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AM117" t="inlineStr">
         <is>
           <t>2791</t>
         </is>
@@ -14508,7 +15198,13 @@
       <c r="AJ118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK118" t="inlineStr">
+      <c r="AK118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14629,7 +15325,13 @@
       <c r="AJ119" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AK119" t="inlineStr">
+      <c r="AK119" t="n">
+        <v>2866</v>
+      </c>
+      <c r="AL119" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AM119" t="inlineStr">
         <is>
           <t>2866</t>
         </is>
@@ -14750,7 +15452,13 @@
       <c r="AJ120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK120" t="inlineStr">
+      <c r="AK120" t="n">
+        <v>2421</v>
+      </c>
+      <c r="AL120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM120" t="inlineStr">
         <is>
           <t>2421</t>
         </is>
@@ -14871,7 +15579,13 @@
       <c r="AJ121" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="AK121" t="inlineStr">
+      <c r="AK121" t="n">
+        <v>2651</v>
+      </c>
+      <c r="AL121" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AM121" t="inlineStr">
         <is>
           <t>2651</t>
         </is>
@@ -14992,7 +15706,13 @@
       <c r="AJ122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK122" t="inlineStr">
+      <c r="AK122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15113,7 +15833,13 @@
       <c r="AJ123" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="AK123" t="inlineStr">
+      <c r="AK123" t="n">
+        <v>2622</v>
+      </c>
+      <c r="AL123" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="AM123" t="inlineStr">
         <is>
           <t>2622</t>
         </is>
@@ -15234,7 +15960,13 @@
       <c r="AJ124" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="AK124" t="inlineStr">
+      <c r="AK124" t="n">
+        <v>2565</v>
+      </c>
+      <c r="AL124" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="AM124" t="inlineStr">
         <is>
           <t>2565</t>
         </is>
@@ -15355,7 +16087,13 @@
       <c r="AJ125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK125" t="inlineStr">
+      <c r="AK125" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM125" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15476,7 +16214,13 @@
       <c r="AJ126" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="AK126" t="inlineStr">
+      <c r="AK126" t="n">
+        <v>2632</v>
+      </c>
+      <c r="AL126" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AM126" t="inlineStr">
         <is>
           <t>2632</t>
         </is>
@@ -15597,7 +16341,13 @@
       <c r="AJ127" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AK127" t="inlineStr">
+      <c r="AK127" t="n">
+        <v>2395</v>
+      </c>
+      <c r="AL127" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM127" t="inlineStr">
         <is>
           <t>2395</t>
         </is>
@@ -15718,7 +16468,13 @@
       <c r="AJ128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK128" t="inlineStr">
+      <c r="AK128" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15839,7 +16595,13 @@
       <c r="AJ129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK129" t="inlineStr">
+      <c r="AK129" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15960,7 +16722,13 @@
       <c r="AJ130" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AK130" t="inlineStr">
+      <c r="AK130" t="n">
+        <v>2492</v>
+      </c>
+      <c r="AL130" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AM130" t="inlineStr">
         <is>
           <t>2492</t>
         </is>
@@ -16081,7 +16849,13 @@
       <c r="AJ131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK131" t="inlineStr">
+      <c r="AK131" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16202,7 +16976,13 @@
       <c r="AJ132" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AK132" t="inlineStr">
+      <c r="AK132" t="n">
+        <v>2470</v>
+      </c>
+      <c r="AL132" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM132" t="inlineStr">
         <is>
           <t>2470</t>
         </is>
@@ -16323,7 +17103,13 @@
       <c r="AJ133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK133" t="inlineStr">
+      <c r="AK133" t="n">
+        <v>2424</v>
+      </c>
+      <c r="AL133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM133" t="inlineStr">
         <is>
           <t>2424</t>
         </is>
@@ -16403,6 +17189,8 @@
       <c r="AI134" t="inlineStr"/>
       <c r="AJ134" s="3" t="inlineStr"/>
       <c r="AK134" t="inlineStr"/>
+      <c r="AL134" s="3" t="inlineStr"/>
+      <c r="AM134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -16470,6 +17258,8 @@
       <c r="AI135" t="inlineStr"/>
       <c r="AJ135" s="3" t="inlineStr"/>
       <c r="AK135" t="inlineStr"/>
+      <c r="AL135" s="3" t="inlineStr"/>
+      <c r="AM135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -16586,7 +17376,13 @@
       <c r="AJ136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK136" t="inlineStr">
+      <c r="AK136" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM136" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16707,7 +17503,13 @@
       <c r="AJ137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK137" t="inlineStr">
+      <c r="AK137" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16779,6 +17581,8 @@
       <c r="AI138" t="inlineStr"/>
       <c r="AJ138" s="3" t="inlineStr"/>
       <c r="AK138" t="inlineStr"/>
+      <c r="AL138" s="3" t="inlineStr"/>
+      <c r="AM138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -16895,7 +17699,13 @@
       <c r="AJ139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK139" t="inlineStr">
+      <c r="AK139" t="n">
+        <v>1997</v>
+      </c>
+      <c r="AL139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM139" t="inlineStr">
         <is>
           <t>1997</t>
         </is>
@@ -17016,7 +17826,13 @@
       <c r="AJ140" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AK140" t="inlineStr">
+      <c r="AK140" t="n">
+        <v>2475</v>
+      </c>
+      <c r="AL140" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AM140" t="inlineStr">
         <is>
           <t>2475</t>
         </is>
@@ -17088,6 +17904,8 @@
       <c r="AI141" t="inlineStr"/>
       <c r="AJ141" s="3" t="inlineStr"/>
       <c r="AK141" t="inlineStr"/>
+      <c r="AL141" s="3" t="inlineStr"/>
+      <c r="AM141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -17204,7 +18022,13 @@
       <c r="AJ142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK142" t="inlineStr">
+      <c r="AK142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM142" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -17276,6 +18100,8 @@
       <c r="AI143" t="inlineStr"/>
       <c r="AJ143" s="3" t="inlineStr"/>
       <c r="AK143" t="inlineStr"/>
+      <c r="AL143" s="3" t="inlineStr"/>
+      <c r="AM143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -17343,6 +18169,8 @@
       <c r="AI144" t="inlineStr"/>
       <c r="AJ144" s="3" t="inlineStr"/>
       <c r="AK144" t="inlineStr"/>
+      <c r="AL144" s="3" t="inlineStr"/>
+      <c r="AM144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -17410,6 +18238,8 @@
       <c r="AI145" t="inlineStr"/>
       <c r="AJ145" s="3" t="inlineStr"/>
       <c r="AK145" t="inlineStr"/>
+      <c r="AL145" s="3" t="inlineStr"/>
+      <c r="AM145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -17477,6 +18307,8 @@
       <c r="AI146" t="inlineStr"/>
       <c r="AJ146" s="3" t="inlineStr"/>
       <c r="AK146" t="inlineStr"/>
+      <c r="AL146" s="3" t="inlineStr"/>
+      <c r="AM146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -17544,6 +18376,8 @@
       <c r="AI147" t="inlineStr"/>
       <c r="AJ147" s="3" t="inlineStr"/>
       <c r="AK147" t="inlineStr"/>
+      <c r="AL147" s="3" t="inlineStr"/>
+      <c r="AM147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -17660,7 +18494,13 @@
       <c r="AJ148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK148" t="inlineStr">
+      <c r="AK148" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -17781,7 +18621,13 @@
       <c r="AJ149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK149" t="inlineStr">
+      <c r="AK149" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AL149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM149" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -17902,7 +18748,13 @@
       <c r="AJ150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK150" t="inlineStr">
+      <c r="AK150" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18023,7 +18875,13 @@
       <c r="AJ151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK151" t="inlineStr">
+      <c r="AK151" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18144,7 +19002,13 @@
       <c r="AJ152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK152" t="inlineStr">
+      <c r="AK152" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18265,7 +19129,13 @@
       <c r="AJ153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK153" t="inlineStr">
+      <c r="AK153" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18386,7 +19256,13 @@
       <c r="AJ154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK154" t="inlineStr">
+      <c r="AK154" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18507,7 +19383,13 @@
       <c r="AJ155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK155" t="inlineStr">
+      <c r="AK155" t="n">
+        <v>2490</v>
+      </c>
+      <c r="AL155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM155" t="inlineStr">
         <is>
           <t>2490</t>
         </is>
@@ -18622,7 +19504,13 @@
       <c r="AJ156" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="AK156" t="inlineStr">
+      <c r="AK156" t="n">
+        <v>2712</v>
+      </c>
+      <c r="AL156" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AM156" t="inlineStr">
         <is>
           <t>2712</t>
         </is>
@@ -18688,6 +19576,8 @@
       <c r="AI157" t="inlineStr"/>
       <c r="AJ157" s="3" t="inlineStr"/>
       <c r="AK157" t="inlineStr"/>
+      <c r="AL157" s="3" t="inlineStr"/>
+      <c r="AM157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -18798,7 +19688,13 @@
       <c r="AJ158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK158" t="inlineStr">
+      <c r="AK158" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18913,7 +19809,13 @@
       <c r="AJ159" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AK159" t="inlineStr">
+      <c r="AK159" t="n">
+        <v>2551</v>
+      </c>
+      <c r="AL159" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM159" t="inlineStr">
         <is>
           <t>2551</t>
         </is>
@@ -18979,6 +19881,8 @@
       <c r="AI160" t="inlineStr"/>
       <c r="AJ160" s="3" t="inlineStr"/>
       <c r="AK160" t="inlineStr"/>
+      <c r="AL160" s="3" t="inlineStr"/>
+      <c r="AM160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -19077,7 +19981,13 @@
       <c r="AJ161" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="AK161" t="inlineStr">
+      <c r="AK161" t="n">
+        <v>2632</v>
+      </c>
+      <c r="AL161" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="AM161" t="inlineStr">
         <is>
           <t>2632</t>
         </is>
@@ -19180,7 +20090,13 @@
       <c r="AJ162" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AK162" t="inlineStr">
+      <c r="AK162" t="n">
+        <v>2570</v>
+      </c>
+      <c r="AL162" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM162" t="inlineStr">
         <is>
           <t>2570</t>
         </is>
@@ -19279,7 +20195,13 @@
       <c r="AJ163" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK163" t="inlineStr">
+      <c r="AK163" t="n">
+        <v>2548</v>
+      </c>
+      <c r="AL163" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM163" t="inlineStr">
         <is>
           <t>2548</t>
         </is>
@@ -19362,7 +20284,13 @@
       <c r="AJ164" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK164" t="inlineStr">
+      <c r="AK164" t="n">
+        <v>2473</v>
+      </c>
+      <c r="AL164" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM164" t="inlineStr">
         <is>
           <t>2473</t>
         </is>
@@ -19449,7 +20377,13 @@
       <c r="AJ165" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="AK165" t="inlineStr">
+      <c r="AK165" t="n">
+        <v>2530</v>
+      </c>
+      <c r="AL165" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="AM165" t="inlineStr">
         <is>
           <t>2530</t>
         </is>
@@ -19528,7 +20462,13 @@
       <c r="AJ166" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK166" t="inlineStr">
+      <c r="AK166" t="n">
+        <v>2448</v>
+      </c>
+      <c r="AL166" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM166" t="inlineStr">
         <is>
           <t>2448</t>
         </is>
@@ -19595,7 +20535,13 @@
       <c r="AJ167" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK167" t="inlineStr">
+      <c r="AK167" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL167" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM167" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -19658,7 +20604,13 @@
       <c r="AJ168" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="AK168" t="inlineStr">
+      <c r="AK168" t="n">
+        <v>1421</v>
+      </c>
+      <c r="AL168" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AM168" t="inlineStr">
         <is>
           <t>1421</t>
         </is>
@@ -19716,6 +20668,8 @@
       </c>
       <c r="AJ169" s="3" t="inlineStr"/>
       <c r="AK169" t="inlineStr"/>
+      <c r="AL169" s="3" t="inlineStr"/>
+      <c r="AM169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="n">
@@ -19770,7 +20724,13 @@
       <c r="AJ170" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK170" t="inlineStr">
+      <c r="AK170" t="n">
+        <v>1489</v>
+      </c>
+      <c r="AL170" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM170" t="inlineStr">
         <is>
           <t>1489</t>
         </is>

</xml_diff>

<commit_message>
Code updated 23-03-02 11:30:35
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AM170"/>
+  <dimension ref="A1:AO173"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -586,6 +586,16 @@
           <t>02-28_0</t>
         </is>
       </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>03-01_A</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>03-01_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -708,9 +718,15 @@
       <c r="AL2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM2" t="inlineStr">
-        <is>
-          <t>2512</t>
+      <c r="AM2" t="n">
+        <v>2512</v>
+      </c>
+      <c r="AN2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO2" t="inlineStr">
+        <is>
+          <t>2517</t>
         </is>
       </c>
     </row>
@@ -835,9 +851,15 @@
       <c r="AL3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AM3" t="inlineStr">
-        <is>
-          <t>3094</t>
+      <c r="AM3" t="n">
+        <v>3094</v>
+      </c>
+      <c r="AN3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO3" t="inlineStr">
+        <is>
+          <t>3853</t>
         </is>
       </c>
     </row>
@@ -962,9 +984,15 @@
       <c r="AL4" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AM4" t="inlineStr">
-        <is>
-          <t>3406</t>
+      <c r="AM4" t="n">
+        <v>3406</v>
+      </c>
+      <c r="AN4" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO4" t="inlineStr">
+        <is>
+          <t>4003</t>
         </is>
       </c>
     </row>
@@ -1089,9 +1117,15 @@
       <c r="AL5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AM5" t="inlineStr">
-        <is>
-          <t>3102</t>
+      <c r="AM5" t="n">
+        <v>3102</v>
+      </c>
+      <c r="AN5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO5" t="inlineStr">
+        <is>
+          <t>3737</t>
         </is>
       </c>
     </row>
@@ -1216,9 +1250,15 @@
       <c r="AL6" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AM6" t="inlineStr">
-        <is>
-          <t>3141</t>
+      <c r="AM6" t="n">
+        <v>3141</v>
+      </c>
+      <c r="AN6" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO6" t="inlineStr">
+        <is>
+          <t>3716</t>
         </is>
       </c>
     </row>
@@ -1241,7 +1281,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F7" s="5" t="n">
@@ -1343,9 +1383,15 @@
       <c r="AL7" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AM7" t="inlineStr">
-        <is>
-          <t>3466</t>
+      <c r="AM7" t="n">
+        <v>3466</v>
+      </c>
+      <c r="AN7" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AO7" t="inlineStr">
+        <is>
+          <t>4013</t>
         </is>
       </c>
     </row>
@@ -1470,9 +1516,15 @@
       <c r="AL8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AM8" t="inlineStr">
-        <is>
-          <t>2984</t>
+      <c r="AM8" t="n">
+        <v>2984</v>
+      </c>
+      <c r="AN8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO8" t="inlineStr">
+        <is>
+          <t>3582</t>
         </is>
       </c>
     </row>
@@ -1597,9 +1649,15 @@
       <c r="AL9" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AM9" t="inlineStr">
-        <is>
-          <t>3095</t>
+      <c r="AM9" t="n">
+        <v>3095</v>
+      </c>
+      <c r="AN9" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AO9" t="inlineStr">
+        <is>
+          <t>3572</t>
         </is>
       </c>
     </row>
@@ -1724,9 +1782,15 @@
       <c r="AL10" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AM10" t="inlineStr">
-        <is>
-          <t>3188</t>
+      <c r="AM10" t="n">
+        <v>3188</v>
+      </c>
+      <c r="AN10" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO10" t="inlineStr">
+        <is>
+          <t>3821</t>
         </is>
       </c>
     </row>
@@ -1851,9 +1915,15 @@
       <c r="AL11" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AM11" t="inlineStr">
-        <is>
-          <t>3105</t>
+      <c r="AM11" t="n">
+        <v>3105</v>
+      </c>
+      <c r="AN11" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO11" t="inlineStr">
+        <is>
+          <t>3529</t>
         </is>
       </c>
     </row>
@@ -1978,7 +2048,13 @@
       <c r="AL12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM12" t="inlineStr">
+      <c r="AM12" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AN12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO12" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2003,7 +2079,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F13" s="5" t="n">
@@ -2105,9 +2181,15 @@
       <c r="AL13" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="AM13" t="inlineStr">
-        <is>
-          <t>3458</t>
+      <c r="AM13" t="n">
+        <v>3458</v>
+      </c>
+      <c r="AN13" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="AO13" t="inlineStr">
+        <is>
+          <t>4252</t>
         </is>
       </c>
     </row>
@@ -2232,9 +2314,15 @@
       <c r="AL14" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AM14" t="inlineStr">
-        <is>
-          <t>3150</t>
+      <c r="AM14" t="n">
+        <v>3150</v>
+      </c>
+      <c r="AN14" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AO14" t="inlineStr">
+        <is>
+          <t>3731</t>
         </is>
       </c>
     </row>
@@ -2359,9 +2447,15 @@
       <c r="AL15" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM15" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="AM15" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AN15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO15" t="inlineStr">
+        <is>
+          <t>2539</t>
         </is>
       </c>
     </row>
@@ -2486,9 +2580,15 @@
       <c r="AL16" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="AM16" t="inlineStr">
-        <is>
-          <t>3289</t>
+      <c r="AM16" t="n">
+        <v>3289</v>
+      </c>
+      <c r="AN16" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO16" t="inlineStr">
+        <is>
+          <t>3956</t>
         </is>
       </c>
     </row>
@@ -2613,9 +2713,15 @@
       <c r="AL17" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AM17" t="inlineStr">
-        <is>
-          <t>3111</t>
+      <c r="AM17" t="n">
+        <v>3111</v>
+      </c>
+      <c r="AN17" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO17" t="inlineStr">
+        <is>
+          <t>3282</t>
         </is>
       </c>
     </row>
@@ -2740,9 +2846,15 @@
       <c r="AL18" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AM18" t="inlineStr">
-        <is>
-          <t>2919</t>
+      <c r="AM18" t="n">
+        <v>2919</v>
+      </c>
+      <c r="AN18" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO18" t="inlineStr">
+        <is>
+          <t>3424</t>
         </is>
       </c>
     </row>
@@ -2765,7 +2877,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F19" s="3" t="n">
@@ -2867,9 +2979,15 @@
       <c r="AL19" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AM19" t="inlineStr">
-        <is>
-          <t>3257</t>
+      <c r="AM19" t="n">
+        <v>3257</v>
+      </c>
+      <c r="AN19" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO19" t="inlineStr">
+        <is>
+          <t>3842</t>
         </is>
       </c>
     </row>
@@ -2892,7 +3010,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F20" s="3" t="n">
@@ -2994,9 +3112,15 @@
       <c r="AL20" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AM20" t="inlineStr">
-        <is>
-          <t>3604</t>
+      <c r="AM20" t="n">
+        <v>3604</v>
+      </c>
+      <c r="AN20" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AO20" t="inlineStr">
+        <is>
+          <t>4404</t>
         </is>
       </c>
     </row>
@@ -3121,9 +3245,15 @@
       <c r="AL21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM21" t="inlineStr">
-        <is>
-          <t>2781</t>
+      <c r="AM21" t="n">
+        <v>2781</v>
+      </c>
+      <c r="AN21" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO21" t="inlineStr">
+        <is>
+          <t>3093</t>
         </is>
       </c>
     </row>
@@ -3248,9 +3378,15 @@
       <c r="AL22" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AM22" t="inlineStr">
-        <is>
-          <t>3132</t>
+      <c r="AM22" t="n">
+        <v>3132</v>
+      </c>
+      <c r="AN22" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AO22" t="inlineStr">
+        <is>
+          <t>3689</t>
         </is>
       </c>
     </row>
@@ -3375,9 +3511,15 @@
       <c r="AL23" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AM23" t="inlineStr">
-        <is>
-          <t>2990</t>
+      <c r="AM23" t="n">
+        <v>2990</v>
+      </c>
+      <c r="AN23" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO23" t="inlineStr">
+        <is>
+          <t>3528</t>
         </is>
       </c>
     </row>
@@ -3502,9 +3644,15 @@
       <c r="AL24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AM24" t="inlineStr">
-        <is>
-          <t>3276</t>
+      <c r="AM24" t="n">
+        <v>3276</v>
+      </c>
+      <c r="AN24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AO24" t="inlineStr">
+        <is>
+          <t>3893</t>
         </is>
       </c>
     </row>
@@ -3629,7 +3777,13 @@
       <c r="AL25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM25" t="inlineStr">
+      <c r="AM25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3756,9 +3910,15 @@
       <c r="AL26" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AM26" t="inlineStr">
-        <is>
-          <t>3330</t>
+      <c r="AM26" t="n">
+        <v>3330</v>
+      </c>
+      <c r="AN26" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="AO26" t="inlineStr">
+        <is>
+          <t>3945</t>
         </is>
       </c>
     </row>
@@ -3883,9 +4043,15 @@
       <c r="AL27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM27" t="inlineStr">
-        <is>
-          <t>2891</t>
+      <c r="AM27" t="n">
+        <v>2891</v>
+      </c>
+      <c r="AN27" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO27" t="inlineStr">
+        <is>
+          <t>3401</t>
         </is>
       </c>
     </row>
@@ -4010,9 +4176,15 @@
       <c r="AL28" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="AM28" t="inlineStr">
-        <is>
-          <t>3000</t>
+      <c r="AM28" t="n">
+        <v>3000</v>
+      </c>
+      <c r="AN28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="AO28" t="inlineStr">
+        <is>
+          <t>3255</t>
         </is>
       </c>
     </row>
@@ -4137,9 +4309,15 @@
       <c r="AL29" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AM29" t="inlineStr">
-        <is>
-          <t>3599</t>
+      <c r="AM29" t="n">
+        <v>3599</v>
+      </c>
+      <c r="AN29" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AO29" t="inlineStr">
+        <is>
+          <t>4287</t>
         </is>
       </c>
     </row>
@@ -4264,9 +4442,15 @@
       <c r="AL30" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AM30" t="inlineStr">
-        <is>
-          <t>3089</t>
+      <c r="AM30" t="n">
+        <v>3089</v>
+      </c>
+      <c r="AN30" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AO30" t="inlineStr">
+        <is>
+          <t>3583</t>
         </is>
       </c>
     </row>
@@ -4391,9 +4575,15 @@
       <c r="AL31" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AM31" t="inlineStr">
-        <is>
-          <t>3384</t>
+      <c r="AM31" t="n">
+        <v>3384</v>
+      </c>
+      <c r="AN31" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AO31" t="inlineStr">
+        <is>
+          <t>4033</t>
         </is>
       </c>
     </row>
@@ -4416,7 +4606,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F32" s="5" t="n">
@@ -4518,9 +4708,15 @@
       <c r="AL32" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="AM32" t="inlineStr">
-        <is>
-          <t>3312</t>
+      <c r="AM32" t="n">
+        <v>3312</v>
+      </c>
+      <c r="AN32" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AO32" t="inlineStr">
+        <is>
+          <t>3857</t>
         </is>
       </c>
     </row>
@@ -4645,9 +4841,15 @@
       <c r="AL33" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="AM33" t="inlineStr">
-        <is>
-          <t>3023</t>
+      <c r="AM33" t="n">
+        <v>3023</v>
+      </c>
+      <c r="AN33" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AO33" t="inlineStr">
+        <is>
+          <t>3514</t>
         </is>
       </c>
     </row>
@@ -4772,9 +4974,15 @@
       <c r="AL34" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AM34" t="inlineStr">
-        <is>
-          <t>3179</t>
+      <c r="AM34" t="n">
+        <v>3179</v>
+      </c>
+      <c r="AN34" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO34" t="inlineStr">
+        <is>
+          <t>3682</t>
         </is>
       </c>
     </row>
@@ -4797,7 +5005,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F35" s="5" t="n">
@@ -4899,9 +5107,15 @@
       <c r="AL35" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AM35" t="inlineStr">
-        <is>
-          <t>3313</t>
+      <c r="AM35" t="n">
+        <v>3313</v>
+      </c>
+      <c r="AN35" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AO35" t="inlineStr">
+        <is>
+          <t>3804</t>
         </is>
       </c>
     </row>
@@ -5026,9 +5240,15 @@
       <c r="AL36" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AM36" t="inlineStr">
-        <is>
-          <t>3061</t>
+      <c r="AM36" t="n">
+        <v>3061</v>
+      </c>
+      <c r="AN36" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="AO36" t="inlineStr">
+        <is>
+          <t>3508</t>
         </is>
       </c>
     </row>
@@ -5153,9 +5373,15 @@
       <c r="AL37" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AM37" t="inlineStr">
-        <is>
-          <t>3114</t>
+      <c r="AM37" t="n">
+        <v>3114</v>
+      </c>
+      <c r="AN37" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AO37" t="inlineStr">
+        <is>
+          <t>3532</t>
         </is>
       </c>
     </row>
@@ -5280,9 +5506,15 @@
       <c r="AL38" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AM38" t="inlineStr">
-        <is>
-          <t>3205</t>
+      <c r="AM38" t="n">
+        <v>3205</v>
+      </c>
+      <c r="AN38" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO38" t="inlineStr">
+        <is>
+          <t>3801</t>
         </is>
       </c>
     </row>
@@ -5407,9 +5639,15 @@
       <c r="AL39" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AM39" t="inlineStr">
-        <is>
-          <t>3200</t>
+      <c r="AM39" t="n">
+        <v>3200</v>
+      </c>
+      <c r="AN39" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AO39" t="inlineStr">
+        <is>
+          <t>3816</t>
         </is>
       </c>
     </row>
@@ -5534,9 +5772,15 @@
       <c r="AL40" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AM40" t="inlineStr">
-        <is>
-          <t>3382</t>
+      <c r="AM40" t="n">
+        <v>3382</v>
+      </c>
+      <c r="AN40" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AO40" t="inlineStr">
+        <is>
+          <t>3801</t>
         </is>
       </c>
     </row>
@@ -5661,7 +5905,13 @@
       <c r="AL41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM41" t="inlineStr">
+      <c r="AM41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO41" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5788,9 +6038,15 @@
       <c r="AL42" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AM42" t="inlineStr">
-        <is>
-          <t>3512</t>
+      <c r="AM42" t="n">
+        <v>3512</v>
+      </c>
+      <c r="AN42" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="AO42" t="inlineStr">
+        <is>
+          <t>4202</t>
         </is>
       </c>
     </row>
@@ -5915,9 +6171,15 @@
       <c r="AL43" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AM43" t="inlineStr">
-        <is>
-          <t>3371</t>
+      <c r="AM43" t="n">
+        <v>3371</v>
+      </c>
+      <c r="AN43" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AO43" t="inlineStr">
+        <is>
+          <t>3779</t>
         </is>
       </c>
     </row>
@@ -6042,9 +6304,15 @@
       <c r="AL44" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AM44" t="inlineStr">
-        <is>
-          <t>3147</t>
+      <c r="AM44" t="n">
+        <v>3147</v>
+      </c>
+      <c r="AN44" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AO44" t="inlineStr">
+        <is>
+          <t>3973</t>
         </is>
       </c>
     </row>
@@ -6169,9 +6437,15 @@
       <c r="AL45" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AM45" t="inlineStr">
-        <is>
-          <t>3115</t>
+      <c r="AM45" t="n">
+        <v>3115</v>
+      </c>
+      <c r="AN45" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AO45" t="inlineStr">
+        <is>
+          <t>3543</t>
         </is>
       </c>
     </row>
@@ -6296,9 +6570,15 @@
       <c r="AL46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AM46" t="inlineStr">
-        <is>
-          <t>3161</t>
+      <c r="AM46" t="n">
+        <v>3161</v>
+      </c>
+      <c r="AN46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO46" t="inlineStr">
+        <is>
+          <t>3554</t>
         </is>
       </c>
     </row>
@@ -6423,9 +6703,15 @@
       <c r="AL47" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AM47" t="inlineStr">
-        <is>
-          <t>3103</t>
+      <c r="AM47" t="n">
+        <v>3103</v>
+      </c>
+      <c r="AN47" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO47" t="inlineStr">
+        <is>
+          <t>3576</t>
         </is>
       </c>
     </row>
@@ -6550,9 +6836,15 @@
       <c r="AL48" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AM48" t="inlineStr">
-        <is>
-          <t>3372</t>
+      <c r="AM48" t="n">
+        <v>3372</v>
+      </c>
+      <c r="AN48" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="AO48" t="inlineStr">
+        <is>
+          <t>4011</t>
         </is>
       </c>
     </row>
@@ -6677,9 +6969,15 @@
       <c r="AL49" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AM49" t="inlineStr">
-        <is>
-          <t>2769</t>
+      <c r="AM49" t="n">
+        <v>2769</v>
+      </c>
+      <c r="AN49" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO49" t="inlineStr">
+        <is>
+          <t>3005</t>
         </is>
       </c>
     </row>
@@ -6804,9 +7102,15 @@
       <c r="AL50" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AM50" t="inlineStr">
-        <is>
-          <t>3233</t>
+      <c r="AM50" t="n">
+        <v>3233</v>
+      </c>
+      <c r="AN50" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AO50" t="inlineStr">
+        <is>
+          <t>3982</t>
         </is>
       </c>
     </row>
@@ -6931,9 +7235,15 @@
       <c r="AL51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM51" t="inlineStr">
-        <is>
-          <t>2481</t>
+      <c r="AM51" t="n">
+        <v>2481</v>
+      </c>
+      <c r="AN51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO51" t="inlineStr">
+        <is>
+          <t>2523</t>
         </is>
       </c>
     </row>
@@ -7058,9 +7368,15 @@
       <c r="AL52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM52" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="AM52" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO52" t="inlineStr">
+        <is>
+          <t>2535</t>
         </is>
       </c>
     </row>
@@ -7185,9 +7501,15 @@
       <c r="AL53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM53" t="inlineStr">
-        <is>
-          <t>2567</t>
+      <c r="AM53" t="n">
+        <v>2567</v>
+      </c>
+      <c r="AN53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO53" t="inlineStr">
+        <is>
+          <t>2935</t>
         </is>
       </c>
     </row>
@@ -7312,9 +7634,15 @@
       <c r="AL54" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AM54" t="inlineStr">
-        <is>
-          <t>3336</t>
+      <c r="AM54" t="n">
+        <v>3336</v>
+      </c>
+      <c r="AN54" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AO54" t="inlineStr">
+        <is>
+          <t>3833</t>
         </is>
       </c>
     </row>
@@ -7439,9 +7767,15 @@
       <c r="AL55" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AM55" t="inlineStr">
-        <is>
-          <t>2924</t>
+      <c r="AM55" t="n">
+        <v>2924</v>
+      </c>
+      <c r="AN55" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AO55" t="inlineStr">
+        <is>
+          <t>3308</t>
         </is>
       </c>
     </row>
@@ -7566,9 +7900,15 @@
       <c r="AL56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AM56" t="inlineStr">
-        <is>
-          <t>2915</t>
+      <c r="AM56" t="n">
+        <v>2915</v>
+      </c>
+      <c r="AN56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO56" t="inlineStr">
+        <is>
+          <t>3296</t>
         </is>
       </c>
     </row>
@@ -7693,9 +8033,15 @@
       <c r="AL57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AM57" t="inlineStr">
-        <is>
-          <t>3108</t>
+      <c r="AM57" t="n">
+        <v>3108</v>
+      </c>
+      <c r="AN57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO57" t="inlineStr">
+        <is>
+          <t>3665</t>
         </is>
       </c>
     </row>
@@ -7820,9 +8166,15 @@
       <c r="AL58" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AM58" t="inlineStr">
-        <is>
-          <t>2892</t>
+      <c r="AM58" t="n">
+        <v>2892</v>
+      </c>
+      <c r="AN58" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AO58" t="inlineStr">
+        <is>
+          <t>3224</t>
         </is>
       </c>
     </row>
@@ -7878,6 +8230,8 @@
       <c r="AK59" t="inlineStr"/>
       <c r="AL59" s="3" t="inlineStr"/>
       <c r="AM59" t="inlineStr"/>
+      <c r="AN59" s="3" t="inlineStr"/>
+      <c r="AO59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -7931,6 +8285,8 @@
       <c r="AK60" t="inlineStr"/>
       <c r="AL60" s="3" t="inlineStr"/>
       <c r="AM60" t="inlineStr"/>
+      <c r="AN60" s="3" t="inlineStr"/>
+      <c r="AO60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -8053,9 +8409,15 @@
       <c r="AL61" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="AM61" t="inlineStr">
-        <is>
-          <t>2978</t>
+      <c r="AM61" t="n">
+        <v>2978</v>
+      </c>
+      <c r="AN61" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO61" t="inlineStr">
+        <is>
+          <t>3549</t>
         </is>
       </c>
     </row>
@@ -8180,7 +8542,13 @@
       <c r="AL62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM62" t="inlineStr">
+      <c r="AM62" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8307,9 +8675,15 @@
       <c r="AL63" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="AM63" t="inlineStr">
-        <is>
-          <t>3181</t>
+      <c r="AM63" t="n">
+        <v>3181</v>
+      </c>
+      <c r="AN63" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AO63" t="inlineStr">
+        <is>
+          <t>3633</t>
         </is>
       </c>
     </row>
@@ -8434,9 +8808,15 @@
       <c r="AL64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM64" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="AM64" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AN64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO64" t="inlineStr">
+        <is>
+          <t>2499</t>
         </is>
       </c>
     </row>
@@ -8492,6 +8872,8 @@
       <c r="AK65" t="inlineStr"/>
       <c r="AL65" s="3" t="inlineStr"/>
       <c r="AM65" t="inlineStr"/>
+      <c r="AN65" s="3" t="inlineStr"/>
+      <c r="AO65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -8614,9 +8996,15 @@
       <c r="AL66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM66" t="inlineStr">
-        <is>
-          <t>2495</t>
+      <c r="AM66" t="n">
+        <v>2495</v>
+      </c>
+      <c r="AN66" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AO66" t="inlineStr">
+        <is>
+          <t>2542</t>
         </is>
       </c>
     </row>
@@ -8741,9 +9129,15 @@
       <c r="AL67" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AM67" t="inlineStr">
-        <is>
-          <t>3101</t>
+      <c r="AM67" t="n">
+        <v>3101</v>
+      </c>
+      <c r="AN67" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AO67" t="inlineStr">
+        <is>
+          <t>3605</t>
         </is>
       </c>
     </row>
@@ -8868,9 +9262,15 @@
       <c r="AL68" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AM68" t="inlineStr">
-        <is>
-          <t>3233</t>
+      <c r="AM68" t="n">
+        <v>3233</v>
+      </c>
+      <c r="AN68" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AO68" t="inlineStr">
+        <is>
+          <t>3672</t>
         </is>
       </c>
     </row>
@@ -8995,9 +9395,15 @@
       <c r="AL69" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AM69" t="inlineStr">
-        <is>
-          <t>2895</t>
+      <c r="AM69" t="n">
+        <v>2895</v>
+      </c>
+      <c r="AN69" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO69" t="inlineStr">
+        <is>
+          <t>3333</t>
         </is>
       </c>
     </row>
@@ -9122,9 +9528,15 @@
       <c r="AL70" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="AM70" t="inlineStr">
-        <is>
-          <t>2494</t>
+      <c r="AM70" t="n">
+        <v>2494</v>
+      </c>
+      <c r="AN70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO70" t="inlineStr">
+        <is>
+          <t>2485</t>
         </is>
       </c>
     </row>
@@ -9249,9 +9661,15 @@
       <c r="AL71" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AM71" t="inlineStr">
-        <is>
-          <t>2945</t>
+      <c r="AM71" t="n">
+        <v>2945</v>
+      </c>
+      <c r="AN71" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AO71" t="inlineStr">
+        <is>
+          <t>3411</t>
         </is>
       </c>
     </row>
@@ -9376,9 +9794,15 @@
       <c r="AL72" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="AM72" t="inlineStr">
-        <is>
-          <t>2643</t>
+      <c r="AM72" t="n">
+        <v>2643</v>
+      </c>
+      <c r="AN72" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="AO72" t="inlineStr">
+        <is>
+          <t>2941</t>
         </is>
       </c>
     </row>
@@ -9503,9 +9927,15 @@
       <c r="AL73" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AM73" t="inlineStr">
-        <is>
-          <t>2990</t>
+      <c r="AM73" t="n">
+        <v>2990</v>
+      </c>
+      <c r="AN73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO73" t="inlineStr">
+        <is>
+          <t>3295</t>
         </is>
       </c>
     </row>
@@ -9630,9 +10060,15 @@
       <c r="AL74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM74" t="inlineStr">
-        <is>
-          <t>2597</t>
+      <c r="AM74" t="n">
+        <v>2597</v>
+      </c>
+      <c r="AN74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO74" t="inlineStr">
+        <is>
+          <t>2625</t>
         </is>
       </c>
     </row>
@@ -9757,9 +10193,15 @@
       <c r="AL75" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="AM75" t="inlineStr">
-        <is>
-          <t>2905</t>
+      <c r="AM75" t="n">
+        <v>2905</v>
+      </c>
+      <c r="AN75" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="AO75" t="inlineStr">
+        <is>
+          <t>3165</t>
         </is>
       </c>
     </row>
@@ -9884,9 +10326,15 @@
       <c r="AL76" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AM76" t="inlineStr">
-        <is>
-          <t>3215</t>
+      <c r="AM76" t="n">
+        <v>3215</v>
+      </c>
+      <c r="AN76" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AO76" t="inlineStr">
+        <is>
+          <t>3666</t>
         </is>
       </c>
     </row>
@@ -10011,7 +10459,13 @@
       <c r="AL77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM77" t="inlineStr">
+      <c r="AM77" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO77" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10138,9 +10592,15 @@
       <c r="AL78" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AM78" t="inlineStr">
-        <is>
-          <t>3168</t>
+      <c r="AM78" t="n">
+        <v>3168</v>
+      </c>
+      <c r="AN78" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO78" t="inlineStr">
+        <is>
+          <t>3634</t>
         </is>
       </c>
     </row>
@@ -10265,7 +10725,13 @@
       <c r="AL79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM79" t="inlineStr">
+      <c r="AM79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10392,9 +10858,15 @@
       <c r="AL80" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="AM80" t="inlineStr">
-        <is>
-          <t>3045</t>
+      <c r="AM80" t="n">
+        <v>3045</v>
+      </c>
+      <c r="AN80" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="AO80" t="inlineStr">
+        <is>
+          <t>3534</t>
         </is>
       </c>
     </row>
@@ -10519,9 +10991,15 @@
       <c r="AL81" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AM81" t="inlineStr">
-        <is>
-          <t>3067</t>
+      <c r="AM81" t="n">
+        <v>3067</v>
+      </c>
+      <c r="AN81" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AO81" t="inlineStr">
+        <is>
+          <t>3620</t>
         </is>
       </c>
     </row>
@@ -10646,9 +11124,15 @@
       <c r="AL82" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AM82" t="inlineStr">
-        <is>
-          <t>3132</t>
+      <c r="AM82" t="n">
+        <v>3132</v>
+      </c>
+      <c r="AN82" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO82" t="inlineStr">
+        <is>
+          <t>3399</t>
         </is>
       </c>
     </row>
@@ -10773,9 +11257,15 @@
       <c r="AL83" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AM83" t="inlineStr">
-        <is>
-          <t>2936</t>
+      <c r="AM83" t="n">
+        <v>2936</v>
+      </c>
+      <c r="AN83" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AO83" t="inlineStr">
+        <is>
+          <t>3341</t>
         </is>
       </c>
     </row>
@@ -10891,6 +11381,8 @@
       <c r="AK84" t="inlineStr"/>
       <c r="AL84" s="3" t="inlineStr"/>
       <c r="AM84" t="inlineStr"/>
+      <c r="AN84" s="3" t="inlineStr"/>
+      <c r="AO84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -11013,9 +11505,15 @@
       <c r="AL85" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AM85" t="inlineStr">
-        <is>
-          <t>2856</t>
+      <c r="AM85" t="n">
+        <v>2856</v>
+      </c>
+      <c r="AN85" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO85" t="inlineStr">
+        <is>
+          <t>3135</t>
         </is>
       </c>
     </row>
@@ -11140,9 +11638,15 @@
       <c r="AL86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM86" t="inlineStr">
-        <is>
-          <t>2467</t>
+      <c r="AM86" t="n">
+        <v>2467</v>
+      </c>
+      <c r="AN86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO86" t="inlineStr">
+        <is>
+          <t>2485</t>
         </is>
       </c>
     </row>
@@ -11267,9 +11771,15 @@
       <c r="AL87" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AM87" t="inlineStr">
-        <is>
-          <t>3176</t>
+      <c r="AM87" t="n">
+        <v>3176</v>
+      </c>
+      <c r="AN87" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AO87" t="inlineStr">
+        <is>
+          <t>3601</t>
         </is>
       </c>
     </row>
@@ -11394,9 +11904,15 @@
       <c r="AL88" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AM88" t="inlineStr">
-        <is>
-          <t>2557</t>
+      <c r="AM88" t="n">
+        <v>2557</v>
+      </c>
+      <c r="AN88" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO88" t="inlineStr">
+        <is>
+          <t>2706</t>
         </is>
       </c>
     </row>
@@ -11521,9 +12037,15 @@
       <c r="AL89" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AM89" t="inlineStr">
-        <is>
-          <t>2766</t>
+      <c r="AM89" t="n">
+        <v>2766</v>
+      </c>
+      <c r="AN89" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO89" t="inlineStr">
+        <is>
+          <t>2882</t>
         </is>
       </c>
     </row>
@@ -11648,9 +12170,15 @@
       <c r="AL90" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AM90" t="inlineStr">
-        <is>
-          <t>2580</t>
+      <c r="AM90" t="n">
+        <v>2580</v>
+      </c>
+      <c r="AN90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO90" t="inlineStr">
+        <is>
+          <t>2516</t>
         </is>
       </c>
     </row>
@@ -11775,9 +12303,15 @@
       <c r="AL91" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AM91" t="inlineStr">
-        <is>
-          <t>2515</t>
+      <c r="AM91" t="n">
+        <v>2515</v>
+      </c>
+      <c r="AN91" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO91" t="inlineStr">
+        <is>
+          <t>2653</t>
         </is>
       </c>
     </row>
@@ -11902,7 +12436,13 @@
       <c r="AL92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM92" t="inlineStr">
+      <c r="AM92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12029,9 +12569,15 @@
       <c r="AL93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM93" t="inlineStr">
-        <is>
-          <t>2395</t>
+      <c r="AM93" t="n">
+        <v>2395</v>
+      </c>
+      <c r="AN93" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO93" t="inlineStr">
+        <is>
+          <t>2334</t>
         </is>
       </c>
     </row>
@@ -12156,7 +12702,13 @@
       <c r="AL94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM94" t="inlineStr">
+      <c r="AM94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12283,9 +12835,15 @@
       <c r="AL95" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AM95" t="inlineStr">
-        <is>
-          <t>2496</t>
+      <c r="AM95" t="n">
+        <v>2496</v>
+      </c>
+      <c r="AN95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO95" t="inlineStr">
+        <is>
+          <t>2417</t>
         </is>
       </c>
     </row>
@@ -12410,9 +12968,15 @@
       <c r="AL96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM96" t="inlineStr">
-        <is>
-          <t>2545</t>
+      <c r="AM96" t="n">
+        <v>2545</v>
+      </c>
+      <c r="AN96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO96" t="inlineStr">
+        <is>
+          <t>2516</t>
         </is>
       </c>
     </row>
@@ -12537,9 +13101,15 @@
       <c r="AL97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM97" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="AM97" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AN97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO97" t="inlineStr">
+        <is>
+          <t>2495</t>
         </is>
       </c>
     </row>
@@ -12664,7 +13234,13 @@
       <c r="AL98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM98" t="inlineStr">
+      <c r="AM98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12791,9 +13367,15 @@
       <c r="AL99" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="AM99" t="inlineStr">
-        <is>
-          <t>2690</t>
+      <c r="AM99" t="n">
+        <v>2690</v>
+      </c>
+      <c r="AN99" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="AO99" t="inlineStr">
+        <is>
+          <t>2966</t>
         </is>
       </c>
     </row>
@@ -12918,9 +13500,15 @@
       <c r="AL100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM100" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="AM100" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AN100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO100" t="inlineStr">
+        <is>
+          <t>2443</t>
         </is>
       </c>
     </row>
@@ -13045,9 +13633,15 @@
       <c r="AL101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AM101" t="inlineStr">
-        <is>
-          <t>3075</t>
+      <c r="AM101" t="n">
+        <v>3075</v>
+      </c>
+      <c r="AN101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO101" t="inlineStr">
+        <is>
+          <t>3481</t>
         </is>
       </c>
     </row>
@@ -13172,9 +13766,15 @@
       <c r="AL102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AM102" t="inlineStr">
-        <is>
-          <t>2851</t>
+      <c r="AM102" t="n">
+        <v>2851</v>
+      </c>
+      <c r="AN102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO102" t="inlineStr">
+        <is>
+          <t>3124</t>
         </is>
       </c>
     </row>
@@ -13299,9 +13899,15 @@
       <c r="AL103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM103" t="inlineStr">
-        <is>
-          <t>2475</t>
+      <c r="AM103" t="n">
+        <v>2475</v>
+      </c>
+      <c r="AN103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO103" t="inlineStr">
+        <is>
+          <t>2453</t>
         </is>
       </c>
     </row>
@@ -13426,9 +14032,15 @@
       <c r="AL104" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AM104" t="inlineStr">
-        <is>
-          <t>3068</t>
+      <c r="AM104" t="n">
+        <v>3068</v>
+      </c>
+      <c r="AN104" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO104" t="inlineStr">
+        <is>
+          <t>3541</t>
         </is>
       </c>
     </row>
@@ -13553,9 +14165,15 @@
       <c r="AL105" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="AM105" t="inlineStr">
-        <is>
-          <t>2932</t>
+      <c r="AM105" t="n">
+        <v>2932</v>
+      </c>
+      <c r="AN105" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AO105" t="inlineStr">
+        <is>
+          <t>3275</t>
         </is>
       </c>
     </row>
@@ -13680,7 +14298,13 @@
       <c r="AL106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM106" t="inlineStr">
+      <c r="AM106" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13807,9 +14431,15 @@
       <c r="AL107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM107" t="inlineStr">
-        <is>
-          <t>2506</t>
+      <c r="AM107" t="n">
+        <v>2506</v>
+      </c>
+      <c r="AN107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO107" t="inlineStr">
+        <is>
+          <t>2545</t>
         </is>
       </c>
     </row>
@@ -13934,7 +14564,13 @@
       <c r="AL108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM108" t="inlineStr">
+      <c r="AM108" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14061,9 +14697,15 @@
       <c r="AL109" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="AM109" t="inlineStr">
-        <is>
-          <t>2713</t>
+      <c r="AM109" t="n">
+        <v>2713</v>
+      </c>
+      <c r="AN109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO109" t="inlineStr">
+        <is>
+          <t>2893</t>
         </is>
       </c>
     </row>
@@ -14188,9 +14830,15 @@
       <c r="AL110" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AM110" t="inlineStr">
-        <is>
-          <t>2796</t>
+      <c r="AM110" t="n">
+        <v>2796</v>
+      </c>
+      <c r="AN110" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO110" t="inlineStr">
+        <is>
+          <t>3017</t>
         </is>
       </c>
     </row>
@@ -14315,9 +14963,15 @@
       <c r="AL111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM111" t="inlineStr">
-        <is>
-          <t>2497</t>
+      <c r="AM111" t="n">
+        <v>2497</v>
+      </c>
+      <c r="AN111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO111" t="inlineStr">
+        <is>
+          <t>2539</t>
         </is>
       </c>
     </row>
@@ -14442,9 +15096,15 @@
       <c r="AL112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM112" t="inlineStr">
-        <is>
-          <t>2508</t>
+      <c r="AM112" t="n">
+        <v>2508</v>
+      </c>
+      <c r="AN112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO112" t="inlineStr">
+        <is>
+          <t>2566</t>
         </is>
       </c>
     </row>
@@ -14569,9 +15229,15 @@
       <c r="AL113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM113" t="inlineStr">
-        <is>
-          <t>2611</t>
+      <c r="AM113" t="n">
+        <v>2611</v>
+      </c>
+      <c r="AN113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO113" t="inlineStr">
+        <is>
+          <t>2747</t>
         </is>
       </c>
     </row>
@@ -14696,9 +15362,15 @@
       <c r="AL114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM114" t="inlineStr">
-        <is>
-          <t>2690</t>
+      <c r="AM114" t="n">
+        <v>2690</v>
+      </c>
+      <c r="AN114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO114" t="inlineStr">
+        <is>
+          <t>2900</t>
         </is>
       </c>
     </row>
@@ -14823,9 +15495,15 @@
       <c r="AL115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM115" t="inlineStr">
-        <is>
-          <t>2027</t>
+      <c r="AM115" t="n">
+        <v>2027</v>
+      </c>
+      <c r="AN115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO115" t="inlineStr">
+        <is>
+          <t>2008</t>
         </is>
       </c>
     </row>
@@ -14950,9 +15628,15 @@
       <c r="AL116" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AM116" t="inlineStr">
-        <is>
-          <t>2665</t>
+      <c r="AM116" t="n">
+        <v>2665</v>
+      </c>
+      <c r="AN116" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="AO116" t="inlineStr">
+        <is>
+          <t>2752</t>
         </is>
       </c>
     </row>
@@ -15077,9 +15761,15 @@
       <c r="AL117" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AM117" t="inlineStr">
-        <is>
-          <t>2791</t>
+      <c r="AM117" t="n">
+        <v>2791</v>
+      </c>
+      <c r="AN117" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO117" t="inlineStr">
+        <is>
+          <t>2997</t>
         </is>
       </c>
     </row>
@@ -15204,7 +15894,13 @@
       <c r="AL118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM118" t="inlineStr">
+      <c r="AM118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15331,9 +16027,15 @@
       <c r="AL119" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AM119" t="inlineStr">
-        <is>
-          <t>2866</t>
+      <c r="AM119" t="n">
+        <v>2866</v>
+      </c>
+      <c r="AN119" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="AO119" t="inlineStr">
+        <is>
+          <t>3172</t>
         </is>
       </c>
     </row>
@@ -15458,9 +16160,15 @@
       <c r="AL120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM120" t="inlineStr">
-        <is>
-          <t>2421</t>
+      <c r="AM120" t="n">
+        <v>2421</v>
+      </c>
+      <c r="AN120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO120" t="inlineStr">
+        <is>
+          <t>2398</t>
         </is>
       </c>
     </row>
@@ -15585,9 +16293,15 @@
       <c r="AL121" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="AM121" t="inlineStr">
-        <is>
-          <t>2651</t>
+      <c r="AM121" t="n">
+        <v>2651</v>
+      </c>
+      <c r="AN121" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AO121" t="inlineStr">
+        <is>
+          <t>2829</t>
         </is>
       </c>
     </row>
@@ -15712,7 +16426,13 @@
       <c r="AL122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM122" t="inlineStr">
+      <c r="AM122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15839,9 +16559,15 @@
       <c r="AL123" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="AM123" t="inlineStr">
-        <is>
-          <t>2622</t>
+      <c r="AM123" t="n">
+        <v>2622</v>
+      </c>
+      <c r="AN123" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO123" t="inlineStr">
+        <is>
+          <t>2777</t>
         </is>
       </c>
     </row>
@@ -15966,9 +16692,15 @@
       <c r="AL124" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="AM124" t="inlineStr">
-        <is>
-          <t>2565</t>
+      <c r="AM124" t="n">
+        <v>2565</v>
+      </c>
+      <c r="AN124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO124" t="inlineStr">
+        <is>
+          <t>2819</t>
         </is>
       </c>
     </row>
@@ -16093,9 +16825,15 @@
       <c r="AL125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM125" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="AM125" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO125" t="inlineStr">
+        <is>
+          <t>2569</t>
         </is>
       </c>
     </row>
@@ -16220,9 +16958,15 @@
       <c r="AL126" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="AM126" t="inlineStr">
-        <is>
-          <t>2632</t>
+      <c r="AM126" t="n">
+        <v>2632</v>
+      </c>
+      <c r="AN126" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AO126" t="inlineStr">
+        <is>
+          <t>2857</t>
         </is>
       </c>
     </row>
@@ -16347,9 +17091,15 @@
       <c r="AL127" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AM127" t="inlineStr">
-        <is>
-          <t>2395</t>
+      <c r="AM127" t="n">
+        <v>2395</v>
+      </c>
+      <c r="AN127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO127" t="inlineStr">
+        <is>
+          <t>2389</t>
         </is>
       </c>
     </row>
@@ -16474,7 +17224,13 @@
       <c r="AL128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM128" t="inlineStr">
+      <c r="AM128" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16601,7 +17357,13 @@
       <c r="AL129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM129" t="inlineStr">
+      <c r="AM129" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16728,9 +17490,15 @@
       <c r="AL130" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AM130" t="inlineStr">
-        <is>
-          <t>2492</t>
+      <c r="AM130" t="n">
+        <v>2492</v>
+      </c>
+      <c r="AN130" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AO130" t="inlineStr">
+        <is>
+          <t>2630</t>
         </is>
       </c>
     </row>
@@ -16855,7 +17623,13 @@
       <c r="AL131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM131" t="inlineStr">
+      <c r="AM131" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16982,9 +17756,15 @@
       <c r="AL132" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AM132" t="inlineStr">
-        <is>
-          <t>2470</t>
+      <c r="AM132" t="n">
+        <v>2470</v>
+      </c>
+      <c r="AN132" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO132" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -17109,9 +17889,15 @@
       <c r="AL133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM133" t="inlineStr">
-        <is>
-          <t>2424</t>
+      <c r="AM133" t="n">
+        <v>2424</v>
+      </c>
+      <c r="AN133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO133" t="inlineStr">
+        <is>
+          <t>2472</t>
         </is>
       </c>
     </row>
@@ -17191,6 +17977,8 @@
       <c r="AK134" t="inlineStr"/>
       <c r="AL134" s="3" t="inlineStr"/>
       <c r="AM134" t="inlineStr"/>
+      <c r="AN134" s="3" t="inlineStr"/>
+      <c r="AO134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -17260,6 +18048,8 @@
       <c r="AK135" t="inlineStr"/>
       <c r="AL135" s="3" t="inlineStr"/>
       <c r="AM135" t="inlineStr"/>
+      <c r="AN135" s="3" t="inlineStr"/>
+      <c r="AO135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -17382,7 +18172,13 @@
       <c r="AL136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM136" t="inlineStr">
+      <c r="AM136" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO136" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -17509,7 +18305,13 @@
       <c r="AL137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM137" t="inlineStr">
+      <c r="AM137" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -17583,6 +18385,8 @@
       <c r="AK138" t="inlineStr"/>
       <c r="AL138" s="3" t="inlineStr"/>
       <c r="AM138" t="inlineStr"/>
+      <c r="AN138" s="3" t="inlineStr"/>
+      <c r="AO138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -17705,9 +18509,15 @@
       <c r="AL139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM139" t="inlineStr">
-        <is>
-          <t>1997</t>
+      <c r="AM139" t="n">
+        <v>1997</v>
+      </c>
+      <c r="AN139" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AO139" t="inlineStr">
+        <is>
+          <t>2046</t>
         </is>
       </c>
     </row>
@@ -17832,9 +18642,15 @@
       <c r="AL140" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AM140" t="inlineStr">
-        <is>
-          <t>2475</t>
+      <c r="AM140" t="n">
+        <v>2475</v>
+      </c>
+      <c r="AN140" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AO140" t="inlineStr">
+        <is>
+          <t>2570</t>
         </is>
       </c>
     </row>
@@ -17906,6 +18722,8 @@
       <c r="AK141" t="inlineStr"/>
       <c r="AL141" s="3" t="inlineStr"/>
       <c r="AM141" t="inlineStr"/>
+      <c r="AN141" s="3" t="inlineStr"/>
+      <c r="AO141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -18028,7 +18846,13 @@
       <c r="AL142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM142" t="inlineStr">
+      <c r="AM142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO142" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18102,6 +18926,8 @@
       <c r="AK143" t="inlineStr"/>
       <c r="AL143" s="3" t="inlineStr"/>
       <c r="AM143" t="inlineStr"/>
+      <c r="AN143" s="3" t="inlineStr"/>
+      <c r="AO143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -18171,6 +18997,8 @@
       <c r="AK144" t="inlineStr"/>
       <c r="AL144" s="3" t="inlineStr"/>
       <c r="AM144" t="inlineStr"/>
+      <c r="AN144" s="3" t="inlineStr"/>
+      <c r="AO144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -18240,6 +19068,8 @@
       <c r="AK145" t="inlineStr"/>
       <c r="AL145" s="3" t="inlineStr"/>
       <c r="AM145" t="inlineStr"/>
+      <c r="AN145" s="3" t="inlineStr"/>
+      <c r="AO145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -18309,6 +19139,8 @@
       <c r="AK146" t="inlineStr"/>
       <c r="AL146" s="3" t="inlineStr"/>
       <c r="AM146" t="inlineStr"/>
+      <c r="AN146" s="3" t="inlineStr"/>
+      <c r="AO146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -18378,6 +19210,8 @@
       <c r="AK147" t="inlineStr"/>
       <c r="AL147" s="3" t="inlineStr"/>
       <c r="AM147" t="inlineStr"/>
+      <c r="AN147" s="3" t="inlineStr"/>
+      <c r="AO147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -18500,7 +19334,13 @@
       <c r="AL148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM148" t="inlineStr">
+      <c r="AM148" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18627,9 +19467,15 @@
       <c r="AL149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM149" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="AM149" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AN149" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO149" t="inlineStr">
+        <is>
+          <t>2926</t>
         </is>
       </c>
     </row>
@@ -18754,7 +19600,13 @@
       <c r="AL150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM150" t="inlineStr">
+      <c r="AM150" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18881,9 +19733,15 @@
       <c r="AL151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM151" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="AM151" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO151" t="inlineStr">
+        <is>
+          <t>2552</t>
         </is>
       </c>
     </row>
@@ -19008,7 +19866,13 @@
       <c r="AL152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM152" t="inlineStr">
+      <c r="AM152" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -19135,7 +19999,13 @@
       <c r="AL153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM153" t="inlineStr">
+      <c r="AM153" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -19262,7 +20132,13 @@
       <c r="AL154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM154" t="inlineStr">
+      <c r="AM154" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -19389,9 +20265,15 @@
       <c r="AL155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM155" t="inlineStr">
-        <is>
-          <t>2490</t>
+      <c r="AM155" t="n">
+        <v>2490</v>
+      </c>
+      <c r="AN155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO155" t="inlineStr">
+        <is>
+          <t>2549</t>
         </is>
       </c>
     </row>
@@ -19510,9 +20392,15 @@
       <c r="AL156" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="AM156" t="inlineStr">
-        <is>
-          <t>2712</t>
+      <c r="AM156" t="n">
+        <v>2712</v>
+      </c>
+      <c r="AN156" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="AO156" t="inlineStr">
+        <is>
+          <t>2956</t>
         </is>
       </c>
     </row>
@@ -19578,6 +20466,8 @@
       <c r="AK157" t="inlineStr"/>
       <c r="AL157" s="3" t="inlineStr"/>
       <c r="AM157" t="inlineStr"/>
+      <c r="AN157" s="3" t="inlineStr"/>
+      <c r="AO157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -19694,7 +20584,13 @@
       <c r="AL158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM158" t="inlineStr">
+      <c r="AM158" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -19706,7 +20602,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>青龙偃月灯</t>
+          <t>每逢佳节胖六斤</t>
         </is>
       </c>
       <c r="C159" t="inlineStr"/>
@@ -19815,9 +20711,15 @@
       <c r="AL159" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AM159" t="inlineStr">
-        <is>
-          <t>2551</t>
+      <c r="AM159" t="n">
+        <v>2551</v>
+      </c>
+      <c r="AN159" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO159" t="inlineStr">
+        <is>
+          <t>2729</t>
         </is>
       </c>
     </row>
@@ -19883,6 +20785,8 @@
       <c r="AK160" t="inlineStr"/>
       <c r="AL160" s="3" t="inlineStr"/>
       <c r="AM160" t="inlineStr"/>
+      <c r="AN160" s="3" t="inlineStr"/>
+      <c r="AO160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -19987,9 +20891,15 @@
       <c r="AL161" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="AM161" t="inlineStr">
-        <is>
-          <t>2632</t>
+      <c r="AM161" t="n">
+        <v>2632</v>
+      </c>
+      <c r="AN161" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AO161" t="inlineStr">
+        <is>
+          <t>2778</t>
         </is>
       </c>
     </row>
@@ -20096,9 +21006,15 @@
       <c r="AL162" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AM162" t="inlineStr">
-        <is>
-          <t>2570</t>
+      <c r="AM162" t="n">
+        <v>2570</v>
+      </c>
+      <c r="AN162" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO162" t="inlineStr">
+        <is>
+          <t>2685</t>
         </is>
       </c>
     </row>
@@ -20201,9 +21117,15 @@
       <c r="AL163" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM163" t="inlineStr">
-        <is>
-          <t>2548</t>
+      <c r="AM163" t="n">
+        <v>2548</v>
+      </c>
+      <c r="AN163" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO163" t="inlineStr">
+        <is>
+          <t>2789</t>
         </is>
       </c>
     </row>
@@ -20290,9 +21212,15 @@
       <c r="AL164" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM164" t="inlineStr">
-        <is>
-          <t>2473</t>
+      <c r="AM164" t="n">
+        <v>2473</v>
+      </c>
+      <c r="AN164" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AO164" t="inlineStr">
+        <is>
+          <t>2786</t>
         </is>
       </c>
     </row>
@@ -20383,9 +21311,15 @@
       <c r="AL165" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="AM165" t="inlineStr">
-        <is>
-          <t>2530</t>
+      <c r="AM165" t="n">
+        <v>2530</v>
+      </c>
+      <c r="AN165" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AO165" t="inlineStr">
+        <is>
+          <t>2505</t>
         </is>
       </c>
     </row>
@@ -20468,9 +21402,15 @@
       <c r="AL166" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM166" t="inlineStr">
-        <is>
-          <t>2448</t>
+      <c r="AM166" t="n">
+        <v>2448</v>
+      </c>
+      <c r="AN166" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="AO166" t="inlineStr">
+        <is>
+          <t>2828</t>
         </is>
       </c>
     </row>
@@ -20541,7 +21481,13 @@
       <c r="AL167" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM167" t="inlineStr">
+      <c r="AM167" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN167" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO167" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -20610,9 +21556,15 @@
       <c r="AL168" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="AM168" t="inlineStr">
-        <is>
-          <t>1421</t>
+      <c r="AM168" t="n">
+        <v>1421</v>
+      </c>
+      <c r="AN168" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO168" t="inlineStr">
+        <is>
+          <t>1536</t>
         </is>
       </c>
     </row>
@@ -20670,6 +21622,8 @@
       <c r="AK169" t="inlineStr"/>
       <c r="AL169" s="3" t="inlineStr"/>
       <c r="AM169" t="inlineStr"/>
+      <c r="AN169" s="3" t="inlineStr"/>
+      <c r="AO169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="n">
@@ -20730,9 +21684,198 @@
       <c r="AL170" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM170" t="inlineStr">
-        <is>
-          <t>1489</t>
+      <c r="AM170" t="n">
+        <v>1489</v>
+      </c>
+      <c r="AN170" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO170" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>41231396</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>ollsthebro</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr"/>
+      <c r="D171" t="inlineStr"/>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F171" s="3" t="inlineStr"/>
+      <c r="G171" t="inlineStr"/>
+      <c r="H171" s="3" t="inlineStr"/>
+      <c r="I171" t="inlineStr"/>
+      <c r="J171" s="3" t="inlineStr"/>
+      <c r="K171" t="inlineStr"/>
+      <c r="L171" s="3" t="inlineStr"/>
+      <c r="M171" t="inlineStr"/>
+      <c r="N171" s="3" t="inlineStr"/>
+      <c r="O171" t="inlineStr"/>
+      <c r="P171" s="3" t="inlineStr"/>
+      <c r="Q171" t="inlineStr"/>
+      <c r="R171" s="3" t="inlineStr"/>
+      <c r="S171" t="inlineStr"/>
+      <c r="T171" s="3" t="inlineStr"/>
+      <c r="U171" t="inlineStr"/>
+      <c r="V171" s="3" t="inlineStr"/>
+      <c r="W171" t="inlineStr"/>
+      <c r="X171" s="3" t="inlineStr"/>
+      <c r="Y171" t="inlineStr"/>
+      <c r="Z171" s="3" t="inlineStr"/>
+      <c r="AA171" t="inlineStr"/>
+      <c r="AB171" s="3" t="inlineStr"/>
+      <c r="AC171" t="inlineStr"/>
+      <c r="AD171" s="3" t="inlineStr"/>
+      <c r="AE171" t="inlineStr"/>
+      <c r="AF171" s="3" t="inlineStr"/>
+      <c r="AG171" t="inlineStr"/>
+      <c r="AH171" s="3" t="inlineStr"/>
+      <c r="AI171" t="inlineStr"/>
+      <c r="AJ171" s="3" t="inlineStr"/>
+      <c r="AK171" t="inlineStr"/>
+      <c r="AL171" s="3" t="inlineStr"/>
+      <c r="AM171" t="inlineStr"/>
+      <c r="AN171" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO171" t="inlineStr">
+        <is>
+          <t>1555</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>58174442</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>Player-58174442</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr"/>
+      <c r="D172" t="inlineStr"/>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F172" s="3" t="inlineStr"/>
+      <c r="G172" t="inlineStr"/>
+      <c r="H172" s="3" t="inlineStr"/>
+      <c r="I172" t="inlineStr"/>
+      <c r="J172" s="3" t="inlineStr"/>
+      <c r="K172" t="inlineStr"/>
+      <c r="L172" s="3" t="inlineStr"/>
+      <c r="M172" t="inlineStr"/>
+      <c r="N172" s="3" t="inlineStr"/>
+      <c r="O172" t="inlineStr"/>
+      <c r="P172" s="3" t="inlineStr"/>
+      <c r="Q172" t="inlineStr"/>
+      <c r="R172" s="3" t="inlineStr"/>
+      <c r="S172" t="inlineStr"/>
+      <c r="T172" s="3" t="inlineStr"/>
+      <c r="U172" t="inlineStr"/>
+      <c r="V172" s="3" t="inlineStr"/>
+      <c r="W172" t="inlineStr"/>
+      <c r="X172" s="3" t="inlineStr"/>
+      <c r="Y172" t="inlineStr"/>
+      <c r="Z172" s="3" t="inlineStr"/>
+      <c r="AA172" t="inlineStr"/>
+      <c r="AB172" s="3" t="inlineStr"/>
+      <c r="AC172" t="inlineStr"/>
+      <c r="AD172" s="3" t="inlineStr"/>
+      <c r="AE172" t="inlineStr"/>
+      <c r="AF172" s="3" t="inlineStr"/>
+      <c r="AG172" t="inlineStr"/>
+      <c r="AH172" s="3" t="inlineStr"/>
+      <c r="AI172" t="inlineStr"/>
+      <c r="AJ172" s="3" t="inlineStr"/>
+      <c r="AK172" t="inlineStr"/>
+      <c r="AL172" s="3" t="inlineStr"/>
+      <c r="AM172" t="inlineStr"/>
+      <c r="AN172" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO172" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>58671339</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>"quang pro"</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr"/>
+      <c r="D173" t="inlineStr"/>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F173" s="3" t="inlineStr"/>
+      <c r="G173" t="inlineStr"/>
+      <c r="H173" s="3" t="inlineStr"/>
+      <c r="I173" t="inlineStr"/>
+      <c r="J173" s="3" t="inlineStr"/>
+      <c r="K173" t="inlineStr"/>
+      <c r="L173" s="3" t="inlineStr"/>
+      <c r="M173" t="inlineStr"/>
+      <c r="N173" s="3" t="inlineStr"/>
+      <c r="O173" t="inlineStr"/>
+      <c r="P173" s="3" t="inlineStr"/>
+      <c r="Q173" t="inlineStr"/>
+      <c r="R173" s="3" t="inlineStr"/>
+      <c r="S173" t="inlineStr"/>
+      <c r="T173" s="3" t="inlineStr"/>
+      <c r="U173" t="inlineStr"/>
+      <c r="V173" s="3" t="inlineStr"/>
+      <c r="W173" t="inlineStr"/>
+      <c r="X173" s="3" t="inlineStr"/>
+      <c r="Y173" t="inlineStr"/>
+      <c r="Z173" s="3" t="inlineStr"/>
+      <c r="AA173" t="inlineStr"/>
+      <c r="AB173" s="3" t="inlineStr"/>
+      <c r="AC173" t="inlineStr"/>
+      <c r="AD173" s="3" t="inlineStr"/>
+      <c r="AE173" t="inlineStr"/>
+      <c r="AF173" s="3" t="inlineStr"/>
+      <c r="AG173" t="inlineStr"/>
+      <c r="AH173" s="3" t="inlineStr"/>
+      <c r="AI173" t="inlineStr"/>
+      <c r="AJ173" s="3" t="inlineStr"/>
+      <c r="AK173" t="inlineStr"/>
+      <c r="AL173" s="3" t="inlineStr"/>
+      <c r="AM173" t="inlineStr"/>
+      <c r="AN173" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="AO173" t="inlineStr">
+        <is>
+          <t>1708</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-03-03 07:46:49
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AO173"/>
+  <dimension ref="A1:AQ173"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -596,6 +596,16 @@
           <t>03-01_0</t>
         </is>
       </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>03-02_A</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>03-02_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -724,7 +734,13 @@
       <c r="AN2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO2" t="inlineStr">
+      <c r="AO2" t="n">
+        <v>2517</v>
+      </c>
+      <c r="AP2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ2" t="inlineStr">
         <is>
           <t>2517</t>
         </is>
@@ -857,7 +873,13 @@
       <c r="AN3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AO3" t="inlineStr">
+      <c r="AO3" t="n">
+        <v>3853</v>
+      </c>
+      <c r="AP3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ3" t="inlineStr">
         <is>
           <t>3853</t>
         </is>
@@ -990,7 +1012,13 @@
       <c r="AN4" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AO4" t="inlineStr">
+      <c r="AO4" t="n">
+        <v>4003</v>
+      </c>
+      <c r="AP4" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AQ4" t="inlineStr">
         <is>
           <t>4003</t>
         </is>
@@ -1123,7 +1151,13 @@
       <c r="AN5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AO5" t="inlineStr">
+      <c r="AO5" t="n">
+        <v>3737</v>
+      </c>
+      <c r="AP5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ5" t="inlineStr">
         <is>
           <t>3737</t>
         </is>
@@ -1256,7 +1290,13 @@
       <c r="AN6" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AO6" t="inlineStr">
+      <c r="AO6" t="n">
+        <v>3716</v>
+      </c>
+      <c r="AP6" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ6" t="inlineStr">
         <is>
           <t>3716</t>
         </is>
@@ -1389,7 +1429,13 @@
       <c r="AN7" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AO7" t="inlineStr">
+      <c r="AO7" t="n">
+        <v>4013</v>
+      </c>
+      <c r="AP7" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AQ7" t="inlineStr">
         <is>
           <t>4013</t>
         </is>
@@ -1522,7 +1568,13 @@
       <c r="AN8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AO8" t="inlineStr">
+      <c r="AO8" t="n">
+        <v>3582</v>
+      </c>
+      <c r="AP8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ8" t="inlineStr">
         <is>
           <t>3582</t>
         </is>
@@ -1655,7 +1707,13 @@
       <c r="AN9" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AO9" t="inlineStr">
+      <c r="AO9" t="n">
+        <v>3572</v>
+      </c>
+      <c r="AP9" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AQ9" t="inlineStr">
         <is>
           <t>3572</t>
         </is>
@@ -1788,7 +1846,13 @@
       <c r="AN10" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AO10" t="inlineStr">
+      <c r="AO10" t="n">
+        <v>3821</v>
+      </c>
+      <c r="AP10" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AQ10" t="inlineStr">
         <is>
           <t>3821</t>
         </is>
@@ -1921,7 +1985,13 @@
       <c r="AN11" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AO11" t="inlineStr">
+      <c r="AO11" t="n">
+        <v>3529</v>
+      </c>
+      <c r="AP11" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ11" t="inlineStr">
         <is>
           <t>3529</t>
         </is>
@@ -2054,7 +2124,13 @@
       <c r="AN12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO12" t="inlineStr">
+      <c r="AO12" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AP12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ12" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2187,7 +2263,13 @@
       <c r="AN13" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="AO13" t="inlineStr">
+      <c r="AO13" t="n">
+        <v>4252</v>
+      </c>
+      <c r="AP13" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="AQ13" t="inlineStr">
         <is>
           <t>4252</t>
         </is>
@@ -2320,7 +2402,13 @@
       <c r="AN14" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AO14" t="inlineStr">
+      <c r="AO14" t="n">
+        <v>3731</v>
+      </c>
+      <c r="AP14" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AQ14" t="inlineStr">
         <is>
           <t>3731</t>
         </is>
@@ -2453,7 +2541,13 @@
       <c r="AN15" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO15" t="inlineStr">
+      <c r="AO15" t="n">
+        <v>2539</v>
+      </c>
+      <c r="AP15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ15" t="inlineStr">
         <is>
           <t>2539</t>
         </is>
@@ -2586,7 +2680,13 @@
       <c r="AN16" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AO16" t="inlineStr">
+      <c r="AO16" t="n">
+        <v>3956</v>
+      </c>
+      <c r="AP16" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AQ16" t="inlineStr">
         <is>
           <t>3956</t>
         </is>
@@ -2719,7 +2819,13 @@
       <c r="AN17" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AO17" t="inlineStr">
+      <c r="AO17" t="n">
+        <v>3282</v>
+      </c>
+      <c r="AP17" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AQ17" t="inlineStr">
         <is>
           <t>3282</t>
         </is>
@@ -2852,7 +2958,13 @@
       <c r="AN18" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AO18" t="inlineStr">
+      <c r="AO18" t="n">
+        <v>3424</v>
+      </c>
+      <c r="AP18" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AQ18" t="inlineStr">
         <is>
           <t>3424</t>
         </is>
@@ -2985,7 +3097,13 @@
       <c r="AN19" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AO19" t="inlineStr">
+      <c r="AO19" t="n">
+        <v>3842</v>
+      </c>
+      <c r="AP19" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AQ19" t="inlineStr">
         <is>
           <t>3842</t>
         </is>
@@ -3118,7 +3236,13 @@
       <c r="AN20" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AO20" t="inlineStr">
+      <c r="AO20" t="n">
+        <v>4404</v>
+      </c>
+      <c r="AP20" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AQ20" t="inlineStr">
         <is>
           <t>4404</t>
         </is>
@@ -3251,7 +3375,13 @@
       <c r="AN21" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AO21" t="inlineStr">
+      <c r="AO21" t="n">
+        <v>3093</v>
+      </c>
+      <c r="AP21" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ21" t="inlineStr">
         <is>
           <t>3093</t>
         </is>
@@ -3384,7 +3514,13 @@
       <c r="AN22" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AO22" t="inlineStr">
+      <c r="AO22" t="n">
+        <v>3689</v>
+      </c>
+      <c r="AP22" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AQ22" t="inlineStr">
         <is>
           <t>3689</t>
         </is>
@@ -3517,7 +3653,13 @@
       <c r="AN23" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AO23" t="inlineStr">
+      <c r="AO23" t="n">
+        <v>3528</v>
+      </c>
+      <c r="AP23" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ23" t="inlineStr">
         <is>
           <t>3528</t>
         </is>
@@ -3650,7 +3792,13 @@
       <c r="AN24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AO24" t="inlineStr">
+      <c r="AO24" t="n">
+        <v>3893</v>
+      </c>
+      <c r="AP24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AQ24" t="inlineStr">
         <is>
           <t>3893</t>
         </is>
@@ -3783,7 +3931,13 @@
       <c r="AN25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO25" t="inlineStr">
+      <c r="AO25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3916,7 +4070,13 @@
       <c r="AN26" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="AO26" t="inlineStr">
+      <c r="AO26" t="n">
+        <v>3945</v>
+      </c>
+      <c r="AP26" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="AQ26" t="inlineStr">
         <is>
           <t>3945</t>
         </is>
@@ -4049,7 +4209,13 @@
       <c r="AN27" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AO27" t="inlineStr">
+      <c r="AO27" t="n">
+        <v>3401</v>
+      </c>
+      <c r="AP27" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ27" t="inlineStr">
         <is>
           <t>3401</t>
         </is>
@@ -4182,7 +4348,13 @@
       <c r="AN28" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="AO28" t="inlineStr">
+      <c r="AO28" t="n">
+        <v>3255</v>
+      </c>
+      <c r="AP28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="AQ28" t="inlineStr">
         <is>
           <t>3255</t>
         </is>
@@ -4315,7 +4487,13 @@
       <c r="AN29" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AO29" t="inlineStr">
+      <c r="AO29" t="n">
+        <v>4287</v>
+      </c>
+      <c r="AP29" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AQ29" t="inlineStr">
         <is>
           <t>4287</t>
         </is>
@@ -4448,7 +4626,13 @@
       <c r="AN30" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AO30" t="inlineStr">
+      <c r="AO30" t="n">
+        <v>3583</v>
+      </c>
+      <c r="AP30" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AQ30" t="inlineStr">
         <is>
           <t>3583</t>
         </is>
@@ -4581,7 +4765,13 @@
       <c r="AN31" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AO31" t="inlineStr">
+      <c r="AO31" t="n">
+        <v>4033</v>
+      </c>
+      <c r="AP31" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AQ31" t="inlineStr">
         <is>
           <t>4033</t>
         </is>
@@ -4714,7 +4904,13 @@
       <c r="AN32" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AO32" t="inlineStr">
+      <c r="AO32" t="n">
+        <v>3857</v>
+      </c>
+      <c r="AP32" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AQ32" t="inlineStr">
         <is>
           <t>3857</t>
         </is>
@@ -4847,7 +5043,13 @@
       <c r="AN33" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AO33" t="inlineStr">
+      <c r="AO33" t="n">
+        <v>3514</v>
+      </c>
+      <c r="AP33" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AQ33" t="inlineStr">
         <is>
           <t>3514</t>
         </is>
@@ -4980,7 +5182,13 @@
       <c r="AN34" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AO34" t="inlineStr">
+      <c r="AO34" t="n">
+        <v>3682</v>
+      </c>
+      <c r="AP34" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AQ34" t="inlineStr">
         <is>
           <t>3682</t>
         </is>
@@ -5113,7 +5321,13 @@
       <c r="AN35" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AO35" t="inlineStr">
+      <c r="AO35" t="n">
+        <v>3804</v>
+      </c>
+      <c r="AP35" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AQ35" t="inlineStr">
         <is>
           <t>3804</t>
         </is>
@@ -5246,7 +5460,13 @@
       <c r="AN36" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="AO36" t="inlineStr">
+      <c r="AO36" t="n">
+        <v>3508</v>
+      </c>
+      <c r="AP36" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="AQ36" t="inlineStr">
         <is>
           <t>3508</t>
         </is>
@@ -5379,7 +5599,13 @@
       <c r="AN37" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AO37" t="inlineStr">
+      <c r="AO37" t="n">
+        <v>3532</v>
+      </c>
+      <c r="AP37" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AQ37" t="inlineStr">
         <is>
           <t>3532</t>
         </is>
@@ -5512,7 +5738,13 @@
       <c r="AN38" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AO38" t="inlineStr">
+      <c r="AO38" t="n">
+        <v>3801</v>
+      </c>
+      <c r="AP38" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AQ38" t="inlineStr">
         <is>
           <t>3801</t>
         </is>
@@ -5645,7 +5877,13 @@
       <c r="AN39" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AO39" t="inlineStr">
+      <c r="AO39" t="n">
+        <v>3816</v>
+      </c>
+      <c r="AP39" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AQ39" t="inlineStr">
         <is>
           <t>3816</t>
         </is>
@@ -5778,7 +6016,13 @@
       <c r="AN40" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AO40" t="inlineStr">
+      <c r="AO40" t="n">
+        <v>3801</v>
+      </c>
+      <c r="AP40" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AQ40" t="inlineStr">
         <is>
           <t>3801</t>
         </is>
@@ -5911,7 +6155,13 @@
       <c r="AN41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO41" t="inlineStr">
+      <c r="AO41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ41" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6044,7 +6294,13 @@
       <c r="AN42" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="AO42" t="inlineStr">
+      <c r="AO42" t="n">
+        <v>4202</v>
+      </c>
+      <c r="AP42" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="AQ42" t="inlineStr">
         <is>
           <t>4202</t>
         </is>
@@ -6177,7 +6433,13 @@
       <c r="AN43" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AO43" t="inlineStr">
+      <c r="AO43" t="n">
+        <v>3779</v>
+      </c>
+      <c r="AP43" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AQ43" t="inlineStr">
         <is>
           <t>3779</t>
         </is>
@@ -6310,7 +6572,13 @@
       <c r="AN44" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AO44" t="inlineStr">
+      <c r="AO44" t="n">
+        <v>3973</v>
+      </c>
+      <c r="AP44" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AQ44" t="inlineStr">
         <is>
           <t>3973</t>
         </is>
@@ -6443,7 +6711,13 @@
       <c r="AN45" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AO45" t="inlineStr">
+      <c r="AO45" t="n">
+        <v>3543</v>
+      </c>
+      <c r="AP45" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AQ45" t="inlineStr">
         <is>
           <t>3543</t>
         </is>
@@ -6576,7 +6850,13 @@
       <c r="AN46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AO46" t="inlineStr">
+      <c r="AO46" t="n">
+        <v>3554</v>
+      </c>
+      <c r="AP46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AQ46" t="inlineStr">
         <is>
           <t>3554</t>
         </is>
@@ -6709,7 +6989,13 @@
       <c r="AN47" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AO47" t="inlineStr">
+      <c r="AO47" t="n">
+        <v>3576</v>
+      </c>
+      <c r="AP47" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ47" t="inlineStr">
         <is>
           <t>3576</t>
         </is>
@@ -6842,7 +7128,13 @@
       <c r="AN48" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="AO48" t="inlineStr">
+      <c r="AO48" t="n">
+        <v>4011</v>
+      </c>
+      <c r="AP48" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="AQ48" t="inlineStr">
         <is>
           <t>4011</t>
         </is>
@@ -6975,7 +7267,13 @@
       <c r="AN49" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AO49" t="inlineStr">
+      <c r="AO49" t="n">
+        <v>3005</v>
+      </c>
+      <c r="AP49" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ49" t="inlineStr">
         <is>
           <t>3005</t>
         </is>
@@ -7108,7 +7406,13 @@
       <c r="AN50" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AO50" t="inlineStr">
+      <c r="AO50" t="n">
+        <v>3982</v>
+      </c>
+      <c r="AP50" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AQ50" t="inlineStr">
         <is>
           <t>3982</t>
         </is>
@@ -7241,7 +7545,13 @@
       <c r="AN51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO51" t="inlineStr">
+      <c r="AO51" t="n">
+        <v>2523</v>
+      </c>
+      <c r="AP51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ51" t="inlineStr">
         <is>
           <t>2523</t>
         </is>
@@ -7374,7 +7684,13 @@
       <c r="AN52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO52" t="inlineStr">
+      <c r="AO52" t="n">
+        <v>2535</v>
+      </c>
+      <c r="AP52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ52" t="inlineStr">
         <is>
           <t>2535</t>
         </is>
@@ -7507,7 +7823,13 @@
       <c r="AN53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO53" t="inlineStr">
+      <c r="AO53" t="n">
+        <v>2935</v>
+      </c>
+      <c r="AP53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ53" t="inlineStr">
         <is>
           <t>2935</t>
         </is>
@@ -7640,7 +7962,13 @@
       <c r="AN54" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AO54" t="inlineStr">
+      <c r="AO54" t="n">
+        <v>3833</v>
+      </c>
+      <c r="AP54" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AQ54" t="inlineStr">
         <is>
           <t>3833</t>
         </is>
@@ -7773,7 +8101,13 @@
       <c r="AN55" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AO55" t="inlineStr">
+      <c r="AO55" t="n">
+        <v>3308</v>
+      </c>
+      <c r="AP55" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AQ55" t="inlineStr">
         <is>
           <t>3308</t>
         </is>
@@ -7906,7 +8240,13 @@
       <c r="AN56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AO56" t="inlineStr">
+      <c r="AO56" t="n">
+        <v>3296</v>
+      </c>
+      <c r="AP56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ56" t="inlineStr">
         <is>
           <t>3296</t>
         </is>
@@ -8039,7 +8379,13 @@
       <c r="AN57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AO57" t="inlineStr">
+      <c r="AO57" t="n">
+        <v>3665</v>
+      </c>
+      <c r="AP57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ57" t="inlineStr">
         <is>
           <t>3665</t>
         </is>
@@ -8172,7 +8518,13 @@
       <c r="AN58" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AO58" t="inlineStr">
+      <c r="AO58" t="n">
+        <v>3224</v>
+      </c>
+      <c r="AP58" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AQ58" t="inlineStr">
         <is>
           <t>3224</t>
         </is>
@@ -8232,6 +8584,8 @@
       <c r="AM59" t="inlineStr"/>
       <c r="AN59" s="3" t="inlineStr"/>
       <c r="AO59" t="inlineStr"/>
+      <c r="AP59" s="3" t="inlineStr"/>
+      <c r="AQ59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -8287,6 +8641,8 @@
       <c r="AM60" t="inlineStr"/>
       <c r="AN60" s="3" t="inlineStr"/>
       <c r="AO60" t="inlineStr"/>
+      <c r="AP60" s="3" t="inlineStr"/>
+      <c r="AQ60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -8415,7 +8771,13 @@
       <c r="AN61" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AO61" t="inlineStr">
+      <c r="AO61" t="n">
+        <v>3549</v>
+      </c>
+      <c r="AP61" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AQ61" t="inlineStr">
         <is>
           <t>3549</t>
         </is>
@@ -8548,7 +8910,13 @@
       <c r="AN62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO62" t="inlineStr">
+      <c r="AO62" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8681,7 +9049,13 @@
       <c r="AN63" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AO63" t="inlineStr">
+      <c r="AO63" t="n">
+        <v>3633</v>
+      </c>
+      <c r="AP63" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AQ63" t="inlineStr">
         <is>
           <t>3633</t>
         </is>
@@ -8814,7 +9188,13 @@
       <c r="AN64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO64" t="inlineStr">
+      <c r="AO64" t="n">
+        <v>2499</v>
+      </c>
+      <c r="AP64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ64" t="inlineStr">
         <is>
           <t>2499</t>
         </is>
@@ -8874,6 +9254,8 @@
       <c r="AM65" t="inlineStr"/>
       <c r="AN65" s="3" t="inlineStr"/>
       <c r="AO65" t="inlineStr"/>
+      <c r="AP65" s="3" t="inlineStr"/>
+      <c r="AQ65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -9002,7 +9384,13 @@
       <c r="AN66" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AO66" t="inlineStr">
+      <c r="AO66" t="n">
+        <v>2542</v>
+      </c>
+      <c r="AP66" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AQ66" t="inlineStr">
         <is>
           <t>2542</t>
         </is>
@@ -9135,7 +9523,13 @@
       <c r="AN67" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AO67" t="inlineStr">
+      <c r="AO67" t="n">
+        <v>3605</v>
+      </c>
+      <c r="AP67" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AQ67" t="inlineStr">
         <is>
           <t>3605</t>
         </is>
@@ -9268,7 +9662,13 @@
       <c r="AN68" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AO68" t="inlineStr">
+      <c r="AO68" t="n">
+        <v>3672</v>
+      </c>
+      <c r="AP68" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AQ68" t="inlineStr">
         <is>
           <t>3672</t>
         </is>
@@ -9401,7 +9801,13 @@
       <c r="AN69" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AO69" t="inlineStr">
+      <c r="AO69" t="n">
+        <v>3333</v>
+      </c>
+      <c r="AP69" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AQ69" t="inlineStr">
         <is>
           <t>3333</t>
         </is>
@@ -9534,7 +9940,13 @@
       <c r="AN70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO70" t="inlineStr">
+      <c r="AO70" t="n">
+        <v>2485</v>
+      </c>
+      <c r="AP70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ70" t="inlineStr">
         <is>
           <t>2485</t>
         </is>
@@ -9667,7 +10079,13 @@
       <c r="AN71" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="AO71" t="inlineStr">
+      <c r="AO71" t="n">
+        <v>3411</v>
+      </c>
+      <c r="AP71" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AQ71" t="inlineStr">
         <is>
           <t>3411</t>
         </is>
@@ -9800,7 +10218,13 @@
       <c r="AN72" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="AO72" t="inlineStr">
+      <c r="AO72" t="n">
+        <v>2941</v>
+      </c>
+      <c r="AP72" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="AQ72" t="inlineStr">
         <is>
           <t>2941</t>
         </is>
@@ -9933,7 +10357,13 @@
       <c r="AN73" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AO73" t="inlineStr">
+      <c r="AO73" t="n">
+        <v>3295</v>
+      </c>
+      <c r="AP73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ73" t="inlineStr">
         <is>
           <t>3295</t>
         </is>
@@ -10066,7 +10496,13 @@
       <c r="AN74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO74" t="inlineStr">
+      <c r="AO74" t="n">
+        <v>2625</v>
+      </c>
+      <c r="AP74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ74" t="inlineStr">
         <is>
           <t>2625</t>
         </is>
@@ -10199,7 +10635,13 @@
       <c r="AN75" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="AO75" t="inlineStr">
+      <c r="AO75" t="n">
+        <v>3165</v>
+      </c>
+      <c r="AP75" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="AQ75" t="inlineStr">
         <is>
           <t>3165</t>
         </is>
@@ -10332,7 +10774,13 @@
       <c r="AN76" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AO76" t="inlineStr">
+      <c r="AO76" t="n">
+        <v>3666</v>
+      </c>
+      <c r="AP76" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AQ76" t="inlineStr">
         <is>
           <t>3666</t>
         </is>
@@ -10465,7 +10913,13 @@
       <c r="AN77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO77" t="inlineStr">
+      <c r="AO77" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ77" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10598,7 +11052,13 @@
       <c r="AN78" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AO78" t="inlineStr">
+      <c r="AO78" t="n">
+        <v>3634</v>
+      </c>
+      <c r="AP78" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AQ78" t="inlineStr">
         <is>
           <t>3634</t>
         </is>
@@ -10731,7 +11191,13 @@
       <c r="AN79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO79" t="inlineStr">
+      <c r="AO79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10864,7 +11330,13 @@
       <c r="AN80" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="AO80" t="inlineStr">
+      <c r="AO80" t="n">
+        <v>3534</v>
+      </c>
+      <c r="AP80" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="AQ80" t="inlineStr">
         <is>
           <t>3534</t>
         </is>
@@ -10997,7 +11469,13 @@
       <c r="AN81" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AO81" t="inlineStr">
+      <c r="AO81" t="n">
+        <v>3620</v>
+      </c>
+      <c r="AP81" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AQ81" t="inlineStr">
         <is>
           <t>3620</t>
         </is>
@@ -11130,7 +11608,13 @@
       <c r="AN82" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AO82" t="inlineStr">
+      <c r="AO82" t="n">
+        <v>3399</v>
+      </c>
+      <c r="AP82" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AQ82" t="inlineStr">
         <is>
           <t>3399</t>
         </is>
@@ -11263,7 +11747,13 @@
       <c r="AN83" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AO83" t="inlineStr">
+      <c r="AO83" t="n">
+        <v>3341</v>
+      </c>
+      <c r="AP83" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AQ83" t="inlineStr">
         <is>
           <t>3341</t>
         </is>
@@ -11383,6 +11873,8 @@
       <c r="AM84" t="inlineStr"/>
       <c r="AN84" s="3" t="inlineStr"/>
       <c r="AO84" t="inlineStr"/>
+      <c r="AP84" s="3" t="inlineStr"/>
+      <c r="AQ84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -11511,7 +12003,13 @@
       <c r="AN85" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AO85" t="inlineStr">
+      <c r="AO85" t="n">
+        <v>3135</v>
+      </c>
+      <c r="AP85" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ85" t="inlineStr">
         <is>
           <t>3135</t>
         </is>
@@ -11644,7 +12142,13 @@
       <c r="AN86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO86" t="inlineStr">
+      <c r="AO86" t="n">
+        <v>2485</v>
+      </c>
+      <c r="AP86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ86" t="inlineStr">
         <is>
           <t>2485</t>
         </is>
@@ -11777,7 +12281,13 @@
       <c r="AN87" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AO87" t="inlineStr">
+      <c r="AO87" t="n">
+        <v>3601</v>
+      </c>
+      <c r="AP87" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AQ87" t="inlineStr">
         <is>
           <t>3601</t>
         </is>
@@ -11910,7 +12420,13 @@
       <c r="AN88" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AO88" t="inlineStr">
+      <c r="AO88" t="n">
+        <v>2706</v>
+      </c>
+      <c r="AP88" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ88" t="inlineStr">
         <is>
           <t>2706</t>
         </is>
@@ -12043,7 +12559,13 @@
       <c r="AN89" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AO89" t="inlineStr">
+      <c r="AO89" t="n">
+        <v>2882</v>
+      </c>
+      <c r="AP89" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ89" t="inlineStr">
         <is>
           <t>2882</t>
         </is>
@@ -12176,7 +12698,13 @@
       <c r="AN90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO90" t="inlineStr">
+      <c r="AO90" t="n">
+        <v>2516</v>
+      </c>
+      <c r="AP90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ90" t="inlineStr">
         <is>
           <t>2516</t>
         </is>
@@ -12309,7 +12837,13 @@
       <c r="AN91" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AO91" t="inlineStr">
+      <c r="AO91" t="n">
+        <v>2653</v>
+      </c>
+      <c r="AP91" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ91" t="inlineStr">
         <is>
           <t>2653</t>
         </is>
@@ -12442,7 +12976,13 @@
       <c r="AN92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO92" t="inlineStr">
+      <c r="AO92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12575,7 +13115,13 @@
       <c r="AN93" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="AO93" t="inlineStr">
+      <c r="AO93" t="n">
+        <v>2334</v>
+      </c>
+      <c r="AP93" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ93" t="inlineStr">
         <is>
           <t>2334</t>
         </is>
@@ -12708,7 +13254,13 @@
       <c r="AN94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO94" t="inlineStr">
+      <c r="AO94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12841,7 +13393,13 @@
       <c r="AN95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO95" t="inlineStr">
+      <c r="AO95" t="n">
+        <v>2417</v>
+      </c>
+      <c r="AP95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ95" t="inlineStr">
         <is>
           <t>2417</t>
         </is>
@@ -12974,7 +13532,13 @@
       <c r="AN96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO96" t="inlineStr">
+      <c r="AO96" t="n">
+        <v>2516</v>
+      </c>
+      <c r="AP96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ96" t="inlineStr">
         <is>
           <t>2516</t>
         </is>
@@ -13107,7 +13671,13 @@
       <c r="AN97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO97" t="inlineStr">
+      <c r="AO97" t="n">
+        <v>2495</v>
+      </c>
+      <c r="AP97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ97" t="inlineStr">
         <is>
           <t>2495</t>
         </is>
@@ -13240,7 +13810,13 @@
       <c r="AN98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO98" t="inlineStr">
+      <c r="AO98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13373,7 +13949,13 @@
       <c r="AN99" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="AO99" t="inlineStr">
+      <c r="AO99" t="n">
+        <v>2966</v>
+      </c>
+      <c r="AP99" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="AQ99" t="inlineStr">
         <is>
           <t>2966</t>
         </is>
@@ -13506,7 +14088,13 @@
       <c r="AN100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO100" t="inlineStr">
+      <c r="AO100" t="n">
+        <v>2443</v>
+      </c>
+      <c r="AP100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ100" t="inlineStr">
         <is>
           <t>2443</t>
         </is>
@@ -13639,7 +14227,13 @@
       <c r="AN101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AO101" t="inlineStr">
+      <c r="AO101" t="n">
+        <v>3481</v>
+      </c>
+      <c r="AP101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AQ101" t="inlineStr">
         <is>
           <t>3481</t>
         </is>
@@ -13772,7 +14366,13 @@
       <c r="AN102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AO102" t="inlineStr">
+      <c r="AO102" t="n">
+        <v>3124</v>
+      </c>
+      <c r="AP102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ102" t="inlineStr">
         <is>
           <t>3124</t>
         </is>
@@ -13905,7 +14505,13 @@
       <c r="AN103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO103" t="inlineStr">
+      <c r="AO103" t="n">
+        <v>2453</v>
+      </c>
+      <c r="AP103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ103" t="inlineStr">
         <is>
           <t>2453</t>
         </is>
@@ -14038,7 +14644,13 @@
       <c r="AN104" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AO104" t="inlineStr">
+      <c r="AO104" t="n">
+        <v>3541</v>
+      </c>
+      <c r="AP104" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AQ104" t="inlineStr">
         <is>
           <t>3541</t>
         </is>
@@ -14171,7 +14783,13 @@
       <c r="AN105" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="AO105" t="inlineStr">
+      <c r="AO105" t="n">
+        <v>3275</v>
+      </c>
+      <c r="AP105" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AQ105" t="inlineStr">
         <is>
           <t>3275</t>
         </is>
@@ -14304,7 +14922,13 @@
       <c r="AN106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO106" t="inlineStr">
+      <c r="AO106" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14437,7 +15061,13 @@
       <c r="AN107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO107" t="inlineStr">
+      <c r="AO107" t="n">
+        <v>2545</v>
+      </c>
+      <c r="AP107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ107" t="inlineStr">
         <is>
           <t>2545</t>
         </is>
@@ -14570,7 +15200,13 @@
       <c r="AN108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO108" t="inlineStr">
+      <c r="AO108" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14703,7 +15339,13 @@
       <c r="AN109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO109" t="inlineStr">
+      <c r="AO109" t="n">
+        <v>2893</v>
+      </c>
+      <c r="AP109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ109" t="inlineStr">
         <is>
           <t>2893</t>
         </is>
@@ -14836,7 +15478,13 @@
       <c r="AN110" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AO110" t="inlineStr">
+      <c r="AO110" t="n">
+        <v>3017</v>
+      </c>
+      <c r="AP110" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AQ110" t="inlineStr">
         <is>
           <t>3017</t>
         </is>
@@ -14969,7 +15617,13 @@
       <c r="AN111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO111" t="inlineStr">
+      <c r="AO111" t="n">
+        <v>2539</v>
+      </c>
+      <c r="AP111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ111" t="inlineStr">
         <is>
           <t>2539</t>
         </is>
@@ -15102,7 +15756,13 @@
       <c r="AN112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO112" t="inlineStr">
+      <c r="AO112" t="n">
+        <v>2566</v>
+      </c>
+      <c r="AP112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ112" t="inlineStr">
         <is>
           <t>2566</t>
         </is>
@@ -15235,7 +15895,13 @@
       <c r="AN113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO113" t="inlineStr">
+      <c r="AO113" t="n">
+        <v>2747</v>
+      </c>
+      <c r="AP113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ113" t="inlineStr">
         <is>
           <t>2747</t>
         </is>
@@ -15368,7 +16034,13 @@
       <c r="AN114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO114" t="inlineStr">
+      <c r="AO114" t="n">
+        <v>2900</v>
+      </c>
+      <c r="AP114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ114" t="inlineStr">
         <is>
           <t>2900</t>
         </is>
@@ -15501,7 +16173,13 @@
       <c r="AN115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO115" t="inlineStr">
+      <c r="AO115" t="n">
+        <v>2008</v>
+      </c>
+      <c r="AP115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ115" t="inlineStr">
         <is>
           <t>2008</t>
         </is>
@@ -15634,7 +16312,13 @@
       <c r="AN116" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="AO116" t="inlineStr">
+      <c r="AO116" t="n">
+        <v>2752</v>
+      </c>
+      <c r="AP116" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="AQ116" t="inlineStr">
         <is>
           <t>2752</t>
         </is>
@@ -15767,7 +16451,13 @@
       <c r="AN117" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AO117" t="inlineStr">
+      <c r="AO117" t="n">
+        <v>2997</v>
+      </c>
+      <c r="AP117" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AQ117" t="inlineStr">
         <is>
           <t>2997</t>
         </is>
@@ -15900,7 +16590,13 @@
       <c r="AN118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO118" t="inlineStr">
+      <c r="AO118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16033,7 +16729,13 @@
       <c r="AN119" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="AO119" t="inlineStr">
+      <c r="AO119" t="n">
+        <v>3172</v>
+      </c>
+      <c r="AP119" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="AQ119" t="inlineStr">
         <is>
           <t>3172</t>
         </is>
@@ -16166,7 +16868,13 @@
       <c r="AN120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO120" t="inlineStr">
+      <c r="AO120" t="n">
+        <v>2398</v>
+      </c>
+      <c r="AP120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ120" t="inlineStr">
         <is>
           <t>2398</t>
         </is>
@@ -16299,7 +17007,13 @@
       <c r="AN121" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AO121" t="inlineStr">
+      <c r="AO121" t="n">
+        <v>2829</v>
+      </c>
+      <c r="AP121" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AQ121" t="inlineStr">
         <is>
           <t>2829</t>
         </is>
@@ -16432,7 +17146,13 @@
       <c r="AN122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO122" t="inlineStr">
+      <c r="AO122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16565,7 +17285,13 @@
       <c r="AN123" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AO123" t="inlineStr">
+      <c r="AO123" t="n">
+        <v>2777</v>
+      </c>
+      <c r="AP123" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ123" t="inlineStr">
         <is>
           <t>2777</t>
         </is>
@@ -16698,7 +17424,13 @@
       <c r="AN124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AO124" t="inlineStr">
+      <c r="AO124" t="n">
+        <v>2819</v>
+      </c>
+      <c r="AP124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ124" t="inlineStr">
         <is>
           <t>2819</t>
         </is>
@@ -16831,7 +17563,13 @@
       <c r="AN125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO125" t="inlineStr">
+      <c r="AO125" t="n">
+        <v>2569</v>
+      </c>
+      <c r="AP125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ125" t="inlineStr">
         <is>
           <t>2569</t>
         </is>
@@ -16964,7 +17702,13 @@
       <c r="AN126" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AO126" t="inlineStr">
+      <c r="AO126" t="n">
+        <v>2857</v>
+      </c>
+      <c r="AP126" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AQ126" t="inlineStr">
         <is>
           <t>2857</t>
         </is>
@@ -17097,7 +17841,13 @@
       <c r="AN127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO127" t="inlineStr">
+      <c r="AO127" t="n">
+        <v>2389</v>
+      </c>
+      <c r="AP127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ127" t="inlineStr">
         <is>
           <t>2389</t>
         </is>
@@ -17230,7 +17980,13 @@
       <c r="AN128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO128" t="inlineStr">
+      <c r="AO128" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -17363,7 +18119,13 @@
       <c r="AN129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO129" t="inlineStr">
+      <c r="AO129" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -17496,7 +18258,13 @@
       <c r="AN130" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AO130" t="inlineStr">
+      <c r="AO130" t="n">
+        <v>2630</v>
+      </c>
+      <c r="AP130" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AQ130" t="inlineStr">
         <is>
           <t>2630</t>
         </is>
@@ -17629,7 +18397,13 @@
       <c r="AN131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO131" t="inlineStr">
+      <c r="AO131" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -17762,7 +18536,13 @@
       <c r="AN132" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AO132" t="inlineStr">
+      <c r="AO132" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AP132" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ132" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -17895,7 +18675,13 @@
       <c r="AN133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO133" t="inlineStr">
+      <c r="AO133" t="n">
+        <v>2472</v>
+      </c>
+      <c r="AP133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ133" t="inlineStr">
         <is>
           <t>2472</t>
         </is>
@@ -17979,6 +18765,8 @@
       <c r="AM134" t="inlineStr"/>
       <c r="AN134" s="3" t="inlineStr"/>
       <c r="AO134" t="inlineStr"/>
+      <c r="AP134" s="3" t="inlineStr"/>
+      <c r="AQ134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -18050,6 +18838,8 @@
       <c r="AM135" t="inlineStr"/>
       <c r="AN135" s="3" t="inlineStr"/>
       <c r="AO135" t="inlineStr"/>
+      <c r="AP135" s="3" t="inlineStr"/>
+      <c r="AQ135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -18178,7 +18968,13 @@
       <c r="AN136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO136" t="inlineStr">
+      <c r="AO136" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ136" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18311,7 +19107,13 @@
       <c r="AN137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO137" t="inlineStr">
+      <c r="AO137" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18387,6 +19189,8 @@
       <c r="AM138" t="inlineStr"/>
       <c r="AN138" s="3" t="inlineStr"/>
       <c r="AO138" t="inlineStr"/>
+      <c r="AP138" s="3" t="inlineStr"/>
+      <c r="AQ138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -18515,7 +19319,13 @@
       <c r="AN139" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AO139" t="inlineStr">
+      <c r="AO139" t="n">
+        <v>2046</v>
+      </c>
+      <c r="AP139" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AQ139" t="inlineStr">
         <is>
           <t>2046</t>
         </is>
@@ -18648,7 +19458,13 @@
       <c r="AN140" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AO140" t="inlineStr">
+      <c r="AO140" t="n">
+        <v>2570</v>
+      </c>
+      <c r="AP140" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AQ140" t="inlineStr">
         <is>
           <t>2570</t>
         </is>
@@ -18724,6 +19540,8 @@
       <c r="AM141" t="inlineStr"/>
       <c r="AN141" s="3" t="inlineStr"/>
       <c r="AO141" t="inlineStr"/>
+      <c r="AP141" s="3" t="inlineStr"/>
+      <c r="AQ141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -18852,7 +19670,13 @@
       <c r="AN142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO142" t="inlineStr">
+      <c r="AO142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ142" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18928,6 +19752,8 @@
       <c r="AM143" t="inlineStr"/>
       <c r="AN143" s="3" t="inlineStr"/>
       <c r="AO143" t="inlineStr"/>
+      <c r="AP143" s="3" t="inlineStr"/>
+      <c r="AQ143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -18999,6 +19825,8 @@
       <c r="AM144" t="inlineStr"/>
       <c r="AN144" s="3" t="inlineStr"/>
       <c r="AO144" t="inlineStr"/>
+      <c r="AP144" s="3" t="inlineStr"/>
+      <c r="AQ144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -19070,6 +19898,8 @@
       <c r="AM145" t="inlineStr"/>
       <c r="AN145" s="3" t="inlineStr"/>
       <c r="AO145" t="inlineStr"/>
+      <c r="AP145" s="3" t="inlineStr"/>
+      <c r="AQ145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -19141,6 +19971,8 @@
       <c r="AM146" t="inlineStr"/>
       <c r="AN146" s="3" t="inlineStr"/>
       <c r="AO146" t="inlineStr"/>
+      <c r="AP146" s="3" t="inlineStr"/>
+      <c r="AQ146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -19212,6 +20044,8 @@
       <c r="AM147" t="inlineStr"/>
       <c r="AN147" s="3" t="inlineStr"/>
       <c r="AO147" t="inlineStr"/>
+      <c r="AP147" s="3" t="inlineStr"/>
+      <c r="AQ147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -19340,7 +20174,13 @@
       <c r="AN148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO148" t="inlineStr">
+      <c r="AO148" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -19473,7 +20313,13 @@
       <c r="AN149" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AO149" t="inlineStr">
+      <c r="AO149" t="n">
+        <v>2926</v>
+      </c>
+      <c r="AP149" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ149" t="inlineStr">
         <is>
           <t>2926</t>
         </is>
@@ -19606,7 +20452,13 @@
       <c r="AN150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO150" t="inlineStr">
+      <c r="AO150" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -19739,7 +20591,13 @@
       <c r="AN151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO151" t="inlineStr">
+      <c r="AO151" t="n">
+        <v>2552</v>
+      </c>
+      <c r="AP151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ151" t="inlineStr">
         <is>
           <t>2552</t>
         </is>
@@ -19872,7 +20730,13 @@
       <c r="AN152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO152" t="inlineStr">
+      <c r="AO152" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -20005,7 +20869,13 @@
       <c r="AN153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO153" t="inlineStr">
+      <c r="AO153" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -20138,7 +21008,13 @@
       <c r="AN154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO154" t="inlineStr">
+      <c r="AO154" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -20271,7 +21147,13 @@
       <c r="AN155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO155" t="inlineStr">
+      <c r="AO155" t="n">
+        <v>2549</v>
+      </c>
+      <c r="AP155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ155" t="inlineStr">
         <is>
           <t>2549</t>
         </is>
@@ -20398,7 +21280,13 @@
       <c r="AN156" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="AO156" t="inlineStr">
+      <c r="AO156" t="n">
+        <v>2956</v>
+      </c>
+      <c r="AP156" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="AQ156" t="inlineStr">
         <is>
           <t>2956</t>
         </is>
@@ -20468,6 +21356,8 @@
       <c r="AM157" t="inlineStr"/>
       <c r="AN157" s="3" t="inlineStr"/>
       <c r="AO157" t="inlineStr"/>
+      <c r="AP157" s="3" t="inlineStr"/>
+      <c r="AQ157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -20590,7 +21480,13 @@
       <c r="AN158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO158" t="inlineStr">
+      <c r="AO158" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -20717,7 +21613,13 @@
       <c r="AN159" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AO159" t="inlineStr">
+      <c r="AO159" t="n">
+        <v>2729</v>
+      </c>
+      <c r="AP159" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ159" t="inlineStr">
         <is>
           <t>2729</t>
         </is>
@@ -20787,6 +21689,8 @@
       <c r="AM160" t="inlineStr"/>
       <c r="AN160" s="3" t="inlineStr"/>
       <c r="AO160" t="inlineStr"/>
+      <c r="AP160" s="3" t="inlineStr"/>
+      <c r="AQ160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -20897,7 +21801,13 @@
       <c r="AN161" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AO161" t="inlineStr">
+      <c r="AO161" t="n">
+        <v>2778</v>
+      </c>
+      <c r="AP161" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AQ161" t="inlineStr">
         <is>
           <t>2778</t>
         </is>
@@ -21012,7 +21922,13 @@
       <c r="AN162" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AO162" t="inlineStr">
+      <c r="AO162" t="n">
+        <v>2685</v>
+      </c>
+      <c r="AP162" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ162" t="inlineStr">
         <is>
           <t>2685</t>
         </is>
@@ -21123,7 +22039,13 @@
       <c r="AN163" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AO163" t="inlineStr">
+      <c r="AO163" t="n">
+        <v>2789</v>
+      </c>
+      <c r="AP163" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ163" t="inlineStr">
         <is>
           <t>2789</t>
         </is>
@@ -21218,7 +22140,13 @@
       <c r="AN164" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AO164" t="inlineStr">
+      <c r="AO164" t="n">
+        <v>2786</v>
+      </c>
+      <c r="AP164" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AQ164" t="inlineStr">
         <is>
           <t>2786</t>
         </is>
@@ -21317,7 +22245,13 @@
       <c r="AN165" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="AO165" t="inlineStr">
+      <c r="AO165" t="n">
+        <v>2505</v>
+      </c>
+      <c r="AP165" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AQ165" t="inlineStr">
         <is>
           <t>2505</t>
         </is>
@@ -21408,7 +22342,13 @@
       <c r="AN166" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="AO166" t="inlineStr">
+      <c r="AO166" t="n">
+        <v>2828</v>
+      </c>
+      <c r="AP166" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="AQ166" t="inlineStr">
         <is>
           <t>2828</t>
         </is>
@@ -21487,7 +22427,13 @@
       <c r="AN167" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO167" t="inlineStr">
+      <c r="AO167" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP167" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ167" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -21562,7 +22508,13 @@
       <c r="AN168" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="AO168" t="inlineStr">
+      <c r="AO168" t="n">
+        <v>1536</v>
+      </c>
+      <c r="AP168" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AQ168" t="inlineStr">
         <is>
           <t>1536</t>
         </is>
@@ -21624,6 +22576,8 @@
       <c r="AM169" t="inlineStr"/>
       <c r="AN169" s="3" t="inlineStr"/>
       <c r="AO169" t="inlineStr"/>
+      <c r="AP169" s="3" t="inlineStr"/>
+      <c r="AQ169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="n">
@@ -21690,17 +22644,21 @@
       <c r="AN170" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO170" t="inlineStr">
+      <c r="AO170" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP170" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ170" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
     </row>
     <row r="171">
-      <c r="A171" t="inlineStr">
-        <is>
-          <t>41231396</t>
-        </is>
+      <c r="A171" t="n">
+        <v>41231396</v>
       </c>
       <c r="B171" t="inlineStr">
         <is>
@@ -21751,17 +22709,21 @@
       <c r="AN171" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="AO171" t="inlineStr">
+      <c r="AO171" t="n">
+        <v>1555</v>
+      </c>
+      <c r="AP171" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ171" t="inlineStr">
         <is>
           <t>1555</t>
         </is>
       </c>
     </row>
     <row r="172">
-      <c r="A172" t="inlineStr">
-        <is>
-          <t>58174442</t>
-        </is>
+      <c r="A172" t="n">
+        <v>58174442</v>
       </c>
       <c r="B172" t="inlineStr">
         <is>
@@ -21812,17 +22774,21 @@
       <c r="AN172" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO172" t="inlineStr">
+      <c r="AO172" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP172" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ172" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
     </row>
     <row r="173">
-      <c r="A173" t="inlineStr">
-        <is>
-          <t>58671339</t>
-        </is>
+      <c r="A173" t="n">
+        <v>58671339</v>
       </c>
       <c r="B173" t="inlineStr">
         <is>
@@ -21873,7 +22839,13 @@
       <c r="AN173" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="AO173" t="inlineStr">
+      <c r="AO173" t="n">
+        <v>1708</v>
+      </c>
+      <c r="AP173" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="AQ173" t="inlineStr">
         <is>
           <t>1708</t>
         </is>

</xml_diff>

<commit_message>
Code updated 23-03-03 11:30:34
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -742,7 +742,7 @@
       </c>
       <c r="AQ2" t="inlineStr">
         <is>
-          <t>2517</t>
+          <t>2575</t>
         </is>
       </c>
     </row>
@@ -876,12 +876,12 @@
       <c r="AO3" t="n">
         <v>3853</v>
       </c>
-      <c r="AP3" s="3" t="n">
-        <v>20</v>
+      <c r="AP3" s="4" t="n">
+        <v>15</v>
       </c>
       <c r="AQ3" t="inlineStr">
         <is>
-          <t>3853</t>
+          <t>4096</t>
         </is>
       </c>
     </row>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="AQ4" t="inlineStr">
         <is>
-          <t>4003</t>
+          <t>4263</t>
         </is>
       </c>
     </row>
@@ -1043,7 +1043,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F5" s="3" t="n">
@@ -1159,7 +1159,7 @@
       </c>
       <c r="AQ5" t="inlineStr">
         <is>
-          <t>3737</t>
+          <t>4040</t>
         </is>
       </c>
     </row>
@@ -1294,11 +1294,11 @@
         <v>3716</v>
       </c>
       <c r="AP6" s="3" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="AQ6" t="inlineStr">
         <is>
-          <t>3716</t>
+          <t>4035</t>
         </is>
       </c>
     </row>
@@ -1437,7 +1437,7 @@
       </c>
       <c r="AQ7" t="inlineStr">
         <is>
-          <t>4013</t>
+          <t>4409</t>
         </is>
       </c>
     </row>
@@ -1576,7 +1576,7 @@
       </c>
       <c r="AQ8" t="inlineStr">
         <is>
-          <t>3582</t>
+          <t>3838</t>
         </is>
       </c>
     </row>
@@ -1715,7 +1715,7 @@
       </c>
       <c r="AQ9" t="inlineStr">
         <is>
-          <t>3572</t>
+          <t>3865</t>
         </is>
       </c>
     </row>
@@ -1854,7 +1854,7 @@
       </c>
       <c r="AQ10" t="inlineStr">
         <is>
-          <t>3821</t>
+          <t>3976</t>
         </is>
       </c>
     </row>
@@ -1993,7 +1993,7 @@
       </c>
       <c r="AQ11" t="inlineStr">
         <is>
-          <t>3529</t>
+          <t>3727</t>
         </is>
       </c>
     </row>
@@ -2267,11 +2267,11 @@
         <v>4252</v>
       </c>
       <c r="AP13" s="5" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AQ13" t="inlineStr">
         <is>
-          <t>4252</t>
+          <t>4544</t>
         </is>
       </c>
     </row>
@@ -2410,7 +2410,7 @@
       </c>
       <c r="AQ14" t="inlineStr">
         <is>
-          <t>3731</t>
+          <t>4033</t>
         </is>
       </c>
     </row>
@@ -2688,7 +2688,7 @@
       </c>
       <c r="AQ16" t="inlineStr">
         <is>
-          <t>3956</t>
+          <t>4209</t>
         </is>
       </c>
     </row>
@@ -2827,7 +2827,7 @@
       </c>
       <c r="AQ17" t="inlineStr">
         <is>
-          <t>3282</t>
+          <t>3587</t>
         </is>
       </c>
     </row>
@@ -2962,11 +2962,11 @@
         <v>3424</v>
       </c>
       <c r="AP18" s="3" t="n">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="AQ18" t="inlineStr">
         <is>
-          <t>3424</t>
+          <t>3552</t>
         </is>
       </c>
     </row>
@@ -3105,7 +3105,7 @@
       </c>
       <c r="AQ19" t="inlineStr">
         <is>
-          <t>3842</t>
+          <t>4144</t>
         </is>
       </c>
     </row>
@@ -3240,11 +3240,11 @@
         <v>4404</v>
       </c>
       <c r="AP20" s="5" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AQ20" t="inlineStr">
         <is>
-          <t>4404</t>
+          <t>4681</t>
         </is>
       </c>
     </row>
@@ -3378,12 +3378,12 @@
       <c r="AO21" t="n">
         <v>3093</v>
       </c>
-      <c r="AP21" s="3" t="n">
-        <v>20</v>
+      <c r="AP21" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AQ21" t="inlineStr">
         <is>
-          <t>3093</t>
+          <t>3092</t>
         </is>
       </c>
     </row>
@@ -3522,7 +3522,7 @@
       </c>
       <c r="AQ22" t="inlineStr">
         <is>
-          <t>3689</t>
+          <t>3976</t>
         </is>
       </c>
     </row>
@@ -3656,8 +3656,8 @@
       <c r="AO23" t="n">
         <v>3528</v>
       </c>
-      <c r="AP23" s="3" t="n">
-        <v>20</v>
+      <c r="AP23" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AQ23" t="inlineStr">
         <is>
@@ -3684,7 +3684,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F24" s="5" t="n">
@@ -3800,7 +3800,7 @@
       </c>
       <c r="AQ24" t="inlineStr">
         <is>
-          <t>3893</t>
+          <t>4131</t>
         </is>
       </c>
     </row>
@@ -4074,11 +4074,11 @@
         <v>3945</v>
       </c>
       <c r="AP26" s="5" t="n">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="AQ26" t="inlineStr">
         <is>
-          <t>3945</t>
+          <t>4186</t>
         </is>
       </c>
     </row>
@@ -4217,7 +4217,7 @@
       </c>
       <c r="AQ27" t="inlineStr">
         <is>
-          <t>3401</t>
+          <t>3908</t>
         </is>
       </c>
     </row>
@@ -4356,7 +4356,7 @@
       </c>
       <c r="AQ28" t="inlineStr">
         <is>
-          <t>3255</t>
+          <t>3427</t>
         </is>
       </c>
     </row>
@@ -4495,7 +4495,7 @@
       </c>
       <c r="AQ29" t="inlineStr">
         <is>
-          <t>4287</t>
+          <t>4796</t>
         </is>
       </c>
     </row>
@@ -4634,7 +4634,7 @@
       </c>
       <c r="AQ30" t="inlineStr">
         <is>
-          <t>3583</t>
+          <t>3715</t>
         </is>
       </c>
     </row>
@@ -4769,11 +4769,11 @@
         <v>4033</v>
       </c>
       <c r="AP31" s="5" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AQ31" t="inlineStr">
         <is>
-          <t>4033</t>
+          <t>4372</t>
         </is>
       </c>
     </row>
@@ -4912,7 +4912,7 @@
       </c>
       <c r="AQ32" t="inlineStr">
         <is>
-          <t>3857</t>
+          <t>4278</t>
         </is>
       </c>
     </row>
@@ -5047,11 +5047,11 @@
         <v>3514</v>
       </c>
       <c r="AP33" s="3" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AQ33" t="inlineStr">
         <is>
-          <t>3514</t>
+          <t>3813</t>
         </is>
       </c>
     </row>
@@ -5190,7 +5190,7 @@
       </c>
       <c r="AQ34" t="inlineStr">
         <is>
-          <t>3682</t>
+          <t>3965</t>
         </is>
       </c>
     </row>
@@ -5325,11 +5325,11 @@
         <v>3804</v>
       </c>
       <c r="AP35" s="5" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AQ35" t="inlineStr">
         <is>
-          <t>3804</t>
+          <t>3943</t>
         </is>
       </c>
     </row>
@@ -5463,12 +5463,12 @@
       <c r="AO36" t="n">
         <v>3508</v>
       </c>
-      <c r="AP36" s="4" t="n">
-        <v>19</v>
+      <c r="AP36" s="3" t="n">
+        <v>20</v>
       </c>
       <c r="AQ36" t="inlineStr">
         <is>
-          <t>3508</t>
+          <t>3905</t>
         </is>
       </c>
     </row>
@@ -5607,7 +5607,7 @@
       </c>
       <c r="AQ37" t="inlineStr">
         <is>
-          <t>3532</t>
+          <t>3652</t>
         </is>
       </c>
     </row>
@@ -5746,7 +5746,7 @@
       </c>
       <c r="AQ38" t="inlineStr">
         <is>
-          <t>3801</t>
+          <t>4042</t>
         </is>
       </c>
     </row>
@@ -5885,7 +5885,7 @@
       </c>
       <c r="AQ39" t="inlineStr">
         <is>
-          <t>3816</t>
+          <t>4043</t>
         </is>
       </c>
     </row>
@@ -6019,12 +6019,12 @@
       <c r="AO40" t="n">
         <v>3801</v>
       </c>
-      <c r="AP40" s="5" t="n">
-        <v>33</v>
+      <c r="AP40" s="3" t="n">
+        <v>30</v>
       </c>
       <c r="AQ40" t="inlineStr">
         <is>
-          <t>3801</t>
+          <t>4073</t>
         </is>
       </c>
     </row>
@@ -6298,11 +6298,11 @@
         <v>4202</v>
       </c>
       <c r="AP42" s="5" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="AQ42" t="inlineStr">
         <is>
-          <t>4202</t>
+          <t>4494</t>
         </is>
       </c>
     </row>
@@ -6325,7 +6325,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F43" s="5" t="n">
@@ -6441,7 +6441,7 @@
       </c>
       <c r="AQ43" t="inlineStr">
         <is>
-          <t>3779</t>
+          <t>4197</t>
         </is>
       </c>
     </row>
@@ -6580,7 +6580,7 @@
       </c>
       <c r="AQ44" t="inlineStr">
         <is>
-          <t>3973</t>
+          <t>4233</t>
         </is>
       </c>
     </row>
@@ -6715,11 +6715,11 @@
         <v>3543</v>
       </c>
       <c r="AP45" s="3" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AQ45" t="inlineStr">
         <is>
-          <t>3543</t>
+          <t>3740</t>
         </is>
       </c>
     </row>
@@ -6858,7 +6858,7 @@
       </c>
       <c r="AQ46" t="inlineStr">
         <is>
-          <t>3554</t>
+          <t>3661</t>
         </is>
       </c>
     </row>
@@ -6997,7 +6997,7 @@
       </c>
       <c r="AQ47" t="inlineStr">
         <is>
-          <t>3576</t>
+          <t>3712</t>
         </is>
       </c>
     </row>
@@ -7132,11 +7132,11 @@
         <v>4011</v>
       </c>
       <c r="AP48" s="5" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AQ48" t="inlineStr">
         <is>
-          <t>4011</t>
+          <t>4347</t>
         </is>
       </c>
     </row>
@@ -7275,7 +7275,7 @@
       </c>
       <c r="AQ49" t="inlineStr">
         <is>
-          <t>3005</t>
+          <t>3173</t>
         </is>
       </c>
     </row>
@@ -7409,12 +7409,12 @@
       <c r="AO50" t="n">
         <v>3982</v>
       </c>
-      <c r="AP50" s="5" t="n">
-        <v>33</v>
+      <c r="AP50" s="3" t="n">
+        <v>30</v>
       </c>
       <c r="AQ50" t="inlineStr">
         <is>
-          <t>3982</t>
+          <t>4272</t>
         </is>
       </c>
     </row>
@@ -7553,7 +7553,7 @@
       </c>
       <c r="AQ51" t="inlineStr">
         <is>
-          <t>2523</t>
+          <t>2521</t>
         </is>
       </c>
     </row>
@@ -7692,7 +7692,7 @@
       </c>
       <c r="AQ52" t="inlineStr">
         <is>
-          <t>2535</t>
+          <t>2533</t>
         </is>
       </c>
     </row>
@@ -7831,7 +7831,7 @@
       </c>
       <c r="AQ53" t="inlineStr">
         <is>
-          <t>2935</t>
+          <t>3062</t>
         </is>
       </c>
     </row>
@@ -7965,12 +7965,12 @@
       <c r="AO54" t="n">
         <v>3833</v>
       </c>
-      <c r="AP54" s="5" t="n">
-        <v>31</v>
+      <c r="AP54" s="3" t="n">
+        <v>30</v>
       </c>
       <c r="AQ54" t="inlineStr">
         <is>
-          <t>3833</t>
+          <t>4135</t>
         </is>
       </c>
     </row>
@@ -8109,7 +8109,7 @@
       </c>
       <c r="AQ55" t="inlineStr">
         <is>
-          <t>3308</t>
+          <t>3385</t>
         </is>
       </c>
     </row>
@@ -8248,7 +8248,7 @@
       </c>
       <c r="AQ56" t="inlineStr">
         <is>
-          <t>3296</t>
+          <t>3448</t>
         </is>
       </c>
     </row>
@@ -8387,7 +8387,7 @@
       </c>
       <c r="AQ57" t="inlineStr">
         <is>
-          <t>3665</t>
+          <t>3913</t>
         </is>
       </c>
     </row>
@@ -8526,7 +8526,7 @@
       </c>
       <c r="AQ58" t="inlineStr">
         <is>
-          <t>3224</t>
+          <t>3452</t>
         </is>
       </c>
     </row>
@@ -8779,7 +8779,7 @@
       </c>
       <c r="AQ61" t="inlineStr">
         <is>
-          <t>3549</t>
+          <t>3832</t>
         </is>
       </c>
     </row>
@@ -9053,11 +9053,11 @@
         <v>3633</v>
       </c>
       <c r="AP63" s="3" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AQ63" t="inlineStr">
         <is>
-          <t>3633</t>
+          <t>3934</t>
         </is>
       </c>
     </row>
@@ -9387,12 +9387,12 @@
       <c r="AO66" t="n">
         <v>2542</v>
       </c>
-      <c r="AP66" s="4" t="n">
-        <v>5</v>
+      <c r="AP66" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AQ66" t="inlineStr">
         <is>
-          <t>2542</t>
+          <t>2553</t>
         </is>
       </c>
     </row>
@@ -9527,11 +9527,11 @@
         <v>3605</v>
       </c>
       <c r="AP67" s="3" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AQ67" t="inlineStr">
         <is>
-          <t>3605</t>
+          <t>3829</t>
         </is>
       </c>
     </row>
@@ -9666,11 +9666,11 @@
         <v>3672</v>
       </c>
       <c r="AP68" s="5" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AQ68" t="inlineStr">
         <is>
-          <t>3672</t>
+          <t>3814</t>
         </is>
       </c>
     </row>
@@ -9804,12 +9804,12 @@
       <c r="AO69" t="n">
         <v>3333</v>
       </c>
-      <c r="AP69" s="3" t="n">
-        <v>30</v>
+      <c r="AP69" s="5" t="n">
+        <v>33</v>
       </c>
       <c r="AQ69" t="inlineStr">
         <is>
-          <t>3333</t>
+          <t>3484</t>
         </is>
       </c>
     </row>
@@ -9948,7 +9948,7 @@
       </c>
       <c r="AQ70" t="inlineStr">
         <is>
-          <t>2485</t>
+          <t>2483</t>
         </is>
       </c>
     </row>
@@ -9971,7 +9971,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F71" s="3" t="n">
@@ -10087,7 +10087,7 @@
       </c>
       <c r="AQ71" t="inlineStr">
         <is>
-          <t>3411</t>
+          <t>3581</t>
         </is>
       </c>
     </row>
@@ -10222,11 +10222,11 @@
         <v>2941</v>
       </c>
       <c r="AP72" s="4" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="AQ72" t="inlineStr">
         <is>
-          <t>2941</t>
+          <t>2986</t>
         </is>
       </c>
     </row>
@@ -10365,7 +10365,7 @@
       </c>
       <c r="AQ73" t="inlineStr">
         <is>
-          <t>3295</t>
+          <t>3472</t>
         </is>
       </c>
     </row>
@@ -10504,7 +10504,7 @@
       </c>
       <c r="AQ74" t="inlineStr">
         <is>
-          <t>2625</t>
+          <t>2624</t>
         </is>
       </c>
     </row>
@@ -10639,11 +10639,11 @@
         <v>3165</v>
       </c>
       <c r="AP75" s="3" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AQ75" t="inlineStr">
         <is>
-          <t>3165</t>
+          <t>3321</t>
         </is>
       </c>
     </row>
@@ -10782,7 +10782,7 @@
       </c>
       <c r="AQ76" t="inlineStr">
         <is>
-          <t>3666</t>
+          <t>3951</t>
         </is>
       </c>
     </row>
@@ -11060,7 +11060,7 @@
       </c>
       <c r="AQ78" t="inlineStr">
         <is>
-          <t>3634</t>
+          <t>3858</t>
         </is>
       </c>
     </row>
@@ -11334,11 +11334,11 @@
         <v>3534</v>
       </c>
       <c r="AP80" s="3" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AQ80" t="inlineStr">
         <is>
-          <t>3534</t>
+          <t>3702</t>
         </is>
       </c>
     </row>
@@ -11477,7 +11477,7 @@
       </c>
       <c r="AQ81" t="inlineStr">
         <is>
-          <t>3620</t>
+          <t>3736</t>
         </is>
       </c>
     </row>
@@ -11616,7 +11616,7 @@
       </c>
       <c r="AQ82" t="inlineStr">
         <is>
-          <t>3399</t>
+          <t>3625</t>
         </is>
       </c>
     </row>
@@ -11755,7 +11755,7 @@
       </c>
       <c r="AQ83" t="inlineStr">
         <is>
-          <t>3341</t>
+          <t>3460</t>
         </is>
       </c>
     </row>
@@ -12011,7 +12011,7 @@
       </c>
       <c r="AQ85" t="inlineStr">
         <is>
-          <t>3135</t>
+          <t>3278</t>
         </is>
       </c>
     </row>
@@ -12150,7 +12150,7 @@
       </c>
       <c r="AQ86" t="inlineStr">
         <is>
-          <t>2485</t>
+          <t>2477</t>
         </is>
       </c>
     </row>
@@ -12285,11 +12285,11 @@
         <v>3601</v>
       </c>
       <c r="AP87" s="3" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="AQ87" t="inlineStr">
         <is>
-          <t>3601</t>
+          <t>3746</t>
         </is>
       </c>
     </row>
@@ -12428,7 +12428,7 @@
       </c>
       <c r="AQ88" t="inlineStr">
         <is>
-          <t>2706</t>
+          <t>2746</t>
         </is>
       </c>
     </row>
@@ -12567,7 +12567,7 @@
       </c>
       <c r="AQ89" t="inlineStr">
         <is>
-          <t>2882</t>
+          <t>2895</t>
         </is>
       </c>
     </row>
@@ -12701,12 +12701,12 @@
       <c r="AO90" t="n">
         <v>2516</v>
       </c>
-      <c r="AP90" s="2" t="n">
-        <v>0</v>
+      <c r="AP90" s="3" t="n">
+        <v>20</v>
       </c>
       <c r="AQ90" t="inlineStr">
         <is>
-          <t>2516</t>
+          <t>2637</t>
         </is>
       </c>
     </row>
@@ -12845,7 +12845,7 @@
       </c>
       <c r="AQ91" t="inlineStr">
         <is>
-          <t>2653</t>
+          <t>2671</t>
         </is>
       </c>
     </row>
@@ -13118,12 +13118,12 @@
       <c r="AO93" t="n">
         <v>2334</v>
       </c>
-      <c r="AP93" s="4" t="n">
-        <v>1</v>
+      <c r="AP93" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AQ93" t="inlineStr">
         <is>
-          <t>2334</t>
+          <t>2317</t>
         </is>
       </c>
     </row>
@@ -13401,7 +13401,7 @@
       </c>
       <c r="AQ95" t="inlineStr">
         <is>
-          <t>2417</t>
+          <t>2394</t>
         </is>
       </c>
     </row>
@@ -13540,7 +13540,7 @@
       </c>
       <c r="AQ96" t="inlineStr">
         <is>
-          <t>2516</t>
+          <t>2499</t>
         </is>
       </c>
     </row>
@@ -13953,11 +13953,11 @@
         <v>2966</v>
       </c>
       <c r="AP99" s="4" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AQ99" t="inlineStr">
         <is>
-          <t>2966</t>
+          <t>3038</t>
         </is>
       </c>
     </row>
@@ -14096,7 +14096,7 @@
       </c>
       <c r="AQ100" t="inlineStr">
         <is>
-          <t>2443</t>
+          <t>2432</t>
         </is>
       </c>
     </row>
@@ -14235,7 +14235,7 @@
       </c>
       <c r="AQ101" t="inlineStr">
         <is>
-          <t>3481</t>
+          <t>3651</t>
         </is>
       </c>
     </row>
@@ -14374,7 +14374,7 @@
       </c>
       <c r="AQ102" t="inlineStr">
         <is>
-          <t>3124</t>
+          <t>3270</t>
         </is>
       </c>
     </row>
@@ -14513,7 +14513,7 @@
       </c>
       <c r="AQ103" t="inlineStr">
         <is>
-          <t>2453</t>
+          <t>2450</t>
         </is>
       </c>
     </row>
@@ -14652,7 +14652,7 @@
       </c>
       <c r="AQ104" t="inlineStr">
         <is>
-          <t>3541</t>
+          <t>3695</t>
         </is>
       </c>
     </row>
@@ -14786,12 +14786,12 @@
       <c r="AO105" t="n">
         <v>3275</v>
       </c>
-      <c r="AP105" s="3" t="n">
-        <v>22</v>
+      <c r="AP105" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AQ105" t="inlineStr">
         <is>
-          <t>3275</t>
+          <t>3228</t>
         </is>
       </c>
     </row>
@@ -15069,7 +15069,7 @@
       </c>
       <c r="AQ107" t="inlineStr">
         <is>
-          <t>2545</t>
+          <t>2577</t>
         </is>
       </c>
     </row>
@@ -15347,7 +15347,7 @@
       </c>
       <c r="AQ109" t="inlineStr">
         <is>
-          <t>2893</t>
+          <t>2940</t>
         </is>
       </c>
     </row>
@@ -15486,7 +15486,7 @@
       </c>
       <c r="AQ110" t="inlineStr">
         <is>
-          <t>3017</t>
+          <t>3181</t>
         </is>
       </c>
     </row>
@@ -15625,7 +15625,7 @@
       </c>
       <c r="AQ111" t="inlineStr">
         <is>
-          <t>2539</t>
+          <t>2545</t>
         </is>
       </c>
     </row>
@@ -15764,7 +15764,7 @@
       </c>
       <c r="AQ112" t="inlineStr">
         <is>
-          <t>2566</t>
+          <t>2572</t>
         </is>
       </c>
     </row>
@@ -15903,7 +15903,7 @@
       </c>
       <c r="AQ113" t="inlineStr">
         <is>
-          <t>2747</t>
+          <t>2983</t>
         </is>
       </c>
     </row>
@@ -16042,7 +16042,7 @@
       </c>
       <c r="AQ114" t="inlineStr">
         <is>
-          <t>2900</t>
+          <t>3059</t>
         </is>
       </c>
     </row>
@@ -16181,7 +16181,7 @@
       </c>
       <c r="AQ115" t="inlineStr">
         <is>
-          <t>2008</t>
+          <t>2001</t>
         </is>
       </c>
     </row>
@@ -16316,11 +16316,11 @@
         <v>2752</v>
       </c>
       <c r="AP116" s="4" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AQ116" t="inlineStr">
         <is>
-          <t>2752</t>
+          <t>2834</t>
         </is>
       </c>
     </row>
@@ -16459,7 +16459,7 @@
       </c>
       <c r="AQ117" t="inlineStr">
         <is>
-          <t>2997</t>
+          <t>3099</t>
         </is>
       </c>
     </row>
@@ -16732,12 +16732,12 @@
       <c r="AO119" t="n">
         <v>3172</v>
       </c>
-      <c r="AP119" s="4" t="n">
-        <v>11</v>
+      <c r="AP119" s="5" t="n">
+        <v>36</v>
       </c>
       <c r="AQ119" t="inlineStr">
         <is>
-          <t>3172</t>
+          <t>3363</t>
         </is>
       </c>
     </row>
@@ -16876,7 +16876,7 @@
       </c>
       <c r="AQ120" t="inlineStr">
         <is>
-          <t>2398</t>
+          <t>2423</t>
         </is>
       </c>
     </row>
@@ -17015,7 +17015,7 @@
       </c>
       <c r="AQ121" t="inlineStr">
         <is>
-          <t>2829</t>
+          <t>2921</t>
         </is>
       </c>
     </row>
@@ -17288,12 +17288,12 @@
       <c r="AO123" t="n">
         <v>2777</v>
       </c>
-      <c r="AP123" s="3" t="n">
-        <v>20</v>
+      <c r="AP123" s="4" t="n">
+        <v>11</v>
       </c>
       <c r="AQ123" t="inlineStr">
         <is>
-          <t>2777</t>
+          <t>2822</t>
         </is>
       </c>
     </row>
@@ -17432,7 +17432,7 @@
       </c>
       <c r="AQ124" t="inlineStr">
         <is>
-          <t>2819</t>
+          <t>2991</t>
         </is>
       </c>
     </row>
@@ -17571,7 +17571,7 @@
       </c>
       <c r="AQ125" t="inlineStr">
         <is>
-          <t>2569</t>
+          <t>2633</t>
         </is>
       </c>
     </row>
@@ -17710,7 +17710,7 @@
       </c>
       <c r="AQ126" t="inlineStr">
         <is>
-          <t>2857</t>
+          <t>2923</t>
         </is>
       </c>
     </row>
@@ -17849,7 +17849,7 @@
       </c>
       <c r="AQ127" t="inlineStr">
         <is>
-          <t>2389</t>
+          <t>2355</t>
         </is>
       </c>
     </row>
@@ -18262,11 +18262,11 @@
         <v>2630</v>
       </c>
       <c r="AP130" s="3" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AQ130" t="inlineStr">
         <is>
-          <t>2630</t>
+          <t>2706</t>
         </is>
       </c>
     </row>
@@ -18544,7 +18544,7 @@
       </c>
       <c r="AQ132" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>2532</t>
         </is>
       </c>
     </row>
@@ -18678,12 +18678,12 @@
       <c r="AO133" t="n">
         <v>2472</v>
       </c>
-      <c r="AP133" s="2" t="n">
-        <v>0</v>
+      <c r="AP133" s="4" t="n">
+        <v>5</v>
       </c>
       <c r="AQ133" t="inlineStr">
         <is>
-          <t>2472</t>
+          <t>2578</t>
         </is>
       </c>
     </row>
@@ -19322,12 +19322,12 @@
       <c r="AO139" t="n">
         <v>2046</v>
       </c>
-      <c r="AP139" s="4" t="n">
-        <v>5</v>
+      <c r="AP139" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AQ139" t="inlineStr">
         <is>
-          <t>2046</t>
+          <t>2043</t>
         </is>
       </c>
     </row>
@@ -19461,12 +19461,12 @@
       <c r="AO140" t="n">
         <v>2570</v>
       </c>
-      <c r="AP140" s="4" t="n">
-        <v>5</v>
+      <c r="AP140" s="3" t="n">
+        <v>20</v>
       </c>
       <c r="AQ140" t="inlineStr">
         <is>
-          <t>2570</t>
+          <t>2676</t>
         </is>
       </c>
     </row>
@@ -20316,12 +20316,12 @@
       <c r="AO149" t="n">
         <v>2926</v>
       </c>
-      <c r="AP149" s="3" t="n">
-        <v>20</v>
+      <c r="AP149" s="4" t="n">
+        <v>19</v>
       </c>
       <c r="AQ149" t="inlineStr">
         <is>
-          <t>2926</t>
+          <t>3324</t>
         </is>
       </c>
     </row>
@@ -21155,7 +21155,7 @@
       </c>
       <c r="AQ155" t="inlineStr">
         <is>
-          <t>2549</t>
+          <t>2586</t>
         </is>
       </c>
     </row>
@@ -21283,12 +21283,12 @@
       <c r="AO156" t="n">
         <v>2956</v>
       </c>
-      <c r="AP156" s="4" t="n">
-        <v>15</v>
+      <c r="AP156" s="3" t="n">
+        <v>21</v>
       </c>
       <c r="AQ156" t="inlineStr">
         <is>
-          <t>2956</t>
+          <t>3118</t>
         </is>
       </c>
     </row>
@@ -21621,7 +21621,7 @@
       </c>
       <c r="AQ159" t="inlineStr">
         <is>
-          <t>2729</t>
+          <t>2816</t>
         </is>
       </c>
     </row>
@@ -21809,7 +21809,7 @@
       </c>
       <c r="AQ161" t="inlineStr">
         <is>
-          <t>2778</t>
+          <t>2925</t>
         </is>
       </c>
     </row>
@@ -21925,12 +21925,12 @@
       <c r="AO162" t="n">
         <v>2685</v>
       </c>
-      <c r="AP162" s="3" t="n">
-        <v>20</v>
+      <c r="AP162" s="4" t="n">
+        <v>3</v>
       </c>
       <c r="AQ162" t="inlineStr">
         <is>
-          <t>2685</t>
+          <t>2579</t>
         </is>
       </c>
     </row>
@@ -22047,7 +22047,7 @@
       </c>
       <c r="AQ163" t="inlineStr">
         <is>
-          <t>2789</t>
+          <t>2988</t>
         </is>
       </c>
     </row>
@@ -22144,11 +22144,11 @@
         <v>2786</v>
       </c>
       <c r="AP164" s="3" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AQ164" t="inlineStr">
         <is>
-          <t>2786</t>
+          <t>2935</t>
         </is>
       </c>
     </row>
@@ -22248,12 +22248,12 @@
       <c r="AO165" t="n">
         <v>2505</v>
       </c>
-      <c r="AP165" s="4" t="n">
-        <v>6</v>
+      <c r="AP165" s="3" t="n">
+        <v>23</v>
       </c>
       <c r="AQ165" t="inlineStr">
         <is>
-          <t>2505</t>
+          <t>2647</t>
         </is>
       </c>
     </row>
@@ -22345,12 +22345,12 @@
       <c r="AO166" t="n">
         <v>2828</v>
       </c>
-      <c r="AP166" s="4" t="n">
-        <v>9</v>
+      <c r="AP166" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AQ166" t="inlineStr">
         <is>
-          <t>2828</t>
+          <t>2791</t>
         </is>
       </c>
     </row>
@@ -22511,8 +22511,8 @@
       <c r="AO168" t="n">
         <v>1536</v>
       </c>
-      <c r="AP168" s="4" t="n">
-        <v>3</v>
+      <c r="AP168" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AQ168" t="inlineStr">
         <is>
@@ -22713,11 +22713,11 @@
         <v>1555</v>
       </c>
       <c r="AP171" s="4" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="AQ171" t="inlineStr">
         <is>
-          <t>1555</t>
+          <t>1647</t>
         </is>
       </c>
     </row>
@@ -22843,11 +22843,11 @@
         <v>1708</v>
       </c>
       <c r="AP173" s="4" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="AQ173" t="inlineStr">
         <is>
-          <t>1708</t>
+          <t>1640</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-03-04 00:03:32
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ173"/>
+  <dimension ref="A1:AS173"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -606,6 +606,16 @@
           <t>03-02_0</t>
         </is>
       </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>03-03_A</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>03-03_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -740,7 +750,13 @@
       <c r="AP2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ2" t="inlineStr">
+      <c r="AQ2" t="n">
+        <v>2575</v>
+      </c>
+      <c r="AR2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS2" t="inlineStr">
         <is>
           <t>2575</t>
         </is>
@@ -879,7 +895,13 @@
       <c r="AP3" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="AQ3" t="inlineStr">
+      <c r="AQ3" t="n">
+        <v>4096</v>
+      </c>
+      <c r="AR3" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="AS3" t="inlineStr">
         <is>
           <t>4096</t>
         </is>
@@ -1018,7 +1040,13 @@
       <c r="AP4" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AQ4" t="inlineStr">
+      <c r="AQ4" t="n">
+        <v>4263</v>
+      </c>
+      <c r="AR4" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AS4" t="inlineStr">
         <is>
           <t>4263</t>
         </is>
@@ -1157,7 +1185,13 @@
       <c r="AP5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AQ5" t="inlineStr">
+      <c r="AQ5" t="n">
+        <v>4040</v>
+      </c>
+      <c r="AR5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AS5" t="inlineStr">
         <is>
           <t>4040</t>
         </is>
@@ -1296,7 +1330,13 @@
       <c r="AP6" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AQ6" t="inlineStr">
+      <c r="AQ6" t="n">
+        <v>4035</v>
+      </c>
+      <c r="AR6" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AS6" t="inlineStr">
         <is>
           <t>4035</t>
         </is>
@@ -1435,7 +1475,13 @@
       <c r="AP7" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AQ7" t="inlineStr">
+      <c r="AQ7" t="n">
+        <v>4409</v>
+      </c>
+      <c r="AR7" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AS7" t="inlineStr">
         <is>
           <t>4409</t>
         </is>
@@ -1574,7 +1620,13 @@
       <c r="AP8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AQ8" t="inlineStr">
+      <c r="AQ8" t="n">
+        <v>3838</v>
+      </c>
+      <c r="AR8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AS8" t="inlineStr">
         <is>
           <t>3838</t>
         </is>
@@ -1713,7 +1765,13 @@
       <c r="AP9" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AQ9" t="inlineStr">
+      <c r="AQ9" t="n">
+        <v>3865</v>
+      </c>
+      <c r="AR9" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AS9" t="inlineStr">
         <is>
           <t>3865</t>
         </is>
@@ -1852,7 +1910,13 @@
       <c r="AP10" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AQ10" t="inlineStr">
+      <c r="AQ10" t="n">
+        <v>3976</v>
+      </c>
+      <c r="AR10" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AS10" t="inlineStr">
         <is>
           <t>3976</t>
         </is>
@@ -1991,7 +2055,13 @@
       <c r="AP11" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AQ11" t="inlineStr">
+      <c r="AQ11" t="n">
+        <v>3727</v>
+      </c>
+      <c r="AR11" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AS11" t="inlineStr">
         <is>
           <t>3727</t>
         </is>
@@ -2130,7 +2200,13 @@
       <c r="AP12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ12" t="inlineStr">
+      <c r="AQ12" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AR12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS12" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2269,7 +2345,13 @@
       <c r="AP13" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AQ13" t="inlineStr">
+      <c r="AQ13" t="n">
+        <v>4544</v>
+      </c>
+      <c r="AR13" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AS13" t="inlineStr">
         <is>
           <t>4544</t>
         </is>
@@ -2408,7 +2490,13 @@
       <c r="AP14" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AQ14" t="inlineStr">
+      <c r="AQ14" t="n">
+        <v>4033</v>
+      </c>
+      <c r="AR14" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AS14" t="inlineStr">
         <is>
           <t>4033</t>
         </is>
@@ -2547,7 +2635,13 @@
       <c r="AP15" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ15" t="inlineStr">
+      <c r="AQ15" t="n">
+        <v>2539</v>
+      </c>
+      <c r="AR15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS15" t="inlineStr">
         <is>
           <t>2539</t>
         </is>
@@ -2686,7 +2780,13 @@
       <c r="AP16" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AQ16" t="inlineStr">
+      <c r="AQ16" t="n">
+        <v>4209</v>
+      </c>
+      <c r="AR16" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AS16" t="inlineStr">
         <is>
           <t>4209</t>
         </is>
@@ -2825,7 +2925,13 @@
       <c r="AP17" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AQ17" t="inlineStr">
+      <c r="AQ17" t="n">
+        <v>3587</v>
+      </c>
+      <c r="AR17" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AS17" t="inlineStr">
         <is>
           <t>3587</t>
         </is>
@@ -2964,7 +3070,13 @@
       <c r="AP18" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="AQ18" t="inlineStr">
+      <c r="AQ18" t="n">
+        <v>3552</v>
+      </c>
+      <c r="AR18" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AS18" t="inlineStr">
         <is>
           <t>3552</t>
         </is>
@@ -3103,7 +3215,13 @@
       <c r="AP19" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AQ19" t="inlineStr">
+      <c r="AQ19" t="n">
+        <v>4144</v>
+      </c>
+      <c r="AR19" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AS19" t="inlineStr">
         <is>
           <t>4144</t>
         </is>
@@ -3242,7 +3360,13 @@
       <c r="AP20" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AQ20" t="inlineStr">
+      <c r="AQ20" t="n">
+        <v>4681</v>
+      </c>
+      <c r="AR20" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AS20" t="inlineStr">
         <is>
           <t>4681</t>
         </is>
@@ -3381,7 +3505,13 @@
       <c r="AP21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ21" t="inlineStr">
+      <c r="AQ21" t="n">
+        <v>3092</v>
+      </c>
+      <c r="AR21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS21" t="inlineStr">
         <is>
           <t>3092</t>
         </is>
@@ -3520,7 +3650,13 @@
       <c r="AP22" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AQ22" t="inlineStr">
+      <c r="AQ22" t="n">
+        <v>3976</v>
+      </c>
+      <c r="AR22" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AS22" t="inlineStr">
         <is>
           <t>3976</t>
         </is>
@@ -3659,7 +3795,13 @@
       <c r="AP23" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ23" t="inlineStr">
+      <c r="AQ23" t="n">
+        <v>3528</v>
+      </c>
+      <c r="AR23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS23" t="inlineStr">
         <is>
           <t>3528</t>
         </is>
@@ -3798,7 +3940,13 @@
       <c r="AP24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AQ24" t="inlineStr">
+      <c r="AQ24" t="n">
+        <v>4131</v>
+      </c>
+      <c r="AR24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AS24" t="inlineStr">
         <is>
           <t>4131</t>
         </is>
@@ -3937,7 +4085,13 @@
       <c r="AP25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ25" t="inlineStr">
+      <c r="AQ25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4076,7 +4230,13 @@
       <c r="AP26" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AQ26" t="inlineStr">
+      <c r="AQ26" t="n">
+        <v>4186</v>
+      </c>
+      <c r="AR26" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AS26" t="inlineStr">
         <is>
           <t>4186</t>
         </is>
@@ -4215,7 +4375,13 @@
       <c r="AP27" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AQ27" t="inlineStr">
+      <c r="AQ27" t="n">
+        <v>3908</v>
+      </c>
+      <c r="AR27" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AS27" t="inlineStr">
         <is>
           <t>3908</t>
         </is>
@@ -4354,7 +4520,13 @@
       <c r="AP28" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="AQ28" t="inlineStr">
+      <c r="AQ28" t="n">
+        <v>3427</v>
+      </c>
+      <c r="AR28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="AS28" t="inlineStr">
         <is>
           <t>3427</t>
         </is>
@@ -4493,7 +4665,13 @@
       <c r="AP29" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AQ29" t="inlineStr">
+      <c r="AQ29" t="n">
+        <v>4796</v>
+      </c>
+      <c r="AR29" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AS29" t="inlineStr">
         <is>
           <t>4796</t>
         </is>
@@ -4632,7 +4810,13 @@
       <c r="AP30" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AQ30" t="inlineStr">
+      <c r="AQ30" t="n">
+        <v>3715</v>
+      </c>
+      <c r="AR30" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AS30" t="inlineStr">
         <is>
           <t>3715</t>
         </is>
@@ -4771,7 +4955,13 @@
       <c r="AP31" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AQ31" t="inlineStr">
+      <c r="AQ31" t="n">
+        <v>4372</v>
+      </c>
+      <c r="AR31" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AS31" t="inlineStr">
         <is>
           <t>4372</t>
         </is>
@@ -4910,7 +5100,13 @@
       <c r="AP32" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AQ32" t="inlineStr">
+      <c r="AQ32" t="n">
+        <v>4278</v>
+      </c>
+      <c r="AR32" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AS32" t="inlineStr">
         <is>
           <t>4278</t>
         </is>
@@ -5049,7 +5245,13 @@
       <c r="AP33" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="AQ33" t="inlineStr">
+      <c r="AQ33" t="n">
+        <v>3813</v>
+      </c>
+      <c r="AR33" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AS33" t="inlineStr">
         <is>
           <t>3813</t>
         </is>
@@ -5188,7 +5390,13 @@
       <c r="AP34" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AQ34" t="inlineStr">
+      <c r="AQ34" t="n">
+        <v>3965</v>
+      </c>
+      <c r="AR34" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AS34" t="inlineStr">
         <is>
           <t>3965</t>
         </is>
@@ -5327,7 +5535,13 @@
       <c r="AP35" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AQ35" t="inlineStr">
+      <c r="AQ35" t="n">
+        <v>3943</v>
+      </c>
+      <c r="AR35" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AS35" t="inlineStr">
         <is>
           <t>3943</t>
         </is>
@@ -5466,7 +5680,13 @@
       <c r="AP36" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AQ36" t="inlineStr">
+      <c r="AQ36" t="n">
+        <v>3905</v>
+      </c>
+      <c r="AR36" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AS36" t="inlineStr">
         <is>
           <t>3905</t>
         </is>
@@ -5605,7 +5825,13 @@
       <c r="AP37" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AQ37" t="inlineStr">
+      <c r="AQ37" t="n">
+        <v>3652</v>
+      </c>
+      <c r="AR37" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AS37" t="inlineStr">
         <is>
           <t>3652</t>
         </is>
@@ -5744,7 +5970,13 @@
       <c r="AP38" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AQ38" t="inlineStr">
+      <c r="AQ38" t="n">
+        <v>4042</v>
+      </c>
+      <c r="AR38" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AS38" t="inlineStr">
         <is>
           <t>4042</t>
         </is>
@@ -5883,7 +6115,13 @@
       <c r="AP39" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AQ39" t="inlineStr">
+      <c r="AQ39" t="n">
+        <v>4043</v>
+      </c>
+      <c r="AR39" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AS39" t="inlineStr">
         <is>
           <t>4043</t>
         </is>
@@ -6022,7 +6260,13 @@
       <c r="AP40" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AQ40" t="inlineStr">
+      <c r="AQ40" t="n">
+        <v>4073</v>
+      </c>
+      <c r="AR40" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AS40" t="inlineStr">
         <is>
           <t>4073</t>
         </is>
@@ -6161,7 +6405,13 @@
       <c r="AP41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ41" t="inlineStr">
+      <c r="AQ41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS41" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6300,7 +6550,13 @@
       <c r="AP42" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AQ42" t="inlineStr">
+      <c r="AQ42" t="n">
+        <v>4494</v>
+      </c>
+      <c r="AR42" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AS42" t="inlineStr">
         <is>
           <t>4494</t>
         </is>
@@ -6439,7 +6695,13 @@
       <c r="AP43" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AQ43" t="inlineStr">
+      <c r="AQ43" t="n">
+        <v>4197</v>
+      </c>
+      <c r="AR43" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AS43" t="inlineStr">
         <is>
           <t>4197</t>
         </is>
@@ -6578,7 +6840,13 @@
       <c r="AP44" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AQ44" t="inlineStr">
+      <c r="AQ44" t="n">
+        <v>4233</v>
+      </c>
+      <c r="AR44" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AS44" t="inlineStr">
         <is>
           <t>4233</t>
         </is>
@@ -6717,7 +6985,13 @@
       <c r="AP45" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="AQ45" t="inlineStr">
+      <c r="AQ45" t="n">
+        <v>3740</v>
+      </c>
+      <c r="AR45" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="AS45" t="inlineStr">
         <is>
           <t>3740</t>
         </is>
@@ -6856,7 +7130,13 @@
       <c r="AP46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AQ46" t="inlineStr">
+      <c r="AQ46" t="n">
+        <v>3661</v>
+      </c>
+      <c r="AR46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AS46" t="inlineStr">
         <is>
           <t>3661</t>
         </is>
@@ -6995,7 +7275,13 @@
       <c r="AP47" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AQ47" t="inlineStr">
+      <c r="AQ47" t="n">
+        <v>3712</v>
+      </c>
+      <c r="AR47" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AS47" t="inlineStr">
         <is>
           <t>3712</t>
         </is>
@@ -7134,7 +7420,13 @@
       <c r="AP48" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AQ48" t="inlineStr">
+      <c r="AQ48" t="n">
+        <v>4347</v>
+      </c>
+      <c r="AR48" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AS48" t="inlineStr">
         <is>
           <t>4347</t>
         </is>
@@ -7273,7 +7565,13 @@
       <c r="AP49" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AQ49" t="inlineStr">
+      <c r="AQ49" t="n">
+        <v>3173</v>
+      </c>
+      <c r="AR49" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AS49" t="inlineStr">
         <is>
           <t>3173</t>
         </is>
@@ -7412,7 +7710,13 @@
       <c r="AP50" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AQ50" t="inlineStr">
+      <c r="AQ50" t="n">
+        <v>4272</v>
+      </c>
+      <c r="AR50" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AS50" t="inlineStr">
         <is>
           <t>4272</t>
         </is>
@@ -7551,7 +7855,13 @@
       <c r="AP51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ51" t="inlineStr">
+      <c r="AQ51" t="n">
+        <v>2521</v>
+      </c>
+      <c r="AR51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS51" t="inlineStr">
         <is>
           <t>2521</t>
         </is>
@@ -7690,7 +8000,13 @@
       <c r="AP52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ52" t="inlineStr">
+      <c r="AQ52" t="n">
+        <v>2533</v>
+      </c>
+      <c r="AR52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS52" t="inlineStr">
         <is>
           <t>2533</t>
         </is>
@@ -7829,7 +8145,13 @@
       <c r="AP53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ53" t="inlineStr">
+      <c r="AQ53" t="n">
+        <v>3062</v>
+      </c>
+      <c r="AR53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS53" t="inlineStr">
         <is>
           <t>3062</t>
         </is>
@@ -7968,7 +8290,13 @@
       <c r="AP54" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AQ54" t="inlineStr">
+      <c r="AQ54" t="n">
+        <v>4135</v>
+      </c>
+      <c r="AR54" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AS54" t="inlineStr">
         <is>
           <t>4135</t>
         </is>
@@ -8107,7 +8435,13 @@
       <c r="AP55" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AQ55" t="inlineStr">
+      <c r="AQ55" t="n">
+        <v>3385</v>
+      </c>
+      <c r="AR55" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AS55" t="inlineStr">
         <is>
           <t>3385</t>
         </is>
@@ -8246,7 +8580,13 @@
       <c r="AP56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AQ56" t="inlineStr">
+      <c r="AQ56" t="n">
+        <v>3448</v>
+      </c>
+      <c r="AR56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AS56" t="inlineStr">
         <is>
           <t>3448</t>
         </is>
@@ -8385,7 +8725,13 @@
       <c r="AP57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AQ57" t="inlineStr">
+      <c r="AQ57" t="n">
+        <v>3913</v>
+      </c>
+      <c r="AR57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AS57" t="inlineStr">
         <is>
           <t>3913</t>
         </is>
@@ -8524,7 +8870,13 @@
       <c r="AP58" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AQ58" t="inlineStr">
+      <c r="AQ58" t="n">
+        <v>3452</v>
+      </c>
+      <c r="AR58" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AS58" t="inlineStr">
         <is>
           <t>3452</t>
         </is>
@@ -8586,6 +8938,8 @@
       <c r="AO59" t="inlineStr"/>
       <c r="AP59" s="3" t="inlineStr"/>
       <c r="AQ59" t="inlineStr"/>
+      <c r="AR59" s="3" t="inlineStr"/>
+      <c r="AS59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -8643,6 +8997,8 @@
       <c r="AO60" t="inlineStr"/>
       <c r="AP60" s="3" t="inlineStr"/>
       <c r="AQ60" t="inlineStr"/>
+      <c r="AR60" s="3" t="inlineStr"/>
+      <c r="AS60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -8777,7 +9133,13 @@
       <c r="AP61" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AQ61" t="inlineStr">
+      <c r="AQ61" t="n">
+        <v>3832</v>
+      </c>
+      <c r="AR61" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AS61" t="inlineStr">
         <is>
           <t>3832</t>
         </is>
@@ -8916,7 +9278,13 @@
       <c r="AP62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ62" t="inlineStr">
+      <c r="AQ62" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9055,7 +9423,13 @@
       <c r="AP63" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="AQ63" t="inlineStr">
+      <c r="AQ63" t="n">
+        <v>3934</v>
+      </c>
+      <c r="AR63" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="AS63" t="inlineStr">
         <is>
           <t>3934</t>
         </is>
@@ -9194,7 +9568,13 @@
       <c r="AP64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ64" t="inlineStr">
+      <c r="AQ64" t="n">
+        <v>2499</v>
+      </c>
+      <c r="AR64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS64" t="inlineStr">
         <is>
           <t>2499</t>
         </is>
@@ -9256,6 +9636,8 @@
       <c r="AO65" t="inlineStr"/>
       <c r="AP65" s="3" t="inlineStr"/>
       <c r="AQ65" t="inlineStr"/>
+      <c r="AR65" s="3" t="inlineStr"/>
+      <c r="AS65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -9390,7 +9772,13 @@
       <c r="AP66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ66" t="inlineStr">
+      <c r="AQ66" t="n">
+        <v>2553</v>
+      </c>
+      <c r="AR66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS66" t="inlineStr">
         <is>
           <t>2553</t>
         </is>
@@ -9529,7 +9917,13 @@
       <c r="AP67" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="AQ67" t="inlineStr">
+      <c r="AQ67" t="n">
+        <v>3829</v>
+      </c>
+      <c r="AR67" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AS67" t="inlineStr">
         <is>
           <t>3829</t>
         </is>
@@ -9668,7 +10062,13 @@
       <c r="AP68" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AQ68" t="inlineStr">
+      <c r="AQ68" t="n">
+        <v>3814</v>
+      </c>
+      <c r="AR68" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AS68" t="inlineStr">
         <is>
           <t>3814</t>
         </is>
@@ -9807,7 +10207,13 @@
       <c r="AP69" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AQ69" t="inlineStr">
+      <c r="AQ69" t="n">
+        <v>3484</v>
+      </c>
+      <c r="AR69" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AS69" t="inlineStr">
         <is>
           <t>3484</t>
         </is>
@@ -9946,7 +10352,13 @@
       <c r="AP70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ70" t="inlineStr">
+      <c r="AQ70" t="n">
+        <v>2483</v>
+      </c>
+      <c r="AR70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS70" t="inlineStr">
         <is>
           <t>2483</t>
         </is>
@@ -10085,7 +10497,13 @@
       <c r="AP71" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="AQ71" t="inlineStr">
+      <c r="AQ71" t="n">
+        <v>3581</v>
+      </c>
+      <c r="AR71" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AS71" t="inlineStr">
         <is>
           <t>3581</t>
         </is>
@@ -10224,7 +10642,13 @@
       <c r="AP72" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="AQ72" t="inlineStr">
+      <c r="AQ72" t="n">
+        <v>2986</v>
+      </c>
+      <c r="AR72" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS72" t="inlineStr">
         <is>
           <t>2986</t>
         </is>
@@ -10363,7 +10787,13 @@
       <c r="AP73" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AQ73" t="inlineStr">
+      <c r="AQ73" t="n">
+        <v>3472</v>
+      </c>
+      <c r="AR73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AS73" t="inlineStr">
         <is>
           <t>3472</t>
         </is>
@@ -10502,7 +10932,13 @@
       <c r="AP74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ74" t="inlineStr">
+      <c r="AQ74" t="n">
+        <v>2624</v>
+      </c>
+      <c r="AR74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS74" t="inlineStr">
         <is>
           <t>2624</t>
         </is>
@@ -10641,7 +11077,13 @@
       <c r="AP75" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="AQ75" t="inlineStr">
+      <c r="AQ75" t="n">
+        <v>3321</v>
+      </c>
+      <c r="AR75" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="AS75" t="inlineStr">
         <is>
           <t>3321</t>
         </is>
@@ -10780,7 +11222,13 @@
       <c r="AP76" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AQ76" t="inlineStr">
+      <c r="AQ76" t="n">
+        <v>3951</v>
+      </c>
+      <c r="AR76" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AS76" t="inlineStr">
         <is>
           <t>3951</t>
         </is>
@@ -10919,7 +11367,13 @@
       <c r="AP77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ77" t="inlineStr">
+      <c r="AQ77" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS77" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11058,7 +11512,13 @@
       <c r="AP78" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AQ78" t="inlineStr">
+      <c r="AQ78" t="n">
+        <v>3858</v>
+      </c>
+      <c r="AR78" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AS78" t="inlineStr">
         <is>
           <t>3858</t>
         </is>
@@ -11197,7 +11657,13 @@
       <c r="AP79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ79" t="inlineStr">
+      <c r="AQ79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11336,7 +11802,13 @@
       <c r="AP80" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="AQ80" t="inlineStr">
+      <c r="AQ80" t="n">
+        <v>3702</v>
+      </c>
+      <c r="AR80" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AS80" t="inlineStr">
         <is>
           <t>3702</t>
         </is>
@@ -11475,7 +11947,13 @@
       <c r="AP81" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AQ81" t="inlineStr">
+      <c r="AQ81" t="n">
+        <v>3736</v>
+      </c>
+      <c r="AR81" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AS81" t="inlineStr">
         <is>
           <t>3736</t>
         </is>
@@ -11614,7 +12092,13 @@
       <c r="AP82" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AQ82" t="inlineStr">
+      <c r="AQ82" t="n">
+        <v>3625</v>
+      </c>
+      <c r="AR82" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AS82" t="inlineStr">
         <is>
           <t>3625</t>
         </is>
@@ -11753,7 +12237,13 @@
       <c r="AP83" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AQ83" t="inlineStr">
+      <c r="AQ83" t="n">
+        <v>3460</v>
+      </c>
+      <c r="AR83" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AS83" t="inlineStr">
         <is>
           <t>3460</t>
         </is>
@@ -11875,6 +12365,8 @@
       <c r="AO84" t="inlineStr"/>
       <c r="AP84" s="3" t="inlineStr"/>
       <c r="AQ84" t="inlineStr"/>
+      <c r="AR84" s="3" t="inlineStr"/>
+      <c r="AS84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -12009,7 +12501,13 @@
       <c r="AP85" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AQ85" t="inlineStr">
+      <c r="AQ85" t="n">
+        <v>3278</v>
+      </c>
+      <c r="AR85" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AS85" t="inlineStr">
         <is>
           <t>3278</t>
         </is>
@@ -12148,7 +12646,13 @@
       <c r="AP86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ86" t="inlineStr">
+      <c r="AQ86" t="n">
+        <v>2477</v>
+      </c>
+      <c r="AR86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS86" t="inlineStr">
         <is>
           <t>2477</t>
         </is>
@@ -12287,7 +12791,13 @@
       <c r="AP87" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AQ87" t="inlineStr">
+      <c r="AQ87" t="n">
+        <v>3746</v>
+      </c>
+      <c r="AR87" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AS87" t="inlineStr">
         <is>
           <t>3746</t>
         </is>
@@ -12426,7 +12936,13 @@
       <c r="AP88" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AQ88" t="inlineStr">
+      <c r="AQ88" t="n">
+        <v>2746</v>
+      </c>
+      <c r="AR88" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AS88" t="inlineStr">
         <is>
           <t>2746</t>
         </is>
@@ -12565,7 +13081,13 @@
       <c r="AP89" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AQ89" t="inlineStr">
+      <c r="AQ89" t="n">
+        <v>2895</v>
+      </c>
+      <c r="AR89" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AS89" t="inlineStr">
         <is>
           <t>2895</t>
         </is>
@@ -12704,7 +13226,13 @@
       <c r="AP90" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AQ90" t="inlineStr">
+      <c r="AQ90" t="n">
+        <v>2637</v>
+      </c>
+      <c r="AR90" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AS90" t="inlineStr">
         <is>
           <t>2637</t>
         </is>
@@ -12843,7 +13371,13 @@
       <c r="AP91" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AQ91" t="inlineStr">
+      <c r="AQ91" t="n">
+        <v>2671</v>
+      </c>
+      <c r="AR91" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AS91" t="inlineStr">
         <is>
           <t>2671</t>
         </is>
@@ -12982,7 +13516,13 @@
       <c r="AP92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ92" t="inlineStr">
+      <c r="AQ92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13121,7 +13661,13 @@
       <c r="AP93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ93" t="inlineStr">
+      <c r="AQ93" t="n">
+        <v>2317</v>
+      </c>
+      <c r="AR93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS93" t="inlineStr">
         <is>
           <t>2317</t>
         </is>
@@ -13260,7 +13806,13 @@
       <c r="AP94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ94" t="inlineStr">
+      <c r="AQ94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13399,7 +13951,13 @@
       <c r="AP95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ95" t="inlineStr">
+      <c r="AQ95" t="n">
+        <v>2394</v>
+      </c>
+      <c r="AR95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS95" t="inlineStr">
         <is>
           <t>2394</t>
         </is>
@@ -13538,7 +14096,13 @@
       <c r="AP96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ96" t="inlineStr">
+      <c r="AQ96" t="n">
+        <v>2499</v>
+      </c>
+      <c r="AR96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS96" t="inlineStr">
         <is>
           <t>2499</t>
         </is>
@@ -13677,7 +14241,13 @@
       <c r="AP97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ97" t="inlineStr">
+      <c r="AQ97" t="n">
+        <v>2495</v>
+      </c>
+      <c r="AR97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS97" t="inlineStr">
         <is>
           <t>2495</t>
         </is>
@@ -13816,7 +14386,13 @@
       <c r="AP98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ98" t="inlineStr">
+      <c r="AQ98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13955,7 +14531,13 @@
       <c r="AP99" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="AQ99" t="inlineStr">
+      <c r="AQ99" t="n">
+        <v>3038</v>
+      </c>
+      <c r="AR99" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AS99" t="inlineStr">
         <is>
           <t>3038</t>
         </is>
@@ -14094,7 +14676,13 @@
       <c r="AP100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ100" t="inlineStr">
+      <c r="AQ100" t="n">
+        <v>2432</v>
+      </c>
+      <c r="AR100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS100" t="inlineStr">
         <is>
           <t>2432</t>
         </is>
@@ -14233,7 +14821,13 @@
       <c r="AP101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AQ101" t="inlineStr">
+      <c r="AQ101" t="n">
+        <v>3651</v>
+      </c>
+      <c r="AR101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AS101" t="inlineStr">
         <is>
           <t>3651</t>
         </is>
@@ -14372,7 +14966,13 @@
       <c r="AP102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AQ102" t="inlineStr">
+      <c r="AQ102" t="n">
+        <v>3270</v>
+      </c>
+      <c r="AR102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AS102" t="inlineStr">
         <is>
           <t>3270</t>
         </is>
@@ -14511,7 +15111,13 @@
       <c r="AP103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ103" t="inlineStr">
+      <c r="AQ103" t="n">
+        <v>2450</v>
+      </c>
+      <c r="AR103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS103" t="inlineStr">
         <is>
           <t>2450</t>
         </is>
@@ -14650,7 +15256,13 @@
       <c r="AP104" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AQ104" t="inlineStr">
+      <c r="AQ104" t="n">
+        <v>3695</v>
+      </c>
+      <c r="AR104" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AS104" t="inlineStr">
         <is>
           <t>3695</t>
         </is>
@@ -14789,7 +15401,13 @@
       <c r="AP105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ105" t="inlineStr">
+      <c r="AQ105" t="n">
+        <v>3228</v>
+      </c>
+      <c r="AR105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS105" t="inlineStr">
         <is>
           <t>3228</t>
         </is>
@@ -14928,7 +15546,13 @@
       <c r="AP106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ106" t="inlineStr">
+      <c r="AQ106" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15067,7 +15691,13 @@
       <c r="AP107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ107" t="inlineStr">
+      <c r="AQ107" t="n">
+        <v>2577</v>
+      </c>
+      <c r="AR107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS107" t="inlineStr">
         <is>
           <t>2577</t>
         </is>
@@ -15206,7 +15836,13 @@
       <c r="AP108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ108" t="inlineStr">
+      <c r="AQ108" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15345,7 +15981,13 @@
       <c r="AP109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ109" t="inlineStr">
+      <c r="AQ109" t="n">
+        <v>2940</v>
+      </c>
+      <c r="AR109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS109" t="inlineStr">
         <is>
           <t>2940</t>
         </is>
@@ -15484,7 +16126,13 @@
       <c r="AP110" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AQ110" t="inlineStr">
+      <c r="AQ110" t="n">
+        <v>3181</v>
+      </c>
+      <c r="AR110" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AS110" t="inlineStr">
         <is>
           <t>3181</t>
         </is>
@@ -15623,7 +16271,13 @@
       <c r="AP111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ111" t="inlineStr">
+      <c r="AQ111" t="n">
+        <v>2545</v>
+      </c>
+      <c r="AR111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS111" t="inlineStr">
         <is>
           <t>2545</t>
         </is>
@@ -15762,7 +16416,13 @@
       <c r="AP112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ112" t="inlineStr">
+      <c r="AQ112" t="n">
+        <v>2572</v>
+      </c>
+      <c r="AR112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS112" t="inlineStr">
         <is>
           <t>2572</t>
         </is>
@@ -15901,7 +16561,13 @@
       <c r="AP113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ113" t="inlineStr">
+      <c r="AQ113" t="n">
+        <v>2983</v>
+      </c>
+      <c r="AR113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS113" t="inlineStr">
         <is>
           <t>2983</t>
         </is>
@@ -16040,7 +16706,13 @@
       <c r="AP114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ114" t="inlineStr">
+      <c r="AQ114" t="n">
+        <v>3059</v>
+      </c>
+      <c r="AR114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS114" t="inlineStr">
         <is>
           <t>3059</t>
         </is>
@@ -16179,7 +16851,13 @@
       <c r="AP115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ115" t="inlineStr">
+      <c r="AQ115" t="n">
+        <v>2001</v>
+      </c>
+      <c r="AR115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS115" t="inlineStr">
         <is>
           <t>2001</t>
         </is>
@@ -16318,7 +16996,13 @@
       <c r="AP116" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="AQ116" t="inlineStr">
+      <c r="AQ116" t="n">
+        <v>2834</v>
+      </c>
+      <c r="AR116" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="AS116" t="inlineStr">
         <is>
           <t>2834</t>
         </is>
@@ -16457,7 +17141,13 @@
       <c r="AP117" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AQ117" t="inlineStr">
+      <c r="AQ117" t="n">
+        <v>3099</v>
+      </c>
+      <c r="AR117" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AS117" t="inlineStr">
         <is>
           <t>3099</t>
         </is>
@@ -16596,7 +17286,13 @@
       <c r="AP118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ118" t="inlineStr">
+      <c r="AQ118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16735,7 +17431,13 @@
       <c r="AP119" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="AQ119" t="inlineStr">
+      <c r="AQ119" t="n">
+        <v>3363</v>
+      </c>
+      <c r="AR119" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="AS119" t="inlineStr">
         <is>
           <t>3363</t>
         </is>
@@ -16874,7 +17576,13 @@
       <c r="AP120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ120" t="inlineStr">
+      <c r="AQ120" t="n">
+        <v>2423</v>
+      </c>
+      <c r="AR120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS120" t="inlineStr">
         <is>
           <t>2423</t>
         </is>
@@ -17013,7 +17721,13 @@
       <c r="AP121" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AQ121" t="inlineStr">
+      <c r="AQ121" t="n">
+        <v>2921</v>
+      </c>
+      <c r="AR121" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AS121" t="inlineStr">
         <is>
           <t>2921</t>
         </is>
@@ -17152,7 +17866,13 @@
       <c r="AP122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ122" t="inlineStr">
+      <c r="AQ122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -17291,7 +18011,13 @@
       <c r="AP123" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="AQ123" t="inlineStr">
+      <c r="AQ123" t="n">
+        <v>2822</v>
+      </c>
+      <c r="AR123" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="AS123" t="inlineStr">
         <is>
           <t>2822</t>
         </is>
@@ -17430,7 +18156,13 @@
       <c r="AP124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AQ124" t="inlineStr">
+      <c r="AQ124" t="n">
+        <v>2991</v>
+      </c>
+      <c r="AR124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AS124" t="inlineStr">
         <is>
           <t>2991</t>
         </is>
@@ -17569,7 +18301,13 @@
       <c r="AP125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ125" t="inlineStr">
+      <c r="AQ125" t="n">
+        <v>2633</v>
+      </c>
+      <c r="AR125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS125" t="inlineStr">
         <is>
           <t>2633</t>
         </is>
@@ -17708,7 +18446,13 @@
       <c r="AP126" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AQ126" t="inlineStr">
+      <c r="AQ126" t="n">
+        <v>2923</v>
+      </c>
+      <c r="AR126" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AS126" t="inlineStr">
         <is>
           <t>2923</t>
         </is>
@@ -17847,7 +18591,13 @@
       <c r="AP127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ127" t="inlineStr">
+      <c r="AQ127" t="n">
+        <v>2355</v>
+      </c>
+      <c r="AR127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS127" t="inlineStr">
         <is>
           <t>2355</t>
         </is>
@@ -17986,7 +18736,13 @@
       <c r="AP128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ128" t="inlineStr">
+      <c r="AQ128" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18125,7 +18881,13 @@
       <c r="AP129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ129" t="inlineStr">
+      <c r="AQ129" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18264,7 +19026,13 @@
       <c r="AP130" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AQ130" t="inlineStr">
+      <c r="AQ130" t="n">
+        <v>2706</v>
+      </c>
+      <c r="AR130" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AS130" t="inlineStr">
         <is>
           <t>2706</t>
         </is>
@@ -18403,7 +19171,13 @@
       <c r="AP131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ131" t="inlineStr">
+      <c r="AQ131" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18542,7 +19316,13 @@
       <c r="AP132" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AQ132" t="inlineStr">
+      <c r="AQ132" t="n">
+        <v>2532</v>
+      </c>
+      <c r="AR132" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AS132" t="inlineStr">
         <is>
           <t>2532</t>
         </is>
@@ -18681,7 +19461,13 @@
       <c r="AP133" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AQ133" t="inlineStr">
+      <c r="AQ133" t="n">
+        <v>2578</v>
+      </c>
+      <c r="AR133" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AS133" t="inlineStr">
         <is>
           <t>2578</t>
         </is>
@@ -18767,6 +19553,8 @@
       <c r="AO134" t="inlineStr"/>
       <c r="AP134" s="3" t="inlineStr"/>
       <c r="AQ134" t="inlineStr"/>
+      <c r="AR134" s="3" t="inlineStr"/>
+      <c r="AS134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -18840,6 +19628,8 @@
       <c r="AO135" t="inlineStr"/>
       <c r="AP135" s="3" t="inlineStr"/>
       <c r="AQ135" t="inlineStr"/>
+      <c r="AR135" s="3" t="inlineStr"/>
+      <c r="AS135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -18974,7 +19764,13 @@
       <c r="AP136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ136" t="inlineStr">
+      <c r="AQ136" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS136" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -19113,7 +19909,13 @@
       <c r="AP137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ137" t="inlineStr">
+      <c r="AQ137" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -19191,6 +19993,8 @@
       <c r="AO138" t="inlineStr"/>
       <c r="AP138" s="3" t="inlineStr"/>
       <c r="AQ138" t="inlineStr"/>
+      <c r="AR138" s="3" t="inlineStr"/>
+      <c r="AS138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -19325,7 +20129,13 @@
       <c r="AP139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ139" t="inlineStr">
+      <c r="AQ139" t="n">
+        <v>2043</v>
+      </c>
+      <c r="AR139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS139" t="inlineStr">
         <is>
           <t>2043</t>
         </is>
@@ -19464,7 +20274,13 @@
       <c r="AP140" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AQ140" t="inlineStr">
+      <c r="AQ140" t="n">
+        <v>2676</v>
+      </c>
+      <c r="AR140" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AS140" t="inlineStr">
         <is>
           <t>2676</t>
         </is>
@@ -19542,6 +20358,8 @@
       <c r="AO141" t="inlineStr"/>
       <c r="AP141" s="3" t="inlineStr"/>
       <c r="AQ141" t="inlineStr"/>
+      <c r="AR141" s="3" t="inlineStr"/>
+      <c r="AS141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -19676,7 +20494,13 @@
       <c r="AP142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ142" t="inlineStr">
+      <c r="AQ142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS142" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -19754,6 +20578,8 @@
       <c r="AO143" t="inlineStr"/>
       <c r="AP143" s="3" t="inlineStr"/>
       <c r="AQ143" t="inlineStr"/>
+      <c r="AR143" s="3" t="inlineStr"/>
+      <c r="AS143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -19827,6 +20653,8 @@
       <c r="AO144" t="inlineStr"/>
       <c r="AP144" s="3" t="inlineStr"/>
       <c r="AQ144" t="inlineStr"/>
+      <c r="AR144" s="3" t="inlineStr"/>
+      <c r="AS144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -19900,6 +20728,8 @@
       <c r="AO145" t="inlineStr"/>
       <c r="AP145" s="3" t="inlineStr"/>
       <c r="AQ145" t="inlineStr"/>
+      <c r="AR145" s="3" t="inlineStr"/>
+      <c r="AS145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -19973,6 +20803,8 @@
       <c r="AO146" t="inlineStr"/>
       <c r="AP146" s="3" t="inlineStr"/>
       <c r="AQ146" t="inlineStr"/>
+      <c r="AR146" s="3" t="inlineStr"/>
+      <c r="AS146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -20046,6 +20878,8 @@
       <c r="AO147" t="inlineStr"/>
       <c r="AP147" s="3" t="inlineStr"/>
       <c r="AQ147" t="inlineStr"/>
+      <c r="AR147" s="3" t="inlineStr"/>
+      <c r="AS147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -20180,7 +21014,13 @@
       <c r="AP148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ148" t="inlineStr">
+      <c r="AQ148" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -20319,7 +21159,13 @@
       <c r="AP149" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="AQ149" t="inlineStr">
+      <c r="AQ149" t="n">
+        <v>3324</v>
+      </c>
+      <c r="AR149" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="AS149" t="inlineStr">
         <is>
           <t>3324</t>
         </is>
@@ -20458,7 +21304,13 @@
       <c r="AP150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ150" t="inlineStr">
+      <c r="AQ150" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -20597,7 +21449,13 @@
       <c r="AP151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ151" t="inlineStr">
+      <c r="AQ151" t="n">
+        <v>2552</v>
+      </c>
+      <c r="AR151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS151" t="inlineStr">
         <is>
           <t>2552</t>
         </is>
@@ -20736,7 +21594,13 @@
       <c r="AP152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ152" t="inlineStr">
+      <c r="AQ152" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -20875,7 +21739,13 @@
       <c r="AP153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ153" t="inlineStr">
+      <c r="AQ153" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -21014,7 +21884,13 @@
       <c r="AP154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ154" t="inlineStr">
+      <c r="AQ154" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -21153,7 +22029,13 @@
       <c r="AP155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ155" t="inlineStr">
+      <c r="AQ155" t="n">
+        <v>2586</v>
+      </c>
+      <c r="AR155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS155" t="inlineStr">
         <is>
           <t>2586</t>
         </is>
@@ -21286,7 +22168,13 @@
       <c r="AP156" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AQ156" t="inlineStr">
+      <c r="AQ156" t="n">
+        <v>3118</v>
+      </c>
+      <c r="AR156" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AS156" t="inlineStr">
         <is>
           <t>3118</t>
         </is>
@@ -21358,6 +22246,8 @@
       <c r="AO157" t="inlineStr"/>
       <c r="AP157" s="3" t="inlineStr"/>
       <c r="AQ157" t="inlineStr"/>
+      <c r="AR157" s="3" t="inlineStr"/>
+      <c r="AS157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -21486,7 +22376,13 @@
       <c r="AP158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ158" t="inlineStr">
+      <c r="AQ158" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -21619,7 +22515,13 @@
       <c r="AP159" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AQ159" t="inlineStr">
+      <c r="AQ159" t="n">
+        <v>2816</v>
+      </c>
+      <c r="AR159" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AS159" t="inlineStr">
         <is>
           <t>2816</t>
         </is>
@@ -21691,6 +22593,8 @@
       <c r="AO160" t="inlineStr"/>
       <c r="AP160" s="3" t="inlineStr"/>
       <c r="AQ160" t="inlineStr"/>
+      <c r="AR160" s="3" t="inlineStr"/>
+      <c r="AS160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -21807,7 +22711,13 @@
       <c r="AP161" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AQ161" t="inlineStr">
+      <c r="AQ161" t="n">
+        <v>2925</v>
+      </c>
+      <c r="AR161" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AS161" t="inlineStr">
         <is>
           <t>2925</t>
         </is>
@@ -21928,7 +22838,13 @@
       <c r="AP162" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="AQ162" t="inlineStr">
+      <c r="AQ162" t="n">
+        <v>2579</v>
+      </c>
+      <c r="AR162" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS162" t="inlineStr">
         <is>
           <t>2579</t>
         </is>
@@ -22045,7 +22961,13 @@
       <c r="AP163" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AQ163" t="inlineStr">
+      <c r="AQ163" t="n">
+        <v>2988</v>
+      </c>
+      <c r="AR163" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AS163" t="inlineStr">
         <is>
           <t>2988</t>
         </is>
@@ -22146,7 +23068,13 @@
       <c r="AP164" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="AQ164" t="inlineStr">
+      <c r="AQ164" t="n">
+        <v>2935</v>
+      </c>
+      <c r="AR164" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AS164" t="inlineStr">
         <is>
           <t>2935</t>
         </is>
@@ -22251,7 +23179,13 @@
       <c r="AP165" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AQ165" t="inlineStr">
+      <c r="AQ165" t="n">
+        <v>2647</v>
+      </c>
+      <c r="AR165" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AS165" t="inlineStr">
         <is>
           <t>2647</t>
         </is>
@@ -22348,7 +23282,13 @@
       <c r="AP166" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ166" t="inlineStr">
+      <c r="AQ166" t="n">
+        <v>2791</v>
+      </c>
+      <c r="AR166" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS166" t="inlineStr">
         <is>
           <t>2791</t>
         </is>
@@ -22433,7 +23373,13 @@
       <c r="AP167" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ167" t="inlineStr">
+      <c r="AQ167" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR167" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS167" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -22514,7 +23460,13 @@
       <c r="AP168" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ168" t="inlineStr">
+      <c r="AQ168" t="n">
+        <v>1536</v>
+      </c>
+      <c r="AR168" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS168" t="inlineStr">
         <is>
           <t>1536</t>
         </is>
@@ -22578,6 +23530,8 @@
       <c r="AO169" t="inlineStr"/>
       <c r="AP169" s="3" t="inlineStr"/>
       <c r="AQ169" t="inlineStr"/>
+      <c r="AR169" s="3" t="inlineStr"/>
+      <c r="AS169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="n">
@@ -22650,7 +23604,13 @@
       <c r="AP170" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ170" t="inlineStr">
+      <c r="AQ170" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR170" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS170" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -22715,7 +23675,13 @@
       <c r="AP171" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="AQ171" t="inlineStr">
+      <c r="AQ171" t="n">
+        <v>1647</v>
+      </c>
+      <c r="AR171" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="AS171" t="inlineStr">
         <is>
           <t>1647</t>
         </is>
@@ -22780,7 +23746,13 @@
       <c r="AP172" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ172" t="inlineStr">
+      <c r="AQ172" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR172" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS172" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -22845,7 +23817,13 @@
       <c r="AP173" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="AQ173" t="inlineStr">
+      <c r="AQ173" t="n">
+        <v>1640</v>
+      </c>
+      <c r="AR173" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AS173" t="inlineStr">
         <is>
           <t>1640</t>
         </is>

</xml_diff>

<commit_message>
Code updated 23-03-04 16:00:49
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -758,7 +758,7 @@
       </c>
       <c r="AS2" t="inlineStr">
         <is>
-          <t>2575</t>
+          <t>2602</t>
         </is>
       </c>
     </row>
@@ -898,12 +898,12 @@
       <c r="AQ3" t="n">
         <v>4096</v>
       </c>
-      <c r="AR3" s="4" t="n">
-        <v>15</v>
+      <c r="AR3" s="3" t="n">
+        <v>20</v>
       </c>
       <c r="AS3" t="inlineStr">
         <is>
-          <t>4096</t>
+          <t>4489</t>
         </is>
       </c>
     </row>
@@ -1043,12 +1043,12 @@
       <c r="AQ4" t="n">
         <v>4263</v>
       </c>
-      <c r="AR4" s="3" t="n">
-        <v>30</v>
+      <c r="AR4" s="5" t="n">
+        <v>35</v>
       </c>
       <c r="AS4" t="inlineStr">
         <is>
-          <t>4263</t>
+          <t>4641</t>
         </is>
       </c>
     </row>
@@ -1193,7 +1193,7 @@
       </c>
       <c r="AS5" t="inlineStr">
         <is>
-          <t>4040</t>
+          <t>4353</t>
         </is>
       </c>
     </row>
@@ -1338,7 +1338,7 @@
       </c>
       <c r="AS6" t="inlineStr">
         <is>
-          <t>4035</t>
+          <t>4400</t>
         </is>
       </c>
     </row>
@@ -1483,7 +1483,7 @@
       </c>
       <c r="AS7" t="inlineStr">
         <is>
-          <t>4409</t>
+          <t>4689</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="AS8" t="inlineStr">
         <is>
-          <t>3838</t>
+          <t>4128</t>
         </is>
       </c>
     </row>
@@ -1769,11 +1769,11 @@
         <v>3865</v>
       </c>
       <c r="AR9" s="5" t="n">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="AS9" t="inlineStr">
         <is>
-          <t>3865</t>
+          <t>4260</t>
         </is>
       </c>
     </row>
@@ -1918,7 +1918,7 @@
       </c>
       <c r="AS10" t="inlineStr">
         <is>
-          <t>3976</t>
+          <t>4278</t>
         </is>
       </c>
     </row>
@@ -2063,7 +2063,7 @@
       </c>
       <c r="AS11" t="inlineStr">
         <is>
-          <t>3727</t>
+          <t>3865</t>
         </is>
       </c>
     </row>
@@ -2353,7 +2353,7 @@
       </c>
       <c r="AS13" t="inlineStr">
         <is>
-          <t>4544</t>
+          <t>4881</t>
         </is>
       </c>
     </row>
@@ -2498,7 +2498,7 @@
       </c>
       <c r="AS14" t="inlineStr">
         <is>
-          <t>4033</t>
+          <t>4304</t>
         </is>
       </c>
     </row>
@@ -2784,11 +2784,11 @@
         <v>4209</v>
       </c>
       <c r="AR16" s="3" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AS16" t="inlineStr">
         <is>
-          <t>4209</t>
+          <t>4415</t>
         </is>
       </c>
     </row>
@@ -2928,12 +2928,12 @@
       <c r="AQ17" t="n">
         <v>3587</v>
       </c>
-      <c r="AR17" s="3" t="n">
-        <v>30</v>
+      <c r="AR17" s="5" t="n">
+        <v>33</v>
       </c>
       <c r="AS17" t="inlineStr">
         <is>
-          <t>3587</t>
+          <t>3788</t>
         </is>
       </c>
     </row>
@@ -3074,11 +3074,11 @@
         <v>3552</v>
       </c>
       <c r="AR18" s="3" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="AS18" t="inlineStr">
         <is>
-          <t>3552</t>
+          <t>3801</t>
         </is>
       </c>
     </row>
@@ -3218,12 +3218,12 @@
       <c r="AQ19" t="n">
         <v>4144</v>
       </c>
-      <c r="AR19" s="3" t="n">
-        <v>30</v>
+      <c r="AR19" s="5" t="n">
+        <v>31</v>
       </c>
       <c r="AS19" t="inlineStr">
         <is>
-          <t>4144</t>
+          <t>4425</t>
         </is>
       </c>
     </row>
@@ -3364,11 +3364,11 @@
         <v>4681</v>
       </c>
       <c r="AR20" s="5" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AS20" t="inlineStr">
         <is>
-          <t>4681</t>
+          <t>4916</t>
         </is>
       </c>
     </row>
@@ -3513,7 +3513,7 @@
       </c>
       <c r="AS21" t="inlineStr">
         <is>
-          <t>3092</t>
+          <t>3108</t>
         </is>
       </c>
     </row>
@@ -3658,7 +3658,7 @@
       </c>
       <c r="AS22" t="inlineStr">
         <is>
-          <t>3976</t>
+          <t>4298</t>
         </is>
       </c>
     </row>
@@ -3948,7 +3948,7 @@
       </c>
       <c r="AS24" t="inlineStr">
         <is>
-          <t>4131</t>
+          <t>4362</t>
         </is>
       </c>
     </row>
@@ -4234,11 +4234,11 @@
         <v>4186</v>
       </c>
       <c r="AR26" s="5" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AS26" t="inlineStr">
         <is>
-          <t>4186</t>
+          <t>4488</t>
         </is>
       </c>
     </row>
@@ -4379,11 +4379,11 @@
         <v>3908</v>
       </c>
       <c r="AR27" s="3" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AS27" t="inlineStr">
         <is>
-          <t>3908</t>
+          <t>4307</t>
         </is>
       </c>
     </row>
@@ -4406,7 +4406,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F28" s="3" t="n">
@@ -4528,7 +4528,7 @@
       </c>
       <c r="AS28" t="inlineStr">
         <is>
-          <t>3427</t>
+          <t>3603</t>
         </is>
       </c>
     </row>
@@ -4669,11 +4669,11 @@
         <v>4796</v>
       </c>
       <c r="AR29" s="5" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="AS29" t="inlineStr">
         <is>
-          <t>4796</t>
+          <t>5051</t>
         </is>
       </c>
     </row>
@@ -4818,7 +4818,7 @@
       </c>
       <c r="AS30" t="inlineStr">
         <is>
-          <t>3715</t>
+          <t>3822</t>
         </is>
       </c>
     </row>
@@ -4959,11 +4959,11 @@
         <v>4372</v>
       </c>
       <c r="AR31" s="5" t="n">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AS31" t="inlineStr">
         <is>
-          <t>4372</t>
+          <t>4784</t>
         </is>
       </c>
     </row>
@@ -5104,11 +5104,11 @@
         <v>4278</v>
       </c>
       <c r="AR32" s="5" t="n">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="AS32" t="inlineStr">
         <is>
-          <t>4278</t>
+          <t>4654</t>
         </is>
       </c>
     </row>
@@ -5248,12 +5248,12 @@
       <c r="AQ33" t="n">
         <v>3813</v>
       </c>
-      <c r="AR33" s="3" t="n">
-        <v>22</v>
+      <c r="AR33" s="4" t="n">
+        <v>14</v>
       </c>
       <c r="AS33" t="inlineStr">
         <is>
-          <t>3813</t>
+          <t>3971</t>
         </is>
       </c>
     </row>
@@ -5398,7 +5398,7 @@
       </c>
       <c r="AS34" t="inlineStr">
         <is>
-          <t>3965</t>
+          <t>4247</t>
         </is>
       </c>
     </row>
@@ -5539,11 +5539,11 @@
         <v>3943</v>
       </c>
       <c r="AR35" s="5" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AS35" t="inlineStr">
         <is>
-          <t>3943</t>
+          <t>4128</t>
         </is>
       </c>
     </row>
@@ -5688,7 +5688,7 @@
       </c>
       <c r="AS36" t="inlineStr">
         <is>
-          <t>3905</t>
+          <t>4200</t>
         </is>
       </c>
     </row>
@@ -5829,11 +5829,11 @@
         <v>3652</v>
       </c>
       <c r="AR37" s="5" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="AS37" t="inlineStr">
         <is>
-          <t>3652</t>
+          <t>3732</t>
         </is>
       </c>
     </row>
@@ -5978,7 +5978,7 @@
       </c>
       <c r="AS38" t="inlineStr">
         <is>
-          <t>4042</t>
+          <t>4243</t>
         </is>
       </c>
     </row>
@@ -6123,7 +6123,7 @@
       </c>
       <c r="AS39" t="inlineStr">
         <is>
-          <t>4043</t>
+          <t>4277</t>
         </is>
       </c>
     </row>
@@ -6268,7 +6268,7 @@
       </c>
       <c r="AS40" t="inlineStr">
         <is>
-          <t>4073</t>
+          <t>4335</t>
         </is>
       </c>
     </row>
@@ -6558,7 +6558,7 @@
       </c>
       <c r="AS42" t="inlineStr">
         <is>
-          <t>4494</t>
+          <t>4725</t>
         </is>
       </c>
     </row>
@@ -6703,7 +6703,7 @@
       </c>
       <c r="AS43" t="inlineStr">
         <is>
-          <t>4197</t>
+          <t>4508</t>
         </is>
       </c>
     </row>
@@ -6848,7 +6848,7 @@
       </c>
       <c r="AS44" t="inlineStr">
         <is>
-          <t>4233</t>
+          <t>4239</t>
         </is>
       </c>
     </row>
@@ -6989,11 +6989,11 @@
         <v>3740</v>
       </c>
       <c r="AR45" s="3" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AS45" t="inlineStr">
         <is>
-          <t>3740</t>
+          <t>3998</t>
         </is>
       </c>
     </row>
@@ -7138,7 +7138,7 @@
       </c>
       <c r="AS46" t="inlineStr">
         <is>
-          <t>3661</t>
+          <t>3875</t>
         </is>
       </c>
     </row>
@@ -7283,7 +7283,7 @@
       </c>
       <c r="AS47" t="inlineStr">
         <is>
-          <t>3712</t>
+          <t>3918</t>
         </is>
       </c>
     </row>
@@ -7424,11 +7424,11 @@
         <v>4347</v>
       </c>
       <c r="AR48" s="5" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="AS48" t="inlineStr">
         <is>
-          <t>4347</t>
+          <t>4573</t>
         </is>
       </c>
     </row>
@@ -7573,7 +7573,7 @@
       </c>
       <c r="AS49" t="inlineStr">
         <is>
-          <t>3173</t>
+          <t>3273</t>
         </is>
       </c>
     </row>
@@ -7718,7 +7718,7 @@
       </c>
       <c r="AS50" t="inlineStr">
         <is>
-          <t>4272</t>
+          <t>4617</t>
         </is>
       </c>
     </row>
@@ -7863,7 +7863,7 @@
       </c>
       <c r="AS51" t="inlineStr">
         <is>
-          <t>2521</t>
+          <t>2548</t>
         </is>
       </c>
     </row>
@@ -8008,7 +8008,7 @@
       </c>
       <c r="AS52" t="inlineStr">
         <is>
-          <t>2533</t>
+          <t>2552</t>
         </is>
       </c>
     </row>
@@ -8293,12 +8293,12 @@
       <c r="AQ54" t="n">
         <v>4135</v>
       </c>
-      <c r="AR54" s="3" t="n">
-        <v>30</v>
+      <c r="AR54" s="5" t="n">
+        <v>34</v>
       </c>
       <c r="AS54" t="inlineStr">
         <is>
-          <t>4135</t>
+          <t>4488</t>
         </is>
       </c>
     </row>
@@ -8443,7 +8443,7 @@
       </c>
       <c r="AS55" t="inlineStr">
         <is>
-          <t>3385</t>
+          <t>3576</t>
         </is>
       </c>
     </row>
@@ -8588,7 +8588,7 @@
       </c>
       <c r="AS56" t="inlineStr">
         <is>
-          <t>3448</t>
+          <t>3625</t>
         </is>
       </c>
     </row>
@@ -8733,7 +8733,7 @@
       </c>
       <c r="AS57" t="inlineStr">
         <is>
-          <t>3913</t>
+          <t>4166</t>
         </is>
       </c>
     </row>
@@ -8878,7 +8878,7 @@
       </c>
       <c r="AS58" t="inlineStr">
         <is>
-          <t>3452</t>
+          <t>3689</t>
         </is>
       </c>
     </row>
@@ -9141,7 +9141,7 @@
       </c>
       <c r="AS61" t="inlineStr">
         <is>
-          <t>3832</t>
+          <t>4072</t>
         </is>
       </c>
     </row>
@@ -9427,11 +9427,11 @@
         <v>3934</v>
       </c>
       <c r="AR63" s="3" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AS63" t="inlineStr">
         <is>
-          <t>3934</t>
+          <t>4153</t>
         </is>
       </c>
     </row>
@@ -9571,12 +9571,12 @@
       <c r="AQ64" t="n">
         <v>2499</v>
       </c>
-      <c r="AR64" s="2" t="n">
-        <v>0</v>
+      <c r="AR64" s="4" t="n">
+        <v>7</v>
       </c>
       <c r="AS64" t="inlineStr">
         <is>
-          <t>2499</t>
+          <t>2669</t>
         </is>
       </c>
     </row>
@@ -9775,12 +9775,12 @@
       <c r="AQ66" t="n">
         <v>2553</v>
       </c>
-      <c r="AR66" s="2" t="n">
-        <v>0</v>
+      <c r="AR66" s="4" t="n">
+        <v>6</v>
       </c>
       <c r="AS66" t="inlineStr">
         <is>
-          <t>2553</t>
+          <t>2580</t>
         </is>
       </c>
     </row>
@@ -9921,11 +9921,11 @@
         <v>3829</v>
       </c>
       <c r="AR67" s="3" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AS67" t="inlineStr">
         <is>
-          <t>3829</t>
+          <t>4027</t>
         </is>
       </c>
     </row>
@@ -10070,7 +10070,7 @@
       </c>
       <c r="AS68" t="inlineStr">
         <is>
-          <t>3814</t>
+          <t>3990</t>
         </is>
       </c>
     </row>
@@ -10215,7 +10215,7 @@
       </c>
       <c r="AS69" t="inlineStr">
         <is>
-          <t>3484</t>
+          <t>3645</t>
         </is>
       </c>
     </row>
@@ -10355,12 +10355,12 @@
       <c r="AQ70" t="n">
         <v>2483</v>
       </c>
-      <c r="AR70" s="2" t="n">
-        <v>0</v>
+      <c r="AR70" s="4" t="n">
+        <v>1</v>
       </c>
       <c r="AS70" t="inlineStr">
         <is>
-          <t>2483</t>
+          <t>2512</t>
         </is>
       </c>
     </row>
@@ -10500,12 +10500,12 @@
       <c r="AQ71" t="n">
         <v>3581</v>
       </c>
-      <c r="AR71" s="4" t="n">
-        <v>8</v>
+      <c r="AR71" s="3" t="n">
+        <v>23</v>
       </c>
       <c r="AS71" t="inlineStr">
         <is>
-          <t>3581</t>
+          <t>3781</t>
         </is>
       </c>
     </row>
@@ -10646,11 +10646,11 @@
         <v>2986</v>
       </c>
       <c r="AR72" s="4" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="AS72" t="inlineStr">
         <is>
-          <t>2986</t>
+          <t>3159</t>
         </is>
       </c>
     </row>
@@ -10795,7 +10795,7 @@
       </c>
       <c r="AS73" t="inlineStr">
         <is>
-          <t>3472</t>
+          <t>3655</t>
         </is>
       </c>
     </row>
@@ -10940,7 +10940,7 @@
       </c>
       <c r="AS74" t="inlineStr">
         <is>
-          <t>2624</t>
+          <t>2705</t>
         </is>
       </c>
     </row>
@@ -11081,11 +11081,11 @@
         <v>3321</v>
       </c>
       <c r="AR75" s="3" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="AS75" t="inlineStr">
         <is>
-          <t>3321</t>
+          <t>3493</t>
         </is>
       </c>
     </row>
@@ -11230,7 +11230,7 @@
       </c>
       <c r="AS76" t="inlineStr">
         <is>
-          <t>3951</t>
+          <t>4191</t>
         </is>
       </c>
     </row>
@@ -11520,7 +11520,7 @@
       </c>
       <c r="AS78" t="inlineStr">
         <is>
-          <t>3858</t>
+          <t>4090</t>
         </is>
       </c>
     </row>
@@ -11806,11 +11806,11 @@
         <v>3702</v>
       </c>
       <c r="AR80" s="3" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AS80" t="inlineStr">
         <is>
-          <t>3702</t>
+          <t>3893</t>
         </is>
       </c>
     </row>
@@ -11951,11 +11951,11 @@
         <v>3736</v>
       </c>
       <c r="AR81" s="5" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="AS81" t="inlineStr">
         <is>
-          <t>3736</t>
+          <t>4088</t>
         </is>
       </c>
     </row>
@@ -12100,7 +12100,7 @@
       </c>
       <c r="AS82" t="inlineStr">
         <is>
-          <t>3625</t>
+          <t>3871</t>
         </is>
       </c>
     </row>
@@ -12245,7 +12245,7 @@
       </c>
       <c r="AS83" t="inlineStr">
         <is>
-          <t>3460</t>
+          <t>3637</t>
         </is>
       </c>
     </row>
@@ -12509,7 +12509,7 @@
       </c>
       <c r="AS85" t="inlineStr">
         <is>
-          <t>3278</t>
+          <t>3371</t>
         </is>
       </c>
     </row>
@@ -12654,7 +12654,7 @@
       </c>
       <c r="AS86" t="inlineStr">
         <is>
-          <t>2477</t>
+          <t>2560</t>
         </is>
       </c>
     </row>
@@ -12799,7 +12799,7 @@
       </c>
       <c r="AS87" t="inlineStr">
         <is>
-          <t>3746</t>
+          <t>3823</t>
         </is>
       </c>
     </row>
@@ -12939,12 +12939,12 @@
       <c r="AQ88" t="n">
         <v>2746</v>
       </c>
-      <c r="AR88" s="3" t="n">
-        <v>20</v>
+      <c r="AR88" s="4" t="n">
+        <v>10</v>
       </c>
       <c r="AS88" t="inlineStr">
         <is>
-          <t>2746</t>
+          <t>2617</t>
         </is>
       </c>
     </row>
@@ -13089,7 +13089,7 @@
       </c>
       <c r="AS89" t="inlineStr">
         <is>
-          <t>2895</t>
+          <t>2963</t>
         </is>
       </c>
     </row>
@@ -13229,12 +13229,12 @@
       <c r="AQ90" t="n">
         <v>2637</v>
       </c>
-      <c r="AR90" s="3" t="n">
-        <v>20</v>
+      <c r="AR90" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AS90" t="inlineStr">
         <is>
-          <t>2637</t>
+          <t>2602</t>
         </is>
       </c>
     </row>
@@ -13379,7 +13379,7 @@
       </c>
       <c r="AS91" t="inlineStr">
         <is>
-          <t>2671</t>
+          <t>2732</t>
         </is>
       </c>
     </row>
@@ -13669,7 +13669,7 @@
       </c>
       <c r="AS93" t="inlineStr">
         <is>
-          <t>2317</t>
+          <t>2295</t>
         </is>
       </c>
     </row>
@@ -13954,12 +13954,12 @@
       <c r="AQ95" t="n">
         <v>2394</v>
       </c>
-      <c r="AR95" s="2" t="n">
-        <v>0</v>
+      <c r="AR95" s="4" t="n">
+        <v>3</v>
       </c>
       <c r="AS95" t="inlineStr">
         <is>
-          <t>2394</t>
+          <t>2422</t>
         </is>
       </c>
     </row>
@@ -14244,12 +14244,12 @@
       <c r="AQ97" t="n">
         <v>2495</v>
       </c>
-      <c r="AR97" s="2" t="n">
-        <v>0</v>
+      <c r="AR97" s="3" t="n">
+        <v>20</v>
       </c>
       <c r="AS97" t="inlineStr">
         <is>
-          <t>2495</t>
+          <t>2809</t>
         </is>
       </c>
     </row>
@@ -14535,11 +14535,11 @@
         <v>3038</v>
       </c>
       <c r="AR99" s="4" t="n">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="AS99" t="inlineStr">
         <is>
-          <t>3038</t>
+          <t>3214</t>
         </is>
       </c>
     </row>
@@ -14684,7 +14684,7 @@
       </c>
       <c r="AS100" t="inlineStr">
         <is>
-          <t>2432</t>
+          <t>2416</t>
         </is>
       </c>
     </row>
@@ -14829,7 +14829,7 @@
       </c>
       <c r="AS101" t="inlineStr">
         <is>
-          <t>3651</t>
+          <t>3793</t>
         </is>
       </c>
     </row>
@@ -14974,7 +14974,7 @@
       </c>
       <c r="AS102" t="inlineStr">
         <is>
-          <t>3270</t>
+          <t>3405</t>
         </is>
       </c>
     </row>
@@ -15114,12 +15114,12 @@
       <c r="AQ103" t="n">
         <v>2450</v>
       </c>
-      <c r="AR103" s="2" t="n">
-        <v>0</v>
+      <c r="AR103" s="3" t="n">
+        <v>20</v>
       </c>
       <c r="AS103" t="inlineStr">
         <is>
-          <t>2450</t>
+          <t>2787</t>
         </is>
       </c>
     </row>
@@ -15259,12 +15259,12 @@
       <c r="AQ104" t="n">
         <v>3695</v>
       </c>
-      <c r="AR104" s="3" t="n">
-        <v>30</v>
+      <c r="AR104" s="5" t="n">
+        <v>31</v>
       </c>
       <c r="AS104" t="inlineStr">
         <is>
-          <t>3695</t>
+          <t>3864</t>
         </is>
       </c>
     </row>
@@ -15404,12 +15404,12 @@
       <c r="AQ105" t="n">
         <v>3228</v>
       </c>
-      <c r="AR105" s="2" t="n">
-        <v>0</v>
+      <c r="AR105" s="4" t="n">
+        <v>17</v>
       </c>
       <c r="AS105" t="inlineStr">
         <is>
-          <t>3228</t>
+          <t>3495</t>
         </is>
       </c>
     </row>
@@ -15699,7 +15699,7 @@
       </c>
       <c r="AS107" t="inlineStr">
         <is>
-          <t>2577</t>
+          <t>2557</t>
         </is>
       </c>
     </row>
@@ -15984,12 +15984,12 @@
       <c r="AQ109" t="n">
         <v>2940</v>
       </c>
-      <c r="AR109" s="2" t="n">
-        <v>0</v>
+      <c r="AR109" s="4" t="n">
+        <v>18</v>
       </c>
       <c r="AS109" t="inlineStr">
         <is>
-          <t>2940</t>
+          <t>3321</t>
         </is>
       </c>
     </row>
@@ -16134,7 +16134,7 @@
       </c>
       <c r="AS110" t="inlineStr">
         <is>
-          <t>3181</t>
+          <t>3265</t>
         </is>
       </c>
     </row>
@@ -16277,10 +16277,8 @@
       <c r="AR111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS111" t="inlineStr">
-        <is>
-          <t>2545</t>
-        </is>
+      <c r="AS111" t="n">
+        <v>2545</v>
       </c>
     </row>
     <row r="112">
@@ -16424,7 +16422,7 @@
       </c>
       <c r="AS112" t="inlineStr">
         <is>
-          <t>2572</t>
+          <t>2563</t>
         </is>
       </c>
     </row>
@@ -16569,7 +16567,7 @@
       </c>
       <c r="AS113" t="inlineStr">
         <is>
-          <t>2983</t>
+          <t>3093</t>
         </is>
       </c>
     </row>
@@ -16714,7 +16712,7 @@
       </c>
       <c r="AS114" t="inlineStr">
         <is>
-          <t>3059</t>
+          <t>3155</t>
         </is>
       </c>
     </row>
@@ -16859,7 +16857,7 @@
       </c>
       <c r="AS115" t="inlineStr">
         <is>
-          <t>2001</t>
+          <t>2020</t>
         </is>
       </c>
     </row>
@@ -17000,11 +16998,11 @@
         <v>2834</v>
       </c>
       <c r="AR116" s="4" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AS116" t="inlineStr">
         <is>
-          <t>2834</t>
+          <t>2917</t>
         </is>
       </c>
     </row>
@@ -17149,7 +17147,7 @@
       </c>
       <c r="AS117" t="inlineStr">
         <is>
-          <t>3099</t>
+          <t>3259</t>
         </is>
       </c>
     </row>
@@ -17434,12 +17432,12 @@
       <c r="AQ119" t="n">
         <v>3363</v>
       </c>
-      <c r="AR119" s="5" t="n">
-        <v>36</v>
+      <c r="AR119" s="4" t="n">
+        <v>16</v>
       </c>
       <c r="AS119" t="inlineStr">
         <is>
-          <t>3363</t>
+          <t>3483</t>
         </is>
       </c>
     </row>
@@ -17579,12 +17577,12 @@
       <c r="AQ120" t="n">
         <v>2423</v>
       </c>
-      <c r="AR120" s="2" t="n">
-        <v>0</v>
+      <c r="AR120" s="4" t="n">
+        <v>5</v>
       </c>
       <c r="AS120" t="inlineStr">
         <is>
-          <t>2423</t>
+          <t>2481</t>
         </is>
       </c>
     </row>
@@ -17724,12 +17722,12 @@
       <c r="AQ121" t="n">
         <v>2921</v>
       </c>
-      <c r="AR121" s="4" t="n">
-        <v>5</v>
+      <c r="AR121" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AS121" t="inlineStr">
         <is>
-          <t>2921</t>
+          <t>2947</t>
         </is>
       </c>
     </row>
@@ -18015,11 +18013,11 @@
         <v>2822</v>
       </c>
       <c r="AR123" s="4" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AS123" t="inlineStr">
         <is>
-          <t>2822</t>
+          <t>2845</t>
         </is>
       </c>
     </row>
@@ -18164,7 +18162,7 @@
       </c>
       <c r="AS124" t="inlineStr">
         <is>
-          <t>2991</t>
+          <t>2995</t>
         </is>
       </c>
     </row>
@@ -18304,12 +18302,12 @@
       <c r="AQ125" t="n">
         <v>2633</v>
       </c>
-      <c r="AR125" s="2" t="n">
-        <v>0</v>
+      <c r="AR125" s="3" t="n">
+        <v>20</v>
       </c>
       <c r="AS125" t="inlineStr">
         <is>
-          <t>2633</t>
+          <t>2904</t>
         </is>
       </c>
     </row>
@@ -18450,11 +18448,11 @@
         <v>2923</v>
       </c>
       <c r="AR126" s="3" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="AS126" t="inlineStr">
         <is>
-          <t>2923</t>
+          <t>3048</t>
         </is>
       </c>
     </row>
@@ -18599,7 +18597,7 @@
       </c>
       <c r="AS127" t="inlineStr">
         <is>
-          <t>2355</t>
+          <t>2339</t>
         </is>
       </c>
     </row>
@@ -19034,7 +19032,7 @@
       </c>
       <c r="AS130" t="inlineStr">
         <is>
-          <t>2706</t>
+          <t>2789</t>
         </is>
       </c>
     </row>
@@ -19324,7 +19322,7 @@
       </c>
       <c r="AS132" t="inlineStr">
         <is>
-          <t>2532</t>
+          <t>2528</t>
         </is>
       </c>
     </row>
@@ -19464,12 +19462,12 @@
       <c r="AQ133" t="n">
         <v>2578</v>
       </c>
-      <c r="AR133" s="4" t="n">
-        <v>5</v>
+      <c r="AR133" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AS133" t="inlineStr">
         <is>
-          <t>2578</t>
+          <t>2597</t>
         </is>
       </c>
     </row>
@@ -20137,7 +20135,7 @@
       </c>
       <c r="AS139" t="inlineStr">
         <is>
-          <t>2043</t>
+          <t>2036</t>
         </is>
       </c>
     </row>
@@ -20282,7 +20280,7 @@
       </c>
       <c r="AS140" t="inlineStr">
         <is>
-          <t>2676</t>
+          <t>2716</t>
         </is>
       </c>
     </row>
@@ -21163,11 +21161,11 @@
         <v>3324</v>
       </c>
       <c r="AR149" s="4" t="n">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="AS149" t="inlineStr">
         <is>
-          <t>3324</t>
+          <t>3342</t>
         </is>
       </c>
     </row>
@@ -21457,7 +21455,7 @@
       </c>
       <c r="AS151" t="inlineStr">
         <is>
-          <t>2552</t>
+          <t>2550</t>
         </is>
       </c>
     </row>
@@ -22037,7 +22035,7 @@
       </c>
       <c r="AS155" t="inlineStr">
         <is>
-          <t>2586</t>
+          <t>2614</t>
         </is>
       </c>
     </row>
@@ -22171,12 +22169,12 @@
       <c r="AQ156" t="n">
         <v>3118</v>
       </c>
-      <c r="AR156" s="3" t="n">
-        <v>21</v>
+      <c r="AR156" s="4" t="n">
+        <v>10</v>
       </c>
       <c r="AS156" t="inlineStr">
         <is>
-          <t>3118</t>
+          <t>3190</t>
         </is>
       </c>
     </row>
@@ -22523,7 +22521,7 @@
       </c>
       <c r="AS159" t="inlineStr">
         <is>
-          <t>2816</t>
+          <t>2821</t>
         </is>
       </c>
     </row>
@@ -22719,7 +22717,7 @@
       </c>
       <c r="AS161" t="inlineStr">
         <is>
-          <t>2925</t>
+          <t>2988</t>
         </is>
       </c>
     </row>
@@ -22841,12 +22839,12 @@
       <c r="AQ162" t="n">
         <v>2579</v>
       </c>
-      <c r="AR162" s="4" t="n">
-        <v>3</v>
+      <c r="AR162" s="3" t="n">
+        <v>20</v>
       </c>
       <c r="AS162" t="inlineStr">
         <is>
-          <t>2579</t>
+          <t>2656</t>
         </is>
       </c>
     </row>
@@ -22969,7 +22967,7 @@
       </c>
       <c r="AS163" t="inlineStr">
         <is>
-          <t>2988</t>
+          <t>3219</t>
         </is>
       </c>
     </row>
@@ -23072,11 +23070,11 @@
         <v>2935</v>
       </c>
       <c r="AR164" s="3" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AS164" t="inlineStr">
         <is>
-          <t>2935</t>
+          <t>3016</t>
         </is>
       </c>
     </row>
@@ -23187,7 +23185,7 @@
       </c>
       <c r="AS165" t="inlineStr">
         <is>
-          <t>2647</t>
+          <t>2759</t>
         </is>
       </c>
     </row>
@@ -23290,7 +23288,7 @@
       </c>
       <c r="AS166" t="inlineStr">
         <is>
-          <t>2791</t>
+          <t>2768</t>
         </is>
       </c>
     </row>
@@ -23607,12 +23605,12 @@
       <c r="AQ170" t="n">
         <v>0</v>
       </c>
-      <c r="AR170" s="2" t="n">
-        <v>0</v>
+      <c r="AR170" s="4" t="n">
+        <v>3</v>
       </c>
       <c r="AS170" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1517</t>
         </is>
       </c>
     </row>
@@ -23678,8 +23676,8 @@
       <c r="AQ171" t="n">
         <v>1647</v>
       </c>
-      <c r="AR171" s="4" t="n">
-        <v>13</v>
+      <c r="AR171" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AS171" t="inlineStr">
         <is>
@@ -23821,11 +23819,11 @@
         <v>1640</v>
       </c>
       <c r="AR173" s="4" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="AS173" t="inlineStr">
         <is>
-          <t>1640</t>
+          <t>1758</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-03-05 11:30:36
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AS173"/>
+  <dimension ref="A1:AU173"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -616,6 +616,16 @@
           <t>03-03_0</t>
         </is>
       </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>03-04_A</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>03-04_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -756,9 +766,15 @@
       <c r="AR2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS2" t="inlineStr">
-        <is>
-          <t>2602</t>
+      <c r="AS2" t="n">
+        <v>2602</v>
+      </c>
+      <c r="AT2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU2" t="inlineStr">
+        <is>
+          <t>2659</t>
         </is>
       </c>
     </row>
@@ -901,9 +917,15 @@
       <c r="AR3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AS3" t="inlineStr">
-        <is>
-          <t>4489</t>
+      <c r="AS3" t="n">
+        <v>4489</v>
+      </c>
+      <c r="AT3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU3" t="inlineStr">
+        <is>
+          <t>4836</t>
         </is>
       </c>
     </row>
@@ -913,7 +935,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>摸鱼者三战</t>
+          <t>摸鱼爱好者三战</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1046,9 +1068,15 @@
       <c r="AR4" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AS4" t="inlineStr">
-        <is>
-          <t>4641</t>
+      <c r="AS4" t="n">
+        <v>4641</v>
+      </c>
+      <c r="AT4" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AU4" t="inlineStr">
+        <is>
+          <t>4884</t>
         </is>
       </c>
     </row>
@@ -1191,9 +1219,15 @@
       <c r="AR5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AS5" t="inlineStr">
-        <is>
-          <t>4353</t>
+      <c r="AS5" t="n">
+        <v>4353</v>
+      </c>
+      <c r="AT5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU5" t="inlineStr">
+        <is>
+          <t>4492</t>
         </is>
       </c>
     </row>
@@ -1336,9 +1370,15 @@
       <c r="AR6" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AS6" t="inlineStr">
-        <is>
-          <t>4400</t>
+      <c r="AS6" t="n">
+        <v>4400</v>
+      </c>
+      <c r="AT6" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AU6" t="inlineStr">
+        <is>
+          <t>4637</t>
         </is>
       </c>
     </row>
@@ -1481,9 +1521,15 @@
       <c r="AR7" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AS7" t="inlineStr">
-        <is>
-          <t>4689</t>
+      <c r="AS7" t="n">
+        <v>4689</v>
+      </c>
+      <c r="AT7" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AU7" t="inlineStr">
+        <is>
+          <t>5089</t>
         </is>
       </c>
     </row>
@@ -1626,9 +1672,15 @@
       <c r="AR8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AS8" t="inlineStr">
-        <is>
-          <t>4128</t>
+      <c r="AS8" t="n">
+        <v>4128</v>
+      </c>
+      <c r="AT8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU8" t="inlineStr">
+        <is>
+          <t>4341</t>
         </is>
       </c>
     </row>
@@ -1771,9 +1823,15 @@
       <c r="AR9" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AS9" t="inlineStr">
-        <is>
-          <t>4260</t>
+      <c r="AS9" t="n">
+        <v>4260</v>
+      </c>
+      <c r="AT9" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="AU9" t="inlineStr">
+        <is>
+          <t>4440</t>
         </is>
       </c>
     </row>
@@ -1916,9 +1974,15 @@
       <c r="AR10" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AS10" t="inlineStr">
-        <is>
-          <t>4278</t>
+      <c r="AS10" t="n">
+        <v>4278</v>
+      </c>
+      <c r="AT10" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AU10" t="inlineStr">
+        <is>
+          <t>4566</t>
         </is>
       </c>
     </row>
@@ -2061,9 +2125,15 @@
       <c r="AR11" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AS11" t="inlineStr">
-        <is>
-          <t>3865</t>
+      <c r="AS11" t="n">
+        <v>3865</v>
+      </c>
+      <c r="AT11" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU11" t="inlineStr">
+        <is>
+          <t>4102</t>
         </is>
       </c>
     </row>
@@ -2206,7 +2276,13 @@
       <c r="AR12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS12" t="inlineStr">
+      <c r="AS12" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AT12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU12" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2351,9 +2427,15 @@
       <c r="AR13" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AS13" t="inlineStr">
-        <is>
-          <t>4881</t>
+      <c r="AS13" t="n">
+        <v>4881</v>
+      </c>
+      <c r="AT13" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="AU13" t="inlineStr">
+        <is>
+          <t>5145</t>
         </is>
       </c>
     </row>
@@ -2496,9 +2578,15 @@
       <c r="AR14" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AS14" t="inlineStr">
-        <is>
-          <t>4304</t>
+      <c r="AS14" t="n">
+        <v>4304</v>
+      </c>
+      <c r="AT14" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AU14" t="inlineStr">
+        <is>
+          <t>4507</t>
         </is>
       </c>
     </row>
@@ -2641,7 +2729,13 @@
       <c r="AR15" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS15" t="inlineStr">
+      <c r="AS15" t="n">
+        <v>2539</v>
+      </c>
+      <c r="AT15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU15" t="inlineStr">
         <is>
           <t>2539</t>
         </is>
@@ -2786,9 +2880,15 @@
       <c r="AR16" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="AS16" t="inlineStr">
-        <is>
-          <t>4415</t>
+      <c r="AS16" t="n">
+        <v>4415</v>
+      </c>
+      <c r="AT16" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AU16" t="inlineStr">
+        <is>
+          <t>4692</t>
         </is>
       </c>
     </row>
@@ -2931,9 +3031,15 @@
       <c r="AR17" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AS17" t="inlineStr">
-        <is>
-          <t>3788</t>
+      <c r="AS17" t="n">
+        <v>3788</v>
+      </c>
+      <c r="AT17" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AU17" t="inlineStr">
+        <is>
+          <t>3896</t>
         </is>
       </c>
     </row>
@@ -3076,9 +3182,15 @@
       <c r="AR18" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AS18" t="inlineStr">
-        <is>
-          <t>3801</t>
+      <c r="AS18" t="n">
+        <v>3801</v>
+      </c>
+      <c r="AT18" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AU18" t="inlineStr">
+        <is>
+          <t>3942</t>
         </is>
       </c>
     </row>
@@ -3221,9 +3333,15 @@
       <c r="AR19" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AS19" t="inlineStr">
-        <is>
-          <t>4425</t>
+      <c r="AS19" t="n">
+        <v>4425</v>
+      </c>
+      <c r="AT19" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AU19" t="inlineStr">
+        <is>
+          <t>4725</t>
         </is>
       </c>
     </row>
@@ -3366,9 +3484,15 @@
       <c r="AR20" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AS20" t="inlineStr">
-        <is>
-          <t>4916</t>
+      <c r="AS20" t="n">
+        <v>4916</v>
+      </c>
+      <c r="AT20" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AU20" t="inlineStr">
+        <is>
+          <t>5263</t>
         </is>
       </c>
     </row>
@@ -3511,9 +3635,15 @@
       <c r="AR21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS21" t="inlineStr">
-        <is>
-          <t>3108</t>
+      <c r="AS21" t="n">
+        <v>3108</v>
+      </c>
+      <c r="AT21" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU21" t="inlineStr">
+        <is>
+          <t>3435</t>
         </is>
       </c>
     </row>
@@ -3656,9 +3786,15 @@
       <c r="AR22" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AS22" t="inlineStr">
-        <is>
-          <t>4298</t>
+      <c r="AS22" t="n">
+        <v>4298</v>
+      </c>
+      <c r="AT22" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AU22" t="inlineStr">
+        <is>
+          <t>4581</t>
         </is>
       </c>
     </row>
@@ -3801,9 +3937,15 @@
       <c r="AR23" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS23" t="inlineStr">
-        <is>
-          <t>3528</t>
+      <c r="AS23" t="n">
+        <v>3528</v>
+      </c>
+      <c r="AT23" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU23" t="inlineStr">
+        <is>
+          <t>3790</t>
         </is>
       </c>
     </row>
@@ -3946,9 +4088,15 @@
       <c r="AR24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AS24" t="inlineStr">
-        <is>
-          <t>4362</t>
+      <c r="AS24" t="n">
+        <v>4362</v>
+      </c>
+      <c r="AT24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AU24" t="inlineStr">
+        <is>
+          <t>4641</t>
         </is>
       </c>
     </row>
@@ -4091,7 +4239,13 @@
       <c r="AR25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS25" t="inlineStr">
+      <c r="AS25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4236,9 +4390,15 @@
       <c r="AR26" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AS26" t="inlineStr">
-        <is>
-          <t>4488</t>
+      <c r="AS26" t="n">
+        <v>4488</v>
+      </c>
+      <c r="AT26" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AU26" t="inlineStr">
+        <is>
+          <t>4646</t>
         </is>
       </c>
     </row>
@@ -4381,9 +4541,15 @@
       <c r="AR27" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AS27" t="inlineStr">
-        <is>
-          <t>4307</t>
+      <c r="AS27" t="n">
+        <v>4307</v>
+      </c>
+      <c r="AT27" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU27" t="inlineStr">
+        <is>
+          <t>4485</t>
         </is>
       </c>
     </row>
@@ -4526,9 +4692,15 @@
       <c r="AR28" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="AS28" t="inlineStr">
-        <is>
-          <t>3603</t>
+      <c r="AS28" t="n">
+        <v>3603</v>
+      </c>
+      <c r="AT28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="AU28" t="inlineStr">
+        <is>
+          <t>3757</t>
         </is>
       </c>
     </row>
@@ -4671,9 +4843,15 @@
       <c r="AR29" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AS29" t="inlineStr">
-        <is>
-          <t>5051</t>
+      <c r="AS29" t="n">
+        <v>5051</v>
+      </c>
+      <c r="AT29" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AU29" t="inlineStr">
+        <is>
+          <t>5447</t>
         </is>
       </c>
     </row>
@@ -4816,9 +4994,15 @@
       <c r="AR30" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AS30" t="inlineStr">
-        <is>
-          <t>3822</t>
+      <c r="AS30" t="n">
+        <v>3822</v>
+      </c>
+      <c r="AT30" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AU30" t="inlineStr">
+        <is>
+          <t>4021</t>
         </is>
       </c>
     </row>
@@ -4961,9 +5145,15 @@
       <c r="AR31" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="AS31" t="inlineStr">
-        <is>
-          <t>4784</t>
+      <c r="AS31" t="n">
+        <v>4784</v>
+      </c>
+      <c r="AT31" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AU31" t="inlineStr">
+        <is>
+          <t>4957</t>
         </is>
       </c>
     </row>
@@ -5106,9 +5296,15 @@
       <c r="AR32" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AS32" t="inlineStr">
-        <is>
-          <t>4654</t>
+      <c r="AS32" t="n">
+        <v>4654</v>
+      </c>
+      <c r="AT32" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="AU32" t="inlineStr">
+        <is>
+          <t>4990</t>
         </is>
       </c>
     </row>
@@ -5251,9 +5447,15 @@
       <c r="AR33" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="AS33" t="inlineStr">
-        <is>
-          <t>3971</t>
+      <c r="AS33" t="n">
+        <v>3971</v>
+      </c>
+      <c r="AT33" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AU33" t="inlineStr">
+        <is>
+          <t>4259</t>
         </is>
       </c>
     </row>
@@ -5396,9 +5598,15 @@
       <c r="AR34" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AS34" t="inlineStr">
-        <is>
-          <t>4247</t>
+      <c r="AS34" t="n">
+        <v>4247</v>
+      </c>
+      <c r="AT34" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AU34" t="inlineStr">
+        <is>
+          <t>4482</t>
         </is>
       </c>
     </row>
@@ -5541,9 +5749,15 @@
       <c r="AR35" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AS35" t="inlineStr">
-        <is>
-          <t>4128</t>
+      <c r="AS35" t="n">
+        <v>4128</v>
+      </c>
+      <c r="AT35" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AU35" t="inlineStr">
+        <is>
+          <t>4379</t>
         </is>
       </c>
     </row>
@@ -5686,9 +5900,15 @@
       <c r="AR36" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AS36" t="inlineStr">
-        <is>
-          <t>4200</t>
+      <c r="AS36" t="n">
+        <v>4200</v>
+      </c>
+      <c r="AT36" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU36" t="inlineStr">
+        <is>
+          <t>4567</t>
         </is>
       </c>
     </row>
@@ -5831,9 +6051,15 @@
       <c r="AR37" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AS37" t="inlineStr">
-        <is>
-          <t>3732</t>
+      <c r="AS37" t="n">
+        <v>3732</v>
+      </c>
+      <c r="AT37" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AU37" t="inlineStr">
+        <is>
+          <t>3846</t>
         </is>
       </c>
     </row>
@@ -5976,9 +6202,15 @@
       <c r="AR38" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AS38" t="inlineStr">
-        <is>
-          <t>4243</t>
+      <c r="AS38" t="n">
+        <v>4243</v>
+      </c>
+      <c r="AT38" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AU38" t="inlineStr">
+        <is>
+          <t>4515</t>
         </is>
       </c>
     </row>
@@ -6121,9 +6353,15 @@
       <c r="AR39" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AS39" t="inlineStr">
-        <is>
-          <t>4277</t>
+      <c r="AS39" t="n">
+        <v>4277</v>
+      </c>
+      <c r="AT39" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AU39" t="inlineStr">
+        <is>
+          <t>4542</t>
         </is>
       </c>
     </row>
@@ -6266,9 +6504,15 @@
       <c r="AR40" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AS40" t="inlineStr">
-        <is>
-          <t>4335</t>
+      <c r="AS40" t="n">
+        <v>4335</v>
+      </c>
+      <c r="AT40" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AU40" t="inlineStr">
+        <is>
+          <t>4662</t>
         </is>
       </c>
     </row>
@@ -6411,7 +6655,13 @@
       <c r="AR41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS41" t="inlineStr">
+      <c r="AS41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU41" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6556,9 +6806,15 @@
       <c r="AR42" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AS42" t="inlineStr">
-        <is>
-          <t>4725</t>
+      <c r="AS42" t="n">
+        <v>4725</v>
+      </c>
+      <c r="AT42" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AU42" t="inlineStr">
+        <is>
+          <t>4868</t>
         </is>
       </c>
     </row>
@@ -6701,9 +6957,15 @@
       <c r="AR43" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AS43" t="inlineStr">
-        <is>
-          <t>4508</t>
+      <c r="AS43" t="n">
+        <v>4508</v>
+      </c>
+      <c r="AT43" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AU43" t="inlineStr">
+        <is>
+          <t>4763</t>
         </is>
       </c>
     </row>
@@ -6846,9 +7108,15 @@
       <c r="AR44" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AS44" t="inlineStr">
-        <is>
-          <t>4239</t>
+      <c r="AS44" t="n">
+        <v>4239</v>
+      </c>
+      <c r="AT44" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AU44" t="inlineStr">
+        <is>
+          <t>4654</t>
         </is>
       </c>
     </row>
@@ -6991,9 +7259,15 @@
       <c r="AR45" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AS45" t="inlineStr">
-        <is>
-          <t>3998</t>
+      <c r="AS45" t="n">
+        <v>3998</v>
+      </c>
+      <c r="AT45" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AU45" t="inlineStr">
+        <is>
+          <t>4111</t>
         </is>
       </c>
     </row>
@@ -7136,9 +7410,15 @@
       <c r="AR46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AS46" t="inlineStr">
-        <is>
-          <t>3875</t>
+      <c r="AS46" t="n">
+        <v>3875</v>
+      </c>
+      <c r="AT46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AU46" t="inlineStr">
+        <is>
+          <t>4042</t>
         </is>
       </c>
     </row>
@@ -7281,9 +7561,15 @@
       <c r="AR47" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AS47" t="inlineStr">
-        <is>
-          <t>3918</t>
+      <c r="AS47" t="n">
+        <v>3918</v>
+      </c>
+      <c r="AT47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU47" t="inlineStr">
+        <is>
+          <t>3912</t>
         </is>
       </c>
     </row>
@@ -7426,9 +7712,15 @@
       <c r="AR48" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AS48" t="inlineStr">
-        <is>
-          <t>4573</t>
+      <c r="AS48" t="n">
+        <v>4573</v>
+      </c>
+      <c r="AT48" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="AU48" t="inlineStr">
+        <is>
+          <t>4877</t>
         </is>
       </c>
     </row>
@@ -7571,9 +7863,15 @@
       <c r="AR49" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AS49" t="inlineStr">
-        <is>
-          <t>3273</t>
+      <c r="AS49" t="n">
+        <v>3273</v>
+      </c>
+      <c r="AT49" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU49" t="inlineStr">
+        <is>
+          <t>3496</t>
         </is>
       </c>
     </row>
@@ -7716,9 +8014,15 @@
       <c r="AR50" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AS50" t="inlineStr">
-        <is>
-          <t>4617</t>
+      <c r="AS50" t="n">
+        <v>4617</v>
+      </c>
+      <c r="AT50" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AU50" t="inlineStr">
+        <is>
+          <t>4880</t>
         </is>
       </c>
     </row>
@@ -7861,9 +8165,15 @@
       <c r="AR51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS51" t="inlineStr">
-        <is>
-          <t>2548</t>
+      <c r="AS51" t="n">
+        <v>2548</v>
+      </c>
+      <c r="AT51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU51" t="inlineStr">
+        <is>
+          <t>2546</t>
         </is>
       </c>
     </row>
@@ -8006,9 +8316,15 @@
       <c r="AR52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS52" t="inlineStr">
-        <is>
-          <t>2552</t>
+      <c r="AS52" t="n">
+        <v>2552</v>
+      </c>
+      <c r="AT52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU52" t="inlineStr">
+        <is>
+          <t>2548</t>
         </is>
       </c>
     </row>
@@ -8151,7 +8467,13 @@
       <c r="AR53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS53" t="inlineStr">
+      <c r="AS53" t="n">
+        <v>3062</v>
+      </c>
+      <c r="AT53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU53" t="inlineStr">
         <is>
           <t>3062</t>
         </is>
@@ -8296,9 +8618,15 @@
       <c r="AR54" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AS54" t="inlineStr">
-        <is>
-          <t>4488</t>
+      <c r="AS54" t="n">
+        <v>4488</v>
+      </c>
+      <c r="AT54" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="AU54" t="inlineStr">
+        <is>
+          <t>4615</t>
         </is>
       </c>
     </row>
@@ -8441,9 +8769,15 @@
       <c r="AR55" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AS55" t="inlineStr">
-        <is>
-          <t>3576</t>
+      <c r="AS55" t="n">
+        <v>3576</v>
+      </c>
+      <c r="AT55" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="AU55" t="inlineStr">
+        <is>
+          <t>3748</t>
         </is>
       </c>
     </row>
@@ -8586,9 +8920,15 @@
       <c r="AR56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AS56" t="inlineStr">
-        <is>
-          <t>3625</t>
+      <c r="AS56" t="n">
+        <v>3625</v>
+      </c>
+      <c r="AT56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU56" t="inlineStr">
+        <is>
+          <t>3671</t>
         </is>
       </c>
     </row>
@@ -8731,9 +9071,15 @@
       <c r="AR57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AS57" t="inlineStr">
-        <is>
-          <t>4166</t>
+      <c r="AS57" t="n">
+        <v>4166</v>
+      </c>
+      <c r="AT57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU57" t="inlineStr">
+        <is>
+          <t>4333</t>
         </is>
       </c>
     </row>
@@ -8876,9 +9222,15 @@
       <c r="AR58" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AS58" t="inlineStr">
-        <is>
-          <t>3689</t>
+      <c r="AS58" t="n">
+        <v>3689</v>
+      </c>
+      <c r="AT58" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AU58" t="inlineStr">
+        <is>
+          <t>3806</t>
         </is>
       </c>
     </row>
@@ -8940,6 +9292,8 @@
       <c r="AQ59" t="inlineStr"/>
       <c r="AR59" s="3" t="inlineStr"/>
       <c r="AS59" t="inlineStr"/>
+      <c r="AT59" s="3" t="inlineStr"/>
+      <c r="AU59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -8999,6 +9353,8 @@
       <c r="AQ60" t="inlineStr"/>
       <c r="AR60" s="3" t="inlineStr"/>
       <c r="AS60" t="inlineStr"/>
+      <c r="AT60" s="3" t="inlineStr"/>
+      <c r="AU60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -9139,9 +9495,15 @@
       <c r="AR61" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AS61" t="inlineStr">
-        <is>
-          <t>4072</t>
+      <c r="AS61" t="n">
+        <v>4072</v>
+      </c>
+      <c r="AT61" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AU61" t="inlineStr">
+        <is>
+          <t>4231</t>
         </is>
       </c>
     </row>
@@ -9284,7 +9646,13 @@
       <c r="AR62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS62" t="inlineStr">
+      <c r="AS62" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9429,9 +9797,15 @@
       <c r="AR63" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AS63" t="inlineStr">
-        <is>
-          <t>4153</t>
+      <c r="AS63" t="n">
+        <v>4153</v>
+      </c>
+      <c r="AT63" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AU63" t="inlineStr">
+        <is>
+          <t>4367</t>
         </is>
       </c>
     </row>
@@ -9574,7 +9948,13 @@
       <c r="AR64" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="AS64" t="inlineStr">
+      <c r="AS64" t="n">
+        <v>2669</v>
+      </c>
+      <c r="AT64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU64" t="inlineStr">
         <is>
           <t>2669</t>
         </is>
@@ -9638,6 +10018,8 @@
       <c r="AQ65" t="inlineStr"/>
       <c r="AR65" s="3" t="inlineStr"/>
       <c r="AS65" t="inlineStr"/>
+      <c r="AT65" s="3" t="inlineStr"/>
+      <c r="AU65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -9778,9 +10160,15 @@
       <c r="AR66" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="AS66" t="inlineStr">
-        <is>
-          <t>2580</t>
+      <c r="AS66" t="n">
+        <v>2580</v>
+      </c>
+      <c r="AT66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU66" t="inlineStr">
+        <is>
+          <t>2570</t>
         </is>
       </c>
     </row>
@@ -9923,9 +10311,15 @@
       <c r="AR67" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AS67" t="inlineStr">
-        <is>
-          <t>4027</t>
+      <c r="AS67" t="n">
+        <v>4027</v>
+      </c>
+      <c r="AT67" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AU67" t="inlineStr">
+        <is>
+          <t>4231</t>
         </is>
       </c>
     </row>
@@ -10068,9 +10462,15 @@
       <c r="AR68" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AS68" t="inlineStr">
-        <is>
-          <t>3990</t>
+      <c r="AS68" t="n">
+        <v>3990</v>
+      </c>
+      <c r="AT68" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AU68" t="inlineStr">
+        <is>
+          <t>4186</t>
         </is>
       </c>
     </row>
@@ -10213,9 +10613,15 @@
       <c r="AR69" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AS69" t="inlineStr">
-        <is>
-          <t>3645</t>
+      <c r="AS69" t="n">
+        <v>3645</v>
+      </c>
+      <c r="AT69" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AU69" t="inlineStr">
+        <is>
+          <t>3793</t>
         </is>
       </c>
     </row>
@@ -10358,9 +10764,15 @@
       <c r="AR70" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="AS70" t="inlineStr">
-        <is>
-          <t>2512</t>
+      <c r="AS70" t="n">
+        <v>2512</v>
+      </c>
+      <c r="AT70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU70" t="inlineStr">
+        <is>
+          <t>2551</t>
         </is>
       </c>
     </row>
@@ -10503,9 +10915,15 @@
       <c r="AR71" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AS71" t="inlineStr">
-        <is>
-          <t>3781</t>
+      <c r="AS71" t="n">
+        <v>3781</v>
+      </c>
+      <c r="AT71" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AU71" t="inlineStr">
+        <is>
+          <t>3880</t>
         </is>
       </c>
     </row>
@@ -10648,9 +11066,15 @@
       <c r="AR72" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="AS72" t="inlineStr">
-        <is>
-          <t>3159</t>
+      <c r="AS72" t="n">
+        <v>3159</v>
+      </c>
+      <c r="AT72" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AU72" t="inlineStr">
+        <is>
+          <t>3292</t>
         </is>
       </c>
     </row>
@@ -10793,9 +11217,15 @@
       <c r="AR73" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AS73" t="inlineStr">
-        <is>
-          <t>3655</t>
+      <c r="AS73" t="n">
+        <v>3655</v>
+      </c>
+      <c r="AT73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU73" t="inlineStr">
+        <is>
+          <t>3790</t>
         </is>
       </c>
     </row>
@@ -10938,9 +11368,15 @@
       <c r="AR74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS74" t="inlineStr">
-        <is>
-          <t>2705</t>
+      <c r="AS74" t="n">
+        <v>2705</v>
+      </c>
+      <c r="AT74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU74" t="inlineStr">
+        <is>
+          <t>2796</t>
         </is>
       </c>
     </row>
@@ -11083,9 +11519,15 @@
       <c r="AR75" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="AS75" t="inlineStr">
-        <is>
-          <t>3493</t>
+      <c r="AS75" t="n">
+        <v>3493</v>
+      </c>
+      <c r="AT75" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AU75" t="inlineStr">
+        <is>
+          <t>3572</t>
         </is>
       </c>
     </row>
@@ -11228,9 +11670,15 @@
       <c r="AR76" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AS76" t="inlineStr">
-        <is>
-          <t>4191</t>
+      <c r="AS76" t="n">
+        <v>4191</v>
+      </c>
+      <c r="AT76" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AU76" t="inlineStr">
+        <is>
+          <t>4279</t>
         </is>
       </c>
     </row>
@@ -11373,7 +11821,13 @@
       <c r="AR77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS77" t="inlineStr">
+      <c r="AS77" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU77" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11518,9 +11972,15 @@
       <c r="AR78" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AS78" t="inlineStr">
-        <is>
-          <t>4090</t>
+      <c r="AS78" t="n">
+        <v>4090</v>
+      </c>
+      <c r="AT78" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AU78" t="inlineStr">
+        <is>
+          <t>4294</t>
         </is>
       </c>
     </row>
@@ -11663,7 +12123,13 @@
       <c r="AR79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS79" t="inlineStr">
+      <c r="AS79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11808,9 +12274,15 @@
       <c r="AR80" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="AS80" t="inlineStr">
-        <is>
-          <t>3893</t>
+      <c r="AS80" t="n">
+        <v>3893</v>
+      </c>
+      <c r="AT80" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AU80" t="inlineStr">
+        <is>
+          <t>4125</t>
         </is>
       </c>
     </row>
@@ -11953,9 +12425,15 @@
       <c r="AR81" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AS81" t="inlineStr">
-        <is>
-          <t>4088</t>
+      <c r="AS81" t="n">
+        <v>4088</v>
+      </c>
+      <c r="AT81" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AU81" t="inlineStr">
+        <is>
+          <t>4224</t>
         </is>
       </c>
     </row>
@@ -12098,9 +12576,15 @@
       <c r="AR82" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AS82" t="inlineStr">
-        <is>
-          <t>3871</t>
+      <c r="AS82" t="n">
+        <v>3871</v>
+      </c>
+      <c r="AT82" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AU82" t="inlineStr">
+        <is>
+          <t>3980</t>
         </is>
       </c>
     </row>
@@ -12243,9 +12727,15 @@
       <c r="AR83" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AS83" t="inlineStr">
-        <is>
-          <t>3637</t>
+      <c r="AS83" t="n">
+        <v>3637</v>
+      </c>
+      <c r="AT83" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AU83" t="inlineStr">
+        <is>
+          <t>3822</t>
         </is>
       </c>
     </row>
@@ -12367,6 +12857,8 @@
       <c r="AQ84" t="inlineStr"/>
       <c r="AR84" s="3" t="inlineStr"/>
       <c r="AS84" t="inlineStr"/>
+      <c r="AT84" s="3" t="inlineStr"/>
+      <c r="AU84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -12507,9 +12999,15 @@
       <c r="AR85" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AS85" t="inlineStr">
-        <is>
-          <t>3371</t>
+      <c r="AS85" t="n">
+        <v>3371</v>
+      </c>
+      <c r="AT85" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AU85" t="inlineStr">
+        <is>
+          <t>3346</t>
         </is>
       </c>
     </row>
@@ -12652,9 +13150,15 @@
       <c r="AR86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS86" t="inlineStr">
-        <is>
-          <t>2560</t>
+      <c r="AS86" t="n">
+        <v>2560</v>
+      </c>
+      <c r="AT86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU86" t="inlineStr">
+        <is>
+          <t>2657</t>
         </is>
       </c>
     </row>
@@ -12797,9 +13301,15 @@
       <c r="AR87" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AS87" t="inlineStr">
-        <is>
-          <t>3823</t>
+      <c r="AS87" t="n">
+        <v>3823</v>
+      </c>
+      <c r="AT87" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AU87" t="inlineStr">
+        <is>
+          <t>4007</t>
         </is>
       </c>
     </row>
@@ -12942,9 +13452,15 @@
       <c r="AR88" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="AS88" t="inlineStr">
-        <is>
-          <t>2617</t>
+      <c r="AS88" t="n">
+        <v>2617</v>
+      </c>
+      <c r="AT88" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AU88" t="inlineStr">
+        <is>
+          <t>2604</t>
         </is>
       </c>
     </row>
@@ -13087,9 +13603,15 @@
       <c r="AR89" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AS89" t="inlineStr">
-        <is>
-          <t>2963</t>
+      <c r="AS89" t="n">
+        <v>2963</v>
+      </c>
+      <c r="AT89" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU89" t="inlineStr">
+        <is>
+          <t>3018</t>
         </is>
       </c>
     </row>
@@ -13232,9 +13754,15 @@
       <c r="AR90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS90" t="inlineStr">
-        <is>
-          <t>2602</t>
+      <c r="AS90" t="n">
+        <v>2602</v>
+      </c>
+      <c r="AT90" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU90" t="inlineStr">
+        <is>
+          <t>2670</t>
         </is>
       </c>
     </row>
@@ -13377,9 +13905,15 @@
       <c r="AR91" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AS91" t="inlineStr">
-        <is>
-          <t>2732</t>
+      <c r="AS91" t="n">
+        <v>2732</v>
+      </c>
+      <c r="AT91" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU91" t="inlineStr">
+        <is>
+          <t>2731</t>
         </is>
       </c>
     </row>
@@ -13522,7 +14056,13 @@
       <c r="AR92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS92" t="inlineStr">
+      <c r="AS92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13667,9 +14207,15 @@
       <c r="AR93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS93" t="inlineStr">
-        <is>
-          <t>2295</t>
+      <c r="AS93" t="n">
+        <v>2295</v>
+      </c>
+      <c r="AT93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU93" t="inlineStr">
+        <is>
+          <t>2305</t>
         </is>
       </c>
     </row>
@@ -13812,9 +14358,15 @@
       <c r="AR94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS94" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="AS94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU94" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -13957,9 +14509,15 @@
       <c r="AR95" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="AS95" t="inlineStr">
-        <is>
-          <t>2422</t>
+      <c r="AS95" t="n">
+        <v>2422</v>
+      </c>
+      <c r="AT95" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="AU95" t="inlineStr">
+        <is>
+          <t>2530</t>
         </is>
       </c>
     </row>
@@ -14102,9 +14660,15 @@
       <c r="AR96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS96" t="inlineStr">
-        <is>
-          <t>2499</t>
+      <c r="AS96" t="n">
+        <v>2499</v>
+      </c>
+      <c r="AT96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU96" t="inlineStr">
+        <is>
+          <t>2488</t>
         </is>
       </c>
     </row>
@@ -14247,9 +14811,15 @@
       <c r="AR97" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AS97" t="inlineStr">
-        <is>
-          <t>2809</t>
+      <c r="AS97" t="n">
+        <v>2809</v>
+      </c>
+      <c r="AT97" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AU97" t="inlineStr">
+        <is>
+          <t>2932</t>
         </is>
       </c>
     </row>
@@ -14392,7 +14962,13 @@
       <c r="AR98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS98" t="inlineStr">
+      <c r="AS98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14537,9 +15113,15 @@
       <c r="AR99" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="AS99" t="inlineStr">
-        <is>
-          <t>3214</t>
+      <c r="AS99" t="n">
+        <v>3214</v>
+      </c>
+      <c r="AT99" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="AU99" t="inlineStr">
+        <is>
+          <t>3382</t>
         </is>
       </c>
     </row>
@@ -14682,9 +15264,15 @@
       <c r="AR100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS100" t="inlineStr">
-        <is>
-          <t>2416</t>
+      <c r="AS100" t="n">
+        <v>2416</v>
+      </c>
+      <c r="AT100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU100" t="inlineStr">
+        <is>
+          <t>2403</t>
         </is>
       </c>
     </row>
@@ -14827,9 +15415,15 @@
       <c r="AR101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AS101" t="inlineStr">
-        <is>
-          <t>3793</t>
+      <c r="AS101" t="n">
+        <v>3793</v>
+      </c>
+      <c r="AT101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AU101" t="inlineStr">
+        <is>
+          <t>3932</t>
         </is>
       </c>
     </row>
@@ -14972,9 +15566,15 @@
       <c r="AR102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AS102" t="inlineStr">
-        <is>
-          <t>3405</t>
+      <c r="AS102" t="n">
+        <v>3405</v>
+      </c>
+      <c r="AT102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU102" t="inlineStr">
+        <is>
+          <t>3572</t>
         </is>
       </c>
     </row>
@@ -15117,9 +15717,15 @@
       <c r="AR103" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AS103" t="inlineStr">
-        <is>
-          <t>2787</t>
+      <c r="AS103" t="n">
+        <v>2787</v>
+      </c>
+      <c r="AT103" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU103" t="inlineStr">
+        <is>
+          <t>3110</t>
         </is>
       </c>
     </row>
@@ -15262,9 +15868,15 @@
       <c r="AR104" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AS104" t="inlineStr">
-        <is>
-          <t>3864</t>
+      <c r="AS104" t="n">
+        <v>3864</v>
+      </c>
+      <c r="AT104" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AU104" t="inlineStr">
+        <is>
+          <t>4007</t>
         </is>
       </c>
     </row>
@@ -15407,9 +16019,15 @@
       <c r="AR105" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="AS105" t="inlineStr">
-        <is>
-          <t>3495</t>
+      <c r="AS105" t="n">
+        <v>3495</v>
+      </c>
+      <c r="AT105" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AU105" t="inlineStr">
+        <is>
+          <t>3638</t>
         </is>
       </c>
     </row>
@@ -15552,7 +16170,13 @@
       <c r="AR106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS106" t="inlineStr">
+      <c r="AS106" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15697,9 +16321,15 @@
       <c r="AR107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS107" t="inlineStr">
-        <is>
-          <t>2557</t>
+      <c r="AS107" t="n">
+        <v>2557</v>
+      </c>
+      <c r="AT107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU107" t="inlineStr">
+        <is>
+          <t>2519</t>
         </is>
       </c>
     </row>
@@ -15842,7 +16472,13 @@
       <c r="AR108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS108" t="inlineStr">
+      <c r="AS108" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15987,9 +16623,15 @@
       <c r="AR109" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="AS109" t="inlineStr">
-        <is>
-          <t>3321</t>
+      <c r="AS109" t="n">
+        <v>3321</v>
+      </c>
+      <c r="AT109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU109" t="inlineStr">
+        <is>
+          <t>3416</t>
         </is>
       </c>
     </row>
@@ -16132,9 +16774,15 @@
       <c r="AR110" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AS110" t="inlineStr">
-        <is>
-          <t>3265</t>
+      <c r="AS110" t="n">
+        <v>3265</v>
+      </c>
+      <c r="AT110" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AU110" t="inlineStr">
+        <is>
+          <t>3264</t>
         </is>
       </c>
     </row>
@@ -16280,6 +16928,8 @@
       <c r="AS111" t="n">
         <v>2545</v>
       </c>
+      <c r="AT111" s="3" t="inlineStr"/>
+      <c r="AU111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -16420,9 +17070,15 @@
       <c r="AR112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS112" t="inlineStr">
-        <is>
-          <t>2563</t>
+      <c r="AS112" t="n">
+        <v>2563</v>
+      </c>
+      <c r="AT112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU112" t="inlineStr">
+        <is>
+          <t>2571</t>
         </is>
       </c>
     </row>
@@ -16565,9 +17221,15 @@
       <c r="AR113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS113" t="inlineStr">
-        <is>
-          <t>3093</t>
+      <c r="AS113" t="n">
+        <v>3093</v>
+      </c>
+      <c r="AT113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU113" t="inlineStr">
+        <is>
+          <t>3169</t>
         </is>
       </c>
     </row>
@@ -16710,9 +17372,15 @@
       <c r="AR114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS114" t="inlineStr">
-        <is>
-          <t>3155</t>
+      <c r="AS114" t="n">
+        <v>3155</v>
+      </c>
+      <c r="AT114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU114" t="inlineStr">
+        <is>
+          <t>3349</t>
         </is>
       </c>
     </row>
@@ -16855,9 +17523,15 @@
       <c r="AR115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS115" t="inlineStr">
-        <is>
-          <t>2020</t>
+      <c r="AS115" t="n">
+        <v>2020</v>
+      </c>
+      <c r="AT115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU115" t="inlineStr">
+        <is>
+          <t>2006</t>
         </is>
       </c>
     </row>
@@ -17000,9 +17674,15 @@
       <c r="AR116" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AS116" t="inlineStr">
-        <is>
-          <t>2917</t>
+      <c r="AS116" t="n">
+        <v>2917</v>
+      </c>
+      <c r="AT116" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AU116" t="inlineStr">
+        <is>
+          <t>2928</t>
         </is>
       </c>
     </row>
@@ -17145,9 +17825,15 @@
       <c r="AR117" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AS117" t="inlineStr">
-        <is>
-          <t>3259</t>
+      <c r="AS117" t="n">
+        <v>3259</v>
+      </c>
+      <c r="AT117" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AU117" t="inlineStr">
+        <is>
+          <t>3346</t>
         </is>
       </c>
     </row>
@@ -17290,7 +17976,13 @@
       <c r="AR118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS118" t="inlineStr">
+      <c r="AS118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -17435,9 +18127,15 @@
       <c r="AR119" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="AS119" t="inlineStr">
-        <is>
-          <t>3483</t>
+      <c r="AS119" t="n">
+        <v>3483</v>
+      </c>
+      <c r="AT119" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AU119" t="inlineStr">
+        <is>
+          <t>3675</t>
         </is>
       </c>
     </row>
@@ -17580,9 +18278,15 @@
       <c r="AR120" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AS120" t="inlineStr">
-        <is>
-          <t>2481</t>
+      <c r="AS120" t="n">
+        <v>2481</v>
+      </c>
+      <c r="AT120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU120" t="inlineStr">
+        <is>
+          <t>2463</t>
         </is>
       </c>
     </row>
@@ -17725,9 +18429,15 @@
       <c r="AR121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS121" t="inlineStr">
-        <is>
-          <t>2947</t>
+      <c r="AS121" t="n">
+        <v>2947</v>
+      </c>
+      <c r="AT121" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AU121" t="inlineStr">
+        <is>
+          <t>2987</t>
         </is>
       </c>
     </row>
@@ -17870,7 +18580,13 @@
       <c r="AR122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS122" t="inlineStr">
+      <c r="AS122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18015,9 +18731,15 @@
       <c r="AR123" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="AS123" t="inlineStr">
-        <is>
-          <t>2845</t>
+      <c r="AS123" t="n">
+        <v>2845</v>
+      </c>
+      <c r="AT123" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU123" t="inlineStr">
+        <is>
+          <t>3026</t>
         </is>
       </c>
     </row>
@@ -18160,9 +18882,15 @@
       <c r="AR124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AS124" t="inlineStr">
-        <is>
-          <t>2995</t>
+      <c r="AS124" t="n">
+        <v>2995</v>
+      </c>
+      <c r="AT124" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AU124" t="inlineStr">
+        <is>
+          <t>2985</t>
         </is>
       </c>
     </row>
@@ -18305,9 +19033,15 @@
       <c r="AR125" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AS125" t="inlineStr">
-        <is>
-          <t>2904</t>
+      <c r="AS125" t="n">
+        <v>2904</v>
+      </c>
+      <c r="AT125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU125" t="inlineStr">
+        <is>
+          <t>2914</t>
         </is>
       </c>
     </row>
@@ -18450,9 +19184,15 @@
       <c r="AR126" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AS126" t="inlineStr">
-        <is>
-          <t>3048</t>
+      <c r="AS126" t="n">
+        <v>3048</v>
+      </c>
+      <c r="AT126" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AU126" t="inlineStr">
+        <is>
+          <t>3068</t>
         </is>
       </c>
     </row>
@@ -18595,9 +19335,15 @@
       <c r="AR127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS127" t="inlineStr">
-        <is>
-          <t>2339</t>
+      <c r="AS127" t="n">
+        <v>2339</v>
+      </c>
+      <c r="AT127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU127" t="inlineStr">
+        <is>
+          <t>2322</t>
         </is>
       </c>
     </row>
@@ -18740,7 +19486,13 @@
       <c r="AR128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS128" t="inlineStr">
+      <c r="AS128" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18885,7 +19637,13 @@
       <c r="AR129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS129" t="inlineStr">
+      <c r="AS129" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -19030,9 +19788,15 @@
       <c r="AR130" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AS130" t="inlineStr">
-        <is>
-          <t>2789</t>
+      <c r="AS130" t="n">
+        <v>2789</v>
+      </c>
+      <c r="AT130" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU130" t="inlineStr">
+        <is>
+          <t>2842</t>
         </is>
       </c>
     </row>
@@ -19175,7 +19939,13 @@
       <c r="AR131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS131" t="inlineStr">
+      <c r="AS131" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -19320,9 +20090,15 @@
       <c r="AR132" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AS132" t="inlineStr">
-        <is>
-          <t>2528</t>
+      <c r="AS132" t="n">
+        <v>2528</v>
+      </c>
+      <c r="AT132" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU132" t="inlineStr">
+        <is>
+          <t>2557</t>
         </is>
       </c>
     </row>
@@ -19465,9 +20241,15 @@
       <c r="AR133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS133" t="inlineStr">
-        <is>
-          <t>2597</t>
+      <c r="AS133" t="n">
+        <v>2597</v>
+      </c>
+      <c r="AT133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU133" t="inlineStr">
+        <is>
+          <t>2701</t>
         </is>
       </c>
     </row>
@@ -19553,6 +20335,8 @@
       <c r="AQ134" t="inlineStr"/>
       <c r="AR134" s="3" t="inlineStr"/>
       <c r="AS134" t="inlineStr"/>
+      <c r="AT134" s="3" t="inlineStr"/>
+      <c r="AU134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -19628,6 +20412,8 @@
       <c r="AQ135" t="inlineStr"/>
       <c r="AR135" s="3" t="inlineStr"/>
       <c r="AS135" t="inlineStr"/>
+      <c r="AT135" s="3" t="inlineStr"/>
+      <c r="AU135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -19768,7 +20554,13 @@
       <c r="AR136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS136" t="inlineStr">
+      <c r="AS136" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU136" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -19913,7 +20705,13 @@
       <c r="AR137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS137" t="inlineStr">
+      <c r="AS137" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -19993,6 +20791,8 @@
       <c r="AQ138" t="inlineStr"/>
       <c r="AR138" s="3" t="inlineStr"/>
       <c r="AS138" t="inlineStr"/>
+      <c r="AT138" s="3" t="inlineStr"/>
+      <c r="AU138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -20133,9 +20933,15 @@
       <c r="AR139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS139" t="inlineStr">
-        <is>
-          <t>2036</t>
+      <c r="AS139" t="n">
+        <v>2036</v>
+      </c>
+      <c r="AT139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU139" t="inlineStr">
+        <is>
+          <t>2029</t>
         </is>
       </c>
     </row>
@@ -20278,9 +21084,15 @@
       <c r="AR140" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AS140" t="inlineStr">
-        <is>
-          <t>2716</t>
+      <c r="AS140" t="n">
+        <v>2716</v>
+      </c>
+      <c r="AT140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU140" t="inlineStr">
+        <is>
+          <t>2671</t>
         </is>
       </c>
     </row>
@@ -20358,6 +21170,8 @@
       <c r="AQ141" t="inlineStr"/>
       <c r="AR141" s="3" t="inlineStr"/>
       <c r="AS141" t="inlineStr"/>
+      <c r="AT141" s="3" t="inlineStr"/>
+      <c r="AU141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -20498,7 +21312,13 @@
       <c r="AR142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS142" t="inlineStr">
+      <c r="AS142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU142" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -20578,6 +21398,8 @@
       <c r="AQ143" t="inlineStr"/>
       <c r="AR143" s="3" t="inlineStr"/>
       <c r="AS143" t="inlineStr"/>
+      <c r="AT143" s="3" t="inlineStr"/>
+      <c r="AU143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -20653,6 +21475,8 @@
       <c r="AQ144" t="inlineStr"/>
       <c r="AR144" s="3" t="inlineStr"/>
       <c r="AS144" t="inlineStr"/>
+      <c r="AT144" s="3" t="inlineStr"/>
+      <c r="AU144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -20728,6 +21552,8 @@
       <c r="AQ145" t="inlineStr"/>
       <c r="AR145" s="3" t="inlineStr"/>
       <c r="AS145" t="inlineStr"/>
+      <c r="AT145" s="3" t="inlineStr"/>
+      <c r="AU145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -20803,6 +21629,8 @@
       <c r="AQ146" t="inlineStr"/>
       <c r="AR146" s="3" t="inlineStr"/>
       <c r="AS146" t="inlineStr"/>
+      <c r="AT146" s="3" t="inlineStr"/>
+      <c r="AU146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -20878,6 +21706,8 @@
       <c r="AQ147" t="inlineStr"/>
       <c r="AR147" s="3" t="inlineStr"/>
       <c r="AS147" t="inlineStr"/>
+      <c r="AT147" s="3" t="inlineStr"/>
+      <c r="AU147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -21018,7 +21848,13 @@
       <c r="AR148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS148" t="inlineStr">
+      <c r="AS148" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -21163,9 +21999,15 @@
       <c r="AR149" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="AS149" t="inlineStr">
-        <is>
-          <t>3342</t>
+      <c r="AS149" t="n">
+        <v>3342</v>
+      </c>
+      <c r="AT149" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="AU149" t="inlineStr">
+        <is>
+          <t>3568</t>
         </is>
       </c>
     </row>
@@ -21308,7 +22150,13 @@
       <c r="AR150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS150" t="inlineStr">
+      <c r="AS150" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -21453,9 +22301,15 @@
       <c r="AR151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS151" t="inlineStr">
-        <is>
-          <t>2550</t>
+      <c r="AS151" t="n">
+        <v>2550</v>
+      </c>
+      <c r="AT151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU151" t="inlineStr">
+        <is>
+          <t>2578</t>
         </is>
       </c>
     </row>
@@ -21598,7 +22452,13 @@
       <c r="AR152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS152" t="inlineStr">
+      <c r="AS152" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -21743,7 +22603,13 @@
       <c r="AR153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS153" t="inlineStr">
+      <c r="AS153" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -21888,7 +22754,13 @@
       <c r="AR154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS154" t="inlineStr">
+      <c r="AS154" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -22033,9 +22905,15 @@
       <c r="AR155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS155" t="inlineStr">
-        <is>
-          <t>2614</t>
+      <c r="AS155" t="n">
+        <v>2614</v>
+      </c>
+      <c r="AT155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU155" t="inlineStr">
+        <is>
+          <t>2611</t>
         </is>
       </c>
     </row>
@@ -22172,9 +23050,15 @@
       <c r="AR156" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="AS156" t="inlineStr">
-        <is>
-          <t>3190</t>
+      <c r="AS156" t="n">
+        <v>3190</v>
+      </c>
+      <c r="AT156" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="AU156" t="inlineStr">
+        <is>
+          <t>3191</t>
         </is>
       </c>
     </row>
@@ -22246,6 +23130,8 @@
       <c r="AQ157" t="inlineStr"/>
       <c r="AR157" s="3" t="inlineStr"/>
       <c r="AS157" t="inlineStr"/>
+      <c r="AT157" s="3" t="inlineStr"/>
+      <c r="AU157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -22380,7 +23266,13 @@
       <c r="AR158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS158" t="inlineStr">
+      <c r="AS158" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -22519,9 +23411,15 @@
       <c r="AR159" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AS159" t="inlineStr">
-        <is>
-          <t>2821</t>
+      <c r="AS159" t="n">
+        <v>2821</v>
+      </c>
+      <c r="AT159" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU159" t="inlineStr">
+        <is>
+          <t>2888</t>
         </is>
       </c>
     </row>
@@ -22593,6 +23491,8 @@
       <c r="AQ160" t="inlineStr"/>
       <c r="AR160" s="3" t="inlineStr"/>
       <c r="AS160" t="inlineStr"/>
+      <c r="AT160" s="3" t="inlineStr"/>
+      <c r="AU160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -22715,9 +23615,15 @@
       <c r="AR161" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AS161" t="inlineStr">
-        <is>
-          <t>2988</t>
+      <c r="AS161" t="n">
+        <v>2988</v>
+      </c>
+      <c r="AT161" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="AU161" t="inlineStr">
+        <is>
+          <t>3004</t>
         </is>
       </c>
     </row>
@@ -22842,9 +23748,15 @@
       <c r="AR162" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AS162" t="inlineStr">
-        <is>
-          <t>2656</t>
+      <c r="AS162" t="n">
+        <v>2656</v>
+      </c>
+      <c r="AT162" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU162" t="inlineStr">
+        <is>
+          <t>2622</t>
         </is>
       </c>
     </row>
@@ -22965,9 +23877,15 @@
       <c r="AR163" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AS163" t="inlineStr">
-        <is>
-          <t>3219</t>
+      <c r="AS163" t="n">
+        <v>3219</v>
+      </c>
+      <c r="AT163" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU163" t="inlineStr">
+        <is>
+          <t>3318</t>
         </is>
       </c>
     </row>
@@ -23072,9 +23990,15 @@
       <c r="AR164" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AS164" t="inlineStr">
-        <is>
-          <t>3016</t>
+      <c r="AS164" t="n">
+        <v>3016</v>
+      </c>
+      <c r="AT164" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU164" t="inlineStr">
+        <is>
+          <t>3106</t>
         </is>
       </c>
     </row>
@@ -23183,9 +24107,15 @@
       <c r="AR165" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AS165" t="inlineStr">
-        <is>
-          <t>2759</t>
+      <c r="AS165" t="n">
+        <v>2759</v>
+      </c>
+      <c r="AT165" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AU165" t="inlineStr">
+        <is>
+          <t>2762</t>
         </is>
       </c>
     </row>
@@ -23286,9 +24216,15 @@
       <c r="AR166" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS166" t="inlineStr">
-        <is>
-          <t>2768</t>
+      <c r="AS166" t="n">
+        <v>2768</v>
+      </c>
+      <c r="AT166" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU166" t="inlineStr">
+        <is>
+          <t>2773</t>
         </is>
       </c>
     </row>
@@ -23377,7 +24313,13 @@
       <c r="AR167" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS167" t="inlineStr">
+      <c r="AS167" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT167" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU167" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -23464,9 +24406,15 @@
       <c r="AR168" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS168" t="inlineStr">
-        <is>
-          <t>1536</t>
+      <c r="AS168" t="n">
+        <v>1536</v>
+      </c>
+      <c r="AT168" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU168" t="inlineStr">
+        <is>
+          <t>1529</t>
         </is>
       </c>
     </row>
@@ -23530,6 +24478,8 @@
       <c r="AQ169" t="inlineStr"/>
       <c r="AR169" s="3" t="inlineStr"/>
       <c r="AS169" t="inlineStr"/>
+      <c r="AT169" s="3" t="inlineStr"/>
+      <c r="AU169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="n">
@@ -23608,7 +24558,13 @@
       <c r="AR170" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="AS170" t="inlineStr">
+      <c r="AS170" t="n">
+        <v>1517</v>
+      </c>
+      <c r="AT170" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU170" t="inlineStr">
         <is>
           <t>1517</t>
         </is>
@@ -23679,9 +24635,15 @@
       <c r="AR171" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS171" t="inlineStr">
-        <is>
-          <t>1647</t>
+      <c r="AS171" t="n">
+        <v>1647</v>
+      </c>
+      <c r="AT171" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="AU171" t="inlineStr">
+        <is>
+          <t>1736</t>
         </is>
       </c>
     </row>
@@ -23750,7 +24712,13 @@
       <c r="AR172" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS172" t="inlineStr">
+      <c r="AS172" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT172" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU172" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -23821,9 +24789,15 @@
       <c r="AR173" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="AS173" t="inlineStr">
-        <is>
-          <t>1758</t>
+      <c r="AS173" t="n">
+        <v>1758</v>
+      </c>
+      <c r="AT173" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AU173" t="inlineStr">
+        <is>
+          <t>1836</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-03-06 10:56:14
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AU173"/>
+  <dimension ref="A1:AW173"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -626,6 +626,16 @@
           <t>03-04_0</t>
         </is>
       </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>03-05_A</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>03-05_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -772,9 +782,15 @@
       <c r="AT2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU2" t="inlineStr">
-        <is>
-          <t>2659</t>
+      <c r="AU2" t="n">
+        <v>2659</v>
+      </c>
+      <c r="AV2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW2" t="inlineStr">
+        <is>
+          <t>2715</t>
         </is>
       </c>
     </row>
@@ -923,9 +939,15 @@
       <c r="AT3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AU3" t="inlineStr">
-        <is>
-          <t>4836</t>
+      <c r="AU3" t="n">
+        <v>4836</v>
+      </c>
+      <c r="AV3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW3" t="inlineStr">
+        <is>
+          <t>5155</t>
         </is>
       </c>
     </row>
@@ -1074,9 +1096,15 @@
       <c r="AT4" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AU4" t="inlineStr">
-        <is>
-          <t>4884</t>
+      <c r="AU4" t="n">
+        <v>4884</v>
+      </c>
+      <c r="AV4" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AW4" t="inlineStr">
+        <is>
+          <t>5108</t>
         </is>
       </c>
     </row>
@@ -1225,9 +1253,15 @@
       <c r="AT5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AU5" t="inlineStr">
-        <is>
-          <t>4492</t>
+      <c r="AU5" t="n">
+        <v>4492</v>
+      </c>
+      <c r="AV5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW5" t="inlineStr">
+        <is>
+          <t>4656</t>
         </is>
       </c>
     </row>
@@ -1376,9 +1410,15 @@
       <c r="AT6" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AU6" t="inlineStr">
-        <is>
-          <t>4637</t>
+      <c r="AU6" t="n">
+        <v>4637</v>
+      </c>
+      <c r="AV6" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AW6" t="inlineStr">
+        <is>
+          <t>4861</t>
         </is>
       </c>
     </row>
@@ -1527,9 +1567,15 @@
       <c r="AT7" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AU7" t="inlineStr">
-        <is>
-          <t>5089</t>
+      <c r="AU7" t="n">
+        <v>5089</v>
+      </c>
+      <c r="AV7" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AW7" t="inlineStr">
+        <is>
+          <t>5376</t>
         </is>
       </c>
     </row>
@@ -1678,9 +1724,15 @@
       <c r="AT8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AU8" t="inlineStr">
-        <is>
-          <t>4341</t>
+      <c r="AU8" t="n">
+        <v>4341</v>
+      </c>
+      <c r="AV8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW8" t="inlineStr">
+        <is>
+          <t>4569</t>
         </is>
       </c>
     </row>
@@ -1829,9 +1881,15 @@
       <c r="AT9" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="AU9" t="inlineStr">
-        <is>
-          <t>4440</t>
+      <c r="AU9" t="n">
+        <v>4440</v>
+      </c>
+      <c r="AV9" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AW9" t="inlineStr">
+        <is>
+          <t>4720</t>
         </is>
       </c>
     </row>
@@ -1980,9 +2038,15 @@
       <c r="AT10" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AU10" t="inlineStr">
-        <is>
-          <t>4566</t>
+      <c r="AU10" t="n">
+        <v>4566</v>
+      </c>
+      <c r="AV10" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AW10" t="inlineStr">
+        <is>
+          <t>4685</t>
         </is>
       </c>
     </row>
@@ -2131,9 +2195,15 @@
       <c r="AT11" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AU11" t="inlineStr">
-        <is>
-          <t>4102</t>
+      <c r="AU11" t="n">
+        <v>4102</v>
+      </c>
+      <c r="AV11" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW11" t="inlineStr">
+        <is>
+          <t>4280</t>
         </is>
       </c>
     </row>
@@ -2282,7 +2352,13 @@
       <c r="AT12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU12" t="inlineStr">
+      <c r="AU12" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AV12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW12" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2433,9 +2509,15 @@
       <c r="AT13" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="AU13" t="inlineStr">
-        <is>
-          <t>5145</t>
+      <c r="AU13" t="n">
+        <v>5145</v>
+      </c>
+      <c r="AV13" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="AW13" t="inlineStr">
+        <is>
+          <t>5464</t>
         </is>
       </c>
     </row>
@@ -2584,9 +2666,15 @@
       <c r="AT14" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AU14" t="inlineStr">
-        <is>
-          <t>4507</t>
+      <c r="AU14" t="n">
+        <v>4507</v>
+      </c>
+      <c r="AV14" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AW14" t="inlineStr">
+        <is>
+          <t>4731</t>
         </is>
       </c>
     </row>
@@ -2735,7 +2823,13 @@
       <c r="AT15" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU15" t="inlineStr">
+      <c r="AU15" t="n">
+        <v>2539</v>
+      </c>
+      <c r="AV15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW15" t="inlineStr">
         <is>
           <t>2539</t>
         </is>
@@ -2886,9 +2980,15 @@
       <c r="AT16" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AU16" t="inlineStr">
-        <is>
-          <t>4692</t>
+      <c r="AU16" t="n">
+        <v>4692</v>
+      </c>
+      <c r="AV16" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AW16" t="inlineStr">
+        <is>
+          <t>4875</t>
         </is>
       </c>
     </row>
@@ -3037,9 +3137,15 @@
       <c r="AT17" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AU17" t="inlineStr">
-        <is>
-          <t>3896</t>
+      <c r="AU17" t="n">
+        <v>3896</v>
+      </c>
+      <c r="AV17" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AW17" t="inlineStr">
+        <is>
+          <t>3908</t>
         </is>
       </c>
     </row>
@@ -3188,9 +3294,15 @@
       <c r="AT18" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AU18" t="inlineStr">
-        <is>
-          <t>3942</t>
+      <c r="AU18" t="n">
+        <v>3942</v>
+      </c>
+      <c r="AV18" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="AW18" t="inlineStr">
+        <is>
+          <t>4258</t>
         </is>
       </c>
     </row>
@@ -3339,9 +3451,15 @@
       <c r="AT19" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AU19" t="inlineStr">
-        <is>
-          <t>4725</t>
+      <c r="AU19" t="n">
+        <v>4725</v>
+      </c>
+      <c r="AV19" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AW19" t="inlineStr">
+        <is>
+          <t>4990</t>
         </is>
       </c>
     </row>
@@ -3490,9 +3608,15 @@
       <c r="AT20" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AU20" t="inlineStr">
-        <is>
-          <t>5263</t>
+      <c r="AU20" t="n">
+        <v>5263</v>
+      </c>
+      <c r="AV20" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AW20" t="inlineStr">
+        <is>
+          <t>5593</t>
         </is>
       </c>
     </row>
@@ -3641,9 +3765,15 @@
       <c r="AT21" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AU21" t="inlineStr">
-        <is>
-          <t>3435</t>
+      <c r="AU21" t="n">
+        <v>3435</v>
+      </c>
+      <c r="AV21" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW21" t="inlineStr">
+        <is>
+          <t>3847</t>
         </is>
       </c>
     </row>
@@ -3792,9 +3922,15 @@
       <c r="AT22" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AU22" t="inlineStr">
-        <is>
-          <t>4581</t>
+      <c r="AU22" t="n">
+        <v>4581</v>
+      </c>
+      <c r="AV22" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AW22" t="inlineStr">
+        <is>
+          <t>4864</t>
         </is>
       </c>
     </row>
@@ -3943,9 +4079,15 @@
       <c r="AT23" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AU23" t="inlineStr">
-        <is>
-          <t>3790</t>
+      <c r="AU23" t="n">
+        <v>3790</v>
+      </c>
+      <c r="AV23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW23" t="inlineStr">
+        <is>
+          <t>3811</t>
         </is>
       </c>
     </row>
@@ -4094,9 +4236,15 @@
       <c r="AT24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AU24" t="inlineStr">
-        <is>
-          <t>4641</t>
+      <c r="AU24" t="n">
+        <v>4641</v>
+      </c>
+      <c r="AV24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AW24" t="inlineStr">
+        <is>
+          <t>4920</t>
         </is>
       </c>
     </row>
@@ -4245,7 +4393,13 @@
       <c r="AT25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU25" t="inlineStr">
+      <c r="AU25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4396,9 +4550,15 @@
       <c r="AT26" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AU26" t="inlineStr">
-        <is>
-          <t>4646</t>
+      <c r="AU26" t="n">
+        <v>4646</v>
+      </c>
+      <c r="AV26" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AW26" t="inlineStr">
+        <is>
+          <t>4866</t>
         </is>
       </c>
     </row>
@@ -4547,9 +4707,15 @@
       <c r="AT27" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AU27" t="inlineStr">
-        <is>
-          <t>4485</t>
+      <c r="AU27" t="n">
+        <v>4485</v>
+      </c>
+      <c r="AV27" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW27" t="inlineStr">
+        <is>
+          <t>4879</t>
         </is>
       </c>
     </row>
@@ -4698,9 +4864,15 @@
       <c r="AT28" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="AU28" t="inlineStr">
-        <is>
-          <t>3757</t>
+      <c r="AU28" t="n">
+        <v>3757</v>
+      </c>
+      <c r="AV28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="AW28" t="inlineStr">
+        <is>
+          <t>3970</t>
         </is>
       </c>
     </row>
@@ -4849,9 +5021,15 @@
       <c r="AT29" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AU29" t="inlineStr">
-        <is>
-          <t>5447</t>
+      <c r="AU29" t="n">
+        <v>5447</v>
+      </c>
+      <c r="AV29" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AW29" t="inlineStr">
+        <is>
+          <t>5683</t>
         </is>
       </c>
     </row>
@@ -5000,9 +5178,15 @@
       <c r="AT30" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AU30" t="inlineStr">
-        <is>
-          <t>4021</t>
+      <c r="AU30" t="n">
+        <v>4021</v>
+      </c>
+      <c r="AV30" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AW30" t="inlineStr">
+        <is>
+          <t>4408</t>
         </is>
       </c>
     </row>
@@ -5151,9 +5335,15 @@
       <c r="AT31" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AU31" t="inlineStr">
-        <is>
-          <t>4957</t>
+      <c r="AU31" t="n">
+        <v>4957</v>
+      </c>
+      <c r="AV31" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AW31" t="inlineStr">
+        <is>
+          <t>5287</t>
         </is>
       </c>
     </row>
@@ -5302,9 +5492,15 @@
       <c r="AT32" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="AU32" t="inlineStr">
-        <is>
-          <t>4990</t>
+      <c r="AU32" t="n">
+        <v>4990</v>
+      </c>
+      <c r="AV32" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="AW32" t="inlineStr">
+        <is>
+          <t>5334</t>
         </is>
       </c>
     </row>
@@ -5453,9 +5649,15 @@
       <c r="AT33" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AU33" t="inlineStr">
-        <is>
-          <t>4259</t>
+      <c r="AU33" t="n">
+        <v>4259</v>
+      </c>
+      <c r="AV33" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AW33" t="inlineStr">
+        <is>
+          <t>4536</t>
         </is>
       </c>
     </row>
@@ -5604,9 +5806,15 @@
       <c r="AT34" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AU34" t="inlineStr">
-        <is>
-          <t>4482</t>
+      <c r="AU34" t="n">
+        <v>4482</v>
+      </c>
+      <c r="AV34" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AW34" t="inlineStr">
+        <is>
+          <t>4579</t>
         </is>
       </c>
     </row>
@@ -5629,7 +5837,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F35" s="5" t="n">
@@ -5755,9 +5963,15 @@
       <c r="AT35" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AU35" t="inlineStr">
-        <is>
-          <t>4379</t>
+      <c r="AU35" t="n">
+        <v>4379</v>
+      </c>
+      <c r="AV35" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="AW35" t="inlineStr">
+        <is>
+          <t>4734</t>
         </is>
       </c>
     </row>
@@ -5906,9 +6120,15 @@
       <c r="AT36" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AU36" t="inlineStr">
-        <is>
-          <t>4567</t>
+      <c r="AU36" t="n">
+        <v>4567</v>
+      </c>
+      <c r="AV36" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW36" t="inlineStr">
+        <is>
+          <t>4777</t>
         </is>
       </c>
     </row>
@@ -6057,9 +6277,15 @@
       <c r="AT37" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AU37" t="inlineStr">
-        <is>
-          <t>3846</t>
+      <c r="AU37" t="n">
+        <v>3846</v>
+      </c>
+      <c r="AV37" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AW37" t="inlineStr">
+        <is>
+          <t>4047</t>
         </is>
       </c>
     </row>
@@ -6208,9 +6434,15 @@
       <c r="AT38" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AU38" t="inlineStr">
-        <is>
-          <t>4515</t>
+      <c r="AU38" t="n">
+        <v>4515</v>
+      </c>
+      <c r="AV38" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AW38" t="inlineStr">
+        <is>
+          <t>4703</t>
         </is>
       </c>
     </row>
@@ -6359,9 +6591,15 @@
       <c r="AT39" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AU39" t="inlineStr">
-        <is>
-          <t>4542</t>
+      <c r="AU39" t="n">
+        <v>4542</v>
+      </c>
+      <c r="AV39" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AW39" t="inlineStr">
+        <is>
+          <t>4756</t>
         </is>
       </c>
     </row>
@@ -6510,9 +6748,15 @@
       <c r="AT40" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AU40" t="inlineStr">
-        <is>
-          <t>4662</t>
+      <c r="AU40" t="n">
+        <v>4662</v>
+      </c>
+      <c r="AV40" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AW40" t="inlineStr">
+        <is>
+          <t>5014</t>
         </is>
       </c>
     </row>
@@ -6661,7 +6905,13 @@
       <c r="AT41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU41" t="inlineStr">
+      <c r="AU41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW41" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6812,9 +7062,15 @@
       <c r="AT42" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AU42" t="inlineStr">
-        <is>
-          <t>4868</t>
+      <c r="AU42" t="n">
+        <v>4868</v>
+      </c>
+      <c r="AV42" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AW42" t="inlineStr">
+        <is>
+          <t>5358</t>
         </is>
       </c>
     </row>
@@ -6837,7 +7093,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F43" s="5" t="n">
@@ -6963,9 +7219,15 @@
       <c r="AT43" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AU43" t="inlineStr">
-        <is>
-          <t>4763</t>
+      <c r="AU43" t="n">
+        <v>4763</v>
+      </c>
+      <c r="AV43" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AW43" t="inlineStr">
+        <is>
+          <t>4993</t>
         </is>
       </c>
     </row>
@@ -7114,9 +7376,15 @@
       <c r="AT44" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AU44" t="inlineStr">
-        <is>
-          <t>4654</t>
+      <c r="AU44" t="n">
+        <v>4654</v>
+      </c>
+      <c r="AV44" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AW44" t="inlineStr">
+        <is>
+          <t>4736</t>
         </is>
       </c>
     </row>
@@ -7265,9 +7533,15 @@
       <c r="AT45" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AU45" t="inlineStr">
-        <is>
-          <t>4111</t>
+      <c r="AU45" t="n">
+        <v>4111</v>
+      </c>
+      <c r="AV45" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AW45" t="inlineStr">
+        <is>
+          <t>4255</t>
         </is>
       </c>
     </row>
@@ -7416,9 +7690,15 @@
       <c r="AT46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AU46" t="inlineStr">
-        <is>
-          <t>4042</t>
+      <c r="AU46" t="n">
+        <v>4042</v>
+      </c>
+      <c r="AV46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AW46" t="inlineStr">
+        <is>
+          <t>4180</t>
         </is>
       </c>
     </row>
@@ -7567,9 +7847,15 @@
       <c r="AT47" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU47" t="inlineStr">
-        <is>
-          <t>3912</t>
+      <c r="AU47" t="n">
+        <v>3912</v>
+      </c>
+      <c r="AV47" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW47" t="inlineStr">
+        <is>
+          <t>3928</t>
         </is>
       </c>
     </row>
@@ -7718,9 +8004,15 @@
       <c r="AT48" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="AU48" t="inlineStr">
-        <is>
-          <t>4877</t>
+      <c r="AU48" t="n">
+        <v>4877</v>
+      </c>
+      <c r="AV48" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AW48" t="inlineStr">
+        <is>
+          <t>5142</t>
         </is>
       </c>
     </row>
@@ -7869,9 +8161,15 @@
       <c r="AT49" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AU49" t="inlineStr">
-        <is>
-          <t>3496</t>
+      <c r="AU49" t="n">
+        <v>3496</v>
+      </c>
+      <c r="AV49" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW49" t="inlineStr">
+        <is>
+          <t>3622</t>
         </is>
       </c>
     </row>
@@ -8020,9 +8318,15 @@
       <c r="AT50" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AU50" t="inlineStr">
-        <is>
-          <t>4880</t>
+      <c r="AU50" t="n">
+        <v>4880</v>
+      </c>
+      <c r="AV50" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AW50" t="inlineStr">
+        <is>
+          <t>5133</t>
         </is>
       </c>
     </row>
@@ -8171,9 +8475,15 @@
       <c r="AT51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU51" t="inlineStr">
-        <is>
-          <t>2546</t>
+      <c r="AU51" t="n">
+        <v>2546</v>
+      </c>
+      <c r="AV51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW51" t="inlineStr">
+        <is>
+          <t>2599</t>
         </is>
       </c>
     </row>
@@ -8322,9 +8632,15 @@
       <c r="AT52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU52" t="inlineStr">
-        <is>
-          <t>2548</t>
+      <c r="AU52" t="n">
+        <v>2548</v>
+      </c>
+      <c r="AV52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW52" t="inlineStr">
+        <is>
+          <t>2607</t>
         </is>
       </c>
     </row>
@@ -8473,9 +8789,15 @@
       <c r="AT53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU53" t="inlineStr">
-        <is>
-          <t>3062</t>
+      <c r="AU53" t="n">
+        <v>3062</v>
+      </c>
+      <c r="AV53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW53" t="inlineStr">
+        <is>
+          <t>3143</t>
         </is>
       </c>
     </row>
@@ -8624,9 +8946,15 @@
       <c r="AT54" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="AU54" t="inlineStr">
-        <is>
-          <t>4615</t>
+      <c r="AU54" t="n">
+        <v>4615</v>
+      </c>
+      <c r="AV54" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AW54" t="inlineStr">
+        <is>
+          <t>4865</t>
         </is>
       </c>
     </row>
@@ -8775,9 +9103,15 @@
       <c r="AT55" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="AU55" t="inlineStr">
-        <is>
-          <t>3748</t>
+      <c r="AU55" t="n">
+        <v>3748</v>
+      </c>
+      <c r="AV55" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AW55" t="inlineStr">
+        <is>
+          <t>3818</t>
         </is>
       </c>
     </row>
@@ -8926,9 +9260,15 @@
       <c r="AT56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AU56" t="inlineStr">
-        <is>
-          <t>3671</t>
+      <c r="AU56" t="n">
+        <v>3671</v>
+      </c>
+      <c r="AV56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW56" t="inlineStr">
+        <is>
+          <t>3887</t>
         </is>
       </c>
     </row>
@@ -9077,9 +9417,15 @@
       <c r="AT57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AU57" t="inlineStr">
-        <is>
-          <t>4333</t>
+      <c r="AU57" t="n">
+        <v>4333</v>
+      </c>
+      <c r="AV57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW57" t="inlineStr">
+        <is>
+          <t>4678</t>
         </is>
       </c>
     </row>
@@ -9228,9 +9574,15 @@
       <c r="AT58" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AU58" t="inlineStr">
-        <is>
-          <t>3806</t>
+      <c r="AU58" t="n">
+        <v>3806</v>
+      </c>
+      <c r="AV58" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AW58" t="inlineStr">
+        <is>
+          <t>3949</t>
         </is>
       </c>
     </row>
@@ -9294,6 +9646,8 @@
       <c r="AS59" t="inlineStr"/>
       <c r="AT59" s="3" t="inlineStr"/>
       <c r="AU59" t="inlineStr"/>
+      <c r="AV59" s="3" t="inlineStr"/>
+      <c r="AW59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -9355,6 +9709,8 @@
       <c r="AS60" t="inlineStr"/>
       <c r="AT60" s="3" t="inlineStr"/>
       <c r="AU60" t="inlineStr"/>
+      <c r="AV60" s="3" t="inlineStr"/>
+      <c r="AW60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -9501,9 +9857,15 @@
       <c r="AT61" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AU61" t="inlineStr">
-        <is>
-          <t>4231</t>
+      <c r="AU61" t="n">
+        <v>4231</v>
+      </c>
+      <c r="AV61" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AW61" t="inlineStr">
+        <is>
+          <t>4382</t>
         </is>
       </c>
     </row>
@@ -9652,7 +10014,13 @@
       <c r="AT62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU62" t="inlineStr">
+      <c r="AU62" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9803,9 +10171,15 @@
       <c r="AT63" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AU63" t="inlineStr">
-        <is>
-          <t>4367</t>
+      <c r="AU63" t="n">
+        <v>4367</v>
+      </c>
+      <c r="AV63" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AW63" t="inlineStr">
+        <is>
+          <t>4657</t>
         </is>
       </c>
     </row>
@@ -9954,9 +10328,15 @@
       <c r="AT64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU64" t="inlineStr">
-        <is>
-          <t>2669</t>
+      <c r="AU64" t="n">
+        <v>2669</v>
+      </c>
+      <c r="AV64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW64" t="inlineStr">
+        <is>
+          <t>2685</t>
         </is>
       </c>
     </row>
@@ -10020,6 +10400,8 @@
       <c r="AS65" t="inlineStr"/>
       <c r="AT65" s="3" t="inlineStr"/>
       <c r="AU65" t="inlineStr"/>
+      <c r="AV65" s="3" t="inlineStr"/>
+      <c r="AW65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -10166,9 +10548,15 @@
       <c r="AT66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU66" t="inlineStr">
-        <is>
-          <t>2570</t>
+      <c r="AU66" t="n">
+        <v>2570</v>
+      </c>
+      <c r="AV66" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AW66" t="inlineStr">
+        <is>
+          <t>2604</t>
         </is>
       </c>
     </row>
@@ -10317,9 +10705,15 @@
       <c r="AT67" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AU67" t="inlineStr">
-        <is>
-          <t>4231</t>
+      <c r="AU67" t="n">
+        <v>4231</v>
+      </c>
+      <c r="AV67" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AW67" t="inlineStr">
+        <is>
+          <t>4449</t>
         </is>
       </c>
     </row>
@@ -10468,9 +10862,15 @@
       <c r="AT68" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AU68" t="inlineStr">
-        <is>
-          <t>4186</t>
+      <c r="AU68" t="n">
+        <v>4186</v>
+      </c>
+      <c r="AV68" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AW68" t="inlineStr">
+        <is>
+          <t>4337</t>
         </is>
       </c>
     </row>
@@ -10619,9 +11019,15 @@
       <c r="AT69" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AU69" t="inlineStr">
-        <is>
-          <t>3793</t>
+      <c r="AU69" t="n">
+        <v>3793</v>
+      </c>
+      <c r="AV69" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AW69" t="inlineStr">
+        <is>
+          <t>3959</t>
         </is>
       </c>
     </row>
@@ -10770,9 +11176,15 @@
       <c r="AT70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU70" t="inlineStr">
-        <is>
-          <t>2551</t>
+      <c r="AU70" t="n">
+        <v>2551</v>
+      </c>
+      <c r="AV70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW70" t="inlineStr">
+        <is>
+          <t>2581</t>
         </is>
       </c>
     </row>
@@ -10921,9 +11333,15 @@
       <c r="AT71" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AU71" t="inlineStr">
-        <is>
-          <t>3880</t>
+      <c r="AU71" t="n">
+        <v>3880</v>
+      </c>
+      <c r="AV71" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AW71" t="inlineStr">
+        <is>
+          <t>4173</t>
         </is>
       </c>
     </row>
@@ -11072,9 +11490,15 @@
       <c r="AT72" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="AU72" t="inlineStr">
-        <is>
-          <t>3292</t>
+      <c r="AU72" t="n">
+        <v>3292</v>
+      </c>
+      <c r="AV72" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="AW72" t="inlineStr">
+        <is>
+          <t>3427</t>
         </is>
       </c>
     </row>
@@ -11223,9 +11647,15 @@
       <c r="AT73" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AU73" t="inlineStr">
-        <is>
-          <t>3790</t>
+      <c r="AU73" t="n">
+        <v>3790</v>
+      </c>
+      <c r="AV73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW73" t="inlineStr">
+        <is>
+          <t>3958</t>
         </is>
       </c>
     </row>
@@ -11374,9 +11804,15 @@
       <c r="AT74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU74" t="inlineStr">
-        <is>
-          <t>2796</t>
+      <c r="AU74" t="n">
+        <v>2796</v>
+      </c>
+      <c r="AV74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW74" t="inlineStr">
+        <is>
+          <t>2925</t>
         </is>
       </c>
     </row>
@@ -11525,9 +11961,15 @@
       <c r="AT75" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AU75" t="inlineStr">
-        <is>
-          <t>3572</t>
+      <c r="AU75" t="n">
+        <v>3572</v>
+      </c>
+      <c r="AV75" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AW75" t="inlineStr">
+        <is>
+          <t>3659</t>
         </is>
       </c>
     </row>
@@ -11676,9 +12118,15 @@
       <c r="AT76" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AU76" t="inlineStr">
-        <is>
-          <t>4279</t>
+      <c r="AU76" t="n">
+        <v>4279</v>
+      </c>
+      <c r="AV76" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AW76" t="inlineStr">
+        <is>
+          <t>4548</t>
         </is>
       </c>
     </row>
@@ -11827,7 +12275,13 @@
       <c r="AT77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU77" t="inlineStr">
+      <c r="AU77" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW77" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11978,9 +12432,15 @@
       <c r="AT78" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AU78" t="inlineStr">
-        <is>
-          <t>4294</t>
+      <c r="AU78" t="n">
+        <v>4294</v>
+      </c>
+      <c r="AV78" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AW78" t="inlineStr">
+        <is>
+          <t>4369</t>
         </is>
       </c>
     </row>
@@ -12129,7 +12589,13 @@
       <c r="AT79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU79" t="inlineStr">
+      <c r="AU79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12280,9 +12746,15 @@
       <c r="AT80" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="AU80" t="inlineStr">
-        <is>
-          <t>4125</t>
+      <c r="AU80" t="n">
+        <v>4125</v>
+      </c>
+      <c r="AV80" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="AW80" t="inlineStr">
+        <is>
+          <t>4271</t>
         </is>
       </c>
     </row>
@@ -12431,9 +12903,15 @@
       <c r="AT81" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AU81" t="inlineStr">
-        <is>
-          <t>4224</t>
+      <c r="AU81" t="n">
+        <v>4224</v>
+      </c>
+      <c r="AV81" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AW81" t="inlineStr">
+        <is>
+          <t>4339</t>
         </is>
       </c>
     </row>
@@ -12582,9 +13060,15 @@
       <c r="AT82" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="AU82" t="inlineStr">
-        <is>
-          <t>3980</t>
+      <c r="AU82" t="n">
+        <v>3980</v>
+      </c>
+      <c r="AV82" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AW82" t="inlineStr">
+        <is>
+          <t>4219</t>
         </is>
       </c>
     </row>
@@ -12733,9 +13217,15 @@
       <c r="AT83" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AU83" t="inlineStr">
-        <is>
-          <t>3822</t>
+      <c r="AU83" t="n">
+        <v>3822</v>
+      </c>
+      <c r="AV83" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AW83" t="inlineStr">
+        <is>
+          <t>3943</t>
         </is>
       </c>
     </row>
@@ -12859,6 +13349,8 @@
       <c r="AS84" t="inlineStr"/>
       <c r="AT84" s="3" t="inlineStr"/>
       <c r="AU84" t="inlineStr"/>
+      <c r="AV84" s="3" t="inlineStr"/>
+      <c r="AW84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -13005,9 +13497,15 @@
       <c r="AT85" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="AU85" t="inlineStr">
-        <is>
-          <t>3346</t>
+      <c r="AU85" t="n">
+        <v>3346</v>
+      </c>
+      <c r="AV85" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW85" t="inlineStr">
+        <is>
+          <t>3519</t>
         </is>
       </c>
     </row>
@@ -13156,9 +13654,15 @@
       <c r="AT86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU86" t="inlineStr">
-        <is>
-          <t>2657</t>
+      <c r="AU86" t="n">
+        <v>2657</v>
+      </c>
+      <c r="AV86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW86" t="inlineStr">
+        <is>
+          <t>2688</t>
         </is>
       </c>
     </row>
@@ -13307,9 +13811,15 @@
       <c r="AT87" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AU87" t="inlineStr">
-        <is>
-          <t>4007</t>
+      <c r="AU87" t="n">
+        <v>4007</v>
+      </c>
+      <c r="AV87" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AW87" t="inlineStr">
+        <is>
+          <t>3947</t>
         </is>
       </c>
     </row>
@@ -13458,9 +13968,15 @@
       <c r="AT88" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="AU88" t="inlineStr">
-        <is>
-          <t>2604</t>
+      <c r="AU88" t="n">
+        <v>2604</v>
+      </c>
+      <c r="AV88" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW88" t="inlineStr">
+        <is>
+          <t>2628</t>
         </is>
       </c>
     </row>
@@ -13609,9 +14125,15 @@
       <c r="AT89" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AU89" t="inlineStr">
-        <is>
-          <t>3018</t>
+      <c r="AU89" t="n">
+        <v>3018</v>
+      </c>
+      <c r="AV89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW89" t="inlineStr">
+        <is>
+          <t>2991</t>
         </is>
       </c>
     </row>
@@ -13760,9 +14282,15 @@
       <c r="AT90" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AU90" t="inlineStr">
-        <is>
-          <t>2670</t>
+      <c r="AU90" t="n">
+        <v>2670</v>
+      </c>
+      <c r="AV90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW90" t="inlineStr">
+        <is>
+          <t>2618</t>
         </is>
       </c>
     </row>
@@ -13911,9 +14439,15 @@
       <c r="AT91" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AU91" t="inlineStr">
-        <is>
-          <t>2731</t>
+      <c r="AU91" t="n">
+        <v>2731</v>
+      </c>
+      <c r="AV91" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW91" t="inlineStr">
+        <is>
+          <t>2711</t>
         </is>
       </c>
     </row>
@@ -14062,7 +14596,13 @@
       <c r="AT92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU92" t="inlineStr">
+      <c r="AU92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14213,9 +14753,15 @@
       <c r="AT93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU93" t="inlineStr">
-        <is>
-          <t>2305</t>
+      <c r="AU93" t="n">
+        <v>2305</v>
+      </c>
+      <c r="AV93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW93" t="inlineStr">
+        <is>
+          <t>2290</t>
         </is>
       </c>
     </row>
@@ -14364,9 +14910,15 @@
       <c r="AT94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU94" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="AU94" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AV94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW94" t="inlineStr">
+        <is>
+          <t>2540</t>
         </is>
       </c>
     </row>
@@ -14515,9 +15067,15 @@
       <c r="AT95" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="AU95" t="inlineStr">
-        <is>
-          <t>2530</t>
+      <c r="AU95" t="n">
+        <v>2530</v>
+      </c>
+      <c r="AV95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW95" t="inlineStr">
+        <is>
+          <t>2496</t>
         </is>
       </c>
     </row>
@@ -14666,9 +15224,15 @@
       <c r="AT96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU96" t="inlineStr">
-        <is>
-          <t>2488</t>
+      <c r="AU96" t="n">
+        <v>2488</v>
+      </c>
+      <c r="AV96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW96" t="inlineStr">
+        <is>
+          <t>2482</t>
         </is>
       </c>
     </row>
@@ -14817,9 +15381,15 @@
       <c r="AT97" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="AU97" t="inlineStr">
-        <is>
-          <t>2932</t>
+      <c r="AU97" t="n">
+        <v>2932</v>
+      </c>
+      <c r="AV97" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AW97" t="inlineStr">
+        <is>
+          <t>3008</t>
         </is>
       </c>
     </row>
@@ -14968,7 +15538,13 @@
       <c r="AT98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU98" t="inlineStr">
+      <c r="AU98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15119,9 +15695,15 @@
       <c r="AT99" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="AU99" t="inlineStr">
-        <is>
-          <t>3382</t>
+      <c r="AU99" t="n">
+        <v>3382</v>
+      </c>
+      <c r="AV99" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="AW99" t="inlineStr">
+        <is>
+          <t>3455</t>
         </is>
       </c>
     </row>
@@ -15270,9 +15852,15 @@
       <c r="AT100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU100" t="inlineStr">
-        <is>
-          <t>2403</t>
+      <c r="AU100" t="n">
+        <v>2403</v>
+      </c>
+      <c r="AV100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW100" t="inlineStr">
+        <is>
+          <t>2365</t>
         </is>
       </c>
     </row>
@@ -15421,9 +16009,15 @@
       <c r="AT101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AU101" t="inlineStr">
-        <is>
-          <t>3932</t>
+      <c r="AU101" t="n">
+        <v>3932</v>
+      </c>
+      <c r="AV101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AW101" t="inlineStr">
+        <is>
+          <t>4090</t>
         </is>
       </c>
     </row>
@@ -15572,9 +16166,15 @@
       <c r="AT102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AU102" t="inlineStr">
-        <is>
-          <t>3572</t>
+      <c r="AU102" t="n">
+        <v>3572</v>
+      </c>
+      <c r="AV102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW102" t="inlineStr">
+        <is>
+          <t>3733</t>
         </is>
       </c>
     </row>
@@ -15723,9 +16323,15 @@
       <c r="AT103" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AU103" t="inlineStr">
-        <is>
-          <t>3110</t>
+      <c r="AU103" t="n">
+        <v>3110</v>
+      </c>
+      <c r="AV103" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW103" t="inlineStr">
+        <is>
+          <t>3365</t>
         </is>
       </c>
     </row>
@@ -15874,9 +16480,15 @@
       <c r="AT104" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AU104" t="inlineStr">
-        <is>
-          <t>4007</t>
+      <c r="AU104" t="n">
+        <v>4007</v>
+      </c>
+      <c r="AV104" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AW104" t="inlineStr">
+        <is>
+          <t>4146</t>
         </is>
       </c>
     </row>
@@ -16025,9 +16637,15 @@
       <c r="AT105" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="AU105" t="inlineStr">
-        <is>
-          <t>3638</t>
+      <c r="AU105" t="n">
+        <v>3638</v>
+      </c>
+      <c r="AV105" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AW105" t="inlineStr">
+        <is>
+          <t>3763</t>
         </is>
       </c>
     </row>
@@ -16176,7 +16794,13 @@
       <c r="AT106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU106" t="inlineStr">
+      <c r="AU106" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16327,9 +16951,15 @@
       <c r="AT107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU107" t="inlineStr">
-        <is>
-          <t>2519</t>
+      <c r="AU107" t="n">
+        <v>2519</v>
+      </c>
+      <c r="AV107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW107" t="inlineStr">
+        <is>
+          <t>2510</t>
         </is>
       </c>
     </row>
@@ -16478,7 +17108,13 @@
       <c r="AT108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU108" t="inlineStr">
+      <c r="AU108" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16629,9 +17265,15 @@
       <c r="AT109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU109" t="inlineStr">
-        <is>
-          <t>3416</t>
+      <c r="AU109" t="n">
+        <v>3416</v>
+      </c>
+      <c r="AV109" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW109" t="inlineStr">
+        <is>
+          <t>3613</t>
         </is>
       </c>
     </row>
@@ -16780,9 +17422,15 @@
       <c r="AT110" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="AU110" t="inlineStr">
-        <is>
-          <t>3264</t>
+      <c r="AU110" t="n">
+        <v>3264</v>
+      </c>
+      <c r="AV110" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AW110" t="inlineStr">
+        <is>
+          <t>3369</t>
         </is>
       </c>
     </row>
@@ -16930,6 +17578,8 @@
       </c>
       <c r="AT111" s="3" t="inlineStr"/>
       <c r="AU111" t="inlineStr"/>
+      <c r="AV111" s="3" t="inlineStr"/>
+      <c r="AW111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -17076,9 +17726,15 @@
       <c r="AT112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU112" t="inlineStr">
-        <is>
-          <t>2571</t>
+      <c r="AU112" t="n">
+        <v>2571</v>
+      </c>
+      <c r="AV112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW112" t="inlineStr">
+        <is>
+          <t>2565</t>
         </is>
       </c>
     </row>
@@ -17227,9 +17883,15 @@
       <c r="AT113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU113" t="inlineStr">
-        <is>
-          <t>3169</t>
+      <c r="AU113" t="n">
+        <v>3169</v>
+      </c>
+      <c r="AV113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW113" t="inlineStr">
+        <is>
+          <t>3320</t>
         </is>
       </c>
     </row>
@@ -17378,9 +18040,15 @@
       <c r="AT114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU114" t="inlineStr">
-        <is>
-          <t>3349</t>
+      <c r="AU114" t="n">
+        <v>3349</v>
+      </c>
+      <c r="AV114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW114" t="inlineStr">
+        <is>
+          <t>3439</t>
         </is>
       </c>
     </row>
@@ -17529,9 +18197,15 @@
       <c r="AT115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU115" t="inlineStr">
-        <is>
-          <t>2006</t>
+      <c r="AU115" t="n">
+        <v>2006</v>
+      </c>
+      <c r="AV115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW115" t="inlineStr">
+        <is>
+          <t>2021</t>
         </is>
       </c>
     </row>
@@ -17680,9 +18354,15 @@
       <c r="AT116" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AU116" t="inlineStr">
-        <is>
-          <t>2928</t>
+      <c r="AU116" t="n">
+        <v>2928</v>
+      </c>
+      <c r="AV116" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="AW116" t="inlineStr">
+        <is>
+          <t>2948</t>
         </is>
       </c>
     </row>
@@ -17831,9 +18511,15 @@
       <c r="AT117" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AU117" t="inlineStr">
-        <is>
-          <t>3346</t>
+      <c r="AU117" t="n">
+        <v>3346</v>
+      </c>
+      <c r="AV117" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AW117" t="inlineStr">
+        <is>
+          <t>3275</t>
         </is>
       </c>
     </row>
@@ -17982,7 +18668,13 @@
       <c r="AT118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU118" t="inlineStr">
+      <c r="AU118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18133,9 +18825,15 @@
       <c r="AT119" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AU119" t="inlineStr">
-        <is>
-          <t>3675</t>
+      <c r="AU119" t="n">
+        <v>3675</v>
+      </c>
+      <c r="AV119" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AW119" t="inlineStr">
+        <is>
+          <t>3668</t>
         </is>
       </c>
     </row>
@@ -18284,9 +18982,15 @@
       <c r="AT120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU120" t="inlineStr">
-        <is>
-          <t>2463</t>
+      <c r="AU120" t="n">
+        <v>2463</v>
+      </c>
+      <c r="AV120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW120" t="inlineStr">
+        <is>
+          <t>2466</t>
         </is>
       </c>
     </row>
@@ -18435,9 +19139,15 @@
       <c r="AT121" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AU121" t="inlineStr">
-        <is>
-          <t>2987</t>
+      <c r="AU121" t="n">
+        <v>2987</v>
+      </c>
+      <c r="AV121" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AW121" t="inlineStr">
+        <is>
+          <t>3063</t>
         </is>
       </c>
     </row>
@@ -18586,7 +19296,13 @@
       <c r="AT122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU122" t="inlineStr">
+      <c r="AU122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18737,9 +19453,15 @@
       <c r="AT123" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AU123" t="inlineStr">
-        <is>
-          <t>3026</t>
+      <c r="AU123" t="n">
+        <v>3026</v>
+      </c>
+      <c r="AV123" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW123" t="inlineStr">
+        <is>
+          <t>3126</t>
         </is>
       </c>
     </row>
@@ -18888,9 +19610,15 @@
       <c r="AT124" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="AU124" t="inlineStr">
-        <is>
-          <t>2985</t>
+      <c r="AU124" t="n">
+        <v>2985</v>
+      </c>
+      <c r="AV124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW124" t="inlineStr">
+        <is>
+          <t>3062</t>
         </is>
       </c>
     </row>
@@ -19039,9 +19767,15 @@
       <c r="AT125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU125" t="inlineStr">
-        <is>
-          <t>2914</t>
+      <c r="AU125" t="n">
+        <v>2914</v>
+      </c>
+      <c r="AV125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW125" t="inlineStr">
+        <is>
+          <t>2919</t>
         </is>
       </c>
     </row>
@@ -19190,9 +19924,15 @@
       <c r="AT126" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="AU126" t="inlineStr">
-        <is>
-          <t>3068</t>
+      <c r="AU126" t="n">
+        <v>3068</v>
+      </c>
+      <c r="AV126" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AW126" t="inlineStr">
+        <is>
+          <t>3115</t>
         </is>
       </c>
     </row>
@@ -19341,9 +20081,15 @@
       <c r="AT127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU127" t="inlineStr">
-        <is>
-          <t>2322</t>
+      <c r="AU127" t="n">
+        <v>2322</v>
+      </c>
+      <c r="AV127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW127" t="inlineStr">
+        <is>
+          <t>2307</t>
         </is>
       </c>
     </row>
@@ -19492,7 +20238,13 @@
       <c r="AT128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU128" t="inlineStr">
+      <c r="AU128" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -19643,7 +20395,13 @@
       <c r="AT129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU129" t="inlineStr">
+      <c r="AU129" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -19794,9 +20552,15 @@
       <c r="AT130" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AU130" t="inlineStr">
-        <is>
-          <t>2842</t>
+      <c r="AU130" t="n">
+        <v>2842</v>
+      </c>
+      <c r="AV130" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AW130" t="inlineStr">
+        <is>
+          <t>2847</t>
         </is>
       </c>
     </row>
@@ -19945,7 +20709,13 @@
       <c r="AT131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU131" t="inlineStr">
+      <c r="AU131" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -20096,9 +20866,15 @@
       <c r="AT132" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AU132" t="inlineStr">
-        <is>
-          <t>2557</t>
+      <c r="AU132" t="n">
+        <v>2557</v>
+      </c>
+      <c r="AV132" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW132" t="inlineStr">
+        <is>
+          <t>2635</t>
         </is>
       </c>
     </row>
@@ -20247,9 +21023,15 @@
       <c r="AT133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU133" t="inlineStr">
-        <is>
-          <t>2701</t>
+      <c r="AU133" t="n">
+        <v>2701</v>
+      </c>
+      <c r="AV133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW133" t="inlineStr">
+        <is>
+          <t>2731</t>
         </is>
       </c>
     </row>
@@ -20337,6 +21119,8 @@
       <c r="AS134" t="inlineStr"/>
       <c r="AT134" s="3" t="inlineStr"/>
       <c r="AU134" t="inlineStr"/>
+      <c r="AV134" s="3" t="inlineStr"/>
+      <c r="AW134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -20414,6 +21198,8 @@
       <c r="AS135" t="inlineStr"/>
       <c r="AT135" s="3" t="inlineStr"/>
       <c r="AU135" t="inlineStr"/>
+      <c r="AV135" s="3" t="inlineStr"/>
+      <c r="AW135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -20560,7 +21346,13 @@
       <c r="AT136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU136" t="inlineStr">
+      <c r="AU136" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW136" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -20711,7 +21503,13 @@
       <c r="AT137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU137" t="inlineStr">
+      <c r="AU137" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -20793,6 +21591,8 @@
       <c r="AS138" t="inlineStr"/>
       <c r="AT138" s="3" t="inlineStr"/>
       <c r="AU138" t="inlineStr"/>
+      <c r="AV138" s="3" t="inlineStr"/>
+      <c r="AW138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -20939,9 +21739,15 @@
       <c r="AT139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU139" t="inlineStr">
-        <is>
-          <t>2029</t>
+      <c r="AU139" t="n">
+        <v>2029</v>
+      </c>
+      <c r="AV139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW139" t="inlineStr">
+        <is>
+          <t>2095</t>
         </is>
       </c>
     </row>
@@ -21090,9 +21896,15 @@
       <c r="AT140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU140" t="inlineStr">
-        <is>
-          <t>2671</t>
+      <c r="AU140" t="n">
+        <v>2671</v>
+      </c>
+      <c r="AV140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW140" t="inlineStr">
+        <is>
+          <t>2616</t>
         </is>
       </c>
     </row>
@@ -21172,6 +21984,8 @@
       <c r="AS141" t="inlineStr"/>
       <c r="AT141" s="3" t="inlineStr"/>
       <c r="AU141" t="inlineStr"/>
+      <c r="AV141" s="3" t="inlineStr"/>
+      <c r="AW141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -21318,7 +22132,13 @@
       <c r="AT142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU142" t="inlineStr">
+      <c r="AU142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW142" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -21400,6 +22220,8 @@
       <c r="AS143" t="inlineStr"/>
       <c r="AT143" s="3" t="inlineStr"/>
       <c r="AU143" t="inlineStr"/>
+      <c r="AV143" s="3" t="inlineStr"/>
+      <c r="AW143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -21477,6 +22299,8 @@
       <c r="AS144" t="inlineStr"/>
       <c r="AT144" s="3" t="inlineStr"/>
       <c r="AU144" t="inlineStr"/>
+      <c r="AV144" s="3" t="inlineStr"/>
+      <c r="AW144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -21554,6 +22378,8 @@
       <c r="AS145" t="inlineStr"/>
       <c r="AT145" s="3" t="inlineStr"/>
       <c r="AU145" t="inlineStr"/>
+      <c r="AV145" s="3" t="inlineStr"/>
+      <c r="AW145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -21631,6 +22457,8 @@
       <c r="AS146" t="inlineStr"/>
       <c r="AT146" s="3" t="inlineStr"/>
       <c r="AU146" t="inlineStr"/>
+      <c r="AV146" s="3" t="inlineStr"/>
+      <c r="AW146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -21708,6 +22536,8 @@
       <c r="AS147" t="inlineStr"/>
       <c r="AT147" s="3" t="inlineStr"/>
       <c r="AU147" t="inlineStr"/>
+      <c r="AV147" s="3" t="inlineStr"/>
+      <c r="AW147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -21854,7 +22684,13 @@
       <c r="AT148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU148" t="inlineStr">
+      <c r="AU148" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -22005,9 +22841,15 @@
       <c r="AT149" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="AU149" t="inlineStr">
-        <is>
-          <t>3568</t>
+      <c r="AU149" t="n">
+        <v>3568</v>
+      </c>
+      <c r="AV149" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AW149" t="inlineStr">
+        <is>
+          <t>3727</t>
         </is>
       </c>
     </row>
@@ -22156,7 +22998,13 @@
       <c r="AT150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU150" t="inlineStr">
+      <c r="AU150" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -22307,7 +23155,13 @@
       <c r="AT151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU151" t="inlineStr">
+      <c r="AU151" t="n">
+        <v>2578</v>
+      </c>
+      <c r="AV151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW151" t="inlineStr">
         <is>
           <t>2578</t>
         </is>
@@ -22458,7 +23312,13 @@
       <c r="AT152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU152" t="inlineStr">
+      <c r="AU152" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -22609,7 +23469,13 @@
       <c r="AT153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU153" t="inlineStr">
+      <c r="AU153" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -22760,7 +23626,13 @@
       <c r="AT154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU154" t="inlineStr">
+      <c r="AU154" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -22911,9 +23783,15 @@
       <c r="AT155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU155" t="inlineStr">
-        <is>
-          <t>2611</t>
+      <c r="AU155" t="n">
+        <v>2611</v>
+      </c>
+      <c r="AV155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW155" t="inlineStr">
+        <is>
+          <t>2687</t>
         </is>
       </c>
     </row>
@@ -23056,9 +23934,15 @@
       <c r="AT156" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="AU156" t="inlineStr">
-        <is>
-          <t>3191</t>
+      <c r="AU156" t="n">
+        <v>3191</v>
+      </c>
+      <c r="AV156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW156" t="inlineStr">
+        <is>
+          <t>3195</t>
         </is>
       </c>
     </row>
@@ -23132,6 +24016,8 @@
       <c r="AS157" t="inlineStr"/>
       <c r="AT157" s="3" t="inlineStr"/>
       <c r="AU157" t="inlineStr"/>
+      <c r="AV157" s="3" t="inlineStr"/>
+      <c r="AW157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -23272,7 +24158,13 @@
       <c r="AT158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU158" t="inlineStr">
+      <c r="AU158" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -23417,9 +24309,15 @@
       <c r="AT159" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AU159" t="inlineStr">
-        <is>
-          <t>2888</t>
+      <c r="AU159" t="n">
+        <v>2888</v>
+      </c>
+      <c r="AV159" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW159" t="inlineStr">
+        <is>
+          <t>2957</t>
         </is>
       </c>
     </row>
@@ -23493,6 +24391,8 @@
       <c r="AS160" t="inlineStr"/>
       <c r="AT160" s="3" t="inlineStr"/>
       <c r="AU160" t="inlineStr"/>
+      <c r="AV160" s="3" t="inlineStr"/>
+      <c r="AW160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -23621,9 +24521,15 @@
       <c r="AT161" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="AU161" t="inlineStr">
-        <is>
-          <t>3004</t>
+      <c r="AU161" t="n">
+        <v>3004</v>
+      </c>
+      <c r="AV161" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AW161" t="inlineStr">
+        <is>
+          <t>3096</t>
         </is>
       </c>
     </row>
@@ -23754,9 +24660,15 @@
       <c r="AT162" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU162" t="inlineStr">
-        <is>
-          <t>2622</t>
+      <c r="AU162" t="n">
+        <v>2622</v>
+      </c>
+      <c r="AV162" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="AW162" t="inlineStr">
+        <is>
+          <t>2617</t>
         </is>
       </c>
     </row>
@@ -23883,9 +24795,15 @@
       <c r="AT163" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AU163" t="inlineStr">
-        <is>
-          <t>3318</t>
+      <c r="AU163" t="n">
+        <v>3318</v>
+      </c>
+      <c r="AV163" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW163" t="inlineStr">
+        <is>
+          <t>3264</t>
         </is>
       </c>
     </row>
@@ -23996,9 +24914,15 @@
       <c r="AT164" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AU164" t="inlineStr">
-        <is>
-          <t>3106</t>
+      <c r="AU164" t="n">
+        <v>3106</v>
+      </c>
+      <c r="AV164" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW164" t="inlineStr">
+        <is>
+          <t>3274</t>
         </is>
       </c>
     </row>
@@ -24113,9 +25037,15 @@
       <c r="AT165" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AU165" t="inlineStr">
-        <is>
-          <t>2762</t>
+      <c r="AU165" t="n">
+        <v>2762</v>
+      </c>
+      <c r="AV165" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AW165" t="inlineStr">
+        <is>
+          <t>2730</t>
         </is>
       </c>
     </row>
@@ -24222,9 +25152,15 @@
       <c r="AT166" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU166" t="inlineStr">
-        <is>
-          <t>2773</t>
+      <c r="AU166" t="n">
+        <v>2773</v>
+      </c>
+      <c r="AV166" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW166" t="inlineStr">
+        <is>
+          <t>2774</t>
         </is>
       </c>
     </row>
@@ -24319,7 +25255,13 @@
       <c r="AT167" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU167" t="inlineStr">
+      <c r="AU167" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV167" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW167" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -24412,9 +25354,15 @@
       <c r="AT168" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU168" t="inlineStr">
-        <is>
-          <t>1529</t>
+      <c r="AU168" t="n">
+        <v>1529</v>
+      </c>
+      <c r="AV168" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW168" t="inlineStr">
+        <is>
+          <t>1521</t>
         </is>
       </c>
     </row>
@@ -24480,6 +25428,8 @@
       <c r="AS169" t="inlineStr"/>
       <c r="AT169" s="3" t="inlineStr"/>
       <c r="AU169" t="inlineStr"/>
+      <c r="AV169" s="3" t="inlineStr"/>
+      <c r="AW169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="n">
@@ -24564,9 +25514,15 @@
       <c r="AT170" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU170" t="inlineStr">
-        <is>
-          <t>1517</t>
+      <c r="AU170" t="n">
+        <v>1517</v>
+      </c>
+      <c r="AV170" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW170" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -24641,9 +25597,15 @@
       <c r="AT171" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="AU171" t="inlineStr">
-        <is>
-          <t>1736</t>
+      <c r="AU171" t="n">
+        <v>1736</v>
+      </c>
+      <c r="AV171" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW171" t="inlineStr">
+        <is>
+          <t>1737</t>
         </is>
       </c>
     </row>
@@ -24718,7 +25680,13 @@
       <c r="AT172" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU172" t="inlineStr">
+      <c r="AU172" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV172" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW172" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -24795,9 +25763,15 @@
       <c r="AT173" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="AU173" t="inlineStr">
-        <is>
-          <t>1836</t>
+      <c r="AU173" t="n">
+        <v>1836</v>
+      </c>
+      <c r="AV173" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AW173" t="inlineStr">
+        <is>
+          <t>1839</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-03-07 10:22:48
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AW173"/>
+  <dimension ref="A1:AY173"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -636,6 +636,16 @@
           <t>03-05_0</t>
         </is>
       </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>03-06_A</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>03-06_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -788,9 +798,15 @@
       <c r="AV2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW2" t="inlineStr">
-        <is>
-          <t>2715</t>
+      <c r="AW2" t="n">
+        <v>2715</v>
+      </c>
+      <c r="AX2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY2" t="inlineStr">
+        <is>
+          <t>2740</t>
         </is>
       </c>
     </row>
@@ -945,9 +961,15 @@
       <c r="AV3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AW3" t="inlineStr">
-        <is>
-          <t>5155</t>
+      <c r="AW3" t="n">
+        <v>5155</v>
+      </c>
+      <c r="AX3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AY3" t="inlineStr">
+        <is>
+          <t>5471</t>
         </is>
       </c>
     </row>
@@ -1102,9 +1124,15 @@
       <c r="AV4" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AW4" t="inlineStr">
-        <is>
-          <t>5108</t>
+      <c r="AW4" t="n">
+        <v>5108</v>
+      </c>
+      <c r="AX4" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AY4" t="inlineStr">
+        <is>
+          <t>5318</t>
         </is>
       </c>
     </row>
@@ -1259,9 +1287,15 @@
       <c r="AV5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AW5" t="inlineStr">
-        <is>
-          <t>4656</t>
+      <c r="AW5" t="n">
+        <v>4656</v>
+      </c>
+      <c r="AX5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AY5" t="inlineStr">
+        <is>
+          <t>4984</t>
         </is>
       </c>
     </row>
@@ -1416,9 +1450,15 @@
       <c r="AV6" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AW6" t="inlineStr">
-        <is>
-          <t>4861</t>
+      <c r="AW6" t="n">
+        <v>4861</v>
+      </c>
+      <c r="AX6" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AY6" t="inlineStr">
+        <is>
+          <t>5150</t>
         </is>
       </c>
     </row>
@@ -1441,7 +1481,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F7" s="5" t="n">
@@ -1573,9 +1613,15 @@
       <c r="AV7" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AW7" t="inlineStr">
-        <is>
-          <t>5376</t>
+      <c r="AW7" t="n">
+        <v>5376</v>
+      </c>
+      <c r="AX7" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AY7" t="inlineStr">
+        <is>
+          <t>5707</t>
         </is>
       </c>
     </row>
@@ -1730,9 +1776,15 @@
       <c r="AV8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AW8" t="inlineStr">
-        <is>
-          <t>4569</t>
+      <c r="AW8" t="n">
+        <v>4569</v>
+      </c>
+      <c r="AX8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AY8" t="inlineStr">
+        <is>
+          <t>4816</t>
         </is>
       </c>
     </row>
@@ -1887,9 +1939,15 @@
       <c r="AV9" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AW9" t="inlineStr">
-        <is>
-          <t>4720</t>
+      <c r="AW9" t="n">
+        <v>4720</v>
+      </c>
+      <c r="AX9" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AY9" t="inlineStr">
+        <is>
+          <t>4913</t>
         </is>
       </c>
     </row>
@@ -2044,9 +2102,15 @@
       <c r="AV10" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AW10" t="inlineStr">
-        <is>
-          <t>4685</t>
+      <c r="AW10" t="n">
+        <v>4685</v>
+      </c>
+      <c r="AX10" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AY10" t="inlineStr">
+        <is>
+          <t>4992</t>
         </is>
       </c>
     </row>
@@ -2201,9 +2265,15 @@
       <c r="AV11" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AW11" t="inlineStr">
-        <is>
-          <t>4280</t>
+      <c r="AW11" t="n">
+        <v>4280</v>
+      </c>
+      <c r="AX11" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AY11" t="inlineStr">
+        <is>
+          <t>4413</t>
         </is>
       </c>
     </row>
@@ -2358,9 +2428,15 @@
       <c r="AV12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW12" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="AW12" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AX12" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AY12" t="inlineStr">
+        <is>
+          <t>2592</t>
         </is>
       </c>
     </row>
@@ -2515,9 +2591,15 @@
       <c r="AV13" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="AW13" t="inlineStr">
-        <is>
-          <t>5464</t>
+      <c r="AW13" t="n">
+        <v>5464</v>
+      </c>
+      <c r="AX13" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AY13" t="inlineStr">
+        <is>
+          <t>5744</t>
         </is>
       </c>
     </row>
@@ -2672,9 +2754,15 @@
       <c r="AV14" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AW14" t="inlineStr">
-        <is>
-          <t>4731</t>
+      <c r="AW14" t="n">
+        <v>4731</v>
+      </c>
+      <c r="AX14" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="AY14" t="inlineStr">
+        <is>
+          <t>4946</t>
         </is>
       </c>
     </row>
@@ -2829,9 +2917,15 @@
       <c r="AV15" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW15" t="inlineStr">
-        <is>
-          <t>2539</t>
+      <c r="AW15" t="n">
+        <v>2539</v>
+      </c>
+      <c r="AX15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY15" t="inlineStr">
+        <is>
+          <t>2555</t>
         </is>
       </c>
     </row>
@@ -2986,9 +3080,15 @@
       <c r="AV16" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AW16" t="inlineStr">
-        <is>
-          <t>4875</t>
+      <c r="AW16" t="n">
+        <v>4875</v>
+      </c>
+      <c r="AX16" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AY16" t="inlineStr">
+        <is>
+          <t>5057</t>
         </is>
       </c>
     </row>
@@ -3143,9 +3243,15 @@
       <c r="AV17" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="AW17" t="inlineStr">
-        <is>
-          <t>3908</t>
+      <c r="AW17" t="n">
+        <v>3908</v>
+      </c>
+      <c r="AX17" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AY17" t="inlineStr">
+        <is>
+          <t>3995</t>
         </is>
       </c>
     </row>
@@ -3300,9 +3406,15 @@
       <c r="AV18" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="AW18" t="inlineStr">
-        <is>
-          <t>4258</t>
+      <c r="AW18" t="n">
+        <v>4258</v>
+      </c>
+      <c r="AX18" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="AY18" t="inlineStr">
+        <is>
+          <t>4425</t>
         </is>
       </c>
     </row>
@@ -3457,9 +3569,15 @@
       <c r="AV19" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AW19" t="inlineStr">
-        <is>
-          <t>4990</t>
+      <c r="AW19" t="n">
+        <v>4990</v>
+      </c>
+      <c r="AX19" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AY19" t="inlineStr">
+        <is>
+          <t>5171</t>
         </is>
       </c>
     </row>
@@ -3614,9 +3732,15 @@
       <c r="AV20" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AW20" t="inlineStr">
-        <is>
-          <t>5593</t>
+      <c r="AW20" t="n">
+        <v>5593</v>
+      </c>
+      <c r="AX20" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AY20" t="inlineStr">
+        <is>
+          <t>5788</t>
         </is>
       </c>
     </row>
@@ -3771,9 +3895,15 @@
       <c r="AV21" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AW21" t="inlineStr">
-        <is>
-          <t>3847</t>
+      <c r="AW21" t="n">
+        <v>3847</v>
+      </c>
+      <c r="AX21" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AY21" t="inlineStr">
+        <is>
+          <t>4236</t>
         </is>
       </c>
     </row>
@@ -3928,9 +4058,15 @@
       <c r="AV22" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AW22" t="inlineStr">
-        <is>
-          <t>4864</t>
+      <c r="AW22" t="n">
+        <v>4864</v>
+      </c>
+      <c r="AX22" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AY22" t="inlineStr">
+        <is>
+          <t>5058</t>
         </is>
       </c>
     </row>
@@ -4085,9 +4221,15 @@
       <c r="AV23" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW23" t="inlineStr">
-        <is>
-          <t>3811</t>
+      <c r="AW23" t="n">
+        <v>3811</v>
+      </c>
+      <c r="AX23" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="AY23" t="inlineStr">
+        <is>
+          <t>4034</t>
         </is>
       </c>
     </row>
@@ -4242,9 +4384,15 @@
       <c r="AV24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AW24" t="inlineStr">
-        <is>
-          <t>4920</t>
+      <c r="AW24" t="n">
+        <v>4920</v>
+      </c>
+      <c r="AX24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AY24" t="inlineStr">
+        <is>
+          <t>5262</t>
         </is>
       </c>
     </row>
@@ -4399,7 +4547,13 @@
       <c r="AV25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW25" t="inlineStr">
+      <c r="AW25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4556,9 +4710,15 @@
       <c r="AV26" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AW26" t="inlineStr">
-        <is>
-          <t>4866</t>
+      <c r="AW26" t="n">
+        <v>4866</v>
+      </c>
+      <c r="AX26" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AY26" t="inlineStr">
+        <is>
+          <t>5394</t>
         </is>
       </c>
     </row>
@@ -4713,9 +4873,15 @@
       <c r="AV27" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AW27" t="inlineStr">
-        <is>
-          <t>4879</t>
+      <c r="AW27" t="n">
+        <v>4879</v>
+      </c>
+      <c r="AX27" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AY27" t="inlineStr">
+        <is>
+          <t>5156</t>
         </is>
       </c>
     </row>
@@ -4870,9 +5036,15 @@
       <c r="AV28" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="AW28" t="inlineStr">
-        <is>
-          <t>3970</t>
+      <c r="AW28" t="n">
+        <v>3970</v>
+      </c>
+      <c r="AX28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="AY28" t="inlineStr">
+        <is>
+          <t>4624</t>
         </is>
       </c>
     </row>
@@ -5027,9 +5199,15 @@
       <c r="AV29" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AW29" t="inlineStr">
-        <is>
-          <t>5683</t>
+      <c r="AW29" t="n">
+        <v>5683</v>
+      </c>
+      <c r="AX29" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AY29" t="inlineStr">
+        <is>
+          <t>6029</t>
         </is>
       </c>
     </row>
@@ -5184,9 +5362,15 @@
       <c r="AV30" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AW30" t="inlineStr">
-        <is>
-          <t>4408</t>
+      <c r="AW30" t="n">
+        <v>4408</v>
+      </c>
+      <c r="AX30" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AY30" t="inlineStr">
+        <is>
+          <t>4723</t>
         </is>
       </c>
     </row>
@@ -5341,9 +5525,15 @@
       <c r="AV31" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AW31" t="inlineStr">
-        <is>
-          <t>5287</t>
+      <c r="AW31" t="n">
+        <v>5287</v>
+      </c>
+      <c r="AX31" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AY31" t="inlineStr">
+        <is>
+          <t>5692</t>
         </is>
       </c>
     </row>
@@ -5498,9 +5688,15 @@
       <c r="AV32" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="AW32" t="inlineStr">
-        <is>
-          <t>5334</t>
+      <c r="AW32" t="n">
+        <v>5334</v>
+      </c>
+      <c r="AX32" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AY32" t="inlineStr">
+        <is>
+          <t>5620</t>
         </is>
       </c>
     </row>
@@ -5655,9 +5851,15 @@
       <c r="AV33" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="AW33" t="inlineStr">
-        <is>
-          <t>4536</t>
+      <c r="AW33" t="n">
+        <v>4536</v>
+      </c>
+      <c r="AX33" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AY33" t="inlineStr">
+        <is>
+          <t>4777</t>
         </is>
       </c>
     </row>
@@ -5812,9 +6014,15 @@
       <c r="AV34" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AW34" t="inlineStr">
-        <is>
-          <t>4579</t>
+      <c r="AW34" t="n">
+        <v>4579</v>
+      </c>
+      <c r="AX34" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AY34" t="inlineStr">
+        <is>
+          <t>4815</t>
         </is>
       </c>
     </row>
@@ -5969,9 +6177,15 @@
       <c r="AV35" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="AW35" t="inlineStr">
-        <is>
-          <t>4734</t>
+      <c r="AW35" t="n">
+        <v>4734</v>
+      </c>
+      <c r="AX35" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AY35" t="inlineStr">
+        <is>
+          <t>5200</t>
         </is>
       </c>
     </row>
@@ -6126,9 +6340,15 @@
       <c r="AV36" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AW36" t="inlineStr">
-        <is>
-          <t>4777</t>
+      <c r="AW36" t="n">
+        <v>4777</v>
+      </c>
+      <c r="AX36" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AY36" t="inlineStr">
+        <is>
+          <t>5056</t>
         </is>
       </c>
     </row>
@@ -6283,9 +6503,15 @@
       <c r="AV37" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AW37" t="inlineStr">
-        <is>
-          <t>4047</t>
+      <c r="AW37" t="n">
+        <v>4047</v>
+      </c>
+      <c r="AX37" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AY37" t="inlineStr">
+        <is>
+          <t>4156</t>
         </is>
       </c>
     </row>
@@ -6440,9 +6666,15 @@
       <c r="AV38" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AW38" t="inlineStr">
-        <is>
-          <t>4703</t>
+      <c r="AW38" t="n">
+        <v>4703</v>
+      </c>
+      <c r="AX38" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AY38" t="inlineStr">
+        <is>
+          <t>4963</t>
         </is>
       </c>
     </row>
@@ -6597,9 +6829,15 @@
       <c r="AV39" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AW39" t="inlineStr">
-        <is>
-          <t>4756</t>
+      <c r="AW39" t="n">
+        <v>4756</v>
+      </c>
+      <c r="AX39" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AY39" t="inlineStr">
+        <is>
+          <t>4996</t>
         </is>
       </c>
     </row>
@@ -6754,9 +6992,15 @@
       <c r="AV40" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AW40" t="inlineStr">
-        <is>
-          <t>5014</t>
+      <c r="AW40" t="n">
+        <v>5014</v>
+      </c>
+      <c r="AX40" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AY40" t="inlineStr">
+        <is>
+          <t>5311</t>
         </is>
       </c>
     </row>
@@ -6911,7 +7155,13 @@
       <c r="AV41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW41" t="inlineStr">
+      <c r="AW41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY41" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7068,9 +7318,15 @@
       <c r="AV42" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AW42" t="inlineStr">
-        <is>
-          <t>5358</t>
+      <c r="AW42" t="n">
+        <v>5358</v>
+      </c>
+      <c r="AX42" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AY42" t="inlineStr">
+        <is>
+          <t>5752</t>
         </is>
       </c>
     </row>
@@ -7225,9 +7481,15 @@
       <c r="AV43" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AW43" t="inlineStr">
-        <is>
-          <t>4993</t>
+      <c r="AW43" t="n">
+        <v>4993</v>
+      </c>
+      <c r="AX43" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AY43" t="inlineStr">
+        <is>
+          <t>5226</t>
         </is>
       </c>
     </row>
@@ -7382,9 +7644,15 @@
       <c r="AV44" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AW44" t="inlineStr">
-        <is>
-          <t>4736</t>
+      <c r="AW44" t="n">
+        <v>4736</v>
+      </c>
+      <c r="AX44" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AY44" t="inlineStr">
+        <is>
+          <t>5117</t>
         </is>
       </c>
     </row>
@@ -7539,9 +7807,15 @@
       <c r="AV45" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AW45" t="inlineStr">
-        <is>
-          <t>4255</t>
+      <c r="AW45" t="n">
+        <v>4255</v>
+      </c>
+      <c r="AX45" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AY45" t="inlineStr">
+        <is>
+          <t>4481</t>
         </is>
       </c>
     </row>
@@ -7696,9 +7970,15 @@
       <c r="AV46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AW46" t="inlineStr">
-        <is>
-          <t>4180</t>
+      <c r="AW46" t="n">
+        <v>4180</v>
+      </c>
+      <c r="AX46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AY46" t="inlineStr">
+        <is>
+          <t>4350</t>
         </is>
       </c>
     </row>
@@ -7853,7 +8133,13 @@
       <c r="AV47" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="AW47" t="inlineStr">
+      <c r="AW47" t="n">
+        <v>3928</v>
+      </c>
+      <c r="AX47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY47" t="inlineStr">
         <is>
           <t>3928</t>
         </is>
@@ -8010,9 +8296,15 @@
       <c r="AV48" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AW48" t="inlineStr">
-        <is>
-          <t>5142</t>
+      <c r="AW48" t="n">
+        <v>5142</v>
+      </c>
+      <c r="AX48" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AY48" t="inlineStr">
+        <is>
+          <t>5345</t>
         </is>
       </c>
     </row>
@@ -8167,9 +8459,15 @@
       <c r="AV49" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AW49" t="inlineStr">
-        <is>
-          <t>3622</t>
+      <c r="AW49" t="n">
+        <v>3622</v>
+      </c>
+      <c r="AX49" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AY49" t="inlineStr">
+        <is>
+          <t>3854</t>
         </is>
       </c>
     </row>
@@ -8324,9 +8622,15 @@
       <c r="AV50" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AW50" t="inlineStr">
-        <is>
-          <t>5133</t>
+      <c r="AW50" t="n">
+        <v>5133</v>
+      </c>
+      <c r="AX50" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AY50" t="inlineStr">
+        <is>
+          <t>5377</t>
         </is>
       </c>
     </row>
@@ -8481,9 +8785,15 @@
       <c r="AV51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW51" t="inlineStr">
-        <is>
-          <t>2599</t>
+      <c r="AW51" t="n">
+        <v>2599</v>
+      </c>
+      <c r="AX51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY51" t="inlineStr">
+        <is>
+          <t>2619</t>
         </is>
       </c>
     </row>
@@ -8638,9 +8948,15 @@
       <c r="AV52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW52" t="inlineStr">
-        <is>
-          <t>2607</t>
+      <c r="AW52" t="n">
+        <v>2607</v>
+      </c>
+      <c r="AX52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY52" t="inlineStr">
+        <is>
+          <t>2665</t>
         </is>
       </c>
     </row>
@@ -8795,7 +9111,13 @@
       <c r="AV53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW53" t="inlineStr">
+      <c r="AW53" t="n">
+        <v>3143</v>
+      </c>
+      <c r="AX53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY53" t="inlineStr">
         <is>
           <t>3143</t>
         </is>
@@ -8952,9 +9274,15 @@
       <c r="AV54" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AW54" t="inlineStr">
-        <is>
-          <t>4865</t>
+      <c r="AW54" t="n">
+        <v>4865</v>
+      </c>
+      <c r="AX54" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="AY54" t="inlineStr">
+        <is>
+          <t>5081</t>
         </is>
       </c>
     </row>
@@ -9109,9 +9437,15 @@
       <c r="AV55" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="AW55" t="inlineStr">
-        <is>
-          <t>3818</t>
+      <c r="AW55" t="n">
+        <v>3818</v>
+      </c>
+      <c r="AX55" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AY55" t="inlineStr">
+        <is>
+          <t>3913</t>
         </is>
       </c>
     </row>
@@ -9266,9 +9600,15 @@
       <c r="AV56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AW56" t="inlineStr">
-        <is>
-          <t>3887</t>
+      <c r="AW56" t="n">
+        <v>3887</v>
+      </c>
+      <c r="AX56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AY56" t="inlineStr">
+        <is>
+          <t>4036</t>
         </is>
       </c>
     </row>
@@ -9423,9 +9763,15 @@
       <c r="AV57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AW57" t="inlineStr">
-        <is>
-          <t>4678</t>
+      <c r="AW57" t="n">
+        <v>4678</v>
+      </c>
+      <c r="AX57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AY57" t="inlineStr">
+        <is>
+          <t>4882</t>
         </is>
       </c>
     </row>
@@ -9580,9 +9926,15 @@
       <c r="AV58" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AW58" t="inlineStr">
-        <is>
-          <t>3949</t>
+      <c r="AW58" t="n">
+        <v>3949</v>
+      </c>
+      <c r="AX58" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AY58" t="inlineStr">
+        <is>
+          <t>4076</t>
         </is>
       </c>
     </row>
@@ -9648,6 +10000,8 @@
       <c r="AU59" t="inlineStr"/>
       <c r="AV59" s="3" t="inlineStr"/>
       <c r="AW59" t="inlineStr"/>
+      <c r="AX59" s="3" t="inlineStr"/>
+      <c r="AY59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -9711,6 +10065,8 @@
       <c r="AU60" t="inlineStr"/>
       <c r="AV60" s="3" t="inlineStr"/>
       <c r="AW60" t="inlineStr"/>
+      <c r="AX60" s="3" t="inlineStr"/>
+      <c r="AY60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -9863,9 +10219,15 @@
       <c r="AV61" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AW61" t="inlineStr">
-        <is>
-          <t>4382</t>
+      <c r="AW61" t="n">
+        <v>4382</v>
+      </c>
+      <c r="AX61" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="AY61" t="inlineStr">
+        <is>
+          <t>4481</t>
         </is>
       </c>
     </row>
@@ -10020,7 +10382,13 @@
       <c r="AV62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW62" t="inlineStr">
+      <c r="AW62" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10177,9 +10545,15 @@
       <c r="AV63" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AW63" t="inlineStr">
-        <is>
-          <t>4657</t>
+      <c r="AW63" t="n">
+        <v>4657</v>
+      </c>
+      <c r="AX63" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="AY63" t="inlineStr">
+        <is>
+          <t>4757</t>
         </is>
       </c>
     </row>
@@ -10334,9 +10708,15 @@
       <c r="AV64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW64" t="inlineStr">
-        <is>
-          <t>2685</t>
+      <c r="AW64" t="n">
+        <v>2685</v>
+      </c>
+      <c r="AX64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY64" t="inlineStr">
+        <is>
+          <t>2728</t>
         </is>
       </c>
     </row>
@@ -10402,6 +10782,8 @@
       <c r="AU65" t="inlineStr"/>
       <c r="AV65" s="3" t="inlineStr"/>
       <c r="AW65" t="inlineStr"/>
+      <c r="AX65" s="3" t="inlineStr"/>
+      <c r="AY65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -10554,9 +10936,15 @@
       <c r="AV66" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="AW66" t="inlineStr">
-        <is>
-          <t>2604</t>
+      <c r="AW66" t="n">
+        <v>2604</v>
+      </c>
+      <c r="AX66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY66" t="inlineStr">
+        <is>
+          <t>2580</t>
         </is>
       </c>
     </row>
@@ -10711,9 +11099,15 @@
       <c r="AV67" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AW67" t="inlineStr">
-        <is>
-          <t>4449</t>
+      <c r="AW67" t="n">
+        <v>4449</v>
+      </c>
+      <c r="AX67" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AY67" t="inlineStr">
+        <is>
+          <t>4628</t>
         </is>
       </c>
     </row>
@@ -10868,9 +11262,15 @@
       <c r="AV68" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AW68" t="inlineStr">
-        <is>
-          <t>4337</t>
+      <c r="AW68" t="n">
+        <v>4337</v>
+      </c>
+      <c r="AX68" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AY68" t="inlineStr">
+        <is>
+          <t>4609</t>
         </is>
       </c>
     </row>
@@ -11025,9 +11425,15 @@
       <c r="AV69" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AW69" t="inlineStr">
-        <is>
-          <t>3959</t>
+      <c r="AW69" t="n">
+        <v>3959</v>
+      </c>
+      <c r="AX69" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AY69" t="inlineStr">
+        <is>
+          <t>4114</t>
         </is>
       </c>
     </row>
@@ -11182,9 +11588,15 @@
       <c r="AV70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW70" t="inlineStr">
-        <is>
-          <t>2581</t>
+      <c r="AW70" t="n">
+        <v>2581</v>
+      </c>
+      <c r="AX70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY70" t="inlineStr">
+        <is>
+          <t>2596</t>
         </is>
       </c>
     </row>
@@ -11339,9 +11751,15 @@
       <c r="AV71" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AW71" t="inlineStr">
-        <is>
-          <t>4173</t>
+      <c r="AW71" t="n">
+        <v>4173</v>
+      </c>
+      <c r="AX71" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AY71" t="inlineStr">
+        <is>
+          <t>4264</t>
         </is>
       </c>
     </row>
@@ -11496,9 +11914,15 @@
       <c r="AV72" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="AW72" t="inlineStr">
-        <is>
-          <t>3427</t>
+      <c r="AW72" t="n">
+        <v>3427</v>
+      </c>
+      <c r="AX72" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="AY72" t="inlineStr">
+        <is>
+          <t>3601</t>
         </is>
       </c>
     </row>
@@ -11653,9 +12077,15 @@
       <c r="AV73" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AW73" t="inlineStr">
-        <is>
-          <t>3958</t>
+      <c r="AW73" t="n">
+        <v>3958</v>
+      </c>
+      <c r="AX73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AY73" t="inlineStr">
+        <is>
+          <t>4032</t>
         </is>
       </c>
     </row>
@@ -11810,9 +12240,15 @@
       <c r="AV74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW74" t="inlineStr">
-        <is>
-          <t>2925</t>
+      <c r="AW74" t="n">
+        <v>2925</v>
+      </c>
+      <c r="AX74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY74" t="inlineStr">
+        <is>
+          <t>2972</t>
         </is>
       </c>
     </row>
@@ -11967,9 +12403,15 @@
       <c r="AV75" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AW75" t="inlineStr">
-        <is>
-          <t>3659</t>
+      <c r="AW75" t="n">
+        <v>3659</v>
+      </c>
+      <c r="AX75" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AY75" t="inlineStr">
+        <is>
+          <t>3807</t>
         </is>
       </c>
     </row>
@@ -12124,9 +12566,15 @@
       <c r="AV76" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AW76" t="inlineStr">
-        <is>
-          <t>4548</t>
+      <c r="AW76" t="n">
+        <v>4548</v>
+      </c>
+      <c r="AX76" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AY76" t="inlineStr">
+        <is>
+          <t>4669</t>
         </is>
       </c>
     </row>
@@ -12281,7 +12729,13 @@
       <c r="AV77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW77" t="inlineStr">
+      <c r="AW77" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY77" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12438,9 +12892,15 @@
       <c r="AV78" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AW78" t="inlineStr">
-        <is>
-          <t>4369</t>
+      <c r="AW78" t="n">
+        <v>4369</v>
+      </c>
+      <c r="AX78" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AY78" t="inlineStr">
+        <is>
+          <t>4588</t>
         </is>
       </c>
     </row>
@@ -12595,7 +13055,13 @@
       <c r="AV79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW79" t="inlineStr">
+      <c r="AW79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12752,9 +13218,15 @@
       <c r="AV80" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="AW80" t="inlineStr">
-        <is>
-          <t>4271</t>
+      <c r="AW80" t="n">
+        <v>4271</v>
+      </c>
+      <c r="AX80" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AY80" t="inlineStr">
+        <is>
+          <t>4455</t>
         </is>
       </c>
     </row>
@@ -12909,9 +13381,15 @@
       <c r="AV81" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AW81" t="inlineStr">
-        <is>
-          <t>4339</t>
+      <c r="AW81" t="n">
+        <v>4339</v>
+      </c>
+      <c r="AX81" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AY81" t="inlineStr">
+        <is>
+          <t>4558</t>
         </is>
       </c>
     </row>
@@ -13066,9 +13544,15 @@
       <c r="AV82" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AW82" t="inlineStr">
-        <is>
-          <t>4219</t>
+      <c r="AW82" t="n">
+        <v>4219</v>
+      </c>
+      <c r="AX82" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AY82" t="inlineStr">
+        <is>
+          <t>4484</t>
         </is>
       </c>
     </row>
@@ -13223,9 +13707,15 @@
       <c r="AV83" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AW83" t="inlineStr">
-        <is>
-          <t>3943</t>
+      <c r="AW83" t="n">
+        <v>3943</v>
+      </c>
+      <c r="AX83" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AY83" t="inlineStr">
+        <is>
+          <t>4116</t>
         </is>
       </c>
     </row>
@@ -13351,6 +13841,8 @@
       <c r="AU84" t="inlineStr"/>
       <c r="AV84" s="3" t="inlineStr"/>
       <c r="AW84" t="inlineStr"/>
+      <c r="AX84" s="3" t="inlineStr"/>
+      <c r="AY84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -13503,9 +13995,15 @@
       <c r="AV85" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AW85" t="inlineStr">
-        <is>
-          <t>3519</t>
+      <c r="AW85" t="n">
+        <v>3519</v>
+      </c>
+      <c r="AX85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY85" t="inlineStr">
+        <is>
+          <t>3595</t>
         </is>
       </c>
     </row>
@@ -13660,9 +14158,15 @@
       <c r="AV86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW86" t="inlineStr">
-        <is>
-          <t>2688</t>
+      <c r="AW86" t="n">
+        <v>2688</v>
+      </c>
+      <c r="AX86" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="AY86" t="inlineStr">
+        <is>
+          <t>2992</t>
         </is>
       </c>
     </row>
@@ -13817,9 +14321,15 @@
       <c r="AV87" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AW87" t="inlineStr">
-        <is>
-          <t>3947</t>
+      <c r="AW87" t="n">
+        <v>3947</v>
+      </c>
+      <c r="AX87" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AY87" t="inlineStr">
+        <is>
+          <t>4264</t>
         </is>
       </c>
     </row>
@@ -13974,9 +14484,15 @@
       <c r="AV88" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AW88" t="inlineStr">
-        <is>
-          <t>2628</t>
+      <c r="AW88" t="n">
+        <v>2628</v>
+      </c>
+      <c r="AX88" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AY88" t="inlineStr">
+        <is>
+          <t>2683</t>
         </is>
       </c>
     </row>
@@ -14131,9 +14647,15 @@
       <c r="AV89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW89" t="inlineStr">
-        <is>
-          <t>2991</t>
+      <c r="AW89" t="n">
+        <v>2991</v>
+      </c>
+      <c r="AX89" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AY89" t="inlineStr">
+        <is>
+          <t>3122</t>
         </is>
       </c>
     </row>
@@ -14288,9 +14810,15 @@
       <c r="AV90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW90" t="inlineStr">
-        <is>
-          <t>2618</t>
+      <c r="AW90" t="n">
+        <v>2618</v>
+      </c>
+      <c r="AX90" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="AY90" t="inlineStr">
+        <is>
+          <t>2661</t>
         </is>
       </c>
     </row>
@@ -14445,9 +14973,15 @@
       <c r="AV91" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AW91" t="inlineStr">
-        <is>
-          <t>2711</t>
+      <c r="AW91" t="n">
+        <v>2711</v>
+      </c>
+      <c r="AX91" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AY91" t="inlineStr">
+        <is>
+          <t>2860</t>
         </is>
       </c>
     </row>
@@ -14602,7 +15136,13 @@
       <c r="AV92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW92" t="inlineStr">
+      <c r="AW92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14759,9 +15299,15 @@
       <c r="AV93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW93" t="inlineStr">
-        <is>
-          <t>2290</t>
+      <c r="AW93" t="n">
+        <v>2290</v>
+      </c>
+      <c r="AX93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY93" t="inlineStr">
+        <is>
+          <t>2296</t>
         </is>
       </c>
     </row>
@@ -14916,9 +15462,15 @@
       <c r="AV94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW94" t="inlineStr">
-        <is>
-          <t>2540</t>
+      <c r="AW94" t="n">
+        <v>2540</v>
+      </c>
+      <c r="AX94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY94" t="inlineStr">
+        <is>
+          <t>2626</t>
         </is>
       </c>
     </row>
@@ -15073,9 +15625,15 @@
       <c r="AV95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW95" t="inlineStr">
-        <is>
-          <t>2496</t>
+      <c r="AW95" t="n">
+        <v>2496</v>
+      </c>
+      <c r="AX95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY95" t="inlineStr">
+        <is>
+          <t>2484</t>
         </is>
       </c>
     </row>
@@ -15230,9 +15788,15 @@
       <c r="AV96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW96" t="inlineStr">
-        <is>
-          <t>2482</t>
+      <c r="AW96" t="n">
+        <v>2482</v>
+      </c>
+      <c r="AX96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY96" t="inlineStr">
+        <is>
+          <t>2474</t>
         </is>
       </c>
     </row>
@@ -15387,9 +15951,15 @@
       <c r="AV97" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AW97" t="inlineStr">
-        <is>
-          <t>3008</t>
+      <c r="AW97" t="n">
+        <v>3008</v>
+      </c>
+      <c r="AX97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY97" t="inlineStr">
+        <is>
+          <t>3014</t>
         </is>
       </c>
     </row>
@@ -15544,7 +16114,13 @@
       <c r="AV98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW98" t="inlineStr">
+      <c r="AW98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15701,9 +16277,15 @@
       <c r="AV99" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="AW99" t="inlineStr">
-        <is>
-          <t>3455</t>
+      <c r="AW99" t="n">
+        <v>3455</v>
+      </c>
+      <c r="AX99" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AY99" t="inlineStr">
+        <is>
+          <t>3578</t>
         </is>
       </c>
     </row>
@@ -15858,9 +16440,15 @@
       <c r="AV100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW100" t="inlineStr">
-        <is>
-          <t>2365</t>
+      <c r="AW100" t="n">
+        <v>2365</v>
+      </c>
+      <c r="AX100" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AY100" t="inlineStr">
+        <is>
+          <t>2409</t>
         </is>
       </c>
     </row>
@@ -16015,9 +16603,15 @@
       <c r="AV101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AW101" t="inlineStr">
-        <is>
-          <t>4090</t>
+      <c r="AW101" t="n">
+        <v>4090</v>
+      </c>
+      <c r="AX101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AY101" t="inlineStr">
+        <is>
+          <t>4227</t>
         </is>
       </c>
     </row>
@@ -16172,9 +16766,15 @@
       <c r="AV102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AW102" t="inlineStr">
-        <is>
-          <t>3733</t>
+      <c r="AW102" t="n">
+        <v>3733</v>
+      </c>
+      <c r="AX102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AY102" t="inlineStr">
+        <is>
+          <t>3762</t>
         </is>
       </c>
     </row>
@@ -16329,9 +16929,15 @@
       <c r="AV103" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AW103" t="inlineStr">
-        <is>
-          <t>3365</t>
+      <c r="AW103" t="n">
+        <v>3365</v>
+      </c>
+      <c r="AX103" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AY103" t="inlineStr">
+        <is>
+          <t>3610</t>
         </is>
       </c>
     </row>
@@ -16486,9 +17092,15 @@
       <c r="AV104" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AW104" t="inlineStr">
-        <is>
-          <t>4146</t>
+      <c r="AW104" t="n">
+        <v>4146</v>
+      </c>
+      <c r="AX104" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AY104" t="inlineStr">
+        <is>
+          <t>4281</t>
         </is>
       </c>
     </row>
@@ -16643,9 +17255,15 @@
       <c r="AV105" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AW105" t="inlineStr">
-        <is>
-          <t>3763</t>
+      <c r="AW105" t="n">
+        <v>3763</v>
+      </c>
+      <c r="AX105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY105" t="inlineStr">
+        <is>
+          <t>3794</t>
         </is>
       </c>
     </row>
@@ -16800,7 +17418,13 @@
       <c r="AV106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW106" t="inlineStr">
+      <c r="AW106" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16957,9 +17581,15 @@
       <c r="AV107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW107" t="inlineStr">
-        <is>
-          <t>2510</t>
+      <c r="AW107" t="n">
+        <v>2510</v>
+      </c>
+      <c r="AX107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY107" t="inlineStr">
+        <is>
+          <t>2511</t>
         </is>
       </c>
     </row>
@@ -17114,7 +17744,13 @@
       <c r="AV108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW108" t="inlineStr">
+      <c r="AW108" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -17271,9 +17907,15 @@
       <c r="AV109" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AW109" t="inlineStr">
-        <is>
-          <t>3613</t>
+      <c r="AW109" t="n">
+        <v>3613</v>
+      </c>
+      <c r="AX109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY109" t="inlineStr">
+        <is>
+          <t>3650</t>
         </is>
       </c>
     </row>
@@ -17428,9 +18070,15 @@
       <c r="AV110" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AW110" t="inlineStr">
-        <is>
-          <t>3369</t>
+      <c r="AW110" t="n">
+        <v>3369</v>
+      </c>
+      <c r="AX110" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AY110" t="inlineStr">
+        <is>
+          <t>3608</t>
         </is>
       </c>
     </row>
@@ -17580,6 +18228,8 @@
       <c r="AU111" t="inlineStr"/>
       <c r="AV111" s="3" t="inlineStr"/>
       <c r="AW111" t="inlineStr"/>
+      <c r="AX111" s="3" t="inlineStr"/>
+      <c r="AY111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -17732,9 +18382,15 @@
       <c r="AV112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW112" t="inlineStr">
-        <is>
-          <t>2565</t>
+      <c r="AW112" t="n">
+        <v>2565</v>
+      </c>
+      <c r="AX112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY112" t="inlineStr">
+        <is>
+          <t>2555</t>
         </is>
       </c>
     </row>
@@ -17889,9 +18545,15 @@
       <c r="AV113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW113" t="inlineStr">
-        <is>
-          <t>3320</t>
+      <c r="AW113" t="n">
+        <v>3320</v>
+      </c>
+      <c r="AX113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY113" t="inlineStr">
+        <is>
+          <t>3408</t>
         </is>
       </c>
     </row>
@@ -18046,9 +18708,15 @@
       <c r="AV114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW114" t="inlineStr">
-        <is>
-          <t>3439</t>
+      <c r="AW114" t="n">
+        <v>3439</v>
+      </c>
+      <c r="AX114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY114" t="inlineStr">
+        <is>
+          <t>3470</t>
         </is>
       </c>
     </row>
@@ -18203,9 +18871,15 @@
       <c r="AV115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW115" t="inlineStr">
-        <is>
-          <t>2021</t>
+      <c r="AW115" t="n">
+        <v>2021</v>
+      </c>
+      <c r="AX115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY115" t="inlineStr">
+        <is>
+          <t>2006</t>
         </is>
       </c>
     </row>
@@ -18360,9 +19034,15 @@
       <c r="AV116" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="AW116" t="inlineStr">
-        <is>
-          <t>2948</t>
+      <c r="AW116" t="n">
+        <v>2948</v>
+      </c>
+      <c r="AX116" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AY116" t="inlineStr">
+        <is>
+          <t>3005</t>
         </is>
       </c>
     </row>
@@ -18517,9 +19197,15 @@
       <c r="AV117" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AW117" t="inlineStr">
-        <is>
-          <t>3275</t>
+      <c r="AW117" t="n">
+        <v>3275</v>
+      </c>
+      <c r="AX117" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AY117" t="inlineStr">
+        <is>
+          <t>3536</t>
         </is>
       </c>
     </row>
@@ -18674,7 +19360,13 @@
       <c r="AV118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW118" t="inlineStr">
+      <c r="AW118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18831,9 +19523,15 @@
       <c r="AV119" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AW119" t="inlineStr">
-        <is>
-          <t>3668</t>
+      <c r="AW119" t="n">
+        <v>3668</v>
+      </c>
+      <c r="AX119" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AY119" t="inlineStr">
+        <is>
+          <t>3901</t>
         </is>
       </c>
     </row>
@@ -18988,9 +19686,15 @@
       <c r="AV120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW120" t="inlineStr">
-        <is>
-          <t>2466</t>
+      <c r="AW120" t="n">
+        <v>2466</v>
+      </c>
+      <c r="AX120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY120" t="inlineStr">
+        <is>
+          <t>2475</t>
         </is>
       </c>
     </row>
@@ -19145,9 +19849,15 @@
       <c r="AV121" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="AW121" t="inlineStr">
-        <is>
-          <t>3063</t>
+      <c r="AW121" t="n">
+        <v>3063</v>
+      </c>
+      <c r="AX121" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AY121" t="inlineStr">
+        <is>
+          <t>3147</t>
         </is>
       </c>
     </row>
@@ -19302,7 +20012,13 @@
       <c r="AV122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW122" t="inlineStr">
+      <c r="AW122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -19459,9 +20175,15 @@
       <c r="AV123" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AW123" t="inlineStr">
-        <is>
-          <t>3126</t>
+      <c r="AW123" t="n">
+        <v>3126</v>
+      </c>
+      <c r="AX123" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="AY123" t="inlineStr">
+        <is>
+          <t>3142</t>
         </is>
       </c>
     </row>
@@ -19616,9 +20338,15 @@
       <c r="AV124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AW124" t="inlineStr">
-        <is>
-          <t>3062</t>
+      <c r="AW124" t="n">
+        <v>3062</v>
+      </c>
+      <c r="AX124" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="AY124" t="inlineStr">
+        <is>
+          <t>3210</t>
         </is>
       </c>
     </row>
@@ -19773,9 +20501,15 @@
       <c r="AV125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW125" t="inlineStr">
-        <is>
-          <t>2919</t>
+      <c r="AW125" t="n">
+        <v>2919</v>
+      </c>
+      <c r="AX125" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AY125" t="inlineStr">
+        <is>
+          <t>3182</t>
         </is>
       </c>
     </row>
@@ -19930,9 +20664,15 @@
       <c r="AV126" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="AW126" t="inlineStr">
-        <is>
-          <t>3115</t>
+      <c r="AW126" t="n">
+        <v>3115</v>
+      </c>
+      <c r="AX126" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AY126" t="inlineStr">
+        <is>
+          <t>3193</t>
         </is>
       </c>
     </row>
@@ -20087,9 +20827,15 @@
       <c r="AV127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW127" t="inlineStr">
-        <is>
-          <t>2307</t>
+      <c r="AW127" t="n">
+        <v>2307</v>
+      </c>
+      <c r="AX127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY127" t="inlineStr">
+        <is>
+          <t>2291</t>
         </is>
       </c>
     </row>
@@ -20244,7 +20990,13 @@
       <c r="AV128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW128" t="inlineStr">
+      <c r="AW128" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -20401,7 +21153,13 @@
       <c r="AV129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW129" t="inlineStr">
+      <c r="AW129" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -20558,9 +21316,15 @@
       <c r="AV130" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="AW130" t="inlineStr">
-        <is>
-          <t>2847</t>
+      <c r="AW130" t="n">
+        <v>2847</v>
+      </c>
+      <c r="AX130" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AY130" t="inlineStr">
+        <is>
+          <t>2947</t>
         </is>
       </c>
     </row>
@@ -20715,7 +21479,13 @@
       <c r="AV131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW131" t="inlineStr">
+      <c r="AW131" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -20872,9 +21642,15 @@
       <c r="AV132" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AW132" t="inlineStr">
-        <is>
-          <t>2635</t>
+      <c r="AW132" t="n">
+        <v>2635</v>
+      </c>
+      <c r="AX132" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AY132" t="inlineStr">
+        <is>
+          <t>2681</t>
         </is>
       </c>
     </row>
@@ -21029,9 +21805,15 @@
       <c r="AV133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW133" t="inlineStr">
-        <is>
-          <t>2731</t>
+      <c r="AW133" t="n">
+        <v>2731</v>
+      </c>
+      <c r="AX133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY133" t="inlineStr">
+        <is>
+          <t>2762</t>
         </is>
       </c>
     </row>
@@ -21121,6 +21903,8 @@
       <c r="AU134" t="inlineStr"/>
       <c r="AV134" s="3" t="inlineStr"/>
       <c r="AW134" t="inlineStr"/>
+      <c r="AX134" s="3" t="inlineStr"/>
+      <c r="AY134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -21200,6 +21984,8 @@
       <c r="AU135" t="inlineStr"/>
       <c r="AV135" s="3" t="inlineStr"/>
       <c r="AW135" t="inlineStr"/>
+      <c r="AX135" s="3" t="inlineStr"/>
+      <c r="AY135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -21352,7 +22138,13 @@
       <c r="AV136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW136" t="inlineStr">
+      <c r="AW136" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY136" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -21509,7 +22301,13 @@
       <c r="AV137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW137" t="inlineStr">
+      <c r="AW137" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -21593,6 +22391,8 @@
       <c r="AU138" t="inlineStr"/>
       <c r="AV138" s="3" t="inlineStr"/>
       <c r="AW138" t="inlineStr"/>
+      <c r="AX138" s="3" t="inlineStr"/>
+      <c r="AY138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -21745,9 +22545,15 @@
       <c r="AV139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW139" t="inlineStr">
-        <is>
-          <t>2095</t>
+      <c r="AW139" t="n">
+        <v>2095</v>
+      </c>
+      <c r="AX139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY139" t="inlineStr">
+        <is>
+          <t>2089</t>
         </is>
       </c>
     </row>
@@ -21902,9 +22708,15 @@
       <c r="AV140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW140" t="inlineStr">
-        <is>
-          <t>2616</t>
+      <c r="AW140" t="n">
+        <v>2616</v>
+      </c>
+      <c r="AX140" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AY140" t="inlineStr">
+        <is>
+          <t>2806</t>
         </is>
       </c>
     </row>
@@ -21986,6 +22798,8 @@
       <c r="AU141" t="inlineStr"/>
       <c r="AV141" s="3" t="inlineStr"/>
       <c r="AW141" t="inlineStr"/>
+      <c r="AX141" s="3" t="inlineStr"/>
+      <c r="AY141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -22138,7 +22952,13 @@
       <c r="AV142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW142" t="inlineStr">
+      <c r="AW142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY142" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -22222,6 +23042,8 @@
       <c r="AU143" t="inlineStr"/>
       <c r="AV143" s="3" t="inlineStr"/>
       <c r="AW143" t="inlineStr"/>
+      <c r="AX143" s="3" t="inlineStr"/>
+      <c r="AY143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -22301,6 +23123,8 @@
       <c r="AU144" t="inlineStr"/>
       <c r="AV144" s="3" t="inlineStr"/>
       <c r="AW144" t="inlineStr"/>
+      <c r="AX144" s="3" t="inlineStr"/>
+      <c r="AY144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -22380,6 +23204,8 @@
       <c r="AU145" t="inlineStr"/>
       <c r="AV145" s="3" t="inlineStr"/>
       <c r="AW145" t="inlineStr"/>
+      <c r="AX145" s="3" t="inlineStr"/>
+      <c r="AY145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -22459,6 +23285,8 @@
       <c r="AU146" t="inlineStr"/>
       <c r="AV146" s="3" t="inlineStr"/>
       <c r="AW146" t="inlineStr"/>
+      <c r="AX146" s="3" t="inlineStr"/>
+      <c r="AY146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -22538,6 +23366,8 @@
       <c r="AU147" t="inlineStr"/>
       <c r="AV147" s="3" t="inlineStr"/>
       <c r="AW147" t="inlineStr"/>
+      <c r="AX147" s="3" t="inlineStr"/>
+      <c r="AY147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -22690,7 +23520,13 @@
       <c r="AV148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW148" t="inlineStr">
+      <c r="AW148" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -22847,7 +23683,13 @@
       <c r="AV149" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="AW149" t="inlineStr">
+      <c r="AW149" t="n">
+        <v>3727</v>
+      </c>
+      <c r="AX149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY149" t="inlineStr">
         <is>
           <t>3727</t>
         </is>
@@ -23004,7 +23846,13 @@
       <c r="AV150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW150" t="inlineStr">
+      <c r="AW150" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -23161,7 +24009,13 @@
       <c r="AV151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW151" t="inlineStr">
+      <c r="AW151" t="n">
+        <v>2578</v>
+      </c>
+      <c r="AX151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY151" t="inlineStr">
         <is>
           <t>2578</t>
         </is>
@@ -23318,7 +24172,13 @@
       <c r="AV152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW152" t="inlineStr">
+      <c r="AW152" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -23475,7 +24335,13 @@
       <c r="AV153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW153" t="inlineStr">
+      <c r="AW153" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -23632,7 +24498,13 @@
       <c r="AV154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW154" t="inlineStr">
+      <c r="AW154" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -23789,7 +24661,13 @@
       <c r="AV155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW155" t="inlineStr">
+      <c r="AW155" t="n">
+        <v>2687</v>
+      </c>
+      <c r="AX155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY155" t="inlineStr">
         <is>
           <t>2687</t>
         </is>
@@ -23940,9 +24818,15 @@
       <c r="AV156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW156" t="inlineStr">
-        <is>
-          <t>3195</t>
+      <c r="AW156" t="n">
+        <v>3195</v>
+      </c>
+      <c r="AX156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY156" t="inlineStr">
+        <is>
+          <t>3169</t>
         </is>
       </c>
     </row>
@@ -24018,6 +24902,8 @@
       <c r="AU157" t="inlineStr"/>
       <c r="AV157" s="3" t="inlineStr"/>
       <c r="AW157" t="inlineStr"/>
+      <c r="AX157" s="3" t="inlineStr"/>
+      <c r="AY157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -24164,7 +25050,13 @@
       <c r="AV158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW158" t="inlineStr">
+      <c r="AW158" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -24315,9 +25207,15 @@
       <c r="AV159" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AW159" t="inlineStr">
-        <is>
-          <t>2957</t>
+      <c r="AW159" t="n">
+        <v>2957</v>
+      </c>
+      <c r="AX159" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="AY159" t="inlineStr">
+        <is>
+          <t>2989</t>
         </is>
       </c>
     </row>
@@ -24393,6 +25291,8 @@
       <c r="AU160" t="inlineStr"/>
       <c r="AV160" s="3" t="inlineStr"/>
       <c r="AW160" t="inlineStr"/>
+      <c r="AX160" s="3" t="inlineStr"/>
+      <c r="AY160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -24527,9 +25427,15 @@
       <c r="AV161" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AW161" t="inlineStr">
-        <is>
-          <t>3096</t>
+      <c r="AW161" t="n">
+        <v>3096</v>
+      </c>
+      <c r="AX161" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AY161" t="inlineStr">
+        <is>
+          <t>3085</t>
         </is>
       </c>
     </row>
@@ -24666,9 +25572,15 @@
       <c r="AV162" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="AW162" t="inlineStr">
-        <is>
-          <t>2617</t>
+      <c r="AW162" t="n">
+        <v>2617</v>
+      </c>
+      <c r="AX162" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY162" t="inlineStr">
+        <is>
+          <t>2610</t>
         </is>
       </c>
     </row>
@@ -24801,9 +25713,15 @@
       <c r="AV163" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW163" t="inlineStr">
-        <is>
-          <t>3264</t>
+      <c r="AW163" t="n">
+        <v>3264</v>
+      </c>
+      <c r="AX163" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY163" t="inlineStr">
+        <is>
+          <t>3234</t>
         </is>
       </c>
     </row>
@@ -24920,9 +25838,15 @@
       <c r="AV164" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AW164" t="inlineStr">
-        <is>
-          <t>3274</t>
+      <c r="AW164" t="n">
+        <v>3274</v>
+      </c>
+      <c r="AX164" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AY164" t="inlineStr">
+        <is>
+          <t>3472</t>
         </is>
       </c>
     </row>
@@ -25043,9 +25967,15 @@
       <c r="AV165" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AW165" t="inlineStr">
-        <is>
-          <t>2730</t>
+      <c r="AW165" t="n">
+        <v>2730</v>
+      </c>
+      <c r="AX165" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AY165" t="inlineStr">
+        <is>
+          <t>2710</t>
         </is>
       </c>
     </row>
@@ -25158,9 +26088,15 @@
       <c r="AV166" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW166" t="inlineStr">
-        <is>
-          <t>2774</t>
+      <c r="AW166" t="n">
+        <v>2774</v>
+      </c>
+      <c r="AX166" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY166" t="inlineStr">
+        <is>
+          <t>2794</t>
         </is>
       </c>
     </row>
@@ -25261,7 +26197,13 @@
       <c r="AV167" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW167" t="inlineStr">
+      <c r="AW167" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX167" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY167" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -25360,9 +26302,15 @@
       <c r="AV168" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="AW168" t="inlineStr">
-        <is>
-          <t>1521</t>
+      <c r="AW168" t="n">
+        <v>1521</v>
+      </c>
+      <c r="AX168" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY168" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -25430,6 +26378,8 @@
       <c r="AU169" t="inlineStr"/>
       <c r="AV169" s="3" t="inlineStr"/>
       <c r="AW169" t="inlineStr"/>
+      <c r="AX169" s="3" t="inlineStr"/>
+      <c r="AY169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="n">
@@ -25520,7 +26470,13 @@
       <c r="AV170" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW170" t="inlineStr">
+      <c r="AW170" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX170" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY170" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -25603,9 +26559,15 @@
       <c r="AV171" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW171" t="inlineStr">
-        <is>
-          <t>1737</t>
+      <c r="AW171" t="n">
+        <v>1737</v>
+      </c>
+      <c r="AX171" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY171" t="inlineStr">
+        <is>
+          <t>1719</t>
         </is>
       </c>
     </row>
@@ -25686,7 +26648,13 @@
       <c r="AV172" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW172" t="inlineStr">
+      <c r="AW172" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX172" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY172" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -25769,9 +26737,15 @@
       <c r="AV173" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="AW173" t="inlineStr">
-        <is>
-          <t>1839</t>
+      <c r="AW173" t="n">
+        <v>1839</v>
+      </c>
+      <c r="AX173" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="AY173" t="inlineStr">
+        <is>
+          <t>1932</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-03-09 11:30:34
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AY173"/>
+  <dimension ref="A1:BA174"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -646,6 +646,16 @@
           <t>03-06_0</t>
         </is>
       </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>03-08_A</t>
+        </is>
+      </c>
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>03-08_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -804,9 +814,15 @@
       <c r="AX2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY2" t="inlineStr">
-        <is>
-          <t>2740</t>
+      <c r="AY2" t="n">
+        <v>2740</v>
+      </c>
+      <c r="AZ2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA2" t="inlineStr">
+        <is>
+          <t>2898</t>
         </is>
       </c>
     </row>
@@ -967,9 +983,15 @@
       <c r="AX3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AY3" t="inlineStr">
-        <is>
-          <t>5471</t>
+      <c r="AY3" t="n">
+        <v>5471</v>
+      </c>
+      <c r="AZ3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA3" t="inlineStr">
+        <is>
+          <t>6029</t>
         </is>
       </c>
     </row>
@@ -1130,9 +1152,15 @@
       <c r="AX4" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AY4" t="inlineStr">
-        <is>
-          <t>5318</t>
+      <c r="AY4" t="n">
+        <v>5318</v>
+      </c>
+      <c r="AZ4" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="BA4" t="inlineStr">
+        <is>
+          <t>5891</t>
         </is>
       </c>
     </row>
@@ -1293,9 +1321,15 @@
       <c r="AX5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AY5" t="inlineStr">
-        <is>
-          <t>4984</t>
+      <c r="AY5" t="n">
+        <v>4984</v>
+      </c>
+      <c r="AZ5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA5" t="inlineStr">
+        <is>
+          <t>5536</t>
         </is>
       </c>
     </row>
@@ -1456,9 +1490,15 @@
       <c r="AX6" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AY6" t="inlineStr">
-        <is>
-          <t>5150</t>
+      <c r="AY6" t="n">
+        <v>5150</v>
+      </c>
+      <c r="AZ6" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="BA6" t="inlineStr">
+        <is>
+          <t>5585</t>
         </is>
       </c>
     </row>
@@ -1619,9 +1659,15 @@
       <c r="AX7" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AY7" t="inlineStr">
-        <is>
-          <t>5707</t>
+      <c r="AY7" t="n">
+        <v>5707</v>
+      </c>
+      <c r="AZ7" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="BA7" t="inlineStr">
+        <is>
+          <t>6171</t>
         </is>
       </c>
     </row>
@@ -1782,9 +1828,15 @@
       <c r="AX8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AY8" t="inlineStr">
-        <is>
-          <t>4816</t>
+      <c r="AY8" t="n">
+        <v>4816</v>
+      </c>
+      <c r="AZ8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA8" t="inlineStr">
+        <is>
+          <t>5116</t>
         </is>
       </c>
     </row>
@@ -1945,9 +1997,15 @@
       <c r="AX9" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AY9" t="inlineStr">
-        <is>
-          <t>4913</t>
+      <c r="AY9" t="n">
+        <v>4913</v>
+      </c>
+      <c r="AZ9" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BA9" t="inlineStr">
+        <is>
+          <t>5367</t>
         </is>
       </c>
     </row>
@@ -2108,9 +2166,15 @@
       <c r="AX10" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AY10" t="inlineStr">
-        <is>
-          <t>4992</t>
+      <c r="AY10" t="n">
+        <v>4992</v>
+      </c>
+      <c r="AZ10" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BA10" t="inlineStr">
+        <is>
+          <t>6228</t>
         </is>
       </c>
     </row>
@@ -2271,9 +2335,15 @@
       <c r="AX11" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AY11" t="inlineStr">
-        <is>
-          <t>4413</t>
+      <c r="AY11" t="n">
+        <v>4413</v>
+      </c>
+      <c r="AZ11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA11" t="inlineStr">
+        <is>
+          <t>4721</t>
         </is>
       </c>
     </row>
@@ -2434,9 +2504,15 @@
       <c r="AX12" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="AY12" t="inlineStr">
-        <is>
-          <t>2592</t>
+      <c r="AY12" t="n">
+        <v>2592</v>
+      </c>
+      <c r="AZ12" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA12" t="inlineStr">
+        <is>
+          <t>2640</t>
         </is>
       </c>
     </row>
@@ -2597,9 +2673,15 @@
       <c r="AX13" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AY13" t="inlineStr">
-        <is>
-          <t>5744</t>
+      <c r="AY13" t="n">
+        <v>5744</v>
+      </c>
+      <c r="AZ13" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="BA13" t="inlineStr">
+        <is>
+          <t>6277</t>
         </is>
       </c>
     </row>
@@ -2760,9 +2842,15 @@
       <c r="AX14" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="AY14" t="inlineStr">
-        <is>
-          <t>4946</t>
+      <c r="AY14" t="n">
+        <v>4946</v>
+      </c>
+      <c r="AZ14" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="BA14" t="inlineStr">
+        <is>
+          <t>5450</t>
         </is>
       </c>
     </row>
@@ -2923,9 +3011,15 @@
       <c r="AX15" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY15" t="inlineStr">
-        <is>
-          <t>2555</t>
+      <c r="AY15" t="n">
+        <v>2555</v>
+      </c>
+      <c r="AZ15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA15" t="inlineStr">
+        <is>
+          <t>2743</t>
         </is>
       </c>
     </row>
@@ -3086,9 +3180,15 @@
       <c r="AX16" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AY16" t="inlineStr">
-        <is>
-          <t>5057</t>
+      <c r="AY16" t="n">
+        <v>5057</v>
+      </c>
+      <c r="AZ16" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BA16" t="inlineStr">
+        <is>
+          <t>5692</t>
         </is>
       </c>
     </row>
@@ -3249,9 +3349,15 @@
       <c r="AX17" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AY17" t="inlineStr">
-        <is>
-          <t>3995</t>
+      <c r="AY17" t="n">
+        <v>3995</v>
+      </c>
+      <c r="AZ17" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BA17" t="inlineStr">
+        <is>
+          <t>4279</t>
         </is>
       </c>
     </row>
@@ -3412,9 +3518,15 @@
       <c r="AX18" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="AY18" t="inlineStr">
-        <is>
-          <t>4425</t>
+      <c r="AY18" t="n">
+        <v>4425</v>
+      </c>
+      <c r="AZ18" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="BA18" t="inlineStr">
+        <is>
+          <t>4878</t>
         </is>
       </c>
     </row>
@@ -3575,9 +3687,15 @@
       <c r="AX19" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AY19" t="inlineStr">
-        <is>
-          <t>5171</t>
+      <c r="AY19" t="n">
+        <v>5171</v>
+      </c>
+      <c r="AZ19" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BA19" t="inlineStr">
+        <is>
+          <t>5763</t>
         </is>
       </c>
     </row>
@@ -3738,9 +3856,15 @@
       <c r="AX20" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AY20" t="inlineStr">
-        <is>
-          <t>5788</t>
+      <c r="AY20" t="n">
+        <v>5788</v>
+      </c>
+      <c r="AZ20" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BA20" t="inlineStr">
+        <is>
+          <t>6387</t>
         </is>
       </c>
     </row>
@@ -3901,9 +4025,15 @@
       <c r="AX21" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AY21" t="inlineStr">
-        <is>
-          <t>4236</t>
+      <c r="AY21" t="n">
+        <v>4236</v>
+      </c>
+      <c r="AZ21" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="BA21" t="inlineStr">
+        <is>
+          <t>4680</t>
         </is>
       </c>
     </row>
@@ -4064,9 +4194,15 @@
       <c r="AX22" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AY22" t="inlineStr">
-        <is>
-          <t>5058</t>
+      <c r="AY22" t="n">
+        <v>5058</v>
+      </c>
+      <c r="AZ22" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="BA22" t="inlineStr">
+        <is>
+          <t>5468</t>
         </is>
       </c>
     </row>
@@ -4227,9 +4363,15 @@
       <c r="AX23" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="AY23" t="inlineStr">
-        <is>
-          <t>4034</t>
+      <c r="AY23" t="n">
+        <v>4034</v>
+      </c>
+      <c r="AZ23" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA23" t="inlineStr">
+        <is>
+          <t>4867</t>
         </is>
       </c>
     </row>
@@ -4390,9 +4532,15 @@
       <c r="AX24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AY24" t="inlineStr">
-        <is>
-          <t>5262</t>
+      <c r="AY24" t="n">
+        <v>5262</v>
+      </c>
+      <c r="AZ24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BA24" t="inlineStr">
+        <is>
+          <t>5835</t>
         </is>
       </c>
     </row>
@@ -4553,7 +4701,13 @@
       <c r="AX25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY25" t="inlineStr">
+      <c r="AY25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4716,9 +4870,15 @@
       <c r="AX26" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AY26" t="inlineStr">
-        <is>
-          <t>5394</t>
+      <c r="AY26" t="n">
+        <v>5394</v>
+      </c>
+      <c r="AZ26" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="BA26" t="inlineStr">
+        <is>
+          <t>5819</t>
         </is>
       </c>
     </row>
@@ -4879,9 +5039,15 @@
       <c r="AX27" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AY27" t="inlineStr">
-        <is>
-          <t>5156</t>
+      <c r="AY27" t="n">
+        <v>5156</v>
+      </c>
+      <c r="AZ27" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA27" t="inlineStr">
+        <is>
+          <t>5785</t>
         </is>
       </c>
     </row>
@@ -5042,9 +5208,15 @@
       <c r="AX28" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="AY28" t="inlineStr">
-        <is>
-          <t>4624</t>
+      <c r="AY28" t="n">
+        <v>4624</v>
+      </c>
+      <c r="AZ28" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="BA28" t="inlineStr">
+        <is>
+          <t>5443</t>
         </is>
       </c>
     </row>
@@ -5205,9 +5377,15 @@
       <c r="AX29" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AY29" t="inlineStr">
-        <is>
-          <t>6029</t>
+      <c r="AY29" t="n">
+        <v>6029</v>
+      </c>
+      <c r="AZ29" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BA29" t="inlineStr">
+        <is>
+          <t>6115</t>
         </is>
       </c>
     </row>
@@ -5368,9 +5546,15 @@
       <c r="AX30" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AY30" t="inlineStr">
-        <is>
-          <t>4723</t>
+      <c r="AY30" t="n">
+        <v>4723</v>
+      </c>
+      <c r="AZ30" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BA30" t="inlineStr">
+        <is>
+          <t>5343</t>
         </is>
       </c>
     </row>
@@ -5531,9 +5715,15 @@
       <c r="AX31" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AY31" t="inlineStr">
-        <is>
-          <t>5692</t>
+      <c r="AY31" t="n">
+        <v>5692</v>
+      </c>
+      <c r="AZ31" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="BA31" t="inlineStr">
+        <is>
+          <t>6164</t>
         </is>
       </c>
     </row>
@@ -5694,9 +5884,15 @@
       <c r="AX32" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AY32" t="inlineStr">
-        <is>
-          <t>5620</t>
+      <c r="AY32" t="n">
+        <v>5620</v>
+      </c>
+      <c r="AZ32" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="BA32" t="inlineStr">
+        <is>
+          <t>6009</t>
         </is>
       </c>
     </row>
@@ -5857,9 +6053,15 @@
       <c r="AX33" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="AY33" t="inlineStr">
-        <is>
-          <t>4777</t>
+      <c r="AY33" t="n">
+        <v>4777</v>
+      </c>
+      <c r="AZ33" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA33" t="inlineStr">
+        <is>
+          <t>5370</t>
         </is>
       </c>
     </row>
@@ -6020,9 +6222,15 @@
       <c r="AX34" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AY34" t="inlineStr">
-        <is>
-          <t>4815</t>
+      <c r="AY34" t="n">
+        <v>4815</v>
+      </c>
+      <c r="AZ34" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BA34" t="inlineStr">
+        <is>
+          <t>5388</t>
         </is>
       </c>
     </row>
@@ -6183,9 +6391,15 @@
       <c r="AX35" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AY35" t="inlineStr">
-        <is>
-          <t>5200</t>
+      <c r="AY35" t="n">
+        <v>5200</v>
+      </c>
+      <c r="AZ35" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="BA35" t="inlineStr">
+        <is>
+          <t>5868</t>
         </is>
       </c>
     </row>
@@ -6346,9 +6560,15 @@
       <c r="AX36" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AY36" t="inlineStr">
-        <is>
-          <t>5056</t>
+      <c r="AY36" t="n">
+        <v>5056</v>
+      </c>
+      <c r="AZ36" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA36" t="inlineStr">
+        <is>
+          <t>5424</t>
         </is>
       </c>
     </row>
@@ -6509,9 +6729,15 @@
       <c r="AX37" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AY37" t="inlineStr">
-        <is>
-          <t>4156</t>
+      <c r="AY37" t="n">
+        <v>4156</v>
+      </c>
+      <c r="AZ37" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BA37" t="inlineStr">
+        <is>
+          <t>4457</t>
         </is>
       </c>
     </row>
@@ -6672,9 +6898,15 @@
       <c r="AX38" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AY38" t="inlineStr">
-        <is>
-          <t>4963</t>
+      <c r="AY38" t="n">
+        <v>4963</v>
+      </c>
+      <c r="AZ38" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="BA38" t="inlineStr">
+        <is>
+          <t>5400</t>
         </is>
       </c>
     </row>
@@ -6835,9 +7067,15 @@
       <c r="AX39" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AY39" t="inlineStr">
-        <is>
-          <t>4996</t>
+      <c r="AY39" t="n">
+        <v>4996</v>
+      </c>
+      <c r="AZ39" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="BA39" t="inlineStr">
+        <is>
+          <t>5381</t>
         </is>
       </c>
     </row>
@@ -6998,9 +7236,15 @@
       <c r="AX40" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AY40" t="inlineStr">
-        <is>
-          <t>5311</t>
+      <c r="AY40" t="n">
+        <v>5311</v>
+      </c>
+      <c r="AZ40" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BA40" t="inlineStr">
+        <is>
+          <t>6084</t>
         </is>
       </c>
     </row>
@@ -7161,7 +7405,13 @@
       <c r="AX41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY41" t="inlineStr">
+      <c r="AY41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA41" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7324,9 +7574,15 @@
       <c r="AX42" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AY42" t="inlineStr">
-        <is>
-          <t>5752</t>
+      <c r="AY42" t="n">
+        <v>5752</v>
+      </c>
+      <c r="AZ42" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="BA42" t="inlineStr">
+        <is>
+          <t>6447</t>
         </is>
       </c>
     </row>
@@ -7487,9 +7743,15 @@
       <c r="AX43" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AY43" t="inlineStr">
-        <is>
-          <t>5226</t>
+      <c r="AY43" t="n">
+        <v>5226</v>
+      </c>
+      <c r="AZ43" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BA43" t="inlineStr">
+        <is>
+          <t>5569</t>
         </is>
       </c>
     </row>
@@ -7650,9 +7912,15 @@
       <c r="AX44" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AY44" t="inlineStr">
-        <is>
-          <t>5117</t>
+      <c r="AY44" t="n">
+        <v>5117</v>
+      </c>
+      <c r="AZ44" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BA44" t="inlineStr">
+        <is>
+          <t>5518</t>
         </is>
       </c>
     </row>
@@ -7813,9 +8081,15 @@
       <c r="AX45" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AY45" t="inlineStr">
-        <is>
-          <t>4481</t>
+      <c r="AY45" t="n">
+        <v>4481</v>
+      </c>
+      <c r="AZ45" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="BA45" t="inlineStr">
+        <is>
+          <t>4849</t>
         </is>
       </c>
     </row>
@@ -7976,9 +8250,15 @@
       <c r="AX46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AY46" t="inlineStr">
-        <is>
-          <t>4350</t>
+      <c r="AY46" t="n">
+        <v>4350</v>
+      </c>
+      <c r="AZ46" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="BA46" t="inlineStr">
+        <is>
+          <t>5079</t>
         </is>
       </c>
     </row>
@@ -8139,9 +8419,15 @@
       <c r="AX47" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY47" t="inlineStr">
-        <is>
-          <t>3928</t>
+      <c r="AY47" t="n">
+        <v>3928</v>
+      </c>
+      <c r="AZ47" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="BA47" t="inlineStr">
+        <is>
+          <t>4418</t>
         </is>
       </c>
     </row>
@@ -8302,9 +8588,15 @@
       <c r="AX48" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AY48" t="inlineStr">
-        <is>
-          <t>5345</t>
+      <c r="AY48" t="n">
+        <v>5345</v>
+      </c>
+      <c r="AZ48" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="BA48" t="inlineStr">
+        <is>
+          <t>5786</t>
         </is>
       </c>
     </row>
@@ -8465,9 +8757,15 @@
       <c r="AX49" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AY49" t="inlineStr">
-        <is>
-          <t>3854</t>
+      <c r="AY49" t="n">
+        <v>3854</v>
+      </c>
+      <c r="AZ49" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="BA49" t="inlineStr">
+        <is>
+          <t>4521</t>
         </is>
       </c>
     </row>
@@ -8628,9 +8926,15 @@
       <c r="AX50" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AY50" t="inlineStr">
-        <is>
-          <t>5377</t>
+      <c r="AY50" t="n">
+        <v>5377</v>
+      </c>
+      <c r="AZ50" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="BA50" t="inlineStr">
+        <is>
+          <t>5897</t>
         </is>
       </c>
     </row>
@@ -8791,9 +9095,15 @@
       <c r="AX51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY51" t="inlineStr">
-        <is>
-          <t>2619</t>
+      <c r="AY51" t="n">
+        <v>2619</v>
+      </c>
+      <c r="AZ51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA51" t="inlineStr">
+        <is>
+          <t>2677</t>
         </is>
       </c>
     </row>
@@ -8954,9 +9264,15 @@
       <c r="AX52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY52" t="inlineStr">
-        <is>
-          <t>2665</t>
+      <c r="AY52" t="n">
+        <v>2665</v>
+      </c>
+      <c r="AZ52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA52" t="inlineStr">
+        <is>
+          <t>2770</t>
         </is>
       </c>
     </row>
@@ -9117,9 +9433,15 @@
       <c r="AX53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY53" t="inlineStr">
-        <is>
-          <t>3143</t>
+      <c r="AY53" t="n">
+        <v>3143</v>
+      </c>
+      <c r="AZ53" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BA53" t="inlineStr">
+        <is>
+          <t>3210</t>
         </is>
       </c>
     </row>
@@ -9280,9 +9602,15 @@
       <c r="AX54" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="AY54" t="inlineStr">
-        <is>
-          <t>5081</t>
+      <c r="AY54" t="n">
+        <v>5081</v>
+      </c>
+      <c r="AZ54" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="BA54" t="inlineStr">
+        <is>
+          <t>5483</t>
         </is>
       </c>
     </row>
@@ -9443,9 +9771,15 @@
       <c r="AX55" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AY55" t="inlineStr">
-        <is>
-          <t>3913</t>
+      <c r="AY55" t="n">
+        <v>3913</v>
+      </c>
+      <c r="AZ55" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="BA55" t="inlineStr">
+        <is>
+          <t>4148</t>
         </is>
       </c>
     </row>
@@ -9606,9 +9940,15 @@
       <c r="AX56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AY56" t="inlineStr">
-        <is>
-          <t>4036</t>
+      <c r="AY56" t="n">
+        <v>4036</v>
+      </c>
+      <c r="AZ56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA56" t="inlineStr">
+        <is>
+          <t>4206</t>
         </is>
       </c>
     </row>
@@ -9769,9 +10109,15 @@
       <c r="AX57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AY57" t="inlineStr">
-        <is>
-          <t>4882</t>
+      <c r="AY57" t="n">
+        <v>4882</v>
+      </c>
+      <c r="AZ57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA57" t="inlineStr">
+        <is>
+          <t>5234</t>
         </is>
       </c>
     </row>
@@ -9932,9 +10278,15 @@
       <c r="AX58" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AY58" t="inlineStr">
-        <is>
-          <t>4076</t>
+      <c r="AY58" t="n">
+        <v>4076</v>
+      </c>
+      <c r="AZ58" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BA58" t="inlineStr">
+        <is>
+          <t>4481</t>
         </is>
       </c>
     </row>
@@ -10002,6 +10354,8 @@
       <c r="AW59" t="inlineStr"/>
       <c r="AX59" s="3" t="inlineStr"/>
       <c r="AY59" t="inlineStr"/>
+      <c r="AZ59" s="3" t="inlineStr"/>
+      <c r="BA59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -10067,6 +10421,8 @@
       <c r="AW60" t="inlineStr"/>
       <c r="AX60" s="3" t="inlineStr"/>
       <c r="AY60" t="inlineStr"/>
+      <c r="AZ60" s="3" t="inlineStr"/>
+      <c r="BA60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -10225,9 +10581,15 @@
       <c r="AX61" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="AY61" t="inlineStr">
-        <is>
-          <t>4481</t>
+      <c r="AY61" t="n">
+        <v>4481</v>
+      </c>
+      <c r="AZ61" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BA61" t="inlineStr">
+        <is>
+          <t>4846</t>
         </is>
       </c>
     </row>
@@ -10388,7 +10750,13 @@
       <c r="AX62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY62" t="inlineStr">
+      <c r="AY62" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10551,9 +10919,15 @@
       <c r="AX63" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="AY63" t="inlineStr">
-        <is>
-          <t>4757</t>
+      <c r="AY63" t="n">
+        <v>4757</v>
+      </c>
+      <c r="AZ63" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="BA63" t="inlineStr">
+        <is>
+          <t>5060</t>
         </is>
       </c>
     </row>
@@ -10714,7 +11088,13 @@
       <c r="AX64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY64" t="inlineStr">
+      <c r="AY64" t="n">
+        <v>2728</v>
+      </c>
+      <c r="AZ64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA64" t="inlineStr">
         <is>
           <t>2728</t>
         </is>
@@ -10784,6 +11164,8 @@
       <c r="AW65" t="inlineStr"/>
       <c r="AX65" s="3" t="inlineStr"/>
       <c r="AY65" t="inlineStr"/>
+      <c r="AZ65" s="3" t="inlineStr"/>
+      <c r="BA65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -10942,9 +11324,15 @@
       <c r="AX66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY66" t="inlineStr">
-        <is>
-          <t>2580</t>
+      <c r="AY66" t="n">
+        <v>2580</v>
+      </c>
+      <c r="AZ66" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="BA66" t="inlineStr">
+        <is>
+          <t>2788</t>
         </is>
       </c>
     </row>
@@ -11105,9 +11493,15 @@
       <c r="AX67" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AY67" t="inlineStr">
-        <is>
-          <t>4628</t>
+      <c r="AY67" t="n">
+        <v>4628</v>
+      </c>
+      <c r="AZ67" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BA67" t="inlineStr">
+        <is>
+          <t>4929</t>
         </is>
       </c>
     </row>
@@ -11268,9 +11662,15 @@
       <c r="AX68" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AY68" t="inlineStr">
-        <is>
-          <t>4609</t>
+      <c r="AY68" t="n">
+        <v>4609</v>
+      </c>
+      <c r="AZ68" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BA68" t="inlineStr">
+        <is>
+          <t>4954</t>
         </is>
       </c>
     </row>
@@ -11431,9 +11831,15 @@
       <c r="AX69" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AY69" t="inlineStr">
-        <is>
-          <t>4114</t>
+      <c r="AY69" t="n">
+        <v>4114</v>
+      </c>
+      <c r="AZ69" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BA69" t="inlineStr">
+        <is>
+          <t>4416</t>
         </is>
       </c>
     </row>
@@ -11594,9 +12000,15 @@
       <c r="AX70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY70" t="inlineStr">
-        <is>
-          <t>2596</t>
+      <c r="AY70" t="n">
+        <v>2596</v>
+      </c>
+      <c r="AZ70" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA70" t="inlineStr">
+        <is>
+          <t>3061</t>
         </is>
       </c>
     </row>
@@ -11757,9 +12169,15 @@
       <c r="AX71" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="AY71" t="inlineStr">
-        <is>
-          <t>4264</t>
+      <c r="AY71" t="n">
+        <v>4264</v>
+      </c>
+      <c r="AZ71" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BA71" t="inlineStr">
+        <is>
+          <t>4634</t>
         </is>
       </c>
     </row>
@@ -11920,9 +12338,15 @@
       <c r="AX72" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="AY72" t="inlineStr">
-        <is>
-          <t>3601</t>
+      <c r="AY72" t="n">
+        <v>3601</v>
+      </c>
+      <c r="AZ72" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="BA72" t="inlineStr">
+        <is>
+          <t>3877</t>
         </is>
       </c>
     </row>
@@ -12083,9 +12507,15 @@
       <c r="AX73" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AY73" t="inlineStr">
-        <is>
-          <t>4032</t>
+      <c r="AY73" t="n">
+        <v>4032</v>
+      </c>
+      <c r="AZ73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA73" t="inlineStr">
+        <is>
+          <t>4300</t>
         </is>
       </c>
     </row>
@@ -12246,9 +12676,15 @@
       <c r="AX74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY74" t="inlineStr">
-        <is>
-          <t>2972</t>
+      <c r="AY74" t="n">
+        <v>2972</v>
+      </c>
+      <c r="AZ74" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA74" t="inlineStr">
+        <is>
+          <t>3531</t>
         </is>
       </c>
     </row>
@@ -12409,9 +12845,15 @@
       <c r="AX75" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="AY75" t="inlineStr">
-        <is>
-          <t>3807</t>
+      <c r="AY75" t="n">
+        <v>3807</v>
+      </c>
+      <c r="AZ75" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BA75" t="inlineStr">
+        <is>
+          <t>4035</t>
         </is>
       </c>
     </row>
@@ -12572,9 +13014,15 @@
       <c r="AX76" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AY76" t="inlineStr">
-        <is>
-          <t>4669</t>
+      <c r="AY76" t="n">
+        <v>4669</v>
+      </c>
+      <c r="AZ76" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA76" t="inlineStr">
+        <is>
+          <t>4987</t>
         </is>
       </c>
     </row>
@@ -12735,7 +13183,13 @@
       <c r="AX77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY77" t="inlineStr">
+      <c r="AY77" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA77" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12898,9 +13352,15 @@
       <c r="AX78" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AY78" t="inlineStr">
-        <is>
-          <t>4588</t>
+      <c r="AY78" t="n">
+        <v>4588</v>
+      </c>
+      <c r="AZ78" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BA78" t="inlineStr">
+        <is>
+          <t>4865</t>
         </is>
       </c>
     </row>
@@ -13061,7 +13521,13 @@
       <c r="AX79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY79" t="inlineStr">
+      <c r="AY79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13224,9 +13690,15 @@
       <c r="AX80" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="AY80" t="inlineStr">
-        <is>
-          <t>4455</t>
+      <c r="AY80" t="n">
+        <v>4455</v>
+      </c>
+      <c r="AZ80" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="BA80" t="inlineStr">
+        <is>
+          <t>4783</t>
         </is>
       </c>
     </row>
@@ -13387,9 +13859,15 @@
       <c r="AX81" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AY81" t="inlineStr">
-        <is>
-          <t>4558</t>
+      <c r="AY81" t="n">
+        <v>4558</v>
+      </c>
+      <c r="AZ81" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BA81" t="inlineStr">
+        <is>
+          <t>4979</t>
         </is>
       </c>
     </row>
@@ -13550,9 +14028,15 @@
       <c r="AX82" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AY82" t="inlineStr">
-        <is>
-          <t>4484</t>
+      <c r="AY82" t="n">
+        <v>4484</v>
+      </c>
+      <c r="AZ82" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BA82" t="inlineStr">
+        <is>
+          <t>4636</t>
         </is>
       </c>
     </row>
@@ -13713,9 +14197,15 @@
       <c r="AX83" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AY83" t="inlineStr">
-        <is>
-          <t>4116</t>
+      <c r="AY83" t="n">
+        <v>4116</v>
+      </c>
+      <c r="AZ83" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BA83" t="inlineStr">
+        <is>
+          <t>4421</t>
         </is>
       </c>
     </row>
@@ -13843,6 +14333,8 @@
       <c r="AW84" t="inlineStr"/>
       <c r="AX84" s="3" t="inlineStr"/>
       <c r="AY84" t="inlineStr"/>
+      <c r="AZ84" s="3" t="inlineStr"/>
+      <c r="BA84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -14001,9 +14493,15 @@
       <c r="AX85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY85" t="inlineStr">
-        <is>
-          <t>3595</t>
+      <c r="AY85" t="n">
+        <v>3595</v>
+      </c>
+      <c r="AZ85" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA85" t="inlineStr">
+        <is>
+          <t>3889</t>
         </is>
       </c>
     </row>
@@ -14164,9 +14662,15 @@
       <c r="AX86" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="AY86" t="inlineStr">
-        <is>
-          <t>2992</t>
+      <c r="AY86" t="n">
+        <v>2992</v>
+      </c>
+      <c r="AZ86" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA86" t="inlineStr">
+        <is>
+          <t>3352</t>
         </is>
       </c>
     </row>
@@ -14327,9 +14831,15 @@
       <c r="AX87" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AY87" t="inlineStr">
-        <is>
-          <t>4264</t>
+      <c r="AY87" t="n">
+        <v>4264</v>
+      </c>
+      <c r="AZ87" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA87" t="inlineStr">
+        <is>
+          <t>4579</t>
         </is>
       </c>
     </row>
@@ -14490,9 +15000,15 @@
       <c r="AX88" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AY88" t="inlineStr">
-        <is>
-          <t>2683</t>
+      <c r="AY88" t="n">
+        <v>2683</v>
+      </c>
+      <c r="AZ88" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA88" t="inlineStr">
+        <is>
+          <t>2826</t>
         </is>
       </c>
     </row>
@@ -14653,9 +15169,15 @@
       <c r="AX89" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AY89" t="inlineStr">
-        <is>
-          <t>3122</t>
+      <c r="AY89" t="n">
+        <v>3122</v>
+      </c>
+      <c r="AZ89" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="BA89" t="inlineStr">
+        <is>
+          <t>3312</t>
         </is>
       </c>
     </row>
@@ -14816,9 +15338,15 @@
       <c r="AX90" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="AY90" t="inlineStr">
-        <is>
-          <t>2661</t>
+      <c r="AY90" t="n">
+        <v>2661</v>
+      </c>
+      <c r="AZ90" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="BA90" t="inlineStr">
+        <is>
+          <t>2874</t>
         </is>
       </c>
     </row>
@@ -14979,9 +15507,15 @@
       <c r="AX91" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AY91" t="inlineStr">
-        <is>
-          <t>2860</t>
+      <c r="AY91" t="n">
+        <v>2860</v>
+      </c>
+      <c r="AZ91" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA91" t="inlineStr">
+        <is>
+          <t>3009</t>
         </is>
       </c>
     </row>
@@ -15142,7 +15676,13 @@
       <c r="AX92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY92" t="inlineStr">
+      <c r="AY92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15305,9 +15845,15 @@
       <c r="AX93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY93" t="inlineStr">
-        <is>
-          <t>2296</t>
+      <c r="AY93" t="n">
+        <v>2296</v>
+      </c>
+      <c r="AZ93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA93" t="inlineStr">
+        <is>
+          <t>2294</t>
         </is>
       </c>
     </row>
@@ -15468,9 +16014,15 @@
       <c r="AX94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY94" t="inlineStr">
-        <is>
-          <t>2626</t>
+      <c r="AY94" t="n">
+        <v>2626</v>
+      </c>
+      <c r="AZ94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA94" t="inlineStr">
+        <is>
+          <t>2740</t>
         </is>
       </c>
     </row>
@@ -15631,9 +16183,15 @@
       <c r="AX95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY95" t="inlineStr">
-        <is>
-          <t>2484</t>
+      <c r="AY95" t="n">
+        <v>2484</v>
+      </c>
+      <c r="AZ95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA95" t="inlineStr">
+        <is>
+          <t>2528</t>
         </is>
       </c>
     </row>
@@ -15794,9 +16352,15 @@
       <c r="AX96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY96" t="inlineStr">
-        <is>
-          <t>2474</t>
+      <c r="AY96" t="n">
+        <v>2474</v>
+      </c>
+      <c r="AZ96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA96" t="inlineStr">
+        <is>
+          <t>2467</t>
         </is>
       </c>
     </row>
@@ -15957,9 +16521,15 @@
       <c r="AX97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY97" t="inlineStr">
-        <is>
-          <t>3014</t>
+      <c r="AY97" t="n">
+        <v>3014</v>
+      </c>
+      <c r="AZ97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA97" t="inlineStr">
+        <is>
+          <t>3189</t>
         </is>
       </c>
     </row>
@@ -16120,7 +16690,13 @@
       <c r="AX98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY98" t="inlineStr">
+      <c r="AY98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16283,9 +16859,15 @@
       <c r="AX99" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AY99" t="inlineStr">
-        <is>
-          <t>3578</t>
+      <c r="AY99" t="n">
+        <v>3578</v>
+      </c>
+      <c r="AZ99" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="BA99" t="inlineStr">
+        <is>
+          <t>3684</t>
         </is>
       </c>
     </row>
@@ -16446,9 +17028,15 @@
       <c r="AX100" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="AY100" t="inlineStr">
-        <is>
-          <t>2409</t>
+      <c r="AY100" t="n">
+        <v>2409</v>
+      </c>
+      <c r="AZ100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA100" t="inlineStr">
+        <is>
+          <t>2484</t>
         </is>
       </c>
     </row>
@@ -16609,9 +17197,15 @@
       <c r="AX101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AY101" t="inlineStr">
-        <is>
-          <t>4227</t>
+      <c r="AY101" t="n">
+        <v>4227</v>
+      </c>
+      <c r="AZ101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BA101" t="inlineStr">
+        <is>
+          <t>4502</t>
         </is>
       </c>
     </row>
@@ -16772,9 +17366,15 @@
       <c r="AX102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AY102" t="inlineStr">
-        <is>
-          <t>3762</t>
+      <c r="AY102" t="n">
+        <v>3762</v>
+      </c>
+      <c r="AZ102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA102" t="inlineStr">
+        <is>
+          <t>3963</t>
         </is>
       </c>
     </row>
@@ -16935,9 +17535,15 @@
       <c r="AX103" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AY103" t="inlineStr">
-        <is>
-          <t>3610</t>
+      <c r="AY103" t="n">
+        <v>3610</v>
+      </c>
+      <c r="AZ103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA103" t="inlineStr">
+        <is>
+          <t>3766</t>
         </is>
       </c>
     </row>
@@ -17098,9 +17704,15 @@
       <c r="AX104" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AY104" t="inlineStr">
-        <is>
-          <t>4281</t>
+      <c r="AY104" t="n">
+        <v>4281</v>
+      </c>
+      <c r="AZ104" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BA104" t="inlineStr">
+        <is>
+          <t>4546</t>
         </is>
       </c>
     </row>
@@ -17261,9 +17873,15 @@
       <c r="AX105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY105" t="inlineStr">
-        <is>
-          <t>3794</t>
+      <c r="AY105" t="n">
+        <v>3794</v>
+      </c>
+      <c r="AZ105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA105" t="inlineStr">
+        <is>
+          <t>4023</t>
         </is>
       </c>
     </row>
@@ -17424,7 +18042,13 @@
       <c r="AX106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY106" t="inlineStr">
+      <c r="AY106" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -17587,9 +18211,15 @@
       <c r="AX107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY107" t="inlineStr">
-        <is>
-          <t>2511</t>
+      <c r="AY107" t="n">
+        <v>2511</v>
+      </c>
+      <c r="AZ107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA107" t="inlineStr">
+        <is>
+          <t>2581</t>
         </is>
       </c>
     </row>
@@ -17750,7 +18380,13 @@
       <c r="AX108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY108" t="inlineStr">
+      <c r="AY108" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -17913,9 +18549,15 @@
       <c r="AX109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY109" t="inlineStr">
-        <is>
-          <t>3650</t>
+      <c r="AY109" t="n">
+        <v>3650</v>
+      </c>
+      <c r="AZ109" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="BA109" t="inlineStr">
+        <is>
+          <t>3896</t>
         </is>
       </c>
     </row>
@@ -18076,9 +18718,15 @@
       <c r="AX110" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="AY110" t="inlineStr">
-        <is>
-          <t>3608</t>
+      <c r="AY110" t="n">
+        <v>3608</v>
+      </c>
+      <c r="AZ110" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BA110" t="inlineStr">
+        <is>
+          <t>3786</t>
         </is>
       </c>
     </row>
@@ -18230,6 +18878,8 @@
       <c r="AW111" t="inlineStr"/>
       <c r="AX111" s="3" t="inlineStr"/>
       <c r="AY111" t="inlineStr"/>
+      <c r="AZ111" s="3" t="inlineStr"/>
+      <c r="BA111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -18388,9 +19038,15 @@
       <c r="AX112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY112" t="inlineStr">
-        <is>
-          <t>2555</t>
+      <c r="AY112" t="n">
+        <v>2555</v>
+      </c>
+      <c r="AZ112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA112" t="inlineStr">
+        <is>
+          <t>2612</t>
         </is>
       </c>
     </row>
@@ -18551,9 +19207,15 @@
       <c r="AX113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY113" t="inlineStr">
-        <is>
-          <t>3408</t>
+      <c r="AY113" t="n">
+        <v>3408</v>
+      </c>
+      <c r="AZ113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA113" t="inlineStr">
+        <is>
+          <t>3535</t>
         </is>
       </c>
     </row>
@@ -18714,9 +19376,15 @@
       <c r="AX114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY114" t="inlineStr">
-        <is>
-          <t>3470</t>
+      <c r="AY114" t="n">
+        <v>3470</v>
+      </c>
+      <c r="AZ114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA114" t="inlineStr">
+        <is>
+          <t>3625</t>
         </is>
       </c>
     </row>
@@ -18877,9 +19545,15 @@
       <c r="AX115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY115" t="inlineStr">
-        <is>
-          <t>2006</t>
+      <c r="AY115" t="n">
+        <v>2006</v>
+      </c>
+      <c r="AZ115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA115" t="inlineStr">
+        <is>
+          <t>2007</t>
         </is>
       </c>
     </row>
@@ -19040,9 +19714,15 @@
       <c r="AX116" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="AY116" t="inlineStr">
-        <is>
-          <t>3005</t>
+      <c r="AY116" t="n">
+        <v>3005</v>
+      </c>
+      <c r="AZ116" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="BA116" t="inlineStr">
+        <is>
+          <t>3183</t>
         </is>
       </c>
     </row>
@@ -19203,9 +19883,15 @@
       <c r="AX117" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AY117" t="inlineStr">
-        <is>
-          <t>3536</t>
+      <c r="AY117" t="n">
+        <v>3536</v>
+      </c>
+      <c r="AZ117" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="BA117" t="inlineStr">
+        <is>
+          <t>3696</t>
         </is>
       </c>
     </row>
@@ -19366,7 +20052,13 @@
       <c r="AX118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY118" t="inlineStr">
+      <c r="AY118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -19529,9 +20221,15 @@
       <c r="AX119" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AY119" t="inlineStr">
-        <is>
-          <t>3901</t>
+      <c r="AY119" t="n">
+        <v>3901</v>
+      </c>
+      <c r="AZ119" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BA119" t="inlineStr">
+        <is>
+          <t>3989</t>
         </is>
       </c>
     </row>
@@ -19692,9 +20390,15 @@
       <c r="AX120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY120" t="inlineStr">
-        <is>
-          <t>2475</t>
+      <c r="AY120" t="n">
+        <v>2475</v>
+      </c>
+      <c r="AZ120" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA120" t="inlineStr">
+        <is>
+          <t>2712</t>
         </is>
       </c>
     </row>
@@ -19855,9 +20559,15 @@
       <c r="AX121" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="AY121" t="inlineStr">
-        <is>
-          <t>3147</t>
+      <c r="AY121" t="n">
+        <v>3147</v>
+      </c>
+      <c r="AZ121" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="BA121" t="inlineStr">
+        <is>
+          <t>3372</t>
         </is>
       </c>
     </row>
@@ -20018,7 +20728,13 @@
       <c r="AX122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY122" t="inlineStr">
+      <c r="AY122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -20181,9 +20897,15 @@
       <c r="AX123" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="AY123" t="inlineStr">
-        <is>
-          <t>3142</t>
+      <c r="AY123" t="n">
+        <v>3142</v>
+      </c>
+      <c r="AZ123" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="BA123" t="inlineStr">
+        <is>
+          <t>3338</t>
         </is>
       </c>
     </row>
@@ -20344,9 +21066,15 @@
       <c r="AX124" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="AY124" t="inlineStr">
-        <is>
-          <t>3210</t>
+      <c r="AY124" t="n">
+        <v>3210</v>
+      </c>
+      <c r="AZ124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA124" t="inlineStr">
+        <is>
+          <t>3347</t>
         </is>
       </c>
     </row>
@@ -20507,9 +21235,15 @@
       <c r="AX125" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AY125" t="inlineStr">
-        <is>
-          <t>3182</t>
+      <c r="AY125" t="n">
+        <v>3182</v>
+      </c>
+      <c r="AZ125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA125" t="inlineStr">
+        <is>
+          <t>3440</t>
         </is>
       </c>
     </row>
@@ -20670,9 +21404,15 @@
       <c r="AX126" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AY126" t="inlineStr">
-        <is>
-          <t>3193</t>
+      <c r="AY126" t="n">
+        <v>3193</v>
+      </c>
+      <c r="AZ126" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="BA126" t="inlineStr">
+        <is>
+          <t>3219</t>
         </is>
       </c>
     </row>
@@ -20833,9 +21573,15 @@
       <c r="AX127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY127" t="inlineStr">
-        <is>
-          <t>2291</t>
+      <c r="AY127" t="n">
+        <v>2291</v>
+      </c>
+      <c r="AZ127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA127" t="inlineStr">
+        <is>
+          <t>2263</t>
         </is>
       </c>
     </row>
@@ -20996,7 +21742,13 @@
       <c r="AX128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY128" t="inlineStr">
+      <c r="AY128" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -21159,7 +21911,13 @@
       <c r="AX129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY129" t="inlineStr">
+      <c r="AY129" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -21322,9 +22080,15 @@
       <c r="AX130" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AY130" t="inlineStr">
-        <is>
-          <t>2947</t>
+      <c r="AY130" t="n">
+        <v>2947</v>
+      </c>
+      <c r="AZ130" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA130" t="inlineStr">
+        <is>
+          <t>2998</t>
         </is>
       </c>
     </row>
@@ -21485,7 +22249,13 @@
       <c r="AX131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY131" t="inlineStr">
+      <c r="AY131" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -21648,9 +22418,15 @@
       <c r="AX132" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AY132" t="inlineStr">
-        <is>
-          <t>2681</t>
+      <c r="AY132" t="n">
+        <v>2681</v>
+      </c>
+      <c r="AZ132" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA132" t="inlineStr">
+        <is>
+          <t>2758</t>
         </is>
       </c>
     </row>
@@ -21811,9 +22587,15 @@
       <c r="AX133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY133" t="inlineStr">
-        <is>
-          <t>2762</t>
+      <c r="AY133" t="n">
+        <v>2762</v>
+      </c>
+      <c r="AZ133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA133" t="inlineStr">
+        <is>
+          <t>2779</t>
         </is>
       </c>
     </row>
@@ -21905,6 +22687,8 @@
       <c r="AW134" t="inlineStr"/>
       <c r="AX134" s="3" t="inlineStr"/>
       <c r="AY134" t="inlineStr"/>
+      <c r="AZ134" s="3" t="inlineStr"/>
+      <c r="BA134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -21986,6 +22770,8 @@
       <c r="AW135" t="inlineStr"/>
       <c r="AX135" s="3" t="inlineStr"/>
       <c r="AY135" t="inlineStr"/>
+      <c r="AZ135" s="3" t="inlineStr"/>
+      <c r="BA135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -22144,7 +22930,13 @@
       <c r="AX136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY136" t="inlineStr">
+      <c r="AY136" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA136" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -22307,7 +23099,13 @@
       <c r="AX137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY137" t="inlineStr">
+      <c r="AY137" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -22393,6 +23191,8 @@
       <c r="AW138" t="inlineStr"/>
       <c r="AX138" s="3" t="inlineStr"/>
       <c r="AY138" t="inlineStr"/>
+      <c r="AZ138" s="3" t="inlineStr"/>
+      <c r="BA138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -22551,9 +23351,15 @@
       <c r="AX139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY139" t="inlineStr">
-        <is>
-          <t>2089</t>
+      <c r="AY139" t="n">
+        <v>2089</v>
+      </c>
+      <c r="AZ139" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="BA139" t="inlineStr">
+        <is>
+          <t>2542</t>
         </is>
       </c>
     </row>
@@ -22714,9 +23520,15 @@
       <c r="AX140" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AY140" t="inlineStr">
-        <is>
-          <t>2806</t>
+      <c r="AY140" t="n">
+        <v>2806</v>
+      </c>
+      <c r="AZ140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA140" t="inlineStr">
+        <is>
+          <t>2903</t>
         </is>
       </c>
     </row>
@@ -22800,6 +23612,8 @@
       <c r="AW141" t="inlineStr"/>
       <c r="AX141" s="3" t="inlineStr"/>
       <c r="AY141" t="inlineStr"/>
+      <c r="AZ141" s="3" t="inlineStr"/>
+      <c r="BA141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -22958,7 +23772,13 @@
       <c r="AX142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY142" t="inlineStr">
+      <c r="AY142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA142" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -23044,6 +23864,8 @@
       <c r="AW143" t="inlineStr"/>
       <c r="AX143" s="3" t="inlineStr"/>
       <c r="AY143" t="inlineStr"/>
+      <c r="AZ143" s="3" t="inlineStr"/>
+      <c r="BA143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -23125,6 +23947,8 @@
       <c r="AW144" t="inlineStr"/>
       <c r="AX144" s="3" t="inlineStr"/>
       <c r="AY144" t="inlineStr"/>
+      <c r="AZ144" s="3" t="inlineStr"/>
+      <c r="BA144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -23206,6 +24030,8 @@
       <c r="AW145" t="inlineStr"/>
       <c r="AX145" s="3" t="inlineStr"/>
       <c r="AY145" t="inlineStr"/>
+      <c r="AZ145" s="3" t="inlineStr"/>
+      <c r="BA145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -23287,6 +24113,8 @@
       <c r="AW146" t="inlineStr"/>
       <c r="AX146" s="3" t="inlineStr"/>
       <c r="AY146" t="inlineStr"/>
+      <c r="AZ146" s="3" t="inlineStr"/>
+      <c r="BA146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -23368,6 +24196,8 @@
       <c r="AW147" t="inlineStr"/>
       <c r="AX147" s="3" t="inlineStr"/>
       <c r="AY147" t="inlineStr"/>
+      <c r="AZ147" s="3" t="inlineStr"/>
+      <c r="BA147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -23526,7 +24356,13 @@
       <c r="AX148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY148" t="inlineStr">
+      <c r="AY148" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -23689,7 +24525,13 @@
       <c r="AX149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY149" t="inlineStr">
+      <c r="AY149" t="n">
+        <v>3727</v>
+      </c>
+      <c r="AZ149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA149" t="inlineStr">
         <is>
           <t>3727</t>
         </is>
@@ -23852,7 +24694,13 @@
       <c r="AX150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY150" t="inlineStr">
+      <c r="AY150" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -24015,9 +24863,15 @@
       <c r="AX151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY151" t="inlineStr">
-        <is>
-          <t>2578</t>
+      <c r="AY151" t="n">
+        <v>2578</v>
+      </c>
+      <c r="AZ151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA151" t="inlineStr">
+        <is>
+          <t>2593</t>
         </is>
       </c>
     </row>
@@ -24178,7 +25032,13 @@
       <c r="AX152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY152" t="inlineStr">
+      <c r="AY152" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -24341,7 +25201,13 @@
       <c r="AX153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY153" t="inlineStr">
+      <c r="AY153" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -24504,7 +25370,13 @@
       <c r="AX154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY154" t="inlineStr">
+      <c r="AY154" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -24667,9 +25539,15 @@
       <c r="AX155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY155" t="inlineStr">
-        <is>
-          <t>2687</t>
+      <c r="AY155" t="n">
+        <v>2687</v>
+      </c>
+      <c r="AZ155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA155" t="inlineStr">
+        <is>
+          <t>2731</t>
         </is>
       </c>
     </row>
@@ -24824,9 +25702,15 @@
       <c r="AX156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY156" t="inlineStr">
-        <is>
-          <t>3169</t>
+      <c r="AY156" t="n">
+        <v>3169</v>
+      </c>
+      <c r="AZ156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA156" t="inlineStr">
+        <is>
+          <t>3195</t>
         </is>
       </c>
     </row>
@@ -24904,6 +25788,8 @@
       <c r="AW157" t="inlineStr"/>
       <c r="AX157" s="3" t="inlineStr"/>
       <c r="AY157" t="inlineStr"/>
+      <c r="AZ157" s="3" t="inlineStr"/>
+      <c r="BA157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -25056,7 +25942,13 @@
       <c r="AX158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY158" t="inlineStr">
+      <c r="AY158" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -25213,9 +26105,15 @@
       <c r="AX159" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="AY159" t="inlineStr">
-        <is>
-          <t>2989</t>
+      <c r="AY159" t="n">
+        <v>2989</v>
+      </c>
+      <c r="AZ159" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA159" t="inlineStr">
+        <is>
+          <t>3113</t>
         </is>
       </c>
     </row>
@@ -25293,6 +26191,8 @@
       <c r="AW160" t="inlineStr"/>
       <c r="AX160" s="3" t="inlineStr"/>
       <c r="AY160" t="inlineStr"/>
+      <c r="AZ160" s="3" t="inlineStr"/>
+      <c r="BA160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -25433,9 +26333,15 @@
       <c r="AX161" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AY161" t="inlineStr">
-        <is>
-          <t>3085</t>
+      <c r="AY161" t="n">
+        <v>3085</v>
+      </c>
+      <c r="AZ161" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BA161" t="inlineStr">
+        <is>
+          <t>3266</t>
         </is>
       </c>
     </row>
@@ -25578,9 +26484,15 @@
       <c r="AX162" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY162" t="inlineStr">
-        <is>
-          <t>2610</t>
+      <c r="AY162" t="n">
+        <v>2610</v>
+      </c>
+      <c r="AZ162" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="BA162" t="inlineStr">
+        <is>
+          <t>2859</t>
         </is>
       </c>
     </row>
@@ -25719,9 +26631,15 @@
       <c r="AX163" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY163" t="inlineStr">
-        <is>
-          <t>3234</t>
+      <c r="AY163" t="n">
+        <v>3234</v>
+      </c>
+      <c r="AZ163" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="BA163" t="inlineStr">
+        <is>
+          <t>3405</t>
         </is>
       </c>
     </row>
@@ -25844,9 +26762,15 @@
       <c r="AX164" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AY164" t="inlineStr">
-        <is>
-          <t>3472</t>
+      <c r="AY164" t="n">
+        <v>3472</v>
+      </c>
+      <c r="AZ164" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="BA164" t="inlineStr">
+        <is>
+          <t>3470</t>
         </is>
       </c>
     </row>
@@ -25973,9 +26897,15 @@
       <c r="AX165" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="AY165" t="inlineStr">
-        <is>
-          <t>2710</t>
+      <c r="AY165" t="n">
+        <v>2710</v>
+      </c>
+      <c r="AZ165" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="BA165" t="inlineStr">
+        <is>
+          <t>2883</t>
         </is>
       </c>
     </row>
@@ -26094,9 +27024,15 @@
       <c r="AX166" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY166" t="inlineStr">
-        <is>
-          <t>2794</t>
+      <c r="AY166" t="n">
+        <v>2794</v>
+      </c>
+      <c r="AZ166" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA166" t="inlineStr">
+        <is>
+          <t>2782</t>
         </is>
       </c>
     </row>
@@ -26203,7 +27139,13 @@
       <c r="AX167" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY167" t="inlineStr">
+      <c r="AY167" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ167" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA167" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -26308,7 +27250,13 @@
       <c r="AX168" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY168" t="inlineStr">
+      <c r="AY168" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ168" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA168" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -26380,6 +27328,8 @@
       <c r="AW169" t="inlineStr"/>
       <c r="AX169" s="3" t="inlineStr"/>
       <c r="AY169" t="inlineStr"/>
+      <c r="AZ169" s="3" t="inlineStr"/>
+      <c r="BA169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="n">
@@ -26476,7 +27426,13 @@
       <c r="AX170" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY170" t="inlineStr">
+      <c r="AY170" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ170" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA170" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -26565,9 +27521,15 @@
       <c r="AX171" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="AY171" t="inlineStr">
-        <is>
-          <t>1719</t>
+      <c r="AY171" t="n">
+        <v>1719</v>
+      </c>
+      <c r="AZ171" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA171" t="inlineStr">
+        <is>
+          <t>1781</t>
         </is>
       </c>
     </row>
@@ -26654,7 +27616,13 @@
       <c r="AX172" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY172" t="inlineStr">
+      <c r="AY172" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ172" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA172" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -26743,9 +27711,88 @@
       <c r="AX173" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="AY173" t="inlineStr">
-        <is>
-          <t>1932</t>
+      <c r="AY173" t="n">
+        <v>1932</v>
+      </c>
+      <c r="AZ173" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA173" t="inlineStr">
+        <is>
+          <t>1872</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>50975641</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>"dit nhau"</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr"/>
+      <c r="D174" t="inlineStr"/>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F174" s="3" t="inlineStr"/>
+      <c r="G174" t="inlineStr"/>
+      <c r="H174" s="3" t="inlineStr"/>
+      <c r="I174" t="inlineStr"/>
+      <c r="J174" s="3" t="inlineStr"/>
+      <c r="K174" t="inlineStr"/>
+      <c r="L174" s="3" t="inlineStr"/>
+      <c r="M174" t="inlineStr"/>
+      <c r="N174" s="3" t="inlineStr"/>
+      <c r="O174" t="inlineStr"/>
+      <c r="P174" s="3" t="inlineStr"/>
+      <c r="Q174" t="inlineStr"/>
+      <c r="R174" s="3" t="inlineStr"/>
+      <c r="S174" t="inlineStr"/>
+      <c r="T174" s="3" t="inlineStr"/>
+      <c r="U174" t="inlineStr"/>
+      <c r="V174" s="3" t="inlineStr"/>
+      <c r="W174" t="inlineStr"/>
+      <c r="X174" s="3" t="inlineStr"/>
+      <c r="Y174" t="inlineStr"/>
+      <c r="Z174" s="3" t="inlineStr"/>
+      <c r="AA174" t="inlineStr"/>
+      <c r="AB174" s="3" t="inlineStr"/>
+      <c r="AC174" t="inlineStr"/>
+      <c r="AD174" s="3" t="inlineStr"/>
+      <c r="AE174" t="inlineStr"/>
+      <c r="AF174" s="3" t="inlineStr"/>
+      <c r="AG174" t="inlineStr"/>
+      <c r="AH174" s="3" t="inlineStr"/>
+      <c r="AI174" t="inlineStr"/>
+      <c r="AJ174" s="3" t="inlineStr"/>
+      <c r="AK174" t="inlineStr"/>
+      <c r="AL174" s="3" t="inlineStr"/>
+      <c r="AM174" t="inlineStr"/>
+      <c r="AN174" s="3" t="inlineStr"/>
+      <c r="AO174" t="inlineStr"/>
+      <c r="AP174" s="3" t="inlineStr"/>
+      <c r="AQ174" t="inlineStr"/>
+      <c r="AR174" s="3" t="inlineStr"/>
+      <c r="AS174" t="inlineStr"/>
+      <c r="AT174" s="3" t="inlineStr"/>
+      <c r="AU174" t="inlineStr"/>
+      <c r="AV174" s="3" t="inlineStr"/>
+      <c r="AW174" t="inlineStr"/>
+      <c r="AX174" s="3" t="inlineStr"/>
+      <c r="AY174" t="inlineStr"/>
+      <c r="AZ174" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA174" t="inlineStr">
+        <is>
+          <t>3229</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-03-09 13:56:50
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -27724,10 +27724,8 @@
       </c>
     </row>
     <row r="174">
-      <c r="A174" t="inlineStr">
-        <is>
-          <t>50975641</t>
-        </is>
+      <c r="A174" t="n">
+        <v>50975641</v>
       </c>
       <c r="B174" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Code updated 23-03-10 11:30:34
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BA174"/>
+  <dimension ref="A1:BC174"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -656,6 +656,16 @@
           <t>03-08_0</t>
         </is>
       </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>03-09_A</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>03-09_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -820,9 +830,15 @@
       <c r="AZ2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA2" t="inlineStr">
-        <is>
-          <t>2898</t>
+      <c r="BA2" t="n">
+        <v>2898</v>
+      </c>
+      <c r="BB2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC2" t="inlineStr">
+        <is>
+          <t>2926</t>
         </is>
       </c>
     </row>
@@ -989,9 +1005,15 @@
       <c r="AZ3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BA3" t="inlineStr">
-        <is>
-          <t>6029</t>
+      <c r="BA3" t="n">
+        <v>6029</v>
+      </c>
+      <c r="BB3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC3" t="inlineStr">
+        <is>
+          <t>6170</t>
         </is>
       </c>
     </row>
@@ -1158,9 +1180,15 @@
       <c r="AZ4" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="BA4" t="inlineStr">
-        <is>
-          <t>5891</t>
+      <c r="BA4" t="n">
+        <v>5891</v>
+      </c>
+      <c r="BB4" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="BC4" t="inlineStr">
+        <is>
+          <t>6116</t>
         </is>
       </c>
     </row>
@@ -1327,9 +1355,15 @@
       <c r="AZ5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BA5" t="inlineStr">
-        <is>
-          <t>5536</t>
+      <c r="BA5" t="n">
+        <v>5536</v>
+      </c>
+      <c r="BB5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC5" t="inlineStr">
+        <is>
+          <t>5823</t>
         </is>
       </c>
     </row>
@@ -1496,9 +1530,15 @@
       <c r="AZ6" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="BA6" t="inlineStr">
-        <is>
-          <t>5585</t>
+      <c r="BA6" t="n">
+        <v>5585</v>
+      </c>
+      <c r="BB6" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BC6" t="inlineStr">
+        <is>
+          <t>5838</t>
         </is>
       </c>
     </row>
@@ -1665,9 +1705,15 @@
       <c r="AZ7" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="BA7" t="inlineStr">
-        <is>
-          <t>6171</t>
+      <c r="BA7" t="n">
+        <v>6171</v>
+      </c>
+      <c r="BB7" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="BC7" t="inlineStr">
+        <is>
+          <t>6270</t>
         </is>
       </c>
     </row>
@@ -1834,9 +1880,15 @@
       <c r="AZ8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BA8" t="inlineStr">
-        <is>
-          <t>5116</t>
+      <c r="BA8" t="n">
+        <v>5116</v>
+      </c>
+      <c r="BB8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC8" t="inlineStr">
+        <is>
+          <t>5342</t>
         </is>
       </c>
     </row>
@@ -2003,9 +2055,15 @@
       <c r="AZ9" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BA9" t="inlineStr">
-        <is>
-          <t>5367</t>
+      <c r="BA9" t="n">
+        <v>5367</v>
+      </c>
+      <c r="BB9" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BC9" t="inlineStr">
+        <is>
+          <t>5574</t>
         </is>
       </c>
     </row>
@@ -2172,9 +2230,15 @@
       <c r="AZ10" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BA10" t="inlineStr">
-        <is>
-          <t>6228</t>
+      <c r="BA10" t="n">
+        <v>6228</v>
+      </c>
+      <c r="BB10" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="BC10" t="inlineStr">
+        <is>
+          <t>6595</t>
         </is>
       </c>
     </row>
@@ -2341,9 +2405,15 @@
       <c r="AZ11" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA11" t="inlineStr">
-        <is>
-          <t>4721</t>
+      <c r="BA11" t="n">
+        <v>4721</v>
+      </c>
+      <c r="BB11" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC11" t="inlineStr">
+        <is>
+          <t>4932</t>
         </is>
       </c>
     </row>
@@ -2510,9 +2580,15 @@
       <c r="AZ12" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="BA12" t="inlineStr">
-        <is>
-          <t>2640</t>
+      <c r="BA12" t="n">
+        <v>2640</v>
+      </c>
+      <c r="BB12" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="BC12" t="inlineStr">
+        <is>
+          <t>2752</t>
         </is>
       </c>
     </row>
@@ -2679,9 +2755,15 @@
       <c r="AZ13" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="BA13" t="inlineStr">
-        <is>
-          <t>6277</t>
+      <c r="BA13" t="n">
+        <v>6277</v>
+      </c>
+      <c r="BB13" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="BC13" t="inlineStr">
+        <is>
+          <t>6642</t>
         </is>
       </c>
     </row>
@@ -2848,9 +2930,15 @@
       <c r="AZ14" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="BA14" t="inlineStr">
-        <is>
-          <t>5450</t>
+      <c r="BA14" t="n">
+        <v>5450</v>
+      </c>
+      <c r="BB14" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BC14" t="inlineStr">
+        <is>
+          <t>5683</t>
         </is>
       </c>
     </row>
@@ -3017,7 +3105,13 @@
       <c r="AZ15" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA15" t="inlineStr">
+      <c r="BA15" t="n">
+        <v>2743</v>
+      </c>
+      <c r="BB15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC15" t="inlineStr">
         <is>
           <t>2743</t>
         </is>
@@ -3186,9 +3280,15 @@
       <c r="AZ16" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BA16" t="inlineStr">
-        <is>
-          <t>5692</t>
+      <c r="BA16" t="n">
+        <v>5692</v>
+      </c>
+      <c r="BB16" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BC16" t="inlineStr">
+        <is>
+          <t>5988</t>
         </is>
       </c>
     </row>
@@ -3355,9 +3455,15 @@
       <c r="AZ17" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BA17" t="inlineStr">
-        <is>
-          <t>4279</t>
+      <c r="BA17" t="n">
+        <v>4279</v>
+      </c>
+      <c r="BB17" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BC17" t="inlineStr">
+        <is>
+          <t>4310</t>
         </is>
       </c>
     </row>
@@ -3524,9 +3630,15 @@
       <c r="AZ18" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="BA18" t="inlineStr">
-        <is>
-          <t>4878</t>
+      <c r="BA18" t="n">
+        <v>4878</v>
+      </c>
+      <c r="BB18" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="BC18" t="inlineStr">
+        <is>
+          <t>5069</t>
         </is>
       </c>
     </row>
@@ -3693,9 +3805,15 @@
       <c r="AZ19" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BA19" t="inlineStr">
-        <is>
-          <t>5763</t>
+      <c r="BA19" t="n">
+        <v>5763</v>
+      </c>
+      <c r="BB19" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BC19" t="inlineStr">
+        <is>
+          <t>6129</t>
         </is>
       </c>
     </row>
@@ -3862,9 +3980,15 @@
       <c r="AZ20" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BA20" t="inlineStr">
-        <is>
-          <t>6387</t>
+      <c r="BA20" t="n">
+        <v>6387</v>
+      </c>
+      <c r="BB20" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="BC20" t="inlineStr">
+        <is>
+          <t>6680</t>
         </is>
       </c>
     </row>
@@ -4031,9 +4155,15 @@
       <c r="AZ21" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="BA21" t="inlineStr">
-        <is>
-          <t>4680</t>
+      <c r="BA21" t="n">
+        <v>4680</v>
+      </c>
+      <c r="BB21" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="BC21" t="inlineStr">
+        <is>
+          <t>5116</t>
         </is>
       </c>
     </row>
@@ -4200,9 +4330,15 @@
       <c r="AZ22" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="BA22" t="inlineStr">
-        <is>
-          <t>5468</t>
+      <c r="BA22" t="n">
+        <v>5468</v>
+      </c>
+      <c r="BB22" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="BC22" t="inlineStr">
+        <is>
+          <t>5690</t>
         </is>
       </c>
     </row>
@@ -4369,7 +4505,13 @@
       <c r="AZ23" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BA23" t="inlineStr">
+      <c r="BA23" t="n">
+        <v>4867</v>
+      </c>
+      <c r="BB23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC23" t="inlineStr">
         <is>
           <t>4867</t>
         </is>
@@ -4538,9 +4680,15 @@
       <c r="AZ24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BA24" t="inlineStr">
-        <is>
-          <t>5835</t>
+      <c r="BA24" t="n">
+        <v>5835</v>
+      </c>
+      <c r="BB24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BC24" t="inlineStr">
+        <is>
+          <t>6051</t>
         </is>
       </c>
     </row>
@@ -4707,7 +4855,13 @@
       <c r="AZ25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA25" t="inlineStr">
+      <c r="BA25" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4876,9 +5030,15 @@
       <c r="AZ26" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="BA26" t="inlineStr">
-        <is>
-          <t>5819</t>
+      <c r="BA26" t="n">
+        <v>5819</v>
+      </c>
+      <c r="BB26" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="BC26" t="inlineStr">
+        <is>
+          <t>6044</t>
         </is>
       </c>
     </row>
@@ -5045,9 +5205,15 @@
       <c r="AZ27" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BA27" t="inlineStr">
-        <is>
-          <t>5785</t>
+      <c r="BA27" t="n">
+        <v>5785</v>
+      </c>
+      <c r="BB27" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC27" t="inlineStr">
+        <is>
+          <t>6048</t>
         </is>
       </c>
     </row>
@@ -5214,9 +5380,15 @@
       <c r="AZ28" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="BA28" t="inlineStr">
-        <is>
-          <t>5443</t>
+      <c r="BA28" t="n">
+        <v>5443</v>
+      </c>
+      <c r="BB28" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="BC28" t="inlineStr">
+        <is>
+          <t>5863</t>
         </is>
       </c>
     </row>
@@ -5383,9 +5555,15 @@
       <c r="AZ29" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BA29" t="inlineStr">
-        <is>
-          <t>6115</t>
+      <c r="BA29" t="n">
+        <v>6115</v>
+      </c>
+      <c r="BB29" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BC29" t="inlineStr">
+        <is>
+          <t>6462</t>
         </is>
       </c>
     </row>
@@ -5552,9 +5730,15 @@
       <c r="AZ30" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BA30" t="inlineStr">
-        <is>
-          <t>5343</t>
+      <c r="BA30" t="n">
+        <v>5343</v>
+      </c>
+      <c r="BB30" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="BC30" t="inlineStr">
+        <is>
+          <t>5587</t>
         </is>
       </c>
     </row>
@@ -5721,9 +5905,15 @@
       <c r="AZ31" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="BA31" t="inlineStr">
-        <is>
-          <t>6164</t>
+      <c r="BA31" t="n">
+        <v>6164</v>
+      </c>
+      <c r="BB31" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="BC31" t="inlineStr">
+        <is>
+          <t>6574</t>
         </is>
       </c>
     </row>
@@ -5890,9 +6080,15 @@
       <c r="AZ32" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="BA32" t="inlineStr">
-        <is>
-          <t>6009</t>
+      <c r="BA32" t="n">
+        <v>6009</v>
+      </c>
+      <c r="BB32" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="BC32" t="inlineStr">
+        <is>
+          <t>6289</t>
         </is>
       </c>
     </row>
@@ -6059,9 +6255,15 @@
       <c r="AZ33" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BA33" t="inlineStr">
-        <is>
-          <t>5370</t>
+      <c r="BA33" t="n">
+        <v>5370</v>
+      </c>
+      <c r="BB33" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC33" t="inlineStr">
+        <is>
+          <t>5647</t>
         </is>
       </c>
     </row>
@@ -6228,9 +6430,15 @@
       <c r="AZ34" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BA34" t="inlineStr">
-        <is>
-          <t>5388</t>
+      <c r="BA34" t="n">
+        <v>5388</v>
+      </c>
+      <c r="BB34" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BC34" t="inlineStr">
+        <is>
+          <t>5573</t>
         </is>
       </c>
     </row>
@@ -6397,9 +6605,15 @@
       <c r="AZ35" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="BA35" t="inlineStr">
-        <is>
-          <t>5868</t>
+      <c r="BA35" t="n">
+        <v>5868</v>
+      </c>
+      <c r="BB35" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="BC35" t="inlineStr">
+        <is>
+          <t>6132</t>
         </is>
       </c>
     </row>
@@ -6566,9 +6780,15 @@
       <c r="AZ36" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BA36" t="inlineStr">
-        <is>
-          <t>5424</t>
+      <c r="BA36" t="n">
+        <v>5424</v>
+      </c>
+      <c r="BB36" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC36" t="inlineStr">
+        <is>
+          <t>5661</t>
         </is>
       </c>
     </row>
@@ -6735,9 +6955,15 @@
       <c r="AZ37" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BA37" t="inlineStr">
-        <is>
-          <t>4457</t>
+      <c r="BA37" t="n">
+        <v>4457</v>
+      </c>
+      <c r="BB37" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="BC37" t="inlineStr">
+        <is>
+          <t>4576</t>
         </is>
       </c>
     </row>
@@ -6904,9 +7130,15 @@
       <c r="AZ38" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="BA38" t="inlineStr">
-        <is>
-          <t>5400</t>
+      <c r="BA38" t="n">
+        <v>5400</v>
+      </c>
+      <c r="BB38" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BC38" t="inlineStr">
+        <is>
+          <t>5617</t>
         </is>
       </c>
     </row>
@@ -7073,9 +7305,15 @@
       <c r="AZ39" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="BA39" t="inlineStr">
-        <is>
-          <t>5381</t>
+      <c r="BA39" t="n">
+        <v>5381</v>
+      </c>
+      <c r="BB39" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BC39" t="inlineStr">
+        <is>
+          <t>5853</t>
         </is>
       </c>
     </row>
@@ -7242,9 +7480,15 @@
       <c r="AZ40" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BA40" t="inlineStr">
-        <is>
-          <t>6084</t>
+      <c r="BA40" t="n">
+        <v>6084</v>
+      </c>
+      <c r="BB40" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BC40" t="inlineStr">
+        <is>
+          <t>6462</t>
         </is>
       </c>
     </row>
@@ -7411,7 +7655,13 @@
       <c r="AZ41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA41" t="inlineStr">
+      <c r="BA41" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC41" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7580,9 +7830,15 @@
       <c r="AZ42" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="BA42" t="inlineStr">
-        <is>
-          <t>6447</t>
+      <c r="BA42" t="n">
+        <v>6447</v>
+      </c>
+      <c r="BB42" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="BC42" t="inlineStr">
+        <is>
+          <t>6625</t>
         </is>
       </c>
     </row>
@@ -7749,9 +8005,15 @@
       <c r="AZ43" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BA43" t="inlineStr">
-        <is>
-          <t>5569</t>
+      <c r="BA43" t="n">
+        <v>5569</v>
+      </c>
+      <c r="BB43" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BC43" t="inlineStr">
+        <is>
+          <t>5813</t>
         </is>
       </c>
     </row>
@@ -7918,9 +8180,15 @@
       <c r="AZ44" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BA44" t="inlineStr">
-        <is>
-          <t>5518</t>
+      <c r="BA44" t="n">
+        <v>5518</v>
+      </c>
+      <c r="BB44" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BC44" t="inlineStr">
+        <is>
+          <t>5793</t>
         </is>
       </c>
     </row>
@@ -8087,9 +8355,15 @@
       <c r="AZ45" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="BA45" t="inlineStr">
-        <is>
-          <t>4849</t>
+      <c r="BA45" t="n">
+        <v>4849</v>
+      </c>
+      <c r="BB45" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="BC45" t="inlineStr">
+        <is>
+          <t>5462</t>
         </is>
       </c>
     </row>
@@ -8256,9 +8530,15 @@
       <c r="AZ46" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="BA46" t="inlineStr">
-        <is>
-          <t>5079</t>
+      <c r="BA46" t="n">
+        <v>5079</v>
+      </c>
+      <c r="BB46" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BC46" t="inlineStr">
+        <is>
+          <t>5366</t>
         </is>
       </c>
     </row>
@@ -8425,9 +8705,15 @@
       <c r="AZ47" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="BA47" t="inlineStr">
-        <is>
-          <t>4418</t>
+      <c r="BA47" t="n">
+        <v>4418</v>
+      </c>
+      <c r="BB47" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC47" t="inlineStr">
+        <is>
+          <t>4654</t>
         </is>
       </c>
     </row>
@@ -8594,9 +8880,15 @@
       <c r="AZ48" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="BA48" t="inlineStr">
-        <is>
-          <t>5786</t>
+      <c r="BA48" t="n">
+        <v>5786</v>
+      </c>
+      <c r="BB48" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="BC48" t="inlineStr">
+        <is>
+          <t>6061</t>
         </is>
       </c>
     </row>
@@ -8763,9 +9055,15 @@
       <c r="AZ49" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="BA49" t="inlineStr">
-        <is>
-          <t>4521</t>
+      <c r="BA49" t="n">
+        <v>4521</v>
+      </c>
+      <c r="BB49" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="BC49" t="inlineStr">
+        <is>
+          <t>4840</t>
         </is>
       </c>
     </row>
@@ -8932,9 +9230,15 @@
       <c r="AZ50" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="BA50" t="inlineStr">
-        <is>
-          <t>5897</t>
+      <c r="BA50" t="n">
+        <v>5897</v>
+      </c>
+      <c r="BB50" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BC50" t="inlineStr">
+        <is>
+          <t>6241</t>
         </is>
       </c>
     </row>
@@ -9101,9 +9405,15 @@
       <c r="AZ51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA51" t="inlineStr">
-        <is>
-          <t>2677</t>
+      <c r="BA51" t="n">
+        <v>2677</v>
+      </c>
+      <c r="BB51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC51" t="inlineStr">
+        <is>
+          <t>2676</t>
         </is>
       </c>
     </row>
@@ -9270,9 +9580,15 @@
       <c r="AZ52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA52" t="inlineStr">
-        <is>
-          <t>2770</t>
+      <c r="BA52" t="n">
+        <v>2770</v>
+      </c>
+      <c r="BB52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC52" t="inlineStr">
+        <is>
+          <t>2832</t>
         </is>
       </c>
     </row>
@@ -9439,9 +9755,15 @@
       <c r="AZ53" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="BA53" t="inlineStr">
-        <is>
-          <t>3210</t>
+      <c r="BA53" t="n">
+        <v>3210</v>
+      </c>
+      <c r="BB53" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="BC53" t="inlineStr">
+        <is>
+          <t>3486</t>
         </is>
       </c>
     </row>
@@ -9608,9 +9930,15 @@
       <c r="AZ54" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="BA54" t="inlineStr">
-        <is>
-          <t>5483</t>
+      <c r="BA54" t="n">
+        <v>5483</v>
+      </c>
+      <c r="BB54" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="BC54" t="inlineStr">
+        <is>
+          <t>5750</t>
         </is>
       </c>
     </row>
@@ -9777,9 +10105,15 @@
       <c r="AZ55" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="BA55" t="inlineStr">
-        <is>
-          <t>4148</t>
+      <c r="BA55" t="n">
+        <v>4148</v>
+      </c>
+      <c r="BB55" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BC55" t="inlineStr">
+        <is>
+          <t>4273</t>
         </is>
       </c>
     </row>
@@ -9946,9 +10280,15 @@
       <c r="AZ56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BA56" t="inlineStr">
-        <is>
-          <t>4206</t>
+      <c r="BA56" t="n">
+        <v>4206</v>
+      </c>
+      <c r="BB56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC56" t="inlineStr">
+        <is>
+          <t>4284</t>
         </is>
       </c>
     </row>
@@ -10115,9 +10455,15 @@
       <c r="AZ57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BA57" t="inlineStr">
-        <is>
-          <t>5234</t>
+      <c r="BA57" t="n">
+        <v>5234</v>
+      </c>
+      <c r="BB57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC57" t="inlineStr">
+        <is>
+          <t>5381</t>
         </is>
       </c>
     </row>
@@ -10284,9 +10630,15 @@
       <c r="AZ58" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BA58" t="inlineStr">
-        <is>
-          <t>4481</t>
+      <c r="BA58" t="n">
+        <v>4481</v>
+      </c>
+      <c r="BB58" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="BC58" t="inlineStr">
+        <is>
+          <t>4570</t>
         </is>
       </c>
     </row>
@@ -10356,6 +10708,8 @@
       <c r="AY59" t="inlineStr"/>
       <c r="AZ59" s="3" t="inlineStr"/>
       <c r="BA59" t="inlineStr"/>
+      <c r="BB59" s="3" t="inlineStr"/>
+      <c r="BC59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -10423,6 +10777,8 @@
       <c r="AY60" t="inlineStr"/>
       <c r="AZ60" s="3" t="inlineStr"/>
       <c r="BA60" t="inlineStr"/>
+      <c r="BB60" s="3" t="inlineStr"/>
+      <c r="BC60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -10587,9 +10943,15 @@
       <c r="AZ61" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BA61" t="inlineStr">
-        <is>
-          <t>4846</t>
+      <c r="BA61" t="n">
+        <v>4846</v>
+      </c>
+      <c r="BB61" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BC61" t="inlineStr">
+        <is>
+          <t>4983</t>
         </is>
       </c>
     </row>
@@ -10756,7 +11118,13 @@
       <c r="AZ62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA62" t="inlineStr">
+      <c r="BA62" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10925,9 +11293,15 @@
       <c r="AZ63" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="BA63" t="inlineStr">
-        <is>
-          <t>5060</t>
+      <c r="BA63" t="n">
+        <v>5060</v>
+      </c>
+      <c r="BB63" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="BC63" t="inlineStr">
+        <is>
+          <t>5249</t>
         </is>
       </c>
     </row>
@@ -11094,9 +11468,15 @@
       <c r="AZ64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA64" t="inlineStr">
-        <is>
-          <t>2728</t>
+      <c r="BA64" t="n">
+        <v>2728</v>
+      </c>
+      <c r="BB64" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC64" t="inlineStr">
+        <is>
+          <t>3312</t>
         </is>
       </c>
     </row>
@@ -11166,6 +11546,8 @@
       <c r="AY65" t="inlineStr"/>
       <c r="AZ65" s="3" t="inlineStr"/>
       <c r="BA65" t="inlineStr"/>
+      <c r="BB65" s="3" t="inlineStr"/>
+      <c r="BC65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -11330,9 +11712,15 @@
       <c r="AZ66" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="BA66" t="inlineStr">
-        <is>
-          <t>2788</t>
+      <c r="BA66" t="n">
+        <v>2788</v>
+      </c>
+      <c r="BB66" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC66" t="inlineStr">
+        <is>
+          <t>3048</t>
         </is>
       </c>
     </row>
@@ -11499,9 +11887,15 @@
       <c r="AZ67" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BA67" t="inlineStr">
-        <is>
-          <t>4929</t>
+      <c r="BA67" t="n">
+        <v>4929</v>
+      </c>
+      <c r="BB67" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BC67" t="inlineStr">
+        <is>
+          <t>5091</t>
         </is>
       </c>
     </row>
@@ -11668,9 +12062,15 @@
       <c r="AZ68" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BA68" t="inlineStr">
-        <is>
-          <t>4954</t>
+      <c r="BA68" t="n">
+        <v>4954</v>
+      </c>
+      <c r="BB68" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BC68" t="inlineStr">
+        <is>
+          <t>5401</t>
         </is>
       </c>
     </row>
@@ -11837,9 +12237,15 @@
       <c r="AZ69" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BA69" t="inlineStr">
-        <is>
-          <t>4416</t>
+      <c r="BA69" t="n">
+        <v>4416</v>
+      </c>
+      <c r="BB69" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BC69" t="inlineStr">
+        <is>
+          <t>4510</t>
         </is>
       </c>
     </row>
@@ -12006,9 +12412,15 @@
       <c r="AZ70" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BA70" t="inlineStr">
-        <is>
-          <t>3061</t>
+      <c r="BA70" t="n">
+        <v>3061</v>
+      </c>
+      <c r="BB70" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="BC70" t="inlineStr">
+        <is>
+          <t>3759</t>
         </is>
       </c>
     </row>
@@ -12175,9 +12587,15 @@
       <c r="AZ71" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BA71" t="inlineStr">
-        <is>
-          <t>4634</t>
+      <c r="BA71" t="n">
+        <v>4634</v>
+      </c>
+      <c r="BB71" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BC71" t="inlineStr">
+        <is>
+          <t>4765</t>
         </is>
       </c>
     </row>
@@ -12344,9 +12762,15 @@
       <c r="AZ72" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="BA72" t="inlineStr">
-        <is>
-          <t>3877</t>
+      <c r="BA72" t="n">
+        <v>3877</v>
+      </c>
+      <c r="BB72" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="BC72" t="inlineStr">
+        <is>
+          <t>4081</t>
         </is>
       </c>
     </row>
@@ -12513,9 +12937,15 @@
       <c r="AZ73" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BA73" t="inlineStr">
-        <is>
-          <t>4300</t>
+      <c r="BA73" t="n">
+        <v>4300</v>
+      </c>
+      <c r="BB73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC73" t="inlineStr">
+        <is>
+          <t>4336</t>
         </is>
       </c>
     </row>
@@ -12682,9 +13112,15 @@
       <c r="AZ74" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BA74" t="inlineStr">
-        <is>
-          <t>3531</t>
+      <c r="BA74" t="n">
+        <v>3531</v>
+      </c>
+      <c r="BB74" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC74" t="inlineStr">
+        <is>
+          <t>4016</t>
         </is>
       </c>
     </row>
@@ -12851,9 +13287,15 @@
       <c r="AZ75" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BA75" t="inlineStr">
-        <is>
-          <t>4035</t>
+      <c r="BA75" t="n">
+        <v>4035</v>
+      </c>
+      <c r="BB75" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BC75" t="inlineStr">
+        <is>
+          <t>4180</t>
         </is>
       </c>
     </row>
@@ -13020,9 +13462,15 @@
       <c r="AZ76" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BA76" t="inlineStr">
-        <is>
-          <t>4987</t>
+      <c r="BA76" t="n">
+        <v>4987</v>
+      </c>
+      <c r="BB76" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC76" t="inlineStr">
+        <is>
+          <t>5171</t>
         </is>
       </c>
     </row>
@@ -13189,7 +13637,13 @@
       <c r="AZ77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA77" t="inlineStr">
+      <c r="BA77" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC77" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13358,9 +13812,15 @@
       <c r="AZ78" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BA78" t="inlineStr">
-        <is>
-          <t>4865</t>
+      <c r="BA78" t="n">
+        <v>4865</v>
+      </c>
+      <c r="BB78" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BC78" t="inlineStr">
+        <is>
+          <t>5071</t>
         </is>
       </c>
     </row>
@@ -13527,7 +13987,13 @@
       <c r="AZ79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA79" t="inlineStr">
+      <c r="BA79" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13696,9 +14162,15 @@
       <c r="AZ80" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="BA80" t="inlineStr">
-        <is>
-          <t>4783</t>
+      <c r="BA80" t="n">
+        <v>4783</v>
+      </c>
+      <c r="BB80" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="BC80" t="inlineStr">
+        <is>
+          <t>4960</t>
         </is>
       </c>
     </row>
@@ -13865,9 +14337,15 @@
       <c r="AZ81" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BA81" t="inlineStr">
-        <is>
-          <t>4979</t>
+      <c r="BA81" t="n">
+        <v>4979</v>
+      </c>
+      <c r="BB81" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BC81" t="inlineStr">
+        <is>
+          <t>5041</t>
         </is>
       </c>
     </row>
@@ -14034,9 +14512,15 @@
       <c r="AZ82" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BA82" t="inlineStr">
-        <is>
-          <t>4636</t>
+      <c r="BA82" t="n">
+        <v>4636</v>
+      </c>
+      <c r="BB82" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BC82" t="inlineStr">
+        <is>
+          <t>4686</t>
         </is>
       </c>
     </row>
@@ -14203,9 +14687,15 @@
       <c r="AZ83" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BA83" t="inlineStr">
-        <is>
-          <t>4421</t>
+      <c r="BA83" t="n">
+        <v>4421</v>
+      </c>
+      <c r="BB83" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="BC83" t="inlineStr">
+        <is>
+          <t>4541</t>
         </is>
       </c>
     </row>
@@ -14335,6 +14825,8 @@
       <c r="AY84" t="inlineStr"/>
       <c r="AZ84" s="3" t="inlineStr"/>
       <c r="BA84" t="inlineStr"/>
+      <c r="BB84" s="3" t="inlineStr"/>
+      <c r="BC84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -14499,9 +14991,15 @@
       <c r="AZ85" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BA85" t="inlineStr">
-        <is>
-          <t>3889</t>
+      <c r="BA85" t="n">
+        <v>3889</v>
+      </c>
+      <c r="BB85" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC85" t="inlineStr">
+        <is>
+          <t>3984</t>
         </is>
       </c>
     </row>
@@ -14668,9 +15166,15 @@
       <c r="AZ86" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BA86" t="inlineStr">
-        <is>
-          <t>3352</t>
+      <c r="BA86" t="n">
+        <v>3352</v>
+      </c>
+      <c r="BB86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC86" t="inlineStr">
+        <is>
+          <t>3390</t>
         </is>
       </c>
     </row>
@@ -14837,9 +15341,15 @@
       <c r="AZ87" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BA87" t="inlineStr">
-        <is>
-          <t>4579</t>
+      <c r="BA87" t="n">
+        <v>4579</v>
+      </c>
+      <c r="BB87" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC87" t="inlineStr">
+        <is>
+          <t>4725</t>
         </is>
       </c>
     </row>
@@ -15006,9 +15516,15 @@
       <c r="AZ88" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BA88" t="inlineStr">
-        <is>
-          <t>2826</t>
+      <c r="BA88" t="n">
+        <v>2826</v>
+      </c>
+      <c r="BB88" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC88" t="inlineStr">
+        <is>
+          <t>2916</t>
         </is>
       </c>
     </row>
@@ -15175,9 +15691,15 @@
       <c r="AZ89" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="BA89" t="inlineStr">
-        <is>
-          <t>3312</t>
+      <c r="BA89" t="n">
+        <v>3312</v>
+      </c>
+      <c r="BB89" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC89" t="inlineStr">
+        <is>
+          <t>3415</t>
         </is>
       </c>
     </row>
@@ -15344,9 +15866,15 @@
       <c r="AZ90" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="BA90" t="inlineStr">
-        <is>
-          <t>2874</t>
+      <c r="BA90" t="n">
+        <v>2874</v>
+      </c>
+      <c r="BB90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC90" t="inlineStr">
+        <is>
+          <t>2833</t>
         </is>
       </c>
     </row>
@@ -15513,9 +16041,15 @@
       <c r="AZ91" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BA91" t="inlineStr">
-        <is>
-          <t>3009</t>
+      <c r="BA91" t="n">
+        <v>3009</v>
+      </c>
+      <c r="BB91" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC91" t="inlineStr">
+        <is>
+          <t>2962</t>
         </is>
       </c>
     </row>
@@ -15682,7 +16216,13 @@
       <c r="AZ92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA92" t="inlineStr">
+      <c r="BA92" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15851,9 +16391,15 @@
       <c r="AZ93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA93" t="inlineStr">
-        <is>
-          <t>2294</t>
+      <c r="BA93" t="n">
+        <v>2294</v>
+      </c>
+      <c r="BB93" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="BC93" t="inlineStr">
+        <is>
+          <t>2418</t>
         </is>
       </c>
     </row>
@@ -16020,9 +16566,15 @@
       <c r="AZ94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA94" t="inlineStr">
-        <is>
-          <t>2740</t>
+      <c r="BA94" t="n">
+        <v>2740</v>
+      </c>
+      <c r="BB94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC94" t="inlineStr">
+        <is>
+          <t>2752</t>
         </is>
       </c>
     </row>
@@ -16189,9 +16741,15 @@
       <c r="AZ95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA95" t="inlineStr">
-        <is>
-          <t>2528</t>
+      <c r="BA95" t="n">
+        <v>2528</v>
+      </c>
+      <c r="BB95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC95" t="inlineStr">
+        <is>
+          <t>2513</t>
         </is>
       </c>
     </row>
@@ -16358,9 +16916,15 @@
       <c r="AZ96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA96" t="inlineStr">
-        <is>
-          <t>2467</t>
+      <c r="BA96" t="n">
+        <v>2467</v>
+      </c>
+      <c r="BB96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC96" t="inlineStr">
+        <is>
+          <t>2462</t>
         </is>
       </c>
     </row>
@@ -16527,9 +17091,15 @@
       <c r="AZ97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA97" t="inlineStr">
-        <is>
-          <t>3189</t>
+      <c r="BA97" t="n">
+        <v>3189</v>
+      </c>
+      <c r="BB97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC97" t="inlineStr">
+        <is>
+          <t>3188</t>
         </is>
       </c>
     </row>
@@ -16696,7 +17266,13 @@
       <c r="AZ98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA98" t="inlineStr">
+      <c r="BA98" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16865,9 +17441,15 @@
       <c r="AZ99" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="BA99" t="inlineStr">
-        <is>
-          <t>3684</t>
+      <c r="BA99" t="n">
+        <v>3684</v>
+      </c>
+      <c r="BB99" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="BC99" t="inlineStr">
+        <is>
+          <t>3752</t>
         </is>
       </c>
     </row>
@@ -17034,9 +17616,15 @@
       <c r="AZ100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA100" t="inlineStr">
-        <is>
-          <t>2484</t>
+      <c r="BA100" t="n">
+        <v>2484</v>
+      </c>
+      <c r="BB100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC100" t="inlineStr">
+        <is>
+          <t>2493</t>
         </is>
       </c>
     </row>
@@ -17203,9 +17791,15 @@
       <c r="AZ101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BA101" t="inlineStr">
-        <is>
-          <t>4502</t>
+      <c r="BA101" t="n">
+        <v>4502</v>
+      </c>
+      <c r="BB101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BC101" t="inlineStr">
+        <is>
+          <t>4588</t>
         </is>
       </c>
     </row>
@@ -17372,9 +17966,15 @@
       <c r="AZ102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BA102" t="inlineStr">
-        <is>
-          <t>3963</t>
+      <c r="BA102" t="n">
+        <v>3963</v>
+      </c>
+      <c r="BB102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC102" t="inlineStr">
+        <is>
+          <t>4032</t>
         </is>
       </c>
     </row>
@@ -17541,9 +18141,15 @@
       <c r="AZ103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA103" t="inlineStr">
-        <is>
-          <t>3766</t>
+      <c r="BA103" t="n">
+        <v>3766</v>
+      </c>
+      <c r="BB103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC103" t="inlineStr">
+        <is>
+          <t>3754</t>
         </is>
       </c>
     </row>
@@ -17710,9 +18316,15 @@
       <c r="AZ104" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BA104" t="inlineStr">
-        <is>
-          <t>4546</t>
+      <c r="BA104" t="n">
+        <v>4546</v>
+      </c>
+      <c r="BB104" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="BC104" t="inlineStr">
+        <is>
+          <t>4631</t>
         </is>
       </c>
     </row>
@@ -17879,9 +18491,15 @@
       <c r="AZ105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA105" t="inlineStr">
-        <is>
-          <t>4023</t>
+      <c r="BA105" t="n">
+        <v>4023</v>
+      </c>
+      <c r="BB105" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="BC105" t="inlineStr">
+        <is>
+          <t>4231</t>
         </is>
       </c>
     </row>
@@ -18048,7 +18666,13 @@
       <c r="AZ106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA106" t="inlineStr">
+      <c r="BA106" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18217,9 +18841,15 @@
       <c r="AZ107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA107" t="inlineStr">
-        <is>
-          <t>2581</t>
+      <c r="BA107" t="n">
+        <v>2581</v>
+      </c>
+      <c r="BB107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC107" t="inlineStr">
+        <is>
+          <t>2615</t>
         </is>
       </c>
     </row>
@@ -18386,7 +19016,13 @@
       <c r="AZ108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA108" t="inlineStr">
+      <c r="BA108" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18555,9 +19191,15 @@
       <c r="AZ109" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="BA109" t="inlineStr">
-        <is>
-          <t>3896</t>
+      <c r="BA109" t="n">
+        <v>3896</v>
+      </c>
+      <c r="BB109" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="BC109" t="inlineStr">
+        <is>
+          <t>3969</t>
         </is>
       </c>
     </row>
@@ -18724,9 +19366,15 @@
       <c r="AZ110" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BA110" t="inlineStr">
-        <is>
-          <t>3786</t>
+      <c r="BA110" t="n">
+        <v>3786</v>
+      </c>
+      <c r="BB110" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="BC110" t="inlineStr">
+        <is>
+          <t>3846</t>
         </is>
       </c>
     </row>
@@ -18880,6 +19528,8 @@
       <c r="AY111" t="inlineStr"/>
       <c r="AZ111" s="3" t="inlineStr"/>
       <c r="BA111" t="inlineStr"/>
+      <c r="BB111" s="3" t="inlineStr"/>
+      <c r="BC111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -19044,9 +19694,15 @@
       <c r="AZ112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA112" t="inlineStr">
-        <is>
-          <t>2612</t>
+      <c r="BA112" t="n">
+        <v>2612</v>
+      </c>
+      <c r="BB112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC112" t="inlineStr">
+        <is>
+          <t>2639</t>
         </is>
       </c>
     </row>
@@ -19213,9 +19869,15 @@
       <c r="AZ113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA113" t="inlineStr">
-        <is>
-          <t>3535</t>
+      <c r="BA113" t="n">
+        <v>3535</v>
+      </c>
+      <c r="BB113" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC113" t="inlineStr">
+        <is>
+          <t>3668</t>
         </is>
       </c>
     </row>
@@ -19382,9 +20044,15 @@
       <c r="AZ114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA114" t="inlineStr">
-        <is>
-          <t>3625</t>
+      <c r="BA114" t="n">
+        <v>3625</v>
+      </c>
+      <c r="BB114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC114" t="inlineStr">
+        <is>
+          <t>3738</t>
         </is>
       </c>
     </row>
@@ -19551,9 +20219,15 @@
       <c r="AZ115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA115" t="inlineStr">
-        <is>
-          <t>2007</t>
+      <c r="BA115" t="n">
+        <v>2007</v>
+      </c>
+      <c r="BB115" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="BC115" t="inlineStr">
+        <is>
+          <t>2153</t>
         </is>
       </c>
     </row>
@@ -19720,9 +20394,15 @@
       <c r="AZ116" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="BA116" t="inlineStr">
-        <is>
-          <t>3183</t>
+      <c r="BA116" t="n">
+        <v>3183</v>
+      </c>
+      <c r="BB116" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="BC116" t="inlineStr">
+        <is>
+          <t>3237</t>
         </is>
       </c>
     </row>
@@ -19889,9 +20569,15 @@
       <c r="AZ117" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="BA117" t="inlineStr">
-        <is>
-          <t>3696</t>
+      <c r="BA117" t="n">
+        <v>3696</v>
+      </c>
+      <c r="BB117" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BC117" t="inlineStr">
+        <is>
+          <t>3824</t>
         </is>
       </c>
     </row>
@@ -20058,7 +20744,13 @@
       <c r="AZ118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA118" t="inlineStr">
+      <c r="BA118" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -20227,9 +20919,15 @@
       <c r="AZ119" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BA119" t="inlineStr">
-        <is>
-          <t>3989</t>
+      <c r="BA119" t="n">
+        <v>3989</v>
+      </c>
+      <c r="BB119" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC119" t="inlineStr">
+        <is>
+          <t>4157</t>
         </is>
       </c>
     </row>
@@ -20396,9 +21094,15 @@
       <c r="AZ120" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BA120" t="inlineStr">
-        <is>
-          <t>2712</t>
+      <c r="BA120" t="n">
+        <v>2712</v>
+      </c>
+      <c r="BB120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC120" t="inlineStr">
+        <is>
+          <t>2713</t>
         </is>
       </c>
     </row>
@@ -20565,9 +21269,15 @@
       <c r="AZ121" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="BA121" t="inlineStr">
-        <is>
-          <t>3372</t>
+      <c r="BA121" t="n">
+        <v>3372</v>
+      </c>
+      <c r="BB121" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="BC121" t="inlineStr">
+        <is>
+          <t>3539</t>
         </is>
       </c>
     </row>
@@ -20734,7 +21444,13 @@
       <c r="AZ122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA122" t="inlineStr">
+      <c r="BA122" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -20903,9 +21619,15 @@
       <c r="AZ123" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="BA123" t="inlineStr">
-        <is>
-          <t>3338</t>
+      <c r="BA123" t="n">
+        <v>3338</v>
+      </c>
+      <c r="BB123" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC123" t="inlineStr">
+        <is>
+          <t>3415</t>
         </is>
       </c>
     </row>
@@ -21072,9 +21794,15 @@
       <c r="AZ124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BA124" t="inlineStr">
-        <is>
-          <t>3347</t>
+      <c r="BA124" t="n">
+        <v>3347</v>
+      </c>
+      <c r="BB124" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="BC124" t="inlineStr">
+        <is>
+          <t>3394</t>
         </is>
       </c>
     </row>
@@ -21241,9 +21969,15 @@
       <c r="AZ125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA125" t="inlineStr">
-        <is>
-          <t>3440</t>
+      <c r="BA125" t="n">
+        <v>3440</v>
+      </c>
+      <c r="BB125" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC125" t="inlineStr">
+        <is>
+          <t>3656</t>
         </is>
       </c>
     </row>
@@ -21410,9 +22144,15 @@
       <c r="AZ126" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="BA126" t="inlineStr">
-        <is>
-          <t>3219</t>
+      <c r="BA126" t="n">
+        <v>3219</v>
+      </c>
+      <c r="BB126" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BC126" t="inlineStr">
+        <is>
+          <t>3411</t>
         </is>
       </c>
     </row>
@@ -21579,9 +22319,15 @@
       <c r="AZ127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA127" t="inlineStr">
-        <is>
-          <t>2263</t>
+      <c r="BA127" t="n">
+        <v>2263</v>
+      </c>
+      <c r="BB127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC127" t="inlineStr">
+        <is>
+          <t>2258</t>
         </is>
       </c>
     </row>
@@ -21748,7 +22494,13 @@
       <c r="AZ128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA128" t="inlineStr">
+      <c r="BA128" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -21917,7 +22669,13 @@
       <c r="AZ129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA129" t="inlineStr">
+      <c r="BA129" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -22086,9 +22844,15 @@
       <c r="AZ130" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BA130" t="inlineStr">
-        <is>
-          <t>2998</t>
+      <c r="BA130" t="n">
+        <v>2998</v>
+      </c>
+      <c r="BB130" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="BC130" t="inlineStr">
+        <is>
+          <t>2962</t>
         </is>
       </c>
     </row>
@@ -22255,7 +23019,13 @@
       <c r="AZ131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA131" t="inlineStr">
+      <c r="BA131" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -22424,9 +23194,15 @@
       <c r="AZ132" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BA132" t="inlineStr">
-        <is>
-          <t>2758</t>
+      <c r="BA132" t="n">
+        <v>2758</v>
+      </c>
+      <c r="BB132" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC132" t="inlineStr">
+        <is>
+          <t>2749</t>
         </is>
       </c>
     </row>
@@ -22593,7 +23369,13 @@
       <c r="AZ133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA133" t="inlineStr">
+      <c r="BA133" t="n">
+        <v>2779</v>
+      </c>
+      <c r="BB133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC133" t="inlineStr">
         <is>
           <t>2779</t>
         </is>
@@ -22689,6 +23471,8 @@
       <c r="AY134" t="inlineStr"/>
       <c r="AZ134" s="3" t="inlineStr"/>
       <c r="BA134" t="inlineStr"/>
+      <c r="BB134" s="3" t="inlineStr"/>
+      <c r="BC134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -22772,6 +23556,8 @@
       <c r="AY135" t="inlineStr"/>
       <c r="AZ135" s="3" t="inlineStr"/>
       <c r="BA135" t="inlineStr"/>
+      <c r="BB135" s="3" t="inlineStr"/>
+      <c r="BC135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -22936,7 +23722,13 @@
       <c r="AZ136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA136" t="inlineStr">
+      <c r="BA136" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC136" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -23105,7 +23897,13 @@
       <c r="AZ137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA137" t="inlineStr">
+      <c r="BA137" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -23193,6 +23991,8 @@
       <c r="AY138" t="inlineStr"/>
       <c r="AZ138" s="3" t="inlineStr"/>
       <c r="BA138" t="inlineStr"/>
+      <c r="BB138" s="3" t="inlineStr"/>
+      <c r="BC138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -23357,9 +24157,15 @@
       <c r="AZ139" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="BA139" t="inlineStr">
-        <is>
-          <t>2542</t>
+      <c r="BA139" t="n">
+        <v>2542</v>
+      </c>
+      <c r="BB139" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC139" t="inlineStr">
+        <is>
+          <t>2726</t>
         </is>
       </c>
     </row>
@@ -23526,9 +24332,15 @@
       <c r="AZ140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA140" t="inlineStr">
-        <is>
-          <t>2903</t>
+      <c r="BA140" t="n">
+        <v>2903</v>
+      </c>
+      <c r="BB140" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC140" t="inlineStr">
+        <is>
+          <t>3037</t>
         </is>
       </c>
     </row>
@@ -23614,6 +24426,8 @@
       <c r="AY141" t="inlineStr"/>
       <c r="AZ141" s="3" t="inlineStr"/>
       <c r="BA141" t="inlineStr"/>
+      <c r="BB141" s="3" t="inlineStr"/>
+      <c r="BC141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -23778,7 +24592,13 @@
       <c r="AZ142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA142" t="inlineStr">
+      <c r="BA142" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC142" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -23866,6 +24686,8 @@
       <c r="AY143" t="inlineStr"/>
       <c r="AZ143" s="3" t="inlineStr"/>
       <c r="BA143" t="inlineStr"/>
+      <c r="BB143" s="3" t="inlineStr"/>
+      <c r="BC143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -23949,6 +24771,8 @@
       <c r="AY144" t="inlineStr"/>
       <c r="AZ144" s="3" t="inlineStr"/>
       <c r="BA144" t="inlineStr"/>
+      <c r="BB144" s="3" t="inlineStr"/>
+      <c r="BC144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -24032,6 +24856,8 @@
       <c r="AY145" t="inlineStr"/>
       <c r="AZ145" s="3" t="inlineStr"/>
       <c r="BA145" t="inlineStr"/>
+      <c r="BB145" s="3" t="inlineStr"/>
+      <c r="BC145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -24115,6 +24941,8 @@
       <c r="AY146" t="inlineStr"/>
       <c r="AZ146" s="3" t="inlineStr"/>
       <c r="BA146" t="inlineStr"/>
+      <c r="BB146" s="3" t="inlineStr"/>
+      <c r="BC146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -24198,6 +25026,8 @@
       <c r="AY147" t="inlineStr"/>
       <c r="AZ147" s="3" t="inlineStr"/>
       <c r="BA147" t="inlineStr"/>
+      <c r="BB147" s="3" t="inlineStr"/>
+      <c r="BC147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -24362,7 +25192,13 @@
       <c r="AZ148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA148" t="inlineStr">
+      <c r="BA148" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -24531,9 +25367,15 @@
       <c r="AZ149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA149" t="inlineStr">
-        <is>
-          <t>3727</t>
+      <c r="BA149" t="n">
+        <v>3727</v>
+      </c>
+      <c r="BB149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC149" t="inlineStr">
+        <is>
+          <t>3743</t>
         </is>
       </c>
     </row>
@@ -24700,7 +25542,13 @@
       <c r="AZ150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA150" t="inlineStr">
+      <c r="BA150" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -24869,9 +25717,15 @@
       <c r="AZ151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA151" t="inlineStr">
-        <is>
-          <t>2593</t>
+      <c r="BA151" t="n">
+        <v>2593</v>
+      </c>
+      <c r="BB151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC151" t="inlineStr">
+        <is>
+          <t>2622</t>
         </is>
       </c>
     </row>
@@ -25038,7 +25892,13 @@
       <c r="AZ152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA152" t="inlineStr">
+      <c r="BA152" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -25207,7 +26067,13 @@
       <c r="AZ153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA153" t="inlineStr">
+      <c r="BA153" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -25376,7 +26242,13 @@
       <c r="AZ154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA154" t="inlineStr">
+      <c r="BA154" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -25545,9 +26417,15 @@
       <c r="AZ155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA155" t="inlineStr">
-        <is>
-          <t>2731</t>
+      <c r="BA155" t="n">
+        <v>2731</v>
+      </c>
+      <c r="BB155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC155" t="inlineStr">
+        <is>
+          <t>2755</t>
         </is>
       </c>
     </row>
@@ -25708,9 +26586,15 @@
       <c r="AZ156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA156" t="inlineStr">
-        <is>
-          <t>3195</t>
+      <c r="BA156" t="n">
+        <v>3195</v>
+      </c>
+      <c r="BB156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC156" t="inlineStr">
+        <is>
+          <t>3199</t>
         </is>
       </c>
     </row>
@@ -25790,6 +26674,8 @@
       <c r="AY157" t="inlineStr"/>
       <c r="AZ157" s="3" t="inlineStr"/>
       <c r="BA157" t="inlineStr"/>
+      <c r="BB157" s="3" t="inlineStr"/>
+      <c r="BC157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -25948,7 +26834,13 @@
       <c r="AZ158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA158" t="inlineStr">
+      <c r="BA158" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -26111,9 +27003,15 @@
       <c r="AZ159" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BA159" t="inlineStr">
-        <is>
-          <t>3113</t>
+      <c r="BA159" t="n">
+        <v>3113</v>
+      </c>
+      <c r="BB159" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC159" t="inlineStr">
+        <is>
+          <t>3106</t>
         </is>
       </c>
     </row>
@@ -26193,6 +27091,8 @@
       <c r="AY160" t="inlineStr"/>
       <c r="AZ160" s="3" t="inlineStr"/>
       <c r="BA160" t="inlineStr"/>
+      <c r="BB160" s="3" t="inlineStr"/>
+      <c r="BC160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -26339,9 +27239,15 @@
       <c r="AZ161" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BA161" t="inlineStr">
-        <is>
-          <t>3266</t>
+      <c r="BA161" t="n">
+        <v>3266</v>
+      </c>
+      <c r="BB161" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="BC161" t="inlineStr">
+        <is>
+          <t>3353</t>
         </is>
       </c>
     </row>
@@ -26490,9 +27396,15 @@
       <c r="AZ162" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="BA162" t="inlineStr">
-        <is>
-          <t>2859</t>
+      <c r="BA162" t="n">
+        <v>2859</v>
+      </c>
+      <c r="BB162" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC162" t="inlineStr">
+        <is>
+          <t>2998</t>
         </is>
       </c>
     </row>
@@ -26637,9 +27549,15 @@
       <c r="AZ163" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="BA163" t="inlineStr">
-        <is>
-          <t>3405</t>
+      <c r="BA163" t="n">
+        <v>3405</v>
+      </c>
+      <c r="BB163" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC163" t="inlineStr">
+        <is>
+          <t>3382</t>
         </is>
       </c>
     </row>
@@ -26768,9 +27686,15 @@
       <c r="AZ164" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="BA164" t="inlineStr">
-        <is>
-          <t>3470</t>
+      <c r="BA164" t="n">
+        <v>3470</v>
+      </c>
+      <c r="BB164" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="BC164" t="inlineStr">
+        <is>
+          <t>3577</t>
         </is>
       </c>
     </row>
@@ -26903,9 +27827,15 @@
       <c r="AZ165" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="BA165" t="inlineStr">
-        <is>
-          <t>2883</t>
+      <c r="BA165" t="n">
+        <v>2883</v>
+      </c>
+      <c r="BB165" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="BC165" t="inlineStr">
+        <is>
+          <t>2938</t>
         </is>
       </c>
     </row>
@@ -27030,9 +27960,15 @@
       <c r="AZ166" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA166" t="inlineStr">
-        <is>
-          <t>2782</t>
+      <c r="BA166" t="n">
+        <v>2782</v>
+      </c>
+      <c r="BB166" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC166" t="inlineStr">
+        <is>
+          <t>2803</t>
         </is>
       </c>
     </row>
@@ -27145,7 +28081,13 @@
       <c r="AZ167" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA167" t="inlineStr">
+      <c r="BA167" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB167" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC167" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -27256,7 +28198,13 @@
       <c r="AZ168" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA168" t="inlineStr">
+      <c r="BA168" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB168" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC168" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -27330,6 +28278,8 @@
       <c r="AY169" t="inlineStr"/>
       <c r="AZ169" s="3" t="inlineStr"/>
       <c r="BA169" t="inlineStr"/>
+      <c r="BB169" s="3" t="inlineStr"/>
+      <c r="BC169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="n">
@@ -27432,7 +28382,13 @@
       <c r="AZ170" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA170" t="inlineStr">
+      <c r="BA170" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB170" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC170" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -27527,7 +28483,13 @@
       <c r="AZ171" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA171" t="inlineStr">
+      <c r="BA171" t="n">
+        <v>1781</v>
+      </c>
+      <c r="BB171" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC171" t="inlineStr">
         <is>
           <t>1781</t>
         </is>
@@ -27622,7 +28584,13 @@
       <c r="AZ172" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA172" t="inlineStr">
+      <c r="BA172" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB172" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC172" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -27717,9 +28685,15 @@
       <c r="AZ173" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA173" t="inlineStr">
-        <is>
-          <t>1872</t>
+      <c r="BA173" t="n">
+        <v>1872</v>
+      </c>
+      <c r="BB173" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC173" t="inlineStr">
+        <is>
+          <t>1857</t>
         </is>
       </c>
     </row>
@@ -27788,9 +28762,15 @@
       <c r="AZ174" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BA174" t="inlineStr">
-        <is>
-          <t>3229</t>
+      <c r="BA174" t="n">
+        <v>3229</v>
+      </c>
+      <c r="BB174" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="BC174" t="inlineStr">
+        <is>
+          <t>3257</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-03-11 11:30:39
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BC174"/>
+  <dimension ref="A1:BE174"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -666,6 +666,16 @@
           <t>03-09_0</t>
         </is>
       </c>
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>03-10_A</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>03-10_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -836,9 +846,15 @@
       <c r="BB2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC2" t="inlineStr">
-        <is>
-          <t>2926</t>
+      <c r="BC2" t="n">
+        <v>2926</v>
+      </c>
+      <c r="BD2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE2" t="inlineStr">
+        <is>
+          <t>2951</t>
         </is>
       </c>
     </row>
@@ -1011,9 +1027,15 @@
       <c r="BB3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BC3" t="inlineStr">
-        <is>
-          <t>6170</t>
+      <c r="BC3" t="n">
+        <v>6170</v>
+      </c>
+      <c r="BD3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BE3" t="inlineStr">
+        <is>
+          <t>6482</t>
         </is>
       </c>
     </row>
@@ -1186,9 +1208,15 @@
       <c r="BB4" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="BC4" t="inlineStr">
-        <is>
-          <t>6116</t>
+      <c r="BC4" t="n">
+        <v>6116</v>
+      </c>
+      <c r="BD4" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="BE4" t="inlineStr">
+        <is>
+          <t>6337</t>
         </is>
       </c>
     </row>
@@ -1361,9 +1389,15 @@
       <c r="BB5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BC5" t="inlineStr">
-        <is>
-          <t>5823</t>
+      <c r="BC5" t="n">
+        <v>5823</v>
+      </c>
+      <c r="BD5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BE5" t="inlineStr">
+        <is>
+          <t>6159</t>
         </is>
       </c>
     </row>
@@ -1536,9 +1570,15 @@
       <c r="BB6" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BC6" t="inlineStr">
-        <is>
-          <t>5838</t>
+      <c r="BC6" t="n">
+        <v>5838</v>
+      </c>
+      <c r="BD6" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BE6" t="inlineStr">
+        <is>
+          <t>6033</t>
         </is>
       </c>
     </row>
@@ -1711,9 +1751,15 @@
       <c r="BB7" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="BC7" t="inlineStr">
-        <is>
-          <t>6270</t>
+      <c r="BC7" t="n">
+        <v>6270</v>
+      </c>
+      <c r="BD7" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BE7" t="inlineStr">
+        <is>
+          <t>6594</t>
         </is>
       </c>
     </row>
@@ -1886,9 +1932,15 @@
       <c r="BB8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BC8" t="inlineStr">
-        <is>
-          <t>5342</t>
+      <c r="BC8" t="n">
+        <v>5342</v>
+      </c>
+      <c r="BD8" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BE8" t="inlineStr">
+        <is>
+          <t>5700</t>
         </is>
       </c>
     </row>
@@ -2061,9 +2113,15 @@
       <c r="BB9" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BC9" t="inlineStr">
-        <is>
-          <t>5574</t>
+      <c r="BC9" t="n">
+        <v>5574</v>
+      </c>
+      <c r="BD9" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BE9" t="inlineStr">
+        <is>
+          <t>5864</t>
         </is>
       </c>
     </row>
@@ -2236,9 +2294,15 @@
       <c r="BB10" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="BC10" t="inlineStr">
-        <is>
-          <t>6595</t>
+      <c r="BC10" t="n">
+        <v>6595</v>
+      </c>
+      <c r="BD10" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="BE10" t="inlineStr">
+        <is>
+          <t>6917</t>
         </is>
       </c>
     </row>
@@ -2411,7 +2475,13 @@
       <c r="BB11" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BC11" t="inlineStr">
+      <c r="BC11" t="n">
+        <v>4932</v>
+      </c>
+      <c r="BD11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE11" t="inlineStr">
         <is>
           <t>4932</t>
         </is>
@@ -2586,9 +2656,15 @@
       <c r="BB12" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="BC12" t="inlineStr">
-        <is>
-          <t>2752</t>
+      <c r="BC12" t="n">
+        <v>2752</v>
+      </c>
+      <c r="BD12" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="BE12" t="inlineStr">
+        <is>
+          <t>2928</t>
         </is>
       </c>
     </row>
@@ -2761,9 +2837,15 @@
       <c r="BB13" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="BC13" t="inlineStr">
-        <is>
-          <t>6642</t>
+      <c r="BC13" t="n">
+        <v>6642</v>
+      </c>
+      <c r="BD13" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="BE13" t="inlineStr">
+        <is>
+          <t>6977</t>
         </is>
       </c>
     </row>
@@ -2936,9 +3018,15 @@
       <c r="BB14" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BC14" t="inlineStr">
-        <is>
-          <t>5683</t>
+      <c r="BC14" t="n">
+        <v>5683</v>
+      </c>
+      <c r="BD14" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BE14" t="inlineStr">
+        <is>
+          <t>5798</t>
         </is>
       </c>
     </row>
@@ -3111,7 +3199,13 @@
       <c r="BB15" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC15" t="inlineStr">
+      <c r="BC15" t="n">
+        <v>2743</v>
+      </c>
+      <c r="BD15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE15" t="inlineStr">
         <is>
           <t>2743</t>
         </is>
@@ -3286,9 +3380,15 @@
       <c r="BB16" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BC16" t="inlineStr">
-        <is>
-          <t>5988</t>
+      <c r="BC16" t="n">
+        <v>5988</v>
+      </c>
+      <c r="BD16" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BE16" t="inlineStr">
+        <is>
+          <t>6227</t>
         </is>
       </c>
     </row>
@@ -3461,9 +3561,15 @@
       <c r="BB17" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BC17" t="inlineStr">
-        <is>
-          <t>4310</t>
+      <c r="BC17" t="n">
+        <v>4310</v>
+      </c>
+      <c r="BD17" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BE17" t="inlineStr">
+        <is>
+          <t>4451</t>
         </is>
       </c>
     </row>
@@ -3636,9 +3742,15 @@
       <c r="BB18" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="BC18" t="inlineStr">
-        <is>
-          <t>5069</t>
+      <c r="BC18" t="n">
+        <v>5069</v>
+      </c>
+      <c r="BD18" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="BE18" t="inlineStr">
+        <is>
+          <t>5284</t>
         </is>
       </c>
     </row>
@@ -3811,9 +3923,15 @@
       <c r="BB19" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BC19" t="inlineStr">
-        <is>
-          <t>6129</t>
+      <c r="BC19" t="n">
+        <v>6129</v>
+      </c>
+      <c r="BD19" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BE19" t="inlineStr">
+        <is>
+          <t>6384</t>
         </is>
       </c>
     </row>
@@ -3986,9 +4104,15 @@
       <c r="BB20" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="BC20" t="inlineStr">
-        <is>
-          <t>6680</t>
+      <c r="BC20" t="n">
+        <v>6680</v>
+      </c>
+      <c r="BD20" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="BE20" t="inlineStr">
+        <is>
+          <t>7018</t>
         </is>
       </c>
     </row>
@@ -4161,9 +4285,15 @@
       <c r="BB21" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="BC21" t="inlineStr">
-        <is>
-          <t>5116</t>
+      <c r="BC21" t="n">
+        <v>5116</v>
+      </c>
+      <c r="BD21" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BE21" t="inlineStr">
+        <is>
+          <t>5526</t>
         </is>
       </c>
     </row>
@@ -4336,9 +4466,15 @@
       <c r="BB22" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="BC22" t="inlineStr">
-        <is>
-          <t>5690</t>
+      <c r="BC22" t="n">
+        <v>5690</v>
+      </c>
+      <c r="BD22" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="BE22" t="inlineStr">
+        <is>
+          <t>5995</t>
         </is>
       </c>
     </row>
@@ -4511,9 +4647,15 @@
       <c r="BB23" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC23" t="inlineStr">
-        <is>
-          <t>4867</t>
+      <c r="BC23" t="n">
+        <v>4867</v>
+      </c>
+      <c r="BD23" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BE23" t="inlineStr">
+        <is>
+          <t>5186</t>
         </is>
       </c>
     </row>
@@ -4686,9 +4828,15 @@
       <c r="BB24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BC24" t="inlineStr">
-        <is>
-          <t>6051</t>
+      <c r="BC24" t="n">
+        <v>6051</v>
+      </c>
+      <c r="BD24" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BE24" t="inlineStr">
+        <is>
+          <t>6207</t>
         </is>
       </c>
     </row>
@@ -4861,7 +5009,13 @@
       <c r="BB25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC25" t="inlineStr">
+      <c r="BC25" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5036,9 +5190,15 @@
       <c r="BB26" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="BC26" t="inlineStr">
-        <is>
-          <t>6044</t>
+      <c r="BC26" t="n">
+        <v>6044</v>
+      </c>
+      <c r="BD26" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="BE26" t="inlineStr">
+        <is>
+          <t>6205</t>
         </is>
       </c>
     </row>
@@ -5211,9 +5371,15 @@
       <c r="BB27" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BC27" t="inlineStr">
-        <is>
-          <t>6048</t>
+      <c r="BC27" t="n">
+        <v>6048</v>
+      </c>
+      <c r="BD27" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BE27" t="inlineStr">
+        <is>
+          <t>6323</t>
         </is>
       </c>
     </row>
@@ -5386,9 +5552,15 @@
       <c r="BB28" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="BC28" t="inlineStr">
-        <is>
-          <t>5863</t>
+      <c r="BC28" t="n">
+        <v>5863</v>
+      </c>
+      <c r="BD28" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="BE28" t="inlineStr">
+        <is>
+          <t>6149</t>
         </is>
       </c>
     </row>
@@ -5561,9 +5733,15 @@
       <c r="BB29" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BC29" t="inlineStr">
-        <is>
-          <t>6462</t>
+      <c r="BC29" t="n">
+        <v>6462</v>
+      </c>
+      <c r="BD29" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BE29" t="inlineStr">
+        <is>
+          <t>6938</t>
         </is>
       </c>
     </row>
@@ -5736,9 +5914,15 @@
       <c r="BB30" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="BC30" t="inlineStr">
-        <is>
-          <t>5587</t>
+      <c r="BC30" t="n">
+        <v>5587</v>
+      </c>
+      <c r="BD30" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="BE30" t="inlineStr">
+        <is>
+          <t>5854</t>
         </is>
       </c>
     </row>
@@ -5911,9 +6095,15 @@
       <c r="BB31" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="BC31" t="inlineStr">
-        <is>
-          <t>6574</t>
+      <c r="BC31" t="n">
+        <v>6574</v>
+      </c>
+      <c r="BD31" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BE31" t="inlineStr">
+        <is>
+          <t>6860</t>
         </is>
       </c>
     </row>
@@ -6086,9 +6276,15 @@
       <c r="BB32" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="BC32" t="inlineStr">
-        <is>
-          <t>6289</t>
+      <c r="BC32" t="n">
+        <v>6289</v>
+      </c>
+      <c r="BD32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE32" t="inlineStr">
+        <is>
+          <t>6273</t>
         </is>
       </c>
     </row>
@@ -6261,9 +6457,15 @@
       <c r="BB33" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BC33" t="inlineStr">
-        <is>
-          <t>5647</t>
+      <c r="BC33" t="n">
+        <v>5647</v>
+      </c>
+      <c r="BD33" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="BE33" t="inlineStr">
+        <is>
+          <t>5780</t>
         </is>
       </c>
     </row>
@@ -6436,9 +6638,15 @@
       <c r="BB34" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BC34" t="inlineStr">
-        <is>
-          <t>5573</t>
+      <c r="BC34" t="n">
+        <v>5573</v>
+      </c>
+      <c r="BD34" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BE34" t="inlineStr">
+        <is>
+          <t>5881</t>
         </is>
       </c>
     </row>
@@ -6611,9 +6819,15 @@
       <c r="BB35" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="BC35" t="inlineStr">
-        <is>
-          <t>6132</t>
+      <c r="BC35" t="n">
+        <v>6132</v>
+      </c>
+      <c r="BD35" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="BE35" t="inlineStr">
+        <is>
+          <t>6456</t>
         </is>
       </c>
     </row>
@@ -6786,9 +7000,15 @@
       <c r="BB36" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BC36" t="inlineStr">
-        <is>
-          <t>5661</t>
+      <c r="BC36" t="n">
+        <v>5661</v>
+      </c>
+      <c r="BD36" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BE36" t="inlineStr">
+        <is>
+          <t>5844</t>
         </is>
       </c>
     </row>
@@ -6961,7 +7181,13 @@
       <c r="BB37" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="BC37" t="inlineStr">
+      <c r="BC37" t="n">
+        <v>4576</v>
+      </c>
+      <c r="BD37" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="BE37" t="inlineStr">
         <is>
           <t>4576</t>
         </is>
@@ -7136,9 +7362,15 @@
       <c r="BB38" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BC38" t="inlineStr">
-        <is>
-          <t>5617</t>
+      <c r="BC38" t="n">
+        <v>5617</v>
+      </c>
+      <c r="BD38" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BE38" t="inlineStr">
+        <is>
+          <t>5852</t>
         </is>
       </c>
     </row>
@@ -7311,9 +7543,15 @@
       <c r="BB39" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BC39" t="inlineStr">
-        <is>
-          <t>5853</t>
+      <c r="BC39" t="n">
+        <v>5853</v>
+      </c>
+      <c r="BD39" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BE39" t="inlineStr">
+        <is>
+          <t>5985</t>
         </is>
       </c>
     </row>
@@ -7486,9 +7724,15 @@
       <c r="BB40" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BC40" t="inlineStr">
-        <is>
-          <t>6462</t>
+      <c r="BC40" t="n">
+        <v>6462</v>
+      </c>
+      <c r="BD40" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BE40" t="inlineStr">
+        <is>
+          <t>6779</t>
         </is>
       </c>
     </row>
@@ -7661,7 +7905,13 @@
       <c r="BB41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC41" t="inlineStr">
+      <c r="BC41" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE41" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7836,9 +8086,15 @@
       <c r="BB42" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="BC42" t="inlineStr">
-        <is>
-          <t>6625</t>
+      <c r="BC42" t="n">
+        <v>6625</v>
+      </c>
+      <c r="BD42" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="BE42" t="inlineStr">
+        <is>
+          <t>6831</t>
         </is>
       </c>
     </row>
@@ -8011,9 +8267,15 @@
       <c r="BB43" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BC43" t="inlineStr">
-        <is>
-          <t>5813</t>
+      <c r="BC43" t="n">
+        <v>5813</v>
+      </c>
+      <c r="BD43" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BE43" t="inlineStr">
+        <is>
+          <t>6016</t>
         </is>
       </c>
     </row>
@@ -8186,9 +8448,15 @@
       <c r="BB44" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BC44" t="inlineStr">
-        <is>
-          <t>5793</t>
+      <c r="BC44" t="n">
+        <v>5793</v>
+      </c>
+      <c r="BD44" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BE44" t="inlineStr">
+        <is>
+          <t>6081</t>
         </is>
       </c>
     </row>
@@ -8361,9 +8629,15 @@
       <c r="BB45" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="BC45" t="inlineStr">
-        <is>
-          <t>5462</t>
+      <c r="BC45" t="n">
+        <v>5462</v>
+      </c>
+      <c r="BD45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE45" t="inlineStr">
+        <is>
+          <t>5479</t>
         </is>
       </c>
     </row>
@@ -8536,9 +8810,15 @@
       <c r="BB46" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BC46" t="inlineStr">
-        <is>
-          <t>5366</t>
+      <c r="BC46" t="n">
+        <v>5366</v>
+      </c>
+      <c r="BD46" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="BE46" t="inlineStr">
+        <is>
+          <t>5708</t>
         </is>
       </c>
     </row>
@@ -8711,9 +8991,15 @@
       <c r="BB47" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BC47" t="inlineStr">
-        <is>
-          <t>4654</t>
+      <c r="BC47" t="n">
+        <v>4654</v>
+      </c>
+      <c r="BD47" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BE47" t="inlineStr">
+        <is>
+          <t>4955</t>
         </is>
       </c>
     </row>
@@ -8886,9 +9172,15 @@
       <c r="BB48" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="BC48" t="inlineStr">
-        <is>
-          <t>6061</t>
+      <c r="BC48" t="n">
+        <v>6061</v>
+      </c>
+      <c r="BD48" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="BE48" t="inlineStr">
+        <is>
+          <t>6388</t>
         </is>
       </c>
     </row>
@@ -9061,9 +9353,15 @@
       <c r="BB49" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="BC49" t="inlineStr">
-        <is>
-          <t>4840</t>
+      <c r="BC49" t="n">
+        <v>4840</v>
+      </c>
+      <c r="BD49" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BE49" t="inlineStr">
+        <is>
+          <t>5026</t>
         </is>
       </c>
     </row>
@@ -9236,9 +9534,15 @@
       <c r="BB50" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BC50" t="inlineStr">
-        <is>
-          <t>6241</t>
+      <c r="BC50" t="n">
+        <v>6241</v>
+      </c>
+      <c r="BD50" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BE50" t="inlineStr">
+        <is>
+          <t>6549</t>
         </is>
       </c>
     </row>
@@ -9411,9 +9715,15 @@
       <c r="BB51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC51" t="inlineStr">
-        <is>
-          <t>2676</t>
+      <c r="BC51" t="n">
+        <v>2676</v>
+      </c>
+      <c r="BD51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE51" t="inlineStr">
+        <is>
+          <t>2688</t>
         </is>
       </c>
     </row>
@@ -9586,9 +9896,15 @@
       <c r="BB52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC52" t="inlineStr">
-        <is>
-          <t>2832</t>
+      <c r="BC52" t="n">
+        <v>2832</v>
+      </c>
+      <c r="BD52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE52" t="inlineStr">
+        <is>
+          <t>2893</t>
         </is>
       </c>
     </row>
@@ -9761,9 +10077,15 @@
       <c r="BB53" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="BC53" t="inlineStr">
-        <is>
-          <t>3486</t>
+      <c r="BC53" t="n">
+        <v>3486</v>
+      </c>
+      <c r="BD53" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="BE53" t="inlineStr">
+        <is>
+          <t>3692</t>
         </is>
       </c>
     </row>
@@ -9936,9 +10258,15 @@
       <c r="BB54" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="BC54" t="inlineStr">
-        <is>
-          <t>5750</t>
+      <c r="BC54" t="n">
+        <v>5750</v>
+      </c>
+      <c r="BD54" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="BE54" t="inlineStr">
+        <is>
+          <t>5900</t>
         </is>
       </c>
     </row>
@@ -10111,9 +10439,15 @@
       <c r="BB55" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BC55" t="inlineStr">
-        <is>
-          <t>4273</t>
+      <c r="BC55" t="n">
+        <v>4273</v>
+      </c>
+      <c r="BD55" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BE55" t="inlineStr">
+        <is>
+          <t>4329</t>
         </is>
       </c>
     </row>
@@ -10286,9 +10620,15 @@
       <c r="BB56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BC56" t="inlineStr">
-        <is>
-          <t>4284</t>
+      <c r="BC56" t="n">
+        <v>4284</v>
+      </c>
+      <c r="BD56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BE56" t="inlineStr">
+        <is>
+          <t>4416</t>
         </is>
       </c>
     </row>
@@ -10461,9 +10801,15 @@
       <c r="BB57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BC57" t="inlineStr">
-        <is>
-          <t>5381</t>
+      <c r="BC57" t="n">
+        <v>5381</v>
+      </c>
+      <c r="BD57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BE57" t="inlineStr">
+        <is>
+          <t>5567</t>
         </is>
       </c>
     </row>
@@ -10636,9 +10982,15 @@
       <c r="BB58" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="BC58" t="inlineStr">
-        <is>
-          <t>4570</t>
+      <c r="BC58" t="n">
+        <v>4570</v>
+      </c>
+      <c r="BD58" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="BE58" t="inlineStr">
+        <is>
+          <t>4820</t>
         </is>
       </c>
     </row>
@@ -10710,6 +11062,8 @@
       <c r="BA59" t="inlineStr"/>
       <c r="BB59" s="3" t="inlineStr"/>
       <c r="BC59" t="inlineStr"/>
+      <c r="BD59" s="3" t="inlineStr"/>
+      <c r="BE59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -10779,6 +11133,8 @@
       <c r="BA60" t="inlineStr"/>
       <c r="BB60" s="3" t="inlineStr"/>
       <c r="BC60" t="inlineStr"/>
+      <c r="BD60" s="3" t="inlineStr"/>
+      <c r="BE60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -10949,9 +11305,15 @@
       <c r="BB61" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BC61" t="inlineStr">
-        <is>
-          <t>4983</t>
+      <c r="BC61" t="n">
+        <v>4983</v>
+      </c>
+      <c r="BD61" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BE61" t="inlineStr">
+        <is>
+          <t>5122</t>
         </is>
       </c>
     </row>
@@ -11124,7 +11486,13 @@
       <c r="BB62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC62" t="inlineStr">
+      <c r="BC62" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11299,9 +11667,15 @@
       <c r="BB63" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="BC63" t="inlineStr">
-        <is>
-          <t>5249</t>
+      <c r="BC63" t="n">
+        <v>5249</v>
+      </c>
+      <c r="BD63" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="BE63" t="inlineStr">
+        <is>
+          <t>5525</t>
         </is>
       </c>
     </row>
@@ -11474,9 +11848,15 @@
       <c r="BB64" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BC64" t="inlineStr">
-        <is>
-          <t>3312</t>
+      <c r="BC64" t="n">
+        <v>3312</v>
+      </c>
+      <c r="BD64" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BE64" t="inlineStr">
+        <is>
+          <t>3858</t>
         </is>
       </c>
     </row>
@@ -11548,6 +11928,8 @@
       <c r="BA65" t="inlineStr"/>
       <c r="BB65" s="3" t="inlineStr"/>
       <c r="BC65" t="inlineStr"/>
+      <c r="BD65" s="3" t="inlineStr"/>
+      <c r="BE65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -11718,9 +12100,15 @@
       <c r="BB66" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BC66" t="inlineStr">
-        <is>
-          <t>3048</t>
+      <c r="BC66" t="n">
+        <v>3048</v>
+      </c>
+      <c r="BD66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE66" t="inlineStr">
+        <is>
+          <t>3037</t>
         </is>
       </c>
     </row>
@@ -11893,9 +12281,15 @@
       <c r="BB67" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BC67" t="inlineStr">
-        <is>
-          <t>5091</t>
+      <c r="BC67" t="n">
+        <v>5091</v>
+      </c>
+      <c r="BD67" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="BE67" t="inlineStr">
+        <is>
+          <t>5269</t>
         </is>
       </c>
     </row>
@@ -12068,9 +12462,15 @@
       <c r="BB68" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BC68" t="inlineStr">
-        <is>
-          <t>5401</t>
+      <c r="BC68" t="n">
+        <v>5401</v>
+      </c>
+      <c r="BD68" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="BE68" t="inlineStr">
+        <is>
+          <t>6113</t>
         </is>
       </c>
     </row>
@@ -12243,9 +12643,15 @@
       <c r="BB69" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BC69" t="inlineStr">
-        <is>
-          <t>4510</t>
+      <c r="BC69" t="n">
+        <v>4510</v>
+      </c>
+      <c r="BD69" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BE69" t="inlineStr">
+        <is>
+          <t>4590</t>
         </is>
       </c>
     </row>
@@ -12418,9 +12824,15 @@
       <c r="BB70" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="BC70" t="inlineStr">
-        <is>
-          <t>3759</t>
+      <c r="BC70" t="n">
+        <v>3759</v>
+      </c>
+      <c r="BD70" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="BE70" t="inlineStr">
+        <is>
+          <t>4256</t>
         </is>
       </c>
     </row>
@@ -12593,9 +13005,15 @@
       <c r="BB71" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BC71" t="inlineStr">
-        <is>
-          <t>4765</t>
+      <c r="BC71" t="n">
+        <v>4765</v>
+      </c>
+      <c r="BD71" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="BE71" t="inlineStr">
+        <is>
+          <t>4902</t>
         </is>
       </c>
     </row>
@@ -12768,9 +13186,15 @@
       <c r="BB72" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="BC72" t="inlineStr">
-        <is>
-          <t>4081</t>
+      <c r="BC72" t="n">
+        <v>4081</v>
+      </c>
+      <c r="BD72" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="BE72" t="inlineStr">
+        <is>
+          <t>4118</t>
         </is>
       </c>
     </row>
@@ -12943,9 +13367,15 @@
       <c r="BB73" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BC73" t="inlineStr">
-        <is>
-          <t>4336</t>
+      <c r="BC73" t="n">
+        <v>4336</v>
+      </c>
+      <c r="BD73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BE73" t="inlineStr">
+        <is>
+          <t>4504</t>
         </is>
       </c>
     </row>
@@ -13118,9 +13548,15 @@
       <c r="BB74" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BC74" t="inlineStr">
-        <is>
-          <t>4016</t>
+      <c r="BC74" t="n">
+        <v>4016</v>
+      </c>
+      <c r="BD74" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BE74" t="inlineStr">
+        <is>
+          <t>4353</t>
         </is>
       </c>
     </row>
@@ -13293,9 +13729,15 @@
       <c r="BB75" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BC75" t="inlineStr">
-        <is>
-          <t>4180</t>
+      <c r="BC75" t="n">
+        <v>4180</v>
+      </c>
+      <c r="BD75" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BE75" t="inlineStr">
+        <is>
+          <t>4262</t>
         </is>
       </c>
     </row>
@@ -13468,9 +13910,15 @@
       <c r="BB76" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BC76" t="inlineStr">
-        <is>
-          <t>5171</t>
+      <c r="BC76" t="n">
+        <v>5171</v>
+      </c>
+      <c r="BD76" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="BE76" t="inlineStr">
+        <is>
+          <t>5321</t>
         </is>
       </c>
     </row>
@@ -13643,7 +14091,13 @@
       <c r="BB77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC77" t="inlineStr">
+      <c r="BC77" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE77" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13818,9 +14272,15 @@
       <c r="BB78" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BC78" t="inlineStr">
-        <is>
-          <t>5071</t>
+      <c r="BC78" t="n">
+        <v>5071</v>
+      </c>
+      <c r="BD78" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BE78" t="inlineStr">
+        <is>
+          <t>5253</t>
         </is>
       </c>
     </row>
@@ -13993,7 +14453,13 @@
       <c r="BB79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC79" t="inlineStr">
+      <c r="BC79" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14168,9 +14634,15 @@
       <c r="BB80" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="BC80" t="inlineStr">
-        <is>
-          <t>4960</t>
+      <c r="BC80" t="n">
+        <v>4960</v>
+      </c>
+      <c r="BD80" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BE80" t="inlineStr">
+        <is>
+          <t>5115</t>
         </is>
       </c>
     </row>
@@ -14343,9 +14815,15 @@
       <c r="BB81" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BC81" t="inlineStr">
-        <is>
-          <t>5041</t>
+      <c r="BC81" t="n">
+        <v>5041</v>
+      </c>
+      <c r="BD81" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BE81" t="inlineStr">
+        <is>
+          <t>5272</t>
         </is>
       </c>
     </row>
@@ -14518,9 +14996,15 @@
       <c r="BB82" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BC82" t="inlineStr">
-        <is>
-          <t>4686</t>
+      <c r="BC82" t="n">
+        <v>4686</v>
+      </c>
+      <c r="BD82" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BE82" t="inlineStr">
+        <is>
+          <t>4983</t>
         </is>
       </c>
     </row>
@@ -14693,9 +15177,15 @@
       <c r="BB83" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="BC83" t="inlineStr">
-        <is>
-          <t>4541</t>
+      <c r="BC83" t="n">
+        <v>4541</v>
+      </c>
+      <c r="BD83" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BE83" t="inlineStr">
+        <is>
+          <t>4683</t>
         </is>
       </c>
     </row>
@@ -14827,6 +15317,8 @@
       <c r="BA84" t="inlineStr"/>
       <c r="BB84" s="3" t="inlineStr"/>
       <c r="BC84" t="inlineStr"/>
+      <c r="BD84" s="3" t="inlineStr"/>
+      <c r="BE84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -14997,9 +15489,15 @@
       <c r="BB85" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BC85" t="inlineStr">
-        <is>
-          <t>3984</t>
+      <c r="BC85" t="n">
+        <v>3984</v>
+      </c>
+      <c r="BD85" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BE85" t="inlineStr">
+        <is>
+          <t>4159</t>
         </is>
       </c>
     </row>
@@ -15172,9 +15670,15 @@
       <c r="BB86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC86" t="inlineStr">
-        <is>
-          <t>3390</t>
+      <c r="BC86" t="n">
+        <v>3390</v>
+      </c>
+      <c r="BD86" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BE86" t="inlineStr">
+        <is>
+          <t>3711</t>
         </is>
       </c>
     </row>
@@ -15347,9 +15851,15 @@
       <c r="BB87" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BC87" t="inlineStr">
-        <is>
-          <t>4725</t>
+      <c r="BC87" t="n">
+        <v>4725</v>
+      </c>
+      <c r="BD87" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BE87" t="inlineStr">
+        <is>
+          <t>4836</t>
         </is>
       </c>
     </row>
@@ -15522,9 +16032,15 @@
       <c r="BB88" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BC88" t="inlineStr">
-        <is>
-          <t>2916</t>
+      <c r="BC88" t="n">
+        <v>2916</v>
+      </c>
+      <c r="BD88" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="BE88" t="inlineStr">
+        <is>
+          <t>2921</t>
         </is>
       </c>
     </row>
@@ -15697,9 +16213,15 @@
       <c r="BB89" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BC89" t="inlineStr">
-        <is>
-          <t>3415</t>
+      <c r="BC89" t="n">
+        <v>3415</v>
+      </c>
+      <c r="BD89" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BE89" t="inlineStr">
+        <is>
+          <t>3479</t>
         </is>
       </c>
     </row>
@@ -15872,9 +16394,15 @@
       <c r="BB90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC90" t="inlineStr">
-        <is>
-          <t>2833</t>
+      <c r="BC90" t="n">
+        <v>2833</v>
+      </c>
+      <c r="BD90" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BE90" t="inlineStr">
+        <is>
+          <t>3002</t>
         </is>
       </c>
     </row>
@@ -16047,9 +16575,15 @@
       <c r="BB91" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BC91" t="inlineStr">
-        <is>
-          <t>2962</t>
+      <c r="BC91" t="n">
+        <v>2962</v>
+      </c>
+      <c r="BD91" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BE91" t="inlineStr">
+        <is>
+          <t>2983</t>
         </is>
       </c>
     </row>
@@ -16222,7 +16756,13 @@
       <c r="BB92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC92" t="inlineStr">
+      <c r="BC92" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16397,9 +16937,15 @@
       <c r="BB93" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="BC93" t="inlineStr">
-        <is>
-          <t>2418</t>
+      <c r="BC93" t="n">
+        <v>2418</v>
+      </c>
+      <c r="BD93" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="BE93" t="inlineStr">
+        <is>
+          <t>2460</t>
         </is>
       </c>
     </row>
@@ -16572,9 +17118,15 @@
       <c r="BB94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC94" t="inlineStr">
-        <is>
-          <t>2752</t>
+      <c r="BC94" t="n">
+        <v>2752</v>
+      </c>
+      <c r="BD94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE94" t="inlineStr">
+        <is>
+          <t>2799</t>
         </is>
       </c>
     </row>
@@ -16747,9 +17299,15 @@
       <c r="BB95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC95" t="inlineStr">
-        <is>
-          <t>2513</t>
+      <c r="BC95" t="n">
+        <v>2513</v>
+      </c>
+      <c r="BD95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE95" t="inlineStr">
+        <is>
+          <t>2503</t>
         </is>
       </c>
     </row>
@@ -16922,9 +17480,15 @@
       <c r="BB96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC96" t="inlineStr">
-        <is>
-          <t>2462</t>
+      <c r="BC96" t="n">
+        <v>2462</v>
+      </c>
+      <c r="BD96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE96" t="inlineStr">
+        <is>
+          <t>2467</t>
         </is>
       </c>
     </row>
@@ -17097,9 +17661,15 @@
       <c r="BB97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC97" t="inlineStr">
-        <is>
-          <t>3188</t>
+      <c r="BC97" t="n">
+        <v>3188</v>
+      </c>
+      <c r="BD97" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="BE97" t="inlineStr">
+        <is>
+          <t>3558</t>
         </is>
       </c>
     </row>
@@ -17272,7 +17842,13 @@
       <c r="BB98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC98" t="inlineStr">
+      <c r="BC98" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -17447,9 +18023,15 @@
       <c r="BB99" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="BC99" t="inlineStr">
-        <is>
-          <t>3752</t>
+      <c r="BC99" t="n">
+        <v>3752</v>
+      </c>
+      <c r="BD99" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="BE99" t="inlineStr">
+        <is>
+          <t>3836</t>
         </is>
       </c>
     </row>
@@ -17622,9 +18204,15 @@
       <c r="BB100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC100" t="inlineStr">
-        <is>
-          <t>2493</t>
+      <c r="BC100" t="n">
+        <v>2493</v>
+      </c>
+      <c r="BD100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE100" t="inlineStr">
+        <is>
+          <t>2485</t>
         </is>
       </c>
     </row>
@@ -17797,9 +18385,15 @@
       <c r="BB101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BC101" t="inlineStr">
-        <is>
-          <t>4588</t>
+      <c r="BC101" t="n">
+        <v>4588</v>
+      </c>
+      <c r="BD101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BE101" t="inlineStr">
+        <is>
+          <t>4742</t>
         </is>
       </c>
     </row>
@@ -17972,9 +18566,15 @@
       <c r="BB102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BC102" t="inlineStr">
-        <is>
-          <t>4032</t>
+      <c r="BC102" t="n">
+        <v>4032</v>
+      </c>
+      <c r="BD102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BE102" t="inlineStr">
+        <is>
+          <t>4142</t>
         </is>
       </c>
     </row>
@@ -18147,9 +18747,15 @@
       <c r="BB103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC103" t="inlineStr">
-        <is>
-          <t>3754</t>
+      <c r="BC103" t="n">
+        <v>3754</v>
+      </c>
+      <c r="BD103" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="BE103" t="inlineStr">
+        <is>
+          <t>3966</t>
         </is>
       </c>
     </row>
@@ -18322,9 +18928,15 @@
       <c r="BB104" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="BC104" t="inlineStr">
-        <is>
-          <t>4631</t>
+      <c r="BC104" t="n">
+        <v>4631</v>
+      </c>
+      <c r="BD104" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="BE104" t="inlineStr">
+        <is>
+          <t>4703</t>
         </is>
       </c>
     </row>
@@ -18497,9 +19109,15 @@
       <c r="BB105" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="BC105" t="inlineStr">
-        <is>
-          <t>4231</t>
+      <c r="BC105" t="n">
+        <v>4231</v>
+      </c>
+      <c r="BD105" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="BE105" t="inlineStr">
+        <is>
+          <t>4320</t>
         </is>
       </c>
     </row>
@@ -18672,7 +19290,13 @@
       <c r="BB106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC106" t="inlineStr">
+      <c r="BC106" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18847,9 +19471,15 @@
       <c r="BB107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC107" t="inlineStr">
-        <is>
-          <t>2615</t>
+      <c r="BC107" t="n">
+        <v>2615</v>
+      </c>
+      <c r="BD107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE107" t="inlineStr">
+        <is>
+          <t>2614</t>
         </is>
       </c>
     </row>
@@ -19022,7 +19652,13 @@
       <c r="BB108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC108" t="inlineStr">
+      <c r="BC108" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -19197,9 +19833,15 @@
       <c r="BB109" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="BC109" t="inlineStr">
-        <is>
-          <t>3969</t>
+      <c r="BC109" t="n">
+        <v>3969</v>
+      </c>
+      <c r="BD109" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BE109" t="inlineStr">
+        <is>
+          <t>3937</t>
         </is>
       </c>
     </row>
@@ -19372,9 +20014,15 @@
       <c r="BB110" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="BC110" t="inlineStr">
-        <is>
-          <t>3846</t>
+      <c r="BC110" t="n">
+        <v>3846</v>
+      </c>
+      <c r="BD110" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="BE110" t="inlineStr">
+        <is>
+          <t>3886</t>
         </is>
       </c>
     </row>
@@ -19530,6 +20178,8 @@
       <c r="BA111" t="inlineStr"/>
       <c r="BB111" s="3" t="inlineStr"/>
       <c r="BC111" t="inlineStr"/>
+      <c r="BD111" s="3" t="inlineStr"/>
+      <c r="BE111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -19700,9 +20350,15 @@
       <c r="BB112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC112" t="inlineStr">
-        <is>
-          <t>2639</t>
+      <c r="BC112" t="n">
+        <v>2639</v>
+      </c>
+      <c r="BD112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE112" t="inlineStr">
+        <is>
+          <t>2663</t>
         </is>
       </c>
     </row>
@@ -19875,9 +20531,15 @@
       <c r="BB113" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="BC113" t="inlineStr">
-        <is>
-          <t>3668</t>
+      <c r="BC113" t="n">
+        <v>3668</v>
+      </c>
+      <c r="BD113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE113" t="inlineStr">
+        <is>
+          <t>3657</t>
         </is>
       </c>
     </row>
@@ -20050,9 +20712,15 @@
       <c r="BB114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC114" t="inlineStr">
-        <is>
-          <t>3738</t>
+      <c r="BC114" t="n">
+        <v>3738</v>
+      </c>
+      <c r="BD114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE114" t="inlineStr">
+        <is>
+          <t>3779</t>
         </is>
       </c>
     </row>
@@ -20225,9 +20893,15 @@
       <c r="BB115" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="BC115" t="inlineStr">
-        <is>
-          <t>2153</t>
+      <c r="BC115" t="n">
+        <v>2153</v>
+      </c>
+      <c r="BD115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE115" t="inlineStr">
+        <is>
+          <t>2151</t>
         </is>
       </c>
     </row>
@@ -20400,9 +21074,15 @@
       <c r="BB116" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="BC116" t="inlineStr">
-        <is>
-          <t>3237</t>
+      <c r="BC116" t="n">
+        <v>3237</v>
+      </c>
+      <c r="BD116" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="BE116" t="inlineStr">
+        <is>
+          <t>3297</t>
         </is>
       </c>
     </row>
@@ -20575,9 +21255,15 @@
       <c r="BB117" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BC117" t="inlineStr">
-        <is>
-          <t>3824</t>
+      <c r="BC117" t="n">
+        <v>3824</v>
+      </c>
+      <c r="BD117" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BE117" t="inlineStr">
+        <is>
+          <t>4067</t>
         </is>
       </c>
     </row>
@@ -20750,7 +21436,13 @@
       <c r="BB118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC118" t="inlineStr">
+      <c r="BC118" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -20925,9 +21617,15 @@
       <c r="BB119" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BC119" t="inlineStr">
-        <is>
-          <t>4157</t>
+      <c r="BC119" t="n">
+        <v>4157</v>
+      </c>
+      <c r="BD119" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="BE119" t="inlineStr">
+        <is>
+          <t>4355</t>
         </is>
       </c>
     </row>
@@ -21100,9 +21798,15 @@
       <c r="BB120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC120" t="inlineStr">
-        <is>
-          <t>2713</t>
+      <c r="BC120" t="n">
+        <v>2713</v>
+      </c>
+      <c r="BD120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE120" t="inlineStr">
+        <is>
+          <t>2701</t>
         </is>
       </c>
     </row>
@@ -21275,9 +21979,15 @@
       <c r="BB121" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="BC121" t="inlineStr">
-        <is>
-          <t>3539</t>
+      <c r="BC121" t="n">
+        <v>3539</v>
+      </c>
+      <c r="BD121" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="BE121" t="inlineStr">
+        <is>
+          <t>3645</t>
         </is>
       </c>
     </row>
@@ -21450,7 +22160,13 @@
       <c r="BB122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC122" t="inlineStr">
+      <c r="BC122" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -21625,9 +22341,15 @@
       <c r="BB123" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BC123" t="inlineStr">
-        <is>
-          <t>3415</t>
+      <c r="BC123" t="n">
+        <v>3415</v>
+      </c>
+      <c r="BD123" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="BE123" t="inlineStr">
+        <is>
+          <t>3435</t>
         </is>
       </c>
     </row>
@@ -21800,9 +22522,15 @@
       <c r="BB124" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="BC124" t="inlineStr">
-        <is>
-          <t>3394</t>
+      <c r="BC124" t="n">
+        <v>3394</v>
+      </c>
+      <c r="BD124" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="BE124" t="inlineStr">
+        <is>
+          <t>3452</t>
         </is>
       </c>
     </row>
@@ -21975,9 +22703,15 @@
       <c r="BB125" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BC125" t="inlineStr">
-        <is>
-          <t>3656</t>
+      <c r="BC125" t="n">
+        <v>3656</v>
+      </c>
+      <c r="BD125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE125" t="inlineStr">
+        <is>
+          <t>3649</t>
         </is>
       </c>
     </row>
@@ -22150,9 +22884,15 @@
       <c r="BB126" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BC126" t="inlineStr">
-        <is>
-          <t>3411</t>
+      <c r="BC126" t="n">
+        <v>3411</v>
+      </c>
+      <c r="BD126" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BE126" t="inlineStr">
+        <is>
+          <t>3438</t>
         </is>
       </c>
     </row>
@@ -22325,9 +23065,15 @@
       <c r="BB127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC127" t="inlineStr">
-        <is>
-          <t>2258</t>
+      <c r="BC127" t="n">
+        <v>2258</v>
+      </c>
+      <c r="BD127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE127" t="inlineStr">
+        <is>
+          <t>2241</t>
         </is>
       </c>
     </row>
@@ -22500,7 +23246,13 @@
       <c r="BB128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC128" t="inlineStr">
+      <c r="BC128" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -22675,7 +23427,13 @@
       <c r="BB129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC129" t="inlineStr">
+      <c r="BC129" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -22850,9 +23608,15 @@
       <c r="BB130" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="BC130" t="inlineStr">
-        <is>
-          <t>2962</t>
+      <c r="BC130" t="n">
+        <v>2962</v>
+      </c>
+      <c r="BD130" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BE130" t="inlineStr">
+        <is>
+          <t>3024</t>
         </is>
       </c>
     </row>
@@ -23025,7 +23789,13 @@
       <c r="BB131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC131" t="inlineStr">
+      <c r="BC131" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -23200,7 +23970,13 @@
       <c r="BB132" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BC132" t="inlineStr">
+      <c r="BC132" t="n">
+        <v>2749</v>
+      </c>
+      <c r="BD132" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BE132" t="inlineStr">
         <is>
           <t>2749</t>
         </is>
@@ -23375,9 +24151,15 @@
       <c r="BB133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC133" t="inlineStr">
-        <is>
-          <t>2779</t>
+      <c r="BC133" t="n">
+        <v>2779</v>
+      </c>
+      <c r="BD133" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BE133" t="inlineStr">
+        <is>
+          <t>3039</t>
         </is>
       </c>
     </row>
@@ -23473,6 +24255,8 @@
       <c r="BA134" t="inlineStr"/>
       <c r="BB134" s="3" t="inlineStr"/>
       <c r="BC134" t="inlineStr"/>
+      <c r="BD134" s="3" t="inlineStr"/>
+      <c r="BE134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -23558,6 +24342,8 @@
       <c r="BA135" t="inlineStr"/>
       <c r="BB135" s="3" t="inlineStr"/>
       <c r="BC135" t="inlineStr"/>
+      <c r="BD135" s="3" t="inlineStr"/>
+      <c r="BE135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -23728,7 +24514,13 @@
       <c r="BB136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC136" t="inlineStr">
+      <c r="BC136" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE136" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -23903,7 +24695,13 @@
       <c r="BB137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC137" t="inlineStr">
+      <c r="BC137" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -23993,6 +24791,8 @@
       <c r="BA138" t="inlineStr"/>
       <c r="BB138" s="3" t="inlineStr"/>
       <c r="BC138" t="inlineStr"/>
+      <c r="BD138" s="3" t="inlineStr"/>
+      <c r="BE138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -24163,9 +24963,15 @@
       <c r="BB139" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BC139" t="inlineStr">
-        <is>
-          <t>2726</t>
+      <c r="BC139" t="n">
+        <v>2726</v>
+      </c>
+      <c r="BD139" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BE139" t="inlineStr">
+        <is>
+          <t>2901</t>
         </is>
       </c>
     </row>
@@ -24338,9 +25144,15 @@
       <c r="BB140" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BC140" t="inlineStr">
-        <is>
-          <t>3037</t>
+      <c r="BC140" t="n">
+        <v>3037</v>
+      </c>
+      <c r="BD140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE140" t="inlineStr">
+        <is>
+          <t>2971</t>
         </is>
       </c>
     </row>
@@ -24428,6 +25240,8 @@
       <c r="BA141" t="inlineStr"/>
       <c r="BB141" s="3" t="inlineStr"/>
       <c r="BC141" t="inlineStr"/>
+      <c r="BD141" s="3" t="inlineStr"/>
+      <c r="BE141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -24598,7 +25412,13 @@
       <c r="BB142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC142" t="inlineStr">
+      <c r="BC142" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE142" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -24688,6 +25508,8 @@
       <c r="BA143" t="inlineStr"/>
       <c r="BB143" s="3" t="inlineStr"/>
       <c r="BC143" t="inlineStr"/>
+      <c r="BD143" s="3" t="inlineStr"/>
+      <c r="BE143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -24773,6 +25595,8 @@
       <c r="BA144" t="inlineStr"/>
       <c r="BB144" s="3" t="inlineStr"/>
       <c r="BC144" t="inlineStr"/>
+      <c r="BD144" s="3" t="inlineStr"/>
+      <c r="BE144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -24858,6 +25682,8 @@
       <c r="BA145" t="inlineStr"/>
       <c r="BB145" s="3" t="inlineStr"/>
       <c r="BC145" t="inlineStr"/>
+      <c r="BD145" s="3" t="inlineStr"/>
+      <c r="BE145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -24943,6 +25769,8 @@
       <c r="BA146" t="inlineStr"/>
       <c r="BB146" s="3" t="inlineStr"/>
       <c r="BC146" t="inlineStr"/>
+      <c r="BD146" s="3" t="inlineStr"/>
+      <c r="BE146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -25028,6 +25856,8 @@
       <c r="BA147" t="inlineStr"/>
       <c r="BB147" s="3" t="inlineStr"/>
       <c r="BC147" t="inlineStr"/>
+      <c r="BD147" s="3" t="inlineStr"/>
+      <c r="BE147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -25198,7 +26028,13 @@
       <c r="BB148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC148" t="inlineStr">
+      <c r="BC148" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -25373,9 +26209,15 @@
       <c r="BB149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC149" t="inlineStr">
-        <is>
-          <t>3743</t>
+      <c r="BC149" t="n">
+        <v>3743</v>
+      </c>
+      <c r="BD149" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="BE149" t="inlineStr">
+        <is>
+          <t>3835</t>
         </is>
       </c>
     </row>
@@ -25548,7 +26390,13 @@
       <c r="BB150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC150" t="inlineStr">
+      <c r="BC150" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -25723,7 +26571,13 @@
       <c r="BB151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC151" t="inlineStr">
+      <c r="BC151" t="n">
+        <v>2622</v>
+      </c>
+      <c r="BD151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE151" t="inlineStr">
         <is>
           <t>2622</t>
         </is>
@@ -25898,7 +26752,13 @@
       <c r="BB152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC152" t="inlineStr">
+      <c r="BC152" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -26073,7 +26933,13 @@
       <c r="BB153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC153" t="inlineStr">
+      <c r="BC153" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -26248,7 +27114,13 @@
       <c r="BB154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC154" t="inlineStr">
+      <c r="BC154" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -26423,9 +27295,15 @@
       <c r="BB155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC155" t="inlineStr">
-        <is>
-          <t>2755</t>
+      <c r="BC155" t="n">
+        <v>2755</v>
+      </c>
+      <c r="BD155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE155" t="inlineStr">
+        <is>
+          <t>2753</t>
         </is>
       </c>
     </row>
@@ -26592,9 +27470,15 @@
       <c r="BB156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC156" t="inlineStr">
-        <is>
-          <t>3199</t>
+      <c r="BC156" t="n">
+        <v>3199</v>
+      </c>
+      <c r="BD156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE156" t="inlineStr">
+        <is>
+          <t>3205</t>
         </is>
       </c>
     </row>
@@ -26676,6 +27560,8 @@
       <c r="BA157" t="inlineStr"/>
       <c r="BB157" s="3" t="inlineStr"/>
       <c r="BC157" t="inlineStr"/>
+      <c r="BD157" s="3" t="inlineStr"/>
+      <c r="BE157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -26840,7 +27726,13 @@
       <c r="BB158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC158" t="inlineStr">
+      <c r="BC158" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -27009,9 +27901,15 @@
       <c r="BB159" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BC159" t="inlineStr">
-        <is>
-          <t>3106</t>
+      <c r="BC159" t="n">
+        <v>3106</v>
+      </c>
+      <c r="BD159" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BE159" t="inlineStr">
+        <is>
+          <t>3192</t>
         </is>
       </c>
     </row>
@@ -27093,6 +27991,8 @@
       <c r="BA160" t="inlineStr"/>
       <c r="BB160" s="3" t="inlineStr"/>
       <c r="BC160" t="inlineStr"/>
+      <c r="BD160" s="3" t="inlineStr"/>
+      <c r="BE160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -27245,9 +28145,15 @@
       <c r="BB161" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="BC161" t="inlineStr">
-        <is>
-          <t>3353</t>
+      <c r="BC161" t="n">
+        <v>3353</v>
+      </c>
+      <c r="BD161" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="BE161" t="inlineStr">
+        <is>
+          <t>3429</t>
         </is>
       </c>
     </row>
@@ -27402,9 +28308,15 @@
       <c r="BB162" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BC162" t="inlineStr">
-        <is>
-          <t>2998</t>
+      <c r="BC162" t="n">
+        <v>2998</v>
+      </c>
+      <c r="BD162" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="BE162" t="inlineStr">
+        <is>
+          <t>3013</t>
         </is>
       </c>
     </row>
@@ -27555,9 +28467,15 @@
       <c r="BB163" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC163" t="inlineStr">
-        <is>
-          <t>3382</t>
+      <c r="BC163" t="n">
+        <v>3382</v>
+      </c>
+      <c r="BD163" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE163" t="inlineStr">
+        <is>
+          <t>3385</t>
         </is>
       </c>
     </row>
@@ -27692,9 +28610,15 @@
       <c r="BB164" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="BC164" t="inlineStr">
-        <is>
-          <t>3577</t>
+      <c r="BC164" t="n">
+        <v>3577</v>
+      </c>
+      <c r="BD164" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE164" t="inlineStr">
+        <is>
+          <t>3587</t>
         </is>
       </c>
     </row>
@@ -27833,9 +28757,15 @@
       <c r="BB165" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="BC165" t="inlineStr">
-        <is>
-          <t>2938</t>
+      <c r="BC165" t="n">
+        <v>2938</v>
+      </c>
+      <c r="BD165" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="BE165" t="inlineStr">
+        <is>
+          <t>2918</t>
         </is>
       </c>
     </row>
@@ -27966,9 +28896,15 @@
       <c r="BB166" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC166" t="inlineStr">
-        <is>
-          <t>2803</t>
+      <c r="BC166" t="n">
+        <v>2803</v>
+      </c>
+      <c r="BD166" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE166" t="inlineStr">
+        <is>
+          <t>2800</t>
         </is>
       </c>
     </row>
@@ -28087,7 +29023,13 @@
       <c r="BB167" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC167" t="inlineStr">
+      <c r="BC167" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD167" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE167" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -28204,7 +29146,13 @@
       <c r="BB168" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC168" t="inlineStr">
+      <c r="BC168" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD168" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE168" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -28280,6 +29228,8 @@
       <c r="BA169" t="inlineStr"/>
       <c r="BB169" s="3" t="inlineStr"/>
       <c r="BC169" t="inlineStr"/>
+      <c r="BD169" s="3" t="inlineStr"/>
+      <c r="BE169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="n">
@@ -28388,7 +29338,13 @@
       <c r="BB170" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC170" t="inlineStr">
+      <c r="BC170" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD170" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE170" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -28489,7 +29445,13 @@
       <c r="BB171" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC171" t="inlineStr">
+      <c r="BC171" t="n">
+        <v>1781</v>
+      </c>
+      <c r="BD171" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE171" t="inlineStr">
         <is>
           <t>1781</t>
         </is>
@@ -28590,7 +29552,13 @@
       <c r="BB172" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC172" t="inlineStr">
+      <c r="BC172" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD172" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE172" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -28691,9 +29659,15 @@
       <c r="BB173" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BC173" t="inlineStr">
-        <is>
-          <t>1857</t>
+      <c r="BC173" t="n">
+        <v>1857</v>
+      </c>
+      <c r="BD173" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE173" t="inlineStr">
+        <is>
+          <t>1848</t>
         </is>
       </c>
     </row>
@@ -28768,9 +29742,15 @@
       <c r="BB174" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="BC174" t="inlineStr">
-        <is>
-          <t>3257</t>
+      <c r="BC174" t="n">
+        <v>3257</v>
+      </c>
+      <c r="BD174" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="BE174" t="inlineStr">
+        <is>
+          <t>3352</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-03-12 11:42:44
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BE174"/>
+  <dimension ref="A1:BG175"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -676,6 +676,16 @@
           <t>03-10_0</t>
         </is>
       </c>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>03-11_A</t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="inlineStr">
+        <is>
+          <t>03-11_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -852,9 +862,15 @@
       <c r="BD2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE2" t="inlineStr">
-        <is>
-          <t>2951</t>
+      <c r="BE2" t="n">
+        <v>2951</v>
+      </c>
+      <c r="BF2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG2" t="inlineStr">
+        <is>
+          <t>2981</t>
         </is>
       </c>
     </row>
@@ -1033,9 +1049,15 @@
       <c r="BD3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BE3" t="inlineStr">
-        <is>
-          <t>6482</t>
+      <c r="BE3" t="n">
+        <v>6482</v>
+      </c>
+      <c r="BF3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BG3" t="inlineStr">
+        <is>
+          <t>6803</t>
         </is>
       </c>
     </row>
@@ -1214,9 +1236,15 @@
       <c r="BD4" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="BE4" t="inlineStr">
-        <is>
-          <t>6337</t>
+      <c r="BE4" t="n">
+        <v>6337</v>
+      </c>
+      <c r="BF4" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="BG4" t="inlineStr">
+        <is>
+          <t>6458</t>
         </is>
       </c>
     </row>
@@ -1239,7 +1267,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F5" s="3" t="n">
@@ -1395,9 +1423,15 @@
       <c r="BD5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BE5" t="inlineStr">
-        <is>
-          <t>6159</t>
+      <c r="BE5" t="n">
+        <v>6159</v>
+      </c>
+      <c r="BF5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BG5" t="inlineStr">
+        <is>
+          <t>6410</t>
         </is>
       </c>
     </row>
@@ -1576,9 +1610,15 @@
       <c r="BD6" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BE6" t="inlineStr">
-        <is>
-          <t>6033</t>
+      <c r="BE6" t="n">
+        <v>6033</v>
+      </c>
+      <c r="BF6" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BG6" t="inlineStr">
+        <is>
+          <t>6269</t>
         </is>
       </c>
     </row>
@@ -1757,9 +1797,15 @@
       <c r="BD7" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BE7" t="inlineStr">
-        <is>
-          <t>6594</t>
+      <c r="BE7" t="n">
+        <v>6594</v>
+      </c>
+      <c r="BF7" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="BG7" t="inlineStr">
+        <is>
+          <t>6891</t>
         </is>
       </c>
     </row>
@@ -1938,9 +1984,15 @@
       <c r="BD8" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BE8" t="inlineStr">
-        <is>
-          <t>5700</t>
+      <c r="BE8" t="n">
+        <v>5700</v>
+      </c>
+      <c r="BF8" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="BG8" t="inlineStr">
+        <is>
+          <t>5809</t>
         </is>
       </c>
     </row>
@@ -2119,9 +2171,15 @@
       <c r="BD9" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BE9" t="inlineStr">
-        <is>
-          <t>5864</t>
+      <c r="BE9" t="n">
+        <v>5864</v>
+      </c>
+      <c r="BF9" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BG9" t="inlineStr">
+        <is>
+          <t>6118</t>
         </is>
       </c>
     </row>
@@ -2300,9 +2358,15 @@
       <c r="BD10" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="BE10" t="inlineStr">
-        <is>
-          <t>6917</t>
+      <c r="BE10" t="n">
+        <v>6917</v>
+      </c>
+      <c r="BF10" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BG10" t="inlineStr">
+        <is>
+          <t>7354</t>
         </is>
       </c>
     </row>
@@ -2481,9 +2545,15 @@
       <c r="BD11" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE11" t="inlineStr">
-        <is>
-          <t>4932</t>
+      <c r="BE11" t="n">
+        <v>4932</v>
+      </c>
+      <c r="BF11" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="BG11" t="inlineStr">
+        <is>
+          <t>4994</t>
         </is>
       </c>
     </row>
@@ -2662,9 +2732,15 @@
       <c r="BD12" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="BE12" t="inlineStr">
-        <is>
-          <t>2928</t>
+      <c r="BE12" t="n">
+        <v>2928</v>
+      </c>
+      <c r="BF12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG12" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2687,7 +2763,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F13" s="5" t="n">
@@ -2843,9 +2919,15 @@
       <c r="BD13" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="BE13" t="inlineStr">
-        <is>
-          <t>6977</t>
+      <c r="BE13" t="n">
+        <v>6977</v>
+      </c>
+      <c r="BF13" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="BG13" t="inlineStr">
+        <is>
+          <t>7102</t>
         </is>
       </c>
     </row>
@@ -3024,9 +3106,15 @@
       <c r="BD14" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BE14" t="inlineStr">
-        <is>
-          <t>5798</t>
+      <c r="BE14" t="n">
+        <v>5798</v>
+      </c>
+      <c r="BF14" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BG14" t="inlineStr">
+        <is>
+          <t>6052</t>
         </is>
       </c>
     </row>
@@ -3205,9 +3293,15 @@
       <c r="BD15" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE15" t="inlineStr">
-        <is>
-          <t>2743</t>
+      <c r="BE15" t="n">
+        <v>2743</v>
+      </c>
+      <c r="BF15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG15" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3386,9 +3480,15 @@
       <c r="BD16" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BE16" t="inlineStr">
-        <is>
-          <t>6227</t>
+      <c r="BE16" t="n">
+        <v>6227</v>
+      </c>
+      <c r="BF16" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BG16" t="inlineStr">
+        <is>
+          <t>6558</t>
         </is>
       </c>
     </row>
@@ -3567,9 +3667,15 @@
       <c r="BD17" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BE17" t="inlineStr">
-        <is>
-          <t>4451</t>
+      <c r="BE17" t="n">
+        <v>4451</v>
+      </c>
+      <c r="BF17" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BG17" t="inlineStr">
+        <is>
+          <t>4525</t>
         </is>
       </c>
     </row>
@@ -3748,9 +3854,15 @@
       <c r="BD18" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="BE18" t="inlineStr">
-        <is>
-          <t>5284</t>
+      <c r="BE18" t="n">
+        <v>5284</v>
+      </c>
+      <c r="BF18" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BG18" t="inlineStr">
+        <is>
+          <t>5346</t>
         </is>
       </c>
     </row>
@@ -3773,7 +3885,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F19" s="3" t="n">
@@ -3929,9 +4041,15 @@
       <c r="BD19" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BE19" t="inlineStr">
-        <is>
-          <t>6384</t>
+      <c r="BE19" t="n">
+        <v>6384</v>
+      </c>
+      <c r="BF19" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BG19" t="inlineStr">
+        <is>
+          <t>6549</t>
         </is>
       </c>
     </row>
@@ -3954,7 +4072,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F20" s="3" t="n">
@@ -4110,9 +4228,15 @@
       <c r="BD20" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="BE20" t="inlineStr">
-        <is>
-          <t>7018</t>
+      <c r="BE20" t="n">
+        <v>7018</v>
+      </c>
+      <c r="BF20" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="BG20" t="inlineStr">
+        <is>
+          <t>7464</t>
         </is>
       </c>
     </row>
@@ -4291,9 +4415,15 @@
       <c r="BD21" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BE21" t="inlineStr">
-        <is>
-          <t>5526</t>
+      <c r="BE21" t="n">
+        <v>5526</v>
+      </c>
+      <c r="BF21" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="BG21" t="inlineStr">
+        <is>
+          <t>5550</t>
         </is>
       </c>
     </row>
@@ -4472,9 +4602,15 @@
       <c r="BD22" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="BE22" t="inlineStr">
-        <is>
-          <t>5995</t>
+      <c r="BE22" t="n">
+        <v>5995</v>
+      </c>
+      <c r="BF22" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BG22" t="inlineStr">
+        <is>
+          <t>6297</t>
         </is>
       </c>
     </row>
@@ -4653,9 +4789,15 @@
       <c r="BD23" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BE23" t="inlineStr">
-        <is>
-          <t>5186</t>
+      <c r="BE23" t="n">
+        <v>5186</v>
+      </c>
+      <c r="BF23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG23" t="inlineStr">
+        <is>
+          <t>5208</t>
         </is>
       </c>
     </row>
@@ -4678,7 +4820,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F24" s="5" t="n">
@@ -4834,9 +4976,15 @@
       <c r="BD24" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BE24" t="inlineStr">
-        <is>
-          <t>6207</t>
+      <c r="BE24" t="n">
+        <v>6207</v>
+      </c>
+      <c r="BF24" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BG24" t="inlineStr">
+        <is>
+          <t>6532</t>
         </is>
       </c>
     </row>
@@ -5015,7 +5163,13 @@
       <c r="BD25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE25" t="inlineStr">
+      <c r="BE25" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5196,9 +5350,15 @@
       <c r="BD26" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="BE26" t="inlineStr">
-        <is>
-          <t>6205</t>
+      <c r="BE26" t="n">
+        <v>6205</v>
+      </c>
+      <c r="BF26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG26" t="inlineStr">
+        <is>
+          <t>6210</t>
         </is>
       </c>
     </row>
@@ -5377,9 +5537,15 @@
       <c r="BD27" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BE27" t="inlineStr">
-        <is>
-          <t>6323</t>
+      <c r="BE27" t="n">
+        <v>6323</v>
+      </c>
+      <c r="BF27" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BG27" t="inlineStr">
+        <is>
+          <t>6592</t>
         </is>
       </c>
     </row>
@@ -5402,7 +5568,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F28" s="3" t="n">
@@ -5558,9 +5724,15 @@
       <c r="BD28" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="BE28" t="inlineStr">
-        <is>
-          <t>6149</t>
+      <c r="BE28" t="n">
+        <v>6149</v>
+      </c>
+      <c r="BF28" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BG28" t="inlineStr">
+        <is>
+          <t>6148</t>
         </is>
       </c>
     </row>
@@ -5739,9 +5911,15 @@
       <c r="BD29" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BE29" t="inlineStr">
-        <is>
-          <t>6938</t>
+      <c r="BE29" t="n">
+        <v>6938</v>
+      </c>
+      <c r="BF29" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BG29" t="inlineStr">
+        <is>
+          <t>7139</t>
         </is>
       </c>
     </row>
@@ -5920,9 +6098,15 @@
       <c r="BD30" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="BE30" t="inlineStr">
-        <is>
-          <t>5854</t>
+      <c r="BE30" t="n">
+        <v>5854</v>
+      </c>
+      <c r="BF30" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="BG30" t="inlineStr">
+        <is>
+          <t>6063</t>
         </is>
       </c>
     </row>
@@ -6101,9 +6285,15 @@
       <c r="BD31" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BE31" t="inlineStr">
-        <is>
-          <t>6860</t>
+      <c r="BE31" t="n">
+        <v>6860</v>
+      </c>
+      <c r="BF31" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="BG31" t="inlineStr">
+        <is>
+          <t>6939</t>
         </is>
       </c>
     </row>
@@ -6282,9 +6472,15 @@
       <c r="BD32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE32" t="inlineStr">
-        <is>
-          <t>6273</t>
+      <c r="BE32" t="n">
+        <v>6273</v>
+      </c>
+      <c r="BF32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG32" t="inlineStr">
+        <is>
+          <t>6262</t>
         </is>
       </c>
     </row>
@@ -6463,9 +6659,15 @@
       <c r="BD33" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="BE33" t="inlineStr">
-        <is>
-          <t>5780</t>
+      <c r="BE33" t="n">
+        <v>5780</v>
+      </c>
+      <c r="BF33" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BG33" t="inlineStr">
+        <is>
+          <t>6025</t>
         </is>
       </c>
     </row>
@@ -6644,9 +6846,15 @@
       <c r="BD34" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BE34" t="inlineStr">
-        <is>
-          <t>5881</t>
+      <c r="BE34" t="n">
+        <v>5881</v>
+      </c>
+      <c r="BF34" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BG34" t="inlineStr">
+        <is>
+          <t>5981</t>
         </is>
       </c>
     </row>
@@ -6825,9 +7033,15 @@
       <c r="BD35" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="BE35" t="inlineStr">
-        <is>
-          <t>6456</t>
+      <c r="BE35" t="n">
+        <v>6456</v>
+      </c>
+      <c r="BF35" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="BG35" t="inlineStr">
+        <is>
+          <t>6548</t>
         </is>
       </c>
     </row>
@@ -7006,9 +7220,15 @@
       <c r="BD36" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BE36" t="inlineStr">
-        <is>
-          <t>5844</t>
+      <c r="BE36" t="n">
+        <v>5844</v>
+      </c>
+      <c r="BF36" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="BG36" t="inlineStr">
+        <is>
+          <t>6074</t>
         </is>
       </c>
     </row>
@@ -7187,9 +7407,15 @@
       <c r="BD37" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="BE37" t="inlineStr">
-        <is>
-          <t>4576</t>
+      <c r="BE37" t="n">
+        <v>4576</v>
+      </c>
+      <c r="BF37" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="BG37" t="inlineStr">
+        <is>
+          <t>4600</t>
         </is>
       </c>
     </row>
@@ -7368,9 +7594,15 @@
       <c r="BD38" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BE38" t="inlineStr">
-        <is>
-          <t>5852</t>
+      <c r="BE38" t="n">
+        <v>5852</v>
+      </c>
+      <c r="BF38" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="BG38" t="inlineStr">
+        <is>
+          <t>6105</t>
         </is>
       </c>
     </row>
@@ -7549,9 +7781,15 @@
       <c r="BD39" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BE39" t="inlineStr">
-        <is>
-          <t>5985</t>
+      <c r="BE39" t="n">
+        <v>5985</v>
+      </c>
+      <c r="BF39" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BG39" t="inlineStr">
+        <is>
+          <t>6227</t>
         </is>
       </c>
     </row>
@@ -7730,9 +7968,15 @@
       <c r="BD40" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BE40" t="inlineStr">
-        <is>
-          <t>6779</t>
+      <c r="BE40" t="n">
+        <v>6779</v>
+      </c>
+      <c r="BF40" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BG40" t="inlineStr">
+        <is>
+          <t>7115</t>
         </is>
       </c>
     </row>
@@ -7911,7 +8155,13 @@
       <c r="BD41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE41" t="inlineStr">
+      <c r="BE41" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG41" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8092,9 +8342,15 @@
       <c r="BD42" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="BE42" t="inlineStr">
-        <is>
-          <t>6831</t>
+      <c r="BE42" t="n">
+        <v>6831</v>
+      </c>
+      <c r="BF42" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="BG42" t="inlineStr">
+        <is>
+          <t>7141</t>
         </is>
       </c>
     </row>
@@ -8273,9 +8529,15 @@
       <c r="BD43" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BE43" t="inlineStr">
-        <is>
-          <t>6016</t>
+      <c r="BE43" t="n">
+        <v>6016</v>
+      </c>
+      <c r="BF43" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BG43" t="inlineStr">
+        <is>
+          <t>6368</t>
         </is>
       </c>
     </row>
@@ -8454,9 +8716,15 @@
       <c r="BD44" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BE44" t="inlineStr">
-        <is>
-          <t>6081</t>
+      <c r="BE44" t="n">
+        <v>6081</v>
+      </c>
+      <c r="BF44" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="BG44" t="inlineStr">
+        <is>
+          <t>6271</t>
         </is>
       </c>
     </row>
@@ -8635,9 +8903,15 @@
       <c r="BD45" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE45" t="inlineStr">
-        <is>
-          <t>5479</t>
+      <c r="BE45" t="n">
+        <v>5479</v>
+      </c>
+      <c r="BF45" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BG45" t="inlineStr">
+        <is>
+          <t>6079</t>
         </is>
       </c>
     </row>
@@ -8816,9 +9090,15 @@
       <c r="BD46" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="BE46" t="inlineStr">
-        <is>
-          <t>5708</t>
+      <c r="BE46" t="n">
+        <v>5708</v>
+      </c>
+      <c r="BF46" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="BG46" t="inlineStr">
+        <is>
+          <t>5949</t>
         </is>
       </c>
     </row>
@@ -8997,9 +9277,15 @@
       <c r="BD47" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BE47" t="inlineStr">
-        <is>
-          <t>4955</t>
+      <c r="BE47" t="n">
+        <v>4955</v>
+      </c>
+      <c r="BF47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG47" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -9178,9 +9464,15 @@
       <c r="BD48" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="BE48" t="inlineStr">
-        <is>
-          <t>6388</t>
+      <c r="BE48" t="n">
+        <v>6388</v>
+      </c>
+      <c r="BF48" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="BG48" t="inlineStr">
+        <is>
+          <t>6613</t>
         </is>
       </c>
     </row>
@@ -9359,9 +9651,15 @@
       <c r="BD49" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BE49" t="inlineStr">
-        <is>
-          <t>5026</t>
+      <c r="BE49" t="n">
+        <v>5026</v>
+      </c>
+      <c r="BF49" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="BG49" t="inlineStr">
+        <is>
+          <t>5260</t>
         </is>
       </c>
     </row>
@@ -9540,9 +9838,15 @@
       <c r="BD50" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BE50" t="inlineStr">
-        <is>
-          <t>6549</t>
+      <c r="BE50" t="n">
+        <v>6549</v>
+      </c>
+      <c r="BF50" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="BG50" t="inlineStr">
+        <is>
+          <t>6552</t>
         </is>
       </c>
     </row>
@@ -9721,9 +10025,15 @@
       <c r="BD51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE51" t="inlineStr">
-        <is>
-          <t>2688</t>
+      <c r="BE51" t="n">
+        <v>2688</v>
+      </c>
+      <c r="BF51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG51" t="inlineStr">
+        <is>
+          <t>2686</t>
         </is>
       </c>
     </row>
@@ -9902,9 +10212,15 @@
       <c r="BD52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE52" t="inlineStr">
-        <is>
-          <t>2893</t>
+      <c r="BE52" t="n">
+        <v>2893</v>
+      </c>
+      <c r="BF52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG52" t="inlineStr">
+        <is>
+          <t>2938</t>
         </is>
       </c>
     </row>
@@ -10083,9 +10399,15 @@
       <c r="BD53" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="BE53" t="inlineStr">
-        <is>
-          <t>3692</t>
+      <c r="BE53" t="n">
+        <v>3692</v>
+      </c>
+      <c r="BF53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG53" t="inlineStr">
+        <is>
+          <t>3722</t>
         </is>
       </c>
     </row>
@@ -10264,9 +10586,15 @@
       <c r="BD54" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="BE54" t="inlineStr">
-        <is>
-          <t>5900</t>
+      <c r="BE54" t="n">
+        <v>5900</v>
+      </c>
+      <c r="BF54" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="BG54" t="inlineStr">
+        <is>
+          <t>6139</t>
         </is>
       </c>
     </row>
@@ -10445,9 +10773,15 @@
       <c r="BD55" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BE55" t="inlineStr">
-        <is>
-          <t>4329</t>
+      <c r="BE55" t="n">
+        <v>4329</v>
+      </c>
+      <c r="BF55" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BG55" t="inlineStr">
+        <is>
+          <t>4540</t>
         </is>
       </c>
     </row>
@@ -10626,9 +10960,15 @@
       <c r="BD56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BE56" t="inlineStr">
-        <is>
-          <t>4416</t>
+      <c r="BE56" t="n">
+        <v>4416</v>
+      </c>
+      <c r="BF56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BG56" t="inlineStr">
+        <is>
+          <t>4444</t>
         </is>
       </c>
     </row>
@@ -10807,9 +11147,15 @@
       <c r="BD57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BE57" t="inlineStr">
-        <is>
-          <t>5567</t>
+      <c r="BE57" t="n">
+        <v>5567</v>
+      </c>
+      <c r="BF57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BG57" t="inlineStr">
+        <is>
+          <t>5724</t>
         </is>
       </c>
     </row>
@@ -10988,9 +11334,15 @@
       <c r="BD58" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="BE58" t="inlineStr">
-        <is>
-          <t>4820</t>
+      <c r="BE58" t="n">
+        <v>4820</v>
+      </c>
+      <c r="BF58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG58" t="inlineStr">
+        <is>
+          <t>4769</t>
         </is>
       </c>
     </row>
@@ -11064,6 +11416,8 @@
       <c r="BC59" t="inlineStr"/>
       <c r="BD59" s="3" t="inlineStr"/>
       <c r="BE59" t="inlineStr"/>
+      <c r="BF59" s="3" t="inlineStr"/>
+      <c r="BG59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -11135,6 +11489,8 @@
       <c r="BC60" t="inlineStr"/>
       <c r="BD60" s="3" t="inlineStr"/>
       <c r="BE60" t="inlineStr"/>
+      <c r="BF60" s="3" t="inlineStr"/>
+      <c r="BG60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -11311,9 +11667,15 @@
       <c r="BD61" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BE61" t="inlineStr">
-        <is>
-          <t>5122</t>
+      <c r="BE61" t="n">
+        <v>5122</v>
+      </c>
+      <c r="BF61" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="BG61" t="inlineStr">
+        <is>
+          <t>5391</t>
         </is>
       </c>
     </row>
@@ -11492,7 +11854,13 @@
       <c r="BD62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE62" t="inlineStr">
+      <c r="BE62" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11673,9 +12041,15 @@
       <c r="BD63" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="BE63" t="inlineStr">
-        <is>
-          <t>5525</t>
+      <c r="BE63" t="n">
+        <v>5525</v>
+      </c>
+      <c r="BF63" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="BG63" t="inlineStr">
+        <is>
+          <t>5784</t>
         </is>
       </c>
     </row>
@@ -11854,9 +12228,15 @@
       <c r="BD64" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BE64" t="inlineStr">
-        <is>
-          <t>3858</t>
+      <c r="BE64" t="n">
+        <v>3858</v>
+      </c>
+      <c r="BF64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG64" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -11930,6 +12310,8 @@
       <c r="BC65" t="inlineStr"/>
       <c r="BD65" s="3" t="inlineStr"/>
       <c r="BE65" t="inlineStr"/>
+      <c r="BF65" s="3" t="inlineStr"/>
+      <c r="BG65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -12106,9 +12488,15 @@
       <c r="BD66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE66" t="inlineStr">
-        <is>
-          <t>3037</t>
+      <c r="BE66" t="n">
+        <v>3037</v>
+      </c>
+      <c r="BF66" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BG66" t="inlineStr">
+        <is>
+          <t>3334</t>
         </is>
       </c>
     </row>
@@ -12287,9 +12675,15 @@
       <c r="BD67" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="BE67" t="inlineStr">
-        <is>
-          <t>5269</t>
+      <c r="BE67" t="n">
+        <v>5269</v>
+      </c>
+      <c r="BF67" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="BG67" t="inlineStr">
+        <is>
+          <t>5361</t>
         </is>
       </c>
     </row>
@@ -12468,9 +12862,15 @@
       <c r="BD68" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="BE68" t="inlineStr">
-        <is>
-          <t>6113</t>
+      <c r="BE68" t="n">
+        <v>6113</v>
+      </c>
+      <c r="BF68" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="BG68" t="inlineStr">
+        <is>
+          <t>6444</t>
         </is>
       </c>
     </row>
@@ -12649,9 +13049,15 @@
       <c r="BD69" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BE69" t="inlineStr">
-        <is>
-          <t>4590</t>
+      <c r="BE69" t="n">
+        <v>4590</v>
+      </c>
+      <c r="BF69" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BG69" t="inlineStr">
+        <is>
+          <t>4703</t>
         </is>
       </c>
     </row>
@@ -12830,9 +13236,15 @@
       <c r="BD70" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="BE70" t="inlineStr">
-        <is>
-          <t>4256</t>
+      <c r="BE70" t="n">
+        <v>4256</v>
+      </c>
+      <c r="BF70" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BG70" t="inlineStr">
+        <is>
+          <t>4554</t>
         </is>
       </c>
     </row>
@@ -13011,9 +13423,15 @@
       <c r="BD71" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="BE71" t="inlineStr">
-        <is>
-          <t>4902</t>
+      <c r="BE71" t="n">
+        <v>4902</v>
+      </c>
+      <c r="BF71" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BG71" t="inlineStr">
+        <is>
+          <t>5020</t>
         </is>
       </c>
     </row>
@@ -13192,9 +13610,15 @@
       <c r="BD72" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="BE72" t="inlineStr">
-        <is>
-          <t>4118</t>
+      <c r="BE72" t="n">
+        <v>4118</v>
+      </c>
+      <c r="BF72" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="BG72" t="inlineStr">
+        <is>
+          <t>4273</t>
         </is>
       </c>
     </row>
@@ -13373,9 +13797,15 @@
       <c r="BD73" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BE73" t="inlineStr">
-        <is>
-          <t>4504</t>
+      <c r="BE73" t="n">
+        <v>4504</v>
+      </c>
+      <c r="BF73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BG73" t="inlineStr">
+        <is>
+          <t>4630</t>
         </is>
       </c>
     </row>
@@ -13554,9 +13984,15 @@
       <c r="BD74" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BE74" t="inlineStr">
-        <is>
-          <t>4353</t>
+      <c r="BE74" t="n">
+        <v>4353</v>
+      </c>
+      <c r="BF74" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="BG74" t="inlineStr">
+        <is>
+          <t>4549</t>
         </is>
       </c>
     </row>
@@ -13735,9 +14171,15 @@
       <c r="BD75" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BE75" t="inlineStr">
-        <is>
-          <t>4262</t>
+      <c r="BE75" t="n">
+        <v>4262</v>
+      </c>
+      <c r="BF75" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="BG75" t="inlineStr">
+        <is>
+          <t>4421</t>
         </is>
       </c>
     </row>
@@ -13916,9 +14358,15 @@
       <c r="BD76" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="BE76" t="inlineStr">
-        <is>
-          <t>5321</t>
+      <c r="BE76" t="n">
+        <v>5321</v>
+      </c>
+      <c r="BF76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG76" t="inlineStr">
+        <is>
+          <t>5303</t>
         </is>
       </c>
     </row>
@@ -14097,7 +14545,13 @@
       <c r="BD77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE77" t="inlineStr">
+      <c r="BE77" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG77" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14278,9 +14732,15 @@
       <c r="BD78" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BE78" t="inlineStr">
-        <is>
-          <t>5253</t>
+      <c r="BE78" t="n">
+        <v>5253</v>
+      </c>
+      <c r="BF78" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BG78" t="inlineStr">
+        <is>
+          <t>5334</t>
         </is>
       </c>
     </row>
@@ -14459,7 +14919,13 @@
       <c r="BD79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE79" t="inlineStr">
+      <c r="BE79" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14640,9 +15106,15 @@
       <c r="BD80" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BE80" t="inlineStr">
-        <is>
-          <t>5115</t>
+      <c r="BE80" t="n">
+        <v>5115</v>
+      </c>
+      <c r="BF80" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BG80" t="inlineStr">
+        <is>
+          <t>5246</t>
         </is>
       </c>
     </row>
@@ -14821,9 +15293,15 @@
       <c r="BD81" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BE81" t="inlineStr">
-        <is>
-          <t>5272</t>
+      <c r="BE81" t="n">
+        <v>5272</v>
+      </c>
+      <c r="BF81" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BG81" t="inlineStr">
+        <is>
+          <t>5365</t>
         </is>
       </c>
     </row>
@@ -15002,9 +15480,15 @@
       <c r="BD82" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BE82" t="inlineStr">
-        <is>
-          <t>4983</t>
+      <c r="BE82" t="n">
+        <v>4983</v>
+      </c>
+      <c r="BF82" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="BG82" t="inlineStr">
+        <is>
+          <t>5222</t>
         </is>
       </c>
     </row>
@@ -15183,9 +15667,15 @@
       <c r="BD83" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BE83" t="inlineStr">
-        <is>
-          <t>4683</t>
+      <c r="BE83" t="n">
+        <v>4683</v>
+      </c>
+      <c r="BF83" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BG83" t="inlineStr">
+        <is>
+          <t>4803</t>
         </is>
       </c>
     </row>
@@ -15319,6 +15809,8 @@
       <c r="BC84" t="inlineStr"/>
       <c r="BD84" s="3" t="inlineStr"/>
       <c r="BE84" t="inlineStr"/>
+      <c r="BF84" s="3" t="inlineStr"/>
+      <c r="BG84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -15495,9 +15987,15 @@
       <c r="BD85" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BE85" t="inlineStr">
-        <is>
-          <t>4159</t>
+      <c r="BE85" t="n">
+        <v>4159</v>
+      </c>
+      <c r="BF85" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="BG85" t="inlineStr">
+        <is>
+          <t>4152</t>
         </is>
       </c>
     </row>
@@ -15676,9 +16174,15 @@
       <c r="BD86" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BE86" t="inlineStr">
-        <is>
-          <t>3711</t>
+      <c r="BE86" t="n">
+        <v>3711</v>
+      </c>
+      <c r="BF86" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="BG86" t="inlineStr">
+        <is>
+          <t>3905</t>
         </is>
       </c>
     </row>
@@ -15857,9 +16361,15 @@
       <c r="BD87" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BE87" t="inlineStr">
-        <is>
-          <t>4836</t>
+      <c r="BE87" t="n">
+        <v>4836</v>
+      </c>
+      <c r="BF87" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BG87" t="inlineStr">
+        <is>
+          <t>5004</t>
         </is>
       </c>
     </row>
@@ -16038,9 +16548,15 @@
       <c r="BD88" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="BE88" t="inlineStr">
-        <is>
-          <t>2921</t>
+      <c r="BE88" t="n">
+        <v>2921</v>
+      </c>
+      <c r="BF88" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BG88" t="inlineStr">
+        <is>
+          <t>3015</t>
         </is>
       </c>
     </row>
@@ -16219,9 +16735,15 @@
       <c r="BD89" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BE89" t="inlineStr">
-        <is>
-          <t>3479</t>
+      <c r="BE89" t="n">
+        <v>3479</v>
+      </c>
+      <c r="BF89" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="BG89" t="inlineStr">
+        <is>
+          <t>3494</t>
         </is>
       </c>
     </row>
@@ -16400,9 +16922,15 @@
       <c r="BD90" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BE90" t="inlineStr">
-        <is>
-          <t>3002</t>
+      <c r="BE90" t="n">
+        <v>3002</v>
+      </c>
+      <c r="BF90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG90" t="inlineStr">
+        <is>
+          <t>2988</t>
         </is>
       </c>
     </row>
@@ -16581,9 +17109,15 @@
       <c r="BD91" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BE91" t="inlineStr">
-        <is>
-          <t>2983</t>
+      <c r="BE91" t="n">
+        <v>2983</v>
+      </c>
+      <c r="BF91" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BG91" t="inlineStr">
+        <is>
+          <t>2989</t>
         </is>
       </c>
     </row>
@@ -16762,7 +17296,13 @@
       <c r="BD92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE92" t="inlineStr">
+      <c r="BE92" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16943,9 +17483,15 @@
       <c r="BD93" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="BE93" t="inlineStr">
-        <is>
-          <t>2460</t>
+      <c r="BE93" t="n">
+        <v>2460</v>
+      </c>
+      <c r="BF93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG93" t="inlineStr">
+        <is>
+          <t>2441</t>
         </is>
       </c>
     </row>
@@ -17124,9 +17670,15 @@
       <c r="BD94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE94" t="inlineStr">
-        <is>
-          <t>2799</t>
+      <c r="BE94" t="n">
+        <v>2799</v>
+      </c>
+      <c r="BF94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG94" t="inlineStr">
+        <is>
+          <t>2812</t>
         </is>
       </c>
     </row>
@@ -17305,9 +17857,15 @@
       <c r="BD95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE95" t="inlineStr">
-        <is>
-          <t>2503</t>
+      <c r="BE95" t="n">
+        <v>2503</v>
+      </c>
+      <c r="BF95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG95" t="inlineStr">
+        <is>
+          <t>2517</t>
         </is>
       </c>
     </row>
@@ -17486,9 +18044,15 @@
       <c r="BD96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE96" t="inlineStr">
-        <is>
-          <t>2467</t>
+      <c r="BE96" t="n">
+        <v>2467</v>
+      </c>
+      <c r="BF96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG96" t="inlineStr">
+        <is>
+          <t>2464</t>
         </is>
       </c>
     </row>
@@ -17667,9 +18231,15 @@
       <c r="BD97" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="BE97" t="inlineStr">
-        <is>
-          <t>3558</t>
+      <c r="BE97" t="n">
+        <v>3558</v>
+      </c>
+      <c r="BF97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG97" t="inlineStr">
+        <is>
+          <t>3557</t>
         </is>
       </c>
     </row>
@@ -17848,7 +18418,13 @@
       <c r="BD98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE98" t="inlineStr">
+      <c r="BE98" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18029,9 +18605,15 @@
       <c r="BD99" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="BE99" t="inlineStr">
-        <is>
-          <t>3836</t>
+      <c r="BE99" t="n">
+        <v>3836</v>
+      </c>
+      <c r="BF99" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BG99" t="inlineStr">
+        <is>
+          <t>4084</t>
         </is>
       </c>
     </row>
@@ -18210,9 +18792,15 @@
       <c r="BD100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE100" t="inlineStr">
-        <is>
-          <t>2485</t>
+      <c r="BE100" t="n">
+        <v>2485</v>
+      </c>
+      <c r="BF100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG100" t="inlineStr">
+        <is>
+          <t>2474</t>
         </is>
       </c>
     </row>
@@ -18391,9 +18979,15 @@
       <c r="BD101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BE101" t="inlineStr">
-        <is>
-          <t>4742</t>
+      <c r="BE101" t="n">
+        <v>4742</v>
+      </c>
+      <c r="BF101" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="BG101" t="inlineStr">
+        <is>
+          <t>4812</t>
         </is>
       </c>
     </row>
@@ -18572,9 +19166,15 @@
       <c r="BD102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BE102" t="inlineStr">
-        <is>
-          <t>4142</t>
+      <c r="BE102" t="n">
+        <v>4142</v>
+      </c>
+      <c r="BF102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BG102" t="inlineStr">
+        <is>
+          <t>4209</t>
         </is>
       </c>
     </row>
@@ -18753,9 +19353,15 @@
       <c r="BD103" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="BE103" t="inlineStr">
-        <is>
-          <t>3966</t>
+      <c r="BE103" t="n">
+        <v>3966</v>
+      </c>
+      <c r="BF103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG103" t="inlineStr">
+        <is>
+          <t>3948</t>
         </is>
       </c>
     </row>
@@ -18934,9 +19540,15 @@
       <c r="BD104" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="BE104" t="inlineStr">
-        <is>
-          <t>4703</t>
+      <c r="BE104" t="n">
+        <v>4703</v>
+      </c>
+      <c r="BF104" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="BG104" t="inlineStr">
+        <is>
+          <t>4753</t>
         </is>
       </c>
     </row>
@@ -19115,9 +19727,15 @@
       <c r="BD105" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="BE105" t="inlineStr">
-        <is>
-          <t>4320</t>
+      <c r="BE105" t="n">
+        <v>4320</v>
+      </c>
+      <c r="BF105" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="BG105" t="inlineStr">
+        <is>
+          <t>4308</t>
         </is>
       </c>
     </row>
@@ -19296,7 +19914,13 @@
       <c r="BD106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE106" t="inlineStr">
+      <c r="BE106" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -19477,7 +20101,13 @@
       <c r="BD107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE107" t="inlineStr">
+      <c r="BE107" t="n">
+        <v>2614</v>
+      </c>
+      <c r="BF107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG107" t="inlineStr">
         <is>
           <t>2614</t>
         </is>
@@ -19658,7 +20288,13 @@
       <c r="BD108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE108" t="inlineStr">
+      <c r="BE108" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -19839,9 +20475,15 @@
       <c r="BD109" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="BE109" t="inlineStr">
-        <is>
-          <t>3937</t>
+      <c r="BE109" t="n">
+        <v>3937</v>
+      </c>
+      <c r="BF109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG109" t="inlineStr">
+        <is>
+          <t>4084</t>
         </is>
       </c>
     </row>
@@ -20020,9 +20662,15 @@
       <c r="BD110" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="BE110" t="inlineStr">
-        <is>
-          <t>3886</t>
+      <c r="BE110" t="n">
+        <v>3886</v>
+      </c>
+      <c r="BF110" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="BG110" t="inlineStr">
+        <is>
+          <t>3898</t>
         </is>
       </c>
     </row>
@@ -20180,6 +20828,8 @@
       <c r="BC111" t="inlineStr"/>
       <c r="BD111" s="3" t="inlineStr"/>
       <c r="BE111" t="inlineStr"/>
+      <c r="BF111" s="3" t="inlineStr"/>
+      <c r="BG111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -20356,9 +21006,15 @@
       <c r="BD112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE112" t="inlineStr">
-        <is>
-          <t>2663</t>
+      <c r="BE112" t="n">
+        <v>2663</v>
+      </c>
+      <c r="BF112" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BG112" t="inlineStr">
+        <is>
+          <t>2969</t>
         </is>
       </c>
     </row>
@@ -20537,9 +21193,15 @@
       <c r="BD113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE113" t="inlineStr">
-        <is>
-          <t>3657</t>
+      <c r="BE113" t="n">
+        <v>3657</v>
+      </c>
+      <c r="BF113" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="BG113" t="inlineStr">
+        <is>
+          <t>3795</t>
         </is>
       </c>
     </row>
@@ -20718,9 +21380,15 @@
       <c r="BD114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE114" t="inlineStr">
-        <is>
-          <t>3779</t>
+      <c r="BE114" t="n">
+        <v>3779</v>
+      </c>
+      <c r="BF114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG114" t="inlineStr">
+        <is>
+          <t>3872</t>
         </is>
       </c>
     </row>
@@ -20899,9 +21567,15 @@
       <c r="BD115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE115" t="inlineStr">
-        <is>
-          <t>2151</t>
+      <c r="BE115" t="n">
+        <v>2151</v>
+      </c>
+      <c r="BF115" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="BG115" t="inlineStr">
+        <is>
+          <t>2359</t>
         </is>
       </c>
     </row>
@@ -21080,9 +21754,15 @@
       <c r="BD116" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="BE116" t="inlineStr">
-        <is>
-          <t>3297</t>
+      <c r="BE116" t="n">
+        <v>3297</v>
+      </c>
+      <c r="BF116" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="BG116" t="inlineStr">
+        <is>
+          <t>3400</t>
         </is>
       </c>
     </row>
@@ -21261,9 +21941,15 @@
       <c r="BD117" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BE117" t="inlineStr">
-        <is>
-          <t>4067</t>
+      <c r="BE117" t="n">
+        <v>4067</v>
+      </c>
+      <c r="BF117" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="BG117" t="inlineStr">
+        <is>
+          <t>3863</t>
         </is>
       </c>
     </row>
@@ -21442,7 +22128,13 @@
       <c r="BD118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE118" t="inlineStr">
+      <c r="BE118" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -21623,9 +22315,15 @@
       <c r="BD119" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="BE119" t="inlineStr">
-        <is>
-          <t>4355</t>
+      <c r="BE119" t="n">
+        <v>4355</v>
+      </c>
+      <c r="BF119" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="BG119" t="inlineStr">
+        <is>
+          <t>4413</t>
         </is>
       </c>
     </row>
@@ -21804,9 +22502,15 @@
       <c r="BD120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE120" t="inlineStr">
-        <is>
-          <t>2701</t>
+      <c r="BE120" t="n">
+        <v>2701</v>
+      </c>
+      <c r="BF120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG120" t="inlineStr">
+        <is>
+          <t>2685</t>
         </is>
       </c>
     </row>
@@ -21985,9 +22689,15 @@
       <c r="BD121" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="BE121" t="inlineStr">
-        <is>
-          <t>3645</t>
+      <c r="BE121" t="n">
+        <v>3645</v>
+      </c>
+      <c r="BF121" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="BG121" t="inlineStr">
+        <is>
+          <t>3854</t>
         </is>
       </c>
     </row>
@@ -22166,7 +22876,13 @@
       <c r="BD122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE122" t="inlineStr">
+      <c r="BE122" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -22347,9 +23063,15 @@
       <c r="BD123" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="BE123" t="inlineStr">
-        <is>
-          <t>3435</t>
+      <c r="BE123" t="n">
+        <v>3435</v>
+      </c>
+      <c r="BF123" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BG123" t="inlineStr">
+        <is>
+          <t>3583</t>
         </is>
       </c>
     </row>
@@ -22528,9 +23250,15 @@
       <c r="BD124" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="BE124" t="inlineStr">
-        <is>
-          <t>3452</t>
+      <c r="BE124" t="n">
+        <v>3452</v>
+      </c>
+      <c r="BF124" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="BG124" t="inlineStr">
+        <is>
+          <t>3470</t>
         </is>
       </c>
     </row>
@@ -22709,9 +23437,15 @@
       <c r="BD125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE125" t="inlineStr">
-        <is>
-          <t>3649</t>
+      <c r="BE125" t="n">
+        <v>3649</v>
+      </c>
+      <c r="BF125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG125" t="inlineStr">
+        <is>
+          <t>3728</t>
         </is>
       </c>
     </row>
@@ -22890,9 +23624,15 @@
       <c r="BD126" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BE126" t="inlineStr">
-        <is>
-          <t>3438</t>
+      <c r="BE126" t="n">
+        <v>3438</v>
+      </c>
+      <c r="BF126" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="BG126" t="inlineStr">
+        <is>
+          <t>3523</t>
         </is>
       </c>
     </row>
@@ -23071,9 +23811,15 @@
       <c r="BD127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE127" t="inlineStr">
-        <is>
-          <t>2241</t>
+      <c r="BE127" t="n">
+        <v>2241</v>
+      </c>
+      <c r="BF127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG127" t="inlineStr">
+        <is>
+          <t>2235</t>
         </is>
       </c>
     </row>
@@ -23252,7 +23998,13 @@
       <c r="BD128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE128" t="inlineStr">
+      <c r="BE128" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -23433,7 +24185,13 @@
       <c r="BD129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE129" t="inlineStr">
+      <c r="BE129" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -23614,9 +24372,15 @@
       <c r="BD130" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BE130" t="inlineStr">
-        <is>
-          <t>3024</t>
+      <c r="BE130" t="n">
+        <v>3024</v>
+      </c>
+      <c r="BF130" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="BG130" t="inlineStr">
+        <is>
+          <t>3037</t>
         </is>
       </c>
     </row>
@@ -23795,7 +24559,13 @@
       <c r="BD131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE131" t="inlineStr">
+      <c r="BE131" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -23976,9 +24746,15 @@
       <c r="BD132" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BE132" t="inlineStr">
-        <is>
-          <t>2749</t>
+      <c r="BE132" t="n">
+        <v>2749</v>
+      </c>
+      <c r="BF132" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BG132" t="inlineStr">
+        <is>
+          <t>2790</t>
         </is>
       </c>
     </row>
@@ -24157,9 +24933,15 @@
       <c r="BD133" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BE133" t="inlineStr">
-        <is>
-          <t>3039</t>
+      <c r="BE133" t="n">
+        <v>3039</v>
+      </c>
+      <c r="BF133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG133" t="inlineStr">
+        <is>
+          <t>3071</t>
         </is>
       </c>
     </row>
@@ -24257,6 +25039,8 @@
       <c r="BC134" t="inlineStr"/>
       <c r="BD134" s="3" t="inlineStr"/>
       <c r="BE134" t="inlineStr"/>
+      <c r="BF134" s="3" t="inlineStr"/>
+      <c r="BG134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -24344,6 +25128,8 @@
       <c r="BC135" t="inlineStr"/>
       <c r="BD135" s="3" t="inlineStr"/>
       <c r="BE135" t="inlineStr"/>
+      <c r="BF135" s="3" t="inlineStr"/>
+      <c r="BG135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -24520,7 +25306,13 @@
       <c r="BD136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE136" t="inlineStr">
+      <c r="BE136" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG136" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -24701,7 +25493,13 @@
       <c r="BD137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE137" t="inlineStr">
+      <c r="BE137" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -24793,6 +25591,8 @@
       <c r="BC138" t="inlineStr"/>
       <c r="BD138" s="3" t="inlineStr"/>
       <c r="BE138" t="inlineStr"/>
+      <c r="BF138" s="3" t="inlineStr"/>
+      <c r="BG138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -24969,9 +25769,15 @@
       <c r="BD139" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BE139" t="inlineStr">
-        <is>
-          <t>2901</t>
+      <c r="BE139" t="n">
+        <v>2901</v>
+      </c>
+      <c r="BF139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG139" t="inlineStr">
+        <is>
+          <t>2890</t>
         </is>
       </c>
     </row>
@@ -25150,9 +25956,15 @@
       <c r="BD140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE140" t="inlineStr">
-        <is>
-          <t>2971</t>
+      <c r="BE140" t="n">
+        <v>2971</v>
+      </c>
+      <c r="BF140" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BG140" t="inlineStr">
+        <is>
+          <t>3122</t>
         </is>
       </c>
     </row>
@@ -25242,6 +26054,8 @@
       <c r="BC141" t="inlineStr"/>
       <c r="BD141" s="3" t="inlineStr"/>
       <c r="BE141" t="inlineStr"/>
+      <c r="BF141" s="3" t="inlineStr"/>
+      <c r="BG141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -25418,7 +26232,13 @@
       <c r="BD142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE142" t="inlineStr">
+      <c r="BE142" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG142" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -25510,6 +26330,8 @@
       <c r="BC143" t="inlineStr"/>
       <c r="BD143" s="3" t="inlineStr"/>
       <c r="BE143" t="inlineStr"/>
+      <c r="BF143" s="3" t="inlineStr"/>
+      <c r="BG143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -25597,6 +26419,8 @@
       <c r="BC144" t="inlineStr"/>
       <c r="BD144" s="3" t="inlineStr"/>
       <c r="BE144" t="inlineStr"/>
+      <c r="BF144" s="3" t="inlineStr"/>
+      <c r="BG144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -25684,6 +26508,8 @@
       <c r="BC145" t="inlineStr"/>
       <c r="BD145" s="3" t="inlineStr"/>
       <c r="BE145" t="inlineStr"/>
+      <c r="BF145" s="3" t="inlineStr"/>
+      <c r="BG145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -25771,6 +26597,8 @@
       <c r="BC146" t="inlineStr"/>
       <c r="BD146" s="3" t="inlineStr"/>
       <c r="BE146" t="inlineStr"/>
+      <c r="BF146" s="3" t="inlineStr"/>
+      <c r="BG146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -25858,6 +26686,8 @@
       <c r="BC147" t="inlineStr"/>
       <c r="BD147" s="3" t="inlineStr"/>
       <c r="BE147" t="inlineStr"/>
+      <c r="BF147" s="3" t="inlineStr"/>
+      <c r="BG147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -26034,7 +26864,13 @@
       <c r="BD148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE148" t="inlineStr">
+      <c r="BE148" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -26215,9 +27051,15 @@
       <c r="BD149" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="BE149" t="inlineStr">
-        <is>
-          <t>3835</t>
+      <c r="BE149" t="n">
+        <v>3835</v>
+      </c>
+      <c r="BF149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG149" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -26396,7 +27238,13 @@
       <c r="BD150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE150" t="inlineStr">
+      <c r="BE150" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -26577,9 +27425,15 @@
       <c r="BD151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE151" t="inlineStr">
-        <is>
-          <t>2622</t>
+      <c r="BE151" t="n">
+        <v>2622</v>
+      </c>
+      <c r="BF151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG151" t="inlineStr">
+        <is>
+          <t>2654</t>
         </is>
       </c>
     </row>
@@ -26758,7 +27612,13 @@
       <c r="BD152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE152" t="inlineStr">
+      <c r="BE152" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -26939,9 +27799,15 @@
       <c r="BD153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE153" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="BE153" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG153" t="inlineStr">
+        <is>
+          <t>2558</t>
         </is>
       </c>
     </row>
@@ -27120,7 +27986,13 @@
       <c r="BD154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE154" t="inlineStr">
+      <c r="BE154" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -27301,9 +28173,15 @@
       <c r="BD155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE155" t="inlineStr">
-        <is>
-          <t>2753</t>
+      <c r="BE155" t="n">
+        <v>2753</v>
+      </c>
+      <c r="BF155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG155" t="inlineStr">
+        <is>
+          <t>2748</t>
         </is>
       </c>
     </row>
@@ -27476,9 +28354,15 @@
       <c r="BD156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE156" t="inlineStr">
-        <is>
-          <t>3205</t>
+      <c r="BE156" t="n">
+        <v>3205</v>
+      </c>
+      <c r="BF156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG156" t="inlineStr">
+        <is>
+          <t>3211</t>
         </is>
       </c>
     </row>
@@ -27562,6 +28446,8 @@
       <c r="BC157" t="inlineStr"/>
       <c r="BD157" s="3" t="inlineStr"/>
       <c r="BE157" t="inlineStr"/>
+      <c r="BF157" s="3" t="inlineStr"/>
+      <c r="BG157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -27732,7 +28618,13 @@
       <c r="BD158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE158" t="inlineStr">
+      <c r="BE158" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -27907,9 +28799,15 @@
       <c r="BD159" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BE159" t="inlineStr">
-        <is>
-          <t>3192</t>
+      <c r="BE159" t="n">
+        <v>3192</v>
+      </c>
+      <c r="BF159" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="BG159" t="inlineStr">
+        <is>
+          <t>3410</t>
         </is>
       </c>
     </row>
@@ -27993,6 +28891,8 @@
       <c r="BC160" t="inlineStr"/>
       <c r="BD160" s="3" t="inlineStr"/>
       <c r="BE160" t="inlineStr"/>
+      <c r="BF160" s="3" t="inlineStr"/>
+      <c r="BG160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -28151,9 +29051,15 @@
       <c r="BD161" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="BE161" t="inlineStr">
-        <is>
-          <t>3429</t>
+      <c r="BE161" t="n">
+        <v>3429</v>
+      </c>
+      <c r="BF161" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BG161" t="inlineStr">
+        <is>
+          <t>3509</t>
         </is>
       </c>
     </row>
@@ -28314,9 +29220,15 @@
       <c r="BD162" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="BE162" t="inlineStr">
-        <is>
-          <t>3013</t>
+      <c r="BE162" t="n">
+        <v>3013</v>
+      </c>
+      <c r="BF162" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="BG162" t="inlineStr">
+        <is>
+          <t>3054</t>
         </is>
       </c>
     </row>
@@ -28473,9 +29385,15 @@
       <c r="BD163" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE163" t="inlineStr">
-        <is>
-          <t>3385</t>
+      <c r="BE163" t="n">
+        <v>3385</v>
+      </c>
+      <c r="BF163" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG163" t="inlineStr">
+        <is>
+          <t>3376</t>
         </is>
       </c>
     </row>
@@ -28616,9 +29534,15 @@
       <c r="BD164" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE164" t="inlineStr">
-        <is>
-          <t>3587</t>
+      <c r="BE164" t="n">
+        <v>3587</v>
+      </c>
+      <c r="BF164" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BG164" t="inlineStr">
+        <is>
+          <t>3715</t>
         </is>
       </c>
     </row>
@@ -28763,9 +29687,15 @@
       <c r="BD165" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="BE165" t="inlineStr">
-        <is>
-          <t>2918</t>
+      <c r="BE165" t="n">
+        <v>2918</v>
+      </c>
+      <c r="BF165" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="BG165" t="inlineStr">
+        <is>
+          <t>2879</t>
         </is>
       </c>
     </row>
@@ -28902,9 +29832,15 @@
       <c r="BD166" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE166" t="inlineStr">
-        <is>
-          <t>2800</t>
+      <c r="BE166" t="n">
+        <v>2800</v>
+      </c>
+      <c r="BF166" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG166" t="inlineStr">
+        <is>
+          <t>2791</t>
         </is>
       </c>
     </row>
@@ -29029,7 +29965,13 @@
       <c r="BD167" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE167" t="inlineStr">
+      <c r="BE167" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF167" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG167" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -29152,7 +30094,13 @@
       <c r="BD168" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE168" t="inlineStr">
+      <c r="BE168" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF168" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG168" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -29230,6 +30178,8 @@
       <c r="BC169" t="inlineStr"/>
       <c r="BD169" s="3" t="inlineStr"/>
       <c r="BE169" t="inlineStr"/>
+      <c r="BF169" s="3" t="inlineStr"/>
+      <c r="BG169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="n">
@@ -29344,7 +30294,13 @@
       <c r="BD170" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE170" t="inlineStr">
+      <c r="BE170" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF170" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG170" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -29451,9 +30407,15 @@
       <c r="BD171" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE171" t="inlineStr">
-        <is>
-          <t>1781</t>
+      <c r="BE171" t="n">
+        <v>1781</v>
+      </c>
+      <c r="BF171" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BG171" t="inlineStr">
+        <is>
+          <t>1938</t>
         </is>
       </c>
     </row>
@@ -29558,7 +30520,13 @@
       <c r="BD172" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE172" t="inlineStr">
+      <c r="BE172" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF172" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG172" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -29665,9 +30633,15 @@
       <c r="BD173" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BE173" t="inlineStr">
-        <is>
-          <t>1848</t>
+      <c r="BE173" t="n">
+        <v>1848</v>
+      </c>
+      <c r="BF173" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG173" t="inlineStr">
+        <is>
+          <t>1852</t>
         </is>
       </c>
     </row>
@@ -29748,9 +30722,94 @@
       <c r="BD174" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="BE174" t="inlineStr">
-        <is>
-          <t>3352</t>
+      <c r="BE174" t="n">
+        <v>3352</v>
+      </c>
+      <c r="BF174" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="BG174" t="inlineStr">
+        <is>
+          <t>3449</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>58945536</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Ñîmrā</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr"/>
+      <c r="D175" t="inlineStr"/>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F175" s="3" t="inlineStr"/>
+      <c r="G175" t="inlineStr"/>
+      <c r="H175" s="3" t="inlineStr"/>
+      <c r="I175" t="inlineStr"/>
+      <c r="J175" s="3" t="inlineStr"/>
+      <c r="K175" t="inlineStr"/>
+      <c r="L175" s="3" t="inlineStr"/>
+      <c r="M175" t="inlineStr"/>
+      <c r="N175" s="3" t="inlineStr"/>
+      <c r="O175" t="inlineStr"/>
+      <c r="P175" s="3" t="inlineStr"/>
+      <c r="Q175" t="inlineStr"/>
+      <c r="R175" s="3" t="inlineStr"/>
+      <c r="S175" t="inlineStr"/>
+      <c r="T175" s="3" t="inlineStr"/>
+      <c r="U175" t="inlineStr"/>
+      <c r="V175" s="3" t="inlineStr"/>
+      <c r="W175" t="inlineStr"/>
+      <c r="X175" s="3" t="inlineStr"/>
+      <c r="Y175" t="inlineStr"/>
+      <c r="Z175" s="3" t="inlineStr"/>
+      <c r="AA175" t="inlineStr"/>
+      <c r="AB175" s="3" t="inlineStr"/>
+      <c r="AC175" t="inlineStr"/>
+      <c r="AD175" s="3" t="inlineStr"/>
+      <c r="AE175" t="inlineStr"/>
+      <c r="AF175" s="3" t="inlineStr"/>
+      <c r="AG175" t="inlineStr"/>
+      <c r="AH175" s="3" t="inlineStr"/>
+      <c r="AI175" t="inlineStr"/>
+      <c r="AJ175" s="3" t="inlineStr"/>
+      <c r="AK175" t="inlineStr"/>
+      <c r="AL175" s="3" t="inlineStr"/>
+      <c r="AM175" t="inlineStr"/>
+      <c r="AN175" s="3" t="inlineStr"/>
+      <c r="AO175" t="inlineStr"/>
+      <c r="AP175" s="3" t="inlineStr"/>
+      <c r="AQ175" t="inlineStr"/>
+      <c r="AR175" s="3" t="inlineStr"/>
+      <c r="AS175" t="inlineStr"/>
+      <c r="AT175" s="3" t="inlineStr"/>
+      <c r="AU175" t="inlineStr"/>
+      <c r="AV175" s="3" t="inlineStr"/>
+      <c r="AW175" t="inlineStr"/>
+      <c r="AX175" s="3" t="inlineStr"/>
+      <c r="AY175" t="inlineStr"/>
+      <c r="AZ175" s="3" t="inlineStr"/>
+      <c r="BA175" t="inlineStr"/>
+      <c r="BB175" s="3" t="inlineStr"/>
+      <c r="BC175" t="inlineStr"/>
+      <c r="BD175" s="3" t="inlineStr"/>
+      <c r="BE175" t="inlineStr"/>
+      <c r="BF175" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="BG175" t="inlineStr">
+        <is>
+          <t>3334</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-03-13 11:30:48
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BG175"/>
+  <dimension ref="A1:BI178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -686,6 +686,16 @@
           <t>03-11_0</t>
         </is>
       </c>
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
+          <t>03-12_A</t>
+        </is>
+      </c>
+      <c r="BI1" s="1" t="inlineStr">
+        <is>
+          <t>03-12_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -868,9 +878,15 @@
       <c r="BF2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG2" t="inlineStr">
-        <is>
-          <t>2981</t>
+      <c r="BG2" t="n">
+        <v>2981</v>
+      </c>
+      <c r="BH2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI2" t="inlineStr">
+        <is>
+          <t>2518</t>
         </is>
       </c>
     </row>
@@ -1055,9 +1071,15 @@
       <c r="BF3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BG3" t="inlineStr">
-        <is>
-          <t>6803</t>
+      <c r="BG3" t="n">
+        <v>6803</v>
+      </c>
+      <c r="BH3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BI3" t="inlineStr">
+        <is>
+          <t>2944</t>
         </is>
       </c>
     </row>
@@ -1242,9 +1264,15 @@
       <c r="BF4" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="BG4" t="inlineStr">
-        <is>
-          <t>6458</t>
+      <c r="BG4" t="n">
+        <v>6458</v>
+      </c>
+      <c r="BH4" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="BI4" t="inlineStr">
+        <is>
+          <t>3014</t>
         </is>
       </c>
     </row>
@@ -1429,9 +1457,15 @@
       <c r="BF5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BG5" t="inlineStr">
-        <is>
-          <t>6410</t>
+      <c r="BG5" t="n">
+        <v>6410</v>
+      </c>
+      <c r="BH5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BI5" t="inlineStr">
+        <is>
+          <t>2869</t>
         </is>
       </c>
     </row>
@@ -1616,9 +1650,15 @@
       <c r="BF6" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BG6" t="inlineStr">
-        <is>
-          <t>6269</t>
+      <c r="BG6" t="n">
+        <v>6269</v>
+      </c>
+      <c r="BH6" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BI6" t="inlineStr">
+        <is>
+          <t>2844</t>
         </is>
       </c>
     </row>
@@ -1803,9 +1843,15 @@
       <c r="BF7" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="BG7" t="inlineStr">
-        <is>
-          <t>6891</t>
+      <c r="BG7" t="n">
+        <v>6891</v>
+      </c>
+      <c r="BH7" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="BI7" t="inlineStr">
+        <is>
+          <t>2963</t>
         </is>
       </c>
     </row>
@@ -1990,9 +2036,15 @@
       <c r="BF8" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="BG8" t="inlineStr">
-        <is>
-          <t>5809</t>
+      <c r="BG8" t="n">
+        <v>5809</v>
+      </c>
+      <c r="BH8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BI8" t="inlineStr">
+        <is>
+          <t>2816</t>
         </is>
       </c>
     </row>
@@ -2177,9 +2229,15 @@
       <c r="BF9" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BG9" t="inlineStr">
-        <is>
-          <t>6118</t>
+      <c r="BG9" t="n">
+        <v>6118</v>
+      </c>
+      <c r="BH9" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BI9" t="inlineStr">
+        <is>
+          <t>3120</t>
         </is>
       </c>
     </row>
@@ -2364,9 +2422,15 @@
       <c r="BF10" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BG10" t="inlineStr">
-        <is>
-          <t>7354</t>
+      <c r="BG10" t="n">
+        <v>7354</v>
+      </c>
+      <c r="BH10" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BI10" t="inlineStr">
+        <is>
+          <t>2939</t>
         </is>
       </c>
     </row>
@@ -2551,9 +2615,15 @@
       <c r="BF11" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="BG11" t="inlineStr">
-        <is>
-          <t>4994</t>
+      <c r="BG11" t="n">
+        <v>4994</v>
+      </c>
+      <c r="BH11" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BI11" t="inlineStr">
+        <is>
+          <t>2807</t>
         </is>
       </c>
     </row>
@@ -2738,9 +2808,15 @@
       <c r="BF12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG12" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="BG12" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH12" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="BI12" t="inlineStr">
+        <is>
+          <t>2604</t>
         </is>
       </c>
     </row>
@@ -2925,9 +3001,15 @@
       <c r="BF13" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="BG13" t="inlineStr">
-        <is>
-          <t>7102</t>
+      <c r="BG13" t="n">
+        <v>7102</v>
+      </c>
+      <c r="BH13" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="BI13" t="inlineStr">
+        <is>
+          <t>3168</t>
         </is>
       </c>
     </row>
@@ -3112,9 +3194,15 @@
       <c r="BF14" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BG14" t="inlineStr">
-        <is>
-          <t>6052</t>
+      <c r="BG14" t="n">
+        <v>6052</v>
+      </c>
+      <c r="BH14" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BI14" t="inlineStr">
+        <is>
+          <t>2863</t>
         </is>
       </c>
     </row>
@@ -3299,7 +3387,13 @@
       <c r="BF15" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG15" t="inlineStr">
+      <c r="BG15" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI15" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3486,9 +3580,15 @@
       <c r="BF16" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BG16" t="inlineStr">
-        <is>
-          <t>6558</t>
+      <c r="BG16" t="n">
+        <v>6558</v>
+      </c>
+      <c r="BH16" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="BI16" t="inlineStr">
+        <is>
+          <t>2967</t>
         </is>
       </c>
     </row>
@@ -3673,9 +3773,15 @@
       <c r="BF17" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BG17" t="inlineStr">
-        <is>
-          <t>4525</t>
+      <c r="BG17" t="n">
+        <v>4525</v>
+      </c>
+      <c r="BH17" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BI17" t="inlineStr">
+        <is>
+          <t>2925</t>
         </is>
       </c>
     </row>
@@ -3860,9 +3966,15 @@
       <c r="BF18" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BG18" t="inlineStr">
-        <is>
-          <t>5346</t>
+      <c r="BG18" t="n">
+        <v>5346</v>
+      </c>
+      <c r="BH18" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="BI18" t="inlineStr">
+        <is>
+          <t>2864</t>
         </is>
       </c>
     </row>
@@ -4047,9 +4159,15 @@
       <c r="BF19" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BG19" t="inlineStr">
-        <is>
-          <t>6549</t>
+      <c r="BG19" t="n">
+        <v>6549</v>
+      </c>
+      <c r="BH19" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BI19" t="inlineStr">
+        <is>
+          <t>2808</t>
         </is>
       </c>
     </row>
@@ -4234,9 +4352,15 @@
       <c r="BF20" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="BG20" t="inlineStr">
-        <is>
-          <t>7464</t>
+      <c r="BG20" t="n">
+        <v>7464</v>
+      </c>
+      <c r="BH20" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BI20" t="inlineStr">
+        <is>
+          <t>3003</t>
         </is>
       </c>
     </row>
@@ -4421,9 +4545,15 @@
       <c r="BF21" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="BG21" t="inlineStr">
-        <is>
-          <t>5550</t>
+      <c r="BG21" t="n">
+        <v>5550</v>
+      </c>
+      <c r="BH21" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BI21" t="inlineStr">
+        <is>
+          <t>2816</t>
         </is>
       </c>
     </row>
@@ -4608,9 +4738,15 @@
       <c r="BF22" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BG22" t="inlineStr">
-        <is>
-          <t>6297</t>
+      <c r="BG22" t="n">
+        <v>6297</v>
+      </c>
+      <c r="BH22" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BI22" t="inlineStr">
+        <is>
+          <t>3039</t>
         </is>
       </c>
     </row>
@@ -4795,9 +4931,15 @@
       <c r="BF23" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG23" t="inlineStr">
-        <is>
-          <t>5208</t>
+      <c r="BG23" t="n">
+        <v>5208</v>
+      </c>
+      <c r="BH23" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="BI23" t="inlineStr">
+        <is>
+          <t>2903</t>
         </is>
       </c>
     </row>
@@ -4982,9 +5124,15 @@
       <c r="BF24" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BG24" t="inlineStr">
-        <is>
-          <t>6532</t>
+      <c r="BG24" t="n">
+        <v>6532</v>
+      </c>
+      <c r="BH24" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BI24" t="inlineStr">
+        <is>
+          <t>3066</t>
         </is>
       </c>
     </row>
@@ -5169,7 +5317,13 @@
       <c r="BF25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG25" t="inlineStr">
+      <c r="BG25" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5194,7 +5348,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F26" s="5" t="n">
@@ -5356,9 +5510,15 @@
       <c r="BF26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG26" t="inlineStr">
-        <is>
-          <t>6210</t>
+      <c r="BG26" t="n">
+        <v>6210</v>
+      </c>
+      <c r="BH26" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="BI26" t="inlineStr">
+        <is>
+          <t>2517</t>
         </is>
       </c>
     </row>
@@ -5543,9 +5703,15 @@
       <c r="BF27" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BG27" t="inlineStr">
-        <is>
-          <t>6592</t>
+      <c r="BG27" t="n">
+        <v>6592</v>
+      </c>
+      <c r="BH27" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BI27" t="inlineStr">
+        <is>
+          <t>3035</t>
         </is>
       </c>
     </row>
@@ -5730,9 +5896,15 @@
       <c r="BF28" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BG28" t="inlineStr">
-        <is>
-          <t>6148</t>
+      <c r="BG28" t="n">
+        <v>6148</v>
+      </c>
+      <c r="BH28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="BI28" t="inlineStr">
+        <is>
+          <t>3008</t>
         </is>
       </c>
     </row>
@@ -5917,9 +6089,15 @@
       <c r="BF29" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BG29" t="inlineStr">
-        <is>
-          <t>7139</t>
+      <c r="BG29" t="n">
+        <v>7139</v>
+      </c>
+      <c r="BH29" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BI29" t="inlineStr">
+        <is>
+          <t>3243</t>
         </is>
       </c>
     </row>
@@ -6104,9 +6282,15 @@
       <c r="BF30" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="BG30" t="inlineStr">
-        <is>
-          <t>6063</t>
+      <c r="BG30" t="n">
+        <v>6063</v>
+      </c>
+      <c r="BH30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI30" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -6291,9 +6475,15 @@
       <c r="BF31" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="BG31" t="inlineStr">
-        <is>
-          <t>6939</t>
+      <c r="BG31" t="n">
+        <v>6939</v>
+      </c>
+      <c r="BH31" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BI31" t="inlineStr">
+        <is>
+          <t>3118</t>
         </is>
       </c>
     </row>
@@ -6478,9 +6668,15 @@
       <c r="BF32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG32" t="inlineStr">
-        <is>
-          <t>6262</t>
+      <c r="BG32" t="n">
+        <v>6262</v>
+      </c>
+      <c r="BH32" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="BI32" t="inlineStr">
+        <is>
+          <t>2959</t>
         </is>
       </c>
     </row>
@@ -6665,9 +6861,15 @@
       <c r="BF33" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BG33" t="inlineStr">
-        <is>
-          <t>6025</t>
+      <c r="BG33" t="n">
+        <v>6025</v>
+      </c>
+      <c r="BH33" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BI33" t="inlineStr">
+        <is>
+          <t>2834</t>
         </is>
       </c>
     </row>
@@ -6852,9 +7054,15 @@
       <c r="BF34" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BG34" t="inlineStr">
-        <is>
-          <t>5981</t>
+      <c r="BG34" t="n">
+        <v>5981</v>
+      </c>
+      <c r="BH34" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BI34" t="inlineStr">
+        <is>
+          <t>3022</t>
         </is>
       </c>
     </row>
@@ -6877,7 +7085,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F35" s="5" t="n">
@@ -7039,9 +7247,15 @@
       <c r="BF35" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="BG35" t="inlineStr">
-        <is>
-          <t>6548</t>
+      <c r="BG35" t="n">
+        <v>6548</v>
+      </c>
+      <c r="BH35" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BI35" t="inlineStr">
+        <is>
+          <t>2994</t>
         </is>
       </c>
     </row>
@@ -7226,9 +7440,15 @@
       <c r="BF36" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="BG36" t="inlineStr">
-        <is>
-          <t>6074</t>
+      <c r="BG36" t="n">
+        <v>6074</v>
+      </c>
+      <c r="BH36" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BI36" t="inlineStr">
+        <is>
+          <t>2881</t>
         </is>
       </c>
     </row>
@@ -7413,9 +7633,15 @@
       <c r="BF37" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="BG37" t="inlineStr">
-        <is>
-          <t>4600</t>
+      <c r="BG37" t="n">
+        <v>4600</v>
+      </c>
+      <c r="BH37" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BI37" t="inlineStr">
+        <is>
+          <t>2975</t>
         </is>
       </c>
     </row>
@@ -7600,9 +7826,15 @@
       <c r="BF38" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="BG38" t="inlineStr">
-        <is>
-          <t>6105</t>
+      <c r="BG38" t="n">
+        <v>6105</v>
+      </c>
+      <c r="BH38" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BI38" t="inlineStr">
+        <is>
+          <t>2930</t>
         </is>
       </c>
     </row>
@@ -7787,9 +8019,15 @@
       <c r="BF39" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BG39" t="inlineStr">
-        <is>
-          <t>6227</t>
+      <c r="BG39" t="n">
+        <v>6227</v>
+      </c>
+      <c r="BH39" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="BI39" t="inlineStr">
+        <is>
+          <t>3037</t>
         </is>
       </c>
     </row>
@@ -7974,9 +8212,15 @@
       <c r="BF40" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BG40" t="inlineStr">
-        <is>
-          <t>7115</t>
+      <c r="BG40" t="n">
+        <v>7115</v>
+      </c>
+      <c r="BH40" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BI40" t="inlineStr">
+        <is>
+          <t>2903</t>
         </is>
       </c>
     </row>
@@ -8161,7 +8405,13 @@
       <c r="BF41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG41" t="inlineStr">
+      <c r="BG41" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI41" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8348,9 +8598,15 @@
       <c r="BF42" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="BG42" t="inlineStr">
-        <is>
-          <t>7141</t>
+      <c r="BG42" t="n">
+        <v>7141</v>
+      </c>
+      <c r="BH42" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="BI42" t="inlineStr">
+        <is>
+          <t>2998</t>
         </is>
       </c>
     </row>
@@ -8535,9 +8791,15 @@
       <c r="BF43" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BG43" t="inlineStr">
-        <is>
-          <t>6368</t>
+      <c r="BG43" t="n">
+        <v>6368</v>
+      </c>
+      <c r="BH43" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BI43" t="inlineStr">
+        <is>
+          <t>3060</t>
         </is>
       </c>
     </row>
@@ -8722,9 +8984,15 @@
       <c r="BF44" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="BG44" t="inlineStr">
-        <is>
-          <t>6271</t>
+      <c r="BG44" t="n">
+        <v>6271</v>
+      </c>
+      <c r="BH44" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BI44" t="inlineStr">
+        <is>
+          <t>3166</t>
         </is>
       </c>
     </row>
@@ -8909,9 +9177,15 @@
       <c r="BF45" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BG45" t="inlineStr">
-        <is>
-          <t>6079</t>
+      <c r="BG45" t="n">
+        <v>6079</v>
+      </c>
+      <c r="BH45" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="BI45" t="inlineStr">
+        <is>
+          <t>2876</t>
         </is>
       </c>
     </row>
@@ -9096,9 +9370,15 @@
       <c r="BF46" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="BG46" t="inlineStr">
-        <is>
-          <t>5949</t>
+      <c r="BG46" t="n">
+        <v>5949</v>
+      </c>
+      <c r="BH46" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BI46" t="inlineStr">
+        <is>
+          <t>2847</t>
         </is>
       </c>
     </row>
@@ -9283,9 +9563,15 @@
       <c r="BF47" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG47" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="BG47" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH47" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="BI47" t="inlineStr">
+        <is>
+          <t>2837</t>
         </is>
       </c>
     </row>
@@ -9470,9 +9756,15 @@
       <c r="BF48" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="BG48" t="inlineStr">
-        <is>
-          <t>6613</t>
+      <c r="BG48" t="n">
+        <v>6613</v>
+      </c>
+      <c r="BH48" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="BI48" t="inlineStr">
+        <is>
+          <t>3139</t>
         </is>
       </c>
     </row>
@@ -9657,9 +9949,15 @@
       <c r="BF49" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="BG49" t="inlineStr">
-        <is>
-          <t>5260</t>
+      <c r="BG49" t="n">
+        <v>5260</v>
+      </c>
+      <c r="BH49" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BI49" t="inlineStr">
+        <is>
+          <t>2750</t>
         </is>
       </c>
     </row>
@@ -9844,9 +10142,15 @@
       <c r="BF50" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="BG50" t="inlineStr">
-        <is>
-          <t>6552</t>
+      <c r="BG50" t="n">
+        <v>6552</v>
+      </c>
+      <c r="BH50" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI50" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -10031,9 +10335,15 @@
       <c r="BF51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG51" t="inlineStr">
-        <is>
-          <t>2686</t>
+      <c r="BG51" t="n">
+        <v>2686</v>
+      </c>
+      <c r="BH51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI51" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -10218,9 +10528,15 @@
       <c r="BF52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG52" t="inlineStr">
-        <is>
-          <t>2938</t>
+      <c r="BG52" t="n">
+        <v>2938</v>
+      </c>
+      <c r="BH52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI52" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -10405,9 +10721,15 @@
       <c r="BF53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG53" t="inlineStr">
-        <is>
-          <t>3722</t>
+      <c r="BG53" t="n">
+        <v>3722</v>
+      </c>
+      <c r="BH53" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="BI53" t="inlineStr">
+        <is>
+          <t>2698</t>
         </is>
       </c>
     </row>
@@ -10592,9 +10914,15 @@
       <c r="BF54" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="BG54" t="inlineStr">
-        <is>
-          <t>6139</t>
+      <c r="BG54" t="n">
+        <v>6139</v>
+      </c>
+      <c r="BH54" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="BI54" t="inlineStr">
+        <is>
+          <t>2945</t>
         </is>
       </c>
     </row>
@@ -10779,9 +11107,15 @@
       <c r="BF55" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BG55" t="inlineStr">
-        <is>
-          <t>4540</t>
+      <c r="BG55" t="n">
+        <v>4540</v>
+      </c>
+      <c r="BH55" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BI55" t="inlineStr">
+        <is>
+          <t>2954</t>
         </is>
       </c>
     </row>
@@ -10966,9 +11300,15 @@
       <c r="BF56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BG56" t="inlineStr">
-        <is>
-          <t>4444</t>
+      <c r="BG56" t="n">
+        <v>4444</v>
+      </c>
+      <c r="BH56" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="BI56" t="inlineStr">
+        <is>
+          <t>2793</t>
         </is>
       </c>
     </row>
@@ -11153,9 +11493,15 @@
       <c r="BF57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BG57" t="inlineStr">
-        <is>
-          <t>5724</t>
+      <c r="BG57" t="n">
+        <v>5724</v>
+      </c>
+      <c r="BH57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BI57" t="inlineStr">
+        <is>
+          <t>2854</t>
         </is>
       </c>
     </row>
@@ -11340,9 +11686,15 @@
       <c r="BF58" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG58" t="inlineStr">
-        <is>
-          <t>4769</t>
+      <c r="BG58" t="n">
+        <v>4769</v>
+      </c>
+      <c r="BH58" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="BI58" t="inlineStr">
+        <is>
+          <t>2966</t>
         </is>
       </c>
     </row>
@@ -11418,6 +11770,8 @@
       <c r="BE59" t="inlineStr"/>
       <c r="BF59" s="3" t="inlineStr"/>
       <c r="BG59" t="inlineStr"/>
+      <c r="BH59" s="3" t="inlineStr"/>
+      <c r="BI59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -11491,6 +11845,8 @@
       <c r="BE60" t="inlineStr"/>
       <c r="BF60" s="3" t="inlineStr"/>
       <c r="BG60" t="inlineStr"/>
+      <c r="BH60" s="3" t="inlineStr"/>
+      <c r="BI60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -11673,9 +12029,15 @@
       <c r="BF61" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="BG61" t="inlineStr">
-        <is>
-          <t>5391</t>
+      <c r="BG61" t="n">
+        <v>5391</v>
+      </c>
+      <c r="BH61" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BI61" t="inlineStr">
+        <is>
+          <t>2926</t>
         </is>
       </c>
     </row>
@@ -11860,7 +12222,13 @@
       <c r="BF62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG62" t="inlineStr">
+      <c r="BG62" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12047,9 +12415,15 @@
       <c r="BF63" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="BG63" t="inlineStr">
-        <is>
-          <t>5784</t>
+      <c r="BG63" t="n">
+        <v>5784</v>
+      </c>
+      <c r="BH63" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BI63" t="inlineStr">
+        <is>
+          <t>2896</t>
         </is>
       </c>
     </row>
@@ -12234,9 +12608,15 @@
       <c r="BF64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG64" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="BG64" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI64" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -12312,6 +12692,8 @@
       <c r="BE65" t="inlineStr"/>
       <c r="BF65" s="3" t="inlineStr"/>
       <c r="BG65" t="inlineStr"/>
+      <c r="BH65" s="3" t="inlineStr"/>
+      <c r="BI65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -12494,9 +12876,15 @@
       <c r="BF66" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BG66" t="inlineStr">
-        <is>
-          <t>3334</t>
+      <c r="BG66" t="n">
+        <v>3334</v>
+      </c>
+      <c r="BH66" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="BI66" t="inlineStr">
+        <is>
+          <t>2600</t>
         </is>
       </c>
     </row>
@@ -12681,9 +13069,15 @@
       <c r="BF67" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="BG67" t="inlineStr">
-        <is>
-          <t>5361</t>
+      <c r="BG67" t="n">
+        <v>5361</v>
+      </c>
+      <c r="BH67" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BI67" t="inlineStr">
+        <is>
+          <t>2836</t>
         </is>
       </c>
     </row>
@@ -12868,9 +13262,15 @@
       <c r="BF68" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="BG68" t="inlineStr">
-        <is>
-          <t>6444</t>
+      <c r="BG68" t="n">
+        <v>6444</v>
+      </c>
+      <c r="BH68" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BI68" t="inlineStr">
+        <is>
+          <t>2958</t>
         </is>
       </c>
     </row>
@@ -13055,9 +13455,15 @@
       <c r="BF69" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BG69" t="inlineStr">
-        <is>
-          <t>4703</t>
+      <c r="BG69" t="n">
+        <v>4703</v>
+      </c>
+      <c r="BH69" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="BI69" t="inlineStr">
+        <is>
+          <t>3000</t>
         </is>
       </c>
     </row>
@@ -13242,9 +13648,15 @@
       <c r="BF70" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BG70" t="inlineStr">
-        <is>
-          <t>4554</t>
+      <c r="BG70" t="n">
+        <v>4554</v>
+      </c>
+      <c r="BH70" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="BI70" t="inlineStr">
+        <is>
+          <t>2539</t>
         </is>
       </c>
     </row>
@@ -13429,9 +13841,15 @@
       <c r="BF71" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BG71" t="inlineStr">
-        <is>
-          <t>5020</t>
+      <c r="BG71" t="n">
+        <v>5020</v>
+      </c>
+      <c r="BH71" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BI71" t="inlineStr">
+        <is>
+          <t>2857</t>
         </is>
       </c>
     </row>
@@ -13616,9 +14034,15 @@
       <c r="BF72" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="BG72" t="inlineStr">
-        <is>
-          <t>4273</t>
+      <c r="BG72" t="n">
+        <v>4273</v>
+      </c>
+      <c r="BH72" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BI72" t="inlineStr">
+        <is>
+          <t>2931</t>
         </is>
       </c>
     </row>
@@ -13803,9 +14227,15 @@
       <c r="BF73" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BG73" t="inlineStr">
-        <is>
-          <t>4630</t>
+      <c r="BG73" t="n">
+        <v>4630</v>
+      </c>
+      <c r="BH73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BI73" t="inlineStr">
+        <is>
+          <t>2796</t>
         </is>
       </c>
     </row>
@@ -13990,9 +14420,15 @@
       <c r="BF74" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="BG74" t="inlineStr">
-        <is>
-          <t>4549</t>
+      <c r="BG74" t="n">
+        <v>4549</v>
+      </c>
+      <c r="BH74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI74" t="inlineStr">
+        <is>
+          <t>2514</t>
         </is>
       </c>
     </row>
@@ -14177,9 +14613,15 @@
       <c r="BF75" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="BG75" t="inlineStr">
-        <is>
-          <t>4421</t>
+      <c r="BG75" t="n">
+        <v>4421</v>
+      </c>
+      <c r="BH75" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BI75" t="inlineStr">
+        <is>
+          <t>2864</t>
         </is>
       </c>
     </row>
@@ -14364,9 +14806,15 @@
       <c r="BF76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG76" t="inlineStr">
-        <is>
-          <t>5303</t>
+      <c r="BG76" t="n">
+        <v>5303</v>
+      </c>
+      <c r="BH76" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BI76" t="inlineStr">
+        <is>
+          <t>2896</t>
         </is>
       </c>
     </row>
@@ -14551,7 +14999,13 @@
       <c r="BF77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG77" t="inlineStr">
+      <c r="BG77" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI77" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14738,9 +15192,15 @@
       <c r="BF78" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BG78" t="inlineStr">
-        <is>
-          <t>5334</t>
+      <c r="BG78" t="n">
+        <v>5334</v>
+      </c>
+      <c r="BH78" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BI78" t="inlineStr">
+        <is>
+          <t>3133</t>
         </is>
       </c>
     </row>
@@ -14925,7 +15385,13 @@
       <c r="BF79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG79" t="inlineStr">
+      <c r="BG79" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15112,9 +15578,15 @@
       <c r="BF80" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BG80" t="inlineStr">
-        <is>
-          <t>5246</t>
+      <c r="BG80" t="n">
+        <v>5246</v>
+      </c>
+      <c r="BH80" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="BI80" t="inlineStr">
+        <is>
+          <t>2946</t>
         </is>
       </c>
     </row>
@@ -15299,9 +15771,15 @@
       <c r="BF81" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BG81" t="inlineStr">
-        <is>
-          <t>5365</t>
+      <c r="BG81" t="n">
+        <v>5365</v>
+      </c>
+      <c r="BH81" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BI81" t="inlineStr">
+        <is>
+          <t>3090</t>
         </is>
       </c>
     </row>
@@ -15486,9 +15964,15 @@
       <c r="BF82" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="BG82" t="inlineStr">
-        <is>
-          <t>5222</t>
+      <c r="BG82" t="n">
+        <v>5222</v>
+      </c>
+      <c r="BH82" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="BI82" t="inlineStr">
+        <is>
+          <t>2753</t>
         </is>
       </c>
     </row>
@@ -15673,9 +16157,15 @@
       <c r="BF83" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BG83" t="inlineStr">
-        <is>
-          <t>4803</t>
+      <c r="BG83" t="n">
+        <v>4803</v>
+      </c>
+      <c r="BH83" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BI83" t="inlineStr">
+        <is>
+          <t>2967</t>
         </is>
       </c>
     </row>
@@ -15811,6 +16301,8 @@
       <c r="BE84" t="inlineStr"/>
       <c r="BF84" s="3" t="inlineStr"/>
       <c r="BG84" t="inlineStr"/>
+      <c r="BH84" s="3" t="inlineStr"/>
+      <c r="BI84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -15993,9 +16485,15 @@
       <c r="BF85" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="BG85" t="inlineStr">
-        <is>
-          <t>4152</t>
+      <c r="BG85" t="n">
+        <v>4152</v>
+      </c>
+      <c r="BH85" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="BI85" t="inlineStr">
+        <is>
+          <t>2744</t>
         </is>
       </c>
     </row>
@@ -16180,9 +16678,15 @@
       <c r="BF86" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="BG86" t="inlineStr">
-        <is>
-          <t>3905</t>
+      <c r="BG86" t="n">
+        <v>3905</v>
+      </c>
+      <c r="BH86" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="BI86" t="inlineStr">
+        <is>
+          <t>2509</t>
         </is>
       </c>
     </row>
@@ -16367,9 +16871,15 @@
       <c r="BF87" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BG87" t="inlineStr">
-        <is>
-          <t>5004</t>
+      <c r="BG87" t="n">
+        <v>5004</v>
+      </c>
+      <c r="BH87" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BI87" t="inlineStr">
+        <is>
+          <t>3141</t>
         </is>
       </c>
     </row>
@@ -16554,9 +17064,15 @@
       <c r="BF88" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BG88" t="inlineStr">
-        <is>
-          <t>3015</t>
+      <c r="BG88" t="n">
+        <v>3015</v>
+      </c>
+      <c r="BH88" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BI88" t="inlineStr">
+        <is>
+          <t>2693</t>
         </is>
       </c>
     </row>
@@ -16741,9 +17257,15 @@
       <c r="BF89" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="BG89" t="inlineStr">
-        <is>
-          <t>3494</t>
+      <c r="BG89" t="n">
+        <v>3494</v>
+      </c>
+      <c r="BH89" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BI89" t="inlineStr">
+        <is>
+          <t>2838</t>
         </is>
       </c>
     </row>
@@ -16928,9 +17450,15 @@
       <c r="BF90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG90" t="inlineStr">
-        <is>
-          <t>2988</t>
+      <c r="BG90" t="n">
+        <v>2988</v>
+      </c>
+      <c r="BH90" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BI90" t="inlineStr">
+        <is>
+          <t>2675</t>
         </is>
       </c>
     </row>
@@ -17115,9 +17643,15 @@
       <c r="BF91" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BG91" t="inlineStr">
-        <is>
-          <t>2989</t>
+      <c r="BG91" t="n">
+        <v>2989</v>
+      </c>
+      <c r="BH91" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BI91" t="inlineStr">
+        <is>
+          <t>2697</t>
         </is>
       </c>
     </row>
@@ -17302,7 +17836,13 @@
       <c r="BF92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG92" t="inlineStr">
+      <c r="BG92" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -17489,9 +18029,15 @@
       <c r="BF93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG93" t="inlineStr">
-        <is>
-          <t>2441</t>
+      <c r="BG93" t="n">
+        <v>2441</v>
+      </c>
+      <c r="BH93" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BI93" t="inlineStr">
+        <is>
+          <t>2269</t>
         </is>
       </c>
     </row>
@@ -17676,9 +18222,15 @@
       <c r="BF94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG94" t="inlineStr">
-        <is>
-          <t>2812</t>
+      <c r="BG94" t="n">
+        <v>2812</v>
+      </c>
+      <c r="BH94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI94" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -17863,9 +18415,15 @@
       <c r="BF95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG95" t="inlineStr">
-        <is>
-          <t>2517</t>
+      <c r="BG95" t="n">
+        <v>2517</v>
+      </c>
+      <c r="BH95" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="BI95" t="inlineStr">
+        <is>
+          <t>2504</t>
         </is>
       </c>
     </row>
@@ -18050,9 +18608,15 @@
       <c r="BF96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG96" t="inlineStr">
-        <is>
-          <t>2464</t>
+      <c r="BG96" t="n">
+        <v>2464</v>
+      </c>
+      <c r="BH96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI96" t="inlineStr">
+        <is>
+          <t>2012</t>
         </is>
       </c>
     </row>
@@ -18237,9 +18801,15 @@
       <c r="BF97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG97" t="inlineStr">
-        <is>
-          <t>3557</t>
+      <c r="BG97" t="n">
+        <v>3557</v>
+      </c>
+      <c r="BH97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI97" t="inlineStr">
+        <is>
+          <t>2499</t>
         </is>
       </c>
     </row>
@@ -18424,7 +18994,13 @@
       <c r="BF98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG98" t="inlineStr">
+      <c r="BG98" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18611,9 +19187,15 @@
       <c r="BF99" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BG99" t="inlineStr">
-        <is>
-          <t>4084</t>
+      <c r="BG99" t="n">
+        <v>4084</v>
+      </c>
+      <c r="BH99" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="BI99" t="inlineStr">
+        <is>
+          <t>2489</t>
         </is>
       </c>
     </row>
@@ -18798,9 +19380,15 @@
       <c r="BF100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG100" t="inlineStr">
-        <is>
-          <t>2474</t>
+      <c r="BG100" t="n">
+        <v>2474</v>
+      </c>
+      <c r="BH100" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="BI100" t="inlineStr">
+        <is>
+          <t>2133</t>
         </is>
       </c>
     </row>
@@ -18985,9 +19573,15 @@
       <c r="BF101" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="BG101" t="inlineStr">
-        <is>
-          <t>4812</t>
+      <c r="BG101" t="n">
+        <v>4812</v>
+      </c>
+      <c r="BH101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BI101" t="inlineStr">
+        <is>
+          <t>2915</t>
         </is>
       </c>
     </row>
@@ -19172,9 +19766,15 @@
       <c r="BF102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BG102" t="inlineStr">
-        <is>
-          <t>4209</t>
+      <c r="BG102" t="n">
+        <v>4209</v>
+      </c>
+      <c r="BH102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BI102" t="inlineStr">
+        <is>
+          <t>2770</t>
         </is>
       </c>
     </row>
@@ -19359,9 +19959,15 @@
       <c r="BF103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG103" t="inlineStr">
-        <is>
-          <t>3948</t>
+      <c r="BG103" t="n">
+        <v>3948</v>
+      </c>
+      <c r="BH103" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="BI103" t="inlineStr">
+        <is>
+          <t>2786</t>
         </is>
       </c>
     </row>
@@ -19546,9 +20152,15 @@
       <c r="BF104" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="BG104" t="inlineStr">
-        <is>
-          <t>4753</t>
+      <c r="BG104" t="n">
+        <v>4753</v>
+      </c>
+      <c r="BH104" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="BI104" t="inlineStr">
+        <is>
+          <t>2945</t>
         </is>
       </c>
     </row>
@@ -19733,9 +20345,15 @@
       <c r="BF105" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="BG105" t="inlineStr">
-        <is>
-          <t>4308</t>
+      <c r="BG105" t="n">
+        <v>4308</v>
+      </c>
+      <c r="BH105" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="BI105" t="inlineStr">
+        <is>
+          <t>2910</t>
         </is>
       </c>
     </row>
@@ -19920,7 +20538,13 @@
       <c r="BF106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG106" t="inlineStr">
+      <c r="BG106" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -20107,9 +20731,15 @@
       <c r="BF107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG107" t="inlineStr">
-        <is>
-          <t>2614</t>
+      <c r="BG107" t="n">
+        <v>2614</v>
+      </c>
+      <c r="BH107" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="BI107" t="inlineStr">
+        <is>
+          <t>2620</t>
         </is>
       </c>
     </row>
@@ -20294,7 +20924,13 @@
       <c r="BF108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG108" t="inlineStr">
+      <c r="BG108" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -20481,9 +21117,15 @@
       <c r="BF109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG109" t="inlineStr">
-        <is>
-          <t>4084</t>
+      <c r="BG109" t="n">
+        <v>4084</v>
+      </c>
+      <c r="BH109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI109" t="inlineStr">
+        <is>
+          <t>2550</t>
         </is>
       </c>
     </row>
@@ -20668,9 +21310,15 @@
       <c r="BF110" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="BG110" t="inlineStr">
-        <is>
-          <t>3898</t>
+      <c r="BG110" t="n">
+        <v>3898</v>
+      </c>
+      <c r="BH110" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BI110" t="inlineStr">
+        <is>
+          <t>2894</t>
         </is>
       </c>
     </row>
@@ -20830,6 +21478,8 @@
       <c r="BE111" t="inlineStr"/>
       <c r="BF111" s="3" t="inlineStr"/>
       <c r="BG111" t="inlineStr"/>
+      <c r="BH111" s="3" t="inlineStr"/>
+      <c r="BI111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -21012,9 +21662,15 @@
       <c r="BF112" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BG112" t="inlineStr">
-        <is>
-          <t>2969</t>
+      <c r="BG112" t="n">
+        <v>2969</v>
+      </c>
+      <c r="BH112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI112" t="inlineStr">
+        <is>
+          <t>2509</t>
         </is>
       </c>
     </row>
@@ -21199,9 +21855,15 @@
       <c r="BF113" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="BG113" t="inlineStr">
-        <is>
-          <t>3795</t>
+      <c r="BG113" t="n">
+        <v>3795</v>
+      </c>
+      <c r="BH113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI113" t="inlineStr">
+        <is>
+          <t>2680</t>
         </is>
       </c>
     </row>
@@ -21386,9 +22048,15 @@
       <c r="BF114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG114" t="inlineStr">
-        <is>
-          <t>3872</t>
+      <c r="BG114" t="n">
+        <v>3872</v>
+      </c>
+      <c r="BH114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI114" t="inlineStr">
+        <is>
+          <t>2610</t>
         </is>
       </c>
     </row>
@@ -21573,9 +22241,15 @@
       <c r="BF115" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="BG115" t="inlineStr">
-        <is>
-          <t>2359</t>
+      <c r="BG115" t="n">
+        <v>2359</v>
+      </c>
+      <c r="BH115" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BI115" t="inlineStr">
+        <is>
+          <t>2231</t>
         </is>
       </c>
     </row>
@@ -21760,9 +22434,15 @@
       <c r="BF116" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="BG116" t="inlineStr">
-        <is>
-          <t>3400</t>
+      <c r="BG116" t="n">
+        <v>3400</v>
+      </c>
+      <c r="BH116" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="BI116" t="inlineStr">
+        <is>
+          <t>2524</t>
         </is>
       </c>
     </row>
@@ -21947,9 +22627,15 @@
       <c r="BF117" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="BG117" t="inlineStr">
-        <is>
-          <t>3863</t>
+      <c r="BG117" t="n">
+        <v>3863</v>
+      </c>
+      <c r="BH117" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BI117" t="inlineStr">
+        <is>
+          <t>2863</t>
         </is>
       </c>
     </row>
@@ -22134,7 +22820,13 @@
       <c r="BF118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG118" t="inlineStr">
+      <c r="BG118" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -22321,9 +23013,15 @@
       <c r="BF119" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="BG119" t="inlineStr">
-        <is>
-          <t>4413</t>
+      <c r="BG119" t="n">
+        <v>4413</v>
+      </c>
+      <c r="BH119" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="BI119" t="inlineStr">
+        <is>
+          <t>2862</t>
         </is>
       </c>
     </row>
@@ -22508,9 +23206,15 @@
       <c r="BF120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG120" t="inlineStr">
-        <is>
-          <t>2685</t>
+      <c r="BG120" t="n">
+        <v>2685</v>
+      </c>
+      <c r="BH120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI120" t="inlineStr">
+        <is>
+          <t>2492</t>
         </is>
       </c>
     </row>
@@ -22695,9 +23399,15 @@
       <c r="BF121" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="BG121" t="inlineStr">
-        <is>
-          <t>3854</t>
+      <c r="BG121" t="n">
+        <v>3854</v>
+      </c>
+      <c r="BH121" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="BI121" t="inlineStr">
+        <is>
+          <t>2728</t>
         </is>
       </c>
     </row>
@@ -22882,7 +23592,13 @@
       <c r="BF122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG122" t="inlineStr">
+      <c r="BG122" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -23069,9 +23785,15 @@
       <c r="BF123" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BG123" t="inlineStr">
-        <is>
-          <t>3583</t>
+      <c r="BG123" t="n">
+        <v>3583</v>
+      </c>
+      <c r="BH123" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BI123" t="inlineStr">
+        <is>
+          <t>2770</t>
         </is>
       </c>
     </row>
@@ -23256,9 +23978,15 @@
       <c r="BF124" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="BG124" t="inlineStr">
-        <is>
-          <t>3470</t>
+      <c r="BG124" t="n">
+        <v>3470</v>
+      </c>
+      <c r="BH124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BI124" t="inlineStr">
+        <is>
+          <t>2820</t>
         </is>
       </c>
     </row>
@@ -23443,9 +24171,15 @@
       <c r="BF125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG125" t="inlineStr">
-        <is>
-          <t>3728</t>
+      <c r="BG125" t="n">
+        <v>3728</v>
+      </c>
+      <c r="BH125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI125" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -23630,9 +24364,15 @@
       <c r="BF126" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="BG126" t="inlineStr">
-        <is>
-          <t>3523</t>
+      <c r="BG126" t="n">
+        <v>3523</v>
+      </c>
+      <c r="BH126" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BI126" t="inlineStr">
+        <is>
+          <t>2887</t>
         </is>
       </c>
     </row>
@@ -23817,9 +24557,15 @@
       <c r="BF127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG127" t="inlineStr">
-        <is>
-          <t>2235</t>
+      <c r="BG127" t="n">
+        <v>2235</v>
+      </c>
+      <c r="BH127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI127" t="inlineStr">
+        <is>
+          <t>1997</t>
         </is>
       </c>
     </row>
@@ -24004,7 +24750,13 @@
       <c r="BF128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG128" t="inlineStr">
+      <c r="BG128" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -24191,7 +24943,13 @@
       <c r="BF129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG129" t="inlineStr">
+      <c r="BG129" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -24378,9 +25136,15 @@
       <c r="BF130" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="BG130" t="inlineStr">
-        <is>
-          <t>3037</t>
+      <c r="BG130" t="n">
+        <v>3037</v>
+      </c>
+      <c r="BH130" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BI130" t="inlineStr">
+        <is>
+          <t>2752</t>
         </is>
       </c>
     </row>
@@ -24565,7 +25329,13 @@
       <c r="BF131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG131" t="inlineStr">
+      <c r="BG131" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -24752,9 +25522,15 @@
       <c r="BF132" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BG132" t="inlineStr">
-        <is>
-          <t>2790</t>
+      <c r="BG132" t="n">
+        <v>2790</v>
+      </c>
+      <c r="BH132" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BI132" t="inlineStr">
+        <is>
+          <t>2506</t>
         </is>
       </c>
     </row>
@@ -24939,9 +25715,15 @@
       <c r="BF133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG133" t="inlineStr">
-        <is>
-          <t>3071</t>
+      <c r="BG133" t="n">
+        <v>3071</v>
+      </c>
+      <c r="BH133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI133" t="inlineStr">
+        <is>
+          <t>2513</t>
         </is>
       </c>
     </row>
@@ -25041,6 +25823,8 @@
       <c r="BE134" t="inlineStr"/>
       <c r="BF134" s="3" t="inlineStr"/>
       <c r="BG134" t="inlineStr"/>
+      <c r="BH134" s="3" t="inlineStr"/>
+      <c r="BI134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -25130,6 +25914,8 @@
       <c r="BE135" t="inlineStr"/>
       <c r="BF135" s="3" t="inlineStr"/>
       <c r="BG135" t="inlineStr"/>
+      <c r="BH135" s="3" t="inlineStr"/>
+      <c r="BI135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -25312,7 +26098,13 @@
       <c r="BF136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG136" t="inlineStr">
+      <c r="BG136" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI136" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -25499,7 +26291,13 @@
       <c r="BF137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG137" t="inlineStr">
+      <c r="BG137" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -25593,6 +26391,8 @@
       <c r="BE138" t="inlineStr"/>
       <c r="BF138" s="3" t="inlineStr"/>
       <c r="BG138" t="inlineStr"/>
+      <c r="BH138" s="3" t="inlineStr"/>
+      <c r="BI138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -25775,9 +26575,15 @@
       <c r="BF139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG139" t="inlineStr">
-        <is>
-          <t>2890</t>
+      <c r="BG139" t="n">
+        <v>2890</v>
+      </c>
+      <c r="BH139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI139" t="inlineStr">
+        <is>
+          <t>2492</t>
         </is>
       </c>
     </row>
@@ -25962,9 +26768,15 @@
       <c r="BF140" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BG140" t="inlineStr">
-        <is>
-          <t>3122</t>
+      <c r="BG140" t="n">
+        <v>3122</v>
+      </c>
+      <c r="BH140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI140" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -26056,6 +26868,8 @@
       <c r="BE141" t="inlineStr"/>
       <c r="BF141" s="3" t="inlineStr"/>
       <c r="BG141" t="inlineStr"/>
+      <c r="BH141" s="3" t="inlineStr"/>
+      <c r="BI141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -26238,7 +27052,13 @@
       <c r="BF142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG142" t="inlineStr">
+      <c r="BG142" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI142" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -26332,6 +27152,8 @@
       <c r="BE143" t="inlineStr"/>
       <c r="BF143" s="3" t="inlineStr"/>
       <c r="BG143" t="inlineStr"/>
+      <c r="BH143" s="3" t="inlineStr"/>
+      <c r="BI143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -26421,6 +27243,8 @@
       <c r="BE144" t="inlineStr"/>
       <c r="BF144" s="3" t="inlineStr"/>
       <c r="BG144" t="inlineStr"/>
+      <c r="BH144" s="3" t="inlineStr"/>
+      <c r="BI144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -26510,6 +27334,8 @@
       <c r="BE145" t="inlineStr"/>
       <c r="BF145" s="3" t="inlineStr"/>
       <c r="BG145" t="inlineStr"/>
+      <c r="BH145" s="3" t="inlineStr"/>
+      <c r="BI145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -26599,6 +27425,8 @@
       <c r="BE146" t="inlineStr"/>
       <c r="BF146" s="3" t="inlineStr"/>
       <c r="BG146" t="inlineStr"/>
+      <c r="BH146" s="3" t="inlineStr"/>
+      <c r="BI146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -26688,6 +27516,8 @@
       <c r="BE147" t="inlineStr"/>
       <c r="BF147" s="3" t="inlineStr"/>
       <c r="BG147" t="inlineStr"/>
+      <c r="BH147" s="3" t="inlineStr"/>
+      <c r="BI147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -26870,7 +27700,13 @@
       <c r="BF148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG148" t="inlineStr">
+      <c r="BG148" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -27057,9 +27893,15 @@
       <c r="BF149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG149" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="BG149" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI149" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -27244,7 +28086,13 @@
       <c r="BF150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG150" t="inlineStr">
+      <c r="BG150" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -27431,9 +28279,15 @@
       <c r="BF151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG151" t="inlineStr">
-        <is>
-          <t>2654</t>
+      <c r="BG151" t="n">
+        <v>2654</v>
+      </c>
+      <c r="BH151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI151" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -27618,7 +28472,13 @@
       <c r="BF152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG152" t="inlineStr">
+      <c r="BG152" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -27805,9 +28665,15 @@
       <c r="BF153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG153" t="inlineStr">
-        <is>
-          <t>2558</t>
+      <c r="BG153" t="n">
+        <v>2558</v>
+      </c>
+      <c r="BH153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI153" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -27992,7 +28858,13 @@
       <c r="BF154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG154" t="inlineStr">
+      <c r="BG154" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -28179,9 +29051,15 @@
       <c r="BF155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG155" t="inlineStr">
-        <is>
-          <t>2748</t>
+      <c r="BG155" t="n">
+        <v>2748</v>
+      </c>
+      <c r="BH155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI155" t="inlineStr">
+        <is>
+          <t>2499</t>
         </is>
       </c>
     </row>
@@ -28360,9 +29238,15 @@
       <c r="BF156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG156" t="inlineStr">
-        <is>
-          <t>3211</t>
+      <c r="BG156" t="n">
+        <v>3211</v>
+      </c>
+      <c r="BH156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI156" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -28448,6 +29332,8 @@
       <c r="BE157" t="inlineStr"/>
       <c r="BF157" s="3" t="inlineStr"/>
       <c r="BG157" t="inlineStr"/>
+      <c r="BH157" s="3" t="inlineStr"/>
+      <c r="BI157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -28624,7 +29510,13 @@
       <c r="BF158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG158" t="inlineStr">
+      <c r="BG158" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -28805,9 +29697,15 @@
       <c r="BF159" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="BG159" t="inlineStr">
-        <is>
-          <t>3410</t>
+      <c r="BG159" t="n">
+        <v>3410</v>
+      </c>
+      <c r="BH159" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BI159" t="inlineStr">
+        <is>
+          <t>2865</t>
         </is>
       </c>
     </row>
@@ -28893,6 +29791,8 @@
       <c r="BE160" t="inlineStr"/>
       <c r="BF160" s="3" t="inlineStr"/>
       <c r="BG160" t="inlineStr"/>
+      <c r="BH160" s="3" t="inlineStr"/>
+      <c r="BI160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -29057,9 +29957,15 @@
       <c r="BF161" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BG161" t="inlineStr">
-        <is>
-          <t>3509</t>
+      <c r="BG161" t="n">
+        <v>3509</v>
+      </c>
+      <c r="BH161" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BI161" t="inlineStr">
+        <is>
+          <t>2945</t>
         </is>
       </c>
     </row>
@@ -29226,9 +30132,15 @@
       <c r="BF162" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="BG162" t="inlineStr">
-        <is>
-          <t>3054</t>
+      <c r="BG162" t="n">
+        <v>3054</v>
+      </c>
+      <c r="BH162" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BI162" t="inlineStr">
+        <is>
+          <t>2745</t>
         </is>
       </c>
     </row>
@@ -29391,9 +30303,15 @@
       <c r="BF163" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG163" t="inlineStr">
-        <is>
-          <t>3376</t>
+      <c r="BG163" t="n">
+        <v>3376</v>
+      </c>
+      <c r="BH163" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI163" t="inlineStr">
+        <is>
+          <t>2494</t>
         </is>
       </c>
     </row>
@@ -29540,9 +30458,15 @@
       <c r="BF164" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BG164" t="inlineStr">
-        <is>
-          <t>3715</t>
+      <c r="BG164" t="n">
+        <v>3715</v>
+      </c>
+      <c r="BH164" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI164" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -29693,9 +30617,15 @@
       <c r="BF165" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="BG165" t="inlineStr">
-        <is>
-          <t>2879</t>
+      <c r="BG165" t="n">
+        <v>2879</v>
+      </c>
+      <c r="BH165" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI165" t="inlineStr">
+        <is>
+          <t>2479</t>
         </is>
       </c>
     </row>
@@ -29838,9 +30768,15 @@
       <c r="BF166" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG166" t="inlineStr">
-        <is>
-          <t>2791</t>
+      <c r="BG166" t="n">
+        <v>2791</v>
+      </c>
+      <c r="BH166" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI166" t="inlineStr">
+        <is>
+          <t>2525</t>
         </is>
       </c>
     </row>
@@ -29971,7 +30907,13 @@
       <c r="BF167" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG167" t="inlineStr">
+      <c r="BG167" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH167" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI167" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -30100,7 +31042,13 @@
       <c r="BF168" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG168" t="inlineStr">
+      <c r="BG168" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH168" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI168" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -30180,6 +31128,8 @@
       <c r="BE169" t="inlineStr"/>
       <c r="BF169" s="3" t="inlineStr"/>
       <c r="BG169" t="inlineStr"/>
+      <c r="BH169" s="3" t="inlineStr"/>
+      <c r="BI169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="n">
@@ -30300,7 +31250,13 @@
       <c r="BF170" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG170" t="inlineStr">
+      <c r="BG170" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH170" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI170" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -30413,9 +31369,15 @@
       <c r="BF171" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BG171" t="inlineStr">
-        <is>
-          <t>1938</t>
+      <c r="BG171" t="n">
+        <v>1938</v>
+      </c>
+      <c r="BH171" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI171" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -30526,7 +31488,13 @@
       <c r="BF172" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG172" t="inlineStr">
+      <c r="BG172" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH172" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI172" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -30639,9 +31607,15 @@
       <c r="BF173" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BG173" t="inlineStr">
-        <is>
-          <t>1852</t>
+      <c r="BG173" t="n">
+        <v>1852</v>
+      </c>
+      <c r="BH173" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI173" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -30728,17 +31702,15 @@
       <c r="BF174" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="BG174" t="inlineStr">
-        <is>
-          <t>3449</t>
-        </is>
-      </c>
+      <c r="BG174" t="n">
+        <v>3449</v>
+      </c>
+      <c r="BH174" s="3" t="inlineStr"/>
+      <c r="BI174" t="inlineStr"/>
     </row>
     <row r="175">
-      <c r="A175" t="inlineStr">
-        <is>
-          <t>58945536</t>
-        </is>
+      <c r="A175" t="n">
+        <v>58945536</v>
       </c>
       <c r="B175" t="inlineStr">
         <is>
@@ -30807,9 +31779,258 @@
       <c r="BF175" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="BG175" t="inlineStr">
-        <is>
-          <t>3334</t>
+      <c r="BG175" t="n">
+        <v>3334</v>
+      </c>
+      <c r="BH175" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="BI175" t="inlineStr">
+        <is>
+          <t>2847</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>55317038</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>necman12345</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr"/>
+      <c r="D176" t="inlineStr"/>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F176" s="3" t="inlineStr"/>
+      <c r="G176" t="inlineStr"/>
+      <c r="H176" s="3" t="inlineStr"/>
+      <c r="I176" t="inlineStr"/>
+      <c r="J176" s="3" t="inlineStr"/>
+      <c r="K176" t="inlineStr"/>
+      <c r="L176" s="3" t="inlineStr"/>
+      <c r="M176" t="inlineStr"/>
+      <c r="N176" s="3" t="inlineStr"/>
+      <c r="O176" t="inlineStr"/>
+      <c r="P176" s="3" t="inlineStr"/>
+      <c r="Q176" t="inlineStr"/>
+      <c r="R176" s="3" t="inlineStr"/>
+      <c r="S176" t="inlineStr"/>
+      <c r="T176" s="3" t="inlineStr"/>
+      <c r="U176" t="inlineStr"/>
+      <c r="V176" s="3" t="inlineStr"/>
+      <c r="W176" t="inlineStr"/>
+      <c r="X176" s="3" t="inlineStr"/>
+      <c r="Y176" t="inlineStr"/>
+      <c r="Z176" s="3" t="inlineStr"/>
+      <c r="AA176" t="inlineStr"/>
+      <c r="AB176" s="3" t="inlineStr"/>
+      <c r="AC176" t="inlineStr"/>
+      <c r="AD176" s="3" t="inlineStr"/>
+      <c r="AE176" t="inlineStr"/>
+      <c r="AF176" s="3" t="inlineStr"/>
+      <c r="AG176" t="inlineStr"/>
+      <c r="AH176" s="3" t="inlineStr"/>
+      <c r="AI176" t="inlineStr"/>
+      <c r="AJ176" s="3" t="inlineStr"/>
+      <c r="AK176" t="inlineStr"/>
+      <c r="AL176" s="3" t="inlineStr"/>
+      <c r="AM176" t="inlineStr"/>
+      <c r="AN176" s="3" t="inlineStr"/>
+      <c r="AO176" t="inlineStr"/>
+      <c r="AP176" s="3" t="inlineStr"/>
+      <c r="AQ176" t="inlineStr"/>
+      <c r="AR176" s="3" t="inlineStr"/>
+      <c r="AS176" t="inlineStr"/>
+      <c r="AT176" s="3" t="inlineStr"/>
+      <c r="AU176" t="inlineStr"/>
+      <c r="AV176" s="3" t="inlineStr"/>
+      <c r="AW176" t="inlineStr"/>
+      <c r="AX176" s="3" t="inlineStr"/>
+      <c r="AY176" t="inlineStr"/>
+      <c r="AZ176" s="3" t="inlineStr"/>
+      <c r="BA176" t="inlineStr"/>
+      <c r="BB176" s="3" t="inlineStr"/>
+      <c r="BC176" t="inlineStr"/>
+      <c r="BD176" s="3" t="inlineStr"/>
+      <c r="BE176" t="inlineStr"/>
+      <c r="BF176" s="3" t="inlineStr"/>
+      <c r="BG176" t="inlineStr"/>
+      <c r="BH176" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BI176" t="inlineStr">
+        <is>
+          <t>2964</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>56829330</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>"FLO ALX"</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr"/>
+      <c r="D177" t="inlineStr"/>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F177" s="3" t="inlineStr"/>
+      <c r="G177" t="inlineStr"/>
+      <c r="H177" s="3" t="inlineStr"/>
+      <c r="I177" t="inlineStr"/>
+      <c r="J177" s="3" t="inlineStr"/>
+      <c r="K177" t="inlineStr"/>
+      <c r="L177" s="3" t="inlineStr"/>
+      <c r="M177" t="inlineStr"/>
+      <c r="N177" s="3" t="inlineStr"/>
+      <c r="O177" t="inlineStr"/>
+      <c r="P177" s="3" t="inlineStr"/>
+      <c r="Q177" t="inlineStr"/>
+      <c r="R177" s="3" t="inlineStr"/>
+      <c r="S177" t="inlineStr"/>
+      <c r="T177" s="3" t="inlineStr"/>
+      <c r="U177" t="inlineStr"/>
+      <c r="V177" s="3" t="inlineStr"/>
+      <c r="W177" t="inlineStr"/>
+      <c r="X177" s="3" t="inlineStr"/>
+      <c r="Y177" t="inlineStr"/>
+      <c r="Z177" s="3" t="inlineStr"/>
+      <c r="AA177" t="inlineStr"/>
+      <c r="AB177" s="3" t="inlineStr"/>
+      <c r="AC177" t="inlineStr"/>
+      <c r="AD177" s="3" t="inlineStr"/>
+      <c r="AE177" t="inlineStr"/>
+      <c r="AF177" s="3" t="inlineStr"/>
+      <c r="AG177" t="inlineStr"/>
+      <c r="AH177" s="3" t="inlineStr"/>
+      <c r="AI177" t="inlineStr"/>
+      <c r="AJ177" s="3" t="inlineStr"/>
+      <c r="AK177" t="inlineStr"/>
+      <c r="AL177" s="3" t="inlineStr"/>
+      <c r="AM177" t="inlineStr"/>
+      <c r="AN177" s="3" t="inlineStr"/>
+      <c r="AO177" t="inlineStr"/>
+      <c r="AP177" s="3" t="inlineStr"/>
+      <c r="AQ177" t="inlineStr"/>
+      <c r="AR177" s="3" t="inlineStr"/>
+      <c r="AS177" t="inlineStr"/>
+      <c r="AT177" s="3" t="inlineStr"/>
+      <c r="AU177" t="inlineStr"/>
+      <c r="AV177" s="3" t="inlineStr"/>
+      <c r="AW177" t="inlineStr"/>
+      <c r="AX177" s="3" t="inlineStr"/>
+      <c r="AY177" t="inlineStr"/>
+      <c r="AZ177" s="3" t="inlineStr"/>
+      <c r="BA177" t="inlineStr"/>
+      <c r="BB177" s="3" t="inlineStr"/>
+      <c r="BC177" t="inlineStr"/>
+      <c r="BD177" s="3" t="inlineStr"/>
+      <c r="BE177" t="inlineStr"/>
+      <c r="BF177" s="3" t="inlineStr"/>
+      <c r="BG177" t="inlineStr"/>
+      <c r="BH177" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="BI177" t="inlineStr">
+        <is>
+          <t>2900</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>48738257</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>死亡洲际跳蛋</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr"/>
+      <c r="D178" t="inlineStr"/>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F178" s="3" t="inlineStr"/>
+      <c r="G178" t="inlineStr"/>
+      <c r="H178" s="3" t="inlineStr"/>
+      <c r="I178" t="inlineStr"/>
+      <c r="J178" s="3" t="inlineStr"/>
+      <c r="K178" t="inlineStr"/>
+      <c r="L178" s="3" t="inlineStr"/>
+      <c r="M178" t="inlineStr"/>
+      <c r="N178" s="3" t="inlineStr"/>
+      <c r="O178" t="inlineStr"/>
+      <c r="P178" s="3" t="inlineStr"/>
+      <c r="Q178" t="inlineStr"/>
+      <c r="R178" s="3" t="inlineStr"/>
+      <c r="S178" t="inlineStr"/>
+      <c r="T178" s="3" t="inlineStr"/>
+      <c r="U178" t="inlineStr"/>
+      <c r="V178" s="3" t="inlineStr"/>
+      <c r="W178" t="inlineStr"/>
+      <c r="X178" s="3" t="inlineStr"/>
+      <c r="Y178" t="inlineStr"/>
+      <c r="Z178" s="3" t="inlineStr"/>
+      <c r="AA178" t="inlineStr"/>
+      <c r="AB178" s="3" t="inlineStr"/>
+      <c r="AC178" t="inlineStr"/>
+      <c r="AD178" s="3" t="inlineStr"/>
+      <c r="AE178" t="inlineStr"/>
+      <c r="AF178" s="3" t="inlineStr"/>
+      <c r="AG178" t="inlineStr"/>
+      <c r="AH178" s="3" t="inlineStr"/>
+      <c r="AI178" t="inlineStr"/>
+      <c r="AJ178" s="3" t="inlineStr"/>
+      <c r="AK178" t="inlineStr"/>
+      <c r="AL178" s="3" t="inlineStr"/>
+      <c r="AM178" t="inlineStr"/>
+      <c r="AN178" s="3" t="inlineStr"/>
+      <c r="AO178" t="inlineStr"/>
+      <c r="AP178" s="3" t="inlineStr"/>
+      <c r="AQ178" t="inlineStr"/>
+      <c r="AR178" s="3" t="inlineStr"/>
+      <c r="AS178" t="inlineStr"/>
+      <c r="AT178" s="3" t="inlineStr"/>
+      <c r="AU178" t="inlineStr"/>
+      <c r="AV178" s="3" t="inlineStr"/>
+      <c r="AW178" t="inlineStr"/>
+      <c r="AX178" s="3" t="inlineStr"/>
+      <c r="AY178" t="inlineStr"/>
+      <c r="AZ178" s="3" t="inlineStr"/>
+      <c r="BA178" t="inlineStr"/>
+      <c r="BB178" s="3" t="inlineStr"/>
+      <c r="BC178" t="inlineStr"/>
+      <c r="BD178" s="3" t="inlineStr"/>
+      <c r="BE178" t="inlineStr"/>
+      <c r="BF178" s="3" t="inlineStr"/>
+      <c r="BG178" t="inlineStr"/>
+      <c r="BH178" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI178" t="inlineStr">
+        <is>
+          <t>2559</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-03-14 11:30:37
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BI178"/>
+  <dimension ref="A1:BK178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -696,6 +696,16 @@
           <t>03-12_0</t>
         </is>
       </c>
+      <c r="BJ1" s="1" t="inlineStr">
+        <is>
+          <t>03-13_A</t>
+        </is>
+      </c>
+      <c r="BK1" s="1" t="inlineStr">
+        <is>
+          <t>03-13_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -884,9 +894,15 @@
       <c r="BH2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI2" t="inlineStr">
-        <is>
-          <t>2518</t>
+      <c r="BI2" t="n">
+        <v>2518</v>
+      </c>
+      <c r="BJ2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK2" t="inlineStr">
+        <is>
+          <t>2517</t>
         </is>
       </c>
     </row>
@@ -1077,9 +1093,15 @@
       <c r="BH3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BI3" t="inlineStr">
-        <is>
-          <t>2944</t>
+      <c r="BI3" t="n">
+        <v>2944</v>
+      </c>
+      <c r="BJ3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BK3" t="inlineStr">
+        <is>
+          <t>3335</t>
         </is>
       </c>
     </row>
@@ -1270,9 +1292,15 @@
       <c r="BH4" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="BI4" t="inlineStr">
-        <is>
-          <t>3014</t>
+      <c r="BI4" t="n">
+        <v>3014</v>
+      </c>
+      <c r="BJ4" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="BK4" t="inlineStr">
+        <is>
+          <t>3562</t>
         </is>
       </c>
     </row>
@@ -1463,9 +1491,15 @@
       <c r="BH5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BI5" t="inlineStr">
-        <is>
-          <t>2869</t>
+      <c r="BI5" t="n">
+        <v>2869</v>
+      </c>
+      <c r="BJ5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BK5" t="inlineStr">
+        <is>
+          <t>3277</t>
         </is>
       </c>
     </row>
@@ -1656,9 +1690,15 @@
       <c r="BH6" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BI6" t="inlineStr">
-        <is>
-          <t>2844</t>
+      <c r="BI6" t="n">
+        <v>2844</v>
+      </c>
+      <c r="BJ6" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BK6" t="inlineStr">
+        <is>
+          <t>3200</t>
         </is>
       </c>
     </row>
@@ -1849,9 +1889,15 @@
       <c r="BH7" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="BI7" t="inlineStr">
-        <is>
-          <t>2963</t>
+      <c r="BI7" t="n">
+        <v>2963</v>
+      </c>
+      <c r="BJ7" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="BK7" t="inlineStr">
+        <is>
+          <t>3417</t>
         </is>
       </c>
     </row>
@@ -2042,9 +2088,15 @@
       <c r="BH8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BI8" t="inlineStr">
-        <is>
-          <t>2816</t>
+      <c r="BI8" t="n">
+        <v>2816</v>
+      </c>
+      <c r="BJ8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BK8" t="inlineStr">
+        <is>
+          <t>3123</t>
         </is>
       </c>
     </row>
@@ -2235,9 +2287,15 @@
       <c r="BH9" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BI9" t="inlineStr">
-        <is>
-          <t>3120</t>
+      <c r="BI9" t="n">
+        <v>3120</v>
+      </c>
+      <c r="BJ9" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BK9" t="inlineStr">
+        <is>
+          <t>3655</t>
         </is>
       </c>
     </row>
@@ -2428,9 +2486,15 @@
       <c r="BH10" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BI10" t="inlineStr">
-        <is>
-          <t>2939</t>
+      <c r="BI10" t="n">
+        <v>2939</v>
+      </c>
+      <c r="BJ10" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BK10" t="inlineStr">
+        <is>
+          <t>3419</t>
         </is>
       </c>
     </row>
@@ -2621,9 +2685,15 @@
       <c r="BH11" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BI11" t="inlineStr">
-        <is>
-          <t>2807</t>
+      <c r="BI11" t="n">
+        <v>2807</v>
+      </c>
+      <c r="BJ11" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BK11" t="inlineStr">
+        <is>
+          <t>3122</t>
         </is>
       </c>
     </row>
@@ -2814,9 +2884,15 @@
       <c r="BH12" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="BI12" t="inlineStr">
-        <is>
-          <t>2604</t>
+      <c r="BI12" t="n">
+        <v>2604</v>
+      </c>
+      <c r="BJ12" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="BK12" t="inlineStr">
+        <is>
+          <t>2719</t>
         </is>
       </c>
     </row>
@@ -3007,9 +3083,15 @@
       <c r="BH13" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="BI13" t="inlineStr">
-        <is>
-          <t>3168</t>
+      <c r="BI13" t="n">
+        <v>3168</v>
+      </c>
+      <c r="BJ13" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BK13" t="inlineStr">
+        <is>
+          <t>3643</t>
         </is>
       </c>
     </row>
@@ -3200,9 +3282,15 @@
       <c r="BH14" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BI14" t="inlineStr">
-        <is>
-          <t>2863</t>
+      <c r="BI14" t="n">
+        <v>2863</v>
+      </c>
+      <c r="BJ14" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BK14" t="inlineStr">
+        <is>
+          <t>3224</t>
         </is>
       </c>
     </row>
@@ -3393,7 +3481,13 @@
       <c r="BH15" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI15" t="inlineStr">
+      <c r="BI15" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK15" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3586,9 +3680,15 @@
       <c r="BH16" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="BI16" t="inlineStr">
-        <is>
-          <t>2967</t>
+      <c r="BI16" t="n">
+        <v>2967</v>
+      </c>
+      <c r="BJ16" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="BK16" t="inlineStr">
+        <is>
+          <t>3440</t>
         </is>
       </c>
     </row>
@@ -3779,9 +3879,15 @@
       <c r="BH17" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BI17" t="inlineStr">
-        <is>
-          <t>2925</t>
+      <c r="BI17" t="n">
+        <v>2925</v>
+      </c>
+      <c r="BJ17" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="BK17" t="inlineStr">
+        <is>
+          <t>3261</t>
         </is>
       </c>
     </row>
@@ -3972,9 +4078,15 @@
       <c r="BH18" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="BI18" t="inlineStr">
-        <is>
-          <t>2864</t>
+      <c r="BI18" t="n">
+        <v>2864</v>
+      </c>
+      <c r="BJ18" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="BK18" t="inlineStr">
+        <is>
+          <t>3247</t>
         </is>
       </c>
     </row>
@@ -4165,9 +4277,15 @@
       <c r="BH19" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BI19" t="inlineStr">
-        <is>
-          <t>2808</t>
+      <c r="BI19" t="n">
+        <v>2808</v>
+      </c>
+      <c r="BJ19" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BK19" t="inlineStr">
+        <is>
+          <t>3119</t>
         </is>
       </c>
     </row>
@@ -4358,9 +4476,15 @@
       <c r="BH20" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BI20" t="inlineStr">
-        <is>
-          <t>3003</t>
+      <c r="BI20" t="n">
+        <v>3003</v>
+      </c>
+      <c r="BJ20" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="BK20" t="inlineStr">
+        <is>
+          <t>3598</t>
         </is>
       </c>
     </row>
@@ -4551,7 +4675,13 @@
       <c r="BH21" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BI21" t="inlineStr">
+      <c r="BI21" t="n">
+        <v>2816</v>
+      </c>
+      <c r="BJ21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK21" t="inlineStr">
         <is>
           <t>2816</t>
         </is>
@@ -4744,9 +4874,15 @@
       <c r="BH22" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BI22" t="inlineStr">
-        <is>
-          <t>3039</t>
+      <c r="BI22" t="n">
+        <v>3039</v>
+      </c>
+      <c r="BJ22" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="BK22" t="inlineStr">
+        <is>
+          <t>3570</t>
         </is>
       </c>
     </row>
@@ -4937,7 +5073,13 @@
       <c r="BH23" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="BI23" t="inlineStr">
+      <c r="BI23" t="n">
+        <v>2903</v>
+      </c>
+      <c r="BJ23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK23" t="inlineStr">
         <is>
           <t>2903</t>
         </is>
@@ -5130,9 +5272,15 @@
       <c r="BH24" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BI24" t="inlineStr">
-        <is>
-          <t>3066</t>
+      <c r="BI24" t="n">
+        <v>3066</v>
+      </c>
+      <c r="BJ24" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BK24" t="inlineStr">
+        <is>
+          <t>3570</t>
         </is>
       </c>
     </row>
@@ -5323,7 +5471,13 @@
       <c r="BH25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI25" t="inlineStr">
+      <c r="BI25" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5516,9 +5670,15 @@
       <c r="BH26" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="BI26" t="inlineStr">
-        <is>
-          <t>2517</t>
+      <c r="BI26" t="n">
+        <v>2517</v>
+      </c>
+      <c r="BJ26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK26" t="inlineStr">
+        <is>
+          <t>2572</t>
         </is>
       </c>
     </row>
@@ -5709,9 +5869,15 @@
       <c r="BH27" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BI27" t="inlineStr">
-        <is>
-          <t>3035</t>
+      <c r="BI27" t="n">
+        <v>3035</v>
+      </c>
+      <c r="BJ27" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="BK27" t="inlineStr">
+        <is>
+          <t>3513</t>
         </is>
       </c>
     </row>
@@ -5902,9 +6068,15 @@
       <c r="BH28" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="BI28" t="inlineStr">
-        <is>
-          <t>3008</t>
+      <c r="BI28" t="n">
+        <v>3008</v>
+      </c>
+      <c r="BJ28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="BK28" t="inlineStr">
+        <is>
+          <t>3513</t>
         </is>
       </c>
     </row>
@@ -6095,9 +6267,15 @@
       <c r="BH29" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BI29" t="inlineStr">
-        <is>
-          <t>3243</t>
+      <c r="BI29" t="n">
+        <v>3243</v>
+      </c>
+      <c r="BJ29" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BK29" t="inlineStr">
+        <is>
+          <t>3792</t>
         </is>
       </c>
     </row>
@@ -6288,9 +6466,15 @@
       <c r="BH30" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI30" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="BI30" t="n">
+        <v>2500</v>
+      </c>
+      <c r="BJ30" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BK30" t="inlineStr">
+        <is>
+          <t>2861</t>
         </is>
       </c>
     </row>
@@ -6481,9 +6665,15 @@
       <c r="BH31" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BI31" t="inlineStr">
-        <is>
-          <t>3118</t>
+      <c r="BI31" t="n">
+        <v>3118</v>
+      </c>
+      <c r="BJ31" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="BK31" t="inlineStr">
+        <is>
+          <t>3429</t>
         </is>
       </c>
     </row>
@@ -6674,9 +6864,15 @@
       <c r="BH32" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="BI32" t="inlineStr">
-        <is>
-          <t>2959</t>
+      <c r="BI32" t="n">
+        <v>2959</v>
+      </c>
+      <c r="BJ32" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="BK32" t="inlineStr">
+        <is>
+          <t>3355</t>
         </is>
       </c>
     </row>
@@ -6867,7 +7063,13 @@
       <c r="BH33" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BI33" t="inlineStr">
+      <c r="BI33" t="n">
+        <v>2834</v>
+      </c>
+      <c r="BJ33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK33" t="inlineStr">
         <is>
           <t>2834</t>
         </is>
@@ -7060,9 +7262,15 @@
       <c r="BH34" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BI34" t="inlineStr">
-        <is>
-          <t>3022</t>
+      <c r="BI34" t="n">
+        <v>3022</v>
+      </c>
+      <c r="BJ34" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BK34" t="inlineStr">
+        <is>
+          <t>3403</t>
         </is>
       </c>
     </row>
@@ -7253,9 +7461,15 @@
       <c r="BH35" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BI35" t="inlineStr">
-        <is>
-          <t>2994</t>
+      <c r="BI35" t="n">
+        <v>2994</v>
+      </c>
+      <c r="BJ35" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BK35" t="inlineStr">
+        <is>
+          <t>3420</t>
         </is>
       </c>
     </row>
@@ -7446,9 +7660,15 @@
       <c r="BH36" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BI36" t="inlineStr">
-        <is>
-          <t>2881</t>
+      <c r="BI36" t="n">
+        <v>2881</v>
+      </c>
+      <c r="BJ36" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="BK36" t="inlineStr">
+        <is>
+          <t>2986</t>
         </is>
       </c>
     </row>
@@ -7639,9 +7859,15 @@
       <c r="BH37" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BI37" t="inlineStr">
-        <is>
-          <t>2975</t>
+      <c r="BI37" t="n">
+        <v>2975</v>
+      </c>
+      <c r="BJ37" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BK37" t="inlineStr">
+        <is>
+          <t>3329</t>
         </is>
       </c>
     </row>
@@ -7832,9 +8058,15 @@
       <c r="BH38" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BI38" t="inlineStr">
-        <is>
-          <t>2930</t>
+      <c r="BI38" t="n">
+        <v>2930</v>
+      </c>
+      <c r="BJ38" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BK38" t="inlineStr">
+        <is>
+          <t>3396</t>
         </is>
       </c>
     </row>
@@ -8025,9 +8257,15 @@
       <c r="BH39" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="BI39" t="inlineStr">
-        <is>
-          <t>3037</t>
+      <c r="BI39" t="n">
+        <v>3037</v>
+      </c>
+      <c r="BJ39" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="BK39" t="inlineStr">
+        <is>
+          <t>3597</t>
         </is>
       </c>
     </row>
@@ -8218,9 +8456,15 @@
       <c r="BH40" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BI40" t="inlineStr">
-        <is>
-          <t>2903</t>
+      <c r="BI40" t="n">
+        <v>2903</v>
+      </c>
+      <c r="BJ40" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BK40" t="inlineStr">
+        <is>
+          <t>3353</t>
         </is>
       </c>
     </row>
@@ -8411,7 +8655,13 @@
       <c r="BH41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI41" t="inlineStr">
+      <c r="BI41" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK41" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8604,9 +8854,15 @@
       <c r="BH42" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="BI42" t="inlineStr">
-        <is>
-          <t>2998</t>
+      <c r="BI42" t="n">
+        <v>2998</v>
+      </c>
+      <c r="BJ42" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="BK42" t="inlineStr">
+        <is>
+          <t>3708</t>
         </is>
       </c>
     </row>
@@ -8797,9 +9053,15 @@
       <c r="BH43" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BI43" t="inlineStr">
-        <is>
-          <t>3060</t>
+      <c r="BI43" t="n">
+        <v>3060</v>
+      </c>
+      <c r="BJ43" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BK43" t="inlineStr">
+        <is>
+          <t>3593</t>
         </is>
       </c>
     </row>
@@ -8990,9 +9252,15 @@
       <c r="BH44" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BI44" t="inlineStr">
-        <is>
-          <t>3166</t>
+      <c r="BI44" t="n">
+        <v>3166</v>
+      </c>
+      <c r="BJ44" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BK44" t="inlineStr">
+        <is>
+          <t>3776</t>
         </is>
       </c>
     </row>
@@ -9183,9 +9451,15 @@
       <c r="BH45" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="BI45" t="inlineStr">
-        <is>
-          <t>2876</t>
+      <c r="BI45" t="n">
+        <v>2876</v>
+      </c>
+      <c r="BJ45" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="BK45" t="inlineStr">
+        <is>
+          <t>3219</t>
         </is>
       </c>
     </row>
@@ -9376,9 +9650,15 @@
       <c r="BH46" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BI46" t="inlineStr">
-        <is>
-          <t>2847</t>
+      <c r="BI46" t="n">
+        <v>2847</v>
+      </c>
+      <c r="BJ46" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BK46" t="inlineStr">
+        <is>
+          <t>3163</t>
         </is>
       </c>
     </row>
@@ -9569,9 +9849,15 @@
       <c r="BH47" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="BI47" t="inlineStr">
-        <is>
-          <t>2837</t>
+      <c r="BI47" t="n">
+        <v>2837</v>
+      </c>
+      <c r="BJ47" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BK47" t="inlineStr">
+        <is>
+          <t>3144</t>
         </is>
       </c>
     </row>
@@ -9762,9 +10048,15 @@
       <c r="BH48" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="BI48" t="inlineStr">
-        <is>
-          <t>3139</t>
+      <c r="BI48" t="n">
+        <v>3139</v>
+      </c>
+      <c r="BJ48" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="BK48" t="inlineStr">
+        <is>
+          <t>3686</t>
         </is>
       </c>
     </row>
@@ -9955,9 +10247,15 @@
       <c r="BH49" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BI49" t="inlineStr">
-        <is>
-          <t>2750</t>
+      <c r="BI49" t="n">
+        <v>2750</v>
+      </c>
+      <c r="BJ49" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="BK49" t="inlineStr">
+        <is>
+          <t>3055</t>
         </is>
       </c>
     </row>
@@ -10148,7 +10446,13 @@
       <c r="BH50" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI50" t="inlineStr">
+      <c r="BI50" t="n">
+        <v>2500</v>
+      </c>
+      <c r="BJ50" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK50" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -10341,7 +10645,13 @@
       <c r="BH51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI51" t="inlineStr">
+      <c r="BI51" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK51" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10534,7 +10844,13 @@
       <c r="BH52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI52" t="inlineStr">
+      <c r="BI52" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK52" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10727,9 +11043,15 @@
       <c r="BH53" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="BI53" t="inlineStr">
-        <is>
-          <t>2698</t>
+      <c r="BI53" t="n">
+        <v>2698</v>
+      </c>
+      <c r="BJ53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK53" t="inlineStr">
+        <is>
+          <t>2718</t>
         </is>
       </c>
     </row>
@@ -10920,9 +11242,15 @@
       <c r="BH54" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="BI54" t="inlineStr">
-        <is>
-          <t>2945</t>
+      <c r="BI54" t="n">
+        <v>2945</v>
+      </c>
+      <c r="BJ54" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="BK54" t="inlineStr">
+        <is>
+          <t>3341</t>
         </is>
       </c>
     </row>
@@ -11113,9 +11441,15 @@
       <c r="BH55" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BI55" t="inlineStr">
-        <is>
-          <t>2954</t>
+      <c r="BI55" t="n">
+        <v>2954</v>
+      </c>
+      <c r="BJ55" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BK55" t="inlineStr">
+        <is>
+          <t>3361</t>
         </is>
       </c>
     </row>
@@ -11306,9 +11640,15 @@
       <c r="BH56" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="BI56" t="inlineStr">
-        <is>
-          <t>2793</t>
+      <c r="BI56" t="n">
+        <v>2793</v>
+      </c>
+      <c r="BJ56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BK56" t="inlineStr">
+        <is>
+          <t>3104</t>
         </is>
       </c>
     </row>
@@ -11499,9 +11839,15 @@
       <c r="BH57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BI57" t="inlineStr">
-        <is>
-          <t>2854</t>
+      <c r="BI57" t="n">
+        <v>2854</v>
+      </c>
+      <c r="BJ57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BK57" t="inlineStr">
+        <is>
+          <t>3187</t>
         </is>
       </c>
     </row>
@@ -11692,9 +12038,15 @@
       <c r="BH58" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="BI58" t="inlineStr">
-        <is>
-          <t>2966</t>
+      <c r="BI58" t="n">
+        <v>2966</v>
+      </c>
+      <c r="BJ58" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="BK58" t="inlineStr">
+        <is>
+          <t>3397</t>
         </is>
       </c>
     </row>
@@ -11772,6 +12124,8 @@
       <c r="BG59" t="inlineStr"/>
       <c r="BH59" s="3" t="inlineStr"/>
       <c r="BI59" t="inlineStr"/>
+      <c r="BJ59" s="3" t="inlineStr"/>
+      <c r="BK59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -11847,6 +12201,8 @@
       <c r="BG60" t="inlineStr"/>
       <c r="BH60" s="3" t="inlineStr"/>
       <c r="BI60" t="inlineStr"/>
+      <c r="BJ60" s="3" t="inlineStr"/>
+      <c r="BK60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -12035,9 +12391,15 @@
       <c r="BH61" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BI61" t="inlineStr">
-        <is>
-          <t>2926</t>
+      <c r="BI61" t="n">
+        <v>2926</v>
+      </c>
+      <c r="BJ61" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BK61" t="inlineStr">
+        <is>
+          <t>3328</t>
         </is>
       </c>
     </row>
@@ -12228,7 +12590,13 @@
       <c r="BH62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI62" t="inlineStr">
+      <c r="BI62" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12421,9 +12789,15 @@
       <c r="BH63" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BI63" t="inlineStr">
-        <is>
-          <t>2896</t>
+      <c r="BI63" t="n">
+        <v>2896</v>
+      </c>
+      <c r="BJ63" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BK63" t="inlineStr">
+        <is>
+          <t>3299</t>
         </is>
       </c>
     </row>
@@ -12614,7 +12988,13 @@
       <c r="BH64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI64" t="inlineStr">
+      <c r="BI64" t="n">
+        <v>2500</v>
+      </c>
+      <c r="BJ64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK64" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -12694,6 +13074,8 @@
       <c r="BG65" t="inlineStr"/>
       <c r="BH65" s="3" t="inlineStr"/>
       <c r="BI65" t="inlineStr"/>
+      <c r="BJ65" s="3" t="inlineStr"/>
+      <c r="BK65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -12882,9 +13264,15 @@
       <c r="BH66" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="BI66" t="inlineStr">
-        <is>
-          <t>2600</t>
+      <c r="BI66" t="n">
+        <v>2600</v>
+      </c>
+      <c r="BJ66" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="BK66" t="inlineStr">
+        <is>
+          <t>2775</t>
         </is>
       </c>
     </row>
@@ -13075,9 +13463,15 @@
       <c r="BH67" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BI67" t="inlineStr">
-        <is>
-          <t>2836</t>
+      <c r="BI67" t="n">
+        <v>2836</v>
+      </c>
+      <c r="BJ67" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BK67" t="inlineStr">
+        <is>
+          <t>3183</t>
         </is>
       </c>
     </row>
@@ -13268,9 +13662,15 @@
       <c r="BH68" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BI68" t="inlineStr">
-        <is>
-          <t>2958</t>
+      <c r="BI68" t="n">
+        <v>2958</v>
+      </c>
+      <c r="BJ68" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BK68" t="inlineStr">
+        <is>
+          <t>3383</t>
         </is>
       </c>
     </row>
@@ -13461,9 +13861,15 @@
       <c r="BH69" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="BI69" t="inlineStr">
-        <is>
-          <t>3000</t>
+      <c r="BI69" t="n">
+        <v>3000</v>
+      </c>
+      <c r="BJ69" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BK69" t="inlineStr">
+        <is>
+          <t>3433</t>
         </is>
       </c>
     </row>
@@ -13654,9 +14060,15 @@
       <c r="BH70" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="BI70" t="inlineStr">
-        <is>
-          <t>2539</t>
+      <c r="BI70" t="n">
+        <v>2539</v>
+      </c>
+      <c r="BJ70" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="BK70" t="inlineStr">
+        <is>
+          <t>2609</t>
         </is>
       </c>
     </row>
@@ -13847,9 +14259,15 @@
       <c r="BH71" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BI71" t="inlineStr">
-        <is>
-          <t>2857</t>
+      <c r="BI71" t="n">
+        <v>2857</v>
+      </c>
+      <c r="BJ71" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BK71" t="inlineStr">
+        <is>
+          <t>3203</t>
         </is>
       </c>
     </row>
@@ -14040,9 +14458,15 @@
       <c r="BH72" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BI72" t="inlineStr">
-        <is>
-          <t>2931</t>
+      <c r="BI72" t="n">
+        <v>2931</v>
+      </c>
+      <c r="BJ72" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="BK72" t="inlineStr">
+        <is>
+          <t>3019</t>
         </is>
       </c>
     </row>
@@ -14233,9 +14657,15 @@
       <c r="BH73" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BI73" t="inlineStr">
-        <is>
-          <t>2796</t>
+      <c r="BI73" t="n">
+        <v>2796</v>
+      </c>
+      <c r="BJ73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BK73" t="inlineStr">
+        <is>
+          <t>3060</t>
         </is>
       </c>
     </row>
@@ -14426,9 +14856,15 @@
       <c r="BH74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI74" t="inlineStr">
-        <is>
-          <t>2514</t>
+      <c r="BI74" t="n">
+        <v>2514</v>
+      </c>
+      <c r="BJ74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK74" t="inlineStr">
+        <is>
+          <t>2585</t>
         </is>
       </c>
     </row>
@@ -14619,9 +15055,15 @@
       <c r="BH75" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BI75" t="inlineStr">
-        <is>
-          <t>2864</t>
+      <c r="BI75" t="n">
+        <v>2864</v>
+      </c>
+      <c r="BJ75" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BK75" t="inlineStr">
+        <is>
+          <t>3153</t>
         </is>
       </c>
     </row>
@@ -14812,9 +15254,15 @@
       <c r="BH76" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BI76" t="inlineStr">
-        <is>
-          <t>2896</t>
+      <c r="BI76" t="n">
+        <v>2896</v>
+      </c>
+      <c r="BJ76" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BK76" t="inlineStr">
+        <is>
+          <t>3295</t>
         </is>
       </c>
     </row>
@@ -15005,7 +15453,13 @@
       <c r="BH77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI77" t="inlineStr">
+      <c r="BI77" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK77" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15198,9 +15652,15 @@
       <c r="BH78" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BI78" t="inlineStr">
-        <is>
-          <t>3133</t>
+      <c r="BI78" t="n">
+        <v>3133</v>
+      </c>
+      <c r="BJ78" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BK78" t="inlineStr">
+        <is>
+          <t>3606</t>
         </is>
       </c>
     </row>
@@ -15391,7 +15851,13 @@
       <c r="BH79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI79" t="inlineStr">
+      <c r="BI79" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15584,9 +16050,15 @@
       <c r="BH80" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="BI80" t="inlineStr">
-        <is>
-          <t>2946</t>
+      <c r="BI80" t="n">
+        <v>2946</v>
+      </c>
+      <c r="BJ80" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="BK80" t="inlineStr">
+        <is>
+          <t>3366</t>
         </is>
       </c>
     </row>
@@ -15777,9 +16249,15 @@
       <c r="BH81" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BI81" t="inlineStr">
-        <is>
-          <t>3090</t>
+      <c r="BI81" t="n">
+        <v>3090</v>
+      </c>
+      <c r="BJ81" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BK81" t="inlineStr">
+        <is>
+          <t>3631</t>
         </is>
       </c>
     </row>
@@ -15970,9 +16448,15 @@
       <c r="BH82" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="BI82" t="inlineStr">
-        <is>
-          <t>2753</t>
+      <c r="BI82" t="n">
+        <v>2753</v>
+      </c>
+      <c r="BJ82" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BK82" t="inlineStr">
+        <is>
+          <t>3257</t>
         </is>
       </c>
     </row>
@@ -16163,9 +16647,15 @@
       <c r="BH83" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BI83" t="inlineStr">
-        <is>
-          <t>2967</t>
+      <c r="BI83" t="n">
+        <v>2967</v>
+      </c>
+      <c r="BJ83" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BK83" t="inlineStr">
+        <is>
+          <t>3348</t>
         </is>
       </c>
     </row>
@@ -16303,6 +16793,8 @@
       <c r="BG84" t="inlineStr"/>
       <c r="BH84" s="3" t="inlineStr"/>
       <c r="BI84" t="inlineStr"/>
+      <c r="BJ84" s="3" t="inlineStr"/>
+      <c r="BK84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -16491,9 +16983,15 @@
       <c r="BH85" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="BI85" t="inlineStr">
-        <is>
-          <t>2744</t>
+      <c r="BI85" t="n">
+        <v>2744</v>
+      </c>
+      <c r="BJ85" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BK85" t="inlineStr">
+        <is>
+          <t>3125</t>
         </is>
       </c>
     </row>
@@ -16684,9 +17182,15 @@
       <c r="BH86" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="BI86" t="inlineStr">
-        <is>
-          <t>2509</t>
+      <c r="BI86" t="n">
+        <v>2509</v>
+      </c>
+      <c r="BJ86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK86" t="inlineStr">
+        <is>
+          <t>2551</t>
         </is>
       </c>
     </row>
@@ -16877,9 +17381,15 @@
       <c r="BH87" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BI87" t="inlineStr">
-        <is>
-          <t>3141</t>
+      <c r="BI87" t="n">
+        <v>3141</v>
+      </c>
+      <c r="BJ87" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BK87" t="inlineStr">
+        <is>
+          <t>3692</t>
         </is>
       </c>
     </row>
@@ -17070,9 +17580,15 @@
       <c r="BH88" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BI88" t="inlineStr">
-        <is>
-          <t>2693</t>
+      <c r="BI88" t="n">
+        <v>2693</v>
+      </c>
+      <c r="BJ88" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BK88" t="inlineStr">
+        <is>
+          <t>2832</t>
         </is>
       </c>
     </row>
@@ -17263,9 +17779,15 @@
       <c r="BH89" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BI89" t="inlineStr">
-        <is>
-          <t>2838</t>
+      <c r="BI89" t="n">
+        <v>2838</v>
+      </c>
+      <c r="BJ89" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BK89" t="inlineStr">
+        <is>
+          <t>3043</t>
         </is>
       </c>
     </row>
@@ -17456,9 +17978,15 @@
       <c r="BH90" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BI90" t="inlineStr">
-        <is>
-          <t>2675</t>
+      <c r="BI90" t="n">
+        <v>2675</v>
+      </c>
+      <c r="BJ90" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="BK90" t="inlineStr">
+        <is>
+          <t>2664</t>
         </is>
       </c>
     </row>
@@ -17649,9 +18177,15 @@
       <c r="BH91" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BI91" t="inlineStr">
-        <is>
-          <t>2697</t>
+      <c r="BI91" t="n">
+        <v>2697</v>
+      </c>
+      <c r="BJ91" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BK91" t="inlineStr">
+        <is>
+          <t>2807</t>
         </is>
       </c>
     </row>
@@ -17842,7 +18376,13 @@
       <c r="BH92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI92" t="inlineStr">
+      <c r="BI92" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18035,9 +18575,15 @@
       <c r="BH93" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BI93" t="inlineStr">
-        <is>
-          <t>2269</t>
+      <c r="BI93" t="n">
+        <v>2269</v>
+      </c>
+      <c r="BJ93" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BK93" t="inlineStr">
+        <is>
+          <t>2597</t>
         </is>
       </c>
     </row>
@@ -18228,7 +18774,13 @@
       <c r="BH94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI94" t="inlineStr">
+      <c r="BI94" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18421,9 +18973,15 @@
       <c r="BH95" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="BI95" t="inlineStr">
-        <is>
-          <t>2504</t>
+      <c r="BI95" t="n">
+        <v>2504</v>
+      </c>
+      <c r="BJ95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK95" t="inlineStr">
+        <is>
+          <t>2494</t>
         </is>
       </c>
     </row>
@@ -18614,9 +19172,15 @@
       <c r="BH96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI96" t="inlineStr">
-        <is>
-          <t>2012</t>
+      <c r="BI96" t="n">
+        <v>2012</v>
+      </c>
+      <c r="BJ96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK96" t="inlineStr">
+        <is>
+          <t>2026</t>
         </is>
       </c>
     </row>
@@ -18807,9 +19371,15 @@
       <c r="BH97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI97" t="inlineStr">
-        <is>
-          <t>2499</t>
+      <c r="BI97" t="n">
+        <v>2499</v>
+      </c>
+      <c r="BJ97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK97" t="inlineStr">
+        <is>
+          <t>2496</t>
         </is>
       </c>
     </row>
@@ -19000,9 +19570,15 @@
       <c r="BH98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI98" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="BI98" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK98" t="inlineStr">
+        <is>
+          <t>2499</t>
         </is>
       </c>
     </row>
@@ -19193,9 +19769,15 @@
       <c r="BH99" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="BI99" t="inlineStr">
-        <is>
-          <t>2489</t>
+      <c r="BI99" t="n">
+        <v>2489</v>
+      </c>
+      <c r="BJ99" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="BK99" t="inlineStr">
+        <is>
+          <t>2577</t>
         </is>
       </c>
     </row>
@@ -19386,9 +19968,15 @@
       <c r="BH100" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="BI100" t="inlineStr">
-        <is>
-          <t>2133</t>
+      <c r="BI100" t="n">
+        <v>2133</v>
+      </c>
+      <c r="BJ100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK100" t="inlineStr">
+        <is>
+          <t>2132</t>
         </is>
       </c>
     </row>
@@ -19579,9 +20167,15 @@
       <c r="BH101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BI101" t="inlineStr">
-        <is>
-          <t>2915</t>
+      <c r="BI101" t="n">
+        <v>2915</v>
+      </c>
+      <c r="BJ101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BK101" t="inlineStr">
+        <is>
+          <t>3295</t>
         </is>
       </c>
     </row>
@@ -19772,9 +20366,15 @@
       <c r="BH102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BI102" t="inlineStr">
-        <is>
-          <t>2770</t>
+      <c r="BI102" t="n">
+        <v>2770</v>
+      </c>
+      <c r="BJ102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK102" t="inlineStr">
+        <is>
+          <t>2786</t>
         </is>
       </c>
     </row>
@@ -19965,9 +20565,15 @@
       <c r="BH103" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="BI103" t="inlineStr">
-        <is>
-          <t>2786</t>
+      <c r="BI103" t="n">
+        <v>2786</v>
+      </c>
+      <c r="BJ103" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BK103" t="inlineStr">
+        <is>
+          <t>3011</t>
         </is>
       </c>
     </row>
@@ -20158,9 +20764,15 @@
       <c r="BH104" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="BI104" t="inlineStr">
-        <is>
-          <t>2945</t>
+      <c r="BI104" t="n">
+        <v>2945</v>
+      </c>
+      <c r="BJ104" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BK104" t="inlineStr">
+        <is>
+          <t>3375</t>
         </is>
       </c>
     </row>
@@ -20351,9 +20963,15 @@
       <c r="BH105" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="BI105" t="inlineStr">
-        <is>
-          <t>2910</t>
+      <c r="BI105" t="n">
+        <v>2910</v>
+      </c>
+      <c r="BJ105" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="BK105" t="inlineStr">
+        <is>
+          <t>3396</t>
         </is>
       </c>
     </row>
@@ -20544,7 +21162,13 @@
       <c r="BH106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI106" t="inlineStr">
+      <c r="BI106" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -20737,9 +21361,15 @@
       <c r="BH107" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="BI107" t="inlineStr">
-        <is>
-          <t>2620</t>
+      <c r="BI107" t="n">
+        <v>2620</v>
+      </c>
+      <c r="BJ107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK107" t="inlineStr">
+        <is>
+          <t>2689</t>
         </is>
       </c>
     </row>
@@ -20930,7 +21560,13 @@
       <c r="BH108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI108" t="inlineStr">
+      <c r="BI108" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -21123,9 +21759,15 @@
       <c r="BH109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI109" t="inlineStr">
-        <is>
-          <t>2550</t>
+      <c r="BI109" t="n">
+        <v>2550</v>
+      </c>
+      <c r="BJ109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK109" t="inlineStr">
+        <is>
+          <t>2635</t>
         </is>
       </c>
     </row>
@@ -21316,9 +21958,15 @@
       <c r="BH110" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BI110" t="inlineStr">
-        <is>
-          <t>2894</t>
+      <c r="BI110" t="n">
+        <v>2894</v>
+      </c>
+      <c r="BJ110" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BK110" t="inlineStr">
+        <is>
+          <t>3081</t>
         </is>
       </c>
     </row>
@@ -21341,7 +21989,7 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F111" s="2" t="n">
@@ -21480,6 +22128,14 @@
       <c r="BG111" t="inlineStr"/>
       <c r="BH111" s="3" t="inlineStr"/>
       <c r="BI111" t="inlineStr"/>
+      <c r="BJ111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK111" t="inlineStr">
+        <is>
+          <t>2573</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -21668,9 +22324,15 @@
       <c r="BH112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI112" t="inlineStr">
-        <is>
-          <t>2509</t>
+      <c r="BI112" t="n">
+        <v>2509</v>
+      </c>
+      <c r="BJ112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK112" t="inlineStr">
+        <is>
+          <t>2526</t>
         </is>
       </c>
     </row>
@@ -21861,9 +22523,15 @@
       <c r="BH113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI113" t="inlineStr">
-        <is>
-          <t>2680</t>
+      <c r="BI113" t="n">
+        <v>2680</v>
+      </c>
+      <c r="BJ113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK113" t="inlineStr">
+        <is>
+          <t>2721</t>
         </is>
       </c>
     </row>
@@ -22054,9 +22722,15 @@
       <c r="BH114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI114" t="inlineStr">
-        <is>
-          <t>2610</t>
+      <c r="BI114" t="n">
+        <v>2610</v>
+      </c>
+      <c r="BJ114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK114" t="inlineStr">
+        <is>
+          <t>2678</t>
         </is>
       </c>
     </row>
@@ -22247,9 +22921,15 @@
       <c r="BH115" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BI115" t="inlineStr">
-        <is>
-          <t>2231</t>
+      <c r="BI115" t="n">
+        <v>2231</v>
+      </c>
+      <c r="BJ115" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="BK115" t="inlineStr">
+        <is>
+          <t>2305</t>
         </is>
       </c>
     </row>
@@ -22440,9 +23120,15 @@
       <c r="BH116" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="BI116" t="inlineStr">
-        <is>
-          <t>2524</t>
+      <c r="BI116" t="n">
+        <v>2524</v>
+      </c>
+      <c r="BJ116" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="BK116" t="inlineStr">
+        <is>
+          <t>2623</t>
         </is>
       </c>
     </row>
@@ -22633,9 +23319,15 @@
       <c r="BH117" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BI117" t="inlineStr">
-        <is>
-          <t>2863</t>
+      <c r="BI117" t="n">
+        <v>2863</v>
+      </c>
+      <c r="BJ117" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BK117" t="inlineStr">
+        <is>
+          <t>3278</t>
         </is>
       </c>
     </row>
@@ -22826,7 +23518,13 @@
       <c r="BH118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI118" t="inlineStr">
+      <c r="BI118" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -23019,9 +23717,15 @@
       <c r="BH119" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="BI119" t="inlineStr">
-        <is>
-          <t>2862</t>
+      <c r="BI119" t="n">
+        <v>2862</v>
+      </c>
+      <c r="BJ119" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="BK119" t="inlineStr">
+        <is>
+          <t>3065</t>
         </is>
       </c>
     </row>
@@ -23212,9 +23916,15 @@
       <c r="BH120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI120" t="inlineStr">
-        <is>
-          <t>2492</t>
+      <c r="BI120" t="n">
+        <v>2492</v>
+      </c>
+      <c r="BJ120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK120" t="inlineStr">
+        <is>
+          <t>2485</t>
         </is>
       </c>
     </row>
@@ -23405,9 +24115,15 @@
       <c r="BH121" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="BI121" t="inlineStr">
-        <is>
-          <t>2728</t>
+      <c r="BI121" t="n">
+        <v>2728</v>
+      </c>
+      <c r="BJ121" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BK121" t="inlineStr">
+        <is>
+          <t>3065</t>
         </is>
       </c>
     </row>
@@ -23598,7 +24314,13 @@
       <c r="BH122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI122" t="inlineStr">
+      <c r="BI122" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -23791,9 +24513,15 @@
       <c r="BH123" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BI123" t="inlineStr">
-        <is>
-          <t>2770</t>
+      <c r="BI123" t="n">
+        <v>2770</v>
+      </c>
+      <c r="BJ123" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="BK123" t="inlineStr">
+        <is>
+          <t>2932</t>
         </is>
       </c>
     </row>
@@ -23984,9 +24712,15 @@
       <c r="BH124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BI124" t="inlineStr">
-        <is>
-          <t>2820</t>
+      <c r="BI124" t="n">
+        <v>2820</v>
+      </c>
+      <c r="BJ124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BK124" t="inlineStr">
+        <is>
+          <t>2985</t>
         </is>
       </c>
     </row>
@@ -24177,9 +24911,15 @@
       <c r="BH125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI125" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="BI125" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ125" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BK125" t="inlineStr">
+        <is>
+          <t>2757</t>
         </is>
       </c>
     </row>
@@ -24370,9 +25110,15 @@
       <c r="BH126" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BI126" t="inlineStr">
-        <is>
-          <t>2887</t>
+      <c r="BI126" t="n">
+        <v>2887</v>
+      </c>
+      <c r="BJ126" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BK126" t="inlineStr">
+        <is>
+          <t>3105</t>
         </is>
       </c>
     </row>
@@ -24563,9 +25309,15 @@
       <c r="BH127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI127" t="inlineStr">
-        <is>
-          <t>1997</t>
+      <c r="BI127" t="n">
+        <v>1997</v>
+      </c>
+      <c r="BJ127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK127" t="inlineStr">
+        <is>
+          <t>2001</t>
         </is>
       </c>
     </row>
@@ -24756,7 +25508,13 @@
       <c r="BH128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI128" t="inlineStr">
+      <c r="BI128" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -24949,7 +25707,13 @@
       <c r="BH129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI129" t="inlineStr">
+      <c r="BI129" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -25142,9 +25906,15 @@
       <c r="BH130" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BI130" t="inlineStr">
-        <is>
-          <t>2752</t>
+      <c r="BI130" t="n">
+        <v>2752</v>
+      </c>
+      <c r="BJ130" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BK130" t="inlineStr">
+        <is>
+          <t>2959</t>
         </is>
       </c>
     </row>
@@ -25335,7 +26105,13 @@
       <c r="BH131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI131" t="inlineStr">
+      <c r="BI131" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -25528,9 +26304,15 @@
       <c r="BH132" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BI132" t="inlineStr">
-        <is>
-          <t>2506</t>
+      <c r="BI132" t="n">
+        <v>2506</v>
+      </c>
+      <c r="BJ132" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BK132" t="inlineStr">
+        <is>
+          <t>2611</t>
         </is>
       </c>
     </row>
@@ -25721,9 +26503,15 @@
       <c r="BH133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI133" t="inlineStr">
-        <is>
-          <t>2513</t>
+      <c r="BI133" t="n">
+        <v>2513</v>
+      </c>
+      <c r="BJ133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK133" t="inlineStr">
+        <is>
+          <t>2528</t>
         </is>
       </c>
     </row>
@@ -25825,6 +26613,8 @@
       <c r="BG134" t="inlineStr"/>
       <c r="BH134" s="3" t="inlineStr"/>
       <c r="BI134" t="inlineStr"/>
+      <c r="BJ134" s="3" t="inlineStr"/>
+      <c r="BK134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -25916,6 +26706,8 @@
       <c r="BG135" t="inlineStr"/>
       <c r="BH135" s="3" t="inlineStr"/>
       <c r="BI135" t="inlineStr"/>
+      <c r="BJ135" s="3" t="inlineStr"/>
+      <c r="BK135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -26104,7 +26896,13 @@
       <c r="BH136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI136" t="inlineStr">
+      <c r="BI136" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK136" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -26297,7 +27095,13 @@
       <c r="BH137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI137" t="inlineStr">
+      <c r="BI137" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -26393,6 +27197,8 @@
       <c r="BG138" t="inlineStr"/>
       <c r="BH138" s="3" t="inlineStr"/>
       <c r="BI138" t="inlineStr"/>
+      <c r="BJ138" s="3" t="inlineStr"/>
+      <c r="BK138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -26581,9 +27387,15 @@
       <c r="BH139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI139" t="inlineStr">
-        <is>
-          <t>2492</t>
+      <c r="BI139" t="n">
+        <v>2492</v>
+      </c>
+      <c r="BJ139" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="BK139" t="inlineStr">
+        <is>
+          <t>2723</t>
         </is>
       </c>
     </row>
@@ -26774,9 +27586,15 @@
       <c r="BH140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI140" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="BI140" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK140" t="inlineStr">
+        <is>
+          <t>2497</t>
         </is>
       </c>
     </row>
@@ -26870,6 +27688,8 @@
       <c r="BG141" t="inlineStr"/>
       <c r="BH141" s="3" t="inlineStr"/>
       <c r="BI141" t="inlineStr"/>
+      <c r="BJ141" s="3" t="inlineStr"/>
+      <c r="BK141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -27058,7 +27878,13 @@
       <c r="BH142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI142" t="inlineStr">
+      <c r="BI142" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK142" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -27154,6 +27980,8 @@
       <c r="BG143" t="inlineStr"/>
       <c r="BH143" s="3" t="inlineStr"/>
       <c r="BI143" t="inlineStr"/>
+      <c r="BJ143" s="3" t="inlineStr"/>
+      <c r="BK143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -27245,6 +28073,8 @@
       <c r="BG144" t="inlineStr"/>
       <c r="BH144" s="3" t="inlineStr"/>
       <c r="BI144" t="inlineStr"/>
+      <c r="BJ144" s="3" t="inlineStr"/>
+      <c r="BK144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -27336,6 +28166,8 @@
       <c r="BG145" t="inlineStr"/>
       <c r="BH145" s="3" t="inlineStr"/>
       <c r="BI145" t="inlineStr"/>
+      <c r="BJ145" s="3" t="inlineStr"/>
+      <c r="BK145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -27427,6 +28259,8 @@
       <c r="BG146" t="inlineStr"/>
       <c r="BH146" s="3" t="inlineStr"/>
       <c r="BI146" t="inlineStr"/>
+      <c r="BJ146" s="3" t="inlineStr"/>
+      <c r="BK146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -27518,6 +28352,8 @@
       <c r="BG147" t="inlineStr"/>
       <c r="BH147" s="3" t="inlineStr"/>
       <c r="BI147" t="inlineStr"/>
+      <c r="BJ147" s="3" t="inlineStr"/>
+      <c r="BK147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -27706,7 +28542,13 @@
       <c r="BH148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI148" t="inlineStr">
+      <c r="BI148" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -27899,7 +28741,13 @@
       <c r="BH149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI149" t="inlineStr">
+      <c r="BI149" t="n">
+        <v>2500</v>
+      </c>
+      <c r="BJ149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK149" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -28092,7 +28940,13 @@
       <c r="BH150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI150" t="inlineStr">
+      <c r="BI150" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -28285,7 +29139,13 @@
       <c r="BH151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI151" t="inlineStr">
+      <c r="BI151" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -28478,7 +29338,13 @@
       <c r="BH152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI152" t="inlineStr">
+      <c r="BI152" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -28671,7 +29537,13 @@
       <c r="BH153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI153" t="inlineStr">
+      <c r="BI153" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -28864,7 +29736,13 @@
       <c r="BH154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI154" t="inlineStr">
+      <c r="BI154" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -29057,9 +29935,15 @@
       <c r="BH155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI155" t="inlineStr">
-        <is>
-          <t>2499</t>
+      <c r="BI155" t="n">
+        <v>2499</v>
+      </c>
+      <c r="BJ155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK155" t="inlineStr">
+        <is>
+          <t>2518</t>
         </is>
       </c>
     </row>
@@ -29244,7 +30128,13 @@
       <c r="BH156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI156" t="inlineStr">
+      <c r="BI156" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -29334,6 +30224,8 @@
       <c r="BG157" t="inlineStr"/>
       <c r="BH157" s="3" t="inlineStr"/>
       <c r="BI157" t="inlineStr"/>
+      <c r="BJ157" s="3" t="inlineStr"/>
+      <c r="BK157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -29516,7 +30408,13 @@
       <c r="BH158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI158" t="inlineStr">
+      <c r="BI158" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -29703,9 +30601,15 @@
       <c r="BH159" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BI159" t="inlineStr">
-        <is>
-          <t>2865</t>
+      <c r="BI159" t="n">
+        <v>2865</v>
+      </c>
+      <c r="BJ159" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BK159" t="inlineStr">
+        <is>
+          <t>3075</t>
         </is>
       </c>
     </row>
@@ -29793,6 +30697,8 @@
       <c r="BG160" t="inlineStr"/>
       <c r="BH160" s="3" t="inlineStr"/>
       <c r="BI160" t="inlineStr"/>
+      <c r="BJ160" s="3" t="inlineStr"/>
+      <c r="BK160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -29963,9 +30869,15 @@
       <c r="BH161" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BI161" t="inlineStr">
-        <is>
-          <t>2945</t>
+      <c r="BI161" t="n">
+        <v>2945</v>
+      </c>
+      <c r="BJ161" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BK161" t="inlineStr">
+        <is>
+          <t>3057</t>
         </is>
       </c>
     </row>
@@ -30138,9 +31050,15 @@
       <c r="BH162" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BI162" t="inlineStr">
-        <is>
-          <t>2745</t>
+      <c r="BI162" t="n">
+        <v>2745</v>
+      </c>
+      <c r="BJ162" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="BK162" t="inlineStr">
+        <is>
+          <t>2809</t>
         </is>
       </c>
     </row>
@@ -30309,9 +31227,15 @@
       <c r="BH163" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI163" t="inlineStr">
-        <is>
-          <t>2494</t>
+      <c r="BI163" t="n">
+        <v>2494</v>
+      </c>
+      <c r="BJ163" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BK163" t="inlineStr">
+        <is>
+          <t>2785</t>
         </is>
       </c>
     </row>
@@ -30464,9 +31388,15 @@
       <c r="BH164" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI164" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="BI164" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ164" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BK164" t="inlineStr">
+        <is>
+          <t>2782</t>
         </is>
       </c>
     </row>
@@ -30623,9 +31553,15 @@
       <c r="BH165" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI165" t="inlineStr">
-        <is>
-          <t>2479</t>
+      <c r="BI165" t="n">
+        <v>2479</v>
+      </c>
+      <c r="BJ165" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="BK165" t="inlineStr">
+        <is>
+          <t>2741</t>
         </is>
       </c>
     </row>
@@ -30774,9 +31710,15 @@
       <c r="BH166" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI166" t="inlineStr">
-        <is>
-          <t>2525</t>
+      <c r="BI166" t="n">
+        <v>2525</v>
+      </c>
+      <c r="BJ166" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK166" t="inlineStr">
+        <is>
+          <t>2538</t>
         </is>
       </c>
     </row>
@@ -30913,7 +31855,13 @@
       <c r="BH167" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI167" t="inlineStr">
+      <c r="BI167" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ167" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK167" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -31048,7 +31996,13 @@
       <c r="BH168" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI168" t="inlineStr">
+      <c r="BI168" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ168" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK168" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -31130,6 +32084,8 @@
       <c r="BG169" t="inlineStr"/>
       <c r="BH169" s="3" t="inlineStr"/>
       <c r="BI169" t="inlineStr"/>
+      <c r="BJ169" s="3" t="inlineStr"/>
+      <c r="BK169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="n">
@@ -31256,9 +32212,15 @@
       <c r="BH170" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI170" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="BI170" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ170" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="BK170" t="inlineStr">
+        <is>
+          <t>1527</t>
         </is>
       </c>
     </row>
@@ -31375,9 +32337,15 @@
       <c r="BH171" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI171" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="BI171" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ171" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK171" t="inlineStr">
+        <is>
+          <t>1500</t>
         </is>
       </c>
     </row>
@@ -31494,7 +32462,13 @@
       <c r="BH172" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI172" t="inlineStr">
+      <c r="BI172" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ172" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK172" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -31613,9 +32587,15 @@
       <c r="BH173" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI173" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="BI173" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ173" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BK173" t="inlineStr">
+        <is>
+          <t>1784</t>
         </is>
       </c>
     </row>
@@ -31707,6 +32687,8 @@
       </c>
       <c r="BH174" s="3" t="inlineStr"/>
       <c r="BI174" t="inlineStr"/>
+      <c r="BJ174" s="3" t="inlineStr"/>
+      <c r="BK174" t="inlineStr"/>
     </row>
     <row r="175">
       <c r="A175" t="n">
@@ -31785,17 +32767,21 @@
       <c r="BH175" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="BI175" t="inlineStr">
-        <is>
-          <t>2847</t>
+      <c r="BI175" t="n">
+        <v>2847</v>
+      </c>
+      <c r="BJ175" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="BK175" t="inlineStr">
+        <is>
+          <t>2994</t>
         </is>
       </c>
     </row>
     <row r="176">
-      <c r="A176" t="inlineStr">
-        <is>
-          <t>55317038</t>
-        </is>
+      <c r="A176" t="n">
+        <v>55317038</v>
       </c>
       <c r="B176" t="inlineStr">
         <is>
@@ -31866,17 +32852,21 @@
       <c r="BH176" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BI176" t="inlineStr">
-        <is>
-          <t>2964</t>
+      <c r="BI176" t="n">
+        <v>2964</v>
+      </c>
+      <c r="BJ176" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BK176" t="inlineStr">
+        <is>
+          <t>3299</t>
         </is>
       </c>
     </row>
     <row r="177">
-      <c r="A177" t="inlineStr">
-        <is>
-          <t>56829330</t>
-        </is>
+      <c r="A177" t="n">
+        <v>56829330</v>
       </c>
       <c r="B177" t="inlineStr">
         <is>
@@ -31947,17 +32937,21 @@
       <c r="BH177" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="BI177" t="inlineStr">
-        <is>
-          <t>2900</t>
+      <c r="BI177" t="n">
+        <v>2900</v>
+      </c>
+      <c r="BJ177" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="BK177" t="inlineStr">
+        <is>
+          <t>3083</t>
         </is>
       </c>
     </row>
     <row r="178">
-      <c r="A178" t="inlineStr">
-        <is>
-          <t>48738257</t>
-        </is>
+      <c r="A178" t="n">
+        <v>48738257</v>
       </c>
       <c r="B178" t="inlineStr">
         <is>
@@ -32028,9 +33022,15 @@
       <c r="BH178" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BI178" t="inlineStr">
-        <is>
-          <t>2559</t>
+      <c r="BI178" t="n">
+        <v>2559</v>
+      </c>
+      <c r="BJ178" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK178" t="inlineStr">
+        <is>
+          <t>2744</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-03-15 11:30:37
</commit_message>
<xml_diff>
--- a/Season_Attack/84.xlsx
+++ b/Season_Attack/84.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BK178"/>
+  <dimension ref="A1:BM178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -706,6 +706,16 @@
           <t>03-13_0</t>
         </is>
       </c>
+      <c r="BL1" s="1" t="inlineStr">
+        <is>
+          <t>03-14_A</t>
+        </is>
+      </c>
+      <c r="BM1" s="1" t="inlineStr">
+        <is>
+          <t>03-14_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -900,9 +910,15 @@
       <c r="BJ2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK2" t="inlineStr">
-        <is>
-          <t>2517</t>
+      <c r="BK2" t="n">
+        <v>2517</v>
+      </c>
+      <c r="BL2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM2" t="inlineStr">
+        <is>
+          <t>2558</t>
         </is>
       </c>
     </row>
@@ -1099,9 +1115,15 @@
       <c r="BJ3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BK3" t="inlineStr">
-        <is>
-          <t>3335</t>
+      <c r="BK3" t="n">
+        <v>3335</v>
+      </c>
+      <c r="BL3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM3" t="inlineStr">
+        <is>
+          <t>3705</t>
         </is>
       </c>
     </row>
@@ -1298,9 +1320,15 @@
       <c r="BJ4" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="BK4" t="inlineStr">
-        <is>
-          <t>3562</t>
+      <c r="BK4" t="n">
+        <v>3562</v>
+      </c>
+      <c r="BL4" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="BM4" t="inlineStr">
+        <is>
+          <t>4068</t>
         </is>
       </c>
     </row>
@@ -1497,9 +1525,15 @@
       <c r="BJ5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BK5" t="inlineStr">
-        <is>
-          <t>3277</t>
+      <c r="BK5" t="n">
+        <v>3277</v>
+      </c>
+      <c r="BL5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM5" t="inlineStr">
+        <is>
+          <t>3670</t>
         </is>
       </c>
     </row>
@@ -1696,9 +1730,15 @@
       <c r="BJ6" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BK6" t="inlineStr">
-        <is>
-          <t>3200</t>
+      <c r="BK6" t="n">
+        <v>3200</v>
+      </c>
+      <c r="BL6" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM6" t="inlineStr">
+        <is>
+          <t>3600</t>
         </is>
       </c>
     </row>
@@ -1895,9 +1935,15 @@
       <c r="BJ7" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="BK7" t="inlineStr">
-        <is>
-          <t>3417</t>
+      <c r="BK7" t="n">
+        <v>3417</v>
+      </c>
+      <c r="BL7" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="BM7" t="inlineStr">
+        <is>
+          <t>3934</t>
         </is>
       </c>
     </row>
@@ -2094,9 +2140,15 @@
       <c r="BJ8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BK8" t="inlineStr">
-        <is>
-          <t>3123</t>
+      <c r="BK8" t="n">
+        <v>3123</v>
+      </c>
+      <c r="BL8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM8" t="inlineStr">
+        <is>
+          <t>3482</t>
         </is>
       </c>
     </row>
@@ -2293,9 +2345,15 @@
       <c r="BJ9" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BK9" t="inlineStr">
-        <is>
-          <t>3655</t>
+      <c r="BK9" t="n">
+        <v>3655</v>
+      </c>
+      <c r="BL9" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BM9" t="inlineStr">
+        <is>
+          <t>3992</t>
         </is>
       </c>
     </row>
@@ -2492,9 +2550,15 @@
       <c r="BJ10" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BK10" t="inlineStr">
-        <is>
-          <t>3419</t>
+      <c r="BK10" t="n">
+        <v>3419</v>
+      </c>
+      <c r="BL10" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BM10" t="inlineStr">
+        <is>
+          <t>3804</t>
         </is>
       </c>
     </row>
@@ -2691,9 +2755,15 @@
       <c r="BJ11" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BK11" t="inlineStr">
-        <is>
-          <t>3122</t>
+      <c r="BK11" t="n">
+        <v>3122</v>
+      </c>
+      <c r="BL11" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM11" t="inlineStr">
+        <is>
+          <t>3442</t>
         </is>
       </c>
     </row>
@@ -2890,9 +2960,15 @@
       <c r="BJ12" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="BK12" t="inlineStr">
-        <is>
-          <t>2719</t>
+      <c r="BK12" t="n">
+        <v>2719</v>
+      </c>
+      <c r="BL12" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="BM12" t="inlineStr">
+        <is>
+          <t>2815</t>
         </is>
       </c>
     </row>
@@ -3089,9 +3165,15 @@
       <c r="BJ13" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BK13" t="inlineStr">
-        <is>
-          <t>3643</t>
+      <c r="BK13" t="n">
+        <v>3643</v>
+      </c>
+      <c r="BL13" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="BM13" t="inlineStr">
+        <is>
+          <t>4287</t>
         </is>
       </c>
     </row>
@@ -3288,9 +3370,15 @@
       <c r="BJ14" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BK14" t="inlineStr">
-        <is>
-          <t>3224</t>
+      <c r="BK14" t="n">
+        <v>3224</v>
+      </c>
+      <c r="BL14" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="BM14" t="inlineStr">
+        <is>
+          <t>3592</t>
         </is>
       </c>
     </row>
@@ -3487,7 +3575,13 @@
       <c r="BJ15" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK15" t="inlineStr">
+      <c r="BK15" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM15" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3686,9 +3780,15 @@
       <c r="BJ16" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="BK16" t="inlineStr">
-        <is>
-          <t>3440</t>
+      <c r="BK16" t="n">
+        <v>3440</v>
+      </c>
+      <c r="BL16" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="BM16" t="inlineStr">
+        <is>
+          <t>3890</t>
         </is>
       </c>
     </row>
@@ -3885,9 +3985,15 @@
       <c r="BJ17" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="BK17" t="inlineStr">
-        <is>
-          <t>3261</t>
+      <c r="BK17" t="n">
+        <v>3261</v>
+      </c>
+      <c r="BL17" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="BM17" t="inlineStr">
+        <is>
+          <t>3548</t>
         </is>
       </c>
     </row>
@@ -4084,9 +4190,15 @@
       <c r="BJ18" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="BK18" t="inlineStr">
-        <is>
-          <t>3247</t>
+      <c r="BK18" t="n">
+        <v>3247</v>
+      </c>
+      <c r="BL18" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="BM18" t="inlineStr">
+        <is>
+          <t>3595</t>
         </is>
       </c>
     </row>
@@ -4283,9 +4395,15 @@
       <c r="BJ19" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BK19" t="inlineStr">
-        <is>
-          <t>3119</t>
+      <c r="BK19" t="n">
+        <v>3119</v>
+      </c>
+      <c r="BL19" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM19" t="inlineStr">
+        <is>
+          <t>3446</t>
         </is>
       </c>
     </row>
@@ -4482,9 +4600,15 @@
       <c r="BJ20" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="BK20" t="inlineStr">
-        <is>
-          <t>3598</t>
+      <c r="BK20" t="n">
+        <v>3598</v>
+      </c>
+      <c r="BL20" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BM20" t="inlineStr">
+        <is>
+          <t>4152</t>
         </is>
       </c>
     </row>
@@ -4681,7 +4805,13 @@
       <c r="BJ21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK21" t="inlineStr">
+      <c r="BK21" t="n">
+        <v>2816</v>
+      </c>
+      <c r="BL21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM21" t="inlineStr">
         <is>
           <t>2816</t>
         </is>
@@ -4880,9 +5010,15 @@
       <c r="BJ22" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="BK22" t="inlineStr">
-        <is>
-          <t>3570</t>
+      <c r="BK22" t="n">
+        <v>3570</v>
+      </c>
+      <c r="BL22" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BM22" t="inlineStr">
+        <is>
+          <t>3974</t>
         </is>
       </c>
     </row>
@@ -5079,9 +5215,15 @@
       <c r="BJ23" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK23" t="inlineStr">
-        <is>
-          <t>2903</t>
+      <c r="BK23" t="n">
+        <v>2903</v>
+      </c>
+      <c r="BL23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM23" t="inlineStr">
+        <is>
+          <t>2927</t>
         </is>
       </c>
     </row>
@@ -5278,9 +5420,15 @@
       <c r="BJ24" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BK24" t="inlineStr">
-        <is>
-          <t>3570</t>
+      <c r="BK24" t="n">
+        <v>3570</v>
+      </c>
+      <c r="BL24" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="BM24" t="inlineStr">
+        <is>
+          <t>4022</t>
         </is>
       </c>
     </row>
@@ -5477,7 +5625,13 @@
       <c r="BJ25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK25" t="inlineStr">
+      <c r="BK25" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5676,7 +5830,13 @@
       <c r="BJ26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK26" t="inlineStr">
+      <c r="BK26" t="n">
+        <v>2572</v>
+      </c>
+      <c r="BL26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM26" t="inlineStr">
         <is>
           <t>2572</t>
         </is>
@@ -5875,9 +6035,15 @@
       <c r="BJ27" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="BK27" t="inlineStr">
-        <is>
-          <t>3513</t>
+      <c r="BK27" t="n">
+        <v>3513</v>
+      </c>
+      <c r="BL27" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="BM27" t="inlineStr">
+        <is>
+          <t>3923</t>
         </is>
       </c>
     </row>
@@ -6074,9 +6240,15 @@
       <c r="BJ28" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="BK28" t="inlineStr">
-        <is>
-          <t>3513</t>
+      <c r="BK28" t="n">
+        <v>3513</v>
+      </c>
+      <c r="BL28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="BM28" t="inlineStr">
+        <is>
+          <t>3995</t>
         </is>
       </c>
     </row>
@@ -6273,9 +6445,15 @@
       <c r="BJ29" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BK29" t="inlineStr">
-        <is>
-          <t>3792</t>
+      <c r="BK29" t="n">
+        <v>3792</v>
+      </c>
+      <c r="BL29" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BM29" t="inlineStr">
+        <is>
+          <t>4370</t>
         </is>
       </c>
     </row>
@@ -6472,9 +6650,15 @@
       <c r="BJ30" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BK30" t="inlineStr">
-        <is>
-          <t>2861</t>
+      <c r="BK30" t="n">
+        <v>2861</v>
+      </c>
+      <c r="BL30" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BM30" t="inlineStr">
+        <is>
+          <t>3154</t>
         </is>
       </c>
     </row>
@@ -6671,9 +6855,15 @@
       <c r="BJ31" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="BK31" t="inlineStr">
-        <is>
-          <t>3429</t>
+      <c r="BK31" t="n">
+        <v>3429</v>
+      </c>
+      <c r="BL31" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="BM31" t="inlineStr">
+        <is>
+          <t>4032</t>
         </is>
       </c>
     </row>
@@ -6870,9 +7060,15 @@
       <c r="BJ32" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="BK32" t="inlineStr">
-        <is>
-          <t>3355</t>
+      <c r="BK32" t="n">
+        <v>3355</v>
+      </c>
+      <c r="BL32" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="BM32" t="inlineStr">
+        <is>
+          <t>3736</t>
         </is>
       </c>
     </row>
@@ -7069,9 +7265,15 @@
       <c r="BJ33" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK33" t="inlineStr">
-        <is>
-          <t>2834</t>
+      <c r="BK33" t="n">
+        <v>2834</v>
+      </c>
+      <c r="BL33" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="BM33" t="inlineStr">
+        <is>
+          <t>3117</t>
         </is>
       </c>
     </row>
@@ -7268,9 +7470,15 @@
       <c r="BJ34" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BK34" t="inlineStr">
-        <is>
-          <t>3403</t>
+      <c r="BK34" t="n">
+        <v>3403</v>
+      </c>
+      <c r="BL34" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BM34" t="inlineStr">
+        <is>
+          <t>3883</t>
         </is>
       </c>
     </row>
@@ -7467,9 +7675,15 @@
       <c r="BJ35" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BK35" t="inlineStr">
-        <is>
-          <t>3420</t>
+      <c r="BK35" t="n">
+        <v>3420</v>
+      </c>
+      <c r="BL35" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BM35" t="inlineStr">
+        <is>
+          <t>3848</t>
         </is>
       </c>
     </row>
@@ -7666,9 +7880,15 @@
       <c r="BJ36" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="BK36" t="inlineStr">
-        <is>
-          <t>2986</t>
+      <c r="BK36" t="n">
+        <v>2986</v>
+      </c>
+      <c r="BL36" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM36" t="inlineStr">
+        <is>
+          <t>3462</t>
         </is>
       </c>
     </row>
@@ -7865,9 +8085,15 @@
       <c r="BJ37" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BK37" t="inlineStr">
-        <is>
-          <t>3329</t>
+      <c r="BK37" t="n">
+        <v>3329</v>
+      </c>
+      <c r="BL37" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BM37" t="inlineStr">
+        <is>
+          <t>3586</t>
         </is>
       </c>
     </row>
@@ -8064,9 +8290,15 @@
       <c r="BJ38" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BK38" t="inlineStr">
-        <is>
-          <t>3396</t>
+      <c r="BK38" t="n">
+        <v>3396</v>
+      </c>
+      <c r="BL38" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BM38" t="inlineStr">
+        <is>
+          <t>3869</t>
         </is>
       </c>
     </row>
@@ -8263,9 +8495,15 @@
       <c r="BJ39" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="BK39" t="inlineStr">
-        <is>
-          <t>3597</t>
+      <c r="BK39" t="n">
+        <v>3597</v>
+      </c>
+      <c r="BL39" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="BM39" t="inlineStr">
+        <is>
+          <t>3990</t>
         </is>
       </c>
     </row>
@@ -8462,9 +8700,15 @@
       <c r="BJ40" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BK40" t="inlineStr">
-        <is>
-          <t>3353</t>
+      <c r="BK40" t="n">
+        <v>3353</v>
+      </c>
+      <c r="BL40" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BM40" t="inlineStr">
+        <is>
+          <t>3857</t>
         </is>
       </c>
     </row>
@@ -8661,7 +8905,13 @@
       <c r="BJ41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK41" t="inlineStr">
+      <c r="BK41" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM41" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8860,9 +9110,15 @@
       <c r="BJ42" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="BK42" t="inlineStr">
-        <is>
-          <t>3708</t>
+      <c r="BK42" t="n">
+        <v>3708</v>
+      </c>
+      <c r="BL42" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="BM42" t="inlineStr">
+        <is>
+          <t>4208</t>
         </is>
       </c>
     </row>
@@ -9059,9 +9315,15 @@
       <c r="BJ43" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BK43" t="inlineStr">
-        <is>
-          <t>3593</t>
+      <c r="BK43" t="n">
+        <v>3593</v>
+      </c>
+      <c r="BL43" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BM43" t="inlineStr">
+        <is>
+          <t>4054</t>
         </is>
       </c>
     </row>
@@ -9258,9 +9520,15 @@
       <c r="BJ44" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BK44" t="inlineStr">
-        <is>
-          <t>3776</t>
+      <c r="BK44" t="n">
+        <v>3776</v>
+      </c>
+      <c r="BL44" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BM44" t="inlineStr">
+        <is>
+          <t>3988</t>
         </is>
       </c>
     </row>
@@ -9457,9 +9725,15 @@
       <c r="BJ45" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="BK45" t="inlineStr">
-        <is>
-          <t>3219</t>
+      <c r="BK45" t="n">
+        <v>3219</v>
+      </c>
+      <c r="BL45" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="BM45" t="inlineStr">
+        <is>
+          <t>3569</t>
         </is>
       </c>
     </row>
@@ -9656,9 +9930,15 @@
       <c r="BJ46" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BK46" t="inlineStr">
-        <is>
-          <t>3163</t>
+      <c r="BK46" t="n">
+        <v>3163</v>
+      </c>
+      <c r="BL46" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM46" t="inlineStr">
+        <is>
+          <t>3473</t>
         </is>
       </c>
     </row>
@@ -9855,9 +10135,15 @@
       <c r="BJ47" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BK47" t="inlineStr">
-        <is>
-          <t>3144</t>
+      <c r="BK47" t="n">
+        <v>3144</v>
+      </c>
+      <c r="BL47" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="BM47" t="inlineStr">
+        <is>
+          <t>3553</t>
         </is>
       </c>
     </row>
@@ -10054,9 +10340,15 @@
       <c r="BJ48" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="BK48" t="inlineStr">
-        <is>
-          <t>3686</t>
+      <c r="BK48" t="n">
+        <v>3686</v>
+      </c>
+      <c r="BL48" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="BM48" t="inlineStr">
+        <is>
+          <t>4107</t>
         </is>
       </c>
     </row>
@@ -10253,9 +10545,15 @@
       <c r="BJ49" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="BK49" t="inlineStr">
-        <is>
-          <t>3055</t>
+      <c r="BK49" t="n">
+        <v>3055</v>
+      </c>
+      <c r="BL49" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM49" t="inlineStr">
+        <is>
+          <t>3302</t>
         </is>
       </c>
     </row>
@@ -10452,7 +10750,13 @@
       <c r="BJ50" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK50" t="inlineStr">
+      <c r="BK50" t="n">
+        <v>2500</v>
+      </c>
+      <c r="BL50" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM50" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -10651,7 +10955,13 @@
       <c r="BJ51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK51" t="inlineStr">
+      <c r="BK51" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM51" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10850,7 +11160,13 @@
       <c r="BJ52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK52" t="inlineStr">
+      <c r="BK52" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM52" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11049,9 +11365,15 @@
       <c r="BJ53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK53" t="inlineStr">
-        <is>
-          <t>2718</t>
+      <c r="BK53" t="n">
+        <v>2718</v>
+      </c>
+      <c r="BL53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM53" t="inlineStr">
+        <is>
+          <t>2742</t>
         </is>
       </c>
     </row>
@@ -11248,9 +11570,15 @@
       <c r="BJ54" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="BK54" t="inlineStr">
-        <is>
-          <t>3341</t>
+      <c r="BK54" t="n">
+        <v>3341</v>
+      </c>
+      <c r="BL54" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="BM54" t="inlineStr">
+        <is>
+          <t>3739</t>
         </is>
       </c>
     </row>
@@ -11447,9 +11775,15 @@
       <c r="BJ55" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BK55" t="inlineStr">
-        <is>
-          <t>3361</t>
+      <c r="BK55" t="n">
+        <v>3361</v>
+      </c>
+      <c r="BL55" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BM55" t="inlineStr">
+        <is>
+          <t>3587</t>
         </is>
       </c>
     </row>
@@ -11646,9 +11980,15 @@
       <c r="BJ56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BK56" t="inlineStr">
-        <is>
-          <t>3104</t>
+      <c r="BK56" t="n">
+        <v>3104</v>
+      </c>
+      <c r="BL56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM56" t="inlineStr">
+        <is>
+          <t>3437</t>
         </is>
       </c>
     </row>
@@ -11845,9 +12185,15 @@
       <c r="BJ57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BK57" t="inlineStr">
-        <is>
-          <t>3187</t>
+      <c r="BK57" t="n">
+        <v>3187</v>
+      </c>
+      <c r="BL57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM57" t="inlineStr">
+        <is>
+          <t>3534</t>
         </is>
       </c>
     </row>
@@ -12044,9 +12390,15 @@
       <c r="BJ58" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="BK58" t="inlineStr">
-        <is>
-          <t>3397</t>
+      <c r="BK58" t="n">
+        <v>3397</v>
+      </c>
+      <c r="BL58" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BM58" t="inlineStr">
+        <is>
+          <t>3718</t>
         </is>
       </c>
     </row>
@@ -12126,6 +12478,8 @@
       <c r="BI59" t="inlineStr"/>
       <c r="BJ59" s="3" t="inlineStr"/>
       <c r="BK59" t="inlineStr"/>
+      <c r="BL59" s="3" t="inlineStr"/>
+      <c r="BM59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -12203,6 +12557,8 @@
       <c r="BI60" t="inlineStr"/>
       <c r="BJ60" s="3" t="inlineStr"/>
       <c r="BK60" t="inlineStr"/>
+      <c r="BL60" s="3" t="inlineStr"/>
+      <c r="BM60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -12397,9 +12753,15 @@
       <c r="BJ61" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BK61" t="inlineStr">
-        <is>
-          <t>3328</t>
+      <c r="BK61" t="n">
+        <v>3328</v>
+      </c>
+      <c r="BL61" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BM61" t="inlineStr">
+        <is>
+          <t>3699</t>
         </is>
       </c>
     </row>
@@ -12596,7 +12958,13 @@
       <c r="BJ62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK62" t="inlineStr">
+      <c r="BK62" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12795,9 +13163,15 @@
       <c r="BJ63" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BK63" t="inlineStr">
-        <is>
-          <t>3299</t>
+      <c r="BK63" t="n">
+        <v>3299</v>
+      </c>
+      <c r="BL63" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="BM63" t="inlineStr">
+        <is>
+          <t>3707</t>
         </is>
       </c>
     </row>
@@ -12994,9 +13368,15 @@
       <c r="BJ64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK64" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="BK64" t="n">
+        <v>2500</v>
+      </c>
+      <c r="BL64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM64" t="inlineStr">
+        <is>
+          <t>2499</t>
         </is>
       </c>
     </row>
@@ -13076,6 +13456,8 @@
       <c r="BI65" t="inlineStr"/>
       <c r="BJ65" s="3" t="inlineStr"/>
       <c r="BK65" t="inlineStr"/>
+      <c r="BL65" s="3" t="inlineStr"/>
+      <c r="BM65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -13270,9 +13652,15 @@
       <c r="BJ66" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="BK66" t="inlineStr">
-        <is>
-          <t>2775</t>
+      <c r="BK66" t="n">
+        <v>2775</v>
+      </c>
+      <c r="BL66" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="BM66" t="inlineStr">
+        <is>
+          <t>2978</t>
         </is>
       </c>
     </row>
@@ -13469,9 +13857,15 @@
       <c r="BJ67" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BK67" t="inlineStr">
-        <is>
-          <t>3183</t>
+      <c r="BK67" t="n">
+        <v>3183</v>
+      </c>
+      <c r="BL67" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BM67" t="inlineStr">
+        <is>
+          <t>3506</t>
         </is>
       </c>
     </row>
@@ -13668,9 +14062,15 @@
       <c r="BJ68" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BK68" t="inlineStr">
-        <is>
-          <t>3383</t>
+      <c r="BK68" t="n">
+        <v>3383</v>
+      </c>
+      <c r="BL68" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BM68" t="inlineStr">
+        <is>
+          <t>3766</t>
         </is>
       </c>
     </row>
@@ -13867,9 +14267,15 @@
       <c r="BJ69" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BK69" t="inlineStr">
-        <is>
-          <t>3433</t>
+      <c r="BK69" t="n">
+        <v>3433</v>
+      </c>
+      <c r="BL69" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="BM69" t="inlineStr">
+        <is>
+          <t>3828</t>
         </is>
       </c>
     </row>
@@ -14066,9 +14472,15 @@
       <c r="BJ70" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="BK70" t="inlineStr">
-        <is>
-          <t>2609</t>
+      <c r="BK70" t="n">
+        <v>2609</v>
+      </c>
+      <c r="BL70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM70" t="inlineStr">
+        <is>
+          <t>2624</t>
         </is>
       </c>
     </row>
@@ -14265,9 +14677,15 @@
       <c r="BJ71" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BK71" t="inlineStr">
-        <is>
-          <t>3203</t>
+      <c r="BK71" t="n">
+        <v>3203</v>
+      </c>
+      <c r="BL71" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM71" t="inlineStr">
+        <is>
+          <t>3479</t>
         </is>
       </c>
     </row>
@@ -14464,9 +14882,15 @@
       <c r="BJ72" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="BK72" t="inlineStr">
-        <is>
-          <t>3019</t>
+      <c r="BK72" t="n">
+        <v>3019</v>
+      </c>
+      <c r="BL72" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="BM72" t="inlineStr">
+        <is>
+          <t>3461</t>
         </is>
       </c>
     </row>
@@ -14663,9 +15087,15 @@
       <c r="BJ73" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BK73" t="inlineStr">
-        <is>
-          <t>3060</t>
+      <c r="BK73" t="n">
+        <v>3060</v>
+      </c>
+      <c r="BL73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM73" t="inlineStr">
+        <is>
+          <t>3364</t>
         </is>
       </c>
     </row>
@@ -14862,9 +15292,15 @@
       <c r="BJ74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK74" t="inlineStr">
-        <is>
-          <t>2585</t>
+      <c r="BK74" t="n">
+        <v>2585</v>
+      </c>
+      <c r="BL74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM74" t="inlineStr">
+        <is>
+          <t>2628</t>
         </is>
       </c>
     </row>
@@ -15061,9 +15497,15 @@
       <c r="BJ75" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BK75" t="inlineStr">
-        <is>
-          <t>3153</t>
+      <c r="BK75" t="n">
+        <v>3153</v>
+      </c>
+      <c r="BL75" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BM75" t="inlineStr">
+        <is>
+          <t>3488</t>
         </is>
       </c>
     </row>
@@ -15260,9 +15702,15 @@
       <c r="BJ76" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BK76" t="inlineStr">
-        <is>
-          <t>3295</t>
+      <c r="BK76" t="n">
+        <v>3295</v>
+      </c>
+      <c r="BL76" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BM76" t="inlineStr">
+        <is>
+          <t>3641</t>
         </is>
       </c>
     </row>
@@ -15459,7 +15907,13 @@
       <c r="BJ77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK77" t="inlineStr">
+      <c r="BK77" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM77" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15658,9 +16112,15 @@
       <c r="BJ78" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BK78" t="inlineStr">
-        <is>
-          <t>3606</t>
+      <c r="BK78" t="n">
+        <v>3606</v>
+      </c>
+      <c r="BL78" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BM78" t="inlineStr">
+        <is>
+          <t>3985</t>
         </is>
       </c>
     </row>
@@ -15857,7 +16317,13 @@
       <c r="BJ79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK79" t="inlineStr">
+      <c r="BK79" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16056,9 +16522,15 @@
       <c r="BJ80" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="BK80" t="inlineStr">
-        <is>
-          <t>3366</t>
+      <c r="BK80" t="n">
+        <v>3366</v>
+      </c>
+      <c r="BL80" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="BM80" t="inlineStr">
+        <is>
+          <t>3805</t>
         </is>
       </c>
     </row>
@@ -16255,9 +16727,15 @@
       <c r="BJ81" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BK81" t="inlineStr">
-        <is>
-          <t>3631</t>
+      <c r="BK81" t="n">
+        <v>3631</v>
+      </c>
+      <c r="BL81" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="BM81" t="inlineStr">
+        <is>
+          <t>3998</t>
         </is>
       </c>
     </row>
@@ -16454,9 +16932,15 @@
       <c r="BJ82" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BK82" t="inlineStr">
-        <is>
-          <t>3257</t>
+      <c r="BK82" t="n">
+        <v>3257</v>
+      </c>
+      <c r="BL82" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BM82" t="inlineStr">
+        <is>
+          <t>3755</t>
         </is>
       </c>
     </row>
@@ -16653,9 +17137,15 @@
       <c r="BJ83" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BK83" t="inlineStr">
-        <is>
-          <t>3348</t>
+      <c r="BK83" t="n">
+        <v>3348</v>
+      </c>
+      <c r="BL83" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BM83" t="inlineStr">
+        <is>
+          <t>3858</t>
         </is>
       </c>
     </row>
@@ -16795,6 +17285,8 @@
       <c r="BI84" t="inlineStr"/>
       <c r="BJ84" s="3" t="inlineStr"/>
       <c r="BK84" t="inlineStr"/>
+      <c r="BL84" s="3" t="inlineStr"/>
+      <c r="BM84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -16989,9 +17481,15 @@
       <c r="BJ85" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BK85" t="inlineStr">
-        <is>
-          <t>3125</t>
+      <c r="BK85" t="n">
+        <v>3125</v>
+      </c>
+      <c r="BL85" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM85" t="inlineStr">
+        <is>
+          <t>3520</t>
         </is>
       </c>
     </row>
@@ -17188,9 +17686,15 @@
       <c r="BJ86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK86" t="inlineStr">
-        <is>
-          <t>2551</t>
+      <c r="BK86" t="n">
+        <v>2551</v>
+      </c>
+      <c r="BL86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM86" t="inlineStr">
+        <is>
+          <t>2613</t>
         </is>
       </c>
     </row>
@@ -17387,9 +17891,15 @@
       <c r="BJ87" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BK87" t="inlineStr">
-        <is>
-          <t>3692</t>
+      <c r="BK87" t="n">
+        <v>3692</v>
+      </c>
+      <c r="BL87" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="BM87" t="inlineStr">
+        <is>
+          <t>4099</t>
         </is>
       </c>
     </row>
@@ -17586,9 +18096,15 @@
       <c r="BJ88" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BK88" t="inlineStr">
-        <is>
-          <t>2832</t>
+      <c r="BK88" t="n">
+        <v>2832</v>
+      </c>
+      <c r="BL88" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM88" t="inlineStr">
+        <is>
+          <t>2928</t>
         </is>
       </c>
     </row>
@@ -17785,9 +18301,15 @@
       <c r="BJ89" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BK89" t="inlineStr">
-        <is>
-          <t>3043</t>
+      <c r="BK89" t="n">
+        <v>3043</v>
+      </c>
+      <c r="BL89" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BM89" t="inlineStr">
+        <is>
+          <t>3199</t>
         </is>
       </c>
     </row>
@@ -17984,9 +18506,15 @@
       <c r="BJ90" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="BK90" t="inlineStr">
-        <is>
-          <t>2664</t>
+      <c r="BK90" t="n">
+        <v>2664</v>
+      </c>
+      <c r="BL90" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="BM90" t="inlineStr">
+        <is>
+          <t>2834</t>
         </is>
       </c>
     </row>
@@ -18183,9 +18711,15 @@
       <c r="BJ91" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BK91" t="inlineStr">
-        <is>
-          <t>2807</t>
+      <c r="BK91" t="n">
+        <v>2807</v>
+      </c>
+      <c r="BL91" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BM91" t="inlineStr">
+        <is>
+          <t>3023</t>
         </is>
       </c>
     </row>
@@ -18382,7 +18916,13 @@
       <c r="BJ92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK92" t="inlineStr">
+      <c r="BK92" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18581,9 +19121,15 @@
       <c r="BJ93" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BK93" t="inlineStr">
-        <is>
-          <t>2597</t>
+      <c r="BK93" t="n">
+        <v>2597</v>
+      </c>
+      <c r="BL93" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM93" t="inlineStr">
+        <is>
+          <t>2920</t>
         </is>
       </c>
     </row>
@@ -18780,7 +19326,13 @@
       <c r="BJ94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK94" t="inlineStr">
+      <c r="BK94" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18979,9 +19531,15 @@
       <c r="BJ95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK95" t="inlineStr">
-        <is>
-          <t>2494</t>
+      <c r="BK95" t="n">
+        <v>2494</v>
+      </c>
+      <c r="BL95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM95" t="inlineStr">
+        <is>
+          <t>2493</t>
         </is>
       </c>
     </row>
@@ -19178,9 +19736,15 @@
       <c r="BJ96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK96" t="inlineStr">
-        <is>
-          <t>2026</t>
+      <c r="BK96" t="n">
+        <v>2026</v>
+      </c>
+      <c r="BL96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM96" t="inlineStr">
+        <is>
+          <t>2063</t>
         </is>
       </c>
     </row>
@@ -19377,7 +19941,13 @@
       <c r="BJ97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK97" t="inlineStr">
+      <c r="BK97" t="n">
+        <v>2496</v>
+      </c>
+      <c r="BL97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM97" t="inlineStr">
         <is>
           <t>2496</t>
         </is>
@@ -19576,9 +20146,15 @@
       <c r="BJ98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK98" t="inlineStr">
-        <is>
-          <t>2499</t>
+      <c r="BK98" t="n">
+        <v>2499</v>
+      </c>
+      <c r="BL98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM98" t="inlineStr">
+        <is>
+          <t>2511</t>
         </is>
       </c>
     </row>
@@ -19775,9 +20351,15 @@
       <c r="BJ99" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="BK99" t="inlineStr">
-        <is>
-          <t>2577</t>
+      <c r="BK99" t="n">
+        <v>2577</v>
+      </c>
+      <c r="BL99" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="BM99" t="inlineStr">
+        <is>
+          <t>2760</t>
         </is>
       </c>
     </row>
@@ -19974,9 +20556,15 @@
       <c r="BJ100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK100" t="inlineStr">
-        <is>
-          <t>2132</t>
+      <c r="BK100" t="n">
+        <v>2132</v>
+      </c>
+      <c r="BL100" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="BM100" t="inlineStr">
+        <is>
+          <t>2224</t>
         </is>
       </c>
     </row>
@@ -20173,9 +20761,15 @@
       <c r="BJ101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BK101" t="inlineStr">
-        <is>
-          <t>3295</t>
+      <c r="BK101" t="n">
+        <v>3295</v>
+      </c>
+      <c r="BL101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BM101" t="inlineStr">
+        <is>
+          <t>3638</t>
         </is>
       </c>
     </row>
@@ -20372,9 +20966,15 @@
       <c r="BJ102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK102" t="inlineStr">
-        <is>
-          <t>2786</t>
+      <c r="BK102" t="n">
+        <v>2786</v>
+      </c>
+      <c r="BL102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM102" t="inlineStr">
+        <is>
+          <t>3015</t>
         </is>
       </c>
     </row>
@@ -20571,9 +21171,15 @@
       <c r="BJ103" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BK103" t="inlineStr">
-        <is>
-          <t>3011</t>
+      <c r="BK103" t="n">
+        <v>3011</v>
+      </c>
+      <c r="BL103" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="BM103" t="inlineStr">
+        <is>
+          <t>3249</t>
         </is>
       </c>
     </row>
@@ -20770,9 +21376,15 @@
       <c r="BJ104" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BK104" t="inlineStr">
-        <is>
-          <t>3375</t>
+      <c r="BK104" t="n">
+        <v>3375</v>
+      </c>
+      <c r="BL104" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="BM104" t="inlineStr">
+        <is>
+          <t>3635</t>
         </is>
       </c>
     </row>
@@ -20969,9 +21581,15 @@
       <c r="BJ105" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="BK105" t="inlineStr">
-        <is>
-          <t>3396</t>
+      <c r="BK105" t="n">
+        <v>3396</v>
+      </c>
+      <c r="BL105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM105" t="inlineStr">
+        <is>
+          <t>3539</t>
         </is>
       </c>
     </row>
@@ -21168,7 +21786,13 @@
       <c r="BJ106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK106" t="inlineStr">
+      <c r="BK106" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -21367,9 +21991,15 @@
       <c r="BJ107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK107" t="inlineStr">
-        <is>
-          <t>2689</t>
+      <c r="BK107" t="n">
+        <v>2689</v>
+      </c>
+      <c r="BL107" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="BM107" t="inlineStr">
+        <is>
+          <t>2773</t>
         </is>
       </c>
     </row>
@@ -21566,7 +22196,13 @@
       <c r="BJ108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK108" t="inlineStr">
+      <c r="BK108" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -21765,9 +22401,15 @@
       <c r="BJ109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK109" t="inlineStr">
-        <is>
-          <t>2635</t>
+      <c r="BK109" t="n">
+        <v>2635</v>
+      </c>
+      <c r="BL109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM109" t="inlineStr">
+        <is>
+          <t>2743</t>
         </is>
       </c>
     </row>
@@ -21964,9 +22606,15 @@
       <c r="BJ110" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BK110" t="inlineStr">
-        <is>
-          <t>3081</t>
+      <c r="BK110" t="n">
+        <v>3081</v>
+      </c>
+      <c r="BL110" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BM110" t="inlineStr">
+        <is>
+          <t>3418</t>
         </is>
       </c>
     </row>
@@ -22131,9 +22779,15 @@
       <c r="BJ111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK111" t="inlineStr">
-        <is>
-          <t>2573</t>
+      <c r="BK111" t="n">
+        <v>2573</v>
+      </c>
+      <c r="BL111" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="BM111" t="inlineStr">
+        <is>
+          <t>2660</t>
         </is>
       </c>
     </row>
@@ -22330,9 +22984,15 @@
       <c r="BJ112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK112" t="inlineStr">
-        <is>
-          <t>2526</t>
+      <c r="BK112" t="n">
+        <v>2526</v>
+      </c>
+      <c r="BL112" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="BM112" t="inlineStr">
+        <is>
+          <t>2563</t>
         </is>
       </c>
     </row>
@@ -22529,9 +23189,15 @@
       <c r="BJ113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK113" t="inlineStr">
-        <is>
-          <t>2721</t>
+      <c r="BK113" t="n">
+        <v>2721</v>
+      </c>
+      <c r="BL113" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM113" t="inlineStr">
+        <is>
+          <t>3138</t>
         </is>
       </c>
     </row>
@@ -22728,9 +23394,15 @@
       <c r="BJ114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK114" t="inlineStr">
-        <is>
-          <t>2678</t>
+      <c r="BK114" t="n">
+        <v>2678</v>
+      </c>
+      <c r="BL114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM114" t="inlineStr">
+        <is>
+          <t>2771</t>
         </is>
       </c>
     </row>
@@ -22927,9 +23599,15 @@
       <c r="BJ115" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="BK115" t="inlineStr">
-        <is>
-          <t>2305</t>
+      <c r="BK115" t="n">
+        <v>2305</v>
+      </c>
+      <c r="BL115" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="BM115" t="inlineStr">
+        <is>
+          <t>2375</t>
         </is>
       </c>
     </row>
@@ -23126,9 +23804,15 @@
       <c r="BJ116" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="BK116" t="inlineStr">
-        <is>
-          <t>2623</t>
+      <c r="BK116" t="n">
+        <v>2623</v>
+      </c>
+      <c r="BL116" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="BM116" t="inlineStr">
+        <is>
+          <t>2723</t>
         </is>
       </c>
     </row>
@@ -23325,9 +24009,15 @@
       <c r="BJ117" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BK117" t="inlineStr">
-        <is>
-          <t>3278</t>
+      <c r="BK117" t="n">
+        <v>3278</v>
+      </c>
+      <c r="BL117" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BM117" t="inlineStr">
+        <is>
+          <t>3586</t>
         </is>
       </c>
     </row>
@@ -23524,7 +24214,13 @@
       <c r="BJ118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK118" t="inlineStr">
+      <c r="BK118" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM118" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -23723,9 +24419,15 @@
       <c r="BJ119" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="BK119" t="inlineStr">
-        <is>
-          <t>3065</t>
+      <c r="BK119" t="n">
+        <v>3065</v>
+      </c>
+      <c r="BL119" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM119" t="inlineStr">
+        <is>
+          <t>3351</t>
         </is>
       </c>
     </row>
@@ -23922,9 +24624,15 @@
       <c r="BJ120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK120" t="inlineStr">
-        <is>
-          <t>2485</t>
+      <c r="BK120" t="n">
+        <v>2485</v>
+      </c>
+      <c r="BL120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM120" t="inlineStr">
+        <is>
+          <t>2478</t>
         </is>
       </c>
     </row>
@@ -24121,9 +24829,15 @@
       <c r="BJ121" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BK121" t="inlineStr">
-        <is>
-          <t>3065</t>
+      <c r="BK121" t="n">
+        <v>3065</v>
+      </c>
+      <c r="BL121" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM121" t="inlineStr">
+        <is>
+          <t>3303</t>
         </is>
       </c>
     </row>
@@ -24320,7 +25034,13 @@
       <c r="BJ122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK122" t="inlineStr">
+      <c r="BK122" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -24519,9 +25239,15 @@
       <c r="BJ123" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="BK123" t="inlineStr">
-        <is>
-          <t>2932</t>
+      <c r="BK123" t="n">
+        <v>2932</v>
+      </c>
+      <c r="BL123" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM123" t="inlineStr">
+        <is>
+          <t>3161</t>
         </is>
       </c>
     </row>
@@ -24718,9 +25444,15 @@
       <c r="BJ124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BK124" t="inlineStr">
-        <is>
-          <t>2985</t>
+      <c r="BK124" t="n">
+        <v>2985</v>
+      </c>
+      <c r="BL124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM124" t="inlineStr">
+        <is>
+          <t>3189</t>
         </is>
       </c>
     </row>
@@ -24917,9 +25649,15 @@
       <c r="BJ125" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BK125" t="inlineStr">
-        <is>
-          <t>2757</t>
+      <c r="BK125" t="n">
+        <v>2757</v>
+      </c>
+      <c r="BL125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM125" t="inlineStr">
+        <is>
+          <t>2755</t>
         </is>
       </c>
     </row>
@@ -25116,9 +25854,15 @@
       <c r="BJ126" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BK126" t="inlineStr">
-        <is>
-          <t>3105</t>
+      <c r="BK126" t="n">
+        <v>3105</v>
+      </c>
+      <c r="BL126" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM126" t="inlineStr">
+        <is>
+          <t>3344</t>
         </is>
       </c>
     </row>
@@ -25315,9 +26059,15 @@
       <c r="BJ127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK127" t="inlineStr">
-        <is>
-          <t>2001</t>
+      <c r="BK127" t="n">
+        <v>2001</v>
+      </c>
+      <c r="BL127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM127" t="inlineStr">
+        <is>
+          <t>1999</t>
         </is>
       </c>
     </row>
@@ -25514,7 +26264,13 @@
       <c r="BJ128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK128" t="inlineStr">
+      <c r="BK128" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -25713,7 +26469,13 @@
       <c r="BJ129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK129" t="inlineStr">
+      <c r="BK129" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -25912,9 +26674,15 @@
       <c r="BJ130" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="BK130" t="inlineStr">
-        <is>
-          <t>2959</t>
+      <c r="BK130" t="n">
+        <v>2959</v>
+      </c>
+      <c r="BL130" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="BM130" t="inlineStr">
+        <is>
+          <t>3021</t>
         </is>
       </c>
     </row>
@@ -26111,7 +26879,13 @@
       <c r="BJ131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK131" t="inlineStr">
+      <c r="BK131" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -26310,9 +27084,15 @@
       <c r="BJ132" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BK132" t="inlineStr">
-        <is>
-          <t>2611</t>
+      <c r="BK132" t="n">
+        <v>2611</v>
+      </c>
+      <c r="BL132" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM132" t="inlineStr">
+        <is>
+          <t>2706</t>
         </is>
       </c>
     </row>
@@ -26509,9 +27289,15 @@
       <c r="BJ133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK133" t="inlineStr">
-        <is>
-          <t>2528</t>
+      <c r="BK133" t="n">
+        <v>2528</v>
+      </c>
+      <c r="BL133" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM133" t="inlineStr">
+        <is>
+          <t>2814</t>
         </is>
       </c>
     </row>
@@ -26615,6 +27401,8 @@
       <c r="BI134" t="inlineStr"/>
       <c r="BJ134" s="3" t="inlineStr"/>
       <c r="BK134" t="inlineStr"/>
+      <c r="BL134" s="3" t="inlineStr"/>
+      <c r="BM134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -26708,6 +27496,8 @@
       <c r="BI135" t="inlineStr"/>
       <c r="BJ135" s="3" t="inlineStr"/>
       <c r="BK135" t="inlineStr"/>
+      <c r="BL135" s="3" t="inlineStr"/>
+      <c r="BM135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -26902,7 +27692,13 @@
       <c r="BJ136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK136" t="inlineStr">
+      <c r="BK136" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM136" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -27101,7 +27897,13 @@
       <c r="BJ137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK137" t="inlineStr">
+      <c r="BK137" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -27199,6 +28001,8 @@
       <c r="BI138" t="inlineStr"/>
       <c r="BJ138" s="3" t="inlineStr"/>
       <c r="BK138" t="inlineStr"/>
+      <c r="BL138" s="3" t="inlineStr"/>
+      <c r="BM138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -27393,9 +28197,15 @@
       <c r="BJ139" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="BK139" t="inlineStr">
-        <is>
-          <t>2723</t>
+      <c r="BK139" t="n">
+        <v>2723</v>
+      </c>
+      <c r="BL139" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM139" t="inlineStr">
+        <is>
+          <t>2952</t>
         </is>
       </c>
     </row>
@@ -27592,9 +28402,15 @@
       <c r="BJ140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK140" t="inlineStr">
-        <is>
-          <t>2497</t>
+      <c r="BK140" t="n">
+        <v>2497</v>
+      </c>
+      <c r="BL140" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM140" t="inlineStr">
+        <is>
+          <t>2689</t>
         </is>
       </c>
     </row>
@@ -27690,6 +28506,8 @@
       <c r="BI141" t="inlineStr"/>
       <c r="BJ141" s="3" t="inlineStr"/>
       <c r="BK141" t="inlineStr"/>
+      <c r="BL141" s="3" t="inlineStr"/>
+      <c r="BM141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -27884,7 +28702,13 @@
       <c r="BJ142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK142" t="inlineStr">
+      <c r="BK142" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM142" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -27982,6 +28806,8 @@
       <c r="BI143" t="inlineStr"/>
       <c r="BJ143" s="3" t="inlineStr"/>
       <c r="BK143" t="inlineStr"/>
+      <c r="BL143" s="3" t="inlineStr"/>
+      <c r="BM143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -28075,6 +28901,8 @@
       <c r="BI144" t="inlineStr"/>
       <c r="BJ144" s="3" t="inlineStr"/>
       <c r="BK144" t="inlineStr"/>
+      <c r="BL144" s="3" t="inlineStr"/>
+      <c r="BM144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -28168,6 +28996,8 @@
       <c r="BI145" t="inlineStr"/>
       <c r="BJ145" s="3" t="inlineStr"/>
       <c r="BK145" t="inlineStr"/>
+      <c r="BL145" s="3" t="inlineStr"/>
+      <c r="BM145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -28261,6 +29091,8 @@
       <c r="BI146" t="inlineStr"/>
       <c r="BJ146" s="3" t="inlineStr"/>
       <c r="BK146" t="inlineStr"/>
+      <c r="BL146" s="3" t="inlineStr"/>
+      <c r="BM146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -28354,6 +29186,8 @@
       <c r="BI147" t="inlineStr"/>
       <c r="BJ147" s="3" t="inlineStr"/>
       <c r="BK147" t="inlineStr"/>
+      <c r="BL147" s="3" t="inlineStr"/>
+      <c r="BM147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -28548,7 +29382,13 @@
       <c r="BJ148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK148" t="inlineStr">
+      <c r="BK148" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -28747,7 +29587,13 @@
       <c r="BJ149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK149" t="inlineStr">
+      <c r="BK149" t="n">
+        <v>2500</v>
+      </c>
+      <c r="BL149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM149" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -28946,7 +29792,13 @@
       <c r="BJ150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK150" t="inlineStr">
+      <c r="BK150" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -29145,7 +29997,13 @@
       <c r="BJ151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK151" t="inlineStr">
+      <c r="BK151" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -29344,7 +30202,13 @@
       <c r="BJ152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK152" t="inlineStr">
+      <c r="BK152" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -29543,7 +30407,13 @@
       <c r="BJ153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK153" t="inlineStr">
+      <c r="BK153" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -29742,7 +30612,13 @@
       <c r="BJ154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK154" t="inlineStr">
+      <c r="BK154" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -29941,9 +30817,15 @@
       <c r="BJ155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK155" t="inlineStr">
-        <is>
-          <t>2518</t>
+      <c r="BK155" t="n">
+        <v>2518</v>
+      </c>
+      <c r="BL155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM155" t="inlineStr">
+        <is>
+          <t>2635</t>
         </is>
       </c>
     </row>
@@ -30134,7 +31016,13 @@
       <c r="BJ156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK156" t="inlineStr">
+      <c r="BK156" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -30226,6 +31114,8 @@
       <c r="BI157" t="inlineStr"/>
       <c r="BJ157" s="3" t="inlineStr"/>
       <c r="BK157" t="inlineStr"/>
+      <c r="BL157" s="3" t="inlineStr"/>
+      <c r="BM157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -30414,7 +31304,13 @@
       <c r="BJ158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK158" t="inlineStr">
+      <c r="BK158" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -30607,9 +31503,15 @@
       <c r="BJ159" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BK159" t="inlineStr">
-        <is>
-          <t>3075</t>
+      <c r="BK159" t="n">
+        <v>3075</v>
+      </c>
+      <c r="BL159" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM159" t="inlineStr">
+        <is>
+          <t>3256</t>
         </is>
       </c>
     </row>
@@ -30699,6 +31601,8 @@
       <c r="BI160" t="inlineStr"/>
       <c r="BJ160" s="3" t="inlineStr"/>
       <c r="BK160" t="inlineStr"/>
+      <c r="BL160" s="3" t="inlineStr"/>
+      <c r="BM160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -30875,9 +31779,15 @@
       <c r="BJ161" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="BK161" t="inlineStr">
-        <is>
-          <t>3057</t>
+      <c r="BK161" t="n">
+        <v>3057</v>
+      </c>
+      <c r="BL161" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="BM161" t="inlineStr">
+        <is>
+          <t>3314</t>
         </is>
       </c>
     </row>
@@ -31056,9 +31966,15 @@
       <c r="BJ162" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="BK162" t="inlineStr">
-        <is>
-          <t>2809</t>
+      <c r="BK162" t="n">
+        <v>2809</v>
+      </c>
+      <c r="BL162" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM162" t="inlineStr">
+        <is>
+          <t>2852</t>
         </is>
       </c>
     </row>
@@ -31233,9 +32149,15 @@
       <c r="BJ163" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BK163" t="inlineStr">
-        <is>
-          <t>2785</t>
+      <c r="BK163" t="n">
+        <v>2785</v>
+      </c>
+      <c r="BL163" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM163" t="inlineStr">
+        <is>
+          <t>3060</t>
         </is>
       </c>
     </row>
@@ -31394,9 +32316,15 @@
       <c r="BJ164" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BK164" t="inlineStr">
-        <is>
-          <t>2782</t>
+      <c r="BK164" t="n">
+        <v>2782</v>
+      </c>
+      <c r="BL164" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM164" t="inlineStr">
+        <is>
+          <t>3037</t>
         </is>
       </c>
     </row>
@@ -31559,9 +32487,15 @@
       <c r="BJ165" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="BK165" t="inlineStr">
-        <is>
-          <t>2741</t>
+      <c r="BK165" t="n">
+        <v>2741</v>
+      </c>
+      <c r="BL165" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="BM165" t="inlineStr">
+        <is>
+          <t>2961</t>
         </is>
       </c>
     </row>
@@ -31716,9 +32650,15 @@
       <c r="BJ166" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK166" t="inlineStr">
-        <is>
-          <t>2538</t>
+      <c r="BK166" t="n">
+        <v>2538</v>
+      </c>
+      <c r="BL166" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="BM166" t="inlineStr">
+        <is>
+          <t>2934</t>
         </is>
       </c>
     </row>
@@ -31861,7 +32801,13 @@
       <c r="BJ167" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK167" t="inlineStr">
+      <c r="BK167" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL167" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM167" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -32002,7 +32948,13 @@
       <c r="BJ168" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK168" t="inlineStr">
+      <c r="BK168" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL168" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM168" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -32086,6 +33038,8 @@
       <c r="BI169" t="inlineStr"/>
       <c r="BJ169" s="3" t="inlineStr"/>
       <c r="BK169" t="inlineStr"/>
+      <c r="BL169" s="3" t="inlineStr"/>
+      <c r="BM169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="n">
@@ -32218,9 +33172,15 @@
       <c r="BJ170" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="BK170" t="inlineStr">
-        <is>
-          <t>1527</t>
+      <c r="BK170" t="n">
+        <v>1527</v>
+      </c>
+      <c r="BL170" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="BM170" t="inlineStr">
+        <is>
+          <t>1575</t>
         </is>
       </c>
     </row>
@@ -32343,7 +33303,13 @@
       <c r="BJ171" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK171" t="inlineStr">
+      <c r="BK171" t="n">
+        <v>1500</v>
+      </c>
+      <c r="BL171" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM171" t="inlineStr">
         <is>
           <t>1500</t>
         </is>
@@ -32468,7 +33434,13 @@
       <c r="BJ172" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK172" t="inlineStr">
+      <c r="BK172" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL172" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM172" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -32593,9 +33565,15 @@
       <c r="BJ173" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="BK173" t="inlineStr">
-        <is>
-          <t>1784</t>
+      <c r="BK173" t="n">
+        <v>1784</v>
+      </c>
+      <c r="BL173" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="BM173" t="inlineStr">
+        <is>
+          <t>1980</t>
         </is>
       </c>
     </row>
@@ -32689,6 +33667,8 @@
       <c r="BI174" t="inlineStr"/>
       <c r="BJ174" s="3" t="inlineStr"/>
       <c r="BK174" t="inlineStr"/>
+      <c r="BL174" s="3" t="inlineStr"/>
+      <c r="BM174" t="inlineStr"/>
     </row>
     <row r="175">
       <c r="A175" t="n">
@@ -32773,9 +33753,15 @@
       <c r="BJ175" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="BK175" t="inlineStr">
-        <is>
-          <t>2994</t>
+      <c r="BK175" t="n">
+        <v>2994</v>
+      </c>
+      <c r="BL175" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="BM175" t="inlineStr">
+        <is>
+          <t>3098</t>
         </is>
       </c>
     </row>
@@ -32858,9 +33844,15 @@
       <c r="BJ176" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="BK176" t="inlineStr">
-        <is>
-          <t>3299</t>
+      <c r="BK176" t="n">
+        <v>3299</v>
+      </c>
+      <c r="BL176" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="BM176" t="inlineStr">
+        <is>
+          <t>3601</t>
         </is>
       </c>
     </row>
@@ -32943,9 +33935,15 @@
       <c r="BJ177" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="BK177" t="inlineStr">
-        <is>
-          <t>3083</t>
+      <c r="BK177" t="n">
+        <v>3083</v>
+      </c>
+      <c r="BL177" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="BM177" t="inlineStr">
+        <is>
+          <t>3279</t>
         </is>
       </c>
     </row>
@@ -33028,9 +34026,15 @@
       <c r="BJ178" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BK178" t="inlineStr">
-        <is>
-          <t>2744</t>
+      <c r="BK178" t="n">
+        <v>2744</v>
+      </c>
+      <c r="BL178" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM178" t="inlineStr">
+        <is>
+          <t>2918</t>
         </is>
       </c>
     </row>

</xml_diff>